<commit_message>
update template DDG extracteur
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmy/Desktop/Betagouv/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F139D2-E493-5F48-919C-8D1671F02DF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81F938F-CD76-C846-8210-14F4E0829026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24580" windowHeight="14560" activeTab="5" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
@@ -626,9 +626,6 @@
     <t>#! DUMP_COLS x.actions</t>
   </si>
   <si>
-    <t xml:space="preserve">         Extracteur De Données D'Effectifs</t>
-  </si>
-  <si>
     <t>#` ${arrondissement}</t>
   </si>
   <si>
@@ -672,6 +669,9 @@
   </si>
   <si>
     <t xml:space="preserve">         Extracteur de données d'effectifs - Format DDG (avec réintégration de l'absentéisme)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         Extracteur de données d'effectifs</t>
   </si>
 </sst>
 </file>
@@ -1536,7 +1536,7 @@
   <dimension ref="A1:DN8"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1553,7 +1553,7 @@
   <sheetData>
     <row r="1" spans="1:118" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1868,7 +1868,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1942,10 +1942,10 @@
   <sheetData>
     <row r="1" spans="1:13" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="52" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1953,7 +1953,7 @@
     </row>
     <row r="2" spans="1:13" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="56" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" s="46" t="e">
         <f>VLOOKUP(A2,'codage tribunal'!A:B,2,FALSE)</f>
@@ -1974,37 +1974,37 @@
       <c r="C4" s="39"/>
       <c r="D4" s="40"/>
       <c r="E4" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="42" t="s">
+      <c r="G4" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="42" t="s">
+      <c r="H4" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="H4" s="42" t="s">
+      <c r="I4" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="I4" s="42" t="s">
+      <c r="J4" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="J4" s="42" t="s">
+      <c r="K4" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="K4" s="43" t="s">
-        <v>80</v>
-      </c>
       <c r="L4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="44"/>
       <c r="C5" s="48" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D5" s="47" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E5" s="51" t="e">
         <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"M-TIT",'ETPT Format DDG'!$C:$C,$A$2)</f>
@@ -2035,7 +2035,7 @@
         <v>#N/A</v>
       </c>
       <c r="L5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update template excel données d'effectif
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmy/Desktop/Betagouv/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E054AD9C-5FEE-444C-AC9A-C915ED0C461A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AFA25C5-CCD6-A14E-8507-17C853FC29DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24580" windowHeight="14560" activeTab="5" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
@@ -784,7 +784,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -868,36 +868,37 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -1332,7 +1333,7 @@
   <dimension ref="A1:DN8"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+      <selection activeCell="A161" sqref="A161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1620,7 +1621,7 @@
       <c r="E4"/>
     </row>
     <row r="5" spans="1:118" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+      <c r="B5" s="39" t="s">
         <v>15</v>
       </c>
       <c r="C5"/>
@@ -1653,7 +1654,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A139" sqref="A139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1703,7 +1704,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+      <c r="B5" s="39" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1716,7 +1717,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E893F90-1EC7-764C-B747-7920FCEC73CB}">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1736,7 +1737,7 @@
     <col min="11" max="11" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>35</v>
       </c>
@@ -1747,7 +1748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
         <v>22</v>
       </c>
@@ -1759,13 +1760,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="9"/>
     </row>
-    <row r="4" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="10"/>
       <c r="C4" s="10"/>
       <c r="D4" s="11"/>
@@ -1794,7 +1795,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="15"/>
       <c r="C5" s="19" t="s">
         <v>34</v>
@@ -1834,8 +1835,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="M6" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1882,263 +1883,273 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.1640625" style="36" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" style="36" customWidth="1"/>
-    <col min="3" max="9" width="10.83203125" style="36"/>
-    <col min="10" max="10" width="71.1640625" style="36" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="36"/>
+    <col min="1" max="1" width="8.1640625" style="24" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" style="24" customWidth="1"/>
+    <col min="3" max="9" width="10.83203125" style="24"/>
+    <col min="10" max="10" width="71.1640625" style="24" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="24"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="29" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-    </row>
-    <row r="2" spans="1:10" s="32" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+    </row>
+    <row r="2" spans="1:10" s="10" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-    </row>
-    <row r="3" spans="1:10" s="32" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+    </row>
+    <row r="3" spans="1:10" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="30"/>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
-    </row>
-    <row r="4" spans="1:10" s="32" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+    </row>
+    <row r="4" spans="1:10" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="30"/>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-    </row>
-    <row r="5" spans="1:10" s="32" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+    </row>
+    <row r="5" spans="1:10" s="10" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="30"/>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="34"/>
-    </row>
-    <row r="6" spans="1:10" s="32" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="33" t="s">
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
+    </row>
+    <row r="6" spans="1:10" s="10" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
-    </row>
-    <row r="7" spans="1:10" s="32" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+    </row>
+    <row r="7" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="30"/>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-    </row>
-    <row r="8" spans="1:10" s="32" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="35" t="s">
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+    </row>
+    <row r="8" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-    </row>
-    <row r="9" spans="1:10" s="32" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="35" t="s">
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+    </row>
+    <row r="9" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
-    </row>
-    <row r="10" spans="1:10" s="32" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="35" t="s">
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+    </row>
+    <row r="10" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="35"/>
-    </row>
-    <row r="11" spans="1:10" s="32" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="35" t="s">
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+    </row>
+    <row r="11" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
-    </row>
-    <row r="12" spans="1:10" s="32" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+    </row>
+    <row r="12" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="30" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="32" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" s="32" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="33" t="s">
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
+    </row>
+    <row r="13" spans="1:10" s="10" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="34" t="s">
+      <c r="C13" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-    </row>
-    <row r="14" spans="1:10" s="32" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="33" t="s">
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
+    </row>
+    <row r="14" spans="1:10" s="10" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="34" t="s">
+      <c r="C14" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-    </row>
-    <row r="15" spans="1:10" s="32" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="33" t="s">
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
+    </row>
+    <row r="15" spans="1:10" s="10" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-    </row>
-    <row r="16" spans="1:10" s="32" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="33" t="s">
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="37"/>
+    </row>
+    <row r="16" spans="1:10" s="10" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="37"/>
     </row>
     <row r="18" spans="1:10" s="29" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="38"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="38"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="36"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="17">
+    <mergeCell ref="C14:J14"/>
+    <mergeCell ref="B12:J12"/>
     <mergeCell ref="B7:J7"/>
     <mergeCell ref="A18:J18"/>
     <mergeCell ref="A1:J1"/>
@@ -2154,7 +2165,6 @@
     <mergeCell ref="B10:J10"/>
     <mergeCell ref="B11:J11"/>
     <mergeCell ref="C13:J13"/>
-    <mergeCell ref="C14:J14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update extraction template ddg
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmy/Desktop/Betagouv/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AFA25C5-CCD6-A14E-8507-17C853FC29DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F89413-D477-E346-84BF-35A1BA14109B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24580" windowHeight="14560" activeTab="5" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24580" windowHeight="14560" activeTab="2" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
   <sheets>
     <sheet name="ETPT A-JUST" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="62">
   <si>
     <t>#! END_ROW</t>
   </si>
@@ -134,9 +134,6 @@
     <t>Fonctionnaires placés de substitution</t>
   </si>
   <si>
-    <t>Contractuels</t>
-  </si>
-  <si>
     <t>Code</t>
   </si>
   <si>
@@ -570,6 +567,24 @@
   </si>
   <si>
     <t>Pour toute question, n'hésitez pas à contacter l'équipe A-JUST : support-utilisateurs@a-just.fr</t>
+  </si>
+  <si>
+    <t>SIEGE</t>
+  </si>
+  <si>
+    <t>GREFFE</t>
+  </si>
+  <si>
+    <t>EQUIPE AUTOUR DU MAGISTRAT</t>
+  </si>
+  <si>
+    <t>Contractuels et vacataires</t>
+  </si>
+  <si>
+    <t>TOTAL SIEGE</t>
+  </si>
+  <si>
+    <t>TOTAL GREFFE</t>
   </si>
 </sst>
 </file>
@@ -583,7 +598,7 @@
     <numFmt numFmtId="166" formatCode="General;General;\-"/>
     <numFmt numFmtId="167" formatCode="0.###;0.###;\-"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -660,6 +675,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -705,7 +728,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -777,6 +800,82 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -784,7 +883,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -825,9 +924,6 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -877,6 +973,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -892,13 +992,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -906,7 +1026,22 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{6FC886D6-2077-B34D-B1DF-739B068A66D1}"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1333,7 +1468,7 @@
   <dimension ref="A1:DN8"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A161" sqref="A161"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1350,7 +1485,7 @@
   <sheetData>
     <row r="1" spans="1:118" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1365,131 +1500,131 @@
       </c>
     </row>
     <row r="2" spans="1:118" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
-      <c r="U2" s="24"/>
-      <c r="V2" s="24"/>
-      <c r="W2" s="24"/>
-      <c r="X2" s="24"/>
-      <c r="Y2" s="24"/>
-      <c r="Z2" s="24"/>
-      <c r="AA2" s="24"/>
-      <c r="AB2" s="24"/>
-      <c r="AC2" s="24"/>
-      <c r="AD2" s="24"/>
-      <c r="AE2" s="24"/>
-      <c r="AF2" s="24"/>
-      <c r="AG2" s="24"/>
-      <c r="AH2" s="24"/>
-      <c r="AI2" s="24"/>
-      <c r="AJ2" s="24"/>
-      <c r="AK2" s="24"/>
-      <c r="AL2" s="24"/>
-      <c r="AM2" s="24"/>
-      <c r="AN2" s="24"/>
-      <c r="AO2" s="24"/>
-      <c r="AP2" s="24"/>
-      <c r="AQ2" s="24"/>
-      <c r="AR2" s="24"/>
-      <c r="AS2" s="24"/>
-      <c r="AT2" s="24"/>
-      <c r="AU2" s="24"/>
-      <c r="AV2" s="24"/>
-      <c r="AW2" s="24"/>
-      <c r="AX2" s="24"/>
-      <c r="AY2" s="24"/>
-      <c r="AZ2" s="24"/>
-      <c r="BA2" s="24"/>
-      <c r="BB2" s="24"/>
-      <c r="BC2" s="24"/>
-      <c r="BD2" s="24"/>
-      <c r="BE2" s="24"/>
-      <c r="BF2" s="24"/>
-      <c r="BG2" s="24"/>
-      <c r="BH2" s="24"/>
-      <c r="BI2" s="24"/>
-      <c r="BJ2" s="24"/>
-      <c r="BK2" s="24"/>
-      <c r="BL2" s="24"/>
-      <c r="BM2" s="24"/>
-      <c r="BN2" s="24"/>
-      <c r="BO2" s="24"/>
-      <c r="BP2" s="24"/>
-      <c r="BQ2" s="24"/>
-      <c r="BR2" s="24"/>
-      <c r="BS2" s="24"/>
-      <c r="BT2" s="24"/>
-      <c r="BU2" s="24"/>
-      <c r="BV2" s="24"/>
-      <c r="BW2" s="24"/>
-      <c r="BX2" s="24"/>
-      <c r="BY2" s="24"/>
-      <c r="BZ2" s="24"/>
-      <c r="CA2" s="24"/>
-      <c r="CB2" s="24"/>
-      <c r="CC2" s="24"/>
-      <c r="CD2" s="24"/>
-      <c r="CE2" s="24"/>
-      <c r="CF2" s="24"/>
-      <c r="CG2" s="24"/>
-      <c r="CH2" s="24"/>
-      <c r="CI2" s="24"/>
-      <c r="CJ2" s="24"/>
-      <c r="CK2" s="24"/>
-      <c r="CL2" s="24"/>
-      <c r="CM2" s="24"/>
-      <c r="CN2" s="24"/>
-      <c r="CO2" s="24"/>
-      <c r="CP2" s="24"/>
-      <c r="CQ2" s="24"/>
-      <c r="CR2" s="24"/>
-      <c r="CS2" s="24"/>
-      <c r="CT2" s="24"/>
-      <c r="CU2" s="24"/>
-      <c r="CV2" s="24"/>
-      <c r="CW2" s="24"/>
-      <c r="CX2" s="24"/>
-      <c r="CY2" s="24"/>
-      <c r="CZ2" s="24"/>
-      <c r="DA2" s="24"/>
-      <c r="DB2" s="24"/>
-      <c r="DC2" s="24"/>
-      <c r="DD2" s="24"/>
-      <c r="DE2" s="24"/>
-      <c r="DF2" s="24"/>
-      <c r="DG2" s="24"/>
-      <c r="DH2" s="24"/>
-      <c r="DI2" s="24"/>
-      <c r="DJ2" s="24"/>
-      <c r="DK2" s="24"/>
-      <c r="DL2" s="24"/>
-      <c r="DM2" s="24"/>
-      <c r="DN2" s="24"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="23"/>
+      <c r="W2" s="23"/>
+      <c r="X2" s="23"/>
+      <c r="Y2" s="23"/>
+      <c r="Z2" s="23"/>
+      <c r="AA2" s="23"/>
+      <c r="AB2" s="23"/>
+      <c r="AC2" s="23"/>
+      <c r="AD2" s="23"/>
+      <c r="AE2" s="23"/>
+      <c r="AF2" s="23"/>
+      <c r="AG2" s="23"/>
+      <c r="AH2" s="23"/>
+      <c r="AI2" s="23"/>
+      <c r="AJ2" s="23"/>
+      <c r="AK2" s="23"/>
+      <c r="AL2" s="23"/>
+      <c r="AM2" s="23"/>
+      <c r="AN2" s="23"/>
+      <c r="AO2" s="23"/>
+      <c r="AP2" s="23"/>
+      <c r="AQ2" s="23"/>
+      <c r="AR2" s="23"/>
+      <c r="AS2" s="23"/>
+      <c r="AT2" s="23"/>
+      <c r="AU2" s="23"/>
+      <c r="AV2" s="23"/>
+      <c r="AW2" s="23"/>
+      <c r="AX2" s="23"/>
+      <c r="AY2" s="23"/>
+      <c r="AZ2" s="23"/>
+      <c r="BA2" s="23"/>
+      <c r="BB2" s="23"/>
+      <c r="BC2" s="23"/>
+      <c r="BD2" s="23"/>
+      <c r="BE2" s="23"/>
+      <c r="BF2" s="23"/>
+      <c r="BG2" s="23"/>
+      <c r="BH2" s="23"/>
+      <c r="BI2" s="23"/>
+      <c r="BJ2" s="23"/>
+      <c r="BK2" s="23"/>
+      <c r="BL2" s="23"/>
+      <c r="BM2" s="23"/>
+      <c r="BN2" s="23"/>
+      <c r="BO2" s="23"/>
+      <c r="BP2" s="23"/>
+      <c r="BQ2" s="23"/>
+      <c r="BR2" s="23"/>
+      <c r="BS2" s="23"/>
+      <c r="BT2" s="23"/>
+      <c r="BU2" s="23"/>
+      <c r="BV2" s="23"/>
+      <c r="BW2" s="23"/>
+      <c r="BX2" s="23"/>
+      <c r="BY2" s="23"/>
+      <c r="BZ2" s="23"/>
+      <c r="CA2" s="23"/>
+      <c r="CB2" s="23"/>
+      <c r="CC2" s="23"/>
+      <c r="CD2" s="23"/>
+      <c r="CE2" s="23"/>
+      <c r="CF2" s="23"/>
+      <c r="CG2" s="23"/>
+      <c r="CH2" s="23"/>
+      <c r="CI2" s="23"/>
+      <c r="CJ2" s="23"/>
+      <c r="CK2" s="23"/>
+      <c r="CL2" s="23"/>
+      <c r="CM2" s="23"/>
+      <c r="CN2" s="23"/>
+      <c r="CO2" s="23"/>
+      <c r="CP2" s="23"/>
+      <c r="CQ2" s="23"/>
+      <c r="CR2" s="23"/>
+      <c r="CS2" s="23"/>
+      <c r="CT2" s="23"/>
+      <c r="CU2" s="23"/>
+      <c r="CV2" s="23"/>
+      <c r="CW2" s="23"/>
+      <c r="CX2" s="23"/>
+      <c r="CY2" s="23"/>
+      <c r="CZ2" s="23"/>
+      <c r="DA2" s="23"/>
+      <c r="DB2" s="23"/>
+      <c r="DC2" s="23"/>
+      <c r="DD2" s="23"/>
+      <c r="DE2" s="23"/>
+      <c r="DF2" s="23"/>
+      <c r="DG2" s="23"/>
+      <c r="DH2" s="23"/>
+      <c r="DI2" s="23"/>
+      <c r="DJ2" s="23"/>
+      <c r="DK2" s="23"/>
+      <c r="DL2" s="23"/>
+      <c r="DM2" s="23"/>
+      <c r="DN2" s="23"/>
     </row>
     <row r="3" spans="1:118" x14ac:dyDescent="0.2">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="27" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
@@ -1498,119 +1633,119 @@
       <c r="C3"/>
       <c r="D3"/>
       <c r="E3"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="26"/>
-      <c r="R3" s="26"/>
-      <c r="S3" s="26"/>
-      <c r="T3" s="26"/>
-      <c r="U3" s="26"/>
-      <c r="V3" s="26"/>
-      <c r="W3" s="26"/>
-      <c r="X3" s="26"/>
-      <c r="Y3" s="26"/>
-      <c r="Z3" s="26"/>
-      <c r="AA3" s="26"/>
-      <c r="AB3" s="26"/>
-      <c r="AC3" s="26"/>
-      <c r="AD3" s="26"/>
-      <c r="AE3" s="26"/>
-      <c r="AF3" s="26"/>
-      <c r="AG3" s="26"/>
-      <c r="AH3" s="26"/>
-      <c r="AI3" s="26"/>
-      <c r="AJ3" s="26"/>
-      <c r="AK3" s="26"/>
-      <c r="AL3" s="26"/>
-      <c r="AM3" s="26"/>
-      <c r="AN3" s="26"/>
-      <c r="AO3" s="26"/>
-      <c r="AP3" s="26"/>
-      <c r="AQ3" s="26"/>
-      <c r="AR3" s="26"/>
-      <c r="AS3" s="26"/>
-      <c r="AT3" s="26"/>
-      <c r="AU3" s="26"/>
-      <c r="AV3" s="26"/>
-      <c r="AW3" s="26"/>
-      <c r="AX3" s="26"/>
-      <c r="AY3" s="26"/>
-      <c r="AZ3" s="26"/>
-      <c r="BA3" s="26"/>
-      <c r="BB3" s="26"/>
-      <c r="BC3" s="26"/>
-      <c r="BD3" s="26"/>
-      <c r="BE3" s="26"/>
-      <c r="BF3" s="26"/>
-      <c r="BG3" s="26"/>
-      <c r="BH3" s="26"/>
-      <c r="BI3" s="26"/>
-      <c r="BJ3" s="26"/>
-      <c r="BK3" s="26"/>
-      <c r="BL3" s="26"/>
-      <c r="BM3" s="26"/>
-      <c r="BN3" s="26"/>
-      <c r="BO3" s="26"/>
-      <c r="BP3" s="26"/>
-      <c r="BQ3" s="26"/>
-      <c r="BR3" s="26"/>
-      <c r="BS3" s="26"/>
-      <c r="BT3" s="26"/>
-      <c r="BU3" s="26"/>
-      <c r="BV3" s="26"/>
-      <c r="BW3" s="26"/>
-      <c r="BX3" s="26"/>
-      <c r="BY3" s="26"/>
-      <c r="BZ3" s="26"/>
-      <c r="CA3" s="26"/>
-      <c r="CB3" s="26"/>
-      <c r="CC3" s="26"/>
-      <c r="CD3" s="26"/>
-      <c r="CE3" s="26"/>
-      <c r="CF3" s="26"/>
-      <c r="CG3" s="26"/>
-      <c r="CH3" s="26"/>
-      <c r="CI3" s="26"/>
-      <c r="CJ3" s="26"/>
-      <c r="CK3" s="26"/>
-      <c r="CL3" s="26"/>
-      <c r="CM3" s="26"/>
-      <c r="CN3" s="26"/>
-      <c r="CO3" s="26"/>
-      <c r="CP3" s="26"/>
-      <c r="CQ3" s="26"/>
-      <c r="CR3" s="26"/>
-      <c r="CS3" s="26"/>
-      <c r="CT3" s="26"/>
-      <c r="CU3" s="26"/>
-      <c r="CV3" s="26"/>
-      <c r="CW3" s="26"/>
-      <c r="CX3" s="26"/>
-      <c r="CY3" s="26"/>
-      <c r="CZ3" s="26"/>
-      <c r="DA3" s="26"/>
-      <c r="DB3" s="26"/>
-      <c r="DC3" s="26"/>
-      <c r="DD3" s="26"/>
-      <c r="DE3" s="26"/>
-      <c r="DF3" s="26"/>
-      <c r="DG3" s="26"/>
-      <c r="DH3" s="26"/>
-      <c r="DI3" s="26"/>
-      <c r="DJ3" s="26"/>
-      <c r="DK3" s="26"/>
-      <c r="DL3" s="26"/>
-      <c r="DM3" s="26"/>
-      <c r="DN3" s="26"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
+      <c r="Q3" s="25"/>
+      <c r="R3" s="25"/>
+      <c r="S3" s="25"/>
+      <c r="T3" s="25"/>
+      <c r="U3" s="25"/>
+      <c r="V3" s="25"/>
+      <c r="W3" s="25"/>
+      <c r="X3" s="25"/>
+      <c r="Y3" s="25"/>
+      <c r="Z3" s="25"/>
+      <c r="AA3" s="25"/>
+      <c r="AB3" s="25"/>
+      <c r="AC3" s="25"/>
+      <c r="AD3" s="25"/>
+      <c r="AE3" s="25"/>
+      <c r="AF3" s="25"/>
+      <c r="AG3" s="25"/>
+      <c r="AH3" s="25"/>
+      <c r="AI3" s="25"/>
+      <c r="AJ3" s="25"/>
+      <c r="AK3" s="25"/>
+      <c r="AL3" s="25"/>
+      <c r="AM3" s="25"/>
+      <c r="AN3" s="25"/>
+      <c r="AO3" s="25"/>
+      <c r="AP3" s="25"/>
+      <c r="AQ3" s="25"/>
+      <c r="AR3" s="25"/>
+      <c r="AS3" s="25"/>
+      <c r="AT3" s="25"/>
+      <c r="AU3" s="25"/>
+      <c r="AV3" s="25"/>
+      <c r="AW3" s="25"/>
+      <c r="AX3" s="25"/>
+      <c r="AY3" s="25"/>
+      <c r="AZ3" s="25"/>
+      <c r="BA3" s="25"/>
+      <c r="BB3" s="25"/>
+      <c r="BC3" s="25"/>
+      <c r="BD3" s="25"/>
+      <c r="BE3" s="25"/>
+      <c r="BF3" s="25"/>
+      <c r="BG3" s="25"/>
+      <c r="BH3" s="25"/>
+      <c r="BI3" s="25"/>
+      <c r="BJ3" s="25"/>
+      <c r="BK3" s="25"/>
+      <c r="BL3" s="25"/>
+      <c r="BM3" s="25"/>
+      <c r="BN3" s="25"/>
+      <c r="BO3" s="25"/>
+      <c r="BP3" s="25"/>
+      <c r="BQ3" s="25"/>
+      <c r="BR3" s="25"/>
+      <c r="BS3" s="25"/>
+      <c r="BT3" s="25"/>
+      <c r="BU3" s="25"/>
+      <c r="BV3" s="25"/>
+      <c r="BW3" s="25"/>
+      <c r="BX3" s="25"/>
+      <c r="BY3" s="25"/>
+      <c r="BZ3" s="25"/>
+      <c r="CA3" s="25"/>
+      <c r="CB3" s="25"/>
+      <c r="CC3" s="25"/>
+      <c r="CD3" s="25"/>
+      <c r="CE3" s="25"/>
+      <c r="CF3" s="25"/>
+      <c r="CG3" s="25"/>
+      <c r="CH3" s="25"/>
+      <c r="CI3" s="25"/>
+      <c r="CJ3" s="25"/>
+      <c r="CK3" s="25"/>
+      <c r="CL3" s="25"/>
+      <c r="CM3" s="25"/>
+      <c r="CN3" s="25"/>
+      <c r="CO3" s="25"/>
+      <c r="CP3" s="25"/>
+      <c r="CQ3" s="25"/>
+      <c r="CR3" s="25"/>
+      <c r="CS3" s="25"/>
+      <c r="CT3" s="25"/>
+      <c r="CU3" s="25"/>
+      <c r="CV3" s="25"/>
+      <c r="CW3" s="25"/>
+      <c r="CX3" s="25"/>
+      <c r="CY3" s="25"/>
+      <c r="CZ3" s="25"/>
+      <c r="DA3" s="25"/>
+      <c r="DB3" s="25"/>
+      <c r="DC3" s="25"/>
+      <c r="DD3" s="25"/>
+      <c r="DE3" s="25"/>
+      <c r="DF3" s="25"/>
+      <c r="DG3" s="25"/>
+      <c r="DH3" s="25"/>
+      <c r="DI3" s="25"/>
+      <c r="DJ3" s="25"/>
+      <c r="DK3" s="25"/>
+      <c r="DL3" s="25"/>
+      <c r="DM3" s="25"/>
+      <c r="DN3" s="25"/>
     </row>
     <row r="4" spans="1:118" x14ac:dyDescent="0.2">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="27" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -1621,7 +1756,7 @@
       <c r="E4"/>
     </row>
     <row r="5" spans="1:118" x14ac:dyDescent="0.2">
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="31" t="s">
         <v>15</v>
       </c>
       <c r="C5"/>
@@ -1665,7 +1800,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1680,7 +1815,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>16</v>
       </c>
       <c r="B2" t="s">
@@ -1688,7 +1823,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="27" t="s">
         <v>21</v>
       </c>
       <c r="B3" t="s">
@@ -1696,7 +1831,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="27" t="s">
         <v>21</v>
       </c>
       <c r="B4" t="s">
@@ -1704,7 +1839,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="31" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1717,10 +1852,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E893F90-1EC7-764C-B747-7920FCEC73CB}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="E4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1735,24 +1870,25 @@
     <col min="9" max="9" width="18.33203125" customWidth="1"/>
     <col min="10" max="10" width="20.5" customWidth="1"/>
     <col min="11" max="11" width="16.6640625" customWidth="1"/>
+    <col min="15" max="15" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>30</v>
+    <row r="1" spans="1:16" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>29</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
+    <row r="2" spans="1:16" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="17" t="e">
+      <c r="B2" s="16" t="e">
         <f>VLOOKUP(A2,'codage tribunal'!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
@@ -1760,13 +1896,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:16" ht="40" x14ac:dyDescent="0.2">
+      <c r="C3" s="9"/>
+      <c r="E3" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="41"/>
+      <c r="O3" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="P3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="9"/>
-    </row>
-    <row r="4" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:16" ht="80" x14ac:dyDescent="0.2">
       <c r="A4" s="10"/>
       <c r="C4" s="10"/>
       <c r="D4" s="11"/>
@@ -1779,70 +1932,126 @@
       <c r="G4" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="K4" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="L4" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="K4" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="L4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="15"/>
-      <c r="C5" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="18" t="s">
+      <c r="M4" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="N4" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="O4" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="P4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" s="14"/>
+      <c r="C5" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="22" t="e">
+      <c r="D5" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="21" t="e">
         <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"M-TIT",'ETPT Format DDG'!$C:$C,$A$2)</f>
         <v>#N/A</v>
       </c>
-      <c r="F5" s="20" t="e">
+      <c r="F5" s="19" t="e">
         <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"M-PLAC-ADD",'ETPT Format DDG'!$C:$C,$A$2)</f>
         <v>#N/A</v>
       </c>
-      <c r="G5" s="20" t="e">
+      <c r="G5" s="19" t="e">
         <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"M-PLAC-SUB",'ETPT Format DDG'!$C:$C,$A$2)</f>
         <v>#N/A</v>
       </c>
-      <c r="H5" s="20" t="e">
+      <c r="H5" s="19" t="e">
+        <f>SUMIFS(
+INDEX('ETPT Format DDG'!$A:$DU,
+,
+IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))
+),'ETPT Format DDG'!$I:$I,"C",
+'ETPT Format DDG'!$C:$C,$A$2,
+'ETPT Format DDG'!$G:$G,"Magistrat")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I5" s="46" t="e">
+        <f>SUMIFS(
+INDEX('ETPT Format DDG'!$A:$DU,
+,
+IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))
+),
+'ETPT Format DDG'!$C:$C,$A$2,
+'ETPT Format DDG'!$G:$G,"Magistrat")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J5" s="19" t="e">
         <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"F-TIT",'ETPT Format DDG'!$C:$C,$A$2)</f>
         <v>#N/A</v>
       </c>
-      <c r="I5" s="20" t="e">
+      <c r="K5" s="19" t="e">
         <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"F-PLAC-ADD",'ETPT Format DDG'!$C:$C,$A$2)</f>
         <v>#N/A</v>
       </c>
-      <c r="J5" s="20" t="e">
+      <c r="L5" s="19" t="e">
         <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"F-PLAC-SUB",'ETPT Format DDG'!$C:$C,$A$2)</f>
         <v>#N/A</v>
       </c>
-      <c r="K5" s="21" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"C",'ETPT Format DDG'!$C:$C,$A$2)</f>
+      <c r="M5" s="20" t="e">
+        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"C",'ETPT Format DDG'!$C:$C,$A$2,'ETPT Format DDG'!$G:$G,"Greffe")</f>
         <v>#N/A</v>
       </c>
-      <c r="L5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="L6" t="s">
+      <c r="N5" s="46" t="e">
+        <f>SUMIFS(
+INDEX('ETPT Format DDG'!$A:$DU,
+,
+IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))
+),
+'ETPT Format DDG'!$C:$C,$A$2,
+'ETPT Format DDG'!$G:$G,"Greffe")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O5" s="20" t="e">
+        <f>SUMIFS(
+INDEX('ETPT Format DDG'!$A:$DU,
+,
+IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))
+),'ETPT Format DDG'!$I:$I,"C",
+'ETPT Format DDG'!$C:$C,$A$2,
+'ETPT Format DDG'!$G:$G,"Autour du magistrat")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P6" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C5:K150">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <mergeCells count="2">
+    <mergeCell ref="E3:I3"/>
+    <mergeCell ref="J3:N3"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C5:O150">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>AND(ISBLANK($C5)=FALSE,ISBLANK($D5)=TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1882,130 +2091,130 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C706A55-5422-5B42-B9B4-A00444FB459D}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.1640625" style="24" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" style="24" customWidth="1"/>
-    <col min="3" max="9" width="10.83203125" style="24"/>
-    <col min="10" max="10" width="71.1640625" style="24" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="24"/>
+    <col min="1" max="1" width="8.1640625" style="23" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" style="23" customWidth="1"/>
+    <col min="3" max="9" width="10.83203125" style="23"/>
+    <col min="10" max="10" width="71.1640625" style="23" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="29" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:10" s="28" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+    </row>
+    <row r="2" spans="1:10" s="10" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-    </row>
-    <row r="2" spans="1:10" s="10" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="34" t="s">
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+    </row>
+    <row r="3" spans="1:10" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="29"/>
+      <c r="B3" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-    </row>
-    <row r="3" spans="1:10" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="30"/>
-      <c r="B3" s="31" t="s">
+      <c r="C3" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+    </row>
+    <row r="4" spans="1:10" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="29"/>
+      <c r="B4" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-    </row>
-    <row r="4" spans="1:10" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="30"/>
-      <c r="B4" s="31" t="s">
+      <c r="C4" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+    </row>
+    <row r="5" spans="1:10" s="10" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="29"/>
+      <c r="B5" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-    </row>
-    <row r="5" spans="1:10" s="10" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="30"/>
-      <c r="B5" s="31" t="s">
+      <c r="C5" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+    </row>
+    <row r="6" spans="1:10" s="10" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="37"/>
-    </row>
-    <row r="6" spans="1:10" s="10" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="37" t="s">
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+    </row>
+    <row r="7" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="29"/>
+      <c r="B7" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-    </row>
-    <row r="7" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="30"/>
-      <c r="B7" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
     </row>
     <row r="8" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" s="38"/>
       <c r="D8" s="38"/>
@@ -2031,7 +2240,7 @@
     </row>
     <row r="10" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" s="38"/>
       <c r="D10" s="38"/>
@@ -2044,7 +2253,7 @@
     </row>
     <row r="11" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" s="38"/>
       <c r="D11" s="38"/>
@@ -2056,98 +2265,99 @@
       <c r="J11" s="38"/>
     </row>
     <row r="12" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+    </row>
+    <row r="13" spans="1:10" s="10" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-    </row>
-    <row r="13" spans="1:10" s="10" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="37" t="s">
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
+    </row>
+    <row r="14" spans="1:10" s="10" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="37"/>
-    </row>
-    <row r="14" spans="1:10" s="10" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="37" t="s">
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+    </row>
+    <row r="15" spans="1:10" s="10" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
-    </row>
-    <row r="15" spans="1:10" s="10" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="37" t="s">
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
+    </row>
+    <row r="16" spans="1:10" s="10" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="37"/>
-    </row>
-    <row r="16" spans="1:10" s="10" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="37" t="s">
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+    </row>
+    <row r="18" spans="1:10" s="28" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
-    </row>
-    <row r="18" spans="1:10" s="29" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" s="36"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="36"/>
-      <c r="J18" s="36"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C13:J13"/>
     <mergeCell ref="C14:J14"/>
     <mergeCell ref="B12:J12"/>
     <mergeCell ref="B7:J7"/>
@@ -2164,7 +2374,6 @@
     <mergeCell ref="B9:J9"/>
     <mergeCell ref="B10:J10"/>
     <mergeCell ref="B11:J11"/>
-    <mergeCell ref="C13:J13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update DDG template 2
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmy/Desktop/Betagouv/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F89413-D477-E346-84BF-35A1BA14109B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24816E1E-27A1-9147-92A5-D82FD9079116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24580" windowHeight="14560" activeTab="2" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24580" windowHeight="14560" activeTab="5" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
   <sheets>
     <sheet name="ETPT A-JUST" sheetId="1" r:id="rId1"/>
@@ -1854,8 +1854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E893F90-1EC7-764C-B747-7920FCEC73CB}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2091,7 +2091,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C706A55-5422-5B42-B9B4-A00444FB459D}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update popin extracteur & formatage fichier ETPT
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmy/Desktop/Betagouv/a-just/front/src/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24816E1E-27A1-9147-92A5-D82FD9079116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C34238-0F47-A349-9585-09C806FD1DFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24580" windowHeight="14560" activeTab="5" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="22480" windowHeight="17620" activeTab="5" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
   <sheets>
     <sheet name="ETPT A-JUST" sheetId="1" r:id="rId1"/>
@@ -592,11 +592,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="General;General;\-"/>
-    <numFmt numFmtId="167" formatCode="0.###;0.###;\-"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="General;General;\-"/>
+    <numFmt numFmtId="168" formatCode="0.###;0.###;\-"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -880,8 +880,8 @@
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -918,10 +918,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -933,19 +933,13 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -957,11 +951,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -974,6 +968,30 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -995,53 +1013,20 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="4" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Comma" xfId="3" builtinId="3"/>
     <cellStyle name="Comma 2" xfId="2" xr:uid="{C877C5E8-FCBF-114F-9ECB-F75EF7C9C0EB}"/>
+    <cellStyle name="Milliers" xfId="3" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{6FC886D6-2077-B34D-B1DF-739B068A66D1}"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -1169,7 +1154,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1468,7 +1453,7 @@
   <dimension ref="A1:DN8"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A177" sqref="A177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1500,131 +1485,131 @@
       </c>
     </row>
     <row r="2" spans="1:118" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
-      <c r="S2" s="23"/>
-      <c r="T2" s="23"/>
-      <c r="U2" s="23"/>
-      <c r="V2" s="23"/>
-      <c r="W2" s="23"/>
-      <c r="X2" s="23"/>
-      <c r="Y2" s="23"/>
-      <c r="Z2" s="23"/>
-      <c r="AA2" s="23"/>
-      <c r="AB2" s="23"/>
-      <c r="AC2" s="23"/>
-      <c r="AD2" s="23"/>
-      <c r="AE2" s="23"/>
-      <c r="AF2" s="23"/>
-      <c r="AG2" s="23"/>
-      <c r="AH2" s="23"/>
-      <c r="AI2" s="23"/>
-      <c r="AJ2" s="23"/>
-      <c r="AK2" s="23"/>
-      <c r="AL2" s="23"/>
-      <c r="AM2" s="23"/>
-      <c r="AN2" s="23"/>
-      <c r="AO2" s="23"/>
-      <c r="AP2" s="23"/>
-      <c r="AQ2" s="23"/>
-      <c r="AR2" s="23"/>
-      <c r="AS2" s="23"/>
-      <c r="AT2" s="23"/>
-      <c r="AU2" s="23"/>
-      <c r="AV2" s="23"/>
-      <c r="AW2" s="23"/>
-      <c r="AX2" s="23"/>
-      <c r="AY2" s="23"/>
-      <c r="AZ2" s="23"/>
-      <c r="BA2" s="23"/>
-      <c r="BB2" s="23"/>
-      <c r="BC2" s="23"/>
-      <c r="BD2" s="23"/>
-      <c r="BE2" s="23"/>
-      <c r="BF2" s="23"/>
-      <c r="BG2" s="23"/>
-      <c r="BH2" s="23"/>
-      <c r="BI2" s="23"/>
-      <c r="BJ2" s="23"/>
-      <c r="BK2" s="23"/>
-      <c r="BL2" s="23"/>
-      <c r="BM2" s="23"/>
-      <c r="BN2" s="23"/>
-      <c r="BO2" s="23"/>
-      <c r="BP2" s="23"/>
-      <c r="BQ2" s="23"/>
-      <c r="BR2" s="23"/>
-      <c r="BS2" s="23"/>
-      <c r="BT2" s="23"/>
-      <c r="BU2" s="23"/>
-      <c r="BV2" s="23"/>
-      <c r="BW2" s="23"/>
-      <c r="BX2" s="23"/>
-      <c r="BY2" s="23"/>
-      <c r="BZ2" s="23"/>
-      <c r="CA2" s="23"/>
-      <c r="CB2" s="23"/>
-      <c r="CC2" s="23"/>
-      <c r="CD2" s="23"/>
-      <c r="CE2" s="23"/>
-      <c r="CF2" s="23"/>
-      <c r="CG2" s="23"/>
-      <c r="CH2" s="23"/>
-      <c r="CI2" s="23"/>
-      <c r="CJ2" s="23"/>
-      <c r="CK2" s="23"/>
-      <c r="CL2" s="23"/>
-      <c r="CM2" s="23"/>
-      <c r="CN2" s="23"/>
-      <c r="CO2" s="23"/>
-      <c r="CP2" s="23"/>
-      <c r="CQ2" s="23"/>
-      <c r="CR2" s="23"/>
-      <c r="CS2" s="23"/>
-      <c r="CT2" s="23"/>
-      <c r="CU2" s="23"/>
-      <c r="CV2" s="23"/>
-      <c r="CW2" s="23"/>
-      <c r="CX2" s="23"/>
-      <c r="CY2" s="23"/>
-      <c r="CZ2" s="23"/>
-      <c r="DA2" s="23"/>
-      <c r="DB2" s="23"/>
-      <c r="DC2" s="23"/>
-      <c r="DD2" s="23"/>
-      <c r="DE2" s="23"/>
-      <c r="DF2" s="23"/>
-      <c r="DG2" s="23"/>
-      <c r="DH2" s="23"/>
-      <c r="DI2" s="23"/>
-      <c r="DJ2" s="23"/>
-      <c r="DK2" s="23"/>
-      <c r="DL2" s="23"/>
-      <c r="DM2" s="23"/>
-      <c r="DN2" s="23"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="21"/>
+      <c r="T2" s="21"/>
+      <c r="U2" s="21"/>
+      <c r="V2" s="21"/>
+      <c r="W2" s="21"/>
+      <c r="X2" s="21"/>
+      <c r="Y2" s="21"/>
+      <c r="Z2" s="21"/>
+      <c r="AA2" s="21"/>
+      <c r="AB2" s="21"/>
+      <c r="AC2" s="21"/>
+      <c r="AD2" s="21"/>
+      <c r="AE2" s="21"/>
+      <c r="AF2" s="21"/>
+      <c r="AG2" s="21"/>
+      <c r="AH2" s="21"/>
+      <c r="AI2" s="21"/>
+      <c r="AJ2" s="21"/>
+      <c r="AK2" s="21"/>
+      <c r="AL2" s="21"/>
+      <c r="AM2" s="21"/>
+      <c r="AN2" s="21"/>
+      <c r="AO2" s="21"/>
+      <c r="AP2" s="21"/>
+      <c r="AQ2" s="21"/>
+      <c r="AR2" s="21"/>
+      <c r="AS2" s="21"/>
+      <c r="AT2" s="21"/>
+      <c r="AU2" s="21"/>
+      <c r="AV2" s="21"/>
+      <c r="AW2" s="21"/>
+      <c r="AX2" s="21"/>
+      <c r="AY2" s="21"/>
+      <c r="AZ2" s="21"/>
+      <c r="BA2" s="21"/>
+      <c r="BB2" s="21"/>
+      <c r="BC2" s="21"/>
+      <c r="BD2" s="21"/>
+      <c r="BE2" s="21"/>
+      <c r="BF2" s="21"/>
+      <c r="BG2" s="21"/>
+      <c r="BH2" s="21"/>
+      <c r="BI2" s="21"/>
+      <c r="BJ2" s="21"/>
+      <c r="BK2" s="21"/>
+      <c r="BL2" s="21"/>
+      <c r="BM2" s="21"/>
+      <c r="BN2" s="21"/>
+      <c r="BO2" s="21"/>
+      <c r="BP2" s="21"/>
+      <c r="BQ2" s="21"/>
+      <c r="BR2" s="21"/>
+      <c r="BS2" s="21"/>
+      <c r="BT2" s="21"/>
+      <c r="BU2" s="21"/>
+      <c r="BV2" s="21"/>
+      <c r="BW2" s="21"/>
+      <c r="BX2" s="21"/>
+      <c r="BY2" s="21"/>
+      <c r="BZ2" s="21"/>
+      <c r="CA2" s="21"/>
+      <c r="CB2" s="21"/>
+      <c r="CC2" s="21"/>
+      <c r="CD2" s="21"/>
+      <c r="CE2" s="21"/>
+      <c r="CF2" s="21"/>
+      <c r="CG2" s="21"/>
+      <c r="CH2" s="21"/>
+      <c r="CI2" s="21"/>
+      <c r="CJ2" s="21"/>
+      <c r="CK2" s="21"/>
+      <c r="CL2" s="21"/>
+      <c r="CM2" s="21"/>
+      <c r="CN2" s="21"/>
+      <c r="CO2" s="21"/>
+      <c r="CP2" s="21"/>
+      <c r="CQ2" s="21"/>
+      <c r="CR2" s="21"/>
+      <c r="CS2" s="21"/>
+      <c r="CT2" s="21"/>
+      <c r="CU2" s="21"/>
+      <c r="CV2" s="21"/>
+      <c r="CW2" s="21"/>
+      <c r="CX2" s="21"/>
+      <c r="CY2" s="21"/>
+      <c r="CZ2" s="21"/>
+      <c r="DA2" s="21"/>
+      <c r="DB2" s="21"/>
+      <c r="DC2" s="21"/>
+      <c r="DD2" s="21"/>
+      <c r="DE2" s="21"/>
+      <c r="DF2" s="21"/>
+      <c r="DG2" s="21"/>
+      <c r="DH2" s="21"/>
+      <c r="DI2" s="21"/>
+      <c r="DJ2" s="21"/>
+      <c r="DK2" s="21"/>
+      <c r="DL2" s="21"/>
+      <c r="DM2" s="21"/>
+      <c r="DN2" s="21"/>
     </row>
     <row r="3" spans="1:118" x14ac:dyDescent="0.2">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="25" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
@@ -1633,119 +1618,119 @@
       <c r="C3"/>
       <c r="D3"/>
       <c r="E3"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
-      <c r="S3" s="25"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="25"/>
-      <c r="V3" s="25"/>
-      <c r="W3" s="25"/>
-      <c r="X3" s="25"/>
-      <c r="Y3" s="25"/>
-      <c r="Z3" s="25"/>
-      <c r="AA3" s="25"/>
-      <c r="AB3" s="25"/>
-      <c r="AC3" s="25"/>
-      <c r="AD3" s="25"/>
-      <c r="AE3" s="25"/>
-      <c r="AF3" s="25"/>
-      <c r="AG3" s="25"/>
-      <c r="AH3" s="25"/>
-      <c r="AI3" s="25"/>
-      <c r="AJ3" s="25"/>
-      <c r="AK3" s="25"/>
-      <c r="AL3" s="25"/>
-      <c r="AM3" s="25"/>
-      <c r="AN3" s="25"/>
-      <c r="AO3" s="25"/>
-      <c r="AP3" s="25"/>
-      <c r="AQ3" s="25"/>
-      <c r="AR3" s="25"/>
-      <c r="AS3" s="25"/>
-      <c r="AT3" s="25"/>
-      <c r="AU3" s="25"/>
-      <c r="AV3" s="25"/>
-      <c r="AW3" s="25"/>
-      <c r="AX3" s="25"/>
-      <c r="AY3" s="25"/>
-      <c r="AZ3" s="25"/>
-      <c r="BA3" s="25"/>
-      <c r="BB3" s="25"/>
-      <c r="BC3" s="25"/>
-      <c r="BD3" s="25"/>
-      <c r="BE3" s="25"/>
-      <c r="BF3" s="25"/>
-      <c r="BG3" s="25"/>
-      <c r="BH3" s="25"/>
-      <c r="BI3" s="25"/>
-      <c r="BJ3" s="25"/>
-      <c r="BK3" s="25"/>
-      <c r="BL3" s="25"/>
-      <c r="BM3" s="25"/>
-      <c r="BN3" s="25"/>
-      <c r="BO3" s="25"/>
-      <c r="BP3" s="25"/>
-      <c r="BQ3" s="25"/>
-      <c r="BR3" s="25"/>
-      <c r="BS3" s="25"/>
-      <c r="BT3" s="25"/>
-      <c r="BU3" s="25"/>
-      <c r="BV3" s="25"/>
-      <c r="BW3" s="25"/>
-      <c r="BX3" s="25"/>
-      <c r="BY3" s="25"/>
-      <c r="BZ3" s="25"/>
-      <c r="CA3" s="25"/>
-      <c r="CB3" s="25"/>
-      <c r="CC3" s="25"/>
-      <c r="CD3" s="25"/>
-      <c r="CE3" s="25"/>
-      <c r="CF3" s="25"/>
-      <c r="CG3" s="25"/>
-      <c r="CH3" s="25"/>
-      <c r="CI3" s="25"/>
-      <c r="CJ3" s="25"/>
-      <c r="CK3" s="25"/>
-      <c r="CL3" s="25"/>
-      <c r="CM3" s="25"/>
-      <c r="CN3" s="25"/>
-      <c r="CO3" s="25"/>
-      <c r="CP3" s="25"/>
-      <c r="CQ3" s="25"/>
-      <c r="CR3" s="25"/>
-      <c r="CS3" s="25"/>
-      <c r="CT3" s="25"/>
-      <c r="CU3" s="25"/>
-      <c r="CV3" s="25"/>
-      <c r="CW3" s="25"/>
-      <c r="CX3" s="25"/>
-      <c r="CY3" s="25"/>
-      <c r="CZ3" s="25"/>
-      <c r="DA3" s="25"/>
-      <c r="DB3" s="25"/>
-      <c r="DC3" s="25"/>
-      <c r="DD3" s="25"/>
-      <c r="DE3" s="25"/>
-      <c r="DF3" s="25"/>
-      <c r="DG3" s="25"/>
-      <c r="DH3" s="25"/>
-      <c r="DI3" s="25"/>
-      <c r="DJ3" s="25"/>
-      <c r="DK3" s="25"/>
-      <c r="DL3" s="25"/>
-      <c r="DM3" s="25"/>
-      <c r="DN3" s="25"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="23"/>
+      <c r="U3" s="23"/>
+      <c r="V3" s="23"/>
+      <c r="W3" s="23"/>
+      <c r="X3" s="23"/>
+      <c r="Y3" s="23"/>
+      <c r="Z3" s="23"/>
+      <c r="AA3" s="23"/>
+      <c r="AB3" s="23"/>
+      <c r="AC3" s="23"/>
+      <c r="AD3" s="23"/>
+      <c r="AE3" s="23"/>
+      <c r="AF3" s="23"/>
+      <c r="AG3" s="23"/>
+      <c r="AH3" s="23"/>
+      <c r="AI3" s="23"/>
+      <c r="AJ3" s="23"/>
+      <c r="AK3" s="23"/>
+      <c r="AL3" s="23"/>
+      <c r="AM3" s="23"/>
+      <c r="AN3" s="23"/>
+      <c r="AO3" s="23"/>
+      <c r="AP3" s="23"/>
+      <c r="AQ3" s="23"/>
+      <c r="AR3" s="23"/>
+      <c r="AS3" s="23"/>
+      <c r="AT3" s="23"/>
+      <c r="AU3" s="23"/>
+      <c r="AV3" s="23"/>
+      <c r="AW3" s="23"/>
+      <c r="AX3" s="23"/>
+      <c r="AY3" s="23"/>
+      <c r="AZ3" s="23"/>
+      <c r="BA3" s="23"/>
+      <c r="BB3" s="23"/>
+      <c r="BC3" s="23"/>
+      <c r="BD3" s="23"/>
+      <c r="BE3" s="23"/>
+      <c r="BF3" s="23"/>
+      <c r="BG3" s="23"/>
+      <c r="BH3" s="23"/>
+      <c r="BI3" s="23"/>
+      <c r="BJ3" s="23"/>
+      <c r="BK3" s="23"/>
+      <c r="BL3" s="23"/>
+      <c r="BM3" s="23"/>
+      <c r="BN3" s="23"/>
+      <c r="BO3" s="23"/>
+      <c r="BP3" s="23"/>
+      <c r="BQ3" s="23"/>
+      <c r="BR3" s="23"/>
+      <c r="BS3" s="23"/>
+      <c r="BT3" s="23"/>
+      <c r="BU3" s="23"/>
+      <c r="BV3" s="23"/>
+      <c r="BW3" s="23"/>
+      <c r="BX3" s="23"/>
+      <c r="BY3" s="23"/>
+      <c r="BZ3" s="23"/>
+      <c r="CA3" s="23"/>
+      <c r="CB3" s="23"/>
+      <c r="CC3" s="23"/>
+      <c r="CD3" s="23"/>
+      <c r="CE3" s="23"/>
+      <c r="CF3" s="23"/>
+      <c r="CG3" s="23"/>
+      <c r="CH3" s="23"/>
+      <c r="CI3" s="23"/>
+      <c r="CJ3" s="23"/>
+      <c r="CK3" s="23"/>
+      <c r="CL3" s="23"/>
+      <c r="CM3" s="23"/>
+      <c r="CN3" s="23"/>
+      <c r="CO3" s="23"/>
+      <c r="CP3" s="23"/>
+      <c r="CQ3" s="23"/>
+      <c r="CR3" s="23"/>
+      <c r="CS3" s="23"/>
+      <c r="CT3" s="23"/>
+      <c r="CU3" s="23"/>
+      <c r="CV3" s="23"/>
+      <c r="CW3" s="23"/>
+      <c r="CX3" s="23"/>
+      <c r="CY3" s="23"/>
+      <c r="CZ3" s="23"/>
+      <c r="DA3" s="23"/>
+      <c r="DB3" s="23"/>
+      <c r="DC3" s="23"/>
+      <c r="DD3" s="23"/>
+      <c r="DE3" s="23"/>
+      <c r="DF3" s="23"/>
+      <c r="DG3" s="23"/>
+      <c r="DH3" s="23"/>
+      <c r="DI3" s="23"/>
+      <c r="DJ3" s="23"/>
+      <c r="DK3" s="23"/>
+      <c r="DL3" s="23"/>
+      <c r="DM3" s="23"/>
+      <c r="DN3" s="23"/>
     </row>
     <row r="4" spans="1:118" x14ac:dyDescent="0.2">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="25" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -1756,7 +1741,7 @@
       <c r="E4"/>
     </row>
     <row r="5" spans="1:118" x14ac:dyDescent="0.2">
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="29" t="s">
         <v>15</v>
       </c>
       <c r="C5"/>
@@ -1815,7 +1800,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="22" t="s">
         <v>16</v>
       </c>
       <c r="B2" t="s">
@@ -1823,7 +1808,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="25" t="s">
         <v>21</v>
       </c>
       <c r="B3" t="s">
@@ -1831,7 +1816,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="25" t="s">
         <v>21</v>
       </c>
       <c r="B4" t="s">
@@ -1839,7 +1824,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="29" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1855,7 +1840,7 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1863,18 +1848,19 @@
     <col min="1" max="1" width="21.33203125" customWidth="1"/>
     <col min="2" max="2" width="21.33203125" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="38.33203125" customWidth="1"/>
-    <col min="4" max="4" width="34.6640625" customWidth="1"/>
+    <col min="4" max="4" width="42.83203125" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
     <col min="6" max="6" width="17.6640625" customWidth="1"/>
     <col min="7" max="8" width="16.83203125" customWidth="1"/>
     <col min="9" max="9" width="18.33203125" customWidth="1"/>
     <col min="10" max="10" width="20.5" customWidth="1"/>
     <col min="11" max="11" width="16.6640625" customWidth="1"/>
-    <col min="15" max="15" width="18.1640625" customWidth="1"/>
+    <col min="12" max="13" width="16.83203125" customWidth="1"/>
+    <col min="15" max="15" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>34</v>
       </c>
       <c r="B1" s="15" t="s">
@@ -1885,7 +1871,7 @@
       </c>
     </row>
     <row r="2" spans="1:16" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="24" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="16" t="e">
@@ -1898,28 +1884,28 @@
     </row>
     <row r="3" spans="1:16" ht="40" x14ac:dyDescent="0.2">
       <c r="C3" s="9"/>
-      <c r="E3" s="39" t="s">
+      <c r="E3" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="39" t="s">
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="42" t="s">
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="30" t="s">
         <v>58</v>
       </c>
       <c r="P3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="80" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="10"/>
       <c r="C4" s="10"/>
       <c r="D4" s="11"/>
@@ -1932,10 +1918,10 @@
       <c r="G4" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="43" t="s">
+      <c r="H4" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="I4" s="44" t="s">
+      <c r="I4" s="32" t="s">
         <v>60</v>
       </c>
       <c r="J4" s="13" t="s">
@@ -1947,40 +1933,40 @@
       <c r="L4" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="M4" s="43" t="s">
+      <c r="M4" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="N4" s="44" t="s">
+      <c r="N4" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="O4" s="45" t="s">
+      <c r="O4" s="33" t="s">
         <v>59</v>
       </c>
       <c r="P4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14"/>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="21" t="e">
+      <c r="E5" s="19" t="e">
         <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"M-TIT",'ETPT Format DDG'!$C:$C,$A$2)</f>
         <v>#N/A</v>
       </c>
-      <c r="F5" s="19" t="e">
+      <c r="F5" s="17" t="e">
         <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"M-PLAC-ADD",'ETPT Format DDG'!$C:$C,$A$2)</f>
         <v>#N/A</v>
       </c>
-      <c r="G5" s="19" t="e">
+      <c r="G5" s="17" t="e">
         <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"M-PLAC-SUB",'ETPT Format DDG'!$C:$C,$A$2)</f>
         <v>#N/A</v>
       </c>
-      <c r="H5" s="19" t="e">
+      <c r="H5" s="17" t="e">
         <f>SUMIFS(
 INDEX('ETPT Format DDG'!$A:$DU,
 ,
@@ -1990,7 +1976,7 @@
 'ETPT Format DDG'!$G:$G,"Magistrat")</f>
         <v>#N/A</v>
       </c>
-      <c r="I5" s="46" t="e">
+      <c r="I5" s="34" t="e">
         <f>SUMIFS(
 INDEX('ETPT Format DDG'!$A:$DU,
 ,
@@ -2000,23 +1986,23 @@
 'ETPT Format DDG'!$G:$G,"Magistrat")</f>
         <v>#N/A</v>
       </c>
-      <c r="J5" s="19" t="e">
+      <c r="J5" s="17" t="e">
         <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"F-TIT",'ETPT Format DDG'!$C:$C,$A$2)</f>
         <v>#N/A</v>
       </c>
-      <c r="K5" s="19" t="e">
+      <c r="K5" s="17" t="e">
         <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"F-PLAC-ADD",'ETPT Format DDG'!$C:$C,$A$2)</f>
         <v>#N/A</v>
       </c>
-      <c r="L5" s="19" t="e">
+      <c r="L5" s="17" t="e">
         <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"F-PLAC-SUB",'ETPT Format DDG'!$C:$C,$A$2)</f>
         <v>#N/A</v>
       </c>
-      <c r="M5" s="20" t="e">
+      <c r="M5" s="18" t="e">
         <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"C",'ETPT Format DDG'!$C:$C,$A$2,'ETPT Format DDG'!$G:$G,"Greffe")</f>
         <v>#N/A</v>
       </c>
-      <c r="N5" s="46" t="e">
+      <c r="N5" s="34" t="e">
         <f>SUMIFS(
 INDEX('ETPT Format DDG'!$A:$DU,
 ,
@@ -2026,7 +2012,7 @@
 'ETPT Format DDG'!$G:$G,"Greffe")</f>
         <v>#N/A</v>
       </c>
-      <c r="O5" s="20" t="e">
+      <c r="O5" s="18" t="e">
         <f>SUMIFS(
 INDEX('ETPT Format DDG'!$A:$DU,
 ,
@@ -2051,7 +2037,7 @@
     <mergeCell ref="J3:N3"/>
   </mergeCells>
   <conditionalFormatting sqref="C5:O150">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>AND(ISBLANK($C5)=FALSE,ISBLANK($D5)=TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2097,276 +2083,266 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.1640625" style="23" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" style="23" customWidth="1"/>
-    <col min="3" max="9" width="10.83203125" style="23"/>
-    <col min="10" max="10" width="71.1640625" style="23" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="23"/>
+    <col min="1" max="1" width="8.1640625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" style="21" customWidth="1"/>
+    <col min="3" max="9" width="10.83203125" style="21"/>
+    <col min="10" max="10" width="71.1640625" style="21" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="28" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:10" s="26" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
     </row>
     <row r="2" spans="1:10" s="10" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
     </row>
     <row r="3" spans="1:10" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="29"/>
-      <c r="B3" s="30" t="s">
+      <c r="A3" s="27"/>
+      <c r="B3" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="29"/>
-      <c r="B4" s="30" t="s">
+      <c r="A4" s="27"/>
+      <c r="B4" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
     </row>
     <row r="5" spans="1:10" s="10" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="29"/>
-      <c r="B5" s="30" t="s">
+      <c r="A5" s="27"/>
+      <c r="B5" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
     </row>
     <row r="6" spans="1:10" s="10" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
     </row>
     <row r="7" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="29"/>
-      <c r="B7" s="35" t="s">
+      <c r="A7" s="27"/>
+      <c r="B7" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
     </row>
     <row r="8" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="38"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="44"/>
     </row>
     <row r="9" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="38"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
+      <c r="J9" s="44"/>
     </row>
     <row r="10" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="44"/>
     </row>
     <row r="11" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="38"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
     </row>
     <row r="12" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
     </row>
     <row r="13" spans="1:10" s="10" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
     </row>
     <row r="14" spans="1:10" s="10" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="32"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
     </row>
     <row r="15" spans="1:10" s="10" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
     </row>
     <row r="16" spans="1:10" s="10" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-    </row>
-    <row r="18" spans="1:10" s="28" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="36" t="s">
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+    </row>
+    <row r="18" spans="1:10" s="26" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="37"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C13:J13"/>
-    <mergeCell ref="C14:J14"/>
-    <mergeCell ref="B12:J12"/>
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="A18:J18"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
     <mergeCell ref="B6:J6"/>
     <mergeCell ref="C15:J15"/>
     <mergeCell ref="B16:J16"/>
@@ -2374,6 +2350,16 @@
     <mergeCell ref="B9:J9"/>
     <mergeCell ref="B10:J10"/>
     <mergeCell ref="B11:J11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C13:J13"/>
+    <mergeCell ref="C14:J14"/>
+    <mergeCell ref="B12:J12"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="A18:J18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update extractor Mme DE JONG
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B14F26-027E-9F4C-A957-F1AF0E6DE8ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA203BC9-F64E-6A46-951B-47BBC64CF6DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="22480" windowHeight="17620" activeTab="5" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17760" activeTab="5" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
   <sheets>
     <sheet name="ETPT A-JUST" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,8 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ETPT A-JUST'!$A$2:$DN$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ETPT Format DDG'!$A$2:$DT$2</definedName>
+    <definedName name="J">#REF!</definedName>
+    <definedName name="JA">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="63">
   <si>
     <t>#! END_ROW</t>
   </si>
@@ -152,12 +154,6 @@
     <t>Selectionner une juridiction</t>
   </si>
   <si>
-    <t xml:space="preserve">         Extracteur de données d'effectifs - Format DDG (avec réintégration de l'absentéisme)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">         Extracteur de données d'effectifs</t>
-  </si>
-  <si>
     <t xml:space="preserve">        EXPLICATIONS ET CONTROLES A EFFECTUER</t>
   </si>
   <si>
@@ -301,6 +297,211 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Précisions nécessaires aux DDG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (dans l'onglet "ETPT Format DDG"):</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">La colonne "JURIDICTION" permet de préciser le </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tribunal d'affectation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (TJ / TPRX) -&gt; les données ont été prérenseignées à partir des éléments présents dans A-JUST. LEs magistrats sont, par défaut, affectés au TJ. Il convient de </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>contrôler ces renseignements et de réaffecter, au besoin, les agents dans l'un des TPRX proposés dans le menu déroulant.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Les éventuels </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CET</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ont été répartis entre les CET de</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> moins d'un mois</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (colonne DS), qui sont considérés, lors des DDG, comme de l'absentéisme et ceux de</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> plus d'un mois</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (colonne DR) qui déduisent de l'ETPT (action 99).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dans l'onglet </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Agrégats DDG"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, il convient de </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">sélectionner le tribunal voulu dans le menu déroulant </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(case en bleu) pour que s'affiche une synthèse montrant, pour le tribunal sélectionné (TJ ou TPRX), les ETPT affectés à chaque activité ou contentieux, ainsi que les indisponibilités déduisant de l'ETPT (action 99) et celles qui ont été réintégrées (absentéisme).</t>
+    </r>
+  </si>
+  <si>
+    <t>Pour toute question, n'hésitez pas à contacter l'équipe A-JUST : support-utilisateurs@a-just.fr</t>
+  </si>
+  <si>
+    <t>SIEGE</t>
+  </si>
+  <si>
+    <t>GREFFE</t>
+  </si>
+  <si>
+    <t>EQUIPE AUTOUR DU MAGISTRAT</t>
+  </si>
+  <si>
+    <t>Contractuels et vacataires</t>
+  </si>
+  <si>
+    <t>TOTAL SIEGE</t>
+  </si>
+  <si>
+    <t>TOTAL GREFFE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                Extracteur de données d'effectifs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                Extracteur de données d'effectifs - Format DDG (avec réintégration de l'absentéisme)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                Agrégats DDG</t>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">Un </t>
     </r>
     <r>
@@ -324,114 +525,64 @@
       </rPr>
       <t>appelle une vérification. Soit l'agent était effectivement absent pendant toute la période (en CLM par ex.), soit il n'a pas été ventilé.</t>
     </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Il est nécessaire de ventiler durant les temps d'indisponibilité.</t>
+    </r>
   </si>
   <si>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Précisions nécessaires aux DDG</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (dans l'onglet "ETPT Format DDG"):</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">La colonne "JURIDICTION" permet de préciser le </t>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>La colonne "Fonction"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> est remplie automatiquement mais </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>tribunal d'affectation</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (TJ / TPRX) -&gt; les données ont été prérenseignées à partir des éléments présents dans A-JUST. LEs magistrats sont, par défaut, affectés au TJ. Il convient de </t>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>doit être contrôlée et, au besoin, corrigée pour les agents placés</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> car elle permet de distinguer</t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>contrôler ces renseignements et de réaffecter, au besoin, les agents dans l'un des TPRX proposés dans le menu déroulant.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>La colonne "Code fonction"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> est remplie automatiquement mais </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>doit être contrôlée et, au besoin, corrigée pour les agents placés</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> car elle permet de distinguer</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -447,144 +598,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>. Par défaut, tous les placés ont été codés en "M-PLAC-ADD" (Magistrat placé additionnel) ou "F-PLAC-ADD" (Fonctionnaire placé additionnel). Si des Placés étaient des effectifs de substitution, les recoder "M-PLAC-SUB" pour les magistrats ou "F-PLAC-SUB" pour les fonctionnaires, à l'aide du menu déroulant.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Les éventuels </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CET</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ont été répartis entre les CET de</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> moins d'un mois</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (colonne DS), qui sont considérés, lors des DDG, comme de l'absentéisme et ceux de</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> plus d'un mois</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (colonne DR) qui déduisent de l'ETPT (action 99).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Dans l'onglet </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Agrégats DDG"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, il convient de </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">sélectionner le tribunal voulu dans le menu déroulant </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(case en bleu) pour que s'affiche une synthèse montrant, pour le tribunal sélectionné (TJ ou TPRX), les ETPT affectés à chaque activité ou contentieux, ainsi que les indisponibilités déduisant de l'ETPT (action 99) et celles qui ont été réintégrées (absentéisme).</t>
-    </r>
-  </si>
-  <si>
-    <t>Pour toute question, n'hésitez pas à contacter l'équipe A-JUST : support-utilisateurs@a-just.fr</t>
-  </si>
-  <si>
-    <t>SIEGE</t>
-  </si>
-  <si>
-    <t>GREFFE</t>
-  </si>
-  <si>
-    <t>EQUIPE AUTOUR DU MAGISTRAT</t>
-  </si>
-  <si>
-    <t>Contractuels et vacataires</t>
-  </si>
-  <si>
-    <t>TOTAL SIEGE</t>
-  </si>
-  <si>
-    <t>TOTAL GREFFE</t>
+      <t>. Par défaut, tous les placés sont "* PLACÉ ADDITIONNEL". Si des Placés étaient des effectifs de substitution, il faut les renseigner en "* PLACÉ SUBSTITUTION", à l'aide du menu déroulant.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -598,7 +613,7 @@
     <numFmt numFmtId="167" formatCode="General;General;\-"/>
     <numFmt numFmtId="168" formatCode="0.###;0.###;\-"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -683,6 +698,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -883,7 +913,7 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1001,23 +1031,35 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1060,15 +1102,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>46180</xdr:colOff>
+      <xdr:colOff>103906</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>23090</xdr:rowOff>
+      <xdr:rowOff>57725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>542634</xdr:colOff>
+      <xdr:colOff>923635</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>476535</xdr:rowOff>
+      <xdr:rowOff>806439</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1091,8 +1133,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="46180" y="23090"/>
-          <a:ext cx="496454" cy="453445"/>
+          <a:off x="103906" y="57725"/>
+          <a:ext cx="819729" cy="748714"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1109,22 +1151,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>46180</xdr:colOff>
+      <xdr:colOff>103905</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>23090</xdr:rowOff>
+      <xdr:rowOff>57725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>542634</xdr:colOff>
+      <xdr:colOff>923634</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>476535</xdr:rowOff>
+      <xdr:rowOff>806439</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CD8D5B3-C3E9-E94E-BD8C-2EF269EA8931}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D7A5D8C-BE33-ED45-A77A-8F455267161F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1140,8 +1182,106 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="46180" y="23090"/>
-          <a:ext cx="496454" cy="453445"/>
+          <a:off x="103905" y="57725"/>
+          <a:ext cx="819729" cy="748714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>98777</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>84665</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1114778</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1012648</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD1D57F9-87BD-BD45-83E9-42F2487B9728}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="98777" y="84665"/>
+          <a:ext cx="1016001" cy="927983"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>103910</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>69271</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>300184</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>817985</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DC1CFF2-AC52-DD4F-9E83-87135FE34159}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="103910" y="69271"/>
+          <a:ext cx="819729" cy="748714"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1453,12 +1593,12 @@
   <dimension ref="A1:DN8"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A177" sqref="A177"/>
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
     <col min="2" max="2" width="22.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="7.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="2" customWidth="1"/>
@@ -1468,9 +1608,9 @@
     <col min="8" max="8" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:118" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:118" s="4" customFormat="1" ht="67" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1774,7 +1914,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A139" sqref="A139"/>
+      <selection activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1783,9 +1923,9 @@
     <col min="2" max="2" width="71.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="67" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1837,10 +1977,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E893F90-1EC7-764C-B747-7920FCEC73CB}">
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1859,189 +1999,215 @@
     <col min="15" max="15" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:16" s="4" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+    </row>
+    <row r="2" spans="1:16" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B2" s="15" t="s">
         <v>29</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="16" t="e">
-        <f>VLOOKUP(A2,'codage tribunal'!A:B,2,FALSE)</f>
-        <v>#N/A</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="40" x14ac:dyDescent="0.2">
-      <c r="C3" s="9"/>
-      <c r="E3" s="37" t="s">
+    <row r="3" spans="1:16" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="16" t="e">
+        <f>VLOOKUP(A3,'codage tribunal'!A:B,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="40" x14ac:dyDescent="0.2">
+      <c r="C4" s="9"/>
+      <c r="E4" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="K4" s="38"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="38"/>
+      <c r="N4" s="39"/>
+      <c r="O4" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="P4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="48" x14ac:dyDescent="0.2">
+      <c r="A5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="I5" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="37" t="s">
+      <c r="J5" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="N5" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="P3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="48" x14ac:dyDescent="0.2">
-      <c r="A4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="I4" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="J4" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="L4" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="M4" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="N4" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="O4" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="P4" t="s">
+      <c r="O5" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="P5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
-      <c r="C5" s="35" t="s">
+    <row r="6" spans="1:16" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="14"/>
+      <c r="C6" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D6" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="19" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"M-TIT",'ETPT Format DDG'!$C:$C,$A$2)</f>
+      <c r="E6" s="19" t="e">
+        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(D6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"M-TIT",'ETPT Format DDG'!$C:$C,$A$3)</f>
         <v>#N/A</v>
       </c>
-      <c r="F5" s="17" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"M-PLAC-ADD",'ETPT Format DDG'!$C:$C,$A$2)</f>
+      <c r="F6" s="17" t="e">
+        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(D6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"M-PLAC-ADD",'ETPT Format DDG'!$C:$C,$A$3,'ETPT Format DDG'!$H:$H,"*ADDITIONNEL*")</f>
         <v>#N/A</v>
       </c>
-      <c r="G5" s="17" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"M-PLAC-SUB",'ETPT Format DDG'!$C:$C,$A$2)</f>
+      <c r="G6" s="17" t="e">
+        <f>SUMIFS(
+INDEX('ETPT Format DDG'!$A:$DU,
+,IFERROR(MATCH(D6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"M-PLAC-ADD",'ETPT Format DDG'!$C:$C,$A$3,'ETPT Format DDG'!$H:$H,"*SUBSTITUTION*")</f>
         <v>#N/A</v>
       </c>
-      <c r="H5" s="17" t="e">
+      <c r="H6" s="17" t="e">
         <f>SUMIFS(
 INDEX('ETPT Format DDG'!$A:$DU,
 ,
-IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))
+IFERROR(MATCH(D6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))
 ),'ETPT Format DDG'!$I:$I,"C",
-'ETPT Format DDG'!$C:$C,$A$2,
+'ETPT Format DDG'!$C:$C,$A$3,
 'ETPT Format DDG'!$G:$G,"Magistrat")</f>
         <v>#N/A</v>
       </c>
-      <c r="I5" s="34" t="e">
+      <c r="I6" s="34" t="e">
         <f>SUMIFS(
 INDEX('ETPT Format DDG'!$A:$DU,
 ,
-IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))
+IFERROR(MATCH(D6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))
 ),
-'ETPT Format DDG'!$C:$C,$A$2,
+'ETPT Format DDG'!$C:$C,$A$3,
 'ETPT Format DDG'!$G:$G,"Magistrat")</f>
         <v>#N/A</v>
       </c>
-      <c r="J5" s="17" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"F-TIT",'ETPT Format DDG'!$C:$C,$A$2)</f>
+      <c r="J6" s="17" t="e">
+        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(D6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"F-TIT",'ETPT Format DDG'!$C:$C,$A$3)</f>
         <v>#N/A</v>
       </c>
-      <c r="K5" s="17" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"F-PLAC-ADD",'ETPT Format DDG'!$C:$C,$A$2)</f>
+      <c r="K6" s="17" t="e">
+        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(D6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"F-PLAC-ADD",'ETPT Format DDG'!$C:$C,$A$3,'ETPT Format DDG'!$H:$H,"*ADDITIONNEL*")</f>
         <v>#N/A</v>
       </c>
-      <c r="L5" s="17" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"F-PLAC-SUB",'ETPT Format DDG'!$C:$C,$A$2)</f>
+      <c r="L6" s="17" t="e">
+        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(D6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"F-PLAC-ADD",'ETPT Format DDG'!$C:$C,$A$3,'ETPT Format DDG'!$H:$H,"*SUBSTITUTION*")</f>
         <v>#N/A</v>
       </c>
-      <c r="M5" s="18" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"C",'ETPT Format DDG'!$C:$C,$A$2,'ETPT Format DDG'!$G:$G,"Greffe")</f>
+      <c r="M6" s="18" t="e">
+        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(D6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"C",'ETPT Format DDG'!$C:$C,$A$3,'ETPT Format DDG'!$G:$G,"Greffe")</f>
         <v>#N/A</v>
       </c>
-      <c r="N5" s="34" t="e">
+      <c r="N6" s="34" t="e">
         <f>SUMIFS(
 INDEX('ETPT Format DDG'!$A:$DU,
 ,
-IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))
+IFERROR(MATCH(D6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))
 ),
-'ETPT Format DDG'!$C:$C,$A$2,
+'ETPT Format DDG'!$C:$C,$A$3,
 'ETPT Format DDG'!$G:$G,"Greffe")</f>
         <v>#N/A</v>
       </c>
-      <c r="O5" s="18" t="e">
+      <c r="O6" s="18" t="e">
         <f>SUMIFS(
 INDEX('ETPT Format DDG'!$A:$DU,
 ,
-IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))
+IFERROR(MATCH(D6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))
 ),'ETPT Format DDG'!$I:$I,"C",
-'ETPT Format DDG'!$C:$C,$A$2,
+'ETPT Format DDG'!$C:$C,$A$3,
 'ETPT Format DDG'!$G:$G,"Autour du magistrat")</f>
         <v>#N/A</v>
       </c>
-      <c r="P5" t="s">
+      <c r="P6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="P6" t="s">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P7" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="E3:I3"/>
-    <mergeCell ref="J3:N3"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="J4:N4"/>
   </mergeCells>
-  <conditionalFormatting sqref="C5:O150">
+  <conditionalFormatting sqref="C6:O151">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>AND(ISBLANK($C5)=FALSE,ISBLANK($D5)=TRUE)</formula>
+      <formula>AND(ISBLANK($C6)=FALSE,ISBLANK($D6)=TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2077,8 +2243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C706A55-5422-5B42-B9B4-A00444FB459D}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2090,43 +2256,43 @@
     <col min="11" max="16384" width="10.83203125" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="26" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
+    <row r="1" spans="1:10" s="26" customFormat="1" ht="67" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
     </row>
     <row r="2" spans="1:10" s="10" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="44" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
+      <c r="B2" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="27"/>
       <c r="B3" s="28" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C3" s="40" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D3" s="40"/>
       <c r="E3" s="40"/>
@@ -2139,10 +2305,10 @@
     <row r="4" spans="1:10" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="27"/>
       <c r="B4" s="28" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C4" s="40" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D4" s="40"/>
       <c r="E4" s="40"/>
@@ -2155,10 +2321,10 @@
     <row r="5" spans="1:10" s="10" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="27"/>
       <c r="B5" s="28" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C5" s="40" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D5" s="40"/>
       <c r="E5" s="40"/>
@@ -2173,7 +2339,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C6" s="40"/>
       <c r="D6" s="40"/>
@@ -2186,92 +2352,92 @@
     </row>
     <row r="7" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="27"/>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
+    </row>
+    <row r="8" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="48"/>
+    </row>
+    <row r="9" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="48"/>
+    </row>
+    <row r="10" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="44"/>
-      <c r="J7" s="44"/>
-    </row>
-    <row r="8" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="41" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-    </row>
-    <row r="9" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="41"/>
-    </row>
-    <row r="10" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="41" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="41"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="48"/>
     </row>
     <row r="11" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="41"/>
+      <c r="B11" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="48"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="48"/>
     </row>
     <row r="12" spans="1:10" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="45" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="46"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="46"/>
-      <c r="J12" s="46"/>
+      <c r="B12" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42"/>
     </row>
     <row r="13" spans="1:10" s="10" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="40" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D13" s="40"/>
       <c r="E13" s="40"/>
@@ -2285,8 +2451,8 @@
       <c r="B14" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="40" t="s">
-        <v>52</v>
+      <c r="C14" s="50" t="s">
+        <v>62</v>
       </c>
       <c r="D14" s="40"/>
       <c r="E14" s="40"/>
@@ -2301,7 +2467,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="40" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D15" s="40"/>
       <c r="E15" s="40"/>
@@ -2316,7 +2482,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="40" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C16" s="40"/>
       <c r="D16" s="40"/>
@@ -2328,21 +2494,25 @@
       <c r="J16" s="40"/>
     </row>
     <row r="18" spans="1:10" s="26" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="42" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" s="43"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="43"/>
+      <c r="A18" s="44" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="45"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C13:J13"/>
+    <mergeCell ref="C14:J14"/>
+    <mergeCell ref="B12:J12"/>
+    <mergeCell ref="B7:J7"/>
     <mergeCell ref="A18:J18"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="B2:J2"/>
@@ -2356,12 +2526,9 @@
     <mergeCell ref="B9:J9"/>
     <mergeCell ref="B10:J10"/>
     <mergeCell ref="B11:J11"/>
-    <mergeCell ref="C13:J13"/>
-    <mergeCell ref="C14:J14"/>
-    <mergeCell ref="B12:J12"/>
-    <mergeCell ref="B7:J7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update zoom extractor ddg
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9E73E9-22DA-CD4D-A450-626969BDFFE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA858C80-C3E3-5745-AD6A-7B4D1C9BEFC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="600" windowWidth="22940" windowHeight="13240" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
@@ -13129,7 +13129,9 @@
   </sheetPr>
   <dimension ref="A1:DN8"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -13451,7 +13453,7 @@
   </sheetPr>
   <dimension ref="A1:EF4"/>
   <sheetViews>
-    <sheetView showFormulas="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView showFormulas="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
extractor final display DDG
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F327840D-70B6-7B48-B14F-7A0BA89B1209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F1867FA-6BD2-604C-AC39-EE3945E7A4B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="600" windowWidth="22940" windowHeight="13240" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
@@ -3210,7 +3210,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -3553,19 +3553,6 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color rgb="FF333F4F"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF333F4F"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF333F4F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top style="thick">
         <color rgb="FFFF0000"/>
@@ -3685,6 +3672,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF333F4F"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF333F4F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF333F4F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF333F4F"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF333F4F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -3695,7 +3733,7 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="258">
+  <cellXfs count="260">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -4367,19 +4405,10 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="4" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="4" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="40" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -4393,13 +4422,58 @@
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="25" xfId="6" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="27" xfId="6" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="29" xfId="6" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="40" xfId="6" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="22" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4408,11 +4482,35 @@
     <xf numFmtId="0" fontId="9" fillId="22" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4444,14 +4542,14 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4461,60 +4559,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="25" xfId="6" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="27" xfId="6" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="29" xfId="6" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="41" xfId="6" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -4654,9 +4698,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>13121</xdr:colOff>
+      <xdr:colOff>227016</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>81478</xdr:rowOff>
+      <xdr:rowOff>14635</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="960661" cy="902640"/>
     <xdr:pic>
@@ -4680,7 +4724,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="838621" y="81478"/>
+          <a:off x="320595" y="14635"/>
           <a:ext cx="960661" cy="902640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5290,7 +5334,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5310,11 +5354,11 @@
       <c r="B1" s="197" t="s">
         <v>494</v>
       </c>
-      <c r="C1" s="222" t="s">
+      <c r="C1" s="225" t="s">
         <v>495</v>
       </c>
-      <c r="D1" s="222"/>
-      <c r="E1" s="222"/>
+      <c r="D1" s="225"/>
+      <c r="E1" s="225"/>
       <c r="F1" s="198"/>
       <c r="H1" s="28" t="s">
         <v>0</v>
@@ -5323,11 +5367,11 @@
     <row r="2" spans="1:8" s="202" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="199"/>
       <c r="B2" s="200"/>
-      <c r="C2" s="223" t="s">
+      <c r="C2" s="226" t="s">
         <v>496</v>
       </c>
-      <c r="D2" s="223"/>
-      <c r="E2" s="223"/>
+      <c r="D2" s="226"/>
+      <c r="E2" s="226"/>
       <c r="F2" s="201"/>
       <c r="H2" s="28" t="s">
         <v>0</v>
@@ -5351,156 +5395,163 @@
       <c r="D4" s="207" t="s">
         <v>499</v>
       </c>
-      <c r="E4" s="220" t="s">
+      <c r="E4" s="232" t="s">
         <v>500</v>
       </c>
-      <c r="F4" s="221"/>
+      <c r="F4" s="233"/>
+      <c r="G4" s="221"/>
       <c r="H4" s="28" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="28" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="203"/>
-      <c r="B5" s="240" t="s">
+      <c r="B5" s="214" t="s">
         <v>501</v>
       </c>
-      <c r="C5" s="241" t="s">
+      <c r="C5" s="215" t="s">
         <v>502</v>
       </c>
-      <c r="D5" s="241" t="s">
+      <c r="D5" s="215" t="s">
         <v>503</v>
       </c>
-      <c r="E5" s="242" t="s">
+      <c r="E5" s="234" t="s">
         <v>518</v>
       </c>
-      <c r="F5" s="243"/>
+      <c r="F5" s="235"/>
+      <c r="G5" s="220"/>
       <c r="H5" s="28" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="28" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="203"/>
-      <c r="B6" s="244" t="s">
+      <c r="B6" s="216" t="s">
         <v>504</v>
       </c>
-      <c r="C6" s="245" t="s">
+      <c r="C6" s="217" t="s">
         <v>505</v>
       </c>
-      <c r="D6" s="245" t="s">
+      <c r="D6" s="217" t="s">
         <v>506</v>
       </c>
-      <c r="E6" s="246" t="s">
+      <c r="E6" s="236" t="s">
         <v>519</v>
       </c>
-      <c r="F6" s="247"/>
+      <c r="F6" s="237"/>
+      <c r="G6" s="220"/>
       <c r="H6" s="28" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="28" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="203"/>
-      <c r="B7" s="244" t="s">
+      <c r="B7" s="216" t="s">
         <v>507</v>
       </c>
-      <c r="C7" s="245" t="s">
+      <c r="C7" s="217" t="s">
         <v>508</v>
       </c>
-      <c r="D7" s="245" t="s">
+      <c r="D7" s="217" t="s">
         <v>509</v>
       </c>
-      <c r="E7" s="246" t="s">
+      <c r="E7" s="236" t="s">
         <v>518</v>
       </c>
-      <c r="F7" s="247"/>
+      <c r="F7" s="237"/>
+      <c r="G7" s="220"/>
       <c r="H7" s="28" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="28" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="203"/>
-      <c r="B8" s="248" t="s">
+      <c r="B8" s="218" t="s">
         <v>510</v>
       </c>
-      <c r="C8" s="249" t="s">
+      <c r="C8" s="227" t="s">
         <v>511</v>
       </c>
-      <c r="D8" s="249" t="s">
+      <c r="D8" s="227" t="s">
         <v>512</v>
       </c>
-      <c r="E8" s="250" t="s">
+      <c r="E8" s="238" t="s">
         <v>520</v>
       </c>
-      <c r="F8" s="251"/>
+      <c r="F8" s="239"/>
+      <c r="G8" s="220"/>
       <c r="H8" s="28" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="28" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="203"/>
-      <c r="B9" s="248" t="s">
+      <c r="B9" s="218" t="s">
         <v>513</v>
       </c>
-      <c r="C9" s="249"/>
-      <c r="D9" s="249"/>
-      <c r="E9" s="252"/>
-      <c r="F9" s="253"/>
+      <c r="C9" s="227"/>
+      <c r="D9" s="227"/>
+      <c r="E9" s="240"/>
+      <c r="F9" s="241"/>
+      <c r="G9" s="220"/>
       <c r="H9" s="28" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="28" customFormat="1" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="203"/>
-      <c r="B10" s="254" t="s">
+      <c r="B10" s="219" t="s">
         <v>514</v>
       </c>
-      <c r="C10" s="255"/>
-      <c r="D10" s="255"/>
-      <c r="E10" s="256"/>
-      <c r="F10" s="257"/>
+      <c r="C10" s="228"/>
+      <c r="D10" s="228"/>
+      <c r="E10" s="242"/>
+      <c r="F10" s="243"/>
+      <c r="G10" s="220"/>
       <c r="H10" s="28" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="28" customFormat="1" ht="5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="203"/>
-      <c r="B11" s="209"/>
-      <c r="C11" s="209"/>
-      <c r="D11" s="209"/>
-      <c r="E11" s="209"/>
-      <c r="F11" s="209"/>
+      <c r="B11" s="224"/>
+      <c r="C11" s="224"/>
+      <c r="D11" s="224"/>
+      <c r="E11" s="224"/>
+      <c r="F11" s="224"/>
       <c r="H11" s="28" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="28" customFormat="1" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="203"/>
-      <c r="B12" s="210"/>
-      <c r="C12" s="219" t="s">
+      <c r="B12" s="222"/>
+      <c r="C12" s="231" t="s">
         <v>515</v>
       </c>
-      <c r="D12" s="219"/>
-      <c r="E12" s="219"/>
-      <c r="F12" s="211"/>
+      <c r="D12" s="231"/>
+      <c r="E12" s="231"/>
+      <c r="F12" s="223"/>
       <c r="H12" s="28" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="28" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="212"/>
+      <c r="A13" s="209"/>
       <c r="F13" s="204"/>
       <c r="H13" s="28" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="28" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="217" t="s">
+      <c r="A14" s="229" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="217"/>
-      <c r="C14" s="217"/>
-      <c r="D14" s="217"/>
-      <c r="E14" s="217"/>
-      <c r="F14" s="218"/>
+      <c r="B14" s="229"/>
+      <c r="C14" s="229"/>
+      <c r="D14" s="229"/>
+      <c r="E14" s="229"/>
+      <c r="F14" s="230"/>
       <c r="H14" s="28" t="s">
         <v>0</v>
       </c>
@@ -5561,16 +5612,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A1" s="232" t="s">
+      <c r="A1" s="252" t="s">
         <v>483</v>
       </c>
-      <c r="B1" s="232"/>
-      <c r="C1" s="232"/>
-      <c r="D1" s="232"/>
-      <c r="E1" s="232"/>
-      <c r="F1" s="232"/>
-      <c r="G1" s="232"/>
-      <c r="H1" s="232"/>
+      <c r="B1" s="252"/>
+      <c r="C1" s="252"/>
+      <c r="D1" s="252"/>
+      <c r="E1" s="252"/>
+      <c r="F1" s="252"/>
+      <c r="G1" s="252"/>
+      <c r="H1" s="252"/>
       <c r="I1" s="112"/>
       <c r="J1" s="112"/>
       <c r="K1" s="112"/>
@@ -5609,7 +5660,7 @@
       <c r="G2" s="155" t="s">
         <v>438</v>
       </c>
-      <c r="H2" s="230" t="s">
+      <c r="H2" s="250" t="s">
         <v>437</v>
       </c>
       <c r="I2" s="155" t="s">
@@ -5642,13 +5693,13 @@
       <c r="R2" s="155" t="s">
         <v>436</v>
       </c>
-      <c r="S2" s="230" t="s">
+      <c r="S2" s="250" t="s">
         <v>435</v>
       </c>
       <c r="T2" s="155" t="s">
         <v>152</v>
       </c>
-      <c r="U2" s="230" t="s">
+      <c r="U2" s="250" t="s">
         <v>434</v>
       </c>
       <c r="V2" s="155" t="s">
@@ -5678,7 +5729,7 @@
       <c r="AD2" s="155" t="s">
         <v>433</v>
       </c>
-      <c r="AE2" s="230" t="s">
+      <c r="AE2" s="250" t="s">
         <v>482</v>
       </c>
       <c r="AF2" s="155" t="s">
@@ -5690,7 +5741,7 @@
       <c r="AH2" s="155" t="s">
         <v>481</v>
       </c>
-      <c r="AI2" s="230" t="s">
+      <c r="AI2" s="250" t="s">
         <v>480</v>
       </c>
     </row>
@@ -5704,7 +5755,7 @@
       <c r="G3" s="155" t="s">
         <v>427</v>
       </c>
-      <c r="H3" s="230"/>
+      <c r="H3" s="250"/>
       <c r="I3" s="155" t="s">
         <v>479</v>
       </c>
@@ -5735,11 +5786,11 @@
       <c r="R3" s="155" t="s">
         <v>414</v>
       </c>
-      <c r="S3" s="230"/>
+      <c r="S3" s="250"/>
       <c r="T3" s="155" t="s">
         <v>411</v>
       </c>
-      <c r="U3" s="230"/>
+      <c r="U3" s="250"/>
       <c r="V3" s="155" t="s">
         <v>470</v>
       </c>
@@ -5767,7 +5818,7 @@
       <c r="AD3" s="155" t="s">
         <v>462</v>
       </c>
-      <c r="AE3" s="230"/>
+      <c r="AE3" s="250"/>
       <c r="AF3" s="155" t="s">
         <v>461</v>
       </c>
@@ -5777,7 +5828,7 @@
       <c r="AH3" s="155" t="s">
         <v>391</v>
       </c>
-      <c r="AI3" s="230"/>
+      <c r="AI3" s="250"/>
     </row>
     <row r="4" spans="1:35" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="158"/>
@@ -5799,7 +5850,7 @@
       <c r="G4" s="155" t="s">
         <v>377</v>
       </c>
-      <c r="H4" s="230"/>
+      <c r="H4" s="250"/>
       <c r="I4" s="155" t="s">
         <v>460</v>
       </c>
@@ -5830,11 +5881,11 @@
       <c r="R4" s="155" t="s">
         <v>363</v>
       </c>
-      <c r="S4" s="230"/>
+      <c r="S4" s="250"/>
       <c r="T4" s="155" t="s">
         <v>359</v>
       </c>
-      <c r="U4" s="230"/>
+      <c r="U4" s="250"/>
       <c r="V4" s="155" t="s">
         <v>451</v>
       </c>
@@ -5862,7 +5913,7 @@
       <c r="AD4" s="155" t="s">
         <v>443</v>
       </c>
-      <c r="AE4" s="230"/>
+      <c r="AE4" s="250"/>
       <c r="AF4" s="155" t="s">
         <v>442</v>
       </c>
@@ -5872,7 +5923,7 @@
       <c r="AH4" s="155" t="s">
         <v>338</v>
       </c>
-      <c r="AI4" s="230"/>
+      <c r="AI4" s="250"/>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A5" s="161" t="s">
@@ -6981,13 +7032,13 @@
       <c r="G2" s="155" t="s">
         <v>436</v>
       </c>
-      <c r="H2" s="230" t="s">
+      <c r="H2" s="250" t="s">
         <v>435</v>
       </c>
       <c r="I2" s="155" t="s">
         <v>152</v>
       </c>
-      <c r="J2" s="230" t="s">
+      <c r="J2" s="250" t="s">
         <v>434</v>
       </c>
     </row>
@@ -7001,11 +7052,11 @@
       <c r="G3" s="155" t="s">
         <v>414</v>
       </c>
-      <c r="H3" s="230"/>
+      <c r="H3" s="250"/>
       <c r="I3" s="155" t="s">
         <v>411</v>
       </c>
-      <c r="J3" s="230"/>
+      <c r="J3" s="250"/>
     </row>
     <row r="4" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A4" s="177"/>
@@ -7027,11 +7078,11 @@
       <c r="G4" s="155" t="s">
         <v>363</v>
       </c>
-      <c r="H4" s="230"/>
+      <c r="H4" s="250"/>
       <c r="I4" s="155" t="s">
         <v>359</v>
       </c>
-      <c r="J4" s="230"/>
+      <c r="J4" s="250"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="171" t="s">
@@ -7435,7 +7486,7 @@
       <c r="G2" s="155" t="s">
         <v>438</v>
       </c>
-      <c r="H2" s="230" t="s">
+      <c r="H2" s="250" t="s">
         <v>437</v>
       </c>
       <c r="I2" s="154" t="s">
@@ -7480,7 +7531,7 @@
       <c r="V2" s="154" t="s">
         <v>436</v>
       </c>
-      <c r="W2" s="230" t="s">
+      <c r="W2" s="250" t="s">
         <v>435</v>
       </c>
       <c r="X2" s="155" t="s">
@@ -7495,7 +7546,7 @@
       <c r="AA2" s="155" t="s">
         <v>152</v>
       </c>
-      <c r="AB2" s="230" t="s">
+      <c r="AB2" s="250" t="s">
         <v>434</v>
       </c>
       <c r="AC2" s="152" t="s">
@@ -7525,7 +7576,7 @@
       <c r="AK2" s="152" t="s">
         <v>433</v>
       </c>
-      <c r="AL2" s="230" t="s">
+      <c r="AL2" s="250" t="s">
         <v>432</v>
       </c>
       <c r="AM2" s="152" t="s">
@@ -7567,7 +7618,7 @@
       <c r="AY2" s="152" t="s">
         <v>431</v>
       </c>
-      <c r="AZ2" s="230" t="s">
+      <c r="AZ2" s="250" t="s">
         <v>430</v>
       </c>
       <c r="BA2" s="151" t="s">
@@ -7597,7 +7648,7 @@
       <c r="BI2" s="151" t="s">
         <v>429</v>
       </c>
-      <c r="BJ2" s="230" t="s">
+      <c r="BJ2" s="250" t="s">
         <v>428</v>
       </c>
       <c r="BK2"/>
@@ -7612,7 +7663,7 @@
       <c r="G3" s="155" t="s">
         <v>427</v>
       </c>
-      <c r="H3" s="230"/>
+      <c r="H3" s="250"/>
       <c r="I3" s="154" t="s">
         <v>426</v>
       </c>
@@ -7653,7 +7704,7 @@
       <c r="V3" s="154" t="s">
         <v>414</v>
       </c>
-      <c r="W3" s="230"/>
+      <c r="W3" s="250"/>
       <c r="X3" s="150"/>
       <c r="Y3" s="155" t="s">
         <v>413</v>
@@ -7664,7 +7715,7 @@
       <c r="AA3" s="155" t="s">
         <v>411</v>
       </c>
-      <c r="AB3" s="230"/>
+      <c r="AB3" s="250"/>
       <c r="AC3" s="152" t="s">
         <v>410</v>
       </c>
@@ -7692,7 +7743,7 @@
       <c r="AK3" s="152" t="s">
         <v>404</v>
       </c>
-      <c r="AL3" s="230"/>
+      <c r="AL3" s="250"/>
       <c r="AM3" s="152" t="s">
         <v>403</v>
       </c>
@@ -7732,7 +7783,7 @@
       <c r="AY3" s="152" t="s">
         <v>391</v>
       </c>
-      <c r="AZ3" s="230"/>
+      <c r="AZ3" s="250"/>
       <c r="BA3" s="151" t="s">
         <v>390</v>
       </c>
@@ -7760,7 +7811,7 @@
       <c r="BI3" s="151" t="s">
         <v>382</v>
       </c>
-      <c r="BJ3" s="230"/>
+      <c r="BJ3" s="250"/>
     </row>
     <row r="4" spans="1:63" s="112" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="157"/>
@@ -7782,7 +7833,7 @@
       <c r="G4" s="155" t="s">
         <v>377</v>
       </c>
-      <c r="H4" s="230"/>
+      <c r="H4" s="250"/>
       <c r="I4" s="154" t="s">
         <v>376</v>
       </c>
@@ -7825,7 +7876,7 @@
       <c r="V4" s="154" t="s">
         <v>363</v>
       </c>
-      <c r="W4" s="230"/>
+      <c r="W4" s="250"/>
       <c r="X4" s="153" t="s">
         <v>362</v>
       </c>
@@ -7838,7 +7889,7 @@
       <c r="AA4" s="153" t="s">
         <v>359</v>
       </c>
-      <c r="AB4" s="230"/>
+      <c r="AB4" s="250"/>
       <c r="AC4" s="152" t="s">
         <v>358</v>
       </c>
@@ -7866,7 +7917,7 @@
       <c r="AK4" s="152" t="s">
         <v>351</v>
       </c>
-      <c r="AL4" s="230"/>
+      <c r="AL4" s="250"/>
       <c r="AM4" s="152" t="s">
         <v>350</v>
       </c>
@@ -7906,7 +7957,7 @@
       <c r="AY4" s="152" t="s">
         <v>338</v>
       </c>
-      <c r="AZ4" s="230"/>
+      <c r="AZ4" s="250"/>
       <c r="BA4" s="151" t="s">
         <v>337</v>
       </c>
@@ -7934,7 +7985,7 @@
       <c r="BI4" s="151" t="s">
         <v>329</v>
       </c>
-      <c r="BJ4" s="230"/>
+      <c r="BJ4" s="250"/>
       <c r="BK4"/>
     </row>
     <row r="5" spans="1:63" s="112" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -7943,7 +7994,7 @@
       </c>
       <c r="B5" s="132"/>
       <c r="C5" s="132"/>
-      <c r="D5" s="215"/>
+      <c r="D5" s="212"/>
       <c r="E5" s="132" t="s">
         <v>328</v>
       </c>
@@ -8155,7 +8206,7 @@
       </c>
       <c r="B6" s="132"/>
       <c r="C6" s="132"/>
-      <c r="D6" s="216" t="str">
+      <c r="D6" s="213" t="str">
         <f t="shared" ref="D6:D15" si="6">IF(ISBLANK($D$5),"",$D$5)</f>
         <v/>
       </c>
@@ -8369,7 +8420,7 @@
       </c>
       <c r="B7" s="132"/>
       <c r="C7" s="132"/>
-      <c r="D7" s="216" t="str">
+      <c r="D7" s="213" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -8583,7 +8634,7 @@
       </c>
       <c r="B8" s="132"/>
       <c r="C8" s="132"/>
-      <c r="D8" s="216" t="str">
+      <c r="D8" s="213" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -8797,7 +8848,7 @@
       </c>
       <c r="B9" s="132"/>
       <c r="C9" s="132"/>
-      <c r="D9" s="216" t="str">
+      <c r="D9" s="213" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -9011,7 +9062,7 @@
       </c>
       <c r="B10" s="132"/>
       <c r="C10" s="132"/>
-      <c r="D10" s="216" t="str">
+      <c r="D10" s="213" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -9225,7 +9276,7 @@
       </c>
       <c r="B11" s="132"/>
       <c r="C11" s="132"/>
-      <c r="D11" s="216" t="str">
+      <c r="D11" s="213" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -9439,7 +9490,7 @@
       </c>
       <c r="B12" s="132"/>
       <c r="C12" s="132"/>
-      <c r="D12" s="216" t="str">
+      <c r="D12" s="213" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -9653,7 +9704,7 @@
       </c>
       <c r="B13" s="132"/>
       <c r="C13" s="132"/>
-      <c r="D13" s="216" t="str">
+      <c r="D13" s="213" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -9867,7 +9918,7 @@
       </c>
       <c r="B14" s="132"/>
       <c r="C14" s="132"/>
-      <c r="D14" s="216" t="str">
+      <c r="D14" s="213" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -10081,7 +10132,7 @@
       </c>
       <c r="B15" s="132"/>
       <c r="C15" s="132"/>
-      <c r="D15" s="216" t="str">
+      <c r="D15" s="213" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -10592,17 +10643,17 @@
       <c r="AZ18" s="111"/>
     </row>
     <row r="19" spans="1:62" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E19" s="233" t="s">
+      <c r="E19" s="253" t="s">
         <v>440</v>
       </c>
-      <c r="F19" s="234"/>
-      <c r="G19" s="234"/>
-      <c r="H19" s="234"/>
-      <c r="I19" s="234"/>
-      <c r="J19" s="234"/>
-      <c r="K19" s="234"/>
-      <c r="L19" s="234"/>
-      <c r="M19" s="235"/>
+      <c r="F19" s="254"/>
+      <c r="G19" s="254"/>
+      <c r="H19" s="254"/>
+      <c r="I19" s="254"/>
+      <c r="J19" s="254"/>
+      <c r="K19" s="254"/>
+      <c r="L19" s="254"/>
+      <c r="M19" s="255"/>
     </row>
     <row r="20" spans="1:62" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="22" spans="1:62" x14ac:dyDescent="0.2">
@@ -10723,7 +10774,7 @@
       <c r="G2" s="155" t="s">
         <v>438</v>
       </c>
-      <c r="H2" s="230" t="s">
+      <c r="H2" s="250" t="s">
         <v>437</v>
       </c>
       <c r="I2" s="155" t="s">
@@ -10756,13 +10807,13 @@
       <c r="R2" s="155" t="s">
         <v>436</v>
       </c>
-      <c r="S2" s="230" t="s">
+      <c r="S2" s="250" t="s">
         <v>435</v>
       </c>
       <c r="T2" s="155" t="s">
         <v>152</v>
       </c>
-      <c r="U2" s="230" t="s">
+      <c r="U2" s="250" t="s">
         <v>434</v>
       </c>
       <c r="V2" s="155" t="s">
@@ -10792,7 +10843,7 @@
       <c r="AD2" s="155" t="s">
         <v>433</v>
       </c>
-      <c r="AE2" s="230" t="s">
+      <c r="AE2" s="250" t="s">
         <v>482</v>
       </c>
       <c r="AF2" s="155" t="s">
@@ -10804,7 +10855,7 @@
       <c r="AH2" s="155" t="s">
         <v>481</v>
       </c>
-      <c r="AI2" s="230" t="s">
+      <c r="AI2" s="250" t="s">
         <v>480</v>
       </c>
     </row>
@@ -10818,7 +10869,7 @@
       <c r="G3" s="155" t="s">
         <v>427</v>
       </c>
-      <c r="H3" s="230"/>
+      <c r="H3" s="250"/>
       <c r="I3" s="155" t="s">
         <v>479</v>
       </c>
@@ -10849,11 +10900,11 @@
       <c r="R3" s="155" t="s">
         <v>414</v>
       </c>
-      <c r="S3" s="230"/>
+      <c r="S3" s="250"/>
       <c r="T3" s="155" t="s">
         <v>411</v>
       </c>
-      <c r="U3" s="230"/>
+      <c r="U3" s="250"/>
       <c r="V3" s="155" t="s">
         <v>470</v>
       </c>
@@ -10881,7 +10932,7 @@
       <c r="AD3" s="155" t="s">
         <v>462</v>
       </c>
-      <c r="AE3" s="230"/>
+      <c r="AE3" s="250"/>
       <c r="AF3" s="155" t="s">
         <v>461</v>
       </c>
@@ -10891,7 +10942,7 @@
       <c r="AH3" s="155" t="s">
         <v>391</v>
       </c>
-      <c r="AI3" s="230"/>
+      <c r="AI3" s="250"/>
     </row>
     <row r="4" spans="1:62" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="158"/>
@@ -10913,7 +10964,7 @@
       <c r="G4" s="155" t="s">
         <v>377</v>
       </c>
-      <c r="H4" s="230"/>
+      <c r="H4" s="250"/>
       <c r="I4" s="155" t="s">
         <v>460</v>
       </c>
@@ -10944,11 +10995,11 @@
       <c r="R4" s="155" t="s">
         <v>363</v>
       </c>
-      <c r="S4" s="230"/>
+      <c r="S4" s="250"/>
       <c r="T4" s="155" t="s">
         <v>359</v>
       </c>
-      <c r="U4" s="230"/>
+      <c r="U4" s="250"/>
       <c r="V4" s="155" t="s">
         <v>451</v>
       </c>
@@ -10976,7 +11027,7 @@
       <c r="AD4" s="155" t="s">
         <v>443</v>
       </c>
-      <c r="AE4" s="230"/>
+      <c r="AE4" s="250"/>
       <c r="AF4" s="155" t="s">
         <v>442</v>
       </c>
@@ -10986,7 +11037,7 @@
       <c r="AH4" s="155" t="s">
         <v>338</v>
       </c>
-      <c r="AI4" s="230"/>
+      <c r="AI4" s="250"/>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A5" s="161" t="s">
@@ -12578,32 +12629,32 @@
       <c r="S17" s="111"/>
     </row>
     <row r="18" spans="5:19" ht="21" x14ac:dyDescent="0.25">
-      <c r="E18" s="236" t="s">
+      <c r="E18" s="256" t="s">
         <v>517</v>
       </c>
-      <c r="F18" s="237"/>
-      <c r="G18" s="237"/>
-      <c r="H18" s="237"/>
-      <c r="I18" s="237"/>
-      <c r="J18" s="237"/>
-      <c r="K18" s="237"/>
-      <c r="L18" s="237"/>
-      <c r="M18" s="237"/>
+      <c r="F18" s="257"/>
+      <c r="G18" s="257"/>
+      <c r="H18" s="257"/>
+      <c r="I18" s="257"/>
+      <c r="J18" s="257"/>
+      <c r="K18" s="257"/>
+      <c r="L18" s="257"/>
+      <c r="M18" s="257"/>
     </row>
     <row r="19" spans="5:19" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="5:19" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E20" s="233" t="s">
+      <c r="E20" s="253" t="s">
         <v>440</v>
       </c>
-      <c r="F20" s="234"/>
-      <c r="G20" s="234"/>
-      <c r="H20" s="234"/>
-      <c r="I20" s="234"/>
-      <c r="J20" s="234"/>
-      <c r="K20" s="234"/>
-      <c r="L20" s="234"/>
-      <c r="M20" s="234"/>
-      <c r="N20" s="213"/>
+      <c r="F20" s="254"/>
+      <c r="G20" s="254"/>
+      <c r="H20" s="254"/>
+      <c r="I20" s="254"/>
+      <c r="J20" s="254"/>
+      <c r="K20" s="254"/>
+      <c r="L20" s="254"/>
+      <c r="M20" s="254"/>
+      <c r="N20" s="210"/>
     </row>
     <row r="21" spans="5:19" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="23" spans="5:19" x14ac:dyDescent="0.2">
@@ -12722,13 +12773,13 @@
       <c r="G2" s="155" t="s">
         <v>436</v>
       </c>
-      <c r="H2" s="230" t="s">
+      <c r="H2" s="250" t="s">
         <v>435</v>
       </c>
       <c r="I2" s="155" t="s">
         <v>152</v>
       </c>
-      <c r="J2" s="230" t="s">
+      <c r="J2" s="250" t="s">
         <v>434</v>
       </c>
     </row>
@@ -12742,11 +12793,11 @@
       <c r="G3" s="155" t="s">
         <v>414</v>
       </c>
-      <c r="H3" s="230"/>
+      <c r="H3" s="250"/>
       <c r="I3" s="155" t="s">
         <v>411</v>
       </c>
-      <c r="J3" s="230"/>
+      <c r="J3" s="250"/>
     </row>
     <row r="4" spans="1:62" ht="36" x14ac:dyDescent="0.2">
       <c r="A4" s="177"/>
@@ -12768,11 +12819,11 @@
       <c r="G4" s="155" t="s">
         <v>363</v>
       </c>
-      <c r="H4" s="230"/>
+      <c r="H4" s="250"/>
       <c r="I4" s="155" t="s">
         <v>359</v>
       </c>
-      <c r="J4" s="230"/>
+      <c r="J4" s="250"/>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A5" s="171" t="s">
@@ -13095,23 +13146,23 @@
       </c>
     </row>
     <row r="16" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="E16" s="238" t="s">
+      <c r="E16" s="258" t="s">
         <v>516</v>
       </c>
-      <c r="F16" s="239"/>
-      <c r="G16" s="239"/>
-      <c r="H16" s="239"/>
-      <c r="I16" s="239"/>
-      <c r="J16" s="239"/>
+      <c r="F16" s="259"/>
+      <c r="G16" s="259"/>
+      <c r="H16" s="259"/>
+      <c r="I16" s="259"/>
+      <c r="J16" s="259"/>
     </row>
     <row r="17" spans="4:10" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D17" s="110"/>
-      <c r="E17" s="239"/>
-      <c r="F17" s="239"/>
-      <c r="G17" s="239"/>
-      <c r="H17" s="239"/>
-      <c r="I17" s="239"/>
-      <c r="J17" s="239"/>
+      <c r="E17" s="259"/>
+      <c r="F17" s="259"/>
+      <c r="G17" s="259"/>
+      <c r="H17" s="259"/>
+      <c r="I17" s="259"/>
+      <c r="J17" s="259"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -13132,7 +13183,7 @@
   <dimension ref="A1:DN8"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102"/>
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13456,7 +13507,7 @@
   <dimension ref="A1:EF4"/>
   <sheetViews>
     <sheetView showFormulas="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A116" sqref="A116"/>
+      <selection activeCell="A89" sqref="A89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13490,14 +13541,14 @@
       <c r="H1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="EA1" s="224" t="s">
+      <c r="EA1" s="244" t="s">
         <v>492</v>
       </c>
-      <c r="EB1" s="224"/>
-      <c r="EC1" s="224"/>
-      <c r="ED1" s="224"/>
-      <c r="EE1" s="224"/>
-      <c r="EF1" s="224"/>
+      <c r="EB1" s="244"/>
+      <c r="EC1" s="244"/>
+      <c r="ED1" s="244"/>
+      <c r="EE1" s="244"/>
+      <c r="EF1" s="244"/>
     </row>
     <row r="2" spans="1:136" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
@@ -13579,7 +13630,7 @@
     <row r="1" spans="1:16" s="4" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="5"/>
-      <c r="C1" s="214" t="s">
+      <c r="C1" s="211" t="s">
         <v>507</v>
       </c>
       <c r="D1" s="7"/>
@@ -13624,20 +13675,20 @@
     </row>
     <row r="4" spans="1:16" ht="40" x14ac:dyDescent="0.2">
       <c r="C4" s="9"/>
-      <c r="E4" s="225" t="s">
+      <c r="E4" s="245" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="226"/>
-      <c r="G4" s="226"/>
-      <c r="H4" s="226"/>
-      <c r="I4" s="227"/>
-      <c r="J4" s="225" t="s">
+      <c r="F4" s="246"/>
+      <c r="G4" s="246"/>
+      <c r="H4" s="246"/>
+      <c r="I4" s="247"/>
+      <c r="J4" s="245" t="s">
         <v>28</v>
       </c>
-      <c r="K4" s="226"/>
-      <c r="L4" s="226"/>
-      <c r="M4" s="226"/>
-      <c r="N4" s="227"/>
+      <c r="K4" s="246"/>
+      <c r="L4" s="246"/>
+      <c r="M4" s="246"/>
+      <c r="N4" s="247"/>
       <c r="O4" s="30" t="s">
         <v>29</v>
       </c>
@@ -15257,16 +15308,16 @@
   <sheetData>
     <row r="1" spans="1:62" s="64" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A1" s="107"/>
-      <c r="B1" s="229" t="s">
+      <c r="B1" s="249" t="s">
         <v>439</v>
       </c>
-      <c r="C1" s="229"/>
-      <c r="D1" s="229"/>
-      <c r="E1" s="229"/>
-      <c r="F1" s="229"/>
-      <c r="G1" s="229"/>
-      <c r="H1" s="229"/>
-      <c r="I1" s="229"/>
+      <c r="C1" s="249"/>
+      <c r="D1" s="249"/>
+      <c r="E1" s="249"/>
+      <c r="F1" s="249"/>
+      <c r="G1" s="249"/>
+      <c r="H1" s="249"/>
+      <c r="I1" s="249"/>
       <c r="AC1" s="106"/>
       <c r="AD1" s="106"/>
       <c r="AE1" s="106"/>
@@ -15287,7 +15338,7 @@
       <c r="G2" s="102" t="s">
         <v>438</v>
       </c>
-      <c r="H2" s="228" t="s">
+      <c r="H2" s="248" t="s">
         <v>437</v>
       </c>
       <c r="I2" s="101" t="s">
@@ -15332,7 +15383,7 @@
       <c r="V2" s="101" t="s">
         <v>436</v>
       </c>
-      <c r="W2" s="228" t="s">
+      <c r="W2" s="248" t="s">
         <v>435</v>
       </c>
       <c r="X2" s="102" t="s">
@@ -15347,7 +15398,7 @@
       <c r="AA2" s="102" t="s">
         <v>152</v>
       </c>
-      <c r="AB2" s="228" t="s">
+      <c r="AB2" s="248" t="s">
         <v>434</v>
       </c>
       <c r="AC2" s="98" t="s">
@@ -15377,7 +15428,7 @@
       <c r="AK2" s="98" t="s">
         <v>433</v>
       </c>
-      <c r="AL2" s="228" t="s">
+      <c r="AL2" s="248" t="s">
         <v>432</v>
       </c>
       <c r="AM2" s="98" t="s">
@@ -15419,7 +15470,7 @@
       <c r="AY2" s="98" t="s">
         <v>431</v>
       </c>
-      <c r="AZ2" s="228" t="s">
+      <c r="AZ2" s="248" t="s">
         <v>430</v>
       </c>
       <c r="BA2" s="97" t="s">
@@ -15449,7 +15500,7 @@
       <c r="BI2" s="97" t="s">
         <v>429</v>
       </c>
-      <c r="BJ2" s="228" t="s">
+      <c r="BJ2" s="248" t="s">
         <v>428</v>
       </c>
     </row>
@@ -15463,7 +15514,7 @@
       <c r="G3" s="102" t="s">
         <v>427</v>
       </c>
-      <c r="H3" s="228"/>
+      <c r="H3" s="248"/>
       <c r="I3" s="101" t="s">
         <v>426</v>
       </c>
@@ -15504,7 +15555,7 @@
       <c r="V3" s="101" t="s">
         <v>414</v>
       </c>
-      <c r="W3" s="228"/>
+      <c r="W3" s="248"/>
       <c r="X3" s="96"/>
       <c r="Y3" s="102" t="s">
         <v>413</v>
@@ -15515,7 +15566,7 @@
       <c r="AA3" s="102" t="s">
         <v>411</v>
       </c>
-      <c r="AB3" s="228"/>
+      <c r="AB3" s="248"/>
       <c r="AC3" s="98" t="s">
         <v>410</v>
       </c>
@@ -15543,7 +15594,7 @@
       <c r="AK3" s="98" t="s">
         <v>404</v>
       </c>
-      <c r="AL3" s="228"/>
+      <c r="AL3" s="248"/>
       <c r="AM3" s="98" t="s">
         <v>403</v>
       </c>
@@ -15583,7 +15634,7 @@
       <c r="AY3" s="98" t="s">
         <v>391</v>
       </c>
-      <c r="AZ3" s="228"/>
+      <c r="AZ3" s="248"/>
       <c r="BA3" s="97" t="s">
         <v>390</v>
       </c>
@@ -15611,7 +15662,7 @@
       <c r="BI3" s="97" t="s">
         <v>382</v>
       </c>
-      <c r="BJ3" s="228"/>
+      <c r="BJ3" s="248"/>
     </row>
     <row r="4" spans="1:62" s="64" customFormat="1" ht="60" x14ac:dyDescent="0.15">
       <c r="A4" s="104"/>
@@ -15633,7 +15684,7 @@
       <c r="G4" s="102" t="s">
         <v>377</v>
       </c>
-      <c r="H4" s="228"/>
+      <c r="H4" s="248"/>
       <c r="I4" s="101" t="s">
         <v>376</v>
       </c>
@@ -15676,7 +15727,7 @@
       <c r="V4" s="100" t="s">
         <v>363</v>
       </c>
-      <c r="W4" s="228"/>
+      <c r="W4" s="248"/>
       <c r="X4" s="99" t="s">
         <v>362</v>
       </c>
@@ -15689,7 +15740,7 @@
       <c r="AA4" s="99" t="s">
         <v>359</v>
       </c>
-      <c r="AB4" s="228"/>
+      <c r="AB4" s="248"/>
       <c r="AC4" s="98" t="s">
         <v>358</v>
       </c>
@@ -15717,7 +15768,7 @@
       <c r="AK4" s="98" t="s">
         <v>351</v>
       </c>
-      <c r="AL4" s="228"/>
+      <c r="AL4" s="248"/>
       <c r="AM4" s="98" t="s">
         <v>350</v>
       </c>
@@ -15757,7 +15808,7 @@
       <c r="AY4" s="98" t="s">
         <v>338</v>
       </c>
-      <c r="AZ4" s="228"/>
+      <c r="AZ4" s="248"/>
       <c r="BA4" s="97" t="s">
         <v>337</v>
       </c>
@@ -15785,7 +15836,7 @@
       <c r="BI4" s="97" t="s">
         <v>329</v>
       </c>
-      <c r="BJ4" s="228"/>
+      <c r="BJ4" s="248"/>
     </row>
     <row r="5" spans="1:62" s="64" customFormat="1" ht="144" x14ac:dyDescent="0.15">
       <c r="A5" s="72" t="s">
@@ -16763,7 +16814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:62" s="64" customFormat="1" ht="36" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:62" s="64" customFormat="1" ht="48" x14ac:dyDescent="0.15">
       <c r="A13" s="72" t="s">
         <v>233</v>
       </c>
@@ -17484,16 +17535,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" s="112" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B1" s="231" t="s">
+      <c r="B1" s="251" t="s">
         <v>439</v>
       </c>
-      <c r="C1" s="231"/>
-      <c r="D1" s="231"/>
-      <c r="E1" s="231"/>
-      <c r="F1" s="231"/>
-      <c r="G1" s="231"/>
-      <c r="H1" s="231"/>
-      <c r="I1" s="231"/>
+      <c r="C1" s="251"/>
+      <c r="D1" s="251"/>
+      <c r="E1" s="251"/>
+      <c r="F1" s="251"/>
+      <c r="G1" s="251"/>
+      <c r="H1" s="251"/>
+      <c r="I1" s="251"/>
     </row>
     <row r="2" spans="1:62" s="112" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="158"/>
@@ -17505,7 +17556,7 @@
       <c r="G2" s="155" t="s">
         <v>438</v>
       </c>
-      <c r="H2" s="230" t="s">
+      <c r="H2" s="250" t="s">
         <v>437</v>
       </c>
       <c r="I2" s="154" t="s">
@@ -17550,7 +17601,7 @@
       <c r="V2" s="154" t="s">
         <v>436</v>
       </c>
-      <c r="W2" s="230" t="s">
+      <c r="W2" s="250" t="s">
         <v>435</v>
       </c>
       <c r="X2" s="155" t="s">
@@ -17565,7 +17616,7 @@
       <c r="AA2" s="155" t="s">
         <v>152</v>
       </c>
-      <c r="AB2" s="230" t="s">
+      <c r="AB2" s="250" t="s">
         <v>434</v>
       </c>
       <c r="AC2" s="152" t="s">
@@ -17595,7 +17646,7 @@
       <c r="AK2" s="152" t="s">
         <v>433</v>
       </c>
-      <c r="AL2" s="230" t="s">
+      <c r="AL2" s="250" t="s">
         <v>432</v>
       </c>
       <c r="AM2" s="152" t="s">
@@ -17637,7 +17688,7 @@
       <c r="AY2" s="152" t="s">
         <v>431</v>
       </c>
-      <c r="AZ2" s="230" t="s">
+      <c r="AZ2" s="250" t="s">
         <v>430</v>
       </c>
       <c r="BA2" s="151" t="s">
@@ -17667,7 +17718,7 @@
       <c r="BI2" s="151" t="s">
         <v>429</v>
       </c>
-      <c r="BJ2" s="230" t="s">
+      <c r="BJ2" s="250" t="s">
         <v>428</v>
       </c>
     </row>
@@ -17681,7 +17732,7 @@
       <c r="G3" s="155" t="s">
         <v>427</v>
       </c>
-      <c r="H3" s="230"/>
+      <c r="H3" s="250"/>
       <c r="I3" s="154" t="s">
         <v>426</v>
       </c>
@@ -17722,7 +17773,7 @@
       <c r="V3" s="154" t="s">
         <v>414</v>
       </c>
-      <c r="W3" s="230"/>
+      <c r="W3" s="250"/>
       <c r="X3" s="150"/>
       <c r="Y3" s="155" t="s">
         <v>413</v>
@@ -17733,7 +17784,7 @@
       <c r="AA3" s="155" t="s">
         <v>411</v>
       </c>
-      <c r="AB3" s="230"/>
+      <c r="AB3" s="250"/>
       <c r="AC3" s="152" t="s">
         <v>410</v>
       </c>
@@ -17761,7 +17812,7 @@
       <c r="AK3" s="152" t="s">
         <v>404</v>
       </c>
-      <c r="AL3" s="230"/>
+      <c r="AL3" s="250"/>
       <c r="AM3" s="152" t="s">
         <v>403</v>
       </c>
@@ -17801,7 +17852,7 @@
       <c r="AY3" s="152" t="s">
         <v>391</v>
       </c>
-      <c r="AZ3" s="230"/>
+      <c r="AZ3" s="250"/>
       <c r="BA3" s="151" t="s">
         <v>390</v>
       </c>
@@ -17829,7 +17880,7 @@
       <c r="BI3" s="151" t="s">
         <v>382</v>
       </c>
-      <c r="BJ3" s="230"/>
+      <c r="BJ3" s="250"/>
     </row>
     <row r="4" spans="1:62" s="112" customFormat="1" ht="60" x14ac:dyDescent="0.15">
       <c r="A4" s="157"/>
@@ -17851,7 +17902,7 @@
       <c r="G4" s="155" t="s">
         <v>377</v>
       </c>
-      <c r="H4" s="230"/>
+      <c r="H4" s="250"/>
       <c r="I4" s="154" t="s">
         <v>376</v>
       </c>
@@ -17894,7 +17945,7 @@
       <c r="V4" s="154" t="s">
         <v>363</v>
       </c>
-      <c r="W4" s="230"/>
+      <c r="W4" s="250"/>
       <c r="X4" s="153" t="s">
         <v>362</v>
       </c>
@@ -17907,7 +17958,7 @@
       <c r="AA4" s="153" t="s">
         <v>359</v>
       </c>
-      <c r="AB4" s="230"/>
+      <c r="AB4" s="250"/>
       <c r="AC4" s="152" t="s">
         <v>358</v>
       </c>
@@ -17935,7 +17986,7 @@
       <c r="AK4" s="152" t="s">
         <v>351</v>
       </c>
-      <c r="AL4" s="230"/>
+      <c r="AL4" s="250"/>
       <c r="AM4" s="152" t="s">
         <v>350</v>
       </c>
@@ -17975,7 +18026,7 @@
       <c r="AY4" s="152" t="s">
         <v>338</v>
       </c>
-      <c r="AZ4" s="230"/>
+      <c r="AZ4" s="250"/>
       <c r="BA4" s="151" t="s">
         <v>337</v>
       </c>
@@ -18003,7 +18054,7 @@
       <c r="BI4" s="151" t="s">
         <v>329</v>
       </c>
-      <c r="BJ4" s="230"/>
+      <c r="BJ4" s="250"/>
     </row>
     <row r="5" spans="1:62" s="112" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="122" t="s">

</xml_diff>

<commit_message>
changes extractor format notice
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F1867FA-6BD2-604C-AC39-EE3945E7A4B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E1AFE1-6CA2-E94C-AACA-7E3E27C0DD10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="600" windowWidth="22940" windowHeight="13240" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
@@ -2688,16 +2688,76 @@
     </r>
   </si>
   <si>
-    <t>→ Sélectionner la juridiction souhaitée à partir du menu déroulant qui se trouve dans la cellule D5 identifiée en orange.</t>
+    <t>#! HYPERLINK firstLink.label firstLink.url</t>
+  </si>
+  <si>
+    <t>#! HYPERLINK secondLink.label secondLink.url</t>
+  </si>
+  <si>
+    <t>#! HYPERLINK thirdLink.label thirdLink.url</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">→ Sélectionner la juridiction souhaitée à partir du menu déroulant qui se trouve dans la cellule D5 identifiée en </t>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF2D46E0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>→ Sélectionner la juridiction souhaitée à partir du menu déroulant qui se trouve dans la cellule D5 identifiée en</t>
     </r>
     <r>
       <rPr>
         <b/>
-        <sz val="16"/>
+        <sz val="12"/>
+        <color rgb="FF860000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>orange.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF2D46E0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>→ Sélectionner la juridiction souhaitée à partir du menu déroulant qui se trouve dans la cellule D5 identifiée en</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF860000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
         <color theme="5"/>
         <rFont val="Calibri (Corps)"/>
       </rPr>
@@ -2706,7 +2766,7 @@
     <r>
       <rPr>
         <b/>
-        <sz val="16"/>
+        <sz val="12"/>
         <color rgb="FF860000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -2714,15 +2774,6 @@
       </rPr>
       <t>.</t>
     </r>
-  </si>
-  <si>
-    <t>#! HYPERLINK firstLink.label firstLink.url</t>
-  </si>
-  <si>
-    <t>#! HYPERLINK secondLink.label secondLink.url</t>
-  </si>
-  <si>
-    <t>#! HYPERLINK thirdLink.label thirdLink.url</t>
   </si>
 </sst>
 </file>
@@ -2737,9 +2788,16 @@
     <numFmt numFmtId="168" formatCode="0.###;0.###;\-"/>
     <numFmt numFmtId="169" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
   </numFmts>
-  <fonts count="48" x14ac:knownFonts="1">
+  <fonts count="52" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -3009,14 +3067,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="22"/>
       <color theme="0"/>
@@ -3037,20 +3087,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color rgb="FF860000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="5"/>
-      <name val="Calibri (Corps)"/>
     </font>
     <font>
       <b/>
@@ -3075,8 +3111,53 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF860000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF2D46E0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="5"/>
+      <name val="Calibri (Corps)"/>
+    </font>
   </fonts>
-  <fills count="23">
+  <fills count="29">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3209,8 +3290,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE64B85"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2D46E0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0B0B97"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7F02D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B252"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="46">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -3576,15 +3693,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color rgb="FFFF0000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thick">
         <color rgb="FFFF0000"/>
@@ -3724,16 +3832,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="260">
+  <cellXfs count="262">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -3741,7 +3848,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3750,61 +3857,61 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -3817,287 +3924,520 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="4" applyFont="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="4" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="18" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="169" fontId="21" fillId="10" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="21" fillId="11" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="21" fillId="10" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="21" fillId="11" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="9" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="23" fillId="12" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="24" fillId="13" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="25" fillId="9" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="24" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="169" fontId="25" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="25" fillId="9" borderId="17" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="23" fillId="9" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="21" fillId="10" borderId="18" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="25" fillId="0" borderId="10" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="21" fillId="10" borderId="19" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="25" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="25" fillId="9" borderId="20" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="24" fillId="13" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="23" fillId="12" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="25" fillId="9" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="23" fillId="12" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="25" fillId="12" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="25" fillId="12" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="24" fillId="12" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="24" fillId="12" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="9" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="29" fillId="9" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyProtection="1">
+      <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="4" applyFont="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="4" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="169" fontId="13" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="169" fontId="21" fillId="9" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="17" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="169" fontId="20" fillId="10" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="20" fillId="11" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="20" fillId="10" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="20" fillId="11" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="9" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="22" fillId="12" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="23" fillId="13" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="24" fillId="9" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="23" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="169" fontId="24" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="24" fillId="9" borderId="17" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="22" fillId="9" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="20" fillId="10" borderId="18" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="24" fillId="0" borderId="10" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="20" fillId="10" borderId="19" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="24" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="24" fillId="9" borderId="20" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="23" fillId="13" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="22" fillId="12" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="24" fillId="9" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="22" fillId="12" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="24" fillId="12" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="24" fillId="12" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="23" fillId="12" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="23" fillId="12" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="9" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="28" fillId="9" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="4" applyFont="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="12" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="20" fillId="9" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="169" fontId="21" fillId="10" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="21" fillId="11" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="26" fillId="11" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="169" fontId="20" fillId="10" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="20" fillId="11" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="25" fillId="11" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="23" fillId="9" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="49" fontId="22" fillId="9" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="169" fontId="23" fillId="12" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="24" fillId="13" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="25" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="24" fillId="13" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="23" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="25" fillId="9" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="24" fillId="8" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="26" fillId="10" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="24" fillId="13" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="169" fontId="22" fillId="12" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="169" fontId="23" fillId="13" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="169" fontId="25" fillId="9" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="24" fillId="13" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="24" fillId="8" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="24" fillId="8" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="24" fillId="9" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="24" fillId="9" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="24" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="23" fillId="12" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="24" fillId="8" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="25" fillId="12" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="25" fillId="12" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="24" fillId="13" borderId="15" xfId="4" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="24" fillId="12" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="23" fillId="8" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="23" fillId="8" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="9" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="29" fillId="9" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="16" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="21" fillId="10" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="23" fillId="9" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="29" fillId="10" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="11" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="9" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="9" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="34" fillId="8" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="9" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="9" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="34" fillId="19" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="34" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="34" fillId="9" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="18" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="29" fillId="9" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="35" fillId="9" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="9" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="24" fillId="8" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="21" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="23" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection hidden="1"/>
     </xf>
@@ -4105,269 +4445,36 @@
       <alignment horizontal="right"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="169" fontId="23" fillId="13" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="169" fontId="21" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="169" fontId="22" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="169" fontId="24" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="169" fontId="24" fillId="9" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="169" fontId="25" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="169" fontId="23" fillId="8" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="25" fillId="10" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="23" fillId="13" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="20" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="169" fontId="24" fillId="9" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="23" fillId="13" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="23" fillId="8" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="23" fillId="8" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="23" fillId="9" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="23" fillId="9" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="23" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="22" fillId="12" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="23" fillId="8" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="24" fillId="12" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="24" fillId="12" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="23" fillId="13" borderId="15" xfId="4" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="23" fillId="12" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="22" fillId="8" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="22" fillId="8" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="37" fillId="20" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="9" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="28" fillId="9" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="16" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="20" fillId="10" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="22" fillId="9" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="28" fillId="10" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="11" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="9" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="9" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="33" fillId="8" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="9" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="9" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="33" fillId="19" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="33" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="33" fillId="9" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="18" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="28" fillId="9" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="34" fillId="9" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="30" fillId="9" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="23" fillId="8" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="20" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="22" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="23" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="20" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="23" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="24" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="20" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="36" fillId="20" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="40" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -4393,66 +4500,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="4" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="40" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="9" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="43" fillId="9" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="25" xfId="6" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="27" xfId="6" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="29" xfId="6" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="40" xfId="6" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="40" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -4464,106 +4556,132 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="31" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="31" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="46" fillId="23" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="24" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="25" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="27" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="28" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="6">
     <cellStyle name="Comma 2" xfId="2" xr:uid="{C877C5E8-FCBF-114F-9ECB-F75EF7C9C0EB}"/>
-    <cellStyle name="Lien hypertexte" xfId="6" builtinId="8"/>
     <cellStyle name="Milliers" xfId="3" builtinId="3"/>
     <cellStyle name="Milliers 2" xfId="5" xr:uid="{C98A9282-6AC5-784B-80AA-54BB74A59302}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4588,6 +4706,16 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF01A94F"/>
+      <color rgb="FFF7EF2D"/>
+      <color rgb="FFFE0000"/>
+      <color rgb="FF0B0B97"/>
+      <color rgb="FF2C45E0"/>
+      <color rgb="FFCE4275"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -5334,7 +5462,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="A14" sqref="A14:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5354,11 +5482,11 @@
       <c r="B1" s="197" t="s">
         <v>494</v>
       </c>
-      <c r="C1" s="225" t="s">
+      <c r="C1" s="220" t="s">
         <v>495</v>
       </c>
-      <c r="D1" s="225"/>
-      <c r="E1" s="225"/>
+      <c r="D1" s="220"/>
+      <c r="E1" s="220"/>
       <c r="F1" s="198"/>
       <c r="H1" s="28" t="s">
         <v>0</v>
@@ -5367,11 +5495,11 @@
     <row r="2" spans="1:8" s="202" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="199"/>
       <c r="B2" s="200"/>
-      <c r="C2" s="226" t="s">
+      <c r="C2" s="221" t="s">
         <v>496</v>
       </c>
-      <c r="D2" s="226"/>
-      <c r="E2" s="226"/>
+      <c r="D2" s="221"/>
+      <c r="E2" s="221"/>
       <c r="F2" s="201"/>
       <c r="H2" s="28" t="s">
         <v>0</v>
@@ -5395,143 +5523,143 @@
       <c r="D4" s="207" t="s">
         <v>499</v>
       </c>
-      <c r="E4" s="232" t="s">
+      <c r="E4" s="227" t="s">
         <v>500</v>
       </c>
-      <c r="F4" s="233"/>
-      <c r="G4" s="221"/>
+      <c r="F4" s="228"/>
+      <c r="G4" s="216"/>
       <c r="H4" s="28" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="28" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="203"/>
-      <c r="B5" s="214" t="s">
+      <c r="B5" s="248" t="s">
         <v>501</v>
       </c>
-      <c r="C5" s="215" t="s">
+      <c r="C5" s="213" t="s">
         <v>502</v>
       </c>
-      <c r="D5" s="215" t="s">
+      <c r="D5" s="213" t="s">
         <v>503</v>
       </c>
-      <c r="E5" s="234" t="s">
-        <v>518</v>
-      </c>
-      <c r="F5" s="235"/>
-      <c r="G5" s="220"/>
+      <c r="E5" s="229" t="s">
+        <v>516</v>
+      </c>
+      <c r="F5" s="230"/>
+      <c r="G5" s="215"/>
       <c r="H5" s="28" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="28" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="203"/>
-      <c r="B6" s="216" t="s">
+      <c r="B6" s="249" t="s">
         <v>504</v>
       </c>
-      <c r="C6" s="217" t="s">
+      <c r="C6" s="214" t="s">
         <v>505</v>
       </c>
-      <c r="D6" s="217" t="s">
+      <c r="D6" s="214" t="s">
         <v>506</v>
       </c>
-      <c r="E6" s="236" t="s">
-        <v>519</v>
-      </c>
-      <c r="F6" s="237"/>
-      <c r="G6" s="220"/>
+      <c r="E6" s="231" t="s">
+        <v>517</v>
+      </c>
+      <c r="F6" s="232"/>
+      <c r="G6" s="215"/>
       <c r="H6" s="28" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="28" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="203"/>
-      <c r="B7" s="216" t="s">
+      <c r="B7" s="250" t="s">
         <v>507</v>
       </c>
-      <c r="C7" s="217" t="s">
+      <c r="C7" s="214" t="s">
         <v>508</v>
       </c>
-      <c r="D7" s="217" t="s">
+      <c r="D7" s="214" t="s">
         <v>509</v>
       </c>
-      <c r="E7" s="236" t="s">
-        <v>518</v>
-      </c>
-      <c r="F7" s="237"/>
-      <c r="G7" s="220"/>
+      <c r="E7" s="231" t="s">
+        <v>516</v>
+      </c>
+      <c r="F7" s="232"/>
+      <c r="G7" s="215"/>
       <c r="H7" s="28" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="28" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="203"/>
-      <c r="B8" s="218" t="s">
+      <c r="B8" s="251" t="s">
         <v>510</v>
       </c>
-      <c r="C8" s="227" t="s">
+      <c r="C8" s="222" t="s">
         <v>511</v>
       </c>
-      <c r="D8" s="227" t="s">
+      <c r="D8" s="222" t="s">
         <v>512</v>
       </c>
-      <c r="E8" s="238" t="s">
-        <v>520</v>
-      </c>
-      <c r="F8" s="239"/>
-      <c r="G8" s="220"/>
+      <c r="E8" s="233" t="s">
+        <v>518</v>
+      </c>
+      <c r="F8" s="234"/>
+      <c r="G8" s="215"/>
       <c r="H8" s="28" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="28" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="203"/>
-      <c r="B9" s="218" t="s">
+      <c r="B9" s="252" t="s">
         <v>513</v>
       </c>
-      <c r="C9" s="227"/>
-      <c r="D9" s="227"/>
-      <c r="E9" s="240"/>
-      <c r="F9" s="241"/>
-      <c r="G9" s="220"/>
+      <c r="C9" s="222"/>
+      <c r="D9" s="222"/>
+      <c r="E9" s="235"/>
+      <c r="F9" s="236"/>
+      <c r="G9" s="215"/>
       <c r="H9" s="28" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="28" customFormat="1" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="203"/>
-      <c r="B10" s="219" t="s">
+      <c r="B10" s="253" t="s">
         <v>514</v>
       </c>
-      <c r="C10" s="228"/>
-      <c r="D10" s="228"/>
-      <c r="E10" s="242"/>
-      <c r="F10" s="243"/>
-      <c r="G10" s="220"/>
+      <c r="C10" s="223"/>
+      <c r="D10" s="223"/>
+      <c r="E10" s="237"/>
+      <c r="F10" s="238"/>
+      <c r="G10" s="215"/>
       <c r="H10" s="28" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="28" customFormat="1" ht="5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="203"/>
-      <c r="B11" s="224"/>
-      <c r="C11" s="224"/>
-      <c r="D11" s="224"/>
-      <c r="E11" s="224"/>
-      <c r="F11" s="224"/>
+      <c r="B11" s="219"/>
+      <c r="C11" s="219"/>
+      <c r="D11" s="219"/>
+      <c r="E11" s="219"/>
+      <c r="F11" s="219"/>
       <c r="H11" s="28" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="28" customFormat="1" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="203"/>
-      <c r="B12" s="222"/>
-      <c r="C12" s="231" t="s">
+      <c r="B12" s="217"/>
+      <c r="C12" s="226" t="s">
         <v>515</v>
       </c>
-      <c r="D12" s="231"/>
-      <c r="E12" s="231"/>
-      <c r="F12" s="223"/>
+      <c r="D12" s="226"/>
+      <c r="E12" s="226"/>
+      <c r="F12" s="218"/>
       <c r="H12" s="28" t="s">
         <v>0</v>
       </c>
@@ -5544,14 +5672,14 @@
       </c>
     </row>
     <row r="14" spans="1:8" s="28" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="229" t="s">
+      <c r="A14" s="224" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="229"/>
-      <c r="C14" s="229"/>
-      <c r="D14" s="229"/>
-      <c r="E14" s="229"/>
-      <c r="F14" s="230"/>
+      <c r="B14" s="224"/>
+      <c r="C14" s="224"/>
+      <c r="D14" s="224"/>
+      <c r="E14" s="224"/>
+      <c r="F14" s="225"/>
       <c r="H14" s="28" t="s">
         <v>0</v>
       </c>
@@ -5575,14 +5703,6 @@
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F10"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="B5" location="'ETPT A-JUST'!A1" display="ETPT A-JUST" xr:uid="{A4B55920-38FE-8C44-A223-5786C8919747}"/>
-    <hyperlink ref="B6" location="'ETPT Format DDG'!A1" display="ETPT Format DDG" xr:uid="{79FC5922-FC41-BA4A-995C-9841D25952FF}"/>
-    <hyperlink ref="B7" location="'Agrégats DDG'!A1" display="Agrégats DDG" xr:uid="{81D3F220-88AB-F743-B1AC-13451DEA3C28}"/>
-    <hyperlink ref="B8" location="ETPT_TJ_DDG!A1" display="ETPT_TJ_DDG" xr:uid="{43523AD2-5123-C849-8EFA-27E13C4C136A}"/>
-    <hyperlink ref="B9" location="ETPT_TPRX_DDG!A1" display="ETPT_TPRX-DDG" xr:uid="{97476A23-C1B3-284C-B5B5-53A729579959}"/>
-    <hyperlink ref="B10" location="ETPT_CPH_DDG!A1" display="ETPT_CPH_DDG" xr:uid="{1F598F93-AFA2-E243-9BD5-6F6F6C8A32A5}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
   <drawing r:id="rId1"/>
@@ -5612,16 +5732,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A1" s="252" t="s">
+      <c r="A1" s="247" t="s">
         <v>483</v>
       </c>
-      <c r="B1" s="252"/>
-      <c r="C1" s="252"/>
-      <c r="D1" s="252"/>
-      <c r="E1" s="252"/>
-      <c r="F1" s="252"/>
-      <c r="G1" s="252"/>
-      <c r="H1" s="252"/>
+      <c r="B1" s="247"/>
+      <c r="C1" s="247"/>
+      <c r="D1" s="247"/>
+      <c r="E1" s="247"/>
+      <c r="F1" s="247"/>
+      <c r="G1" s="247"/>
+      <c r="H1" s="247"/>
       <c r="I1" s="112"/>
       <c r="J1" s="112"/>
       <c r="K1" s="112"/>
@@ -5660,7 +5780,7 @@
       <c r="G2" s="155" t="s">
         <v>438</v>
       </c>
-      <c r="H2" s="250" t="s">
+      <c r="H2" s="245" t="s">
         <v>437</v>
       </c>
       <c r="I2" s="155" t="s">
@@ -5693,13 +5813,13 @@
       <c r="R2" s="155" t="s">
         <v>436</v>
       </c>
-      <c r="S2" s="250" t="s">
+      <c r="S2" s="245" t="s">
         <v>435</v>
       </c>
       <c r="T2" s="155" t="s">
         <v>152</v>
       </c>
-      <c r="U2" s="250" t="s">
+      <c r="U2" s="245" t="s">
         <v>434</v>
       </c>
       <c r="V2" s="155" t="s">
@@ -5729,7 +5849,7 @@
       <c r="AD2" s="155" t="s">
         <v>433</v>
       </c>
-      <c r="AE2" s="250" t="s">
+      <c r="AE2" s="245" t="s">
         <v>482</v>
       </c>
       <c r="AF2" s="155" t="s">
@@ -5741,7 +5861,7 @@
       <c r="AH2" s="155" t="s">
         <v>481</v>
       </c>
-      <c r="AI2" s="250" t="s">
+      <c r="AI2" s="245" t="s">
         <v>480</v>
       </c>
     </row>
@@ -5755,7 +5875,7 @@
       <c r="G3" s="155" t="s">
         <v>427</v>
       </c>
-      <c r="H3" s="250"/>
+      <c r="H3" s="245"/>
       <c r="I3" s="155" t="s">
         <v>479</v>
       </c>
@@ -5786,11 +5906,11 @@
       <c r="R3" s="155" t="s">
         <v>414</v>
       </c>
-      <c r="S3" s="250"/>
+      <c r="S3" s="245"/>
       <c r="T3" s="155" t="s">
         <v>411</v>
       </c>
-      <c r="U3" s="250"/>
+      <c r="U3" s="245"/>
       <c r="V3" s="155" t="s">
         <v>470</v>
       </c>
@@ -5818,7 +5938,7 @@
       <c r="AD3" s="155" t="s">
         <v>462</v>
       </c>
-      <c r="AE3" s="250"/>
+      <c r="AE3" s="245"/>
       <c r="AF3" s="155" t="s">
         <v>461</v>
       </c>
@@ -5828,7 +5948,7 @@
       <c r="AH3" s="155" t="s">
         <v>391</v>
       </c>
-      <c r="AI3" s="250"/>
+      <c r="AI3" s="245"/>
     </row>
     <row r="4" spans="1:35" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="158"/>
@@ -5850,7 +5970,7 @@
       <c r="G4" s="155" t="s">
         <v>377</v>
       </c>
-      <c r="H4" s="250"/>
+      <c r="H4" s="245"/>
       <c r="I4" s="155" t="s">
         <v>460</v>
       </c>
@@ -5881,11 +6001,11 @@
       <c r="R4" s="155" t="s">
         <v>363</v>
       </c>
-      <c r="S4" s="250"/>
+      <c r="S4" s="245"/>
       <c r="T4" s="155" t="s">
         <v>359</v>
       </c>
-      <c r="U4" s="250"/>
+      <c r="U4" s="245"/>
       <c r="V4" s="155" t="s">
         <v>451</v>
       </c>
@@ -5913,7 +6033,7 @@
       <c r="AD4" s="155" t="s">
         <v>443</v>
       </c>
-      <c r="AE4" s="250"/>
+      <c r="AE4" s="245"/>
       <c r="AF4" s="155" t="s">
         <v>442</v>
       </c>
@@ -5923,7 +6043,7 @@
       <c r="AH4" s="155" t="s">
         <v>338</v>
       </c>
-      <c r="AI4" s="250"/>
+      <c r="AI4" s="245"/>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A5" s="161" t="s">
@@ -7032,13 +7152,13 @@
       <c r="G2" s="155" t="s">
         <v>436</v>
       </c>
-      <c r="H2" s="250" t="s">
+      <c r="H2" s="245" t="s">
         <v>435</v>
       </c>
       <c r="I2" s="155" t="s">
         <v>152</v>
       </c>
-      <c r="J2" s="250" t="s">
+      <c r="J2" s="245" t="s">
         <v>434</v>
       </c>
     </row>
@@ -7052,11 +7172,11 @@
       <c r="G3" s="155" t="s">
         <v>414</v>
       </c>
-      <c r="H3" s="250"/>
+      <c r="H3" s="245"/>
       <c r="I3" s="155" t="s">
         <v>411</v>
       </c>
-      <c r="J3" s="250"/>
+      <c r="J3" s="245"/>
     </row>
     <row r="4" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A4" s="177"/>
@@ -7078,11 +7198,11 @@
       <c r="G4" s="155" t="s">
         <v>363</v>
       </c>
-      <c r="H4" s="250"/>
+      <c r="H4" s="245"/>
       <c r="I4" s="155" t="s">
         <v>359</v>
       </c>
-      <c r="J4" s="250"/>
+      <c r="J4" s="245"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="171" t="s">
@@ -7381,9 +7501,9 @@
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C2925AE-B1C3-2143-BED8-865F5DD872E0}">
   <sheetPr codeName="Feuil9">
-    <tabColor rgb="FFC00000"/>
+    <tabColor rgb="FFFE0000"/>
   </sheetPr>
-  <dimension ref="A1:BK23"/>
+  <dimension ref="A1:BK21"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
@@ -7486,7 +7606,7 @@
       <c r="G2" s="155" t="s">
         <v>438</v>
       </c>
-      <c r="H2" s="250" t="s">
+      <c r="H2" s="245" t="s">
         <v>437</v>
       </c>
       <c r="I2" s="154" t="s">
@@ -7531,7 +7651,7 @@
       <c r="V2" s="154" t="s">
         <v>436</v>
       </c>
-      <c r="W2" s="250" t="s">
+      <c r="W2" s="245" t="s">
         <v>435</v>
       </c>
       <c r="X2" s="155" t="s">
@@ -7546,7 +7666,7 @@
       <c r="AA2" s="155" t="s">
         <v>152</v>
       </c>
-      <c r="AB2" s="250" t="s">
+      <c r="AB2" s="245" t="s">
         <v>434</v>
       </c>
       <c r="AC2" s="152" t="s">
@@ -7576,7 +7696,7 @@
       <c r="AK2" s="152" t="s">
         <v>433</v>
       </c>
-      <c r="AL2" s="250" t="s">
+      <c r="AL2" s="245" t="s">
         <v>432</v>
       </c>
       <c r="AM2" s="152" t="s">
@@ -7618,7 +7738,7 @@
       <c r="AY2" s="152" t="s">
         <v>431</v>
       </c>
-      <c r="AZ2" s="250" t="s">
+      <c r="AZ2" s="245" t="s">
         <v>430</v>
       </c>
       <c r="BA2" s="151" t="s">
@@ -7648,7 +7768,7 @@
       <c r="BI2" s="151" t="s">
         <v>429</v>
       </c>
-      <c r="BJ2" s="250" t="s">
+      <c r="BJ2" s="245" t="s">
         <v>428</v>
       </c>
       <c r="BK2"/>
@@ -7663,7 +7783,7 @@
       <c r="G3" s="155" t="s">
         <v>427</v>
       </c>
-      <c r="H3" s="250"/>
+      <c r="H3" s="245"/>
       <c r="I3" s="154" t="s">
         <v>426</v>
       </c>
@@ -7704,7 +7824,7 @@
       <c r="V3" s="154" t="s">
         <v>414</v>
       </c>
-      <c r="W3" s="250"/>
+      <c r="W3" s="245"/>
       <c r="X3" s="150"/>
       <c r="Y3" s="155" t="s">
         <v>413</v>
@@ -7715,7 +7835,7 @@
       <c r="AA3" s="155" t="s">
         <v>411</v>
       </c>
-      <c r="AB3" s="250"/>
+      <c r="AB3" s="245"/>
       <c r="AC3" s="152" t="s">
         <v>410</v>
       </c>
@@ -7743,7 +7863,7 @@
       <c r="AK3" s="152" t="s">
         <v>404</v>
       </c>
-      <c r="AL3" s="250"/>
+      <c r="AL3" s="245"/>
       <c r="AM3" s="152" t="s">
         <v>403</v>
       </c>
@@ -7783,7 +7903,7 @@
       <c r="AY3" s="152" t="s">
         <v>391</v>
       </c>
-      <c r="AZ3" s="250"/>
+      <c r="AZ3" s="245"/>
       <c r="BA3" s="151" t="s">
         <v>390</v>
       </c>
@@ -7811,7 +7931,7 @@
       <c r="BI3" s="151" t="s">
         <v>382</v>
       </c>
-      <c r="BJ3" s="250"/>
+      <c r="BJ3" s="245"/>
     </row>
     <row r="4" spans="1:63" s="112" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="157"/>
@@ -7833,7 +7953,7 @@
       <c r="G4" s="155" t="s">
         <v>377</v>
       </c>
-      <c r="H4" s="250"/>
+      <c r="H4" s="245"/>
       <c r="I4" s="154" t="s">
         <v>376</v>
       </c>
@@ -7876,7 +7996,7 @@
       <c r="V4" s="154" t="s">
         <v>363</v>
       </c>
-      <c r="W4" s="250"/>
+      <c r="W4" s="245"/>
       <c r="X4" s="153" t="s">
         <v>362</v>
       </c>
@@ -7889,7 +8009,7 @@
       <c r="AA4" s="153" t="s">
         <v>359</v>
       </c>
-      <c r="AB4" s="250"/>
+      <c r="AB4" s="245"/>
       <c r="AC4" s="152" t="s">
         <v>358</v>
       </c>
@@ -7917,7 +8037,7 @@
       <c r="AK4" s="152" t="s">
         <v>351</v>
       </c>
-      <c r="AL4" s="250"/>
+      <c r="AL4" s="245"/>
       <c r="AM4" s="152" t="s">
         <v>350</v>
       </c>
@@ -7957,7 +8077,7 @@
       <c r="AY4" s="152" t="s">
         <v>338</v>
       </c>
-      <c r="AZ4" s="250"/>
+      <c r="AZ4" s="245"/>
       <c r="BA4" s="151" t="s">
         <v>337</v>
       </c>
@@ -7985,7 +8105,7 @@
       <c r="BI4" s="151" t="s">
         <v>329</v>
       </c>
-      <c r="BJ4" s="250"/>
+      <c r="BJ4" s="245"/>
       <c r="BK4"/>
     </row>
     <row r="5" spans="1:63" s="112" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -7994,7 +8114,7 @@
       </c>
       <c r="B5" s="132"/>
       <c r="C5" s="132"/>
-      <c r="D5" s="212"/>
+      <c r="D5" s="211"/>
       <c r="E5" s="132" t="s">
         <v>328</v>
       </c>
@@ -8206,7 +8326,7 @@
       </c>
       <c r="B6" s="132"/>
       <c r="C6" s="132"/>
-      <c r="D6" s="213" t="str">
+      <c r="D6" s="212" t="str">
         <f t="shared" ref="D6:D15" si="6">IF(ISBLANK($D$5),"",$D$5)</f>
         <v/>
       </c>
@@ -8420,7 +8540,7 @@
       </c>
       <c r="B7" s="132"/>
       <c r="C7" s="132"/>
-      <c r="D7" s="213" t="str">
+      <c r="D7" s="212" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -8634,7 +8754,7 @@
       </c>
       <c r="B8" s="132"/>
       <c r="C8" s="132"/>
-      <c r="D8" s="213" t="str">
+      <c r="D8" s="212" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -8848,7 +8968,7 @@
       </c>
       <c r="B9" s="132"/>
       <c r="C9" s="132"/>
-      <c r="D9" s="213" t="str">
+      <c r="D9" s="212" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -9062,7 +9182,7 @@
       </c>
       <c r="B10" s="132"/>
       <c r="C10" s="132"/>
-      <c r="D10" s="213" t="str">
+      <c r="D10" s="212" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -9276,7 +9396,7 @@
       </c>
       <c r="B11" s="132"/>
       <c r="C11" s="132"/>
-      <c r="D11" s="213" t="str">
+      <c r="D11" s="212" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -9490,7 +9610,7 @@
       </c>
       <c r="B12" s="132"/>
       <c r="C12" s="132"/>
-      <c r="D12" s="213" t="str">
+      <c r="D12" s="212" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -9704,7 +9824,7 @@
       </c>
       <c r="B13" s="132"/>
       <c r="C13" s="132"/>
-      <c r="D13" s="213" t="str">
+      <c r="D13" s="212" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -9918,7 +10038,7 @@
       </c>
       <c r="B14" s="132"/>
       <c r="C14" s="132"/>
-      <c r="D14" s="213" t="str">
+      <c r="D14" s="212" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -10132,7 +10252,7 @@
       </c>
       <c r="B15" s="132"/>
       <c r="C15" s="132"/>
-      <c r="D15" s="213" t="str">
+      <c r="D15" s="212" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -10574,97 +10694,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:62" s="112" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="116"/>
-      <c r="B17" s="115"/>
-      <c r="C17" s="115"/>
-      <c r="D17" s="115"/>
-      <c r="E17" s="115"/>
-      <c r="F17" s="114"/>
-      <c r="G17" s="113"/>
-      <c r="H17" s="113"/>
-      <c r="I17" s="113"/>
-      <c r="J17" s="113"/>
-      <c r="K17" s="113"/>
-      <c r="L17" s="113"/>
-      <c r="M17" s="113"/>
-      <c r="N17" s="113"/>
-      <c r="O17" s="113"/>
-      <c r="P17" s="113"/>
-      <c r="Q17" s="113"/>
-      <c r="R17" s="113"/>
-      <c r="S17" s="113"/>
-      <c r="T17" s="113"/>
-      <c r="U17" s="113"/>
-      <c r="V17" s="113"/>
-      <c r="W17" s="113"/>
-      <c r="X17" s="113"/>
-      <c r="Y17" s="113"/>
-      <c r="Z17" s="113"/>
-      <c r="AA17" s="113"/>
-      <c r="AB17" s="113"/>
-      <c r="AC17" s="113"/>
-      <c r="AD17" s="113"/>
-      <c r="AE17" s="113"/>
-      <c r="AF17" s="113"/>
-      <c r="AG17" s="113"/>
-      <c r="AH17" s="113"/>
-      <c r="AI17" s="113"/>
-      <c r="AJ17" s="113"/>
-      <c r="AK17" s="113"/>
-      <c r="AL17" s="113"/>
-      <c r="AM17" s="113"/>
-      <c r="AN17" s="113"/>
-      <c r="AO17" s="113"/>
-      <c r="AP17" s="113"/>
-      <c r="AQ17" s="113"/>
-      <c r="AR17" s="113"/>
-      <c r="AS17" s="113"/>
-      <c r="AT17" s="113"/>
-      <c r="AU17" s="113"/>
-      <c r="AV17" s="113"/>
-      <c r="AW17" s="113"/>
-      <c r="AX17" s="113"/>
-      <c r="AY17" s="113"/>
-      <c r="AZ17" s="113"/>
-      <c r="BA17" s="113"/>
-      <c r="BB17" s="113"/>
-      <c r="BC17" s="113"/>
-      <c r="BD17" s="113"/>
-      <c r="BE17" s="113"/>
-      <c r="BF17" s="113"/>
-      <c r="BG17" s="113"/>
-      <c r="BH17" s="113"/>
-      <c r="BI17" s="113"/>
-      <c r="BJ17" s="113"/>
-    </row>
-    <row r="18" spans="1:62" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="W18" s="111"/>
-      <c r="AZ18" s="111"/>
-    </row>
-    <row r="19" spans="1:62" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E19" s="253" t="s">
+    <row r="17" spans="4:52" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="W17" s="111"/>
+      <c r="AZ17" s="111"/>
+    </row>
+    <row r="18" spans="4:52" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="258" t="s">
         <v>440</v>
       </c>
-      <c r="F19" s="254"/>
-      <c r="G19" s="254"/>
-      <c r="H19" s="254"/>
-      <c r="I19" s="254"/>
-      <c r="J19" s="254"/>
-      <c r="K19" s="254"/>
-      <c r="L19" s="254"/>
-      <c r="M19" s="255"/>
-    </row>
-    <row r="20" spans="1:62" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="AH22" s="109"/>
-    </row>
-    <row r="23" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="E23" s="110"/>
+      <c r="E18" s="260"/>
+      <c r="F18" s="260"/>
+      <c r="G18" s="260"/>
+      <c r="H18" s="260"/>
+      <c r="I18" s="261"/>
+    </row>
+    <row r="19" spans="4:52" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="4:52" x14ac:dyDescent="0.2">
+      <c r="AH20" s="109"/>
+    </row>
+    <row r="21" spans="4:52" x14ac:dyDescent="0.2">
+      <c r="E21" s="110"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="E19:M19"/>
+  <mergeCells count="6">
     <mergeCell ref="BJ2:BJ4"/>
     <mergeCell ref="H2:H4"/>
     <mergeCell ref="W2:W4"/>
@@ -10680,9 +10732,9 @@
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B695F461-4586-D34F-8E14-1071CB20CB72}">
   <sheetPr codeName="Feuil15">
-    <tabColor rgb="FFFFC000"/>
+    <tabColor rgb="FFF7EF2D"/>
   </sheetPr>
-  <dimension ref="A1:BJ23"/>
+  <dimension ref="A1:BJ21"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
@@ -10774,7 +10826,7 @@
       <c r="G2" s="155" t="s">
         <v>438</v>
       </c>
-      <c r="H2" s="250" t="s">
+      <c r="H2" s="245" t="s">
         <v>437</v>
       </c>
       <c r="I2" s="155" t="s">
@@ -10807,13 +10859,13 @@
       <c r="R2" s="155" t="s">
         <v>436</v>
       </c>
-      <c r="S2" s="250" t="s">
+      <c r="S2" s="245" t="s">
         <v>435</v>
       </c>
       <c r="T2" s="155" t="s">
         <v>152</v>
       </c>
-      <c r="U2" s="250" t="s">
+      <c r="U2" s="245" t="s">
         <v>434</v>
       </c>
       <c r="V2" s="155" t="s">
@@ -10843,7 +10895,7 @@
       <c r="AD2" s="155" t="s">
         <v>433</v>
       </c>
-      <c r="AE2" s="250" t="s">
+      <c r="AE2" s="245" t="s">
         <v>482</v>
       </c>
       <c r="AF2" s="155" t="s">
@@ -10855,7 +10907,7 @@
       <c r="AH2" s="155" t="s">
         <v>481</v>
       </c>
-      <c r="AI2" s="250" t="s">
+      <c r="AI2" s="245" t="s">
         <v>480</v>
       </c>
     </row>
@@ -10869,7 +10921,7 @@
       <c r="G3" s="155" t="s">
         <v>427</v>
       </c>
-      <c r="H3" s="250"/>
+      <c r="H3" s="245"/>
       <c r="I3" s="155" t="s">
         <v>479</v>
       </c>
@@ -10900,11 +10952,11 @@
       <c r="R3" s="155" t="s">
         <v>414</v>
       </c>
-      <c r="S3" s="250"/>
+      <c r="S3" s="245"/>
       <c r="T3" s="155" t="s">
         <v>411</v>
       </c>
-      <c r="U3" s="250"/>
+      <c r="U3" s="245"/>
       <c r="V3" s="155" t="s">
         <v>470</v>
       </c>
@@ -10932,7 +10984,7 @@
       <c r="AD3" s="155" t="s">
         <v>462</v>
       </c>
-      <c r="AE3" s="250"/>
+      <c r="AE3" s="245"/>
       <c r="AF3" s="155" t="s">
         <v>461</v>
       </c>
@@ -10942,7 +10994,7 @@
       <c r="AH3" s="155" t="s">
         <v>391</v>
       </c>
-      <c r="AI3" s="250"/>
+      <c r="AI3" s="245"/>
     </row>
     <row r="4" spans="1:62" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="158"/>
@@ -10964,7 +11016,7 @@
       <c r="G4" s="155" t="s">
         <v>377</v>
       </c>
-      <c r="H4" s="250"/>
+      <c r="H4" s="245"/>
       <c r="I4" s="155" t="s">
         <v>460</v>
       </c>
@@ -10995,11 +11047,11 @@
       <c r="R4" s="155" t="s">
         <v>363</v>
       </c>
-      <c r="S4" s="250"/>
+      <c r="S4" s="245"/>
       <c r="T4" s="155" t="s">
         <v>359</v>
       </c>
-      <c r="U4" s="250"/>
+      <c r="U4" s="245"/>
       <c r="V4" s="155" t="s">
         <v>451</v>
       </c>
@@ -11027,7 +11079,7 @@
       <c r="AD4" s="155" t="s">
         <v>443</v>
       </c>
-      <c r="AE4" s="250"/>
+      <c r="AE4" s="245"/>
       <c r="AF4" s="155" t="s">
         <v>442</v>
       </c>
@@ -11037,7 +11089,7 @@
       <c r="AH4" s="155" t="s">
         <v>338</v>
       </c>
-      <c r="AI4" s="250"/>
+      <c r="AI4" s="245"/>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A5" s="161" t="s">
@@ -12625,45 +12677,46 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="5:19" x14ac:dyDescent="0.2">
+    <row r="17" spans="4:19" x14ac:dyDescent="0.2">
       <c r="S17" s="111"/>
     </row>
-    <row r="18" spans="5:19" ht="21" x14ac:dyDescent="0.25">
-      <c r="E18" s="256" t="s">
-        <v>517</v>
-      </c>
-      <c r="F18" s="257"/>
-      <c r="G18" s="257"/>
-      <c r="H18" s="257"/>
-      <c r="I18" s="257"/>
-      <c r="J18" s="257"/>
-      <c r="K18" s="257"/>
-      <c r="L18" s="257"/>
-      <c r="M18" s="257"/>
-    </row>
-    <row r="19" spans="5:19" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="5:19" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E20" s="253" t="s">
+    <row r="18" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="D18" s="255" t="s">
+        <v>520</v>
+      </c>
+      <c r="E18" s="256"/>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18"/>
+      <c r="K18"/>
+    </row>
+    <row r="19" spans="4:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="257"/>
+      <c r="E19" s="256"/>
+      <c r="F19" s="256"/>
+      <c r="G19" s="256"/>
+      <c r="H19" s="256"/>
+      <c r="I19" s="256"/>
+      <c r="J19" s="256"/>
+      <c r="K19" s="256"/>
+    </row>
+    <row r="20" spans="4:19" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="258" t="s">
         <v>440</v>
       </c>
-      <c r="F20" s="254"/>
-      <c r="G20" s="254"/>
-      <c r="H20" s="254"/>
-      <c r="I20" s="254"/>
-      <c r="J20" s="254"/>
-      <c r="K20" s="254"/>
-      <c r="L20" s="254"/>
-      <c r="M20" s="254"/>
-      <c r="N20" s="210"/>
-    </row>
-    <row r="21" spans="5:19" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="5:19" x14ac:dyDescent="0.2">
-      <c r="F23" s="110"/>
-    </row>
+      <c r="E20" s="259"/>
+      <c r="F20" s="260"/>
+      <c r="G20" s="260"/>
+      <c r="H20" s="260"/>
+      <c r="I20" s="260"/>
+      <c r="J20" s="261"/>
+      <c r="K20" s="4"/>
+    </row>
+    <row r="21" spans="4:19" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="E18:M18"/>
-    <mergeCell ref="E20:M20"/>
+  <mergeCells count="5">
     <mergeCell ref="AI2:AI4"/>
     <mergeCell ref="H2:H4"/>
     <mergeCell ref="S2:S4"/>
@@ -12678,7 +12731,7 @@
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70C2B6A9-5FC7-3A43-BF37-0B81E3F33F51}">
   <sheetPr codeName="Feuil16">
-    <tabColor rgb="FF92D050"/>
+    <tabColor rgb="FF01A94F"/>
   </sheetPr>
   <dimension ref="A1:BJ17"/>
   <sheetViews>
@@ -12773,13 +12826,13 @@
       <c r="G2" s="155" t="s">
         <v>436</v>
       </c>
-      <c r="H2" s="250" t="s">
+      <c r="H2" s="245" t="s">
         <v>435</v>
       </c>
       <c r="I2" s="155" t="s">
         <v>152</v>
       </c>
-      <c r="J2" s="250" t="s">
+      <c r="J2" s="245" t="s">
         <v>434</v>
       </c>
     </row>
@@ -12793,11 +12846,11 @@
       <c r="G3" s="155" t="s">
         <v>414</v>
       </c>
-      <c r="H3" s="250"/>
+      <c r="H3" s="245"/>
       <c r="I3" s="155" t="s">
         <v>411</v>
       </c>
-      <c r="J3" s="250"/>
+      <c r="J3" s="245"/>
     </row>
     <row r="4" spans="1:62" ht="36" x14ac:dyDescent="0.2">
       <c r="A4" s="177"/>
@@ -12819,11 +12872,11 @@
       <c r="G4" s="155" t="s">
         <v>363</v>
       </c>
-      <c r="H4" s="250"/>
+      <c r="H4" s="245"/>
       <c r="I4" s="155" t="s">
         <v>359</v>
       </c>
-      <c r="J4" s="250"/>
+      <c r="J4" s="245"/>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A5" s="171" t="s">
@@ -13146,29 +13199,29 @@
       </c>
     </row>
     <row r="16" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="E16" s="258" t="s">
-        <v>516</v>
-      </c>
-      <c r="F16" s="259"/>
-      <c r="G16" s="259"/>
-      <c r="H16" s="259"/>
-      <c r="I16" s="259"/>
-      <c r="J16" s="259"/>
+      <c r="D16" s="255" t="s">
+        <v>519</v>
+      </c>
+      <c r="E16" s="256"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
     </row>
     <row r="17" spans="4:10" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D17" s="110"/>
-      <c r="E17" s="259"/>
-      <c r="F17" s="259"/>
-      <c r="G17" s="259"/>
-      <c r="H17" s="259"/>
-      <c r="I17" s="259"/>
-      <c r="J17" s="259"/>
+      <c r="D17" s="254"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="H2:H4"/>
     <mergeCell ref="J2:J4"/>
-    <mergeCell ref="E16:J17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -13178,12 +13231,12 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3674A8A-13E9-4EDB-B294-D1FF8F18362C}">
   <sheetPr codeName="Feuil4">
-    <tabColor theme="0"/>
+    <tabColor rgb="FFCE4275"/>
   </sheetPr>
   <dimension ref="A1:DN8"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+      <selection activeCell="A138" sqref="A138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13502,7 +13555,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B89445B-6ECC-4440-B85C-E593AE209933}">
   <sheetPr codeName="Feuil13">
-    <tabColor theme="0"/>
+    <tabColor rgb="FF2C45E0"/>
   </sheetPr>
   <dimension ref="A1:EF4"/>
   <sheetViews>
@@ -13541,14 +13594,14 @@
       <c r="H1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="EA1" s="244" t="s">
+      <c r="EA1" s="239" t="s">
         <v>492</v>
       </c>
-      <c r="EB1" s="244"/>
-      <c r="EC1" s="244"/>
-      <c r="ED1" s="244"/>
-      <c r="EE1" s="244"/>
-      <c r="EF1" s="244"/>
+      <c r="EB1" s="239"/>
+      <c r="EC1" s="239"/>
+      <c r="ED1" s="239"/>
+      <c r="EE1" s="239"/>
+      <c r="EF1" s="239"/>
     </row>
     <row r="2" spans="1:136" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
@@ -13604,7 +13657,7 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E893F90-1EC7-764C-B747-7920FCEC73CB}">
   <sheetPr codeName="Feuil18">
-    <tabColor theme="2" tint="-9.9978637043366805E-2"/>
+    <tabColor rgb="FF0B0B97"/>
   </sheetPr>
   <dimension ref="A1:P7"/>
   <sheetViews>
@@ -13630,7 +13683,7 @@
     <row r="1" spans="1:16" s="4" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="5"/>
-      <c r="C1" s="211" t="s">
+      <c r="C1" s="210" t="s">
         <v>507</v>
       </c>
       <c r="D1" s="7"/>
@@ -13675,20 +13728,20 @@
     </row>
     <row r="4" spans="1:16" ht="40" x14ac:dyDescent="0.2">
       <c r="C4" s="9"/>
-      <c r="E4" s="245" t="s">
+      <c r="E4" s="240" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="246"/>
-      <c r="G4" s="246"/>
-      <c r="H4" s="246"/>
-      <c r="I4" s="247"/>
-      <c r="J4" s="245" t="s">
+      <c r="F4" s="241"/>
+      <c r="G4" s="241"/>
+      <c r="H4" s="241"/>
+      <c r="I4" s="242"/>
+      <c r="J4" s="240" t="s">
         <v>28</v>
       </c>
-      <c r="K4" s="246"/>
-      <c r="L4" s="246"/>
-      <c r="M4" s="246"/>
-      <c r="N4" s="247"/>
+      <c r="K4" s="241"/>
+      <c r="L4" s="241"/>
+      <c r="M4" s="241"/>
+      <c r="N4" s="242"/>
       <c r="O4" s="30" t="s">
         <v>29</v>
       </c>
@@ -15308,16 +15361,16 @@
   <sheetData>
     <row r="1" spans="1:62" s="64" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A1" s="107"/>
-      <c r="B1" s="249" t="s">
+      <c r="B1" s="244" t="s">
         <v>439</v>
       </c>
-      <c r="C1" s="249"/>
-      <c r="D1" s="249"/>
-      <c r="E1" s="249"/>
-      <c r="F1" s="249"/>
-      <c r="G1" s="249"/>
-      <c r="H1" s="249"/>
-      <c r="I1" s="249"/>
+      <c r="C1" s="244"/>
+      <c r="D1" s="244"/>
+      <c r="E1" s="244"/>
+      <c r="F1" s="244"/>
+      <c r="G1" s="244"/>
+      <c r="H1" s="244"/>
+      <c r="I1" s="244"/>
       <c r="AC1" s="106"/>
       <c r="AD1" s="106"/>
       <c r="AE1" s="106"/>
@@ -15338,7 +15391,7 @@
       <c r="G2" s="102" t="s">
         <v>438</v>
       </c>
-      <c r="H2" s="248" t="s">
+      <c r="H2" s="243" t="s">
         <v>437</v>
       </c>
       <c r="I2" s="101" t="s">
@@ -15383,7 +15436,7 @@
       <c r="V2" s="101" t="s">
         <v>436</v>
       </c>
-      <c r="W2" s="248" t="s">
+      <c r="W2" s="243" t="s">
         <v>435</v>
       </c>
       <c r="X2" s="102" t="s">
@@ -15398,7 +15451,7 @@
       <c r="AA2" s="102" t="s">
         <v>152</v>
       </c>
-      <c r="AB2" s="248" t="s">
+      <c r="AB2" s="243" t="s">
         <v>434</v>
       </c>
       <c r="AC2" s="98" t="s">
@@ -15428,7 +15481,7 @@
       <c r="AK2" s="98" t="s">
         <v>433</v>
       </c>
-      <c r="AL2" s="248" t="s">
+      <c r="AL2" s="243" t="s">
         <v>432</v>
       </c>
       <c r="AM2" s="98" t="s">
@@ -15470,7 +15523,7 @@
       <c r="AY2" s="98" t="s">
         <v>431</v>
       </c>
-      <c r="AZ2" s="248" t="s">
+      <c r="AZ2" s="243" t="s">
         <v>430</v>
       </c>
       <c r="BA2" s="97" t="s">
@@ -15500,7 +15553,7 @@
       <c r="BI2" s="97" t="s">
         <v>429</v>
       </c>
-      <c r="BJ2" s="248" t="s">
+      <c r="BJ2" s="243" t="s">
         <v>428</v>
       </c>
     </row>
@@ -15514,7 +15567,7 @@
       <c r="G3" s="102" t="s">
         <v>427</v>
       </c>
-      <c r="H3" s="248"/>
+      <c r="H3" s="243"/>
       <c r="I3" s="101" t="s">
         <v>426</v>
       </c>
@@ -15555,7 +15608,7 @@
       <c r="V3" s="101" t="s">
         <v>414</v>
       </c>
-      <c r="W3" s="248"/>
+      <c r="W3" s="243"/>
       <c r="X3" s="96"/>
       <c r="Y3" s="102" t="s">
         <v>413</v>
@@ -15566,7 +15619,7 @@
       <c r="AA3" s="102" t="s">
         <v>411</v>
       </c>
-      <c r="AB3" s="248"/>
+      <c r="AB3" s="243"/>
       <c r="AC3" s="98" t="s">
         <v>410</v>
       </c>
@@ -15594,7 +15647,7 @@
       <c r="AK3" s="98" t="s">
         <v>404</v>
       </c>
-      <c r="AL3" s="248"/>
+      <c r="AL3" s="243"/>
       <c r="AM3" s="98" t="s">
         <v>403</v>
       </c>
@@ -15634,7 +15687,7 @@
       <c r="AY3" s="98" t="s">
         <v>391</v>
       </c>
-      <c r="AZ3" s="248"/>
+      <c r="AZ3" s="243"/>
       <c r="BA3" s="97" t="s">
         <v>390</v>
       </c>
@@ -15662,7 +15715,7 @@
       <c r="BI3" s="97" t="s">
         <v>382</v>
       </c>
-      <c r="BJ3" s="248"/>
+      <c r="BJ3" s="243"/>
     </row>
     <row r="4" spans="1:62" s="64" customFormat="1" ht="60" x14ac:dyDescent="0.15">
       <c r="A4" s="104"/>
@@ -15684,7 +15737,7 @@
       <c r="G4" s="102" t="s">
         <v>377</v>
       </c>
-      <c r="H4" s="248"/>
+      <c r="H4" s="243"/>
       <c r="I4" s="101" t="s">
         <v>376</v>
       </c>
@@ -15727,7 +15780,7 @@
       <c r="V4" s="100" t="s">
         <v>363</v>
       </c>
-      <c r="W4" s="248"/>
+      <c r="W4" s="243"/>
       <c r="X4" s="99" t="s">
         <v>362</v>
       </c>
@@ -15740,7 +15793,7 @@
       <c r="AA4" s="99" t="s">
         <v>359</v>
       </c>
-      <c r="AB4" s="248"/>
+      <c r="AB4" s="243"/>
       <c r="AC4" s="98" t="s">
         <v>358</v>
       </c>
@@ -15768,7 +15821,7 @@
       <c r="AK4" s="98" t="s">
         <v>351</v>
       </c>
-      <c r="AL4" s="248"/>
+      <c r="AL4" s="243"/>
       <c r="AM4" s="98" t="s">
         <v>350</v>
       </c>
@@ -15808,7 +15861,7 @@
       <c r="AY4" s="98" t="s">
         <v>338</v>
       </c>
-      <c r="AZ4" s="248"/>
+      <c r="AZ4" s="243"/>
       <c r="BA4" s="97" t="s">
         <v>337</v>
       </c>
@@ -15836,7 +15889,7 @@
       <c r="BI4" s="97" t="s">
         <v>329</v>
       </c>
-      <c r="BJ4" s="248"/>
+      <c r="BJ4" s="243"/>
     </row>
     <row r="5" spans="1:62" s="64" customFormat="1" ht="144" x14ac:dyDescent="0.15">
       <c r="A5" s="72" t="s">
@@ -17535,16 +17588,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" s="112" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B1" s="251" t="s">
+      <c r="B1" s="246" t="s">
         <v>439</v>
       </c>
-      <c r="C1" s="251"/>
-      <c r="D1" s="251"/>
-      <c r="E1" s="251"/>
-      <c r="F1" s="251"/>
-      <c r="G1" s="251"/>
-      <c r="H1" s="251"/>
-      <c r="I1" s="251"/>
+      <c r="C1" s="246"/>
+      <c r="D1" s="246"/>
+      <c r="E1" s="246"/>
+      <c r="F1" s="246"/>
+      <c r="G1" s="246"/>
+      <c r="H1" s="246"/>
+      <c r="I1" s="246"/>
     </row>
     <row r="2" spans="1:62" s="112" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="158"/>
@@ -17556,7 +17609,7 @@
       <c r="G2" s="155" t="s">
         <v>438</v>
       </c>
-      <c r="H2" s="250" t="s">
+      <c r="H2" s="245" t="s">
         <v>437</v>
       </c>
       <c r="I2" s="154" t="s">
@@ -17601,7 +17654,7 @@
       <c r="V2" s="154" t="s">
         <v>436</v>
       </c>
-      <c r="W2" s="250" t="s">
+      <c r="W2" s="245" t="s">
         <v>435</v>
       </c>
       <c r="X2" s="155" t="s">
@@ -17616,7 +17669,7 @@
       <c r="AA2" s="155" t="s">
         <v>152</v>
       </c>
-      <c r="AB2" s="250" t="s">
+      <c r="AB2" s="245" t="s">
         <v>434</v>
       </c>
       <c r="AC2" s="152" t="s">
@@ -17646,7 +17699,7 @@
       <c r="AK2" s="152" t="s">
         <v>433</v>
       </c>
-      <c r="AL2" s="250" t="s">
+      <c r="AL2" s="245" t="s">
         <v>432</v>
       </c>
       <c r="AM2" s="152" t="s">
@@ -17688,7 +17741,7 @@
       <c r="AY2" s="152" t="s">
         <v>431</v>
       </c>
-      <c r="AZ2" s="250" t="s">
+      <c r="AZ2" s="245" t="s">
         <v>430</v>
       </c>
       <c r="BA2" s="151" t="s">
@@ -17718,7 +17771,7 @@
       <c r="BI2" s="151" t="s">
         <v>429</v>
       </c>
-      <c r="BJ2" s="250" t="s">
+      <c r="BJ2" s="245" t="s">
         <v>428</v>
       </c>
     </row>
@@ -17732,7 +17785,7 @@
       <c r="G3" s="155" t="s">
         <v>427</v>
       </c>
-      <c r="H3" s="250"/>
+      <c r="H3" s="245"/>
       <c r="I3" s="154" t="s">
         <v>426</v>
       </c>
@@ -17773,7 +17826,7 @@
       <c r="V3" s="154" t="s">
         <v>414</v>
       </c>
-      <c r="W3" s="250"/>
+      <c r="W3" s="245"/>
       <c r="X3" s="150"/>
       <c r="Y3" s="155" t="s">
         <v>413</v>
@@ -17784,7 +17837,7 @@
       <c r="AA3" s="155" t="s">
         <v>411</v>
       </c>
-      <c r="AB3" s="250"/>
+      <c r="AB3" s="245"/>
       <c r="AC3" s="152" t="s">
         <v>410</v>
       </c>
@@ -17812,7 +17865,7 @@
       <c r="AK3" s="152" t="s">
         <v>404</v>
       </c>
-      <c r="AL3" s="250"/>
+      <c r="AL3" s="245"/>
       <c r="AM3" s="152" t="s">
         <v>403</v>
       </c>
@@ -17852,7 +17905,7 @@
       <c r="AY3" s="152" t="s">
         <v>391</v>
       </c>
-      <c r="AZ3" s="250"/>
+      <c r="AZ3" s="245"/>
       <c r="BA3" s="151" t="s">
         <v>390</v>
       </c>
@@ -17880,7 +17933,7 @@
       <c r="BI3" s="151" t="s">
         <v>382</v>
       </c>
-      <c r="BJ3" s="250"/>
+      <c r="BJ3" s="245"/>
     </row>
     <row r="4" spans="1:62" s="112" customFormat="1" ht="60" x14ac:dyDescent="0.15">
       <c r="A4" s="157"/>
@@ -17902,7 +17955,7 @@
       <c r="G4" s="155" t="s">
         <v>377</v>
       </c>
-      <c r="H4" s="250"/>
+      <c r="H4" s="245"/>
       <c r="I4" s="154" t="s">
         <v>376</v>
       </c>
@@ -17945,7 +17998,7 @@
       <c r="V4" s="154" t="s">
         <v>363</v>
       </c>
-      <c r="W4" s="250"/>
+      <c r="W4" s="245"/>
       <c r="X4" s="153" t="s">
         <v>362</v>
       </c>
@@ -17958,7 +18011,7 @@
       <c r="AA4" s="153" t="s">
         <v>359</v>
       </c>
-      <c r="AB4" s="250"/>
+      <c r="AB4" s="245"/>
       <c r="AC4" s="152" t="s">
         <v>358</v>
       </c>
@@ -17986,7 +18039,7 @@
       <c r="AK4" s="152" t="s">
         <v>351</v>
       </c>
-      <c r="AL4" s="250"/>
+      <c r="AL4" s="245"/>
       <c r="AM4" s="152" t="s">
         <v>350</v>
       </c>
@@ -18026,7 +18079,7 @@
       <c r="AY4" s="152" t="s">
         <v>338</v>
       </c>
-      <c r="AZ4" s="250"/>
+      <c r="AZ4" s="245"/>
       <c r="BA4" s="151" t="s">
         <v>337</v>
       </c>
@@ -18054,7 +18107,7 @@
       <c r="BI4" s="151" t="s">
         <v>329</v>
       </c>
-      <c r="BJ4" s="250"/>
+      <c r="BJ4" s="245"/>
     </row>
     <row r="5" spans="1:62" s="112" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="122" t="s">

</xml_diff>

<commit_message>
add JA VIF extractor
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96EFCC9-952B-9C47-8418-74278CEBA416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747CEEAA-2D6B-7D4C-8FEC-C5ACAC0255E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="600" windowWidth="22940" windowHeight="13240" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
@@ -31,7 +31,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ETPT A-JUST'!$A$2:$DN$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ETPT Format DDG'!$A$2:$DT$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Table_Fonctions!$A$1:$F$65</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Table_Fonctions!$A$1:$F$66</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1623" uniqueCount="520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1629" uniqueCount="521">
   <si>
     <t>#! END_ROW</t>
   </si>
@@ -2771,6 +2771,9 @@
   </si>
   <si>
     <t>JA JP</t>
+  </si>
+  <si>
+    <t>JA VIF</t>
   </si>
 </sst>
 </file>
@@ -13980,9 +13983,9 @@
   <sheetPr codeName="Feuil14">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView topLeftCell="B49" zoomScale="125" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="B48" zoomScale="125" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
@@ -15252,7 +15255,7 @@
         <v>143</v>
       </c>
       <c r="C63" s="48" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="D63" s="48" t="s">
         <v>137</v>
@@ -15263,51 +15266,72 @@
       <c r="F63" s="48" t="s">
         <v>132</v>
       </c>
+      <c r="G63" s="42"/>
     </row>
     <row r="64" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="47" t="s">
+      <c r="A64" s="49" t="s">
         <v>140</v>
       </c>
-      <c r="B64" s="42" t="s">
+      <c r="B64" s="48" t="s">
+        <v>143</v>
+      </c>
+      <c r="C64" s="48" t="s">
+        <v>519</v>
+      </c>
+      <c r="D64" s="48" t="s">
+        <v>137</v>
+      </c>
+      <c r="E64" s="48" t="s">
+        <v>109</v>
+      </c>
+      <c r="F64" s="48" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="47" t="s">
+        <v>140</v>
+      </c>
+      <c r="B65" s="42" t="s">
         <v>142</v>
       </c>
-      <c r="C64" s="42" t="s">
+      <c r="C65" s="42" t="s">
         <v>141</v>
       </c>
-      <c r="D64" s="42" t="s">
+      <c r="D65" s="42" t="s">
         <v>137</v>
       </c>
-      <c r="E64" s="42" t="s">
+      <c r="E65" s="42" t="s">
         <v>109</v>
       </c>
-      <c r="F64" s="46"/>
-      <c r="G64" s="42" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="45" t="s">
-        <v>140</v>
-      </c>
-      <c r="B65" s="44" t="s">
-        <v>139</v>
-      </c>
-      <c r="C65" s="44" t="s">
-        <v>138</v>
-      </c>
-      <c r="D65" s="44" t="s">
-        <v>137</v>
-      </c>
-      <c r="E65" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="F65" s="43"/>
+      <c r="F65" s="46"/>
       <c r="G65" s="42" t="s">
         <v>136</v>
       </c>
     </row>
+    <row r="66" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="45" t="s">
+        <v>140</v>
+      </c>
+      <c r="B66" s="44" t="s">
+        <v>139</v>
+      </c>
+      <c r="C66" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="D66" s="44" t="s">
+        <v>137</v>
+      </c>
+      <c r="E66" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="F66" s="43"/>
+      <c r="G66" s="42" t="s">
+        <v>136</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F65" xr:uid="{00000000-0001-0000-0300-000000000000}"/>
+  <autoFilter ref="A1:F66" xr:uid="{00000000-0001-0000-0300-000000000000}"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" scale="74" orientation="landscape" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
DDG ajout cont a jp autour du juge
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7161F2AA-EFD1-F948-B7A2-01F41596DC86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31930DC9-534D-2849-8A1A-BC0A9312649C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="22940" windowHeight="13240" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
@@ -31,7 +31,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ETPT A-JUST'!$A$2:$DN$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ETPT Format DDG'!$A$2:$DT$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Table_Fonctions!$A$1:$F$66</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Table_Fonctions!$A$1:$F$67</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1629" uniqueCount="520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1635" uniqueCount="521">
   <si>
     <t>#! END_ROW</t>
   </si>
@@ -2771,6 +2771,9 @@
   </si>
   <si>
     <t>CONT C JP Greffe</t>
+  </si>
+  <si>
+    <t>CONT A JP Autour du magistrat</t>
   </si>
 </sst>
 </file>
@@ -13980,10 +13983,10 @@
   <sheetPr codeName="Feuil14">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G66"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView topLeftCell="B45" zoomScale="125" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView topLeftCell="B49" zoomScale="125" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15286,49 +15289,69 @@
       </c>
     </row>
     <row r="65" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="47" t="s">
+      <c r="A65" s="49" t="s">
         <v>137</v>
       </c>
-      <c r="B65" s="42" t="s">
+      <c r="B65" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="C65" s="48" t="s">
+        <v>520</v>
+      </c>
+      <c r="D65" s="48" t="s">
+        <v>134</v>
+      </c>
+      <c r="E65" s="48" t="s">
+        <v>109</v>
+      </c>
+      <c r="F65" s="48" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="47" t="s">
+        <v>137</v>
+      </c>
+      <c r="B66" s="42" t="s">
         <v>139</v>
       </c>
-      <c r="C65" s="42" t="s">
+      <c r="C66" s="42" t="s">
         <v>138</v>
       </c>
-      <c r="D65" s="42" t="s">
+      <c r="D66" s="42" t="s">
         <v>134</v>
       </c>
-      <c r="E65" s="42" t="s">
+      <c r="E66" s="42" t="s">
         <v>109</v>
       </c>
-      <c r="F65" s="46"/>
-      <c r="G65" s="42" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="45" t="s">
-        <v>137</v>
-      </c>
-      <c r="B66" s="44" t="s">
-        <v>136</v>
-      </c>
-      <c r="C66" s="44" t="s">
-        <v>135</v>
-      </c>
-      <c r="D66" s="44" t="s">
-        <v>134</v>
-      </c>
-      <c r="E66" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="F66" s="43"/>
+      <c r="F66" s="46"/>
       <c r="G66" s="42" t="s">
         <v>133</v>
       </c>
     </row>
+    <row r="67" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="45" t="s">
+        <v>137</v>
+      </c>
+      <c r="B67" s="44" t="s">
+        <v>136</v>
+      </c>
+      <c r="C67" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="D67" s="44" t="s">
+        <v>134</v>
+      </c>
+      <c r="E67" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="F67" s="43"/>
+      <c r="G67" s="42" t="s">
+        <v>133</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F66" xr:uid="{00000000-0001-0000-0300-000000000000}"/>
+  <autoFilter ref="A1:F67" xr:uid="{00000000-0001-0000-0300-000000000000}"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" scale="74" orientation="landscape" r:id="rId1"/>
 </worksheet>
@@ -16882,7 +16905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:62" s="64" customFormat="1" ht="36" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:62" s="64" customFormat="1" ht="48" x14ac:dyDescent="0.15">
       <c r="A13" s="72" t="s">
         <v>228</v>
       </c>

</xml_diff>

<commit_message>
DDG add cont a jp autour du magistrat
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C175DC4F-D524-694E-A1E8-046EB5A40464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FFF230F-D554-BF4B-801A-5BCCA5A7E477}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="600" windowWidth="22940" windowHeight="13240" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
@@ -31,7 +31,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ETPT A-JUST'!$A$2:$DN$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ETPT Format DDG'!$A$2:$DT$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Table_Fonctions!$A$1:$F$66</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Table_Fonctions!$A$1:$F$67</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1629" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1635" uniqueCount="523">
   <si>
     <t>#! END_ROW</t>
   </si>
@@ -2777,6 +2777,9 @@
   </si>
   <si>
     <t>JA VIF</t>
+  </si>
+  <si>
+    <t>CONT A JP Autour du magistrat</t>
   </si>
 </sst>
 </file>
@@ -4592,6 +4595,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="40" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4678,12 +4687,6 @@
     <xf numFmtId="0" fontId="31" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -5166,9 +5169,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -5206,7 +5209,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -5312,7 +5315,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5454,7 +5457,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5488,11 +5491,11 @@
       <c r="B1" s="197" t="s">
         <v>492</v>
       </c>
-      <c r="C1" s="233" t="s">
+      <c r="C1" s="235" t="s">
         <v>493</v>
       </c>
-      <c r="D1" s="233"/>
-      <c r="E1" s="233"/>
+      <c r="D1" s="235"/>
+      <c r="E1" s="235"/>
       <c r="F1" s="198"/>
       <c r="H1" s="28" t="s">
         <v>0</v>
@@ -5501,11 +5504,11 @@
     <row r="2" spans="1:8" s="202" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="199"/>
       <c r="B2" s="200"/>
-      <c r="C2" s="234" t="s">
+      <c r="C2" s="236" t="s">
         <v>494</v>
       </c>
-      <c r="D2" s="234"/>
-      <c r="E2" s="234"/>
+      <c r="D2" s="236"/>
+      <c r="E2" s="236"/>
       <c r="F2" s="201"/>
       <c r="H2" s="28" t="s">
         <v>0</v>
@@ -5529,10 +5532,10 @@
       <c r="D4" s="207" t="s">
         <v>497</v>
       </c>
-      <c r="E4" s="240" t="s">
+      <c r="E4" s="242" t="s">
         <v>498</v>
       </c>
-      <c r="F4" s="241"/>
+      <c r="F4" s="243"/>
       <c r="G4" s="216"/>
       <c r="H4" s="28" t="s">
         <v>0</v>
@@ -5549,10 +5552,10 @@
       <c r="D5" s="213" t="s">
         <v>501</v>
       </c>
-      <c r="E5" s="242" t="s">
+      <c r="E5" s="244" t="s">
         <v>514</v>
       </c>
-      <c r="F5" s="243"/>
+      <c r="F5" s="245"/>
       <c r="G5" s="215"/>
       <c r="H5" s="28" t="s">
         <v>0</v>
@@ -5569,10 +5572,10 @@
       <c r="D6" s="214" t="s">
         <v>504</v>
       </c>
-      <c r="E6" s="244" t="s">
+      <c r="E6" s="246" t="s">
         <v>515</v>
       </c>
-      <c r="F6" s="245"/>
+      <c r="F6" s="247"/>
       <c r="G6" s="215"/>
       <c r="H6" s="28" t="s">
         <v>0</v>
@@ -5589,10 +5592,10 @@
       <c r="D7" s="214" t="s">
         <v>507</v>
       </c>
-      <c r="E7" s="244" t="s">
+      <c r="E7" s="246" t="s">
         <v>514</v>
       </c>
-      <c r="F7" s="245"/>
+      <c r="F7" s="247"/>
       <c r="G7" s="215"/>
       <c r="H7" s="28" t="s">
         <v>0</v>
@@ -5603,16 +5606,16 @@
       <c r="B8" s="223" t="s">
         <v>508</v>
       </c>
-      <c r="C8" s="235" t="s">
+      <c r="C8" s="237" t="s">
         <v>509</v>
       </c>
-      <c r="D8" s="235" t="s">
+      <c r="D8" s="237" t="s">
         <v>510</v>
       </c>
-      <c r="E8" s="246" t="s">
+      <c r="E8" s="248" t="s">
         <v>516</v>
       </c>
-      <c r="F8" s="247"/>
+      <c r="F8" s="249"/>
       <c r="G8" s="215"/>
       <c r="H8" s="28" t="s">
         <v>0</v>
@@ -5623,10 +5626,10 @@
       <c r="B9" s="224" t="s">
         <v>511</v>
       </c>
-      <c r="C9" s="235"/>
-      <c r="D9" s="235"/>
-      <c r="E9" s="248"/>
-      <c r="F9" s="249"/>
+      <c r="C9" s="237"/>
+      <c r="D9" s="237"/>
+      <c r="E9" s="250"/>
+      <c r="F9" s="251"/>
       <c r="G9" s="215"/>
       <c r="H9" s="28" t="s">
         <v>0</v>
@@ -5637,10 +5640,10 @@
       <c r="B10" s="225" t="s">
         <v>512</v>
       </c>
-      <c r="C10" s="236"/>
-      <c r="D10" s="236"/>
-      <c r="E10" s="250"/>
-      <c r="F10" s="251"/>
+      <c r="C10" s="238"/>
+      <c r="D10" s="238"/>
+      <c r="E10" s="252"/>
+      <c r="F10" s="253"/>
       <c r="G10" s="215"/>
       <c r="H10" s="28" t="s">
         <v>0</v>
@@ -5660,11 +5663,11 @@
     <row r="12" spans="1:8" s="28" customFormat="1" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="203"/>
       <c r="B12" s="217"/>
-      <c r="C12" s="239" t="s">
+      <c r="C12" s="241" t="s">
         <v>513</v>
       </c>
-      <c r="D12" s="239"/>
-      <c r="E12" s="239"/>
+      <c r="D12" s="241"/>
+      <c r="E12" s="241"/>
       <c r="F12" s="218"/>
       <c r="H12" s="28" t="s">
         <v>0</v>
@@ -5678,14 +5681,14 @@
       </c>
     </row>
     <row r="14" spans="1:8" s="28" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="237" t="s">
+      <c r="A14" s="239" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="237"/>
-      <c r="C14" s="237"/>
-      <c r="D14" s="237"/>
-      <c r="E14" s="237"/>
-      <c r="F14" s="238"/>
+      <c r="B14" s="239"/>
+      <c r="C14" s="239"/>
+      <c r="D14" s="239"/>
+      <c r="E14" s="239"/>
+      <c r="F14" s="240"/>
       <c r="H14" s="28" t="s">
         <v>0</v>
       </c>
@@ -5738,16 +5741,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A1" s="260" t="s">
+      <c r="A1" s="262" t="s">
         <v>481</v>
       </c>
-      <c r="B1" s="260"/>
-      <c r="C1" s="260"/>
-      <c r="D1" s="260"/>
-      <c r="E1" s="260"/>
-      <c r="F1" s="260"/>
-      <c r="G1" s="260"/>
-      <c r="H1" s="260"/>
+      <c r="B1" s="262"/>
+      <c r="C1" s="262"/>
+      <c r="D1" s="262"/>
+      <c r="E1" s="262"/>
+      <c r="F1" s="262"/>
+      <c r="G1" s="262"/>
+      <c r="H1" s="262"/>
       <c r="I1" s="112"/>
       <c r="J1" s="112"/>
       <c r="K1" s="112"/>
@@ -5786,7 +5789,7 @@
       <c r="G2" s="155" t="s">
         <v>436</v>
       </c>
-      <c r="H2" s="258" t="s">
+      <c r="H2" s="260" t="s">
         <v>435</v>
       </c>
       <c r="I2" s="155" t="s">
@@ -5819,13 +5822,13 @@
       <c r="R2" s="155" t="s">
         <v>434</v>
       </c>
-      <c r="S2" s="258" t="s">
+      <c r="S2" s="260" t="s">
         <v>433</v>
       </c>
       <c r="T2" s="155" t="s">
         <v>150</v>
       </c>
-      <c r="U2" s="258" t="s">
+      <c r="U2" s="260" t="s">
         <v>432</v>
       </c>
       <c r="V2" s="155" t="s">
@@ -5855,7 +5858,7 @@
       <c r="AD2" s="155" t="s">
         <v>431</v>
       </c>
-      <c r="AE2" s="258" t="s">
+      <c r="AE2" s="260" t="s">
         <v>480</v>
       </c>
       <c r="AF2" s="155" t="s">
@@ -5867,7 +5870,7 @@
       <c r="AH2" s="155" t="s">
         <v>479</v>
       </c>
-      <c r="AI2" s="258" t="s">
+      <c r="AI2" s="260" t="s">
         <v>478</v>
       </c>
     </row>
@@ -5881,7 +5884,7 @@
       <c r="G3" s="155" t="s">
         <v>425</v>
       </c>
-      <c r="H3" s="258"/>
+      <c r="H3" s="260"/>
       <c r="I3" s="155" t="s">
         <v>477</v>
       </c>
@@ -5912,11 +5915,11 @@
       <c r="R3" s="155" t="s">
         <v>412</v>
       </c>
-      <c r="S3" s="258"/>
+      <c r="S3" s="260"/>
       <c r="T3" s="155" t="s">
         <v>409</v>
       </c>
-      <c r="U3" s="258"/>
+      <c r="U3" s="260"/>
       <c r="V3" s="155" t="s">
         <v>468</v>
       </c>
@@ -5944,7 +5947,7 @@
       <c r="AD3" s="155" t="s">
         <v>460</v>
       </c>
-      <c r="AE3" s="258"/>
+      <c r="AE3" s="260"/>
       <c r="AF3" s="155" t="s">
         <v>459</v>
       </c>
@@ -5954,7 +5957,7 @@
       <c r="AH3" s="155" t="s">
         <v>389</v>
       </c>
-      <c r="AI3" s="258"/>
+      <c r="AI3" s="260"/>
     </row>
     <row r="4" spans="1:35" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="158"/>
@@ -5976,7 +5979,7 @@
       <c r="G4" s="155" t="s">
         <v>375</v>
       </c>
-      <c r="H4" s="258"/>
+      <c r="H4" s="260"/>
       <c r="I4" s="155" t="s">
         <v>458</v>
       </c>
@@ -6007,11 +6010,11 @@
       <c r="R4" s="155" t="s">
         <v>361</v>
       </c>
-      <c r="S4" s="258"/>
+      <c r="S4" s="260"/>
       <c r="T4" s="155" t="s">
         <v>357</v>
       </c>
-      <c r="U4" s="258"/>
+      <c r="U4" s="260"/>
       <c r="V4" s="155" t="s">
         <v>449</v>
       </c>
@@ -6039,7 +6042,7 @@
       <c r="AD4" s="155" t="s">
         <v>441</v>
       </c>
-      <c r="AE4" s="258"/>
+      <c r="AE4" s="260"/>
       <c r="AF4" s="155" t="s">
         <v>440</v>
       </c>
@@ -6049,7 +6052,7 @@
       <c r="AH4" s="155" t="s">
         <v>336</v>
       </c>
-      <c r="AI4" s="258"/>
+      <c r="AI4" s="260"/>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A5" s="161" t="s">
@@ -7158,13 +7161,13 @@
       <c r="G2" s="155" t="s">
         <v>434</v>
       </c>
-      <c r="H2" s="258" t="s">
+      <c r="H2" s="260" t="s">
         <v>433</v>
       </c>
       <c r="I2" s="155" t="s">
         <v>150</v>
       </c>
-      <c r="J2" s="258" t="s">
+      <c r="J2" s="260" t="s">
         <v>432</v>
       </c>
     </row>
@@ -7178,11 +7181,11 @@
       <c r="G3" s="155" t="s">
         <v>412</v>
       </c>
-      <c r="H3" s="258"/>
+      <c r="H3" s="260"/>
       <c r="I3" s="155" t="s">
         <v>409</v>
       </c>
-      <c r="J3" s="258"/>
+      <c r="J3" s="260"/>
     </row>
     <row r="4" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A4" s="177"/>
@@ -7204,11 +7207,11 @@
       <c r="G4" s="155" t="s">
         <v>361</v>
       </c>
-      <c r="H4" s="258"/>
+      <c r="H4" s="260"/>
       <c r="I4" s="155" t="s">
         <v>357</v>
       </c>
-      <c r="J4" s="258"/>
+      <c r="J4" s="260"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="171" t="s">
@@ -7612,7 +7615,7 @@
       <c r="G2" s="155" t="s">
         <v>436</v>
       </c>
-      <c r="H2" s="258" t="s">
+      <c r="H2" s="260" t="s">
         <v>435</v>
       </c>
       <c r="I2" s="154" t="s">
@@ -7657,7 +7660,7 @@
       <c r="V2" s="154" t="s">
         <v>434</v>
       </c>
-      <c r="W2" s="258" t="s">
+      <c r="W2" s="260" t="s">
         <v>433</v>
       </c>
       <c r="X2" s="155" t="s">
@@ -7672,7 +7675,7 @@
       <c r="AA2" s="155" t="s">
         <v>150</v>
       </c>
-      <c r="AB2" s="258" t="s">
+      <c r="AB2" s="260" t="s">
         <v>432</v>
       </c>
       <c r="AC2" s="152" t="s">
@@ -7702,7 +7705,7 @@
       <c r="AK2" s="152" t="s">
         <v>431</v>
       </c>
-      <c r="AL2" s="258" t="s">
+      <c r="AL2" s="260" t="s">
         <v>430</v>
       </c>
       <c r="AM2" s="152" t="s">
@@ -7744,7 +7747,7 @@
       <c r="AY2" s="152" t="s">
         <v>429</v>
       </c>
-      <c r="AZ2" s="258" t="s">
+      <c r="AZ2" s="260" t="s">
         <v>428</v>
       </c>
       <c r="BA2" s="151" t="s">
@@ -7774,7 +7777,7 @@
       <c r="BI2" s="151" t="s">
         <v>427</v>
       </c>
-      <c r="BJ2" s="258" t="s">
+      <c r="BJ2" s="260" t="s">
         <v>426</v>
       </c>
       <c r="BK2"/>
@@ -7789,7 +7792,7 @@
       <c r="G3" s="155" t="s">
         <v>425</v>
       </c>
-      <c r="H3" s="258"/>
+      <c r="H3" s="260"/>
       <c r="I3" s="154" t="s">
         <v>424</v>
       </c>
@@ -7830,7 +7833,7 @@
       <c r="V3" s="154" t="s">
         <v>412</v>
       </c>
-      <c r="W3" s="258"/>
+      <c r="W3" s="260"/>
       <c r="X3" s="150"/>
       <c r="Y3" s="155" t="s">
         <v>411</v>
@@ -7841,7 +7844,7 @@
       <c r="AA3" s="155" t="s">
         <v>409</v>
       </c>
-      <c r="AB3" s="258"/>
+      <c r="AB3" s="260"/>
       <c r="AC3" s="152" t="s">
         <v>408</v>
       </c>
@@ -7869,7 +7872,7 @@
       <c r="AK3" s="152" t="s">
         <v>402</v>
       </c>
-      <c r="AL3" s="258"/>
+      <c r="AL3" s="260"/>
       <c r="AM3" s="152" t="s">
         <v>401</v>
       </c>
@@ -7909,7 +7912,7 @@
       <c r="AY3" s="152" t="s">
         <v>389</v>
       </c>
-      <c r="AZ3" s="258"/>
+      <c r="AZ3" s="260"/>
       <c r="BA3" s="151" t="s">
         <v>388</v>
       </c>
@@ -7937,7 +7940,7 @@
       <c r="BI3" s="151" t="s">
         <v>380</v>
       </c>
-      <c r="BJ3" s="258"/>
+      <c r="BJ3" s="260"/>
     </row>
     <row r="4" spans="1:63" s="112" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="157"/>
@@ -7959,7 +7962,7 @@
       <c r="G4" s="155" t="s">
         <v>375</v>
       </c>
-      <c r="H4" s="258"/>
+      <c r="H4" s="260"/>
       <c r="I4" s="154" t="s">
         <v>374</v>
       </c>
@@ -8002,7 +8005,7 @@
       <c r="V4" s="154" t="s">
         <v>361</v>
       </c>
-      <c r="W4" s="258"/>
+      <c r="W4" s="260"/>
       <c r="X4" s="153" t="s">
         <v>360</v>
       </c>
@@ -8015,7 +8018,7 @@
       <c r="AA4" s="153" t="s">
         <v>357</v>
       </c>
-      <c r="AB4" s="258"/>
+      <c r="AB4" s="260"/>
       <c r="AC4" s="152" t="s">
         <v>356</v>
       </c>
@@ -8043,7 +8046,7 @@
       <c r="AK4" s="152" t="s">
         <v>349</v>
       </c>
-      <c r="AL4" s="258"/>
+      <c r="AL4" s="260"/>
       <c r="AM4" s="152" t="s">
         <v>348</v>
       </c>
@@ -8083,7 +8086,7 @@
       <c r="AY4" s="152" t="s">
         <v>336</v>
       </c>
-      <c r="AZ4" s="258"/>
+      <c r="AZ4" s="260"/>
       <c r="BA4" s="151" t="s">
         <v>335</v>
       </c>
@@ -8111,7 +8114,7 @@
       <c r="BI4" s="151" t="s">
         <v>327</v>
       </c>
-      <c r="BJ4" s="258"/>
+      <c r="BJ4" s="260"/>
       <c r="BK4"/>
     </row>
     <row r="5" spans="1:63" s="112" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -10832,7 +10835,7 @@
       <c r="G2" s="155" t="s">
         <v>436</v>
       </c>
-      <c r="H2" s="258" t="s">
+      <c r="H2" s="260" t="s">
         <v>435</v>
       </c>
       <c r="I2" s="155" t="s">
@@ -10865,13 +10868,13 @@
       <c r="R2" s="155" t="s">
         <v>434</v>
       </c>
-      <c r="S2" s="258" t="s">
+      <c r="S2" s="260" t="s">
         <v>433</v>
       </c>
       <c r="T2" s="155" t="s">
         <v>150</v>
       </c>
-      <c r="U2" s="258" t="s">
+      <c r="U2" s="260" t="s">
         <v>432</v>
       </c>
       <c r="V2" s="155" t="s">
@@ -10901,7 +10904,7 @@
       <c r="AD2" s="155" t="s">
         <v>431</v>
       </c>
-      <c r="AE2" s="258" t="s">
+      <c r="AE2" s="260" t="s">
         <v>480</v>
       </c>
       <c r="AF2" s="155" t="s">
@@ -10913,7 +10916,7 @@
       <c r="AH2" s="155" t="s">
         <v>479</v>
       </c>
-      <c r="AI2" s="258" t="s">
+      <c r="AI2" s="260" t="s">
         <v>478</v>
       </c>
     </row>
@@ -10927,7 +10930,7 @@
       <c r="G3" s="155" t="s">
         <v>425</v>
       </c>
-      <c r="H3" s="258"/>
+      <c r="H3" s="260"/>
       <c r="I3" s="155" t="s">
         <v>477</v>
       </c>
@@ -10958,11 +10961,11 @@
       <c r="R3" s="155" t="s">
         <v>412</v>
       </c>
-      <c r="S3" s="258"/>
+      <c r="S3" s="260"/>
       <c r="T3" s="155" t="s">
         <v>409</v>
       </c>
-      <c r="U3" s="258"/>
+      <c r="U3" s="260"/>
       <c r="V3" s="155" t="s">
         <v>468</v>
       </c>
@@ -10990,7 +10993,7 @@
       <c r="AD3" s="155" t="s">
         <v>460</v>
       </c>
-      <c r="AE3" s="258"/>
+      <c r="AE3" s="260"/>
       <c r="AF3" s="155" t="s">
         <v>459</v>
       </c>
@@ -11000,7 +11003,7 @@
       <c r="AH3" s="155" t="s">
         <v>389</v>
       </c>
-      <c r="AI3" s="258"/>
+      <c r="AI3" s="260"/>
     </row>
     <row r="4" spans="1:62" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="158"/>
@@ -11022,7 +11025,7 @@
       <c r="G4" s="155" t="s">
         <v>375</v>
       </c>
-      <c r="H4" s="258"/>
+      <c r="H4" s="260"/>
       <c r="I4" s="155" t="s">
         <v>458</v>
       </c>
@@ -11053,11 +11056,11 @@
       <c r="R4" s="155" t="s">
         <v>361</v>
       </c>
-      <c r="S4" s="258"/>
+      <c r="S4" s="260"/>
       <c r="T4" s="155" t="s">
         <v>357</v>
       </c>
-      <c r="U4" s="258"/>
+      <c r="U4" s="260"/>
       <c r="V4" s="155" t="s">
         <v>449</v>
       </c>
@@ -11085,7 +11088,7 @@
       <c r="AD4" s="155" t="s">
         <v>441</v>
       </c>
-      <c r="AE4" s="258"/>
+      <c r="AE4" s="260"/>
       <c r="AF4" s="155" t="s">
         <v>440</v>
       </c>
@@ -11095,7 +11098,7 @@
       <c r="AH4" s="155" t="s">
         <v>336</v>
       </c>
-      <c r="AI4" s="258"/>
+      <c r="AI4" s="260"/>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A5" s="161" t="s">
@@ -12832,13 +12835,13 @@
       <c r="G2" s="155" t="s">
         <v>434</v>
       </c>
-      <c r="H2" s="258" t="s">
+      <c r="H2" s="260" t="s">
         <v>433</v>
       </c>
       <c r="I2" s="155" t="s">
         <v>150</v>
       </c>
-      <c r="J2" s="258" t="s">
+      <c r="J2" s="260" t="s">
         <v>432</v>
       </c>
     </row>
@@ -12852,11 +12855,11 @@
       <c r="G3" s="155" t="s">
         <v>412</v>
       </c>
-      <c r="H3" s="258"/>
+      <c r="H3" s="260"/>
       <c r="I3" s="155" t="s">
         <v>409</v>
       </c>
-      <c r="J3" s="258"/>
+      <c r="J3" s="260"/>
     </row>
     <row r="4" spans="1:62" ht="36" x14ac:dyDescent="0.2">
       <c r="A4" s="177"/>
@@ -12878,11 +12881,11 @@
       <c r="G4" s="155" t="s">
         <v>361</v>
       </c>
-      <c r="H4" s="258"/>
+      <c r="H4" s="260"/>
       <c r="I4" s="155" t="s">
         <v>357</v>
       </c>
-      <c r="J4" s="258"/>
+      <c r="J4" s="260"/>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A5" s="171" t="s">
@@ -13597,14 +13600,14 @@
       <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="EA1" s="252" t="s">
+      <c r="EA1" s="254" t="s">
         <v>490</v>
       </c>
-      <c r="EB1" s="252"/>
-      <c r="EC1" s="252"/>
-      <c r="ED1" s="252"/>
-      <c r="EE1" s="252"/>
-      <c r="EF1" s="252"/>
+      <c r="EB1" s="254"/>
+      <c r="EC1" s="254"/>
+      <c r="ED1" s="254"/>
+      <c r="EE1" s="254"/>
+      <c r="EF1" s="254"/>
       <c r="EG1" s="8" t="s">
         <v>0</v>
       </c>
@@ -13734,20 +13737,20 @@
     </row>
     <row r="4" spans="1:16" ht="40" x14ac:dyDescent="0.2">
       <c r="C4" s="9"/>
-      <c r="E4" s="253" t="s">
+      <c r="E4" s="255" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="254"/>
-      <c r="G4" s="254"/>
-      <c r="H4" s="254"/>
-      <c r="I4" s="255"/>
-      <c r="J4" s="253" t="s">
+      <c r="F4" s="256"/>
+      <c r="G4" s="256"/>
+      <c r="H4" s="256"/>
+      <c r="I4" s="257"/>
+      <c r="J4" s="255" t="s">
         <v>27</v>
       </c>
-      <c r="K4" s="254"/>
-      <c r="L4" s="254"/>
-      <c r="M4" s="254"/>
-      <c r="N4" s="255"/>
+      <c r="K4" s="256"/>
+      <c r="L4" s="256"/>
+      <c r="M4" s="256"/>
+      <c r="N4" s="257"/>
       <c r="O4" s="30" t="s">
         <v>28</v>
       </c>
@@ -13992,10 +13995,10 @@
   <sheetPr codeName="Feuil14">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G66"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView topLeftCell="B47" zoomScale="125" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+    <sheetView topLeftCell="B53" zoomScale="125" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15237,19 +15240,19 @@
       </c>
     </row>
     <row r="62" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="261" t="s">
+      <c r="A62" s="233" t="s">
         <v>140</v>
       </c>
-      <c r="B62" s="262" t="s">
+      <c r="B62" s="234" t="s">
         <v>520</v>
       </c>
-      <c r="C62" s="262" t="s">
+      <c r="C62" s="234" t="s">
         <v>521</v>
       </c>
-      <c r="D62" s="262" t="s">
+      <c r="D62" s="234" t="s">
         <v>137</v>
       </c>
-      <c r="E62" s="262" t="s">
+      <c r="E62" s="234" t="s">
         <v>109</v>
       </c>
       <c r="F62" s="48" t="s">
@@ -15298,49 +15301,69 @@
       </c>
     </row>
     <row r="65" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="47" t="s">
+      <c r="A65" s="49" t="s">
         <v>140</v>
       </c>
-      <c r="B65" s="42" t="s">
+      <c r="B65" s="48" t="s">
+        <v>143</v>
+      </c>
+      <c r="C65" s="48" t="s">
+        <v>522</v>
+      </c>
+      <c r="D65" s="48" t="s">
+        <v>137</v>
+      </c>
+      <c r="E65" s="48" t="s">
+        <v>109</v>
+      </c>
+      <c r="F65" s="48" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="47" t="s">
+        <v>140</v>
+      </c>
+      <c r="B66" s="42" t="s">
         <v>142</v>
       </c>
-      <c r="C65" s="42" t="s">
+      <c r="C66" s="42" t="s">
         <v>141</v>
       </c>
-      <c r="D65" s="42" t="s">
+      <c r="D66" s="42" t="s">
         <v>137</v>
       </c>
-      <c r="E65" s="42" t="s">
+      <c r="E66" s="42" t="s">
         <v>109</v>
       </c>
-      <c r="F65" s="46"/>
-      <c r="G65" s="42" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="45" t="s">
-        <v>140</v>
-      </c>
-      <c r="B66" s="44" t="s">
-        <v>139</v>
-      </c>
-      <c r="C66" s="44" t="s">
-        <v>138</v>
-      </c>
-      <c r="D66" s="44" t="s">
-        <v>137</v>
-      </c>
-      <c r="E66" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="F66" s="43"/>
+      <c r="F66" s="46"/>
       <c r="G66" s="42" t="s">
         <v>136</v>
       </c>
     </row>
+    <row r="67" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="45" t="s">
+        <v>140</v>
+      </c>
+      <c r="B67" s="44" t="s">
+        <v>139</v>
+      </c>
+      <c r="C67" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="D67" s="44" t="s">
+        <v>137</v>
+      </c>
+      <c r="E67" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="F67" s="43"/>
+      <c r="G67" s="42" t="s">
+        <v>136</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F66" xr:uid="{00000000-0001-0000-0300-000000000000}"/>
+  <autoFilter ref="A1:F67" xr:uid="{00000000-0001-0000-0300-000000000000}"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" scale="74" orientation="landscape" r:id="rId1"/>
 </worksheet>
@@ -15388,16 +15411,16 @@
   <sheetData>
     <row r="1" spans="1:62" s="64" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A1" s="107"/>
-      <c r="B1" s="257" t="s">
+      <c r="B1" s="259" t="s">
         <v>437</v>
       </c>
-      <c r="C1" s="257"/>
-      <c r="D1" s="257"/>
-      <c r="E1" s="257"/>
-      <c r="F1" s="257"/>
-      <c r="G1" s="257"/>
-      <c r="H1" s="257"/>
-      <c r="I1" s="257"/>
+      <c r="C1" s="259"/>
+      <c r="D1" s="259"/>
+      <c r="E1" s="259"/>
+      <c r="F1" s="259"/>
+      <c r="G1" s="259"/>
+      <c r="H1" s="259"/>
+      <c r="I1" s="259"/>
       <c r="AC1" s="106"/>
       <c r="AD1" s="106"/>
       <c r="AE1" s="106"/>
@@ -15418,7 +15441,7 @@
       <c r="G2" s="102" t="s">
         <v>436</v>
       </c>
-      <c r="H2" s="256" t="s">
+      <c r="H2" s="258" t="s">
         <v>435</v>
       </c>
       <c r="I2" s="101" t="s">
@@ -15463,7 +15486,7 @@
       <c r="V2" s="101" t="s">
         <v>434</v>
       </c>
-      <c r="W2" s="256" t="s">
+      <c r="W2" s="258" t="s">
         <v>433</v>
       </c>
       <c r="X2" s="102" t="s">
@@ -15478,7 +15501,7 @@
       <c r="AA2" s="102" t="s">
         <v>150</v>
       </c>
-      <c r="AB2" s="256" t="s">
+      <c r="AB2" s="258" t="s">
         <v>432</v>
       </c>
       <c r="AC2" s="98" t="s">
@@ -15508,7 +15531,7 @@
       <c r="AK2" s="98" t="s">
         <v>431</v>
       </c>
-      <c r="AL2" s="256" t="s">
+      <c r="AL2" s="258" t="s">
         <v>430</v>
       </c>
       <c r="AM2" s="98" t="s">
@@ -15550,7 +15573,7 @@
       <c r="AY2" s="98" t="s">
         <v>429</v>
       </c>
-      <c r="AZ2" s="256" t="s">
+      <c r="AZ2" s="258" t="s">
         <v>428</v>
       </c>
       <c r="BA2" s="97" t="s">
@@ -15580,7 +15603,7 @@
       <c r="BI2" s="97" t="s">
         <v>427</v>
       </c>
-      <c r="BJ2" s="256" t="s">
+      <c r="BJ2" s="258" t="s">
         <v>426</v>
       </c>
     </row>
@@ -15594,7 +15617,7 @@
       <c r="G3" s="102" t="s">
         <v>425</v>
       </c>
-      <c r="H3" s="256"/>
+      <c r="H3" s="258"/>
       <c r="I3" s="101" t="s">
         <v>424</v>
       </c>
@@ -15635,7 +15658,7 @@
       <c r="V3" s="101" t="s">
         <v>412</v>
       </c>
-      <c r="W3" s="256"/>
+      <c r="W3" s="258"/>
       <c r="X3" s="96"/>
       <c r="Y3" s="102" t="s">
         <v>411</v>
@@ -15646,7 +15669,7 @@
       <c r="AA3" s="102" t="s">
         <v>409</v>
       </c>
-      <c r="AB3" s="256"/>
+      <c r="AB3" s="258"/>
       <c r="AC3" s="98" t="s">
         <v>408</v>
       </c>
@@ -15674,7 +15697,7 @@
       <c r="AK3" s="98" t="s">
         <v>402</v>
       </c>
-      <c r="AL3" s="256"/>
+      <c r="AL3" s="258"/>
       <c r="AM3" s="98" t="s">
         <v>401</v>
       </c>
@@ -15714,7 +15737,7 @@
       <c r="AY3" s="98" t="s">
         <v>389</v>
       </c>
-      <c r="AZ3" s="256"/>
+      <c r="AZ3" s="258"/>
       <c r="BA3" s="97" t="s">
         <v>388</v>
       </c>
@@ -15742,7 +15765,7 @@
       <c r="BI3" s="97" t="s">
         <v>380</v>
       </c>
-      <c r="BJ3" s="256"/>
+      <c r="BJ3" s="258"/>
     </row>
     <row r="4" spans="1:62" s="64" customFormat="1" ht="60" x14ac:dyDescent="0.15">
       <c r="A4" s="104"/>
@@ -15764,7 +15787,7 @@
       <c r="G4" s="102" t="s">
         <v>375</v>
       </c>
-      <c r="H4" s="256"/>
+      <c r="H4" s="258"/>
       <c r="I4" s="101" t="s">
         <v>374</v>
       </c>
@@ -15807,7 +15830,7 @@
       <c r="V4" s="100" t="s">
         <v>361</v>
       </c>
-      <c r="W4" s="256"/>
+      <c r="W4" s="258"/>
       <c r="X4" s="99" t="s">
         <v>360</v>
       </c>
@@ -15820,7 +15843,7 @@
       <c r="AA4" s="99" t="s">
         <v>357</v>
       </c>
-      <c r="AB4" s="256"/>
+      <c r="AB4" s="258"/>
       <c r="AC4" s="98" t="s">
         <v>356</v>
       </c>
@@ -15848,7 +15871,7 @@
       <c r="AK4" s="98" t="s">
         <v>349</v>
       </c>
-      <c r="AL4" s="256"/>
+      <c r="AL4" s="258"/>
       <c r="AM4" s="98" t="s">
         <v>348</v>
       </c>
@@ -15888,7 +15911,7 @@
       <c r="AY4" s="98" t="s">
         <v>336</v>
       </c>
-      <c r="AZ4" s="256"/>
+      <c r="AZ4" s="258"/>
       <c r="BA4" s="97" t="s">
         <v>335</v>
       </c>
@@ -15916,7 +15939,7 @@
       <c r="BI4" s="97" t="s">
         <v>327</v>
       </c>
-      <c r="BJ4" s="256"/>
+      <c r="BJ4" s="258"/>
     </row>
     <row r="5" spans="1:62" s="64" customFormat="1" ht="144" x14ac:dyDescent="0.15">
       <c r="A5" s="72" t="s">
@@ -16894,7 +16917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:62" s="64" customFormat="1" ht="48" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:62" s="64" customFormat="1" ht="36" x14ac:dyDescent="0.15">
       <c r="A13" s="72" t="s">
         <v>231</v>
       </c>
@@ -17615,16 +17638,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" s="112" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B1" s="259" t="s">
+      <c r="B1" s="261" t="s">
         <v>437</v>
       </c>
-      <c r="C1" s="259"/>
-      <c r="D1" s="259"/>
-      <c r="E1" s="259"/>
-      <c r="F1" s="259"/>
-      <c r="G1" s="259"/>
-      <c r="H1" s="259"/>
-      <c r="I1" s="259"/>
+      <c r="C1" s="261"/>
+      <c r="D1" s="261"/>
+      <c r="E1" s="261"/>
+      <c r="F1" s="261"/>
+      <c r="G1" s="261"/>
+      <c r="H1" s="261"/>
+      <c r="I1" s="261"/>
     </row>
     <row r="2" spans="1:62" s="112" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="158"/>
@@ -17636,7 +17659,7 @@
       <c r="G2" s="155" t="s">
         <v>436</v>
       </c>
-      <c r="H2" s="258" t="s">
+      <c r="H2" s="260" t="s">
         <v>435</v>
       </c>
       <c r="I2" s="154" t="s">
@@ -17681,7 +17704,7 @@
       <c r="V2" s="154" t="s">
         <v>434</v>
       </c>
-      <c r="W2" s="258" t="s">
+      <c r="W2" s="260" t="s">
         <v>433</v>
       </c>
       <c r="X2" s="155" t="s">
@@ -17696,7 +17719,7 @@
       <c r="AA2" s="155" t="s">
         <v>150</v>
       </c>
-      <c r="AB2" s="258" t="s">
+      <c r="AB2" s="260" t="s">
         <v>432</v>
       </c>
       <c r="AC2" s="152" t="s">
@@ -17726,7 +17749,7 @@
       <c r="AK2" s="152" t="s">
         <v>431</v>
       </c>
-      <c r="AL2" s="258" t="s">
+      <c r="AL2" s="260" t="s">
         <v>430</v>
       </c>
       <c r="AM2" s="152" t="s">
@@ -17768,7 +17791,7 @@
       <c r="AY2" s="152" t="s">
         <v>429</v>
       </c>
-      <c r="AZ2" s="258" t="s">
+      <c r="AZ2" s="260" t="s">
         <v>428</v>
       </c>
       <c r="BA2" s="151" t="s">
@@ -17798,7 +17821,7 @@
       <c r="BI2" s="151" t="s">
         <v>427</v>
       </c>
-      <c r="BJ2" s="258" t="s">
+      <c r="BJ2" s="260" t="s">
         <v>426</v>
       </c>
     </row>
@@ -17812,7 +17835,7 @@
       <c r="G3" s="155" t="s">
         <v>425</v>
       </c>
-      <c r="H3" s="258"/>
+      <c r="H3" s="260"/>
       <c r="I3" s="154" t="s">
         <v>424</v>
       </c>
@@ -17853,7 +17876,7 @@
       <c r="V3" s="154" t="s">
         <v>412</v>
       </c>
-      <c r="W3" s="258"/>
+      <c r="W3" s="260"/>
       <c r="X3" s="150"/>
       <c r="Y3" s="155" t="s">
         <v>411</v>
@@ -17864,7 +17887,7 @@
       <c r="AA3" s="155" t="s">
         <v>409</v>
       </c>
-      <c r="AB3" s="258"/>
+      <c r="AB3" s="260"/>
       <c r="AC3" s="152" t="s">
         <v>408</v>
       </c>
@@ -17892,7 +17915,7 @@
       <c r="AK3" s="152" t="s">
         <v>402</v>
       </c>
-      <c r="AL3" s="258"/>
+      <c r="AL3" s="260"/>
       <c r="AM3" s="152" t="s">
         <v>401</v>
       </c>
@@ -17932,7 +17955,7 @@
       <c r="AY3" s="152" t="s">
         <v>389</v>
       </c>
-      <c r="AZ3" s="258"/>
+      <c r="AZ3" s="260"/>
       <c r="BA3" s="151" t="s">
         <v>388</v>
       </c>
@@ -17960,7 +17983,7 @@
       <c r="BI3" s="151" t="s">
         <v>380</v>
       </c>
-      <c r="BJ3" s="258"/>
+      <c r="BJ3" s="260"/>
     </row>
     <row r="4" spans="1:62" s="112" customFormat="1" ht="60" x14ac:dyDescent="0.15">
       <c r="A4" s="157"/>
@@ -17982,7 +18005,7 @@
       <c r="G4" s="155" t="s">
         <v>375</v>
       </c>
-      <c r="H4" s="258"/>
+      <c r="H4" s="260"/>
       <c r="I4" s="154" t="s">
         <v>374</v>
       </c>
@@ -18025,7 +18048,7 @@
       <c r="V4" s="154" t="s">
         <v>361</v>
       </c>
-      <c r="W4" s="258"/>
+      <c r="W4" s="260"/>
       <c r="X4" s="153" t="s">
         <v>360</v>
       </c>
@@ -18038,7 +18061,7 @@
       <c r="AA4" s="153" t="s">
         <v>357</v>
       </c>
-      <c r="AB4" s="258"/>
+      <c r="AB4" s="260"/>
       <c r="AC4" s="152" t="s">
         <v>356</v>
       </c>
@@ -18066,7 +18089,7 @@
       <c r="AK4" s="152" t="s">
         <v>349</v>
       </c>
-      <c r="AL4" s="258"/>
+      <c r="AL4" s="260"/>
       <c r="AM4" s="152" t="s">
         <v>348</v>
       </c>
@@ -18106,7 +18129,7 @@
       <c r="AY4" s="152" t="s">
         <v>336</v>
       </c>
-      <c r="AZ4" s="258"/>
+      <c r="AZ4" s="260"/>
       <c r="BA4" s="151" t="s">
         <v>335</v>
       </c>
@@ -18134,7 +18157,7 @@
       <c r="BI4" s="151" t="s">
         <v>327</v>
       </c>
-      <c r="BJ4" s="258"/>
+      <c r="BJ4" s="260"/>
     </row>
     <row r="5" spans="1:62" s="112" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="122" t="s">

</xml_diff>

<commit_message>
update extractor and error etp simulator
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2236A0B-2A89-994D-BFA7-9C2642E3F64E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C9A653-5F3B-1848-BAAE-D5C33538B0BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" activeTab="3" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
@@ -2795,13 +2795,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="General;General;\-"/>
     <numFmt numFmtId="168" formatCode="0.###;0.###;\-"/>
     <numFmt numFmtId="169" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
+    <numFmt numFmtId="170" formatCode="0.0%"/>
   </numFmts>
   <fonts count="53" x14ac:knownFonts="1">
     <font>
@@ -4579,6 +4580,22 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="52" fillId="0" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="52" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="40" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4643,6 +4660,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="10" borderId="13" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4663,36 +4689,11 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="52" fillId="0" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="52" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="52" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="52" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="52" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="52" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -4703,67 +4704,7 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{6FC886D6-2077-B34D-B1DF-739B068A66D1}"/>
     <cellStyle name="Normal 3" xfId="4" xr:uid="{6BD57324-3FD5-D341-A299-730D14794802}"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -5572,11 +5513,11 @@
       <c r="B1" s="192" t="s">
         <v>492</v>
       </c>
-      <c r="C1" s="230" t="s">
+      <c r="C1" s="236" t="s">
         <v>493</v>
       </c>
-      <c r="D1" s="230"/>
-      <c r="E1" s="230"/>
+      <c r="D1" s="236"/>
+      <c r="E1" s="236"/>
       <c r="F1" s="193"/>
       <c r="H1" s="27" t="s">
         <v>0</v>
@@ -5585,11 +5526,11 @@
     <row r="2" spans="1:8" s="197" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="194"/>
       <c r="B2" s="195"/>
-      <c r="C2" s="231" t="s">
+      <c r="C2" s="237" t="s">
         <v>494</v>
       </c>
-      <c r="D2" s="231"/>
-      <c r="E2" s="231"/>
+      <c r="D2" s="237"/>
+      <c r="E2" s="237"/>
       <c r="F2" s="196"/>
       <c r="H2" s="27" t="s">
         <v>0</v>
@@ -5613,10 +5554,10 @@
       <c r="D4" s="202" t="s">
         <v>497</v>
       </c>
-      <c r="E4" s="237" t="s">
+      <c r="E4" s="243" t="s">
         <v>498</v>
       </c>
-      <c r="F4" s="238"/>
+      <c r="F4" s="244"/>
       <c r="G4" s="211"/>
       <c r="H4" s="27" t="s">
         <v>0</v>
@@ -5633,10 +5574,10 @@
       <c r="D5" s="208" t="s">
         <v>501</v>
       </c>
-      <c r="E5" s="239" t="s">
+      <c r="E5" s="245" t="s">
         <v>514</v>
       </c>
-      <c r="F5" s="240"/>
+      <c r="F5" s="246"/>
       <c r="G5" s="210"/>
       <c r="H5" s="27" t="s">
         <v>0</v>
@@ -5653,10 +5594,10 @@
       <c r="D6" s="209" t="s">
         <v>504</v>
       </c>
-      <c r="E6" s="241" t="s">
+      <c r="E6" s="247" t="s">
         <v>515</v>
       </c>
-      <c r="F6" s="242"/>
+      <c r="F6" s="248"/>
       <c r="G6" s="210"/>
       <c r="H6" s="27" t="s">
         <v>0</v>
@@ -5673,10 +5614,10 @@
       <c r="D7" s="209" t="s">
         <v>507</v>
       </c>
-      <c r="E7" s="241" t="s">
+      <c r="E7" s="247" t="s">
         <v>514</v>
       </c>
-      <c r="F7" s="242"/>
+      <c r="F7" s="248"/>
       <c r="G7" s="210"/>
       <c r="H7" s="27" t="s">
         <v>0</v>
@@ -5687,16 +5628,16 @@
       <c r="B8" s="218" t="s">
         <v>508</v>
       </c>
-      <c r="C8" s="232" t="s">
+      <c r="C8" s="238" t="s">
         <v>509</v>
       </c>
-      <c r="D8" s="232" t="s">
+      <c r="D8" s="238" t="s">
         <v>510</v>
       </c>
-      <c r="E8" s="243" t="s">
+      <c r="E8" s="249" t="s">
         <v>516</v>
       </c>
-      <c r="F8" s="244"/>
+      <c r="F8" s="250"/>
       <c r="G8" s="210"/>
       <c r="H8" s="27" t="s">
         <v>0</v>
@@ -5707,10 +5648,10 @@
       <c r="B9" s="219" t="s">
         <v>511</v>
       </c>
-      <c r="C9" s="232"/>
-      <c r="D9" s="232"/>
-      <c r="E9" s="245"/>
-      <c r="F9" s="246"/>
+      <c r="C9" s="238"/>
+      <c r="D9" s="238"/>
+      <c r="E9" s="251"/>
+      <c r="F9" s="252"/>
       <c r="G9" s="210"/>
       <c r="H9" s="27" t="s">
         <v>0</v>
@@ -5721,10 +5662,10 @@
       <c r="B10" s="220" t="s">
         <v>512</v>
       </c>
-      <c r="C10" s="233"/>
-      <c r="D10" s="233"/>
-      <c r="E10" s="247"/>
-      <c r="F10" s="248"/>
+      <c r="C10" s="239"/>
+      <c r="D10" s="239"/>
+      <c r="E10" s="253"/>
+      <c r="F10" s="254"/>
       <c r="G10" s="210"/>
       <c r="H10" s="27" t="s">
         <v>0</v>
@@ -5744,11 +5685,11 @@
     <row r="12" spans="1:8" s="27" customFormat="1" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="198"/>
       <c r="B12" s="212"/>
-      <c r="C12" s="236" t="s">
+      <c r="C12" s="242" t="s">
         <v>513</v>
       </c>
-      <c r="D12" s="236"/>
-      <c r="E12" s="236"/>
+      <c r="D12" s="242"/>
+      <c r="E12" s="242"/>
       <c r="F12" s="213"/>
       <c r="H12" s="27" t="s">
         <v>0</v>
@@ -5762,14 +5703,14 @@
       </c>
     </row>
     <row r="14" spans="1:8" s="27" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="234" t="s">
+      <c r="A14" s="240" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="234"/>
-      <c r="C14" s="234"/>
-      <c r="D14" s="234"/>
-      <c r="E14" s="234"/>
-      <c r="F14" s="235"/>
+      <c r="B14" s="240"/>
+      <c r="C14" s="240"/>
+      <c r="D14" s="240"/>
+      <c r="E14" s="240"/>
+      <c r="F14" s="241"/>
       <c r="H14" s="27" t="s">
         <v>0</v>
       </c>
@@ -5822,16 +5763,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A1" s="256" t="s">
+      <c r="A1" s="265" t="s">
         <v>481</v>
       </c>
-      <c r="B1" s="256"/>
-      <c r="C1" s="256"/>
-      <c r="D1" s="256"/>
-      <c r="E1" s="256"/>
-      <c r="F1" s="256"/>
-      <c r="G1" s="256"/>
-      <c r="H1" s="256"/>
+      <c r="B1" s="265"/>
+      <c r="C1" s="265"/>
+      <c r="D1" s="265"/>
+      <c r="E1" s="265"/>
+      <c r="F1" s="265"/>
+      <c r="G1" s="265"/>
+      <c r="H1" s="265"/>
       <c r="I1" s="107"/>
       <c r="J1" s="107"/>
       <c r="K1" s="107"/>
@@ -5870,7 +5811,7 @@
       <c r="G2" s="150" t="s">
         <v>436</v>
       </c>
-      <c r="H2" s="254" t="s">
+      <c r="H2" s="263" t="s">
         <v>435</v>
       </c>
       <c r="I2" s="150" t="s">
@@ -5903,13 +5844,13 @@
       <c r="R2" s="150" t="s">
         <v>434</v>
       </c>
-      <c r="S2" s="254" t="s">
+      <c r="S2" s="263" t="s">
         <v>433</v>
       </c>
       <c r="T2" s="150" t="s">
         <v>150</v>
       </c>
-      <c r="U2" s="254" t="s">
+      <c r="U2" s="263" t="s">
         <v>432</v>
       </c>
       <c r="V2" s="150" t="s">
@@ -5939,7 +5880,7 @@
       <c r="AD2" s="150" t="s">
         <v>431</v>
       </c>
-      <c r="AE2" s="254" t="s">
+      <c r="AE2" s="263" t="s">
         <v>480</v>
       </c>
       <c r="AF2" s="150" t="s">
@@ -5951,7 +5892,7 @@
       <c r="AH2" s="150" t="s">
         <v>479</v>
       </c>
-      <c r="AI2" s="254" t="s">
+      <c r="AI2" s="263" t="s">
         <v>478</v>
       </c>
     </row>
@@ -5965,7 +5906,7 @@
       <c r="G3" s="150" t="s">
         <v>425</v>
       </c>
-      <c r="H3" s="254"/>
+      <c r="H3" s="263"/>
       <c r="I3" s="150" t="s">
         <v>477</v>
       </c>
@@ -5996,11 +5937,11 @@
       <c r="R3" s="150" t="s">
         <v>412</v>
       </c>
-      <c r="S3" s="254"/>
+      <c r="S3" s="263"/>
       <c r="T3" s="150" t="s">
         <v>409</v>
       </c>
-      <c r="U3" s="254"/>
+      <c r="U3" s="263"/>
       <c r="V3" s="150" t="s">
         <v>468</v>
       </c>
@@ -6028,7 +5969,7 @@
       <c r="AD3" s="150" t="s">
         <v>460</v>
       </c>
-      <c r="AE3" s="254"/>
+      <c r="AE3" s="263"/>
       <c r="AF3" s="150" t="s">
         <v>459</v>
       </c>
@@ -6038,7 +5979,7 @@
       <c r="AH3" s="150" t="s">
         <v>389</v>
       </c>
-      <c r="AI3" s="254"/>
+      <c r="AI3" s="263"/>
     </row>
     <row r="4" spans="1:35" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="153"/>
@@ -6060,7 +6001,7 @@
       <c r="G4" s="150" t="s">
         <v>375</v>
       </c>
-      <c r="H4" s="254"/>
+      <c r="H4" s="263"/>
       <c r="I4" s="150" t="s">
         <v>458</v>
       </c>
@@ -6091,11 +6032,11 @@
       <c r="R4" s="150" t="s">
         <v>361</v>
       </c>
-      <c r="S4" s="254"/>
+      <c r="S4" s="263"/>
       <c r="T4" s="150" t="s">
         <v>357</v>
       </c>
-      <c r="U4" s="254"/>
+      <c r="U4" s="263"/>
       <c r="V4" s="150" t="s">
         <v>449</v>
       </c>
@@ -6123,7 +6064,7 @@
       <c r="AD4" s="150" t="s">
         <v>441</v>
       </c>
-      <c r="AE4" s="254"/>
+      <c r="AE4" s="263"/>
       <c r="AF4" s="150" t="s">
         <v>440</v>
       </c>
@@ -6133,7 +6074,7 @@
       <c r="AH4" s="150" t="s">
         <v>336</v>
       </c>
-      <c r="AI4" s="254"/>
+      <c r="AI4" s="263"/>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A5" s="156" t="s">
@@ -7242,13 +7183,13 @@
       <c r="G2" s="150" t="s">
         <v>434</v>
       </c>
-      <c r="H2" s="254" t="s">
+      <c r="H2" s="263" t="s">
         <v>433</v>
       </c>
       <c r="I2" s="150" t="s">
         <v>150</v>
       </c>
-      <c r="J2" s="254" t="s">
+      <c r="J2" s="263" t="s">
         <v>432</v>
       </c>
     </row>
@@ -7262,11 +7203,11 @@
       <c r="G3" s="150" t="s">
         <v>412</v>
       </c>
-      <c r="H3" s="254"/>
+      <c r="H3" s="263"/>
       <c r="I3" s="150" t="s">
         <v>409</v>
       </c>
-      <c r="J3" s="254"/>
+      <c r="J3" s="263"/>
     </row>
     <row r="4" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A4" s="172"/>
@@ -7288,11 +7229,11 @@
       <c r="G4" s="150" t="s">
         <v>361</v>
       </c>
-      <c r="H4" s="254"/>
+      <c r="H4" s="263"/>
       <c r="I4" s="150" t="s">
         <v>357</v>
       </c>
-      <c r="J4" s="254"/>
+      <c r="J4" s="263"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="166" t="s">
@@ -7696,7 +7637,7 @@
       <c r="G2" s="150" t="s">
         <v>436</v>
       </c>
-      <c r="H2" s="254" t="s">
+      <c r="H2" s="263" t="s">
         <v>435</v>
       </c>
       <c r="I2" s="149" t="s">
@@ -7741,7 +7682,7 @@
       <c r="V2" s="149" t="s">
         <v>434</v>
       </c>
-      <c r="W2" s="254" t="s">
+      <c r="W2" s="263" t="s">
         <v>433</v>
       </c>
       <c r="X2" s="150" t="s">
@@ -7756,7 +7697,7 @@
       <c r="AA2" s="150" t="s">
         <v>150</v>
       </c>
-      <c r="AB2" s="254" t="s">
+      <c r="AB2" s="263" t="s">
         <v>432</v>
       </c>
       <c r="AC2" s="147" t="s">
@@ -7786,7 +7727,7 @@
       <c r="AK2" s="147" t="s">
         <v>431</v>
       </c>
-      <c r="AL2" s="254" t="s">
+      <c r="AL2" s="263" t="s">
         <v>430</v>
       </c>
       <c r="AM2" s="147" t="s">
@@ -7828,7 +7769,7 @@
       <c r="AY2" s="147" t="s">
         <v>429</v>
       </c>
-      <c r="AZ2" s="254" t="s">
+      <c r="AZ2" s="263" t="s">
         <v>428</v>
       </c>
       <c r="BA2" s="146" t="s">
@@ -7858,7 +7799,7 @@
       <c r="BI2" s="146" t="s">
         <v>427</v>
       </c>
-      <c r="BJ2" s="254" t="s">
+      <c r="BJ2" s="263" t="s">
         <v>426</v>
       </c>
       <c r="BK2"/>
@@ -7873,7 +7814,7 @@
       <c r="G3" s="150" t="s">
         <v>425</v>
       </c>
-      <c r="H3" s="254"/>
+      <c r="H3" s="263"/>
       <c r="I3" s="149" t="s">
         <v>424</v>
       </c>
@@ -7914,7 +7855,7 @@
       <c r="V3" s="149" t="s">
         <v>412</v>
       </c>
-      <c r="W3" s="254"/>
+      <c r="W3" s="263"/>
       <c r="X3" s="145"/>
       <c r="Y3" s="150" t="s">
         <v>411</v>
@@ -7925,7 +7866,7 @@
       <c r="AA3" s="150" t="s">
         <v>409</v>
       </c>
-      <c r="AB3" s="254"/>
+      <c r="AB3" s="263"/>
       <c r="AC3" s="147" t="s">
         <v>408</v>
       </c>
@@ -7953,7 +7894,7 @@
       <c r="AK3" s="147" t="s">
         <v>402</v>
       </c>
-      <c r="AL3" s="254"/>
+      <c r="AL3" s="263"/>
       <c r="AM3" s="147" t="s">
         <v>401</v>
       </c>
@@ -7993,7 +7934,7 @@
       <c r="AY3" s="147" t="s">
         <v>389</v>
       </c>
-      <c r="AZ3" s="254"/>
+      <c r="AZ3" s="263"/>
       <c r="BA3" s="146" t="s">
         <v>388</v>
       </c>
@@ -8021,7 +7962,7 @@
       <c r="BI3" s="146" t="s">
         <v>380</v>
       </c>
-      <c r="BJ3" s="254"/>
+      <c r="BJ3" s="263"/>
     </row>
     <row r="4" spans="1:63" s="107" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="152"/>
@@ -8043,7 +7984,7 @@
       <c r="G4" s="150" t="s">
         <v>375</v>
       </c>
-      <c r="H4" s="254"/>
+      <c r="H4" s="263"/>
       <c r="I4" s="149" t="s">
         <v>374</v>
       </c>
@@ -8086,7 +8027,7 @@
       <c r="V4" s="149" t="s">
         <v>361</v>
       </c>
-      <c r="W4" s="254"/>
+      <c r="W4" s="263"/>
       <c r="X4" s="148" t="s">
         <v>360</v>
       </c>
@@ -8099,7 +8040,7 @@
       <c r="AA4" s="148" t="s">
         <v>357</v>
       </c>
-      <c r="AB4" s="254"/>
+      <c r="AB4" s="263"/>
       <c r="AC4" s="147" t="s">
         <v>356</v>
       </c>
@@ -8127,7 +8068,7 @@
       <c r="AK4" s="147" t="s">
         <v>349</v>
       </c>
-      <c r="AL4" s="254"/>
+      <c r="AL4" s="263"/>
       <c r="AM4" s="147" t="s">
         <v>348</v>
       </c>
@@ -8167,7 +8108,7 @@
       <c r="AY4" s="147" t="s">
         <v>336</v>
       </c>
-      <c r="AZ4" s="254"/>
+      <c r="AZ4" s="263"/>
       <c r="BA4" s="146" t="s">
         <v>335</v>
       </c>
@@ -8195,7 +8136,7 @@
       <c r="BI4" s="146" t="s">
         <v>327</v>
       </c>
-      <c r="BJ4" s="254"/>
+      <c r="BJ4" s="263"/>
       <c r="BK4"/>
     </row>
     <row r="5" spans="1:63" s="107" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -10916,7 +10857,7 @@
       <c r="G2" s="150" t="s">
         <v>436</v>
       </c>
-      <c r="H2" s="254" t="s">
+      <c r="H2" s="263" t="s">
         <v>435</v>
       </c>
       <c r="I2" s="150" t="s">
@@ -10949,13 +10890,13 @@
       <c r="R2" s="150" t="s">
         <v>434</v>
       </c>
-      <c r="S2" s="254" t="s">
+      <c r="S2" s="263" t="s">
         <v>433</v>
       </c>
       <c r="T2" s="150" t="s">
         <v>150</v>
       </c>
-      <c r="U2" s="254" t="s">
+      <c r="U2" s="263" t="s">
         <v>432</v>
       </c>
       <c r="V2" s="150" t="s">
@@ -10985,7 +10926,7 @@
       <c r="AD2" s="150" t="s">
         <v>431</v>
       </c>
-      <c r="AE2" s="254" t="s">
+      <c r="AE2" s="263" t="s">
         <v>480</v>
       </c>
       <c r="AF2" s="150" t="s">
@@ -10997,7 +10938,7 @@
       <c r="AH2" s="150" t="s">
         <v>479</v>
       </c>
-      <c r="AI2" s="254" t="s">
+      <c r="AI2" s="263" t="s">
         <v>478</v>
       </c>
     </row>
@@ -11011,7 +10952,7 @@
       <c r="G3" s="150" t="s">
         <v>425</v>
       </c>
-      <c r="H3" s="254"/>
+      <c r="H3" s="263"/>
       <c r="I3" s="150" t="s">
         <v>477</v>
       </c>
@@ -11042,11 +10983,11 @@
       <c r="R3" s="150" t="s">
         <v>412</v>
       </c>
-      <c r="S3" s="254"/>
+      <c r="S3" s="263"/>
       <c r="T3" s="150" t="s">
         <v>409</v>
       </c>
-      <c r="U3" s="254"/>
+      <c r="U3" s="263"/>
       <c r="V3" s="150" t="s">
         <v>468</v>
       </c>
@@ -11074,7 +11015,7 @@
       <c r="AD3" s="150" t="s">
         <v>460</v>
       </c>
-      <c r="AE3" s="254"/>
+      <c r="AE3" s="263"/>
       <c r="AF3" s="150" t="s">
         <v>459</v>
       </c>
@@ -11084,7 +11025,7 @@
       <c r="AH3" s="150" t="s">
         <v>389</v>
       </c>
-      <c r="AI3" s="254"/>
+      <c r="AI3" s="263"/>
     </row>
     <row r="4" spans="1:62" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="153"/>
@@ -11106,7 +11047,7 @@
       <c r="G4" s="150" t="s">
         <v>375</v>
       </c>
-      <c r="H4" s="254"/>
+      <c r="H4" s="263"/>
       <c r="I4" s="150" t="s">
         <v>458</v>
       </c>
@@ -11137,11 +11078,11 @@
       <c r="R4" s="150" t="s">
         <v>361</v>
       </c>
-      <c r="S4" s="254"/>
+      <c r="S4" s="263"/>
       <c r="T4" s="150" t="s">
         <v>357</v>
       </c>
-      <c r="U4" s="254"/>
+      <c r="U4" s="263"/>
       <c r="V4" s="150" t="s">
         <v>449</v>
       </c>
@@ -11169,7 +11110,7 @@
       <c r="AD4" s="150" t="s">
         <v>441</v>
       </c>
-      <c r="AE4" s="254"/>
+      <c r="AE4" s="263"/>
       <c r="AF4" s="150" t="s">
         <v>440</v>
       </c>
@@ -11179,7 +11120,7 @@
       <c r="AH4" s="150" t="s">
         <v>336</v>
       </c>
-      <c r="AI4" s="254"/>
+      <c r="AI4" s="263"/>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A5" s="156" t="s">
@@ -12916,13 +12857,13 @@
       <c r="G2" s="150" t="s">
         <v>434</v>
       </c>
-      <c r="H2" s="254" t="s">
+      <c r="H2" s="263" t="s">
         <v>433</v>
       </c>
       <c r="I2" s="150" t="s">
         <v>150</v>
       </c>
-      <c r="J2" s="254" t="s">
+      <c r="J2" s="263" t="s">
         <v>432</v>
       </c>
     </row>
@@ -12936,11 +12877,11 @@
       <c r="G3" s="150" t="s">
         <v>412</v>
       </c>
-      <c r="H3" s="254"/>
+      <c r="H3" s="263"/>
       <c r="I3" s="150" t="s">
         <v>409</v>
       </c>
-      <c r="J3" s="254"/>
+      <c r="J3" s="263"/>
     </row>
     <row r="4" spans="1:62" ht="36" x14ac:dyDescent="0.2">
       <c r="A4" s="172"/>
@@ -12962,11 +12903,11 @@
       <c r="G4" s="150" t="s">
         <v>361</v>
       </c>
-      <c r="H4" s="254"/>
+      <c r="H4" s="263"/>
       <c r="I4" s="150" t="s">
         <v>357</v>
       </c>
-      <c r="J4" s="254"/>
+      <c r="J4" s="263"/>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A5" s="166" t="s">
@@ -13681,14 +13622,14 @@
       <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="EA1" s="249" t="s">
+      <c r="EA1" s="255" t="s">
         <v>490</v>
       </c>
-      <c r="EB1" s="249"/>
-      <c r="EC1" s="249"/>
-      <c r="ED1" s="249"/>
-      <c r="EE1" s="249"/>
-      <c r="EF1" s="249"/>
+      <c r="EB1" s="255"/>
+      <c r="EC1" s="255"/>
+      <c r="ED1" s="255"/>
+      <c r="EE1" s="255"/>
+      <c r="EF1" s="255"/>
       <c r="EG1" s="8" t="s">
         <v>0</v>
       </c>
@@ -13751,8 +13692,8 @@
   </sheetPr>
   <dimension ref="A1:X200"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13830,30 +13771,30 @@
     </row>
     <row r="4" spans="1:24" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D4" s="9"/>
-      <c r="E4" s="264"/>
-      <c r="G4" s="250" t="s">
+      <c r="E4" s="234"/>
+      <c r="G4" s="256" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="251"/>
-      <c r="I4" s="251"/>
-      <c r="J4" s="251"/>
-      <c r="K4" s="251"/>
-      <c r="L4" s="251"/>
-      <c r="M4" s="260"/>
-      <c r="N4" s="250" t="s">
+      <c r="H4" s="257"/>
+      <c r="I4" s="257"/>
+      <c r="J4" s="257"/>
+      <c r="K4" s="257"/>
+      <c r="L4" s="257"/>
+      <c r="M4" s="258"/>
+      <c r="N4" s="256" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="251"/>
-      <c r="P4" s="251"/>
-      <c r="Q4" s="251"/>
-      <c r="R4" s="251"/>
-      <c r="S4" s="261"/>
-      <c r="T4" s="260"/>
-      <c r="U4" s="250" t="s">
+      <c r="O4" s="257"/>
+      <c r="P4" s="257"/>
+      <c r="Q4" s="257"/>
+      <c r="R4" s="257"/>
+      <c r="S4" s="260"/>
+      <c r="T4" s="258"/>
+      <c r="U4" s="256" t="s">
         <v>28</v>
       </c>
-      <c r="V4" s="258"/>
-      <c r="W4" s="267"/>
+      <c r="V4" s="259"/>
+      <c r="W4" s="235"/>
       <c r="X4" t="s">
         <v>0</v>
       </c>
@@ -13866,7 +13807,7 @@
       <c r="G5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="262" t="s">
+      <c r="H5" s="232" t="s">
         <v>525</v>
       </c>
       <c r="I5" s="13" t="s">
@@ -13878,16 +13819,16 @@
       <c r="K5" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="L5" s="259" t="s">
+      <c r="L5" s="231" t="s">
         <v>30</v>
       </c>
-      <c r="M5" s="263" t="s">
+      <c r="M5" s="233" t="s">
         <v>525</v>
       </c>
       <c r="N5" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="O5" s="262" t="s">
+      <c r="O5" s="232" t="s">
         <v>525</v>
       </c>
       <c r="P5" s="13" t="s">
@@ -13899,16 +13840,16 @@
       <c r="R5" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="S5" s="259" t="s">
+      <c r="S5" s="231" t="s">
         <v>31</v>
       </c>
-      <c r="T5" s="263" t="s">
+      <c r="T5" s="233" t="s">
         <v>525</v>
       </c>
       <c r="U5" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="V5" s="263" t="s">
+      <c r="V5" s="233" t="s">
         <v>525</v>
       </c>
       <c r="W5" t="s">
@@ -13965,7 +13906,7 @@
 'ETPT Format DDG'!$G:$G,"Magistrat")</f>
         <v>#N/A</v>
       </c>
-      <c r="M6" s="265" t="str">
+      <c r="M6" s="267" t="str">
         <f>IF(OR(LEFT(C6,3)="12.",LEFT(E6,3)="12.",LEFT(E6,5)="CET &gt;", IFERROR(L6/$L$6,"")=0),"", IFERROR(L6/$L$6,""))</f>
         <v/>
       </c>
@@ -13999,7 +13940,7 @@
 'ETPT Format DDG'!$G:$G,"Greffe")</f>
         <v>#N/A</v>
       </c>
-      <c r="T6" s="265" t="str">
+      <c r="T6" s="267" t="str">
         <f>IF(OR(LEFT(C6,3)="12.",LEFT(E6,3)="12.",LEFT(E6,5)="CET &gt;",IFERROR(S6/$S$6,"")=0),"", IFERROR(S6/$S$6,""))</f>
         <v/>
       </c>
@@ -14013,7 +13954,7 @@
 'ETPT Format DDG'!$G:$G,"Autour du magistrat")</f>
         <v>#N/A</v>
       </c>
-      <c r="V6" s="265" t="str">
+      <c r="V6" s="267" t="str">
         <f>IF(OR(LEFT(C6,3)="12.",LEFT(E6,3)="12.",LEFT(E6,5)="CET &gt;",IFERROR(U6/$U$6,"")=0),"", IFERROR(U6/$U$6,""))</f>
         <v/>
       </c>
@@ -14022,589 +13963,589 @@
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="I7" s="257"/>
+      <c r="I7" s="230"/>
       <c r="W7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="I8" s="257"/>
+      <c r="I8" s="230"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="I9" s="257"/>
+      <c r="I9" s="230"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="I10" s="257"/>
+      <c r="I10" s="230"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="I11" s="257"/>
+      <c r="I11" s="230"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="I12" s="257"/>
+      <c r="I12" s="230"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="I13" s="257"/>
+      <c r="I13" s="230"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="I14" s="257"/>
+      <c r="I14" s="230"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="I15" s="257"/>
+      <c r="I15" s="230"/>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="I16" s="257"/>
+      <c r="I16" s="230"/>
     </row>
     <row r="17" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I17" s="257"/>
+      <c r="I17" s="230"/>
     </row>
     <row r="18" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I18" s="257"/>
+      <c r="I18" s="230"/>
     </row>
     <row r="19" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I19" s="257"/>
+      <c r="I19" s="230"/>
     </row>
     <row r="20" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I20" s="257"/>
+      <c r="I20" s="230"/>
     </row>
     <row r="21" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I21" s="257"/>
+      <c r="I21" s="230"/>
     </row>
     <row r="22" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I22" s="257"/>
+      <c r="I22" s="230"/>
     </row>
     <row r="23" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I23" s="257"/>
+      <c r="I23" s="230"/>
     </row>
     <row r="24" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I24" s="257"/>
+      <c r="I24" s="230"/>
     </row>
     <row r="25" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I25" s="257"/>
+      <c r="I25" s="230"/>
     </row>
     <row r="26" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I26" s="257"/>
+      <c r="I26" s="230"/>
     </row>
     <row r="27" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I27" s="257"/>
+      <c r="I27" s="230"/>
     </row>
     <row r="28" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I28" s="257"/>
+      <c r="I28" s="230"/>
     </row>
     <row r="29" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I29" s="257"/>
+      <c r="I29" s="230"/>
     </row>
     <row r="30" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I30" s="257"/>
+      <c r="I30" s="230"/>
     </row>
     <row r="31" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I31" s="257"/>
+      <c r="I31" s="230"/>
     </row>
     <row r="32" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I32" s="257"/>
+      <c r="I32" s="230"/>
     </row>
     <row r="33" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I33" s="257"/>
+      <c r="I33" s="230"/>
     </row>
     <row r="34" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I34" s="257"/>
+      <c r="I34" s="230"/>
     </row>
     <row r="35" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I35" s="257"/>
+      <c r="I35" s="230"/>
     </row>
     <row r="36" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I36" s="257"/>
+      <c r="I36" s="230"/>
     </row>
     <row r="37" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I37" s="257"/>
+      <c r="I37" s="230"/>
     </row>
     <row r="38" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I38" s="257"/>
+      <c r="I38" s="230"/>
     </row>
     <row r="39" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I39" s="257"/>
+      <c r="I39" s="230"/>
     </row>
     <row r="40" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I40" s="257"/>
+      <c r="I40" s="230"/>
     </row>
     <row r="41" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I41" s="257"/>
+      <c r="I41" s="230"/>
     </row>
     <row r="42" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I42" s="257"/>
+      <c r="I42" s="230"/>
     </row>
     <row r="43" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I43" s="257"/>
+      <c r="I43" s="230"/>
     </row>
     <row r="44" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I44" s="257"/>
+      <c r="I44" s="230"/>
     </row>
     <row r="45" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I45" s="257"/>
+      <c r="I45" s="230"/>
     </row>
     <row r="46" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I46" s="257"/>
+      <c r="I46" s="230"/>
     </row>
     <row r="47" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I47" s="257"/>
+      <c r="I47" s="230"/>
     </row>
     <row r="48" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I48" s="257"/>
+      <c r="I48" s="230"/>
     </row>
     <row r="49" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I49" s="257"/>
+      <c r="I49" s="230"/>
     </row>
     <row r="50" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I50" s="257"/>
+      <c r="I50" s="230"/>
     </row>
     <row r="51" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I51" s="257"/>
+      <c r="I51" s="230"/>
     </row>
     <row r="52" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I52" s="257"/>
+      <c r="I52" s="230"/>
     </row>
     <row r="53" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I53" s="257"/>
+      <c r="I53" s="230"/>
     </row>
     <row r="54" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I54" s="257"/>
+      <c r="I54" s="230"/>
     </row>
     <row r="55" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I55" s="257"/>
+      <c r="I55" s="230"/>
     </row>
     <row r="56" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I56" s="257"/>
+      <c r="I56" s="230"/>
     </row>
     <row r="57" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I57" s="257"/>
+      <c r="I57" s="230"/>
     </row>
     <row r="58" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I58" s="257"/>
+      <c r="I58" s="230"/>
     </row>
     <row r="59" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I59" s="257"/>
+      <c r="I59" s="230"/>
     </row>
     <row r="60" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I60" s="257"/>
+      <c r="I60" s="230"/>
     </row>
     <row r="61" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I61" s="257"/>
+      <c r="I61" s="230"/>
     </row>
     <row r="62" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I62" s="257"/>
+      <c r="I62" s="230"/>
     </row>
     <row r="63" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I63" s="257"/>
+      <c r="I63" s="230"/>
     </row>
     <row r="64" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I64" s="257"/>
+      <c r="I64" s="230"/>
     </row>
     <row r="65" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I65" s="257"/>
+      <c r="I65" s="230"/>
     </row>
     <row r="66" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I66" s="257"/>
+      <c r="I66" s="230"/>
     </row>
     <row r="67" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I67" s="257"/>
+      <c r="I67" s="230"/>
     </row>
     <row r="68" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I68" s="257"/>
+      <c r="I68" s="230"/>
     </row>
     <row r="69" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I69" s="257"/>
+      <c r="I69" s="230"/>
     </row>
     <row r="70" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I70" s="257"/>
+      <c r="I70" s="230"/>
     </row>
     <row r="71" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I71" s="257"/>
+      <c r="I71" s="230"/>
     </row>
     <row r="72" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I72" s="257"/>
+      <c r="I72" s="230"/>
     </row>
     <row r="73" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I73" s="257"/>
+      <c r="I73" s="230"/>
     </row>
     <row r="74" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I74" s="257"/>
+      <c r="I74" s="230"/>
     </row>
     <row r="75" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I75" s="257"/>
+      <c r="I75" s="230"/>
     </row>
     <row r="76" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I76" s="257"/>
+      <c r="I76" s="230"/>
     </row>
     <row r="77" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I77" s="257"/>
+      <c r="I77" s="230"/>
     </row>
     <row r="78" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I78" s="257"/>
+      <c r="I78" s="230"/>
     </row>
     <row r="79" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I79" s="257"/>
+      <c r="I79" s="230"/>
     </row>
     <row r="80" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I80" s="257"/>
+      <c r="I80" s="230"/>
     </row>
     <row r="81" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I81" s="257"/>
+      <c r="I81" s="230"/>
     </row>
     <row r="82" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I82" s="257"/>
+      <c r="I82" s="230"/>
     </row>
     <row r="83" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I83" s="257"/>
+      <c r="I83" s="230"/>
     </row>
     <row r="84" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I84" s="257"/>
+      <c r="I84" s="230"/>
     </row>
     <row r="85" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I85" s="257"/>
+      <c r="I85" s="230"/>
     </row>
     <row r="86" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I86" s="257"/>
+      <c r="I86" s="230"/>
     </row>
     <row r="87" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I87" s="257"/>
+      <c r="I87" s="230"/>
     </row>
     <row r="88" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I88" s="257"/>
+      <c r="I88" s="230"/>
     </row>
     <row r="89" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I89" s="257"/>
+      <c r="I89" s="230"/>
     </row>
     <row r="90" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I90" s="257"/>
+      <c r="I90" s="230"/>
     </row>
     <row r="91" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I91" s="257"/>
+      <c r="I91" s="230"/>
     </row>
     <row r="92" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I92" s="257"/>
+      <c r="I92" s="230"/>
     </row>
     <row r="93" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I93" s="257"/>
+      <c r="I93" s="230"/>
     </row>
     <row r="94" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I94" s="257"/>
+      <c r="I94" s="230"/>
     </row>
     <row r="95" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I95" s="257"/>
+      <c r="I95" s="230"/>
     </row>
     <row r="96" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I96" s="257"/>
+      <c r="I96" s="230"/>
     </row>
     <row r="97" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I97" s="257"/>
+      <c r="I97" s="230"/>
     </row>
     <row r="98" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I98" s="257"/>
+      <c r="I98" s="230"/>
     </row>
     <row r="99" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I99" s="257"/>
+      <c r="I99" s="230"/>
     </row>
     <row r="100" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I100" s="257"/>
+      <c r="I100" s="230"/>
     </row>
     <row r="101" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I101" s="257"/>
+      <c r="I101" s="230"/>
     </row>
     <row r="102" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I102" s="257"/>
+      <c r="I102" s="230"/>
     </row>
     <row r="103" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I103" s="257"/>
+      <c r="I103" s="230"/>
     </row>
     <row r="104" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I104" s="257"/>
+      <c r="I104" s="230"/>
     </row>
     <row r="105" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I105" s="257"/>
+      <c r="I105" s="230"/>
     </row>
     <row r="106" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I106" s="257"/>
+      <c r="I106" s="230"/>
     </row>
     <row r="107" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I107" s="257"/>
+      <c r="I107" s="230"/>
     </row>
     <row r="108" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I108" s="257"/>
+      <c r="I108" s="230"/>
     </row>
     <row r="109" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I109" s="257"/>
+      <c r="I109" s="230"/>
     </row>
     <row r="110" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I110" s="257"/>
+      <c r="I110" s="230"/>
     </row>
     <row r="111" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I111" s="257"/>
+      <c r="I111" s="230"/>
     </row>
     <row r="112" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I112" s="257"/>
+      <c r="I112" s="230"/>
     </row>
     <row r="113" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I113" s="257"/>
+      <c r="I113" s="230"/>
     </row>
     <row r="114" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I114" s="257"/>
+      <c r="I114" s="230"/>
     </row>
     <row r="115" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I115" s="257"/>
+      <c r="I115" s="230"/>
     </row>
     <row r="116" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I116" s="257"/>
+      <c r="I116" s="230"/>
     </row>
     <row r="117" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I117" s="257"/>
+      <c r="I117" s="230"/>
     </row>
     <row r="118" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I118" s="257"/>
+      <c r="I118" s="230"/>
     </row>
     <row r="119" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I119" s="257"/>
+      <c r="I119" s="230"/>
     </row>
     <row r="120" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I120" s="257"/>
+      <c r="I120" s="230"/>
     </row>
     <row r="121" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I121" s="257"/>
+      <c r="I121" s="230"/>
     </row>
     <row r="122" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I122" s="257"/>
+      <c r="I122" s="230"/>
     </row>
     <row r="123" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I123" s="257"/>
+      <c r="I123" s="230"/>
     </row>
     <row r="124" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I124" s="257"/>
+      <c r="I124" s="230"/>
     </row>
     <row r="125" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I125" s="257"/>
+      <c r="I125" s="230"/>
     </row>
     <row r="126" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I126" s="257"/>
+      <c r="I126" s="230"/>
     </row>
     <row r="127" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I127" s="257"/>
+      <c r="I127" s="230"/>
     </row>
     <row r="128" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I128" s="257"/>
+      <c r="I128" s="230"/>
     </row>
     <row r="129" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I129" s="257"/>
+      <c r="I129" s="230"/>
     </row>
     <row r="130" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I130" s="257"/>
+      <c r="I130" s="230"/>
     </row>
     <row r="131" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I131" s="257"/>
+      <c r="I131" s="230"/>
     </row>
     <row r="132" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I132" s="257"/>
+      <c r="I132" s="230"/>
     </row>
     <row r="133" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I133" s="257"/>
+      <c r="I133" s="230"/>
     </row>
     <row r="134" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I134" s="257"/>
+      <c r="I134" s="230"/>
     </row>
     <row r="135" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I135" s="257"/>
+      <c r="I135" s="230"/>
     </row>
     <row r="136" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I136" s="257"/>
+      <c r="I136" s="230"/>
     </row>
     <row r="137" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I137" s="257"/>
+      <c r="I137" s="230"/>
     </row>
     <row r="138" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I138" s="257"/>
+      <c r="I138" s="230"/>
     </row>
     <row r="139" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I139" s="257"/>
+      <c r="I139" s="230"/>
     </row>
     <row r="140" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I140" s="257"/>
+      <c r="I140" s="230"/>
     </row>
     <row r="141" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I141" s="257"/>
+      <c r="I141" s="230"/>
     </row>
     <row r="142" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I142" s="257"/>
+      <c r="I142" s="230"/>
     </row>
     <row r="143" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I143" s="257"/>
+      <c r="I143" s="230"/>
     </row>
     <row r="144" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I144" s="257"/>
+      <c r="I144" s="230"/>
     </row>
     <row r="145" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I145" s="257"/>
+      <c r="I145" s="230"/>
     </row>
     <row r="146" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I146" s="257"/>
+      <c r="I146" s="230"/>
     </row>
     <row r="147" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I147" s="257"/>
+      <c r="I147" s="230"/>
     </row>
     <row r="148" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I148" s="257"/>
+      <c r="I148" s="230"/>
     </row>
     <row r="149" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I149" s="257"/>
+      <c r="I149" s="230"/>
     </row>
     <row r="150" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I150" s="257"/>
+      <c r="I150" s="230"/>
     </row>
     <row r="151" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I151" s="257"/>
+      <c r="I151" s="230"/>
     </row>
     <row r="152" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I152" s="257"/>
+      <c r="I152" s="230"/>
     </row>
     <row r="153" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I153" s="257"/>
+      <c r="I153" s="230"/>
     </row>
     <row r="154" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I154" s="257"/>
+      <c r="I154" s="230"/>
     </row>
     <row r="155" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I155" s="257"/>
+      <c r="I155" s="230"/>
     </row>
     <row r="156" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I156" s="257"/>
+      <c r="I156" s="230"/>
     </row>
     <row r="157" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I157" s="257"/>
+      <c r="I157" s="230"/>
     </row>
     <row r="158" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I158" s="257"/>
+      <c r="I158" s="230"/>
     </row>
     <row r="159" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I159" s="257"/>
+      <c r="I159" s="230"/>
     </row>
     <row r="160" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I160" s="257"/>
+      <c r="I160" s="230"/>
     </row>
     <row r="161" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I161" s="257"/>
+      <c r="I161" s="230"/>
     </row>
     <row r="162" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I162" s="257"/>
+      <c r="I162" s="230"/>
     </row>
     <row r="163" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I163" s="257"/>
+      <c r="I163" s="230"/>
     </row>
     <row r="164" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I164" s="257"/>
+      <c r="I164" s="230"/>
     </row>
     <row r="165" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I165" s="257"/>
+      <c r="I165" s="230"/>
     </row>
     <row r="166" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I166" s="257"/>
+      <c r="I166" s="230"/>
     </row>
     <row r="167" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I167" s="257"/>
+      <c r="I167" s="230"/>
     </row>
     <row r="168" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I168" s="257"/>
+      <c r="I168" s="230"/>
     </row>
     <row r="169" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I169" s="257"/>
+      <c r="I169" s="230"/>
     </row>
     <row r="170" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I170" s="257"/>
+      <c r="I170" s="230"/>
     </row>
     <row r="171" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I171" s="257"/>
+      <c r="I171" s="230"/>
     </row>
     <row r="172" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I172" s="257"/>
+      <c r="I172" s="230"/>
     </row>
     <row r="173" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I173" s="257"/>
+      <c r="I173" s="230"/>
     </row>
     <row r="174" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I174" s="257"/>
+      <c r="I174" s="230"/>
     </row>
     <row r="175" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I175" s="257"/>
+      <c r="I175" s="230"/>
     </row>
     <row r="176" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I176" s="257"/>
+      <c r="I176" s="230"/>
     </row>
     <row r="177" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I177" s="257"/>
+      <c r="I177" s="230"/>
     </row>
     <row r="178" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I178" s="257"/>
+      <c r="I178" s="230"/>
     </row>
     <row r="179" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I179" s="257"/>
+      <c r="I179" s="230"/>
     </row>
     <row r="180" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I180" s="257"/>
+      <c r="I180" s="230"/>
     </row>
     <row r="181" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I181" s="257"/>
+      <c r="I181" s="230"/>
     </row>
     <row r="182" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I182" s="257"/>
+      <c r="I182" s="230"/>
     </row>
     <row r="183" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I183" s="257"/>
+      <c r="I183" s="230"/>
     </row>
     <row r="184" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I184" s="257"/>
+      <c r="I184" s="230"/>
     </row>
     <row r="185" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I185" s="257"/>
+      <c r="I185" s="230"/>
     </row>
     <row r="186" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I186" s="257"/>
+      <c r="I186" s="230"/>
     </row>
     <row r="187" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I187" s="257"/>
+      <c r="I187" s="230"/>
     </row>
     <row r="188" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I188" s="257"/>
+      <c r="I188" s="230"/>
     </row>
     <row r="189" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I189" s="257"/>
+      <c r="I189" s="230"/>
     </row>
     <row r="190" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I190" s="257"/>
+      <c r="I190" s="230"/>
     </row>
     <row r="191" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I191" s="257"/>
+      <c r="I191" s="230"/>
     </row>
     <row r="192" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I192" s="257"/>
+      <c r="I192" s="230"/>
     </row>
     <row r="193" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I193" s="257"/>
+      <c r="I193" s="230"/>
     </row>
     <row r="194" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I194" s="257"/>
+      <c r="I194" s="230"/>
     </row>
     <row r="195" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I195" s="257"/>
+      <c r="I195" s="230"/>
     </row>
     <row r="196" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I196" s="257"/>
+      <c r="I196" s="230"/>
     </row>
     <row r="197" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I197" s="257"/>
+      <c r="I197" s="230"/>
     </row>
     <row r="198" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I198" s="257"/>
+      <c r="I198" s="230"/>
     </row>
     <row r="199" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I199" s="257"/>
+      <c r="I199" s="230"/>
     </row>
     <row r="200" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I200" s="257"/>
+      <c r="I200" s="230"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -14612,13 +14553,13 @@
     <mergeCell ref="U4:V4"/>
     <mergeCell ref="N4:T4"/>
   </mergeCells>
-  <conditionalFormatting sqref="C6:V151">
-    <cfRule type="expression" dxfId="1" priority="2">
+  <conditionalFormatting sqref="C6">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>AND(ISBLANK($D6)=FALSE,ISBLANK($F6)=TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <conditionalFormatting sqref="C6:V151">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>AND(ISBLANK($D6)=FALSE,ISBLANK($F6)=TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16139,16 +16080,16 @@
   <sheetData>
     <row r="1" spans="1:62" s="59" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A1" s="102"/>
-      <c r="B1" s="253" t="s">
+      <c r="B1" s="262" t="s">
         <v>437</v>
       </c>
-      <c r="C1" s="253"/>
-      <c r="D1" s="253"/>
-      <c r="E1" s="253"/>
-      <c r="F1" s="253"/>
-      <c r="G1" s="253"/>
-      <c r="H1" s="253"/>
-      <c r="I1" s="253"/>
+      <c r="C1" s="262"/>
+      <c r="D1" s="262"/>
+      <c r="E1" s="262"/>
+      <c r="F1" s="262"/>
+      <c r="G1" s="262"/>
+      <c r="H1" s="262"/>
+      <c r="I1" s="262"/>
       <c r="AC1" s="101"/>
       <c r="AD1" s="101"/>
       <c r="AE1" s="101"/>
@@ -16169,7 +16110,7 @@
       <c r="G2" s="97" t="s">
         <v>436</v>
       </c>
-      <c r="H2" s="252" t="s">
+      <c r="H2" s="261" t="s">
         <v>435</v>
       </c>
       <c r="I2" s="96" t="s">
@@ -16214,7 +16155,7 @@
       <c r="V2" s="96" t="s">
         <v>434</v>
       </c>
-      <c r="W2" s="252" t="s">
+      <c r="W2" s="261" t="s">
         <v>433</v>
       </c>
       <c r="X2" s="97" t="s">
@@ -16229,7 +16170,7 @@
       <c r="AA2" s="97" t="s">
         <v>150</v>
       </c>
-      <c r="AB2" s="252" t="s">
+      <c r="AB2" s="261" t="s">
         <v>432</v>
       </c>
       <c r="AC2" s="93" t="s">
@@ -16259,7 +16200,7 @@
       <c r="AK2" s="93" t="s">
         <v>431</v>
       </c>
-      <c r="AL2" s="252" t="s">
+      <c r="AL2" s="261" t="s">
         <v>430</v>
       </c>
       <c r="AM2" s="93" t="s">
@@ -16301,7 +16242,7 @@
       <c r="AY2" s="93" t="s">
         <v>429</v>
       </c>
-      <c r="AZ2" s="252" t="s">
+      <c r="AZ2" s="261" t="s">
         <v>428</v>
       </c>
       <c r="BA2" s="92" t="s">
@@ -16331,7 +16272,7 @@
       <c r="BI2" s="92" t="s">
         <v>427</v>
       </c>
-      <c r="BJ2" s="252" t="s">
+      <c r="BJ2" s="261" t="s">
         <v>426</v>
       </c>
     </row>
@@ -16345,7 +16286,7 @@
       <c r="G3" s="97" t="s">
         <v>425</v>
       </c>
-      <c r="H3" s="252"/>
+      <c r="H3" s="261"/>
       <c r="I3" s="96" t="s">
         <v>424</v>
       </c>
@@ -16386,7 +16327,7 @@
       <c r="V3" s="96" t="s">
         <v>412</v>
       </c>
-      <c r="W3" s="252"/>
+      <c r="W3" s="261"/>
       <c r="X3" s="91"/>
       <c r="Y3" s="97" t="s">
         <v>411</v>
@@ -16397,7 +16338,7 @@
       <c r="AA3" s="97" t="s">
         <v>409</v>
       </c>
-      <c r="AB3" s="252"/>
+      <c r="AB3" s="261"/>
       <c r="AC3" s="93" t="s">
         <v>408</v>
       </c>
@@ -16425,7 +16366,7 @@
       <c r="AK3" s="93" t="s">
         <v>402</v>
       </c>
-      <c r="AL3" s="252"/>
+      <c r="AL3" s="261"/>
       <c r="AM3" s="93" t="s">
         <v>401</v>
       </c>
@@ -16465,7 +16406,7 @@
       <c r="AY3" s="93" t="s">
         <v>389</v>
       </c>
-      <c r="AZ3" s="252"/>
+      <c r="AZ3" s="261"/>
       <c r="BA3" s="92" t="s">
         <v>388</v>
       </c>
@@ -16493,7 +16434,7 @@
       <c r="BI3" s="92" t="s">
         <v>380</v>
       </c>
-      <c r="BJ3" s="252"/>
+      <c r="BJ3" s="261"/>
     </row>
     <row r="4" spans="1:62" s="59" customFormat="1" ht="60" x14ac:dyDescent="0.15">
       <c r="A4" s="99"/>
@@ -16515,7 +16456,7 @@
       <c r="G4" s="97" t="s">
         <v>375</v>
       </c>
-      <c r="H4" s="252"/>
+      <c r="H4" s="261"/>
       <c r="I4" s="96" t="s">
         <v>374</v>
       </c>
@@ -16558,7 +16499,7 @@
       <c r="V4" s="95" t="s">
         <v>361</v>
       </c>
-      <c r="W4" s="252"/>
+      <c r="W4" s="261"/>
       <c r="X4" s="94" t="s">
         <v>360</v>
       </c>
@@ -16571,7 +16512,7 @@
       <c r="AA4" s="94" t="s">
         <v>357</v>
       </c>
-      <c r="AB4" s="252"/>
+      <c r="AB4" s="261"/>
       <c r="AC4" s="93" t="s">
         <v>356</v>
       </c>
@@ -16599,7 +16540,7 @@
       <c r="AK4" s="93" t="s">
         <v>349</v>
       </c>
-      <c r="AL4" s="252"/>
+      <c r="AL4" s="261"/>
       <c r="AM4" s="93" t="s">
         <v>348</v>
       </c>
@@ -16639,7 +16580,7 @@
       <c r="AY4" s="93" t="s">
         <v>336</v>
       </c>
-      <c r="AZ4" s="252"/>
+      <c r="AZ4" s="261"/>
       <c r="BA4" s="92" t="s">
         <v>335</v>
       </c>
@@ -16667,7 +16608,7 @@
       <c r="BI4" s="92" t="s">
         <v>327</v>
       </c>
-      <c r="BJ4" s="252"/>
+      <c r="BJ4" s="261"/>
     </row>
     <row r="5" spans="1:62" s="59" customFormat="1" ht="144" x14ac:dyDescent="0.15">
       <c r="A5" s="67" t="s">
@@ -17645,7 +17586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:62" s="59" customFormat="1" ht="48" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:62" s="59" customFormat="1" ht="36" x14ac:dyDescent="0.15">
       <c r="A13" s="67" t="s">
         <v>231</v>
       </c>
@@ -18366,16 +18307,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" s="107" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B1" s="255" t="s">
+      <c r="B1" s="264" t="s">
         <v>437</v>
       </c>
-      <c r="C1" s="255"/>
-      <c r="D1" s="255"/>
-      <c r="E1" s="255"/>
-      <c r="F1" s="255"/>
-      <c r="G1" s="255"/>
-      <c r="H1" s="255"/>
-      <c r="I1" s="255"/>
+      <c r="C1" s="264"/>
+      <c r="D1" s="264"/>
+      <c r="E1" s="264"/>
+      <c r="F1" s="264"/>
+      <c r="G1" s="264"/>
+      <c r="H1" s="264"/>
+      <c r="I1" s="264"/>
     </row>
     <row r="2" spans="1:62" s="107" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="153"/>
@@ -18387,7 +18328,7 @@
       <c r="G2" s="150" t="s">
         <v>436</v>
       </c>
-      <c r="H2" s="254" t="s">
+      <c r="H2" s="263" t="s">
         <v>435</v>
       </c>
       <c r="I2" s="149" t="s">
@@ -18432,7 +18373,7 @@
       <c r="V2" s="149" t="s">
         <v>434</v>
       </c>
-      <c r="W2" s="254" t="s">
+      <c r="W2" s="263" t="s">
         <v>433</v>
       </c>
       <c r="X2" s="150" t="s">
@@ -18447,7 +18388,7 @@
       <c r="AA2" s="150" t="s">
         <v>150</v>
       </c>
-      <c r="AB2" s="254" t="s">
+      <c r="AB2" s="263" t="s">
         <v>432</v>
       </c>
       <c r="AC2" s="147" t="s">
@@ -18477,7 +18418,7 @@
       <c r="AK2" s="147" t="s">
         <v>431</v>
       </c>
-      <c r="AL2" s="254" t="s">
+      <c r="AL2" s="263" t="s">
         <v>430</v>
       </c>
       <c r="AM2" s="147" t="s">
@@ -18519,7 +18460,7 @@
       <c r="AY2" s="147" t="s">
         <v>429</v>
       </c>
-      <c r="AZ2" s="254" t="s">
+      <c r="AZ2" s="263" t="s">
         <v>428</v>
       </c>
       <c r="BA2" s="146" t="s">
@@ -18549,7 +18490,7 @@
       <c r="BI2" s="146" t="s">
         <v>427</v>
       </c>
-      <c r="BJ2" s="254" t="s">
+      <c r="BJ2" s="263" t="s">
         <v>426</v>
       </c>
     </row>
@@ -18563,7 +18504,7 @@
       <c r="G3" s="150" t="s">
         <v>425</v>
       </c>
-      <c r="H3" s="254"/>
+      <c r="H3" s="263"/>
       <c r="I3" s="149" t="s">
         <v>424</v>
       </c>
@@ -18604,7 +18545,7 @@
       <c r="V3" s="149" t="s">
         <v>412</v>
       </c>
-      <c r="W3" s="254"/>
+      <c r="W3" s="263"/>
       <c r="X3" s="145"/>
       <c r="Y3" s="150" t="s">
         <v>411</v>
@@ -18615,7 +18556,7 @@
       <c r="AA3" s="150" t="s">
         <v>409</v>
       </c>
-      <c r="AB3" s="254"/>
+      <c r="AB3" s="263"/>
       <c r="AC3" s="147" t="s">
         <v>408</v>
       </c>
@@ -18643,7 +18584,7 @@
       <c r="AK3" s="147" t="s">
         <v>402</v>
       </c>
-      <c r="AL3" s="254"/>
+      <c r="AL3" s="263"/>
       <c r="AM3" s="147" t="s">
         <v>401</v>
       </c>
@@ -18683,7 +18624,7 @@
       <c r="AY3" s="147" t="s">
         <v>389</v>
       </c>
-      <c r="AZ3" s="254"/>
+      <c r="AZ3" s="263"/>
       <c r="BA3" s="146" t="s">
         <v>388</v>
       </c>
@@ -18711,7 +18652,7 @@
       <c r="BI3" s="146" t="s">
         <v>380</v>
       </c>
-      <c r="BJ3" s="254"/>
+      <c r="BJ3" s="263"/>
     </row>
     <row r="4" spans="1:62" s="107" customFormat="1" ht="60" x14ac:dyDescent="0.15">
       <c r="A4" s="152"/>
@@ -18733,7 +18674,7 @@
       <c r="G4" s="150" t="s">
         <v>375</v>
       </c>
-      <c r="H4" s="254"/>
+      <c r="H4" s="263"/>
       <c r="I4" s="149" t="s">
         <v>374</v>
       </c>
@@ -18776,7 +18717,7 @@
       <c r="V4" s="149" t="s">
         <v>361</v>
       </c>
-      <c r="W4" s="254"/>
+      <c r="W4" s="263"/>
       <c r="X4" s="148" t="s">
         <v>360</v>
       </c>
@@ -18789,7 +18730,7 @@
       <c r="AA4" s="148" t="s">
         <v>357</v>
       </c>
-      <c r="AB4" s="254"/>
+      <c r="AB4" s="263"/>
       <c r="AC4" s="147" t="s">
         <v>356</v>
       </c>
@@ -18817,7 +18758,7 @@
       <c r="AK4" s="147" t="s">
         <v>349</v>
       </c>
-      <c r="AL4" s="254"/>
+      <c r="AL4" s="263"/>
       <c r="AM4" s="147" t="s">
         <v>348</v>
       </c>
@@ -18857,7 +18798,7 @@
       <c r="AY4" s="147" t="s">
         <v>336</v>
       </c>
-      <c r="AZ4" s="254"/>
+      <c r="AZ4" s="263"/>
       <c r="BA4" s="146" t="s">
         <v>335</v>
       </c>
@@ -18885,7 +18826,7 @@
       <c r="BI4" s="146" t="s">
         <v>327</v>
       </c>
-      <c r="BJ4" s="254"/>
+      <c r="BJ4" s="263"/>
     </row>
     <row r="5" spans="1:62" s="107" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="117" t="s">

</xml_diff>

<commit_message>
attaché de justice extracteur CA et TJ
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D69408-9140-1F4F-916F-2356CC71142F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956251AA-BB3D-9C4F-A9C1-8FA0D21741F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1947" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1948" uniqueCount="580">
   <si>
     <t>#! END_ROW</t>
   </si>
@@ -5203,6 +5203,12 @@
       </rPr>
       <t>Critère sur le TPRX</t>
     </r>
+  </si>
+  <si>
+    <t>Att J</t>
+  </si>
+  <si>
+    <t>Pas encore appelé dans la matrice DDG, à voir en fonction de la circulaire 2025/2026</t>
   </si>
 </sst>
 </file>
@@ -6398,7 +6404,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="374">
+  <cellXfs count="373">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -7471,6 +7477,55 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="169" fontId="67" fillId="16" borderId="13" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="71" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="42" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="41" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7587,56 +7642,6 @@
     </xf>
     <xf numFmtId="0" fontId="55" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="67" fillId="16" borderId="13" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="71" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="42" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
   </cellXfs>
@@ -8447,11 +8452,11 @@
       <c r="B1" s="145" t="s">
         <v>384</v>
       </c>
-      <c r="C1" s="321" t="s">
+      <c r="C1" s="336" t="s">
         <v>385</v>
       </c>
-      <c r="D1" s="321"/>
-      <c r="E1" s="321"/>
+      <c r="D1" s="336"/>
+      <c r="E1" s="336"/>
       <c r="F1" s="146"/>
       <c r="H1" s="26" t="s">
         <v>0</v>
@@ -8460,11 +8465,11 @@
     <row r="2" spans="1:8" s="150" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="147"/>
       <c r="B2" s="148"/>
-      <c r="C2" s="322" t="s">
+      <c r="C2" s="337" t="s">
         <v>386</v>
       </c>
-      <c r="D2" s="322"/>
-      <c r="E2" s="322"/>
+      <c r="D2" s="337"/>
+      <c r="E2" s="337"/>
       <c r="F2" s="149"/>
       <c r="H2" s="26" t="s">
         <v>0</v>
@@ -8488,10 +8493,10 @@
       <c r="D4" s="155" t="s">
         <v>389</v>
       </c>
-      <c r="E4" s="328" t="s">
+      <c r="E4" s="343" t="s">
         <v>390</v>
       </c>
-      <c r="F4" s="329"/>
+      <c r="F4" s="344"/>
       <c r="G4" s="164"/>
       <c r="H4" s="26" t="s">
         <v>0</v>
@@ -8508,10 +8513,10 @@
       <c r="D5" s="161" t="s">
         <v>393</v>
       </c>
-      <c r="E5" s="330" t="s">
+      <c r="E5" s="345" t="s">
         <v>406</v>
       </c>
-      <c r="F5" s="331"/>
+      <c r="F5" s="346"/>
       <c r="G5" s="163"/>
       <c r="H5" s="26" t="s">
         <v>0</v>
@@ -8528,10 +8533,10 @@
       <c r="D6" s="162" t="s">
         <v>396</v>
       </c>
-      <c r="E6" s="332" t="s">
+      <c r="E6" s="347" t="s">
         <v>407</v>
       </c>
-      <c r="F6" s="333"/>
+      <c r="F6" s="348"/>
       <c r="G6" s="163"/>
       <c r="H6" s="26" t="s">
         <v>0</v>
@@ -8548,10 +8553,10 @@
       <c r="D7" s="162" t="s">
         <v>399</v>
       </c>
-      <c r="E7" s="332" t="s">
+      <c r="E7" s="347" t="s">
         <v>406</v>
       </c>
-      <c r="F7" s="333"/>
+      <c r="F7" s="348"/>
       <c r="G7" s="163"/>
       <c r="H7" s="26" t="s">
         <v>0</v>
@@ -8562,16 +8567,16 @@
       <c r="B8" s="171" t="s">
         <v>400</v>
       </c>
-      <c r="C8" s="323" t="s">
+      <c r="C8" s="338" t="s">
         <v>401</v>
       </c>
-      <c r="D8" s="323" t="s">
+      <c r="D8" s="338" t="s">
         <v>402</v>
       </c>
-      <c r="E8" s="334" t="s">
+      <c r="E8" s="349" t="s">
         <v>408</v>
       </c>
-      <c r="F8" s="335"/>
+      <c r="F8" s="350"/>
       <c r="G8" s="163"/>
       <c r="H8" s="26" t="s">
         <v>0</v>
@@ -8582,10 +8587,10 @@
       <c r="B9" s="172" t="s">
         <v>403</v>
       </c>
-      <c r="C9" s="323"/>
-      <c r="D9" s="323"/>
-      <c r="E9" s="336"/>
-      <c r="F9" s="337"/>
+      <c r="C9" s="338"/>
+      <c r="D9" s="338"/>
+      <c r="E9" s="351"/>
+      <c r="F9" s="352"/>
       <c r="G9" s="163"/>
       <c r="H9" s="26" t="s">
         <v>0</v>
@@ -8596,10 +8601,10 @@
       <c r="B10" s="173" t="s">
         <v>404</v>
       </c>
-      <c r="C10" s="324"/>
-      <c r="D10" s="324"/>
-      <c r="E10" s="338"/>
-      <c r="F10" s="339"/>
+      <c r="C10" s="339"/>
+      <c r="D10" s="339"/>
+      <c r="E10" s="353"/>
+      <c r="F10" s="354"/>
       <c r="G10" s="163"/>
       <c r="H10" s="26" t="s">
         <v>0</v>
@@ -8619,11 +8624,11 @@
     <row r="12" spans="1:8" s="26" customFormat="1" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="151"/>
       <c r="B12" s="165"/>
-      <c r="C12" s="327" t="s">
+      <c r="C12" s="342" t="s">
         <v>405</v>
       </c>
-      <c r="D12" s="327"/>
-      <c r="E12" s="327"/>
+      <c r="D12" s="342"/>
+      <c r="E12" s="342"/>
       <c r="F12" s="166"/>
       <c r="H12" s="26" t="s">
         <v>0</v>
@@ -8637,14 +8642,14 @@
       </c>
     </row>
     <row r="14" spans="1:8" s="26" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="325" t="s">
+      <c r="A14" s="340" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="325"/>
-      <c r="C14" s="325"/>
-      <c r="D14" s="325"/>
-      <c r="E14" s="325"/>
-      <c r="F14" s="326"/>
+      <c r="B14" s="340"/>
+      <c r="C14" s="340"/>
+      <c r="D14" s="340"/>
+      <c r="E14" s="340"/>
+      <c r="F14" s="341"/>
       <c r="H14" s="26" t="s">
         <v>0</v>
       </c>
@@ -8717,13 +8722,13 @@
       <c r="G2" s="103" t="s">
         <v>326</v>
       </c>
-      <c r="H2" s="347" t="s">
+      <c r="H2" s="362" t="s">
         <v>325</v>
       </c>
       <c r="I2" s="103" t="s">
         <v>144</v>
       </c>
-      <c r="J2" s="347" t="s">
+      <c r="J2" s="362" t="s">
         <v>324</v>
       </c>
     </row>
@@ -8737,11 +8742,11 @@
       <c r="G3" s="103" t="s">
         <v>304</v>
       </c>
-      <c r="H3" s="347"/>
+      <c r="H3" s="362"/>
       <c r="I3" s="103" t="s">
         <v>301</v>
       </c>
-      <c r="J3" s="347"/>
+      <c r="J3" s="362"/>
     </row>
     <row r="4" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A4" s="125"/>
@@ -8763,11 +8768,11 @@
       <c r="G4" s="103" t="s">
         <v>253</v>
       </c>
-      <c r="H4" s="347"/>
+      <c r="H4" s="362"/>
       <c r="I4" s="103" t="s">
         <v>249</v>
       </c>
-      <c r="J4" s="347"/>
+      <c r="J4" s="362"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="119" t="s">
@@ -9171,7 +9176,7 @@
       <c r="G2" s="103" t="s">
         <v>328</v>
       </c>
-      <c r="H2" s="347" t="s">
+      <c r="H2" s="362" t="s">
         <v>327</v>
       </c>
       <c r="I2" s="102" t="s">
@@ -9216,7 +9221,7 @@
       <c r="V2" s="102" t="s">
         <v>326</v>
       </c>
-      <c r="W2" s="347" t="s">
+      <c r="W2" s="362" t="s">
         <v>325</v>
       </c>
       <c r="X2" s="103" t="s">
@@ -9231,7 +9236,7 @@
       <c r="AA2" s="103" t="s">
         <v>144</v>
       </c>
-      <c r="AB2" s="347" t="s">
+      <c r="AB2" s="362" t="s">
         <v>324</v>
       </c>
       <c r="AC2" s="100" t="s">
@@ -9261,7 +9266,7 @@
       <c r="AK2" s="100" t="s">
         <v>323</v>
       </c>
-      <c r="AL2" s="347" t="s">
+      <c r="AL2" s="362" t="s">
         <v>322</v>
       </c>
       <c r="AM2" s="100" t="s">
@@ -9303,7 +9308,7 @@
       <c r="AY2" s="100" t="s">
         <v>321</v>
       </c>
-      <c r="AZ2" s="347" t="s">
+      <c r="AZ2" s="362" t="s">
         <v>320</v>
       </c>
       <c r="BA2" s="99" t="s">
@@ -9333,7 +9338,7 @@
       <c r="BI2" s="99" t="s">
         <v>319</v>
       </c>
-      <c r="BJ2" s="347" t="s">
+      <c r="BJ2" s="362" t="s">
         <v>318</v>
       </c>
       <c r="BK2"/>
@@ -9348,7 +9353,7 @@
       <c r="G3" s="103" t="s">
         <v>317</v>
       </c>
-      <c r="H3" s="347"/>
+      <c r="H3" s="362"/>
       <c r="I3" s="102" t="s">
         <v>316</v>
       </c>
@@ -9389,7 +9394,7 @@
       <c r="V3" s="102" t="s">
         <v>304</v>
       </c>
-      <c r="W3" s="347"/>
+      <c r="W3" s="362"/>
       <c r="X3" s="98"/>
       <c r="Y3" s="103" t="s">
         <v>303</v>
@@ -9400,7 +9405,7 @@
       <c r="AA3" s="103" t="s">
         <v>301</v>
       </c>
-      <c r="AB3" s="347"/>
+      <c r="AB3" s="362"/>
       <c r="AC3" s="100" t="s">
         <v>300</v>
       </c>
@@ -9428,7 +9433,7 @@
       <c r="AK3" s="100" t="s">
         <v>294</v>
       </c>
-      <c r="AL3" s="347"/>
+      <c r="AL3" s="362"/>
       <c r="AM3" s="100" t="s">
         <v>293</v>
       </c>
@@ -9468,7 +9473,7 @@
       <c r="AY3" s="100" t="s">
         <v>281</v>
       </c>
-      <c r="AZ3" s="347"/>
+      <c r="AZ3" s="362"/>
       <c r="BA3" s="99" t="s">
         <v>280</v>
       </c>
@@ -9496,7 +9501,7 @@
       <c r="BI3" s="99" t="s">
         <v>272</v>
       </c>
-      <c r="BJ3" s="347"/>
+      <c r="BJ3" s="362"/>
     </row>
     <row r="4" spans="1:63" s="60" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="105"/>
@@ -9518,7 +9523,7 @@
       <c r="G4" s="103" t="s">
         <v>267</v>
       </c>
-      <c r="H4" s="347"/>
+      <c r="H4" s="362"/>
       <c r="I4" s="102" t="s">
         <v>266</v>
       </c>
@@ -9561,7 +9566,7 @@
       <c r="V4" s="102" t="s">
         <v>253</v>
       </c>
-      <c r="W4" s="347"/>
+      <c r="W4" s="362"/>
       <c r="X4" s="101" t="s">
         <v>252</v>
       </c>
@@ -9574,7 +9579,7 @@
       <c r="AA4" s="101" t="s">
         <v>249</v>
       </c>
-      <c r="AB4" s="347"/>
+      <c r="AB4" s="362"/>
       <c r="AC4" s="100" t="s">
         <v>248</v>
       </c>
@@ -9602,7 +9607,7 @@
       <c r="AK4" s="100" t="s">
         <v>241</v>
       </c>
-      <c r="AL4" s="347"/>
+      <c r="AL4" s="362"/>
       <c r="AM4" s="100" t="s">
         <v>240</v>
       </c>
@@ -9642,7 +9647,7 @@
       <c r="AY4" s="100" t="s">
         <v>228</v>
       </c>
-      <c r="AZ4" s="347"/>
+      <c r="AZ4" s="362"/>
       <c r="BA4" s="99" t="s">
         <v>227</v>
       </c>
@@ -9670,7 +9675,7 @@
       <c r="BI4" s="99" t="s">
         <v>219</v>
       </c>
-      <c r="BJ4" s="347"/>
+      <c r="BJ4" s="362"/>
       <c r="BK4"/>
     </row>
     <row r="5" spans="1:63" s="60" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -12282,15 +12287,15 @@
       </c>
     </row>
     <row r="19" spans="4:52" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="4:52" ht="280" x14ac:dyDescent="0.2">
-      <c r="F20" s="360" t="s">
+    <row r="20" spans="4:52" ht="28" x14ac:dyDescent="0.2">
+      <c r="F20" s="323" t="s">
         <v>553</v>
       </c>
       <c r="G20" s="254" t="str">
         <f>IF(ISBLANK(ETPT_TJ_DDG!$D$5),"",IF(ISERROR(ETPT_TJ!G20),"",IF(ETPT_TJ!G20=0,"",ETPT_TJ!G20)))</f>
         <v/>
       </c>
-      <c r="U20" s="361" t="s">
+      <c r="U20" s="324" t="s">
         <v>555</v>
       </c>
       <c r="V20" s="254" t="str">
@@ -12298,7 +12303,7 @@
         <v/>
       </c>
       <c r="AH20" s="57"/>
-      <c r="AX20" s="359" t="s">
+      <c r="AX20" s="322" t="s">
         <v>551</v>
       </c>
       <c r="AY20" s="196" t="str">
@@ -12420,7 +12425,7 @@
       <c r="G2" s="103" t="s">
         <v>328</v>
       </c>
-      <c r="H2" s="347" t="s">
+      <c r="H2" s="362" t="s">
         <v>327</v>
       </c>
       <c r="I2" s="103" t="s">
@@ -12453,13 +12458,13 @@
       <c r="R2" s="103" t="s">
         <v>326</v>
       </c>
-      <c r="S2" s="347" t="s">
+      <c r="S2" s="362" t="s">
         <v>325</v>
       </c>
       <c r="T2" s="103" t="s">
         <v>144</v>
       </c>
-      <c r="U2" s="347" t="s">
+      <c r="U2" s="362" t="s">
         <v>324</v>
       </c>
       <c r="V2" s="103" t="s">
@@ -12489,7 +12494,7 @@
       <c r="AD2" s="103" t="s">
         <v>323</v>
       </c>
-      <c r="AE2" s="347" t="s">
+      <c r="AE2" s="362" t="s">
         <v>372</v>
       </c>
       <c r="AF2" s="103" t="s">
@@ -12501,7 +12506,7 @@
       <c r="AH2" s="103" t="s">
         <v>371</v>
       </c>
-      <c r="AI2" s="347" t="s">
+      <c r="AI2" s="362" t="s">
         <v>370</v>
       </c>
     </row>
@@ -12515,7 +12520,7 @@
       <c r="G3" s="103" t="s">
         <v>317</v>
       </c>
-      <c r="H3" s="347"/>
+      <c r="H3" s="362"/>
       <c r="I3" s="103" t="s">
         <v>369</v>
       </c>
@@ -12546,11 +12551,11 @@
       <c r="R3" s="103" t="s">
         <v>304</v>
       </c>
-      <c r="S3" s="347"/>
+      <c r="S3" s="362"/>
       <c r="T3" s="103" t="s">
         <v>301</v>
       </c>
-      <c r="U3" s="347"/>
+      <c r="U3" s="362"/>
       <c r="V3" s="103" t="s">
         <v>360</v>
       </c>
@@ -12578,7 +12583,7 @@
       <c r="AD3" s="103" t="s">
         <v>352</v>
       </c>
-      <c r="AE3" s="347"/>
+      <c r="AE3" s="362"/>
       <c r="AF3" s="103" t="s">
         <v>351</v>
       </c>
@@ -12588,7 +12593,7 @@
       <c r="AH3" s="103" t="s">
         <v>281</v>
       </c>
-      <c r="AI3" s="347"/>
+      <c r="AI3" s="362"/>
     </row>
     <row r="4" spans="1:62" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="106"/>
@@ -12610,7 +12615,7 @@
       <c r="G4" s="103" t="s">
         <v>267</v>
       </c>
-      <c r="H4" s="347"/>
+      <c r="H4" s="362"/>
       <c r="I4" s="103" t="s">
         <v>350</v>
       </c>
@@ -12641,11 +12646,11 @@
       <c r="R4" s="103" t="s">
         <v>253</v>
       </c>
-      <c r="S4" s="347"/>
+      <c r="S4" s="362"/>
       <c r="T4" s="103" t="s">
         <v>249</v>
       </c>
-      <c r="U4" s="347"/>
+      <c r="U4" s="362"/>
       <c r="V4" s="103" t="s">
         <v>341</v>
       </c>
@@ -12673,7 +12678,7 @@
       <c r="AD4" s="103" t="s">
         <v>333</v>
       </c>
-      <c r="AE4" s="347"/>
+      <c r="AE4" s="362"/>
       <c r="AF4" s="103" t="s">
         <v>332</v>
       </c>
@@ -12683,7 +12688,7 @@
       <c r="AH4" s="103" t="s">
         <v>228</v>
       </c>
-      <c r="AI4" s="347"/>
+      <c r="AI4" s="362"/>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A5" s="109" t="s">
@@ -14275,9 +14280,9 @@
       <c r="S17" s="59"/>
     </row>
     <row r="18" spans="4:34" ht="93" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D18" s="363"/>
-      <c r="E18" s="364"/>
-      <c r="F18" s="360" t="s">
+      <c r="D18" s="326"/>
+      <c r="E18"/>
+      <c r="F18" s="323" t="s">
         <v>553</v>
       </c>
       <c r="G18" s="254" t="str">
@@ -14288,15 +14293,15 @@
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
-      <c r="Q18" s="361" t="s">
+      <c r="Q18" s="324" t="s">
         <v>555</v>
       </c>
       <c r="R18" s="254" t="str">
         <f>IF(ISBLANK(ETPT_TPRX_DDG!$D$5),"",IF(ISERROR(ETPT_TPRX!R18),"",IF(ETPT_TPRX!R18=0,"",ETPT_TPRX!R18)))</f>
         <v/>
       </c>
-      <c r="AF18" s="362"/>
-      <c r="AG18" s="359" t="s">
+      <c r="AF18" s="325"/>
+      <c r="AG18" s="322" t="s">
         <v>551</v>
       </c>
       <c r="AH18" s="254" t="str">
@@ -14440,13 +14445,13 @@
       <c r="G2" s="103" t="s">
         <v>326</v>
       </c>
-      <c r="H2" s="347" t="s">
+      <c r="H2" s="362" t="s">
         <v>325</v>
       </c>
       <c r="I2" s="103" t="s">
         <v>144</v>
       </c>
-      <c r="J2" s="347" t="s">
+      <c r="J2" s="362" t="s">
         <v>324</v>
       </c>
     </row>
@@ -14460,11 +14465,11 @@
       <c r="G3" s="103" t="s">
         <v>304</v>
       </c>
-      <c r="H3" s="347"/>
+      <c r="H3" s="362"/>
       <c r="I3" s="103" t="s">
         <v>301</v>
       </c>
-      <c r="J3" s="347"/>
+      <c r="J3" s="362"/>
     </row>
     <row r="4" spans="1:62" ht="36" x14ac:dyDescent="0.2">
       <c r="A4" s="125"/>
@@ -14486,11 +14491,11 @@
       <c r="G4" s="103" t="s">
         <v>253</v>
       </c>
-      <c r="H4" s="347"/>
+      <c r="H4" s="362"/>
       <c r="I4" s="103" t="s">
         <v>249</v>
       </c>
-      <c r="J4" s="347"/>
+      <c r="J4" s="362"/>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A5" s="119" t="s">
@@ -14885,13 +14890,13 @@
   <sheetData>
     <row r="1" spans="1:61" s="186" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="185"/>
-      <c r="B1" s="351" t="s">
+      <c r="B1" s="366" t="s">
         <v>329</v>
       </c>
-      <c r="C1" s="351"/>
-      <c r="D1" s="351"/>
-      <c r="E1" s="351"/>
-      <c r="F1" s="351"/>
+      <c r="C1" s="366"/>
+      <c r="D1" s="366"/>
+      <c r="E1" s="366"/>
+      <c r="F1" s="366"/>
       <c r="G1" s="187"/>
       <c r="H1" s="187"/>
       <c r="I1" s="187"/>
@@ -14936,7 +14941,7 @@
       <c r="O2" s="189" t="s">
         <v>323</v>
       </c>
-      <c r="P2" s="350" t="s">
+      <c r="P2" s="365" t="s">
         <v>322</v>
       </c>
       <c r="Q2" s="189" t="s">
@@ -14978,7 +14983,7 @@
       <c r="AC2" s="189" t="s">
         <v>321</v>
       </c>
-      <c r="AD2" s="350" t="s">
+      <c r="AD2" s="365" t="s">
         <v>320</v>
       </c>
       <c r="AE2" s="190" t="s">
@@ -15008,7 +15013,7 @@
       <c r="AM2" s="190" t="s">
         <v>319</v>
       </c>
-      <c r="AN2" s="350" t="s">
+      <c r="AN2" s="365" t="s">
         <v>318</v>
       </c>
       <c r="AQ2" s="189"/>
@@ -15019,7 +15024,7 @@
       <c r="AV2" s="189"/>
       <c r="AW2" s="189"/>
       <c r="AX2" s="189"/>
-      <c r="AY2" s="350"/>
+      <c r="AY2" s="365"/>
       <c r="AZ2" s="190"/>
       <c r="BA2" s="190"/>
       <c r="BB2" s="190"/>
@@ -15029,7 +15034,7 @@
       <c r="BF2" s="190"/>
       <c r="BG2" s="190"/>
       <c r="BH2" s="190"/>
-      <c r="BI2" s="350"/>
+      <c r="BI2" s="365"/>
     </row>
     <row r="3" spans="1:61" s="186" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="188"/>
@@ -15065,7 +15070,7 @@
       <c r="O3" s="189" t="s">
         <v>294</v>
       </c>
-      <c r="P3" s="350"/>
+      <c r="P3" s="365"/>
       <c r="Q3" s="189" t="s">
         <v>293</v>
       </c>
@@ -15105,7 +15110,7 @@
       <c r="AC3" s="189" t="s">
         <v>281</v>
       </c>
-      <c r="AD3" s="350"/>
+      <c r="AD3" s="365"/>
       <c r="AE3" s="190" t="s">
         <v>280</v>
       </c>
@@ -15133,7 +15138,7 @@
       <c r="AM3" s="190" t="s">
         <v>272</v>
       </c>
-      <c r="AN3" s="350"/>
+      <c r="AN3" s="365"/>
       <c r="AQ3" s="189"/>
       <c r="AR3" s="189"/>
       <c r="AS3" s="189"/>
@@ -15142,7 +15147,7 @@
       <c r="AV3" s="189"/>
       <c r="AW3" s="189"/>
       <c r="AX3" s="189"/>
-      <c r="AY3" s="350"/>
+      <c r="AY3" s="365"/>
       <c r="AZ3" s="190"/>
       <c r="BA3" s="190"/>
       <c r="BB3" s="190"/>
@@ -15152,7 +15157,7 @@
       <c r="BF3" s="190"/>
       <c r="BG3" s="190"/>
       <c r="BH3" s="190"/>
-      <c r="BI3" s="350"/>
+      <c r="BI3" s="365"/>
     </row>
     <row r="4" spans="1:61" s="186" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="191"/>
@@ -15198,7 +15203,7 @@
       <c r="O4" s="189" t="s">
         <v>241</v>
       </c>
-      <c r="P4" s="350"/>
+      <c r="P4" s="365"/>
       <c r="Q4" s="189" t="s">
         <v>240</v>
       </c>
@@ -15238,7 +15243,7 @@
       <c r="AC4" s="189" t="s">
         <v>228</v>
       </c>
-      <c r="AD4" s="350"/>
+      <c r="AD4" s="365"/>
       <c r="AE4" s="190" t="s">
         <v>227</v>
       </c>
@@ -15266,7 +15271,7 @@
       <c r="AM4" s="190" t="s">
         <v>219</v>
       </c>
-      <c r="AN4" s="350"/>
+      <c r="AN4" s="365"/>
       <c r="AQ4" s="189"/>
       <c r="AR4" s="189"/>
       <c r="AS4" s="189"/>
@@ -15275,7 +15280,7 @@
       <c r="AV4" s="189"/>
       <c r="AW4" s="189"/>
       <c r="AX4" s="189"/>
-      <c r="AY4" s="350"/>
+      <c r="AY4" s="365"/>
       <c r="AZ4" s="190"/>
       <c r="BA4" s="190"/>
       <c r="BB4" s="190"/>
@@ -15285,7 +15290,7 @@
       <c r="BF4" s="190"/>
       <c r="BG4" s="190"/>
       <c r="BH4" s="190"/>
-      <c r="BI4" s="350"/>
+      <c r="BI4" s="365"/>
     </row>
     <row r="5" spans="1:61" s="186" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="193" t="s">
@@ -16497,492 +16502,492 @@
       <c r="BI16" s="197"/>
     </row>
     <row r="17" spans="1:42" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="365"/>
-      <c r="B17" s="362"/>
-      <c r="C17" s="362"/>
-      <c r="D17" s="365"/>
-      <c r="E17" s="365"/>
-      <c r="F17" s="365"/>
-      <c r="G17" s="362"/>
-      <c r="H17" s="362"/>
-      <c r="I17" s="362"/>
-      <c r="J17" s="362"/>
-      <c r="K17" s="362"/>
-      <c r="L17" s="362"/>
-      <c r="M17" s="362"/>
-      <c r="N17" s="362"/>
-      <c r="O17" s="362"/>
-      <c r="P17" s="362"/>
-      <c r="Q17" s="362"/>
-      <c r="R17" s="362"/>
-      <c r="S17" s="362"/>
-      <c r="T17" s="362"/>
-      <c r="U17" s="362"/>
-      <c r="V17" s="362"/>
-      <c r="W17" s="362"/>
-      <c r="X17" s="362"/>
-      <c r="Y17" s="362"/>
-      <c r="Z17" s="362"/>
-      <c r="AA17" s="362"/>
-      <c r="AB17" s="362"/>
-      <c r="AC17" s="362"/>
-      <c r="AD17" s="362"/>
-      <c r="AE17" s="362"/>
-      <c r="AF17" s="362"/>
-      <c r="AG17" s="362"/>
-      <c r="AH17" s="362"/>
-      <c r="AI17" s="362"/>
-      <c r="AJ17" s="362"/>
-      <c r="AK17" s="362"/>
-      <c r="AL17" s="362"/>
-      <c r="AM17" s="362"/>
-      <c r="AN17" s="362"/>
-      <c r="AO17" s="362"/>
-      <c r="AP17" s="362"/>
+      <c r="A17" s="327"/>
+      <c r="B17" s="325"/>
+      <c r="C17" s="325"/>
+      <c r="D17" s="327"/>
+      <c r="E17" s="327"/>
+      <c r="F17" s="327"/>
+      <c r="G17" s="325"/>
+      <c r="H17" s="325"/>
+      <c r="I17" s="325"/>
+      <c r="J17" s="325"/>
+      <c r="K17" s="325"/>
+      <c r="L17" s="325"/>
+      <c r="M17" s="325"/>
+      <c r="N17" s="325"/>
+      <c r="O17" s="325"/>
+      <c r="P17" s="325"/>
+      <c r="Q17" s="325"/>
+      <c r="R17" s="325"/>
+      <c r="S17" s="325"/>
+      <c r="T17" s="325"/>
+      <c r="U17" s="325"/>
+      <c r="V17" s="325"/>
+      <c r="W17" s="325"/>
+      <c r="X17" s="325"/>
+      <c r="Y17" s="325"/>
+      <c r="Z17" s="325"/>
+      <c r="AA17" s="325"/>
+      <c r="AB17" s="325"/>
+      <c r="AC17" s="325"/>
+      <c r="AD17" s="325"/>
+      <c r="AE17" s="325"/>
+      <c r="AF17" s="325"/>
+      <c r="AG17" s="325"/>
+      <c r="AH17" s="325"/>
+      <c r="AI17" s="325"/>
+      <c r="AJ17" s="325"/>
+      <c r="AK17" s="325"/>
+      <c r="AL17" s="325"/>
+      <c r="AM17" s="325"/>
+      <c r="AN17" s="325"/>
+      <c r="AO17" s="325"/>
+      <c r="AP17" s="325"/>
     </row>
     <row r="18" spans="1:42" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="365"/>
-      <c r="B18" s="362"/>
-      <c r="C18" s="362"/>
-      <c r="D18" s="365"/>
-      <c r="E18" s="365"/>
-      <c r="F18" s="365"/>
-      <c r="G18" s="362"/>
-      <c r="H18" s="362"/>
-      <c r="I18" s="362"/>
-      <c r="J18" s="362"/>
-      <c r="K18" s="362"/>
-      <c r="L18" s="362"/>
-      <c r="M18" s="362"/>
-      <c r="N18" s="362"/>
-      <c r="O18" s="362"/>
-      <c r="P18" s="362"/>
-      <c r="Q18" s="362"/>
-      <c r="R18" s="362"/>
-      <c r="S18" s="362"/>
-      <c r="T18" s="362"/>
-      <c r="U18" s="362"/>
-      <c r="V18" s="362"/>
-      <c r="W18" s="362"/>
-      <c r="X18" s="362"/>
-      <c r="Y18" s="362"/>
-      <c r="Z18" s="362"/>
-      <c r="AA18" s="362"/>
-      <c r="AB18" s="362"/>
-      <c r="AC18" s="362"/>
-      <c r="AD18" s="362"/>
-      <c r="AE18" s="362"/>
-      <c r="AF18" s="362"/>
-      <c r="AG18" s="362"/>
-      <c r="AH18" s="362"/>
-      <c r="AI18" s="362"/>
-      <c r="AJ18" s="362"/>
-      <c r="AK18" s="362"/>
-      <c r="AL18" s="362"/>
-      <c r="AM18" s="362"/>
-      <c r="AN18" s="362"/>
-      <c r="AO18" s="362"/>
-      <c r="AP18" s="362"/>
+      <c r="A18" s="327"/>
+      <c r="B18" s="325"/>
+      <c r="C18" s="325"/>
+      <c r="D18" s="327"/>
+      <c r="E18" s="327"/>
+      <c r="F18" s="327"/>
+      <c r="G18" s="325"/>
+      <c r="H18" s="325"/>
+      <c r="I18" s="325"/>
+      <c r="J18" s="325"/>
+      <c r="K18" s="325"/>
+      <c r="L18" s="325"/>
+      <c r="M18" s="325"/>
+      <c r="N18" s="325"/>
+      <c r="O18" s="325"/>
+      <c r="P18" s="325"/>
+      <c r="Q18" s="325"/>
+      <c r="R18" s="325"/>
+      <c r="S18" s="325"/>
+      <c r="T18" s="325"/>
+      <c r="U18" s="325"/>
+      <c r="V18" s="325"/>
+      <c r="W18" s="325"/>
+      <c r="X18" s="325"/>
+      <c r="Y18" s="325"/>
+      <c r="Z18" s="325"/>
+      <c r="AA18" s="325"/>
+      <c r="AB18" s="325"/>
+      <c r="AC18" s="325"/>
+      <c r="AD18" s="325"/>
+      <c r="AE18" s="325"/>
+      <c r="AF18" s="325"/>
+      <c r="AG18" s="325"/>
+      <c r="AH18" s="325"/>
+      <c r="AI18" s="325"/>
+      <c r="AJ18" s="325"/>
+      <c r="AK18" s="325"/>
+      <c r="AL18" s="325"/>
+      <c r="AM18" s="325"/>
+      <c r="AN18" s="325"/>
+      <c r="AO18" s="325"/>
+      <c r="AP18" s="325"/>
     </row>
     <row r="19" spans="1:42" ht="84" x14ac:dyDescent="0.2">
-      <c r="A19" s="365"/>
-      <c r="B19" s="362"/>
-      <c r="C19" s="362"/>
-      <c r="D19" s="365"/>
-      <c r="E19" s="365"/>
-      <c r="F19" s="365"/>
-      <c r="G19" s="362"/>
-      <c r="H19" s="362"/>
-      <c r="I19" s="362"/>
-      <c r="J19" s="362"/>
-      <c r="K19" s="362"/>
-      <c r="L19" s="362"/>
-      <c r="M19" s="362"/>
-      <c r="N19" s="362"/>
-      <c r="O19" s="362"/>
-      <c r="P19" s="362"/>
-      <c r="Q19" s="362"/>
-      <c r="R19" s="362"/>
-      <c r="S19" s="362"/>
-      <c r="T19" s="362"/>
-      <c r="U19" s="362"/>
-      <c r="V19" s="362"/>
-      <c r="W19" s="362"/>
-      <c r="X19" s="362"/>
-      <c r="Y19" s="362"/>
-      <c r="Z19" s="362"/>
-      <c r="AA19" s="362"/>
-      <c r="AB19" s="359" t="s">
+      <c r="A19" s="327"/>
+      <c r="B19" s="325"/>
+      <c r="C19" s="325"/>
+      <c r="D19" s="327"/>
+      <c r="E19" s="327"/>
+      <c r="F19" s="327"/>
+      <c r="G19" s="325"/>
+      <c r="H19" s="325"/>
+      <c r="I19" s="325"/>
+      <c r="J19" s="325"/>
+      <c r="K19" s="325"/>
+      <c r="L19" s="325"/>
+      <c r="M19" s="325"/>
+      <c r="N19" s="325"/>
+      <c r="O19" s="325"/>
+      <c r="P19" s="325"/>
+      <c r="Q19" s="325"/>
+      <c r="R19" s="325"/>
+      <c r="S19" s="325"/>
+      <c r="T19" s="325"/>
+      <c r="U19" s="325"/>
+      <c r="V19" s="325"/>
+      <c r="W19" s="325"/>
+      <c r="X19" s="325"/>
+      <c r="Y19" s="325"/>
+      <c r="Z19" s="325"/>
+      <c r="AA19" s="325"/>
+      <c r="AB19" s="322" t="s">
         <v>551</v>
       </c>
       <c r="AC19" s="196" t="s">
         <v>552</v>
       </c>
-      <c r="AD19" s="362"/>
-      <c r="AE19" s="362"/>
-      <c r="AF19" s="362"/>
-      <c r="AG19" s="362"/>
-      <c r="AH19" s="362"/>
-      <c r="AI19" s="362"/>
-      <c r="AJ19" s="362"/>
-      <c r="AK19" s="362"/>
-      <c r="AL19" s="362"/>
-      <c r="AM19" s="362"/>
-      <c r="AN19" s="362"/>
-      <c r="AO19" s="362"/>
-      <c r="AP19" s="362"/>
+      <c r="AD19" s="325"/>
+      <c r="AE19" s="325"/>
+      <c r="AF19" s="325"/>
+      <c r="AG19" s="325"/>
+      <c r="AH19" s="325"/>
+      <c r="AI19" s="325"/>
+      <c r="AJ19" s="325"/>
+      <c r="AK19" s="325"/>
+      <c r="AL19" s="325"/>
+      <c r="AM19" s="325"/>
+      <c r="AN19" s="325"/>
+      <c r="AO19" s="325"/>
+      <c r="AP19" s="325"/>
     </row>
     <row r="20" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A20" s="365"/>
-      <c r="B20" s="362"/>
-      <c r="C20" s="362"/>
-      <c r="D20" s="365"/>
-      <c r="E20" s="365"/>
-      <c r="F20" s="365"/>
-      <c r="G20" s="362"/>
-      <c r="H20" s="362"/>
-      <c r="I20" s="362"/>
-      <c r="J20" s="362"/>
-      <c r="K20" s="362"/>
-      <c r="L20" s="362"/>
-      <c r="M20" s="362"/>
-      <c r="N20" s="362"/>
-      <c r="O20" s="362"/>
-      <c r="P20" s="362"/>
-      <c r="Q20" s="362"/>
-      <c r="R20" s="362"/>
-      <c r="S20" s="362"/>
-      <c r="T20" s="362"/>
-      <c r="U20" s="362"/>
-      <c r="V20" s="362"/>
-      <c r="W20" s="362"/>
-      <c r="X20" s="362"/>
-      <c r="Y20" s="362"/>
-      <c r="Z20" s="362"/>
-      <c r="AA20" s="362"/>
-      <c r="AB20" s="362"/>
-      <c r="AC20" s="362"/>
-      <c r="AD20" s="362"/>
-      <c r="AE20" s="362"/>
-      <c r="AF20" s="362"/>
-      <c r="AG20" s="362"/>
-      <c r="AH20" s="362"/>
-      <c r="AI20" s="362"/>
-      <c r="AJ20" s="362"/>
-      <c r="AK20" s="362"/>
-      <c r="AL20" s="362"/>
-      <c r="AM20" s="362"/>
-      <c r="AN20" s="362"/>
-      <c r="AO20" s="362"/>
-      <c r="AP20" s="362"/>
+      <c r="A20" s="327"/>
+      <c r="B20" s="325"/>
+      <c r="C20" s="325"/>
+      <c r="D20" s="327"/>
+      <c r="E20" s="327"/>
+      <c r="F20" s="327"/>
+      <c r="G20" s="325"/>
+      <c r="H20" s="325"/>
+      <c r="I20" s="325"/>
+      <c r="J20" s="325"/>
+      <c r="K20" s="325"/>
+      <c r="L20" s="325"/>
+      <c r="M20" s="325"/>
+      <c r="N20" s="325"/>
+      <c r="O20" s="325"/>
+      <c r="P20" s="325"/>
+      <c r="Q20" s="325"/>
+      <c r="R20" s="325"/>
+      <c r="S20" s="325"/>
+      <c r="T20" s="325"/>
+      <c r="U20" s="325"/>
+      <c r="V20" s="325"/>
+      <c r="W20" s="325"/>
+      <c r="X20" s="325"/>
+      <c r="Y20" s="325"/>
+      <c r="Z20" s="325"/>
+      <c r="AA20" s="325"/>
+      <c r="AB20" s="325"/>
+      <c r="AC20" s="325"/>
+      <c r="AD20" s="325"/>
+      <c r="AE20" s="325"/>
+      <c r="AF20" s="325"/>
+      <c r="AG20" s="325"/>
+      <c r="AH20" s="325"/>
+      <c r="AI20" s="325"/>
+      <c r="AJ20" s="325"/>
+      <c r="AK20" s="325"/>
+      <c r="AL20" s="325"/>
+      <c r="AM20" s="325"/>
+      <c r="AN20" s="325"/>
+      <c r="AO20" s="325"/>
+      <c r="AP20" s="325"/>
     </row>
     <row r="21" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A21" s="365"/>
-      <c r="B21" s="362"/>
-      <c r="C21" s="362"/>
-      <c r="D21" s="365"/>
-      <c r="E21" s="365"/>
-      <c r="F21" s="365"/>
-      <c r="G21" s="362"/>
-      <c r="H21" s="362"/>
-      <c r="I21" s="362"/>
-      <c r="J21" s="362"/>
-      <c r="K21" s="362"/>
-      <c r="L21" s="362"/>
-      <c r="M21" s="362"/>
-      <c r="N21" s="362"/>
-      <c r="O21" s="362"/>
-      <c r="P21" s="362"/>
-      <c r="Q21" s="362"/>
-      <c r="R21" s="362"/>
-      <c r="S21" s="362"/>
-      <c r="T21" s="362"/>
-      <c r="U21" s="362"/>
-      <c r="V21" s="362"/>
-      <c r="W21" s="362"/>
-      <c r="X21" s="362"/>
-      <c r="Y21" s="362"/>
-      <c r="Z21" s="362"/>
-      <c r="AA21" s="362"/>
-      <c r="AB21" s="362"/>
-      <c r="AC21" s="362"/>
-      <c r="AD21" s="362"/>
-      <c r="AE21" s="362"/>
-      <c r="AF21" s="362"/>
-      <c r="AG21" s="362"/>
-      <c r="AH21" s="362"/>
-      <c r="AI21" s="362"/>
-      <c r="AJ21" s="362"/>
-      <c r="AK21" s="362"/>
-      <c r="AL21" s="362"/>
-      <c r="AM21" s="362"/>
-      <c r="AN21" s="362"/>
-      <c r="AO21" s="362"/>
-      <c r="AP21" s="362"/>
+      <c r="A21" s="327"/>
+      <c r="B21" s="325"/>
+      <c r="C21" s="325"/>
+      <c r="D21" s="327"/>
+      <c r="E21" s="327"/>
+      <c r="F21" s="327"/>
+      <c r="G21" s="325"/>
+      <c r="H21" s="325"/>
+      <c r="I21" s="325"/>
+      <c r="J21" s="325"/>
+      <c r="K21" s="325"/>
+      <c r="L21" s="325"/>
+      <c r="M21" s="325"/>
+      <c r="N21" s="325"/>
+      <c r="O21" s="325"/>
+      <c r="P21" s="325"/>
+      <c r="Q21" s="325"/>
+      <c r="R21" s="325"/>
+      <c r="S21" s="325"/>
+      <c r="T21" s="325"/>
+      <c r="U21" s="325"/>
+      <c r="V21" s="325"/>
+      <c r="W21" s="325"/>
+      <c r="X21" s="325"/>
+      <c r="Y21" s="325"/>
+      <c r="Z21" s="325"/>
+      <c r="AA21" s="325"/>
+      <c r="AB21" s="325"/>
+      <c r="AC21" s="325"/>
+      <c r="AD21" s="325"/>
+      <c r="AE21" s="325"/>
+      <c r="AF21" s="325"/>
+      <c r="AG21" s="325"/>
+      <c r="AH21" s="325"/>
+      <c r="AI21" s="325"/>
+      <c r="AJ21" s="325"/>
+      <c r="AK21" s="325"/>
+      <c r="AL21" s="325"/>
+      <c r="AM21" s="325"/>
+      <c r="AN21" s="325"/>
+      <c r="AO21" s="325"/>
+      <c r="AP21" s="325"/>
     </row>
     <row r="22" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A22" s="365"/>
-      <c r="B22" s="362"/>
-      <c r="C22" s="362"/>
-      <c r="D22" s="365"/>
-      <c r="E22" s="365"/>
-      <c r="F22" s="365"/>
-      <c r="G22" s="362"/>
-      <c r="H22" s="362"/>
-      <c r="I22" s="362"/>
-      <c r="J22" s="362"/>
-      <c r="K22" s="362"/>
-      <c r="L22" s="362"/>
-      <c r="M22" s="362"/>
-      <c r="N22" s="362"/>
-      <c r="O22" s="362"/>
-      <c r="P22" s="362"/>
-      <c r="Q22" s="362"/>
-      <c r="R22" s="362"/>
-      <c r="S22" s="362"/>
-      <c r="T22" s="362"/>
-      <c r="U22" s="362"/>
-      <c r="V22" s="362"/>
-      <c r="W22" s="362"/>
-      <c r="X22" s="362"/>
-      <c r="Y22" s="362"/>
-      <c r="Z22" s="362"/>
-      <c r="AA22" s="362"/>
-      <c r="AB22" s="362"/>
-      <c r="AC22" s="362"/>
-      <c r="AD22" s="362"/>
-      <c r="AE22" s="362"/>
-      <c r="AF22" s="362"/>
-      <c r="AG22" s="362"/>
-      <c r="AH22" s="362"/>
-      <c r="AI22" s="362"/>
-      <c r="AJ22" s="362"/>
-      <c r="AK22" s="362"/>
-      <c r="AL22" s="362"/>
-      <c r="AM22" s="362"/>
-      <c r="AN22" s="362"/>
-      <c r="AO22" s="362"/>
-      <c r="AP22" s="362"/>
+      <c r="A22" s="327"/>
+      <c r="B22" s="325"/>
+      <c r="C22" s="325"/>
+      <c r="D22" s="327"/>
+      <c r="E22" s="327"/>
+      <c r="F22" s="327"/>
+      <c r="G22" s="325"/>
+      <c r="H22" s="325"/>
+      <c r="I22" s="325"/>
+      <c r="J22" s="325"/>
+      <c r="K22" s="325"/>
+      <c r="L22" s="325"/>
+      <c r="M22" s="325"/>
+      <c r="N22" s="325"/>
+      <c r="O22" s="325"/>
+      <c r="P22" s="325"/>
+      <c r="Q22" s="325"/>
+      <c r="R22" s="325"/>
+      <c r="S22" s="325"/>
+      <c r="T22" s="325"/>
+      <c r="U22" s="325"/>
+      <c r="V22" s="325"/>
+      <c r="W22" s="325"/>
+      <c r="X22" s="325"/>
+      <c r="Y22" s="325"/>
+      <c r="Z22" s="325"/>
+      <c r="AA22" s="325"/>
+      <c r="AB22" s="325"/>
+      <c r="AC22" s="325"/>
+      <c r="AD22" s="325"/>
+      <c r="AE22" s="325"/>
+      <c r="AF22" s="325"/>
+      <c r="AG22" s="325"/>
+      <c r="AH22" s="325"/>
+      <c r="AI22" s="325"/>
+      <c r="AJ22" s="325"/>
+      <c r="AK22" s="325"/>
+      <c r="AL22" s="325"/>
+      <c r="AM22" s="325"/>
+      <c r="AN22" s="325"/>
+      <c r="AO22" s="325"/>
+      <c r="AP22" s="325"/>
     </row>
     <row r="23" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A23" s="365"/>
-      <c r="B23" s="362"/>
-      <c r="C23" s="362"/>
-      <c r="D23" s="365"/>
-      <c r="E23" s="365"/>
-      <c r="F23" s="365"/>
-      <c r="G23" s="362"/>
-      <c r="H23" s="362"/>
-      <c r="I23" s="362"/>
-      <c r="J23" s="362"/>
-      <c r="K23" s="362"/>
-      <c r="L23" s="362"/>
-      <c r="M23" s="362"/>
-      <c r="N23" s="362"/>
-      <c r="O23" s="362"/>
-      <c r="P23" s="362"/>
-      <c r="Q23" s="362"/>
-      <c r="R23" s="362"/>
-      <c r="S23" s="362"/>
-      <c r="T23" s="362"/>
-      <c r="U23" s="362"/>
-      <c r="V23" s="362"/>
-      <c r="W23" s="362"/>
-      <c r="X23" s="362"/>
-      <c r="Y23" s="362"/>
-      <c r="Z23" s="362"/>
-      <c r="AA23" s="362"/>
-      <c r="AB23" s="362"/>
-      <c r="AC23" s="362"/>
-      <c r="AD23" s="362"/>
-      <c r="AE23" s="362"/>
-      <c r="AF23" s="362"/>
-      <c r="AG23" s="362"/>
-      <c r="AH23" s="362"/>
-      <c r="AI23" s="362"/>
-      <c r="AJ23" s="362"/>
-      <c r="AK23" s="362"/>
-      <c r="AL23" s="362"/>
-      <c r="AM23" s="362"/>
-      <c r="AN23" s="362"/>
-      <c r="AO23" s="362"/>
-      <c r="AP23" s="362"/>
+      <c r="A23" s="327"/>
+      <c r="B23" s="325"/>
+      <c r="C23" s="325"/>
+      <c r="D23" s="327"/>
+      <c r="E23" s="327"/>
+      <c r="F23" s="327"/>
+      <c r="G23" s="325"/>
+      <c r="H23" s="325"/>
+      <c r="I23" s="325"/>
+      <c r="J23" s="325"/>
+      <c r="K23" s="325"/>
+      <c r="L23" s="325"/>
+      <c r="M23" s="325"/>
+      <c r="N23" s="325"/>
+      <c r="O23" s="325"/>
+      <c r="P23" s="325"/>
+      <c r="Q23" s="325"/>
+      <c r="R23" s="325"/>
+      <c r="S23" s="325"/>
+      <c r="T23" s="325"/>
+      <c r="U23" s="325"/>
+      <c r="V23" s="325"/>
+      <c r="W23" s="325"/>
+      <c r="X23" s="325"/>
+      <c r="Y23" s="325"/>
+      <c r="Z23" s="325"/>
+      <c r="AA23" s="325"/>
+      <c r="AB23" s="325"/>
+      <c r="AC23" s="325"/>
+      <c r="AD23" s="325"/>
+      <c r="AE23" s="325"/>
+      <c r="AF23" s="325"/>
+      <c r="AG23" s="325"/>
+      <c r="AH23" s="325"/>
+      <c r="AI23" s="325"/>
+      <c r="AJ23" s="325"/>
+      <c r="AK23" s="325"/>
+      <c r="AL23" s="325"/>
+      <c r="AM23" s="325"/>
+      <c r="AN23" s="325"/>
+      <c r="AO23" s="325"/>
+      <c r="AP23" s="325"/>
     </row>
     <row r="24" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A24" s="365"/>
-      <c r="B24" s="362"/>
-      <c r="C24" s="362"/>
-      <c r="D24" s="365"/>
-      <c r="E24" s="365"/>
-      <c r="F24" s="365"/>
-      <c r="G24" s="362"/>
-      <c r="H24" s="362"/>
-      <c r="I24" s="362"/>
-      <c r="J24" s="362"/>
-      <c r="K24" s="362"/>
-      <c r="L24" s="362"/>
-      <c r="M24" s="362"/>
-      <c r="N24" s="362"/>
-      <c r="O24" s="362"/>
-      <c r="P24" s="362"/>
-      <c r="Q24" s="362"/>
-      <c r="R24" s="362"/>
-      <c r="S24" s="362"/>
-      <c r="T24" s="362"/>
-      <c r="U24" s="362"/>
-      <c r="V24" s="362"/>
-      <c r="W24" s="362"/>
-      <c r="X24" s="362"/>
-      <c r="Y24" s="362"/>
-      <c r="Z24" s="362"/>
-      <c r="AA24" s="362"/>
-      <c r="AB24" s="362"/>
-      <c r="AC24" s="362"/>
-      <c r="AD24" s="362"/>
-      <c r="AE24" s="362"/>
-      <c r="AF24" s="362"/>
-      <c r="AG24" s="362"/>
-      <c r="AH24" s="362"/>
-      <c r="AI24" s="362"/>
-      <c r="AJ24" s="362"/>
-      <c r="AK24" s="362"/>
-      <c r="AL24" s="362"/>
-      <c r="AM24" s="362"/>
-      <c r="AN24" s="362"/>
-      <c r="AO24" s="362"/>
-      <c r="AP24" s="362"/>
+      <c r="A24" s="327"/>
+      <c r="B24" s="325"/>
+      <c r="C24" s="325"/>
+      <c r="D24" s="327"/>
+      <c r="E24" s="327"/>
+      <c r="F24" s="327"/>
+      <c r="G24" s="325"/>
+      <c r="H24" s="325"/>
+      <c r="I24" s="325"/>
+      <c r="J24" s="325"/>
+      <c r="K24" s="325"/>
+      <c r="L24" s="325"/>
+      <c r="M24" s="325"/>
+      <c r="N24" s="325"/>
+      <c r="O24" s="325"/>
+      <c r="P24" s="325"/>
+      <c r="Q24" s="325"/>
+      <c r="R24" s="325"/>
+      <c r="S24" s="325"/>
+      <c r="T24" s="325"/>
+      <c r="U24" s="325"/>
+      <c r="V24" s="325"/>
+      <c r="W24" s="325"/>
+      <c r="X24" s="325"/>
+      <c r="Y24" s="325"/>
+      <c r="Z24" s="325"/>
+      <c r="AA24" s="325"/>
+      <c r="AB24" s="325"/>
+      <c r="AC24" s="325"/>
+      <c r="AD24" s="325"/>
+      <c r="AE24" s="325"/>
+      <c r="AF24" s="325"/>
+      <c r="AG24" s="325"/>
+      <c r="AH24" s="325"/>
+      <c r="AI24" s="325"/>
+      <c r="AJ24" s="325"/>
+      <c r="AK24" s="325"/>
+      <c r="AL24" s="325"/>
+      <c r="AM24" s="325"/>
+      <c r="AN24" s="325"/>
+      <c r="AO24" s="325"/>
+      <c r="AP24" s="325"/>
     </row>
     <row r="25" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A25" s="365"/>
-      <c r="B25" s="362"/>
-      <c r="C25" s="362"/>
-      <c r="D25" s="365"/>
-      <c r="E25" s="365"/>
-      <c r="F25" s="365"/>
-      <c r="G25" s="362"/>
-      <c r="H25" s="362"/>
-      <c r="I25" s="362"/>
-      <c r="J25" s="362"/>
-      <c r="K25" s="362"/>
-      <c r="L25" s="362"/>
-      <c r="M25" s="362"/>
-      <c r="N25" s="362"/>
-      <c r="O25" s="362"/>
-      <c r="P25" s="362"/>
-      <c r="Q25" s="362"/>
-      <c r="R25" s="362"/>
-      <c r="S25" s="362"/>
-      <c r="T25" s="362"/>
-      <c r="U25" s="362"/>
-      <c r="V25" s="362"/>
-      <c r="W25" s="362"/>
-      <c r="X25" s="362"/>
-      <c r="Y25" s="362"/>
-      <c r="Z25" s="362"/>
-      <c r="AA25" s="362"/>
-      <c r="AB25" s="362"/>
-      <c r="AC25" s="362"/>
-      <c r="AD25" s="362"/>
-      <c r="AE25" s="362"/>
-      <c r="AF25" s="362"/>
-      <c r="AG25" s="362"/>
-      <c r="AH25" s="362"/>
-      <c r="AI25" s="362"/>
-      <c r="AJ25" s="362"/>
-      <c r="AK25" s="362"/>
-      <c r="AL25" s="362"/>
-      <c r="AM25" s="362"/>
-      <c r="AN25" s="362"/>
-      <c r="AO25" s="362"/>
-      <c r="AP25" s="362"/>
+      <c r="A25" s="327"/>
+      <c r="B25" s="325"/>
+      <c r="C25" s="325"/>
+      <c r="D25" s="327"/>
+      <c r="E25" s="327"/>
+      <c r="F25" s="327"/>
+      <c r="G25" s="325"/>
+      <c r="H25" s="325"/>
+      <c r="I25" s="325"/>
+      <c r="J25" s="325"/>
+      <c r="K25" s="325"/>
+      <c r="L25" s="325"/>
+      <c r="M25" s="325"/>
+      <c r="N25" s="325"/>
+      <c r="O25" s="325"/>
+      <c r="P25" s="325"/>
+      <c r="Q25" s="325"/>
+      <c r="R25" s="325"/>
+      <c r="S25" s="325"/>
+      <c r="T25" s="325"/>
+      <c r="U25" s="325"/>
+      <c r="V25" s="325"/>
+      <c r="W25" s="325"/>
+      <c r="X25" s="325"/>
+      <c r="Y25" s="325"/>
+      <c r="Z25" s="325"/>
+      <c r="AA25" s="325"/>
+      <c r="AB25" s="325"/>
+      <c r="AC25" s="325"/>
+      <c r="AD25" s="325"/>
+      <c r="AE25" s="325"/>
+      <c r="AF25" s="325"/>
+      <c r="AG25" s="325"/>
+      <c r="AH25" s="325"/>
+      <c r="AI25" s="325"/>
+      <c r="AJ25" s="325"/>
+      <c r="AK25" s="325"/>
+      <c r="AL25" s="325"/>
+      <c r="AM25" s="325"/>
+      <c r="AN25" s="325"/>
+      <c r="AO25" s="325"/>
+      <c r="AP25" s="325"/>
     </row>
     <row r="26" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A26" s="365"/>
-      <c r="B26" s="362"/>
-      <c r="C26" s="362"/>
-      <c r="D26" s="365"/>
-      <c r="E26" s="365"/>
-      <c r="F26" s="365"/>
-      <c r="G26" s="362"/>
-      <c r="H26" s="362"/>
-      <c r="I26" s="362"/>
-      <c r="J26" s="362"/>
-      <c r="K26" s="362"/>
-      <c r="L26" s="362"/>
-      <c r="M26" s="362"/>
-      <c r="N26" s="362"/>
-      <c r="O26" s="362"/>
-      <c r="P26" s="362"/>
-      <c r="Q26" s="362"/>
-      <c r="R26" s="362"/>
-      <c r="S26" s="362"/>
-      <c r="T26" s="362"/>
-      <c r="U26" s="362"/>
-      <c r="V26" s="362"/>
-      <c r="W26" s="362"/>
-      <c r="X26" s="362"/>
-      <c r="Y26" s="362"/>
-      <c r="Z26" s="362"/>
-      <c r="AA26" s="362"/>
-      <c r="AB26" s="362"/>
-      <c r="AC26" s="362"/>
-      <c r="AD26" s="362"/>
-      <c r="AE26" s="362"/>
-      <c r="AF26" s="362"/>
-      <c r="AG26" s="362"/>
-      <c r="AH26" s="362"/>
-      <c r="AI26" s="362"/>
-      <c r="AJ26" s="362"/>
-      <c r="AK26" s="362"/>
-      <c r="AL26" s="362"/>
-      <c r="AM26" s="362"/>
-      <c r="AN26" s="362"/>
-      <c r="AO26" s="362"/>
-      <c r="AP26" s="362"/>
+      <c r="A26" s="327"/>
+      <c r="B26" s="325"/>
+      <c r="C26" s="325"/>
+      <c r="D26" s="327"/>
+      <c r="E26" s="327"/>
+      <c r="F26" s="327"/>
+      <c r="G26" s="325"/>
+      <c r="H26" s="325"/>
+      <c r="I26" s="325"/>
+      <c r="J26" s="325"/>
+      <c r="K26" s="325"/>
+      <c r="L26" s="325"/>
+      <c r="M26" s="325"/>
+      <c r="N26" s="325"/>
+      <c r="O26" s="325"/>
+      <c r="P26" s="325"/>
+      <c r="Q26" s="325"/>
+      <c r="R26" s="325"/>
+      <c r="S26" s="325"/>
+      <c r="T26" s="325"/>
+      <c r="U26" s="325"/>
+      <c r="V26" s="325"/>
+      <c r="W26" s="325"/>
+      <c r="X26" s="325"/>
+      <c r="Y26" s="325"/>
+      <c r="Z26" s="325"/>
+      <c r="AA26" s="325"/>
+      <c r="AB26" s="325"/>
+      <c r="AC26" s="325"/>
+      <c r="AD26" s="325"/>
+      <c r="AE26" s="325"/>
+      <c r="AF26" s="325"/>
+      <c r="AG26" s="325"/>
+      <c r="AH26" s="325"/>
+      <c r="AI26" s="325"/>
+      <c r="AJ26" s="325"/>
+      <c r="AK26" s="325"/>
+      <c r="AL26" s="325"/>
+      <c r="AM26" s="325"/>
+      <c r="AN26" s="325"/>
+      <c r="AO26" s="325"/>
+      <c r="AP26" s="325"/>
     </row>
     <row r="27" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A27" s="365"/>
-      <c r="B27" s="362"/>
-      <c r="C27" s="362"/>
-      <c r="D27" s="365"/>
-      <c r="E27" s="365"/>
-      <c r="F27" s="365"/>
-      <c r="G27" s="362"/>
-      <c r="H27" s="362"/>
-      <c r="I27" s="362"/>
-      <c r="J27" s="362"/>
-      <c r="K27" s="362"/>
-      <c r="L27" s="362"/>
-      <c r="M27" s="362"/>
-      <c r="N27" s="362"/>
-      <c r="O27" s="362"/>
-      <c r="P27" s="362"/>
-      <c r="Q27" s="362"/>
-      <c r="R27" s="362"/>
-      <c r="S27" s="362"/>
-      <c r="T27" s="362"/>
-      <c r="U27" s="362"/>
-      <c r="V27" s="362"/>
-      <c r="W27" s="362"/>
-      <c r="X27" s="362"/>
-      <c r="Y27" s="362"/>
-      <c r="Z27" s="362"/>
-      <c r="AA27" s="362"/>
-      <c r="AB27" s="362"/>
-      <c r="AC27" s="362"/>
-      <c r="AD27" s="362"/>
-      <c r="AE27" s="362"/>
-      <c r="AF27" s="362"/>
-      <c r="AG27" s="362"/>
-      <c r="AH27" s="362"/>
-      <c r="AI27" s="362"/>
-      <c r="AJ27" s="362"/>
-      <c r="AK27" s="362"/>
-      <c r="AL27" s="362"/>
-      <c r="AM27" s="362"/>
-      <c r="AN27" s="362"/>
-      <c r="AO27" s="362"/>
-      <c r="AP27" s="362"/>
+      <c r="A27" s="327"/>
+      <c r="B27" s="325"/>
+      <c r="C27" s="325"/>
+      <c r="D27" s="327"/>
+      <c r="E27" s="327"/>
+      <c r="F27" s="327"/>
+      <c r="G27" s="325"/>
+      <c r="H27" s="325"/>
+      <c r="I27" s="325"/>
+      <c r="J27" s="325"/>
+      <c r="K27" s="325"/>
+      <c r="L27" s="325"/>
+      <c r="M27" s="325"/>
+      <c r="N27" s="325"/>
+      <c r="O27" s="325"/>
+      <c r="P27" s="325"/>
+      <c r="Q27" s="325"/>
+      <c r="R27" s="325"/>
+      <c r="S27" s="325"/>
+      <c r="T27" s="325"/>
+      <c r="U27" s="325"/>
+      <c r="V27" s="325"/>
+      <c r="W27" s="325"/>
+      <c r="X27" s="325"/>
+      <c r="Y27" s="325"/>
+      <c r="Z27" s="325"/>
+      <c r="AA27" s="325"/>
+      <c r="AB27" s="325"/>
+      <c r="AC27" s="325"/>
+      <c r="AD27" s="325"/>
+      <c r="AE27" s="325"/>
+      <c r="AF27" s="325"/>
+      <c r="AG27" s="325"/>
+      <c r="AH27" s="325"/>
+      <c r="AI27" s="325"/>
+      <c r="AJ27" s="325"/>
+      <c r="AK27" s="325"/>
+      <c r="AL27" s="325"/>
+      <c r="AM27" s="325"/>
+      <c r="AN27" s="325"/>
+      <c r="AO27" s="325"/>
+      <c r="AP27" s="325"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -17012,14 +17017,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="352" t="s">
+      <c r="A1" s="367" t="s">
         <v>373</v>
       </c>
-      <c r="B1" s="352"/>
-      <c r="C1" s="352"/>
-      <c r="D1" s="352"/>
-      <c r="E1" s="352"/>
-      <c r="F1" s="352"/>
+      <c r="B1" s="367"/>
+      <c r="C1" s="367"/>
+      <c r="D1" s="367"/>
+      <c r="E1" s="367"/>
+      <c r="F1" s="367"/>
       <c r="G1" s="218"/>
       <c r="H1" s="218"/>
       <c r="I1" s="218"/>
@@ -17069,7 +17074,7 @@
       <c r="O2" s="221" t="s">
         <v>323</v>
       </c>
-      <c r="P2" s="353" t="s">
+      <c r="P2" s="368" t="s">
         <v>372</v>
       </c>
       <c r="Q2" s="221" t="s">
@@ -17081,7 +17086,7 @@
       <c r="S2" s="221" t="s">
         <v>371</v>
       </c>
-      <c r="T2" s="353" t="s">
+      <c r="T2" s="368" t="s">
         <v>370</v>
       </c>
     </row>
@@ -17119,7 +17124,7 @@
       <c r="O3" s="221" t="s">
         <v>352</v>
       </c>
-      <c r="P3" s="353"/>
+      <c r="P3" s="368"/>
       <c r="Q3" s="221" t="s">
         <v>351</v>
       </c>
@@ -17129,7 +17134,7 @@
       <c r="S3" s="221" t="s">
         <v>281</v>
       </c>
-      <c r="T3" s="353"/>
+      <c r="T3" s="368"/>
     </row>
     <row r="4" spans="1:20" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="220"/>
@@ -17175,7 +17180,7 @@
       <c r="O4" s="221" t="s">
         <v>333</v>
       </c>
-      <c r="P4" s="353"/>
+      <c r="P4" s="368"/>
       <c r="Q4" s="221" t="s">
         <v>332</v>
       </c>
@@ -17185,7 +17190,7 @@
       <c r="S4" s="221" t="s">
         <v>228</v>
       </c>
-      <c r="T4" s="353"/>
+      <c r="T4" s="368"/>
     </row>
     <row r="5" spans="1:20" ht="317" x14ac:dyDescent="0.2">
       <c r="A5" s="224" t="s">
@@ -17742,8 +17747,8 @@
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
-      <c r="Q19" s="362"/>
-      <c r="R19" s="359" t="s">
+      <c r="Q19" s="325"/>
+      <c r="R19" s="322" t="s">
         <v>551</v>
       </c>
       <c r="S19" s="196" t="s">
@@ -17776,16 +17781,16 @@
   <sheetData>
     <row r="1" spans="1:28" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="244"/>
-      <c r="B1" s="355" t="s">
+      <c r="B1" s="370" t="s">
         <v>329</v>
       </c>
-      <c r="C1" s="355"/>
-      <c r="D1" s="355"/>
-      <c r="E1" s="355"/>
-      <c r="F1" s="355"/>
-      <c r="G1" s="355"/>
-      <c r="H1" s="355"/>
-      <c r="I1" s="355"/>
+      <c r="C1" s="370"/>
+      <c r="D1" s="370"/>
+      <c r="E1" s="370"/>
+      <c r="F1" s="370"/>
+      <c r="G1" s="370"/>
+      <c r="H1" s="370"/>
+      <c r="I1" s="370"/>
       <c r="J1" s="241"/>
       <c r="K1" s="241"/>
       <c r="L1" s="241"/>
@@ -17816,7 +17821,7 @@
       <c r="G2" s="243" t="s">
         <v>328</v>
       </c>
-      <c r="H2" s="354" t="s">
+      <c r="H2" s="369" t="s">
         <v>327</v>
       </c>
       <c r="I2" s="246" t="s">
@@ -17861,7 +17866,7 @@
       <c r="V2" s="246" t="s">
         <v>326</v>
       </c>
-      <c r="W2" s="354" t="s">
+      <c r="W2" s="369" t="s">
         <v>325</v>
       </c>
       <c r="X2" s="243" t="s">
@@ -17876,7 +17881,7 @@
       <c r="AA2" s="243" t="s">
         <v>144</v>
       </c>
-      <c r="AB2" s="354" t="s">
+      <c r="AB2" s="369" t="s">
         <v>324</v>
       </c>
     </row>
@@ -17890,7 +17895,7 @@
       <c r="G3" s="243" t="s">
         <v>317</v>
       </c>
-      <c r="H3" s="354"/>
+      <c r="H3" s="369"/>
       <c r="I3" s="246" t="s">
         <v>316</v>
       </c>
@@ -17931,7 +17936,7 @@
       <c r="V3" s="246" t="s">
         <v>304</v>
       </c>
-      <c r="W3" s="354"/>
+      <c r="W3" s="369"/>
       <c r="X3" s="245"/>
       <c r="Y3" s="243" t="s">
         <v>303</v>
@@ -17942,7 +17947,7 @@
       <c r="AA3" s="243" t="s">
         <v>301</v>
       </c>
-      <c r="AB3" s="354"/>
+      <c r="AB3" s="369"/>
     </row>
     <row r="4" spans="1:28" ht="98" x14ac:dyDescent="0.2">
       <c r="A4" s="247"/>
@@ -17964,7 +17969,7 @@
       <c r="G4" s="243" t="s">
         <v>267</v>
       </c>
-      <c r="H4" s="354"/>
+      <c r="H4" s="369"/>
       <c r="I4" s="246" t="s">
         <v>266</v>
       </c>
@@ -18007,7 +18012,7 @@
       <c r="V4" s="249" t="s">
         <v>253</v>
       </c>
-      <c r="W4" s="354"/>
+      <c r="W4" s="369"/>
       <c r="X4" s="250" t="s">
         <v>252</v>
       </c>
@@ -18020,7 +18025,7 @@
       <c r="AA4" s="250" t="s">
         <v>249</v>
       </c>
-      <c r="AB4" s="354"/>
+      <c r="AB4" s="369"/>
     </row>
     <row r="5" spans="1:28" ht="196" x14ac:dyDescent="0.2">
       <c r="A5" s="251" t="s">
@@ -18797,102 +18802,102 @@
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A17" s="366"/>
-      <c r="B17" s="366"/>
-      <c r="C17" s="366"/>
-      <c r="D17" s="366"/>
-      <c r="E17" s="366"/>
-      <c r="F17" s="366"/>
-      <c r="G17" s="367"/>
-      <c r="H17" s="367"/>
-      <c r="I17" s="367"/>
-      <c r="J17" s="367"/>
-      <c r="K17" s="367"/>
-      <c r="L17" s="367"/>
-      <c r="M17" s="367"/>
-      <c r="N17" s="367"/>
-      <c r="O17" s="367"/>
-      <c r="P17" s="367"/>
-      <c r="Q17" s="367"/>
-      <c r="R17" s="367"/>
-      <c r="S17" s="367"/>
-      <c r="T17" s="367"/>
-      <c r="U17" s="367"/>
-      <c r="V17" s="367"/>
-      <c r="W17" s="367"/>
-      <c r="X17" s="367"/>
-      <c r="Y17" s="367"/>
-      <c r="Z17" s="367"/>
-      <c r="AA17" s="367"/>
-      <c r="AB17" s="367"/>
+      <c r="A17" s="328"/>
+      <c r="B17" s="328"/>
+      <c r="C17" s="328"/>
+      <c r="D17" s="328"/>
+      <c r="E17" s="328"/>
+      <c r="F17" s="328"/>
+      <c r="G17" s="329"/>
+      <c r="H17" s="329"/>
+      <c r="I17" s="329"/>
+      <c r="J17" s="329"/>
+      <c r="K17" s="329"/>
+      <c r="L17" s="329"/>
+      <c r="M17" s="329"/>
+      <c r="N17" s="329"/>
+      <c r="O17" s="329"/>
+      <c r="P17" s="329"/>
+      <c r="Q17" s="329"/>
+      <c r="R17" s="329"/>
+      <c r="S17" s="329"/>
+      <c r="T17" s="329"/>
+      <c r="U17" s="329"/>
+      <c r="V17" s="329"/>
+      <c r="W17" s="329"/>
+      <c r="X17" s="329"/>
+      <c r="Y17" s="329"/>
+      <c r="Z17" s="329"/>
+      <c r="AA17" s="329"/>
+      <c r="AB17" s="329"/>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A18" s="366"/>
-      <c r="B18" s="366"/>
-      <c r="C18" s="366"/>
-      <c r="D18" s="366"/>
-      <c r="E18" s="366"/>
-      <c r="F18" s="366"/>
-      <c r="G18" s="367"/>
-      <c r="H18" s="367"/>
-      <c r="I18" s="367"/>
-      <c r="J18" s="367"/>
-      <c r="K18" s="367"/>
-      <c r="L18" s="367"/>
-      <c r="M18" s="367"/>
-      <c r="N18" s="367"/>
-      <c r="O18" s="367"/>
-      <c r="P18" s="367"/>
-      <c r="Q18" s="367"/>
-      <c r="R18" s="367"/>
-      <c r="S18" s="367"/>
-      <c r="T18" s="367"/>
-      <c r="U18" s="367"/>
-      <c r="V18" s="367"/>
-      <c r="W18" s="367"/>
-      <c r="X18" s="367"/>
-      <c r="Y18" s="367"/>
-      <c r="Z18" s="367"/>
-      <c r="AA18" s="367"/>
-      <c r="AB18" s="367"/>
+      <c r="A18" s="328"/>
+      <c r="B18" s="328"/>
+      <c r="C18" s="328"/>
+      <c r="D18" s="328"/>
+      <c r="E18" s="328"/>
+      <c r="F18" s="328"/>
+      <c r="G18" s="329"/>
+      <c r="H18" s="329"/>
+      <c r="I18" s="329"/>
+      <c r="J18" s="329"/>
+      <c r="K18" s="329"/>
+      <c r="L18" s="329"/>
+      <c r="M18" s="329"/>
+      <c r="N18" s="329"/>
+      <c r="O18" s="329"/>
+      <c r="P18" s="329"/>
+      <c r="Q18" s="329"/>
+      <c r="R18" s="329"/>
+      <c r="S18" s="329"/>
+      <c r="T18" s="329"/>
+      <c r="U18" s="329"/>
+      <c r="V18" s="329"/>
+      <c r="W18" s="329"/>
+      <c r="X18" s="329"/>
+      <c r="Y18" s="329"/>
+      <c r="Z18" s="329"/>
+      <c r="AA18" s="329"/>
+      <c r="AB18" s="329"/>
     </row>
     <row r="19" spans="1:28" ht="210" x14ac:dyDescent="0.2">
-      <c r="A19" s="366"/>
-      <c r="B19" s="366"/>
-      <c r="C19" s="366"/>
-      <c r="D19" s="366"/>
-      <c r="E19" s="366"/>
-      <c r="F19" s="360" t="s">
+      <c r="A19" s="328"/>
+      <c r="B19" s="328"/>
+      <c r="C19" s="328"/>
+      <c r="D19" s="328"/>
+      <c r="E19" s="328"/>
+      <c r="F19" s="323" t="s">
         <v>553</v>
       </c>
       <c r="G19" s="254" t="s">
         <v>554</v>
       </c>
-      <c r="H19" s="367"/>
-      <c r="I19" s="367"/>
-      <c r="J19" s="367"/>
-      <c r="K19" s="367"/>
-      <c r="L19" s="367"/>
-      <c r="M19" s="367"/>
-      <c r="N19" s="367"/>
-      <c r="O19" s="367"/>
-      <c r="P19" s="367"/>
-      <c r="Q19" s="367"/>
-      <c r="R19" s="367"/>
-      <c r="S19" s="367"/>
-      <c r="T19" s="367"/>
-      <c r="U19" s="361" t="s">
+      <c r="H19" s="329"/>
+      <c r="I19" s="329"/>
+      <c r="J19" s="329"/>
+      <c r="K19" s="329"/>
+      <c r="L19" s="329"/>
+      <c r="M19" s="329"/>
+      <c r="N19" s="329"/>
+      <c r="O19" s="329"/>
+      <c r="P19" s="329"/>
+      <c r="Q19" s="329"/>
+      <c r="R19" s="329"/>
+      <c r="S19" s="329"/>
+      <c r="T19" s="329"/>
+      <c r="U19" s="324" t="s">
         <v>555</v>
       </c>
       <c r="V19" s="254" t="s">
         <v>556</v>
       </c>
-      <c r="W19" s="367"/>
-      <c r="X19" s="367"/>
-      <c r="Y19" s="367"/>
-      <c r="Z19" s="367"/>
-      <c r="AA19" s="367"/>
-      <c r="AB19" s="367"/>
+      <c r="W19" s="329"/>
+      <c r="X19" s="329"/>
+      <c r="Y19" s="329"/>
+      <c r="Z19" s="329"/>
+      <c r="AA19" s="329"/>
+      <c r="AB19" s="329"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -18919,16 +18924,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="357" t="s">
+      <c r="A1" s="372" t="s">
         <v>373</v>
       </c>
-      <c r="B1" s="357"/>
-      <c r="C1" s="357"/>
-      <c r="D1" s="357"/>
-      <c r="E1" s="357"/>
-      <c r="F1" s="357"/>
-      <c r="G1" s="357"/>
-      <c r="H1" s="357"/>
+      <c r="B1" s="372"/>
+      <c r="C1" s="372"/>
+      <c r="D1" s="372"/>
+      <c r="E1" s="372"/>
+      <c r="F1" s="372"/>
+      <c r="G1" s="372"/>
+      <c r="H1" s="372"/>
       <c r="I1" s="291"/>
       <c r="J1" s="291"/>
       <c r="K1" s="291"/>
@@ -18953,7 +18958,7 @@
       <c r="G2" s="293" t="s">
         <v>328</v>
       </c>
-      <c r="H2" s="356" t="s">
+      <c r="H2" s="371" t="s">
         <v>327</v>
       </c>
       <c r="I2" s="293" t="s">
@@ -18986,13 +18991,13 @@
       <c r="R2" s="293" t="s">
         <v>326</v>
       </c>
-      <c r="S2" s="356" t="s">
+      <c r="S2" s="371" t="s">
         <v>325</v>
       </c>
       <c r="T2" s="293" t="s">
         <v>144</v>
       </c>
-      <c r="U2" s="356" t="s">
+      <c r="U2" s="371" t="s">
         <v>324</v>
       </c>
     </row>
@@ -19006,7 +19011,7 @@
       <c r="G3" s="293" t="s">
         <v>317</v>
       </c>
-      <c r="H3" s="356"/>
+      <c r="H3" s="371"/>
       <c r="I3" s="293" t="s">
         <v>369</v>
       </c>
@@ -19037,11 +19042,11 @@
       <c r="R3" s="293" t="s">
         <v>304</v>
       </c>
-      <c r="S3" s="356"/>
+      <c r="S3" s="371"/>
       <c r="T3" s="293" t="s">
         <v>301</v>
       </c>
-      <c r="U3" s="356"/>
+      <c r="U3" s="371"/>
     </row>
     <row r="4" spans="1:21" ht="112" x14ac:dyDescent="0.2">
       <c r="A4" s="290"/>
@@ -19063,7 +19068,7 @@
       <c r="G4" s="293" t="s">
         <v>267</v>
       </c>
-      <c r="H4" s="356"/>
+      <c r="H4" s="371"/>
       <c r="I4" s="293" t="s">
         <v>350</v>
       </c>
@@ -19094,11 +19099,11 @@
       <c r="R4" s="293" t="s">
         <v>253</v>
       </c>
-      <c r="S4" s="356"/>
+      <c r="S4" s="371"/>
       <c r="T4" s="293" t="s">
         <v>249</v>
       </c>
-      <c r="U4" s="356"/>
+      <c r="U4" s="371"/>
     </row>
     <row r="5" spans="1:21" ht="196" x14ac:dyDescent="0.2">
       <c r="A5" s="296" t="s">
@@ -19657,81 +19662,81 @@
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A17" s="368"/>
-      <c r="B17" s="368"/>
-      <c r="C17" s="368"/>
-      <c r="D17" s="368"/>
-      <c r="E17" s="368"/>
-      <c r="F17" s="368"/>
-      <c r="G17" s="368"/>
-      <c r="H17" s="368"/>
-      <c r="I17" s="368"/>
-      <c r="J17" s="368"/>
-      <c r="K17" s="368"/>
-      <c r="L17" s="368"/>
-      <c r="M17" s="368"/>
-      <c r="N17" s="368"/>
-      <c r="O17" s="368"/>
-      <c r="P17" s="368"/>
-      <c r="Q17" s="368"/>
-      <c r="R17" s="368"/>
-      <c r="S17" s="369"/>
-      <c r="T17" s="368"/>
-      <c r="U17" s="368"/>
+      <c r="A17" s="330"/>
+      <c r="B17" s="330"/>
+      <c r="C17" s="330"/>
+      <c r="D17" s="330"/>
+      <c r="E17" s="330"/>
+      <c r="F17" s="330"/>
+      <c r="G17" s="330"/>
+      <c r="H17" s="330"/>
+      <c r="I17" s="330"/>
+      <c r="J17" s="330"/>
+      <c r="K17" s="330"/>
+      <c r="L17" s="330"/>
+      <c r="M17" s="330"/>
+      <c r="N17" s="330"/>
+      <c r="O17" s="330"/>
+      <c r="P17" s="330"/>
+      <c r="Q17" s="330"/>
+      <c r="R17" s="330"/>
+      <c r="S17" s="331"/>
+      <c r="T17" s="330"/>
+      <c r="U17" s="330"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A18" s="368"/>
-      <c r="B18" s="368"/>
-      <c r="C18" s="368"/>
-      <c r="D18" s="368"/>
-      <c r="E18" s="368"/>
-      <c r="F18" s="368"/>
-      <c r="G18" s="368"/>
-      <c r="H18" s="368"/>
-      <c r="I18" s="368"/>
-      <c r="J18" s="368"/>
-      <c r="K18" s="368"/>
-      <c r="L18" s="368"/>
-      <c r="M18" s="368"/>
-      <c r="N18" s="368"/>
-      <c r="O18" s="368"/>
-      <c r="P18" s="368"/>
-      <c r="Q18" s="368"/>
-      <c r="R18" s="368"/>
-      <c r="S18" s="370"/>
-      <c r="T18" s="368"/>
-      <c r="U18" s="368"/>
+      <c r="A18" s="330"/>
+      <c r="B18" s="330"/>
+      <c r="C18" s="330"/>
+      <c r="D18" s="330"/>
+      <c r="E18" s="330"/>
+      <c r="F18" s="330"/>
+      <c r="G18" s="330"/>
+      <c r="H18" s="330"/>
+      <c r="I18" s="330"/>
+      <c r="J18" s="330"/>
+      <c r="K18" s="330"/>
+      <c r="L18" s="330"/>
+      <c r="M18" s="330"/>
+      <c r="N18" s="330"/>
+      <c r="O18" s="330"/>
+      <c r="P18" s="330"/>
+      <c r="Q18" s="330"/>
+      <c r="R18" s="330"/>
+      <c r="S18" s="332"/>
+      <c r="T18" s="330"/>
+      <c r="U18" s="330"/>
     </row>
     <row r="19" spans="1:21" ht="210" x14ac:dyDescent="0.2">
-      <c r="A19" s="371"/>
-      <c r="B19" s="371"/>
-      <c r="C19" s="371"/>
-      <c r="D19" s="372"/>
-      <c r="E19" s="371"/>
-      <c r="F19" s="360" t="s">
+      <c r="A19" s="333"/>
+      <c r="B19" s="333"/>
+      <c r="C19" s="333"/>
+      <c r="D19" s="334"/>
+      <c r="E19" s="333"/>
+      <c r="F19" s="323" t="s">
         <v>553</v>
       </c>
       <c r="G19" s="254" t="s">
         <v>554</v>
       </c>
-      <c r="H19" s="371"/>
-      <c r="I19" s="371"/>
-      <c r="J19" s="371"/>
-      <c r="K19" s="371"/>
-      <c r="L19" s="371"/>
-      <c r="M19" s="371"/>
-      <c r="N19" s="371"/>
-      <c r="O19" s="371"/>
-      <c r="P19" s="371"/>
-      <c r="Q19" s="361" t="s">
+      <c r="H19" s="333"/>
+      <c r="I19" s="333"/>
+      <c r="J19" s="333"/>
+      <c r="K19" s="333"/>
+      <c r="L19" s="333"/>
+      <c r="M19" s="333"/>
+      <c r="N19" s="333"/>
+      <c r="O19" s="333"/>
+      <c r="P19" s="333"/>
+      <c r="Q19" s="324" t="s">
         <v>555</v>
       </c>
       <c r="R19" s="254" t="s">
         <v>556</v>
       </c>
-      <c r="S19" s="371"/>
-      <c r="T19" s="371"/>
-      <c r="U19" s="371"/>
+      <c r="S19" s="333"/>
+      <c r="T19" s="333"/>
+      <c r="U19" s="333"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -19768,9 +19773,9 @@
       <c r="A1" s="269"/>
       <c r="C1" s="271"/>
       <c r="E1" s="269"/>
-      <c r="F1" s="373"/>
+      <c r="F1" s="335"/>
       <c r="G1" s="271"/>
-      <c r="H1" s="373"/>
+      <c r="H1" s="335"/>
       <c r="I1" s="271" t="s">
         <v>375</v>
       </c>
@@ -19794,13 +19799,13 @@
       <c r="K2" s="221" t="s">
         <v>326</v>
       </c>
-      <c r="L2" s="353" t="s">
+      <c r="L2" s="368" t="s">
         <v>325</v>
       </c>
       <c r="M2" s="221" t="s">
         <v>144</v>
       </c>
-      <c r="N2" s="353" t="s">
+      <c r="N2" s="368" t="s">
         <v>324</v>
       </c>
     </row>
@@ -19818,11 +19823,11 @@
       <c r="K3" s="221" t="s">
         <v>304</v>
       </c>
-      <c r="L3" s="353"/>
+      <c r="L3" s="368"/>
       <c r="M3" s="221" t="s">
         <v>301</v>
       </c>
-      <c r="N3" s="353"/>
+      <c r="N3" s="368"/>
     </row>
     <row r="4" spans="1:14" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="274"/>
@@ -19848,11 +19853,11 @@
       <c r="K4" s="221" t="s">
         <v>253</v>
       </c>
-      <c r="L4" s="353"/>
+      <c r="L4" s="368"/>
       <c r="M4" s="221" t="s">
         <v>249</v>
       </c>
-      <c r="N4" s="353"/>
+      <c r="N4" s="368"/>
     </row>
     <row r="5" spans="1:14" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="276"/>
@@ -20145,28 +20150,28 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="37" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E15" s="373"/>
-      <c r="F15" s="373"/>
-      <c r="G15" s="373"/>
-      <c r="H15" s="373"/>
-      <c r="I15" s="373"/>
-      <c r="J15" s="373"/>
-      <c r="K15" s="373"/>
-      <c r="L15" s="373"/>
-      <c r="M15" s="373"/>
-      <c r="N15" s="373"/>
+      <c r="E15" s="335"/>
+      <c r="F15" s="335"/>
+      <c r="G15" s="335"/>
+      <c r="H15" s="335"/>
+      <c r="I15" s="335"/>
+      <c r="J15" s="335"/>
+      <c r="K15" s="335"/>
+      <c r="L15" s="335"/>
+      <c r="M15" s="335"/>
+      <c r="N15" s="335"/>
     </row>
     <row r="16" spans="1:14" ht="37" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E16" s="373"/>
-      <c r="F16" s="373"/>
-      <c r="G16" s="373"/>
-      <c r="H16" s="373"/>
-      <c r="I16" s="373"/>
-      <c r="J16" s="373"/>
-      <c r="K16" s="373"/>
-      <c r="L16" s="373"/>
-      <c r="M16" s="373"/>
-      <c r="N16" s="373"/>
+      <c r="E16" s="335"/>
+      <c r="F16" s="335"/>
+      <c r="G16" s="335"/>
+      <c r="H16" s="335"/>
+      <c r="I16" s="335"/>
+      <c r="J16" s="335"/>
+      <c r="K16" s="335"/>
+      <c r="L16" s="335"/>
+      <c r="M16" s="335"/>
+      <c r="N16" s="335"/>
     </row>
     <row r="17" spans="4:4" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D17" s="289"/>
@@ -20541,14 +20546,14 @@
       <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="FA1" s="340" t="s">
+      <c r="FA1" s="355" t="s">
         <v>382</v>
       </c>
-      <c r="FB1" s="340"/>
-      <c r="FC1" s="340"/>
-      <c r="FD1" s="340"/>
-      <c r="FE1" s="340"/>
-      <c r="FF1" s="340"/>
+      <c r="FB1" s="355"/>
+      <c r="FC1" s="355"/>
+      <c r="FD1" s="355"/>
+      <c r="FE1" s="355"/>
+      <c r="FF1" s="355"/>
       <c r="FG1" s="8" t="s">
         <v>0</v>
       </c>
@@ -20691,28 +20696,28 @@
       <c r="D4" s="312"/>
       <c r="E4" s="312"/>
       <c r="F4" s="312"/>
-      <c r="G4" s="341" t="s">
+      <c r="G4" s="356" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="342"/>
-      <c r="I4" s="342"/>
-      <c r="J4" s="342"/>
-      <c r="K4" s="342"/>
-      <c r="L4" s="343"/>
-      <c r="M4" s="344"/>
-      <c r="N4" s="345" t="s">
+      <c r="H4" s="357"/>
+      <c r="I4" s="357"/>
+      <c r="J4" s="357"/>
+      <c r="K4" s="357"/>
+      <c r="L4" s="358"/>
+      <c r="M4" s="359"/>
+      <c r="N4" s="360" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="343"/>
-      <c r="P4" s="343"/>
-      <c r="Q4" s="343"/>
-      <c r="R4" s="343"/>
-      <c r="S4" s="343"/>
-      <c r="T4" s="346"/>
-      <c r="U4" s="341" t="s">
+      <c r="O4" s="358"/>
+      <c r="P4" s="358"/>
+      <c r="Q4" s="358"/>
+      <c r="R4" s="358"/>
+      <c r="S4" s="358"/>
+      <c r="T4" s="361"/>
+      <c r="U4" s="356" t="s">
         <v>28</v>
       </c>
-      <c r="V4" s="344"/>
+      <c r="V4" s="359"/>
       <c r="W4" s="319"/>
       <c r="X4" t="s">
         <v>0</v>
@@ -21021,8 +21026,8 @@
   </sheetPr>
   <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView zoomScale="94" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView topLeftCell="A43" zoomScale="94" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -22214,9 +22219,11 @@
         <v>105</v>
       </c>
       <c r="F59" s="36" t="s">
-        <v>144</v>
-      </c>
-      <c r="G59" s="36"/>
+        <v>578</v>
+      </c>
+      <c r="G59" s="36" t="s">
+        <v>579</v>
+      </c>
     </row>
     <row r="60" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="43" t="s">
@@ -22445,16 +22452,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" s="60" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B1" s="348" t="s">
+      <c r="B1" s="363" t="s">
         <v>329</v>
       </c>
-      <c r="C1" s="348"/>
-      <c r="D1" s="348"/>
-      <c r="E1" s="348"/>
-      <c r="F1" s="348"/>
-      <c r="G1" s="348"/>
-      <c r="H1" s="348"/>
-      <c r="I1" s="348"/>
+      <c r="C1" s="363"/>
+      <c r="D1" s="363"/>
+      <c r="E1" s="363"/>
+      <c r="F1" s="363"/>
+      <c r="G1" s="363"/>
+      <c r="H1" s="363"/>
+      <c r="I1" s="363"/>
     </row>
     <row r="2" spans="1:62" s="60" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="106"/>
@@ -22466,7 +22473,7 @@
       <c r="G2" s="103" t="s">
         <v>328</v>
       </c>
-      <c r="H2" s="347" t="s">
+      <c r="H2" s="362" t="s">
         <v>327</v>
       </c>
       <c r="I2" s="102" t="s">
@@ -22511,7 +22518,7 @@
       <c r="V2" s="102" t="s">
         <v>326</v>
       </c>
-      <c r="W2" s="347" t="s">
+      <c r="W2" s="362" t="s">
         <v>325</v>
       </c>
       <c r="X2" s="103" t="s">
@@ -22526,7 +22533,7 @@
       <c r="AA2" s="103" t="s">
         <v>144</v>
       </c>
-      <c r="AB2" s="347" t="s">
+      <c r="AB2" s="362" t="s">
         <v>324</v>
       </c>
       <c r="AC2" s="100" t="s">
@@ -22556,7 +22563,7 @@
       <c r="AK2" s="100" t="s">
         <v>323</v>
       </c>
-      <c r="AL2" s="347" t="s">
+      <c r="AL2" s="362" t="s">
         <v>322</v>
       </c>
       <c r="AM2" s="100" t="s">
@@ -22598,7 +22605,7 @@
       <c r="AY2" s="100" t="s">
         <v>321</v>
       </c>
-      <c r="AZ2" s="347" t="s">
+      <c r="AZ2" s="362" t="s">
         <v>320</v>
       </c>
       <c r="BA2" s="99" t="s">
@@ -22628,7 +22635,7 @@
       <c r="BI2" s="99" t="s">
         <v>319</v>
       </c>
-      <c r="BJ2" s="347" t="s">
+      <c r="BJ2" s="362" t="s">
         <v>318</v>
       </c>
     </row>
@@ -22642,7 +22649,7 @@
       <c r="G3" s="103" t="s">
         <v>317</v>
       </c>
-      <c r="H3" s="347"/>
+      <c r="H3" s="362"/>
       <c r="I3" s="102" t="s">
         <v>316</v>
       </c>
@@ -22683,7 +22690,7 @@
       <c r="V3" s="102" t="s">
         <v>304</v>
       </c>
-      <c r="W3" s="347"/>
+      <c r="W3" s="362"/>
       <c r="X3" s="98"/>
       <c r="Y3" s="103" t="s">
         <v>303</v>
@@ -22694,7 +22701,7 @@
       <c r="AA3" s="103" t="s">
         <v>301</v>
       </c>
-      <c r="AB3" s="347"/>
+      <c r="AB3" s="362"/>
       <c r="AC3" s="100" t="s">
         <v>300</v>
       </c>
@@ -22722,7 +22729,7 @@
       <c r="AK3" s="100" t="s">
         <v>294</v>
       </c>
-      <c r="AL3" s="347"/>
+      <c r="AL3" s="362"/>
       <c r="AM3" s="100" t="s">
         <v>293</v>
       </c>
@@ -22762,7 +22769,7 @@
       <c r="AY3" s="100" t="s">
         <v>281</v>
       </c>
-      <c r="AZ3" s="347"/>
+      <c r="AZ3" s="362"/>
       <c r="BA3" s="99" t="s">
         <v>280</v>
       </c>
@@ -22790,7 +22797,7 @@
       <c r="BI3" s="99" t="s">
         <v>272</v>
       </c>
-      <c r="BJ3" s="347"/>
+      <c r="BJ3" s="362"/>
     </row>
     <row r="4" spans="1:62" s="60" customFormat="1" ht="60" x14ac:dyDescent="0.15">
       <c r="A4" s="105"/>
@@ -22812,7 +22819,7 @@
       <c r="G4" s="103" t="s">
         <v>267</v>
       </c>
-      <c r="H4" s="347"/>
+      <c r="H4" s="362"/>
       <c r="I4" s="102" t="s">
         <v>266</v>
       </c>
@@ -22855,7 +22862,7 @@
       <c r="V4" s="102" t="s">
         <v>253</v>
       </c>
-      <c r="W4" s="347"/>
+      <c r="W4" s="362"/>
       <c r="X4" s="101" t="s">
         <v>252</v>
       </c>
@@ -22868,7 +22875,7 @@
       <c r="AA4" s="101" t="s">
         <v>249</v>
       </c>
-      <c r="AB4" s="347"/>
+      <c r="AB4" s="362"/>
       <c r="AC4" s="100" t="s">
         <v>248</v>
       </c>
@@ -22896,7 +22903,7 @@
       <c r="AK4" s="100" t="s">
         <v>241</v>
       </c>
-      <c r="AL4" s="347"/>
+      <c r="AL4" s="362"/>
       <c r="AM4" s="100" t="s">
         <v>240</v>
       </c>
@@ -22936,7 +22943,7 @@
       <c r="AY4" s="100" t="s">
         <v>228</v>
       </c>
-      <c r="AZ4" s="347"/>
+      <c r="AZ4" s="362"/>
       <c r="BA4" s="99" t="s">
         <v>227</v>
       </c>
@@ -22964,7 +22971,7 @@
       <c r="BI4" s="99" t="s">
         <v>219</v>
       </c>
-      <c r="BJ4" s="347"/>
+      <c r="BJ4" s="362"/>
     </row>
     <row r="5" spans="1:62" s="60" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="70" t="s">
@@ -24257,13 +24264,13 @@
         <v>#N/A</v>
       </c>
       <c r="AC13" s="82"/>
-      <c r="AD13" s="358" t="e">
+      <c r="AD13" s="321" t="e">
         <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"JCP")+
 SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"VPCP")+
 SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"1VPCP")</f>
         <v>#N/A</v>
       </c>
-      <c r="AE13" s="358" t="e">
+      <c r="AE13" s="321" t="e">
         <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"JI")+
 SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"VPI")+
 SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"1VPI")</f>
@@ -24272,19 +24279,19 @@
       <c r="AF13" s="82"/>
       <c r="AG13" s="82"/>
       <c r="AH13" s="82"/>
-      <c r="AI13" s="358" t="e">
+      <c r="AI13" s="321" t="e">
         <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"JAP")+
 SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"VPAP")+
 SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"1VPAP")</f>
         <v>#N/A</v>
       </c>
-      <c r="AJ13" s="358" t="e">
+      <c r="AJ13" s="321" t="e">
         <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"JE")+
 SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"VPE")+
 SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"1VPE")</f>
         <v>#N/A</v>
       </c>
-      <c r="AK13" s="358" t="e">
+      <c r="AK13" s="321" t="e">
         <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"VPLD")+
 SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"1VPLD")</f>
         <v>#N/A</v>
@@ -24305,7 +24312,7 @@
       <c r="AV13" s="82"/>
       <c r="AW13" s="82"/>
       <c r="AX13" s="82"/>
-      <c r="AY13" s="358" t="e">
+      <c r="AY13" s="321" t="e">
         <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"Magistrat SIEGE NS")</f>
         <v>#N/A</v>
       </c>
@@ -25085,8 +25092,8 @@
       </c>
       <c r="AZ19" s="57"/>
     </row>
-    <row r="20" spans="1:62" ht="252" x14ac:dyDescent="0.2">
-      <c r="F20" s="360" t="s">
+    <row r="20" spans="1:62" ht="28" x14ac:dyDescent="0.2">
+      <c r="F20" s="323" t="s">
         <v>553</v>
       </c>
       <c r="G20" s="254" t="e">
@@ -25094,7 +25101,7 @@
 SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH placé SUB")</f>
         <v>#N/A</v>
       </c>
-      <c r="U20" s="361" t="s">
+      <c r="U20" s="324" t="s">
         <v>555</v>
       </c>
       <c r="V20" s="254" t="e">
@@ -25103,7 +25110,7 @@
         <v>#N/A</v>
       </c>
       <c r="W20" s="57"/>
-      <c r="AX20" s="359" t="s">
+      <c r="AX20" s="322" t="s">
         <v>551</v>
       </c>
       <c r="AY20" s="196" t="e">
@@ -25161,16 +25168,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A1" s="349" t="s">
+      <c r="A1" s="364" t="s">
         <v>373</v>
       </c>
-      <c r="B1" s="349"/>
-      <c r="C1" s="349"/>
-      <c r="D1" s="349"/>
-      <c r="E1" s="349"/>
-      <c r="F1" s="349"/>
-      <c r="G1" s="349"/>
-      <c r="H1" s="349"/>
+      <c r="B1" s="364"/>
+      <c r="C1" s="364"/>
+      <c r="D1" s="364"/>
+      <c r="E1" s="364"/>
+      <c r="F1" s="364"/>
+      <c r="G1" s="364"/>
+      <c r="H1" s="364"/>
       <c r="I1" s="60"/>
       <c r="J1" s="60"/>
       <c r="K1" s="60"/>
@@ -25209,7 +25216,7 @@
       <c r="G2" s="103" t="s">
         <v>328</v>
       </c>
-      <c r="H2" s="347" t="s">
+      <c r="H2" s="362" t="s">
         <v>327</v>
       </c>
       <c r="I2" s="103" t="s">
@@ -25242,13 +25249,13 @@
       <c r="R2" s="103" t="s">
         <v>326</v>
       </c>
-      <c r="S2" s="347" t="s">
+      <c r="S2" s="362" t="s">
         <v>325</v>
       </c>
       <c r="T2" s="103" t="s">
         <v>144</v>
       </c>
-      <c r="U2" s="347" t="s">
+      <c r="U2" s="362" t="s">
         <v>324</v>
       </c>
       <c r="V2" s="103" t="s">
@@ -25278,7 +25285,7 @@
       <c r="AD2" s="103" t="s">
         <v>323</v>
       </c>
-      <c r="AE2" s="347" t="s">
+      <c r="AE2" s="362" t="s">
         <v>372</v>
       </c>
       <c r="AF2" s="103" t="s">
@@ -25290,7 +25297,7 @@
       <c r="AH2" s="103" t="s">
         <v>371</v>
       </c>
-      <c r="AI2" s="347" t="s">
+      <c r="AI2" s="362" t="s">
         <v>370</v>
       </c>
     </row>
@@ -25304,7 +25311,7 @@
       <c r="G3" s="103" t="s">
         <v>317</v>
       </c>
-      <c r="H3" s="347"/>
+      <c r="H3" s="362"/>
       <c r="I3" s="103" t="s">
         <v>369</v>
       </c>
@@ -25335,11 +25342,11 @@
       <c r="R3" s="103" t="s">
         <v>304</v>
       </c>
-      <c r="S3" s="347"/>
+      <c r="S3" s="362"/>
       <c r="T3" s="103" t="s">
         <v>301</v>
       </c>
-      <c r="U3" s="347"/>
+      <c r="U3" s="362"/>
       <c r="V3" s="103" t="s">
         <v>360</v>
       </c>
@@ -25367,7 +25374,7 @@
       <c r="AD3" s="103" t="s">
         <v>352</v>
       </c>
-      <c r="AE3" s="347"/>
+      <c r="AE3" s="362"/>
       <c r="AF3" s="103" t="s">
         <v>351</v>
       </c>
@@ -25377,7 +25384,7 @@
       <c r="AH3" s="103" t="s">
         <v>281</v>
       </c>
-      <c r="AI3" s="347"/>
+      <c r="AI3" s="362"/>
     </row>
     <row r="4" spans="1:35" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="106"/>
@@ -25399,7 +25406,7 @@
       <c r="G4" s="103" t="s">
         <v>267</v>
       </c>
-      <c r="H4" s="347"/>
+      <c r="H4" s="362"/>
       <c r="I4" s="103" t="s">
         <v>350</v>
       </c>
@@ -25430,11 +25437,11 @@
       <c r="R4" s="103" t="s">
         <v>253</v>
       </c>
-      <c r="S4" s="347"/>
+      <c r="S4" s="362"/>
       <c r="T4" s="103" t="s">
         <v>249</v>
       </c>
-      <c r="U4" s="347"/>
+      <c r="U4" s="362"/>
       <c r="V4" s="103" t="s">
         <v>341</v>
       </c>
@@ -25462,7 +25469,7 @@
       <c r="AD4" s="103" t="s">
         <v>333</v>
       </c>
-      <c r="AE4" s="347"/>
+      <c r="AE4" s="362"/>
       <c r="AF4" s="103" t="s">
         <v>332</v>
       </c>
@@ -25472,7 +25479,7 @@
       <c r="AH4" s="103" t="s">
         <v>228</v>
       </c>
-      <c r="AI4" s="347"/>
+      <c r="AI4" s="362"/>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A5" s="109" t="s">
@@ -26139,7 +26146,7 @@
       </c>
       <c r="AF13" s="82"/>
       <c r="AG13" s="82"/>
-      <c r="AH13" s="358" t="e">
+      <c r="AH13" s="321" t="e">
         <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")</f>
         <v>#N/A</v>
       </c>
@@ -26478,8 +26485,8 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="18" spans="4:34" ht="196" x14ac:dyDescent="0.2">
-      <c r="F18" s="360" t="s">
+    <row r="18" spans="4:34" ht="28" x14ac:dyDescent="0.2">
+      <c r="F18" s="323" t="s">
         <v>553</v>
       </c>
       <c r="G18" s="254" t="e">
@@ -26487,7 +26494,7 @@
 SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH placé SUB")</f>
         <v>#N/A</v>
       </c>
-      <c r="Q18" s="361" t="s">
+      <c r="Q18" s="324" t="s">
         <v>555</v>
       </c>
       <c r="R18" s="254" t="e">
@@ -26496,8 +26503,8 @@
         <v>#N/A</v>
       </c>
       <c r="S18" s="57"/>
-      <c r="AF18" s="362"/>
-      <c r="AG18" s="359" t="s">
+      <c r="AF18" s="325"/>
+      <c r="AG18" s="322" t="s">
         <v>551</v>
       </c>
       <c r="AH18" s="72" t="e">

</xml_diff>

<commit_message>
add column JE JI extractor
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956251AA-BB3D-9C4F-A9C1-8FA0D21741F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{570E6720-6A4F-8F4B-BBDD-39A5917784D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1948" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1950" uniqueCount="582">
   <si>
     <t>#! END_ROW</t>
   </si>
@@ -5209,6 +5209,12 @@
   </si>
   <si>
     <t>Pas encore appelé dans la matrice DDG, à voir en fonction de la circulaire 2025/2026</t>
+  </si>
+  <si>
+    <t>Ecart JE</t>
+  </si>
+  <si>
+    <t>Ecart JI</t>
   </si>
 </sst>
 </file>
@@ -6404,7 +6410,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="373">
+  <cellXfs count="374">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -7585,6 +7591,9 @@
     </xf>
     <xf numFmtId="0" fontId="39" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -8432,7 +8441,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:F14"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8722,13 +8731,13 @@
       <c r="G2" s="103" t="s">
         <v>326</v>
       </c>
-      <c r="H2" s="362" t="s">
+      <c r="H2" s="363" t="s">
         <v>325</v>
       </c>
       <c r="I2" s="103" t="s">
         <v>144</v>
       </c>
-      <c r="J2" s="362" t="s">
+      <c r="J2" s="363" t="s">
         <v>324</v>
       </c>
     </row>
@@ -8742,11 +8751,11 @@
       <c r="G3" s="103" t="s">
         <v>304</v>
       </c>
-      <c r="H3" s="362"/>
+      <c r="H3" s="363"/>
       <c r="I3" s="103" t="s">
         <v>301</v>
       </c>
-      <c r="J3" s="362"/>
+      <c r="J3" s="363"/>
     </row>
     <row r="4" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A4" s="125"/>
@@ -8768,11 +8777,11 @@
       <c r="G4" s="103" t="s">
         <v>253</v>
       </c>
-      <c r="H4" s="362"/>
+      <c r="H4" s="363"/>
       <c r="I4" s="103" t="s">
         <v>249</v>
       </c>
-      <c r="J4" s="362"/>
+      <c r="J4" s="363"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="119" t="s">
@@ -9176,7 +9185,7 @@
       <c r="G2" s="103" t="s">
         <v>328</v>
       </c>
-      <c r="H2" s="362" t="s">
+      <c r="H2" s="363" t="s">
         <v>327</v>
       </c>
       <c r="I2" s="102" t="s">
@@ -9221,7 +9230,7 @@
       <c r="V2" s="102" t="s">
         <v>326</v>
       </c>
-      <c r="W2" s="362" t="s">
+      <c r="W2" s="363" t="s">
         <v>325</v>
       </c>
       <c r="X2" s="103" t="s">
@@ -9236,7 +9245,7 @@
       <c r="AA2" s="103" t="s">
         <v>144</v>
       </c>
-      <c r="AB2" s="362" t="s">
+      <c r="AB2" s="363" t="s">
         <v>324</v>
       </c>
       <c r="AC2" s="100" t="s">
@@ -9266,7 +9275,7 @@
       <c r="AK2" s="100" t="s">
         <v>323</v>
       </c>
-      <c r="AL2" s="362" t="s">
+      <c r="AL2" s="363" t="s">
         <v>322</v>
       </c>
       <c r="AM2" s="100" t="s">
@@ -9308,7 +9317,7 @@
       <c r="AY2" s="100" t="s">
         <v>321</v>
       </c>
-      <c r="AZ2" s="362" t="s">
+      <c r="AZ2" s="363" t="s">
         <v>320</v>
       </c>
       <c r="BA2" s="99" t="s">
@@ -9338,7 +9347,7 @@
       <c r="BI2" s="99" t="s">
         <v>319</v>
       </c>
-      <c r="BJ2" s="362" t="s">
+      <c r="BJ2" s="363" t="s">
         <v>318</v>
       </c>
       <c r="BK2"/>
@@ -9353,7 +9362,7 @@
       <c r="G3" s="103" t="s">
         <v>317</v>
       </c>
-      <c r="H3" s="362"/>
+      <c r="H3" s="363"/>
       <c r="I3" s="102" t="s">
         <v>316</v>
       </c>
@@ -9394,7 +9403,7 @@
       <c r="V3" s="102" t="s">
         <v>304</v>
       </c>
-      <c r="W3" s="362"/>
+      <c r="W3" s="363"/>
       <c r="X3" s="98"/>
       <c r="Y3" s="103" t="s">
         <v>303</v>
@@ -9405,7 +9414,7 @@
       <c r="AA3" s="103" t="s">
         <v>301</v>
       </c>
-      <c r="AB3" s="362"/>
+      <c r="AB3" s="363"/>
       <c r="AC3" s="100" t="s">
         <v>300</v>
       </c>
@@ -9433,7 +9442,7 @@
       <c r="AK3" s="100" t="s">
         <v>294</v>
       </c>
-      <c r="AL3" s="362"/>
+      <c r="AL3" s="363"/>
       <c r="AM3" s="100" t="s">
         <v>293</v>
       </c>
@@ -9473,7 +9482,7 @@
       <c r="AY3" s="100" t="s">
         <v>281</v>
       </c>
-      <c r="AZ3" s="362"/>
+      <c r="AZ3" s="363"/>
       <c r="BA3" s="99" t="s">
         <v>280</v>
       </c>
@@ -9501,7 +9510,7 @@
       <c r="BI3" s="99" t="s">
         <v>272</v>
       </c>
-      <c r="BJ3" s="362"/>
+      <c r="BJ3" s="363"/>
     </row>
     <row r="4" spans="1:63" s="60" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="105"/>
@@ -9523,7 +9532,7 @@
       <c r="G4" s="103" t="s">
         <v>267</v>
       </c>
-      <c r="H4" s="362"/>
+      <c r="H4" s="363"/>
       <c r="I4" s="102" t="s">
         <v>266</v>
       </c>
@@ -9566,7 +9575,7 @@
       <c r="V4" s="102" t="s">
         <v>253</v>
       </c>
-      <c r="W4" s="362"/>
+      <c r="W4" s="363"/>
       <c r="X4" s="101" t="s">
         <v>252</v>
       </c>
@@ -9579,7 +9588,7 @@
       <c r="AA4" s="101" t="s">
         <v>249</v>
       </c>
-      <c r="AB4" s="362"/>
+      <c r="AB4" s="363"/>
       <c r="AC4" s="100" t="s">
         <v>248</v>
       </c>
@@ -9607,7 +9616,7 @@
       <c r="AK4" s="100" t="s">
         <v>241</v>
       </c>
-      <c r="AL4" s="362"/>
+      <c r="AL4" s="363"/>
       <c r="AM4" s="100" t="s">
         <v>240</v>
       </c>
@@ -9647,7 +9656,7 @@
       <c r="AY4" s="100" t="s">
         <v>228</v>
       </c>
-      <c r="AZ4" s="362"/>
+      <c r="AZ4" s="363"/>
       <c r="BA4" s="99" t="s">
         <v>227</v>
       </c>
@@ -9675,7 +9684,7 @@
       <c r="BI4" s="99" t="s">
         <v>219</v>
       </c>
-      <c r="BJ4" s="362"/>
+      <c r="BJ4" s="363"/>
       <c r="BK4"/>
     </row>
     <row r="5" spans="1:63" s="60" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -12425,7 +12434,7 @@
       <c r="G2" s="103" t="s">
         <v>328</v>
       </c>
-      <c r="H2" s="362" t="s">
+      <c r="H2" s="363" t="s">
         <v>327</v>
       </c>
       <c r="I2" s="103" t="s">
@@ -12458,13 +12467,13 @@
       <c r="R2" s="103" t="s">
         <v>326</v>
       </c>
-      <c r="S2" s="362" t="s">
+      <c r="S2" s="363" t="s">
         <v>325</v>
       </c>
       <c r="T2" s="103" t="s">
         <v>144</v>
       </c>
-      <c r="U2" s="362" t="s">
+      <c r="U2" s="363" t="s">
         <v>324</v>
       </c>
       <c r="V2" s="103" t="s">
@@ -12494,7 +12503,7 @@
       <c r="AD2" s="103" t="s">
         <v>323</v>
       </c>
-      <c r="AE2" s="362" t="s">
+      <c r="AE2" s="363" t="s">
         <v>372</v>
       </c>
       <c r="AF2" s="103" t="s">
@@ -12506,7 +12515,7 @@
       <c r="AH2" s="103" t="s">
         <v>371</v>
       </c>
-      <c r="AI2" s="362" t="s">
+      <c r="AI2" s="363" t="s">
         <v>370</v>
       </c>
     </row>
@@ -12520,7 +12529,7 @@
       <c r="G3" s="103" t="s">
         <v>317</v>
       </c>
-      <c r="H3" s="362"/>
+      <c r="H3" s="363"/>
       <c r="I3" s="103" t="s">
         <v>369</v>
       </c>
@@ -12551,11 +12560,11 @@
       <c r="R3" s="103" t="s">
         <v>304</v>
       </c>
-      <c r="S3" s="362"/>
+      <c r="S3" s="363"/>
       <c r="T3" s="103" t="s">
         <v>301</v>
       </c>
-      <c r="U3" s="362"/>
+      <c r="U3" s="363"/>
       <c r="V3" s="103" t="s">
         <v>360</v>
       </c>
@@ -12583,7 +12592,7 @@
       <c r="AD3" s="103" t="s">
         <v>352</v>
       </c>
-      <c r="AE3" s="362"/>
+      <c r="AE3" s="363"/>
       <c r="AF3" s="103" t="s">
         <v>351</v>
       </c>
@@ -12593,7 +12602,7 @@
       <c r="AH3" s="103" t="s">
         <v>281</v>
       </c>
-      <c r="AI3" s="362"/>
+      <c r="AI3" s="363"/>
     </row>
     <row r="4" spans="1:62" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="106"/>
@@ -12615,7 +12624,7 @@
       <c r="G4" s="103" t="s">
         <v>267</v>
       </c>
-      <c r="H4" s="362"/>
+      <c r="H4" s="363"/>
       <c r="I4" s="103" t="s">
         <v>350</v>
       </c>
@@ -12646,11 +12655,11 @@
       <c r="R4" s="103" t="s">
         <v>253</v>
       </c>
-      <c r="S4" s="362"/>
+      <c r="S4" s="363"/>
       <c r="T4" s="103" t="s">
         <v>249</v>
       </c>
-      <c r="U4" s="362"/>
+      <c r="U4" s="363"/>
       <c r="V4" s="103" t="s">
         <v>341</v>
       </c>
@@ -12678,7 +12687,7 @@
       <c r="AD4" s="103" t="s">
         <v>333</v>
       </c>
-      <c r="AE4" s="362"/>
+      <c r="AE4" s="363"/>
       <c r="AF4" s="103" t="s">
         <v>332</v>
       </c>
@@ -12688,7 +12697,7 @@
       <c r="AH4" s="103" t="s">
         <v>228</v>
       </c>
-      <c r="AI4" s="362"/>
+      <c r="AI4" s="363"/>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A5" s="109" t="s">
@@ -14445,13 +14454,13 @@
       <c r="G2" s="103" t="s">
         <v>326</v>
       </c>
-      <c r="H2" s="362" t="s">
+      <c r="H2" s="363" t="s">
         <v>325</v>
       </c>
       <c r="I2" s="103" t="s">
         <v>144</v>
       </c>
-      <c r="J2" s="362" t="s">
+      <c r="J2" s="363" t="s">
         <v>324</v>
       </c>
     </row>
@@ -14465,11 +14474,11 @@
       <c r="G3" s="103" t="s">
         <v>304</v>
       </c>
-      <c r="H3" s="362"/>
+      <c r="H3" s="363"/>
       <c r="I3" s="103" t="s">
         <v>301</v>
       </c>
-      <c r="J3" s="362"/>
+      <c r="J3" s="363"/>
     </row>
     <row r="4" spans="1:62" ht="36" x14ac:dyDescent="0.2">
       <c r="A4" s="125"/>
@@ -14491,11 +14500,11 @@
       <c r="G4" s="103" t="s">
         <v>253</v>
       </c>
-      <c r="H4" s="362"/>
+      <c r="H4" s="363"/>
       <c r="I4" s="103" t="s">
         <v>249</v>
       </c>
-      <c r="J4" s="362"/>
+      <c r="J4" s="363"/>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A5" s="119" t="s">
@@ -14890,13 +14899,13 @@
   <sheetData>
     <row r="1" spans="1:61" s="186" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="185"/>
-      <c r="B1" s="366" t="s">
+      <c r="B1" s="367" t="s">
         <v>329</v>
       </c>
-      <c r="C1" s="366"/>
-      <c r="D1" s="366"/>
-      <c r="E1" s="366"/>
-      <c r="F1" s="366"/>
+      <c r="C1" s="367"/>
+      <c r="D1" s="367"/>
+      <c r="E1" s="367"/>
+      <c r="F1" s="367"/>
       <c r="G1" s="187"/>
       <c r="H1" s="187"/>
       <c r="I1" s="187"/>
@@ -14941,7 +14950,7 @@
       <c r="O2" s="189" t="s">
         <v>323</v>
       </c>
-      <c r="P2" s="365" t="s">
+      <c r="P2" s="366" t="s">
         <v>322</v>
       </c>
       <c r="Q2" s="189" t="s">
@@ -14983,7 +14992,7 @@
       <c r="AC2" s="189" t="s">
         <v>321</v>
       </c>
-      <c r="AD2" s="365" t="s">
+      <c r="AD2" s="366" t="s">
         <v>320</v>
       </c>
       <c r="AE2" s="190" t="s">
@@ -15013,7 +15022,7 @@
       <c r="AM2" s="190" t="s">
         <v>319</v>
       </c>
-      <c r="AN2" s="365" t="s">
+      <c r="AN2" s="366" t="s">
         <v>318</v>
       </c>
       <c r="AQ2" s="189"/>
@@ -15024,7 +15033,7 @@
       <c r="AV2" s="189"/>
       <c r="AW2" s="189"/>
       <c r="AX2" s="189"/>
-      <c r="AY2" s="365"/>
+      <c r="AY2" s="366"/>
       <c r="AZ2" s="190"/>
       <c r="BA2" s="190"/>
       <c r="BB2" s="190"/>
@@ -15034,7 +15043,7 @@
       <c r="BF2" s="190"/>
       <c r="BG2" s="190"/>
       <c r="BH2" s="190"/>
-      <c r="BI2" s="365"/>
+      <c r="BI2" s="366"/>
     </row>
     <row r="3" spans="1:61" s="186" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="188"/>
@@ -15070,7 +15079,7 @@
       <c r="O3" s="189" t="s">
         <v>294</v>
       </c>
-      <c r="P3" s="365"/>
+      <c r="P3" s="366"/>
       <c r="Q3" s="189" t="s">
         <v>293</v>
       </c>
@@ -15110,7 +15119,7 @@
       <c r="AC3" s="189" t="s">
         <v>281</v>
       </c>
-      <c r="AD3" s="365"/>
+      <c r="AD3" s="366"/>
       <c r="AE3" s="190" t="s">
         <v>280</v>
       </c>
@@ -15138,7 +15147,7 @@
       <c r="AM3" s="190" t="s">
         <v>272</v>
       </c>
-      <c r="AN3" s="365"/>
+      <c r="AN3" s="366"/>
       <c r="AQ3" s="189"/>
       <c r="AR3" s="189"/>
       <c r="AS3" s="189"/>
@@ -15147,7 +15156,7 @@
       <c r="AV3" s="189"/>
       <c r="AW3" s="189"/>
       <c r="AX3" s="189"/>
-      <c r="AY3" s="365"/>
+      <c r="AY3" s="366"/>
       <c r="AZ3" s="190"/>
       <c r="BA3" s="190"/>
       <c r="BB3" s="190"/>
@@ -15157,7 +15166,7 @@
       <c r="BF3" s="190"/>
       <c r="BG3" s="190"/>
       <c r="BH3" s="190"/>
-      <c r="BI3" s="365"/>
+      <c r="BI3" s="366"/>
     </row>
     <row r="4" spans="1:61" s="186" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="191"/>
@@ -15203,7 +15212,7 @@
       <c r="O4" s="189" t="s">
         <v>241</v>
       </c>
-      <c r="P4" s="365"/>
+      <c r="P4" s="366"/>
       <c r="Q4" s="189" t="s">
         <v>240</v>
       </c>
@@ -15243,7 +15252,7 @@
       <c r="AC4" s="189" t="s">
         <v>228</v>
       </c>
-      <c r="AD4" s="365"/>
+      <c r="AD4" s="366"/>
       <c r="AE4" s="190" t="s">
         <v>227</v>
       </c>
@@ -15271,7 +15280,7 @@
       <c r="AM4" s="190" t="s">
         <v>219</v>
       </c>
-      <c r="AN4" s="365"/>
+      <c r="AN4" s="366"/>
       <c r="AQ4" s="189"/>
       <c r="AR4" s="189"/>
       <c r="AS4" s="189"/>
@@ -15280,7 +15289,7 @@
       <c r="AV4" s="189"/>
       <c r="AW4" s="189"/>
       <c r="AX4" s="189"/>
-      <c r="AY4" s="365"/>
+      <c r="AY4" s="366"/>
       <c r="AZ4" s="190"/>
       <c r="BA4" s="190"/>
       <c r="BB4" s="190"/>
@@ -15290,7 +15299,7 @@
       <c r="BF4" s="190"/>
       <c r="BG4" s="190"/>
       <c r="BH4" s="190"/>
-      <c r="BI4" s="365"/>
+      <c r="BI4" s="366"/>
     </row>
     <row r="5" spans="1:61" s="186" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="193" t="s">
@@ -17017,14 +17026,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="367" t="s">
+      <c r="A1" s="368" t="s">
         <v>373</v>
       </c>
-      <c r="B1" s="367"/>
-      <c r="C1" s="367"/>
-      <c r="D1" s="367"/>
-      <c r="E1" s="367"/>
-      <c r="F1" s="367"/>
+      <c r="B1" s="368"/>
+      <c r="C1" s="368"/>
+      <c r="D1" s="368"/>
+      <c r="E1" s="368"/>
+      <c r="F1" s="368"/>
       <c r="G1" s="218"/>
       <c r="H1" s="218"/>
       <c r="I1" s="218"/>
@@ -17074,7 +17083,7 @@
       <c r="O2" s="221" t="s">
         <v>323</v>
       </c>
-      <c r="P2" s="368" t="s">
+      <c r="P2" s="369" t="s">
         <v>372</v>
       </c>
       <c r="Q2" s="221" t="s">
@@ -17086,7 +17095,7 @@
       <c r="S2" s="221" t="s">
         <v>371</v>
       </c>
-      <c r="T2" s="368" t="s">
+      <c r="T2" s="369" t="s">
         <v>370</v>
       </c>
     </row>
@@ -17124,7 +17133,7 @@
       <c r="O3" s="221" t="s">
         <v>352</v>
       </c>
-      <c r="P3" s="368"/>
+      <c r="P3" s="369"/>
       <c r="Q3" s="221" t="s">
         <v>351</v>
       </c>
@@ -17134,7 +17143,7 @@
       <c r="S3" s="221" t="s">
         <v>281</v>
       </c>
-      <c r="T3" s="368"/>
+      <c r="T3" s="369"/>
     </row>
     <row r="4" spans="1:20" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="220"/>
@@ -17180,7 +17189,7 @@
       <c r="O4" s="221" t="s">
         <v>333</v>
       </c>
-      <c r="P4" s="368"/>
+      <c r="P4" s="369"/>
       <c r="Q4" s="221" t="s">
         <v>332</v>
       </c>
@@ -17190,7 +17199,7 @@
       <c r="S4" s="221" t="s">
         <v>228</v>
       </c>
-      <c r="T4" s="368"/>
+      <c r="T4" s="369"/>
     </row>
     <row r="5" spans="1:20" ht="317" x14ac:dyDescent="0.2">
       <c r="A5" s="224" t="s">
@@ -17781,16 +17790,16 @@
   <sheetData>
     <row r="1" spans="1:28" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="244"/>
-      <c r="B1" s="370" t="s">
+      <c r="B1" s="371" t="s">
         <v>329</v>
       </c>
-      <c r="C1" s="370"/>
-      <c r="D1" s="370"/>
-      <c r="E1" s="370"/>
-      <c r="F1" s="370"/>
-      <c r="G1" s="370"/>
-      <c r="H1" s="370"/>
-      <c r="I1" s="370"/>
+      <c r="C1" s="371"/>
+      <c r="D1" s="371"/>
+      <c r="E1" s="371"/>
+      <c r="F1" s="371"/>
+      <c r="G1" s="371"/>
+      <c r="H1" s="371"/>
+      <c r="I1" s="371"/>
       <c r="J1" s="241"/>
       <c r="K1" s="241"/>
       <c r="L1" s="241"/>
@@ -17821,7 +17830,7 @@
       <c r="G2" s="243" t="s">
         <v>328</v>
       </c>
-      <c r="H2" s="369" t="s">
+      <c r="H2" s="370" t="s">
         <v>327</v>
       </c>
       <c r="I2" s="246" t="s">
@@ -17866,7 +17875,7 @@
       <c r="V2" s="246" t="s">
         <v>326</v>
       </c>
-      <c r="W2" s="369" t="s">
+      <c r="W2" s="370" t="s">
         <v>325</v>
       </c>
       <c r="X2" s="243" t="s">
@@ -17881,7 +17890,7 @@
       <c r="AA2" s="243" t="s">
         <v>144</v>
       </c>
-      <c r="AB2" s="369" t="s">
+      <c r="AB2" s="370" t="s">
         <v>324</v>
       </c>
     </row>
@@ -17895,7 +17904,7 @@
       <c r="G3" s="243" t="s">
         <v>317</v>
       </c>
-      <c r="H3" s="369"/>
+      <c r="H3" s="370"/>
       <c r="I3" s="246" t="s">
         <v>316</v>
       </c>
@@ -17936,7 +17945,7 @@
       <c r="V3" s="246" t="s">
         <v>304</v>
       </c>
-      <c r="W3" s="369"/>
+      <c r="W3" s="370"/>
       <c r="X3" s="245"/>
       <c r="Y3" s="243" t="s">
         <v>303</v>
@@ -17947,7 +17956,7 @@
       <c r="AA3" s="243" t="s">
         <v>301</v>
       </c>
-      <c r="AB3" s="369"/>
+      <c r="AB3" s="370"/>
     </row>
     <row r="4" spans="1:28" ht="98" x14ac:dyDescent="0.2">
       <c r="A4" s="247"/>
@@ -17969,7 +17978,7 @@
       <c r="G4" s="243" t="s">
         <v>267</v>
       </c>
-      <c r="H4" s="369"/>
+      <c r="H4" s="370"/>
       <c r="I4" s="246" t="s">
         <v>266</v>
       </c>
@@ -18012,7 +18021,7 @@
       <c r="V4" s="249" t="s">
         <v>253</v>
       </c>
-      <c r="W4" s="369"/>
+      <c r="W4" s="370"/>
       <c r="X4" s="250" t="s">
         <v>252</v>
       </c>
@@ -18025,7 +18034,7 @@
       <c r="AA4" s="250" t="s">
         <v>249</v>
       </c>
-      <c r="AB4" s="369"/>
+      <c r="AB4" s="370"/>
     </row>
     <row r="5" spans="1:28" ht="196" x14ac:dyDescent="0.2">
       <c r="A5" s="251" t="s">
@@ -18924,16 +18933,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="372" t="s">
+      <c r="A1" s="373" t="s">
         <v>373</v>
       </c>
-      <c r="B1" s="372"/>
-      <c r="C1" s="372"/>
-      <c r="D1" s="372"/>
-      <c r="E1" s="372"/>
-      <c r="F1" s="372"/>
-      <c r="G1" s="372"/>
-      <c r="H1" s="372"/>
+      <c r="B1" s="373"/>
+      <c r="C1" s="373"/>
+      <c r="D1" s="373"/>
+      <c r="E1" s="373"/>
+      <c r="F1" s="373"/>
+      <c r="G1" s="373"/>
+      <c r="H1" s="373"/>
       <c r="I1" s="291"/>
       <c r="J1" s="291"/>
       <c r="K1" s="291"/>
@@ -18958,7 +18967,7 @@
       <c r="G2" s="293" t="s">
         <v>328</v>
       </c>
-      <c r="H2" s="371" t="s">
+      <c r="H2" s="372" t="s">
         <v>327</v>
       </c>
       <c r="I2" s="293" t="s">
@@ -18991,13 +19000,13 @@
       <c r="R2" s="293" t="s">
         <v>326</v>
       </c>
-      <c r="S2" s="371" t="s">
+      <c r="S2" s="372" t="s">
         <v>325</v>
       </c>
       <c r="T2" s="293" t="s">
         <v>144</v>
       </c>
-      <c r="U2" s="371" t="s">
+      <c r="U2" s="372" t="s">
         <v>324</v>
       </c>
     </row>
@@ -19011,7 +19020,7 @@
       <c r="G3" s="293" t="s">
         <v>317</v>
       </c>
-      <c r="H3" s="371"/>
+      <c r="H3" s="372"/>
       <c r="I3" s="293" t="s">
         <v>369</v>
       </c>
@@ -19042,11 +19051,11 @@
       <c r="R3" s="293" t="s">
         <v>304</v>
       </c>
-      <c r="S3" s="371"/>
+      <c r="S3" s="372"/>
       <c r="T3" s="293" t="s">
         <v>301</v>
       </c>
-      <c r="U3" s="371"/>
+      <c r="U3" s="372"/>
     </row>
     <row r="4" spans="1:21" ht="112" x14ac:dyDescent="0.2">
       <c r="A4" s="290"/>
@@ -19068,7 +19077,7 @@
       <c r="G4" s="293" t="s">
         <v>267</v>
       </c>
-      <c r="H4" s="371"/>
+      <c r="H4" s="372"/>
       <c r="I4" s="293" t="s">
         <v>350</v>
       </c>
@@ -19099,11 +19108,11 @@
       <c r="R4" s="293" t="s">
         <v>253</v>
       </c>
-      <c r="S4" s="371"/>
+      <c r="S4" s="372"/>
       <c r="T4" s="293" t="s">
         <v>249</v>
       </c>
-      <c r="U4" s="371"/>
+      <c r="U4" s="372"/>
     </row>
     <row r="5" spans="1:21" ht="196" x14ac:dyDescent="0.2">
       <c r="A5" s="296" t="s">
@@ -19799,13 +19808,13 @@
       <c r="K2" s="221" t="s">
         <v>326</v>
       </c>
-      <c r="L2" s="368" t="s">
+      <c r="L2" s="369" t="s">
         <v>325</v>
       </c>
       <c r="M2" s="221" t="s">
         <v>144</v>
       </c>
-      <c r="N2" s="368" t="s">
+      <c r="N2" s="369" t="s">
         <v>324</v>
       </c>
     </row>
@@ -19823,11 +19832,11 @@
       <c r="K3" s="221" t="s">
         <v>304</v>
       </c>
-      <c r="L3" s="368"/>
+      <c r="L3" s="369"/>
       <c r="M3" s="221" t="s">
         <v>301</v>
       </c>
-      <c r="N3" s="368"/>
+      <c r="N3" s="369"/>
     </row>
     <row r="4" spans="1:14" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="274"/>
@@ -19853,11 +19862,11 @@
       <c r="K4" s="221" t="s">
         <v>253</v>
       </c>
-      <c r="L4" s="368"/>
+      <c r="L4" s="369"/>
       <c r="M4" s="221" t="s">
         <v>249</v>
       </c>
-      <c r="N4" s="368"/>
+      <c r="N4" s="369"/>
     </row>
     <row r="5" spans="1:14" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="276"/>
@@ -20512,10 +20521,10 @@
   <sheetPr codeName="Feuil13">
     <tabColor rgb="FF2C45E0"/>
   </sheetPr>
-  <dimension ref="A1:FG4"/>
+  <dimension ref="A1:FJ4"/>
   <sheetViews>
-    <sheetView showFormulas="1" topLeftCell="EX1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="EZ1" sqref="EZ1"/>
+    <sheetView showFormulas="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A164" sqref="A164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20534,7 +20543,7 @@
     <col min="170" max="170" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:163" s="4" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:166" s="4" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>377</v>
       </c>
@@ -20554,11 +20563,13 @@
       <c r="FD1" s="355"/>
       <c r="FE1" s="355"/>
       <c r="FF1" s="355"/>
-      <c r="FG1" s="8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:163" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="FG1" s="356"/>
+      <c r="FH1" s="356"/>
+      <c r="FJ1" s="26" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:166" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
         <v>8</v>
       </c>
@@ -20583,8 +20594,15 @@
       <c r="FF2" s="142" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="1:163" x14ac:dyDescent="0.2">
+      <c r="FG2" s="142" t="s">
+        <v>580</v>
+      </c>
+      <c r="FH2" s="142" t="s">
+        <v>581</v>
+      </c>
+      <c r="FJ2" s="26"/>
+    </row>
+    <row r="3" spans="1:166" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
         <v>11</v>
       </c>
@@ -20592,7 +20610,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:163" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:166" x14ac:dyDescent="0.2">
       <c r="B4" s="27" t="s">
         <v>7</v>
       </c>
@@ -20601,7 +20619,7 @@
   </sheetData>
   <autoFilter ref="A2:DT2" xr:uid="{3B89445B-6ECC-4440-B85C-E593AE209933}"/>
   <mergeCells count="1">
-    <mergeCell ref="FA1:FF1"/>
+    <mergeCell ref="FA1:FH1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -20696,28 +20714,28 @@
       <c r="D4" s="312"/>
       <c r="E4" s="312"/>
       <c r="F4" s="312"/>
-      <c r="G4" s="356" t="s">
+      <c r="G4" s="357" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="357"/>
-      <c r="I4" s="357"/>
-      <c r="J4" s="357"/>
-      <c r="K4" s="357"/>
-      <c r="L4" s="358"/>
-      <c r="M4" s="359"/>
-      <c r="N4" s="360" t="s">
+      <c r="H4" s="358"/>
+      <c r="I4" s="358"/>
+      <c r="J4" s="358"/>
+      <c r="K4" s="358"/>
+      <c r="L4" s="359"/>
+      <c r="M4" s="360"/>
+      <c r="N4" s="361" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="358"/>
-      <c r="P4" s="358"/>
-      <c r="Q4" s="358"/>
-      <c r="R4" s="358"/>
-      <c r="S4" s="358"/>
-      <c r="T4" s="361"/>
-      <c r="U4" s="356" t="s">
+      <c r="O4" s="359"/>
+      <c r="P4" s="359"/>
+      <c r="Q4" s="359"/>
+      <c r="R4" s="359"/>
+      <c r="S4" s="359"/>
+      <c r="T4" s="362"/>
+      <c r="U4" s="357" t="s">
         <v>28</v>
       </c>
-      <c r="V4" s="359"/>
+      <c r="V4" s="360"/>
       <c r="W4" s="319"/>
       <c r="X4" t="s">
         <v>0</v>
@@ -22452,16 +22470,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" s="60" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B1" s="363" t="s">
+      <c r="B1" s="364" t="s">
         <v>329</v>
       </c>
-      <c r="C1" s="363"/>
-      <c r="D1" s="363"/>
-      <c r="E1" s="363"/>
-      <c r="F1" s="363"/>
-      <c r="G1" s="363"/>
-      <c r="H1" s="363"/>
-      <c r="I1" s="363"/>
+      <c r="C1" s="364"/>
+      <c r="D1" s="364"/>
+      <c r="E1" s="364"/>
+      <c r="F1" s="364"/>
+      <c r="G1" s="364"/>
+      <c r="H1" s="364"/>
+      <c r="I1" s="364"/>
     </row>
     <row r="2" spans="1:62" s="60" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="106"/>
@@ -22473,7 +22491,7 @@
       <c r="G2" s="103" t="s">
         <v>328</v>
       </c>
-      <c r="H2" s="362" t="s">
+      <c r="H2" s="363" t="s">
         <v>327</v>
       </c>
       <c r="I2" s="102" t="s">
@@ -22518,7 +22536,7 @@
       <c r="V2" s="102" t="s">
         <v>326</v>
       </c>
-      <c r="W2" s="362" t="s">
+      <c r="W2" s="363" t="s">
         <v>325</v>
       </c>
       <c r="X2" s="103" t="s">
@@ -22533,7 +22551,7 @@
       <c r="AA2" s="103" t="s">
         <v>144</v>
       </c>
-      <c r="AB2" s="362" t="s">
+      <c r="AB2" s="363" t="s">
         <v>324</v>
       </c>
       <c r="AC2" s="100" t="s">
@@ -22563,7 +22581,7 @@
       <c r="AK2" s="100" t="s">
         <v>323</v>
       </c>
-      <c r="AL2" s="362" t="s">
+      <c r="AL2" s="363" t="s">
         <v>322</v>
       </c>
       <c r="AM2" s="100" t="s">
@@ -22605,7 +22623,7 @@
       <c r="AY2" s="100" t="s">
         <v>321</v>
       </c>
-      <c r="AZ2" s="362" t="s">
+      <c r="AZ2" s="363" t="s">
         <v>320</v>
       </c>
       <c r="BA2" s="99" t="s">
@@ -22635,7 +22653,7 @@
       <c r="BI2" s="99" t="s">
         <v>319</v>
       </c>
-      <c r="BJ2" s="362" t="s">
+      <c r="BJ2" s="363" t="s">
         <v>318</v>
       </c>
     </row>
@@ -22649,7 +22667,7 @@
       <c r="G3" s="103" t="s">
         <v>317</v>
       </c>
-      <c r="H3" s="362"/>
+      <c r="H3" s="363"/>
       <c r="I3" s="102" t="s">
         <v>316</v>
       </c>
@@ -22690,7 +22708,7 @@
       <c r="V3" s="102" t="s">
         <v>304</v>
       </c>
-      <c r="W3" s="362"/>
+      <c r="W3" s="363"/>
       <c r="X3" s="98"/>
       <c r="Y3" s="103" t="s">
         <v>303</v>
@@ -22701,7 +22719,7 @@
       <c r="AA3" s="103" t="s">
         <v>301</v>
       </c>
-      <c r="AB3" s="362"/>
+      <c r="AB3" s="363"/>
       <c r="AC3" s="100" t="s">
         <v>300</v>
       </c>
@@ -22729,7 +22747,7 @@
       <c r="AK3" s="100" t="s">
         <v>294</v>
       </c>
-      <c r="AL3" s="362"/>
+      <c r="AL3" s="363"/>
       <c r="AM3" s="100" t="s">
         <v>293</v>
       </c>
@@ -22769,7 +22787,7 @@
       <c r="AY3" s="100" t="s">
         <v>281</v>
       </c>
-      <c r="AZ3" s="362"/>
+      <c r="AZ3" s="363"/>
       <c r="BA3" s="99" t="s">
         <v>280</v>
       </c>
@@ -22797,7 +22815,7 @@
       <c r="BI3" s="99" t="s">
         <v>272</v>
       </c>
-      <c r="BJ3" s="362"/>
+      <c r="BJ3" s="363"/>
     </row>
     <row r="4" spans="1:62" s="60" customFormat="1" ht="60" x14ac:dyDescent="0.15">
       <c r="A4" s="105"/>
@@ -22819,7 +22837,7 @@
       <c r="G4" s="103" t="s">
         <v>267</v>
       </c>
-      <c r="H4" s="362"/>
+      <c r="H4" s="363"/>
       <c r="I4" s="102" t="s">
         <v>266</v>
       </c>
@@ -22862,7 +22880,7 @@
       <c r="V4" s="102" t="s">
         <v>253</v>
       </c>
-      <c r="W4" s="362"/>
+      <c r="W4" s="363"/>
       <c r="X4" s="101" t="s">
         <v>252</v>
       </c>
@@ -22875,7 +22893,7 @@
       <c r="AA4" s="101" t="s">
         <v>249</v>
       </c>
-      <c r="AB4" s="362"/>
+      <c r="AB4" s="363"/>
       <c r="AC4" s="100" t="s">
         <v>248</v>
       </c>
@@ -22903,7 +22921,7 @@
       <c r="AK4" s="100" t="s">
         <v>241</v>
       </c>
-      <c r="AL4" s="362"/>
+      <c r="AL4" s="363"/>
       <c r="AM4" s="100" t="s">
         <v>240</v>
       </c>
@@ -22943,7 +22961,7 @@
       <c r="AY4" s="100" t="s">
         <v>228</v>
       </c>
-      <c r="AZ4" s="362"/>
+      <c r="AZ4" s="363"/>
       <c r="BA4" s="99" t="s">
         <v>227</v>
       </c>
@@ -22971,7 +22989,7 @@
       <c r="BI4" s="99" t="s">
         <v>219</v>
       </c>
-      <c r="BJ4" s="362"/>
+      <c r="BJ4" s="363"/>
     </row>
     <row r="5" spans="1:62" s="60" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="70" t="s">
@@ -25168,16 +25186,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A1" s="364" t="s">
+      <c r="A1" s="365" t="s">
         <v>373</v>
       </c>
-      <c r="B1" s="364"/>
-      <c r="C1" s="364"/>
-      <c r="D1" s="364"/>
-      <c r="E1" s="364"/>
-      <c r="F1" s="364"/>
-      <c r="G1" s="364"/>
-      <c r="H1" s="364"/>
+      <c r="B1" s="365"/>
+      <c r="C1" s="365"/>
+      <c r="D1" s="365"/>
+      <c r="E1" s="365"/>
+      <c r="F1" s="365"/>
+      <c r="G1" s="365"/>
+      <c r="H1" s="365"/>
       <c r="I1" s="60"/>
       <c r="J1" s="60"/>
       <c r="K1" s="60"/>
@@ -25216,7 +25234,7 @@
       <c r="G2" s="103" t="s">
         <v>328</v>
       </c>
-      <c r="H2" s="362" t="s">
+      <c r="H2" s="363" t="s">
         <v>327</v>
       </c>
       <c r="I2" s="103" t="s">
@@ -25249,13 +25267,13 @@
       <c r="R2" s="103" t="s">
         <v>326</v>
       </c>
-      <c r="S2" s="362" t="s">
+      <c r="S2" s="363" t="s">
         <v>325</v>
       </c>
       <c r="T2" s="103" t="s">
         <v>144</v>
       </c>
-      <c r="U2" s="362" t="s">
+      <c r="U2" s="363" t="s">
         <v>324</v>
       </c>
       <c r="V2" s="103" t="s">
@@ -25285,7 +25303,7 @@
       <c r="AD2" s="103" t="s">
         <v>323</v>
       </c>
-      <c r="AE2" s="362" t="s">
+      <c r="AE2" s="363" t="s">
         <v>372</v>
       </c>
       <c r="AF2" s="103" t="s">
@@ -25297,7 +25315,7 @@
       <c r="AH2" s="103" t="s">
         <v>371</v>
       </c>
-      <c r="AI2" s="362" t="s">
+      <c r="AI2" s="363" t="s">
         <v>370</v>
       </c>
     </row>
@@ -25311,7 +25329,7 @@
       <c r="G3" s="103" t="s">
         <v>317</v>
       </c>
-      <c r="H3" s="362"/>
+      <c r="H3" s="363"/>
       <c r="I3" s="103" t="s">
         <v>369</v>
       </c>
@@ -25342,11 +25360,11 @@
       <c r="R3" s="103" t="s">
         <v>304</v>
       </c>
-      <c r="S3" s="362"/>
+      <c r="S3" s="363"/>
       <c r="T3" s="103" t="s">
         <v>301</v>
       </c>
-      <c r="U3" s="362"/>
+      <c r="U3" s="363"/>
       <c r="V3" s="103" t="s">
         <v>360</v>
       </c>
@@ -25374,7 +25392,7 @@
       <c r="AD3" s="103" t="s">
         <v>352</v>
       </c>
-      <c r="AE3" s="362"/>
+      <c r="AE3" s="363"/>
       <c r="AF3" s="103" t="s">
         <v>351</v>
       </c>
@@ -25384,7 +25402,7 @@
       <c r="AH3" s="103" t="s">
         <v>281</v>
       </c>
-      <c r="AI3" s="362"/>
+      <c r="AI3" s="363"/>
     </row>
     <row r="4" spans="1:35" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="106"/>
@@ -25406,7 +25424,7 @@
       <c r="G4" s="103" t="s">
         <v>267</v>
       </c>
-      <c r="H4" s="362"/>
+      <c r="H4" s="363"/>
       <c r="I4" s="103" t="s">
         <v>350</v>
       </c>
@@ -25437,11 +25455,11 @@
       <c r="R4" s="103" t="s">
         <v>253</v>
       </c>
-      <c r="S4" s="362"/>
+      <c r="S4" s="363"/>
       <c r="T4" s="103" t="s">
         <v>249</v>
       </c>
-      <c r="U4" s="362"/>
+      <c r="U4" s="363"/>
       <c r="V4" s="103" t="s">
         <v>341</v>
       </c>
@@ -25469,7 +25487,7 @@
       <c r="AD4" s="103" t="s">
         <v>333</v>
       </c>
-      <c r="AE4" s="362"/>
+      <c r="AE4" s="363"/>
       <c r="AF4" s="103" t="s">
         <v>332</v>
       </c>
@@ -25479,7 +25497,7 @@
       <c r="AH4" s="103" t="s">
         <v>228</v>
       </c>
-      <c r="AI4" s="362"/>
+      <c r="AI4" s="363"/>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A5" s="109" t="s">

</xml_diff>

<commit_message>
update extractor JE JI
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F5B946-2296-0149-9C85-A03EEC4EF1D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD0B010-AF30-8243-8434-832785C3597D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1588" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1590" uniqueCount="437">
   <si>
     <t>#! END_ROW</t>
   </si>
@@ -4774,6 +4774,12 @@
   </si>
   <si>
     <t>## f.category_label</t>
+  </si>
+  <si>
+    <t>Ecart JE</t>
+  </si>
+  <si>
+    <t>Ecart JI</t>
   </si>
 </sst>
 </file>
@@ -5952,7 +5958,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="356">
+  <cellXfs count="357">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -7140,6 +7146,9 @@
     <xf numFmtId="0" fontId="53" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -20009,10 +20018,10 @@
   <sheetPr codeName="Feuil13">
     <tabColor rgb="FF2C45E0"/>
   </sheetPr>
-  <dimension ref="A1:FG4"/>
+  <dimension ref="A1:FI4"/>
   <sheetViews>
-    <sheetView showFormulas="1" topLeftCell="EX1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="EZ1" sqref="EZ1"/>
+    <sheetView showFormulas="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="FH3" sqref="FH3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20031,7 +20040,7 @@
     <col min="170" max="170" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:163" s="4" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:165" s="4" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>232</v>
       </c>
@@ -20051,11 +20060,13 @@
       <c r="FD1" s="338"/>
       <c r="FE1" s="338"/>
       <c r="FF1" s="338"/>
-      <c r="FG1" s="8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:163" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="FG1" s="356"/>
+      <c r="FH1" s="356"/>
+      <c r="FI1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:165" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
         <v>8</v>
       </c>
@@ -20080,8 +20091,14 @@
       <c r="FF2" s="126" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="1:163" x14ac:dyDescent="0.2">
+      <c r="FG2" s="126" t="s">
+        <v>435</v>
+      </c>
+      <c r="FH2" s="126" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="3" spans="1:165" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
         <v>11</v>
       </c>
@@ -20089,7 +20106,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:163" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:165" x14ac:dyDescent="0.2">
       <c r="B4" s="27" t="s">
         <v>7</v>
       </c>
@@ -20098,7 +20115,7 @@
   </sheetData>
   <autoFilter ref="A2:DT2" xr:uid="{3B89445B-6ECC-4440-B85C-E593AE209933}"/>
   <mergeCells count="1">
-    <mergeCell ref="FA1:FF1"/>
+    <mergeCell ref="FA1:FH1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -20114,7 +20131,7 @@
   <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fix fct extractor round JE JI and fix agregat
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD0B010-AF30-8243-8434-832785C3597D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93949BE-F58E-7C44-BDD7-AD9F259563F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1590" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="438">
   <si>
     <t>#! END_ROW</t>
   </si>
@@ -4780,6 +4780,9 @@
   </si>
   <si>
     <t>Ecart JI</t>
+  </si>
+  <si>
+    <t>Fonction agrégat</t>
   </si>
 </sst>
 </file>
@@ -7089,6 +7092,9 @@
     <xf numFmtId="0" fontId="37" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -7146,9 +7152,6 @@
     <xf numFmtId="0" fontId="53" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -8228,13 +8231,13 @@
       <c r="G2" s="87" t="s">
         <v>181</v>
       </c>
-      <c r="H2" s="345" t="s">
+      <c r="H2" s="346" t="s">
         <v>180</v>
       </c>
       <c r="I2" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="J2" s="345" t="s">
+      <c r="J2" s="346" t="s">
         <v>179</v>
       </c>
     </row>
@@ -8248,11 +8251,11 @@
       <c r="G3" s="87" t="s">
         <v>159</v>
       </c>
-      <c r="H3" s="345"/>
+      <c r="H3" s="346"/>
       <c r="I3" s="87" t="s">
         <v>156</v>
       </c>
-      <c r="J3" s="345"/>
+      <c r="J3" s="346"/>
     </row>
     <row r="4" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A4" s="109"/>
@@ -8274,11 +8277,11 @@
       <c r="G4" s="87" t="s">
         <v>108</v>
       </c>
-      <c r="H4" s="345"/>
+      <c r="H4" s="346"/>
       <c r="I4" s="87" t="s">
         <v>104</v>
       </c>
-      <c r="J4" s="345"/>
+      <c r="J4" s="346"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="103" t="s">
@@ -8682,7 +8685,7 @@
       <c r="G2" s="87" t="s">
         <v>183</v>
       </c>
-      <c r="H2" s="345" t="s">
+      <c r="H2" s="346" t="s">
         <v>182</v>
       </c>
       <c r="I2" s="86" t="s">
@@ -8727,7 +8730,7 @@
       <c r="V2" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="W2" s="345" t="s">
+      <c r="W2" s="346" t="s">
         <v>180</v>
       </c>
       <c r="X2" s="87" t="s">
@@ -8742,7 +8745,7 @@
       <c r="AA2" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="AB2" s="345" t="s">
+      <c r="AB2" s="346" t="s">
         <v>179</v>
       </c>
       <c r="AC2" s="84" t="s">
@@ -8772,7 +8775,7 @@
       <c r="AK2" s="84" t="s">
         <v>178</v>
       </c>
-      <c r="AL2" s="345" t="s">
+      <c r="AL2" s="346" t="s">
         <v>177</v>
       </c>
       <c r="AM2" s="84" t="s">
@@ -8814,7 +8817,7 @@
       <c r="AY2" s="84" t="s">
         <v>176</v>
       </c>
-      <c r="AZ2" s="345" t="s">
+      <c r="AZ2" s="346" t="s">
         <v>175</v>
       </c>
       <c r="BA2" s="83" t="s">
@@ -8844,7 +8847,7 @@
       <c r="BI2" s="83" t="s">
         <v>174</v>
       </c>
-      <c r="BJ2" s="345" t="s">
+      <c r="BJ2" s="346" t="s">
         <v>173</v>
       </c>
       <c r="BK2"/>
@@ -8859,7 +8862,7 @@
       <c r="G3" s="87" t="s">
         <v>172</v>
       </c>
-      <c r="H3" s="345"/>
+      <c r="H3" s="346"/>
       <c r="I3" s="86" t="s">
         <v>171</v>
       </c>
@@ -8900,7 +8903,7 @@
       <c r="V3" s="86" t="s">
         <v>159</v>
       </c>
-      <c r="W3" s="345"/>
+      <c r="W3" s="346"/>
       <c r="X3" s="82"/>
       <c r="Y3" s="87" t="s">
         <v>158</v>
@@ -8911,7 +8914,7 @@
       <c r="AA3" s="87" t="s">
         <v>156</v>
       </c>
-      <c r="AB3" s="345"/>
+      <c r="AB3" s="346"/>
       <c r="AC3" s="84" t="s">
         <v>155</v>
       </c>
@@ -8939,7 +8942,7 @@
       <c r="AK3" s="84" t="s">
         <v>149</v>
       </c>
-      <c r="AL3" s="345"/>
+      <c r="AL3" s="346"/>
       <c r="AM3" s="84" t="s">
         <v>148</v>
       </c>
@@ -8979,7 +8982,7 @@
       <c r="AY3" s="84" t="s">
         <v>136</v>
       </c>
-      <c r="AZ3" s="345"/>
+      <c r="AZ3" s="346"/>
       <c r="BA3" s="83" t="s">
         <v>135</v>
       </c>
@@ -9007,7 +9010,7 @@
       <c r="BI3" s="83" t="s">
         <v>127</v>
       </c>
-      <c r="BJ3" s="345"/>
+      <c r="BJ3" s="346"/>
     </row>
     <row r="4" spans="1:63" s="44" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="89"/>
@@ -9029,7 +9032,7 @@
       <c r="G4" s="87" t="s">
         <v>122</v>
       </c>
-      <c r="H4" s="345"/>
+      <c r="H4" s="346"/>
       <c r="I4" s="86" t="s">
         <v>121</v>
       </c>
@@ -9072,7 +9075,7 @@
       <c r="V4" s="86" t="s">
         <v>108</v>
       </c>
-      <c r="W4" s="345"/>
+      <c r="W4" s="346"/>
       <c r="X4" s="85" t="s">
         <v>107</v>
       </c>
@@ -9085,7 +9088,7 @@
       <c r="AA4" s="85" t="s">
         <v>104</v>
       </c>
-      <c r="AB4" s="345"/>
+      <c r="AB4" s="346"/>
       <c r="AC4" s="84" t="s">
         <v>103</v>
       </c>
@@ -9113,7 +9116,7 @@
       <c r="AK4" s="84" t="s">
         <v>96</v>
       </c>
-      <c r="AL4" s="345"/>
+      <c r="AL4" s="346"/>
       <c r="AM4" s="84" t="s">
         <v>95</v>
       </c>
@@ -9153,7 +9156,7 @@
       <c r="AY4" s="84" t="s">
         <v>83</v>
       </c>
-      <c r="AZ4" s="345"/>
+      <c r="AZ4" s="346"/>
       <c r="BA4" s="83" t="s">
         <v>82</v>
       </c>
@@ -9181,7 +9184,7 @@
       <c r="BI4" s="83" t="s">
         <v>74</v>
       </c>
-      <c r="BJ4" s="345"/>
+      <c r="BJ4" s="346"/>
       <c r="BK4"/>
     </row>
     <row r="5" spans="1:63" s="44" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -11931,7 +11934,7 @@
       <c r="G2" s="87" t="s">
         <v>183</v>
       </c>
-      <c r="H2" s="345" t="s">
+      <c r="H2" s="346" t="s">
         <v>182</v>
       </c>
       <c r="I2" s="87" t="s">
@@ -11964,13 +11967,13 @@
       <c r="R2" s="87" t="s">
         <v>181</v>
       </c>
-      <c r="S2" s="345" t="s">
+      <c r="S2" s="346" t="s">
         <v>180</v>
       </c>
       <c r="T2" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="U2" s="345" t="s">
+      <c r="U2" s="346" t="s">
         <v>179</v>
       </c>
       <c r="V2" s="87" t="s">
@@ -12000,7 +12003,7 @@
       <c r="AD2" s="87" t="s">
         <v>178</v>
       </c>
-      <c r="AE2" s="345" t="s">
+      <c r="AE2" s="346" t="s">
         <v>227</v>
       </c>
       <c r="AF2" s="87" t="s">
@@ -12012,7 +12015,7 @@
       <c r="AH2" s="87" t="s">
         <v>226</v>
       </c>
-      <c r="AI2" s="345" t="s">
+      <c r="AI2" s="346" t="s">
         <v>225</v>
       </c>
     </row>
@@ -12026,7 +12029,7 @@
       <c r="G3" s="87" t="s">
         <v>172</v>
       </c>
-      <c r="H3" s="345"/>
+      <c r="H3" s="346"/>
       <c r="I3" s="87" t="s">
         <v>224</v>
       </c>
@@ -12057,11 +12060,11 @@
       <c r="R3" s="87" t="s">
         <v>159</v>
       </c>
-      <c r="S3" s="345"/>
+      <c r="S3" s="346"/>
       <c r="T3" s="87" t="s">
         <v>156</v>
       </c>
-      <c r="U3" s="345"/>
+      <c r="U3" s="346"/>
       <c r="V3" s="87" t="s">
         <v>215</v>
       </c>
@@ -12089,7 +12092,7 @@
       <c r="AD3" s="87" t="s">
         <v>207</v>
       </c>
-      <c r="AE3" s="345"/>
+      <c r="AE3" s="346"/>
       <c r="AF3" s="87" t="s">
         <v>206</v>
       </c>
@@ -12099,7 +12102,7 @@
       <c r="AH3" s="87" t="s">
         <v>136</v>
       </c>
-      <c r="AI3" s="345"/>
+      <c r="AI3" s="346"/>
     </row>
     <row r="4" spans="1:62" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="90"/>
@@ -12121,7 +12124,7 @@
       <c r="G4" s="87" t="s">
         <v>122</v>
       </c>
-      <c r="H4" s="345"/>
+      <c r="H4" s="346"/>
       <c r="I4" s="87" t="s">
         <v>205</v>
       </c>
@@ -12152,11 +12155,11 @@
       <c r="R4" s="87" t="s">
         <v>108</v>
       </c>
-      <c r="S4" s="345"/>
+      <c r="S4" s="346"/>
       <c r="T4" s="87" t="s">
         <v>104</v>
       </c>
-      <c r="U4" s="345"/>
+      <c r="U4" s="346"/>
       <c r="V4" s="87" t="s">
         <v>196</v>
       </c>
@@ -12184,7 +12187,7 @@
       <c r="AD4" s="87" t="s">
         <v>188</v>
       </c>
-      <c r="AE4" s="345"/>
+      <c r="AE4" s="346"/>
       <c r="AF4" s="87" t="s">
         <v>187</v>
       </c>
@@ -12194,7 +12197,7 @@
       <c r="AH4" s="87" t="s">
         <v>83</v>
       </c>
-      <c r="AI4" s="345"/>
+      <c r="AI4" s="346"/>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A5" s="93" t="s">
@@ -13951,13 +13954,13 @@
       <c r="G2" s="87" t="s">
         <v>181</v>
       </c>
-      <c r="H2" s="345" t="s">
+      <c r="H2" s="346" t="s">
         <v>180</v>
       </c>
       <c r="I2" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="J2" s="345" t="s">
+      <c r="J2" s="346" t="s">
         <v>179</v>
       </c>
     </row>
@@ -13971,11 +13974,11 @@
       <c r="G3" s="87" t="s">
         <v>159</v>
       </c>
-      <c r="H3" s="345"/>
+      <c r="H3" s="346"/>
       <c r="I3" s="87" t="s">
         <v>156</v>
       </c>
-      <c r="J3" s="345"/>
+      <c r="J3" s="346"/>
     </row>
     <row r="4" spans="1:62" ht="36" x14ac:dyDescent="0.2">
       <c r="A4" s="109"/>
@@ -13997,11 +14000,11 @@
       <c r="G4" s="87" t="s">
         <v>108</v>
       </c>
-      <c r="H4" s="345"/>
+      <c r="H4" s="346"/>
       <c r="I4" s="87" t="s">
         <v>104</v>
       </c>
-      <c r="J4" s="345"/>
+      <c r="J4" s="346"/>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A5" s="103" t="s">
@@ -14396,13 +14399,13 @@
   <sheetData>
     <row r="1" spans="1:61" s="168" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="167"/>
-      <c r="B1" s="349" t="s">
+      <c r="B1" s="350" t="s">
         <v>184</v>
       </c>
-      <c r="C1" s="349"/>
-      <c r="D1" s="349"/>
-      <c r="E1" s="349"/>
-      <c r="F1" s="349"/>
+      <c r="C1" s="350"/>
+      <c r="D1" s="350"/>
+      <c r="E1" s="350"/>
+      <c r="F1" s="350"/>
       <c r="G1" s="169"/>
       <c r="H1" s="169"/>
       <c r="I1" s="169"/>
@@ -14447,7 +14450,7 @@
       <c r="O2" s="171" t="s">
         <v>178</v>
       </c>
-      <c r="P2" s="348" t="s">
+      <c r="P2" s="349" t="s">
         <v>177</v>
       </c>
       <c r="Q2" s="171" t="s">
@@ -14489,7 +14492,7 @@
       <c r="AC2" s="171" t="s">
         <v>176</v>
       </c>
-      <c r="AD2" s="348" t="s">
+      <c r="AD2" s="349" t="s">
         <v>175</v>
       </c>
       <c r="AE2" s="172" t="s">
@@ -14519,7 +14522,7 @@
       <c r="AM2" s="172" t="s">
         <v>174</v>
       </c>
-      <c r="AN2" s="348" t="s">
+      <c r="AN2" s="349" t="s">
         <v>173</v>
       </c>
       <c r="AQ2" s="171"/>
@@ -14530,7 +14533,7 @@
       <c r="AV2" s="171"/>
       <c r="AW2" s="171"/>
       <c r="AX2" s="171"/>
-      <c r="AY2" s="348"/>
+      <c r="AY2" s="349"/>
       <c r="AZ2" s="172"/>
       <c r="BA2" s="172"/>
       <c r="BB2" s="172"/>
@@ -14540,7 +14543,7 @@
       <c r="BF2" s="172"/>
       <c r="BG2" s="172"/>
       <c r="BH2" s="172"/>
-      <c r="BI2" s="348"/>
+      <c r="BI2" s="349"/>
     </row>
     <row r="3" spans="1:61" s="168" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="170"/>
@@ -14576,7 +14579,7 @@
       <c r="O3" s="171" t="s">
         <v>149</v>
       </c>
-      <c r="P3" s="348"/>
+      <c r="P3" s="349"/>
       <c r="Q3" s="171" t="s">
         <v>148</v>
       </c>
@@ -14616,7 +14619,7 @@
       <c r="AC3" s="171" t="s">
         <v>136</v>
       </c>
-      <c r="AD3" s="348"/>
+      <c r="AD3" s="349"/>
       <c r="AE3" s="172" t="s">
         <v>135</v>
       </c>
@@ -14644,7 +14647,7 @@
       <c r="AM3" s="172" t="s">
         <v>127</v>
       </c>
-      <c r="AN3" s="348"/>
+      <c r="AN3" s="349"/>
       <c r="AQ3" s="171"/>
       <c r="AR3" s="171"/>
       <c r="AS3" s="171"/>
@@ -14653,7 +14656,7 @@
       <c r="AV3" s="171"/>
       <c r="AW3" s="171"/>
       <c r="AX3" s="171"/>
-      <c r="AY3" s="348"/>
+      <c r="AY3" s="349"/>
       <c r="AZ3" s="172"/>
       <c r="BA3" s="172"/>
       <c r="BB3" s="172"/>
@@ -14663,7 +14666,7 @@
       <c r="BF3" s="172"/>
       <c r="BG3" s="172"/>
       <c r="BH3" s="172"/>
-      <c r="BI3" s="348"/>
+      <c r="BI3" s="349"/>
     </row>
     <row r="4" spans="1:61" s="168" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="173"/>
@@ -14709,7 +14712,7 @@
       <c r="O4" s="171" t="s">
         <v>96</v>
       </c>
-      <c r="P4" s="348"/>
+      <c r="P4" s="349"/>
       <c r="Q4" s="171" t="s">
         <v>95</v>
       </c>
@@ -14749,7 +14752,7 @@
       <c r="AC4" s="171" t="s">
         <v>83</v>
       </c>
-      <c r="AD4" s="348"/>
+      <c r="AD4" s="349"/>
       <c r="AE4" s="172" t="s">
         <v>82</v>
       </c>
@@ -14777,7 +14780,7 @@
       <c r="AM4" s="172" t="s">
         <v>74</v>
       </c>
-      <c r="AN4" s="348"/>
+      <c r="AN4" s="349"/>
       <c r="AQ4" s="171"/>
       <c r="AR4" s="171"/>
       <c r="AS4" s="171"/>
@@ -14786,7 +14789,7 @@
       <c r="AV4" s="171"/>
       <c r="AW4" s="171"/>
       <c r="AX4" s="171"/>
-      <c r="AY4" s="348"/>
+      <c r="AY4" s="349"/>
       <c r="AZ4" s="172"/>
       <c r="BA4" s="172"/>
       <c r="BB4" s="172"/>
@@ -14796,7 +14799,7 @@
       <c r="BF4" s="172"/>
       <c r="BG4" s="172"/>
       <c r="BH4" s="172"/>
-      <c r="BI4" s="348"/>
+      <c r="BI4" s="349"/>
     </row>
     <row r="5" spans="1:61" s="168" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="175" t="s">
@@ -16523,14 +16526,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="350" t="s">
+      <c r="A1" s="351" t="s">
         <v>228</v>
       </c>
-      <c r="B1" s="350"/>
-      <c r="C1" s="350"/>
-      <c r="D1" s="350"/>
-      <c r="E1" s="350"/>
-      <c r="F1" s="350"/>
+      <c r="B1" s="351"/>
+      <c r="C1" s="351"/>
+      <c r="D1" s="351"/>
+      <c r="E1" s="351"/>
+      <c r="F1" s="351"/>
       <c r="G1" s="200"/>
       <c r="H1" s="200"/>
       <c r="I1" s="200"/>
@@ -16580,7 +16583,7 @@
       <c r="O2" s="203" t="s">
         <v>178</v>
       </c>
-      <c r="P2" s="351" t="s">
+      <c r="P2" s="352" t="s">
         <v>227</v>
       </c>
       <c r="Q2" s="203" t="s">
@@ -16592,7 +16595,7 @@
       <c r="S2" s="203" t="s">
         <v>226</v>
       </c>
-      <c r="T2" s="351" t="s">
+      <c r="T2" s="352" t="s">
         <v>225</v>
       </c>
     </row>
@@ -16630,7 +16633,7 @@
       <c r="O3" s="203" t="s">
         <v>207</v>
       </c>
-      <c r="P3" s="351"/>
+      <c r="P3" s="352"/>
       <c r="Q3" s="203" t="s">
         <v>206</v>
       </c>
@@ -16640,7 +16643,7 @@
       <c r="S3" s="203" t="s">
         <v>136</v>
       </c>
-      <c r="T3" s="351"/>
+      <c r="T3" s="352"/>
     </row>
     <row r="4" spans="1:20" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="202"/>
@@ -16686,7 +16689,7 @@
       <c r="O4" s="203" t="s">
         <v>188</v>
       </c>
-      <c r="P4" s="351"/>
+      <c r="P4" s="352"/>
       <c r="Q4" s="203" t="s">
         <v>187</v>
       </c>
@@ -16696,7 +16699,7 @@
       <c r="S4" s="203" t="s">
         <v>83</v>
       </c>
-      <c r="T4" s="351"/>
+      <c r="T4" s="352"/>
     </row>
     <row r="5" spans="1:20" ht="317" x14ac:dyDescent="0.2">
       <c r="A5" s="206" t="s">
@@ -17287,16 +17290,16 @@
   <sheetData>
     <row r="1" spans="1:28" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="226"/>
-      <c r="B1" s="353" t="s">
+      <c r="B1" s="354" t="s">
         <v>184</v>
       </c>
-      <c r="C1" s="353"/>
-      <c r="D1" s="353"/>
-      <c r="E1" s="353"/>
-      <c r="F1" s="353"/>
-      <c r="G1" s="353"/>
-      <c r="H1" s="353"/>
-      <c r="I1" s="353"/>
+      <c r="C1" s="354"/>
+      <c r="D1" s="354"/>
+      <c r="E1" s="354"/>
+      <c r="F1" s="354"/>
+      <c r="G1" s="354"/>
+      <c r="H1" s="354"/>
+      <c r="I1" s="354"/>
       <c r="J1" s="223"/>
       <c r="K1" s="223"/>
       <c r="L1" s="223"/>
@@ -17327,7 +17330,7 @@
       <c r="G2" s="225" t="s">
         <v>183</v>
       </c>
-      <c r="H2" s="352" t="s">
+      <c r="H2" s="353" t="s">
         <v>182</v>
       </c>
       <c r="I2" s="228" t="s">
@@ -17372,7 +17375,7 @@
       <c r="V2" s="228" t="s">
         <v>181</v>
       </c>
-      <c r="W2" s="352" t="s">
+      <c r="W2" s="353" t="s">
         <v>180</v>
       </c>
       <c r="X2" s="225" t="s">
@@ -17387,7 +17390,7 @@
       <c r="AA2" s="225" t="s">
         <v>45</v>
       </c>
-      <c r="AB2" s="352" t="s">
+      <c r="AB2" s="353" t="s">
         <v>179</v>
       </c>
     </row>
@@ -17401,7 +17404,7 @@
       <c r="G3" s="225" t="s">
         <v>172</v>
       </c>
-      <c r="H3" s="352"/>
+      <c r="H3" s="353"/>
       <c r="I3" s="228" t="s">
         <v>171</v>
       </c>
@@ -17442,7 +17445,7 @@
       <c r="V3" s="228" t="s">
         <v>159</v>
       </c>
-      <c r="W3" s="352"/>
+      <c r="W3" s="353"/>
       <c r="X3" s="227"/>
       <c r="Y3" s="225" t="s">
         <v>158</v>
@@ -17453,7 +17456,7 @@
       <c r="AA3" s="225" t="s">
         <v>156</v>
       </c>
-      <c r="AB3" s="352"/>
+      <c r="AB3" s="353"/>
     </row>
     <row r="4" spans="1:28" ht="98" x14ac:dyDescent="0.2">
       <c r="A4" s="229"/>
@@ -17475,7 +17478,7 @@
       <c r="G4" s="225" t="s">
         <v>122</v>
       </c>
-      <c r="H4" s="352"/>
+      <c r="H4" s="353"/>
       <c r="I4" s="228" t="s">
         <v>121</v>
       </c>
@@ -17518,7 +17521,7 @@
       <c r="V4" s="231" t="s">
         <v>108</v>
       </c>
-      <c r="W4" s="352"/>
+      <c r="W4" s="353"/>
       <c r="X4" s="232" t="s">
         <v>107</v>
       </c>
@@ -17531,7 +17534,7 @@
       <c r="AA4" s="232" t="s">
         <v>104</v>
       </c>
-      <c r="AB4" s="352"/>
+      <c r="AB4" s="353"/>
     </row>
     <row r="5" spans="1:28" ht="196" x14ac:dyDescent="0.2">
       <c r="A5" s="233" t="s">
@@ -18430,16 +18433,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="355" t="s">
+      <c r="A1" s="356" t="s">
         <v>228</v>
       </c>
-      <c r="B1" s="355"/>
-      <c r="C1" s="355"/>
-      <c r="D1" s="355"/>
-      <c r="E1" s="355"/>
-      <c r="F1" s="355"/>
-      <c r="G1" s="355"/>
-      <c r="H1" s="355"/>
+      <c r="B1" s="356"/>
+      <c r="C1" s="356"/>
+      <c r="D1" s="356"/>
+      <c r="E1" s="356"/>
+      <c r="F1" s="356"/>
+      <c r="G1" s="356"/>
+      <c r="H1" s="356"/>
       <c r="I1" s="273"/>
       <c r="J1" s="273"/>
       <c r="K1" s="273"/>
@@ -18464,7 +18467,7 @@
       <c r="G2" s="275" t="s">
         <v>183</v>
       </c>
-      <c r="H2" s="354" t="s">
+      <c r="H2" s="355" t="s">
         <v>182</v>
       </c>
       <c r="I2" s="275" t="s">
@@ -18497,13 +18500,13 @@
       <c r="R2" s="275" t="s">
         <v>181</v>
       </c>
-      <c r="S2" s="354" t="s">
+      <c r="S2" s="355" t="s">
         <v>180</v>
       </c>
       <c r="T2" s="275" t="s">
         <v>45</v>
       </c>
-      <c r="U2" s="354" t="s">
+      <c r="U2" s="355" t="s">
         <v>179</v>
       </c>
     </row>
@@ -18517,7 +18520,7 @@
       <c r="G3" s="275" t="s">
         <v>172</v>
       </c>
-      <c r="H3" s="354"/>
+      <c r="H3" s="355"/>
       <c r="I3" s="275" t="s">
         <v>224</v>
       </c>
@@ -18548,11 +18551,11 @@
       <c r="R3" s="275" t="s">
         <v>159</v>
       </c>
-      <c r="S3" s="354"/>
+      <c r="S3" s="355"/>
       <c r="T3" s="275" t="s">
         <v>156</v>
       </c>
-      <c r="U3" s="354"/>
+      <c r="U3" s="355"/>
     </row>
     <row r="4" spans="1:21" ht="112" x14ac:dyDescent="0.2">
       <c r="A4" s="272"/>
@@ -18574,7 +18577,7 @@
       <c r="G4" s="275" t="s">
         <v>122</v>
       </c>
-      <c r="H4" s="354"/>
+      <c r="H4" s="355"/>
       <c r="I4" s="275" t="s">
         <v>205</v>
       </c>
@@ -18605,11 +18608,11 @@
       <c r="R4" s="275" t="s">
         <v>108</v>
       </c>
-      <c r="S4" s="354"/>
+      <c r="S4" s="355"/>
       <c r="T4" s="275" t="s">
         <v>104</v>
       </c>
-      <c r="U4" s="354"/>
+      <c r="U4" s="355"/>
     </row>
     <row r="5" spans="1:21" ht="196" x14ac:dyDescent="0.2">
       <c r="A5" s="278" t="s">
@@ -19305,13 +19308,13 @@
       <c r="K2" s="203" t="s">
         <v>181</v>
       </c>
-      <c r="L2" s="351" t="s">
+      <c r="L2" s="352" t="s">
         <v>180</v>
       </c>
       <c r="M2" s="203" t="s">
         <v>45</v>
       </c>
-      <c r="N2" s="351" t="s">
+      <c r="N2" s="352" t="s">
         <v>179</v>
       </c>
     </row>
@@ -19329,11 +19332,11 @@
       <c r="K3" s="203" t="s">
         <v>159</v>
       </c>
-      <c r="L3" s="351"/>
+      <c r="L3" s="352"/>
       <c r="M3" s="203" t="s">
         <v>156</v>
       </c>
-      <c r="N3" s="351"/>
+      <c r="N3" s="352"/>
     </row>
     <row r="4" spans="1:14" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="256"/>
@@ -19359,11 +19362,11 @@
       <c r="K4" s="203" t="s">
         <v>108</v>
       </c>
-      <c r="L4" s="351"/>
+      <c r="L4" s="352"/>
       <c r="M4" s="203" t="s">
         <v>104</v>
       </c>
-      <c r="N4" s="351"/>
+      <c r="N4" s="352"/>
     </row>
     <row r="5" spans="1:14" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="258"/>
@@ -20018,10 +20021,10 @@
   <sheetPr codeName="Feuil13">
     <tabColor rgb="FF2C45E0"/>
   </sheetPr>
-  <dimension ref="A1:FI4"/>
+  <dimension ref="A1:FJ4"/>
   <sheetViews>
     <sheetView showFormulas="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="FH3" sqref="FH3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20036,11 +20039,11 @@
     <col min="157" max="157" width="60.6640625" bestFit="1" customWidth="1"/>
     <col min="161" max="161" width="52" bestFit="1" customWidth="1"/>
     <col min="162" max="162" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="169" max="169" width="45.1640625" bestFit="1" customWidth="1"/>
-    <col min="170" max="170" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="170" max="170" width="45.1640625" bestFit="1" customWidth="1"/>
+    <col min="171" max="171" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:165" s="4" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:166" s="4" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>232</v>
       </c>
@@ -20060,13 +20063,14 @@
       <c r="FD1" s="338"/>
       <c r="FE1" s="338"/>
       <c r="FF1" s="338"/>
-      <c r="FG1" s="356"/>
-      <c r="FH1" s="356"/>
-      <c r="FI1" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:165" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="FG1" s="339"/>
+      <c r="FH1" s="339"/>
+      <c r="FI1" s="339"/>
+      <c r="FJ1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:166" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
         <v>8</v>
       </c>
@@ -20092,13 +20096,16 @@
         <v>39</v>
       </c>
       <c r="FG2" s="126" t="s">
+        <v>437</v>
+      </c>
+      <c r="FH2" s="126" t="s">
         <v>435</v>
       </c>
-      <c r="FH2" s="126" t="s">
+      <c r="FI2" s="126" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="3" spans="1:165" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:166" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
         <v>11</v>
       </c>
@@ -20106,7 +20113,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:165" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:166" x14ac:dyDescent="0.2">
       <c r="B4" s="27" t="s">
         <v>7</v>
       </c>
@@ -20115,7 +20122,7 @@
   </sheetData>
   <autoFilter ref="A2:DT2" xr:uid="{3B89445B-6ECC-4440-B85C-E593AE209933}"/>
   <mergeCells count="1">
-    <mergeCell ref="FA1:FH1"/>
+    <mergeCell ref="FA1:FI1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -20210,28 +20217,28 @@
       <c r="D4" s="294"/>
       <c r="E4" s="294"/>
       <c r="F4" s="294"/>
-      <c r="G4" s="339" t="s">
+      <c r="G4" s="340" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="340"/>
-      <c r="I4" s="340"/>
-      <c r="J4" s="340"/>
-      <c r="K4" s="340"/>
-      <c r="L4" s="341"/>
-      <c r="M4" s="342"/>
-      <c r="N4" s="343" t="s">
+      <c r="H4" s="341"/>
+      <c r="I4" s="341"/>
+      <c r="J4" s="341"/>
+      <c r="K4" s="341"/>
+      <c r="L4" s="342"/>
+      <c r="M4" s="343"/>
+      <c r="N4" s="344" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="341"/>
-      <c r="P4" s="341"/>
-      <c r="Q4" s="341"/>
-      <c r="R4" s="341"/>
-      <c r="S4" s="341"/>
-      <c r="T4" s="344"/>
-      <c r="U4" s="339" t="s">
+      <c r="O4" s="342"/>
+      <c r="P4" s="342"/>
+      <c r="Q4" s="342"/>
+      <c r="R4" s="342"/>
+      <c r="S4" s="342"/>
+      <c r="T4" s="345"/>
+      <c r="U4" s="340" t="s">
         <v>28</v>
       </c>
-      <c r="V4" s="342"/>
+      <c r="V4" s="343"/>
       <c r="W4" s="301"/>
       <c r="X4" t="s">
         <v>0</v>
@@ -20309,7 +20316,7 @@
         <v>399</v>
       </c>
       <c r="G6" s="19" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"M-TIT",'ETPT Format DDG'!$C:$C,$A$3)</f>
+        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FG:$FG,"M-TIT",'ETPT Format DDG'!$C:$C,$A$3)</f>
         <v>#N/A</v>
       </c>
       <c r="H6" s="298" t="str">
@@ -20317,11 +20324,11 @@
         <v/>
       </c>
       <c r="I6" s="18" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"M-PLAC-ADD",'ETPT Format DDG'!$C:$C,$A$3)</f>
+        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FG:$FG,"M-PLAC-ADD",'ETPT Format DDG'!$C:$C,$A$3)</f>
         <v>#N/A</v>
       </c>
       <c r="J6" s="18" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"M-PLAC-SUB",'ETPT Format DDG'!$C:$C,$A$3)</f>
+        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FG:$FG,"M-PLAC-SUB",'ETPT Format DDG'!$C:$C,$A$3)</f>
         <v>#N/A</v>
       </c>
       <c r="K6" s="18" t="e">
@@ -20329,7 +20336,7 @@
 INDEX('ETPT Format DDG'!$A:$DU,
 ,
 IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))
-),'ETPT Format DDG'!$I:$I,"C",
+),'ETPT Format DDG'!$FG:$FG,"C",
 'ETPT Format DDG'!$C:$C,$A$3,
 'ETPT Format DDG'!$G:$G,"Magistrat")</f>
         <v>#N/A</v>
@@ -20349,7 +20356,7 @@
         <v/>
       </c>
       <c r="N6" s="18" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"F-TIT",'ETPT Format DDG'!$C:$C,$A$3)</f>
+        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FG:$FG,"F-TIT",'ETPT Format DDG'!$C:$C,$A$3)</f>
         <v>#N/A</v>
       </c>
       <c r="O6" s="298" t="str">
@@ -20357,15 +20364,15 @@
         <v/>
       </c>
       <c r="P6" s="18" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"F-PLAC-ADD",'ETPT Format DDG'!$C:$C,$A$3)</f>
+        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FG:$FG,"F-PLAC-ADD",'ETPT Format DDG'!$C:$C,$A$3)</f>
         <v>#N/A</v>
       </c>
       <c r="Q6" s="18" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"F-PLAC-SUB",'ETPT Format DDG'!$C:$C,$A$3)</f>
+        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FG:$FG,"F-PLAC-SUB",'ETPT Format DDG'!$C:$C,$A$3)</f>
         <v>#N/A</v>
       </c>
       <c r="R6" s="18" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"C",'ETPT Format DDG'!$C:$C,$A$3,'ETPT Format DDG'!$G:$G,"Greffe")</f>
+        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FG:$FG,"C",'ETPT Format DDG'!$C:$C,$A$3,'ETPT Format DDG'!$G:$G,"Greffe")</f>
         <v>#N/A</v>
       </c>
       <c r="S6" s="19" t="e">
@@ -20387,7 +20394,7 @@
 INDEX('ETPT Format DDG'!$A:$DU,
 ,
 IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))
-),'ETPT Format DDG'!$I:$I,"C",
+),'ETPT Format DDG'!$FG:$FG,"C",
 'ETPT Format DDG'!$C:$C,$A$3,
 'ETPT Format DDG'!$G:$G,"Autour du magistrat")</f>
         <v>#N/A</v>
@@ -20834,16 +20841,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" s="44" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B1" s="346" t="s">
+      <c r="B1" s="347" t="s">
         <v>184</v>
       </c>
-      <c r="C1" s="346"/>
-      <c r="D1" s="346"/>
-      <c r="E1" s="346"/>
-      <c r="F1" s="346"/>
-      <c r="G1" s="346"/>
-      <c r="H1" s="346"/>
-      <c r="I1" s="346"/>
+      <c r="C1" s="347"/>
+      <c r="D1" s="347"/>
+      <c r="E1" s="347"/>
+      <c r="F1" s="347"/>
+      <c r="G1" s="347"/>
+      <c r="H1" s="347"/>
+      <c r="I1" s="347"/>
     </row>
     <row r="2" spans="1:62" s="44" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="90"/>
@@ -20855,7 +20862,7 @@
       <c r="G2" s="87" t="s">
         <v>183</v>
       </c>
-      <c r="H2" s="345" t="s">
+      <c r="H2" s="346" t="s">
         <v>182</v>
       </c>
       <c r="I2" s="86" t="s">
@@ -20900,7 +20907,7 @@
       <c r="V2" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="W2" s="345" t="s">
+      <c r="W2" s="346" t="s">
         <v>180</v>
       </c>
       <c r="X2" s="87" t="s">
@@ -20915,7 +20922,7 @@
       <c r="AA2" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="AB2" s="345" t="s">
+      <c r="AB2" s="346" t="s">
         <v>179</v>
       </c>
       <c r="AC2" s="84" t="s">
@@ -20945,7 +20952,7 @@
       <c r="AK2" s="84" t="s">
         <v>178</v>
       </c>
-      <c r="AL2" s="345" t="s">
+      <c r="AL2" s="346" t="s">
         <v>177</v>
       </c>
       <c r="AM2" s="84" t="s">
@@ -20987,7 +20994,7 @@
       <c r="AY2" s="84" t="s">
         <v>176</v>
       </c>
-      <c r="AZ2" s="345" t="s">
+      <c r="AZ2" s="346" t="s">
         <v>175</v>
       </c>
       <c r="BA2" s="83" t="s">
@@ -21017,7 +21024,7 @@
       <c r="BI2" s="83" t="s">
         <v>174</v>
       </c>
-      <c r="BJ2" s="345" t="s">
+      <c r="BJ2" s="346" t="s">
         <v>173</v>
       </c>
     </row>
@@ -21031,7 +21038,7 @@
       <c r="G3" s="87" t="s">
         <v>172</v>
       </c>
-      <c r="H3" s="345"/>
+      <c r="H3" s="346"/>
       <c r="I3" s="86" t="s">
         <v>171</v>
       </c>
@@ -21072,7 +21079,7 @@
       <c r="V3" s="86" t="s">
         <v>159</v>
       </c>
-      <c r="W3" s="345"/>
+      <c r="W3" s="346"/>
       <c r="X3" s="82"/>
       <c r="Y3" s="87" t="s">
         <v>158</v>
@@ -21083,7 +21090,7 @@
       <c r="AA3" s="87" t="s">
         <v>156</v>
       </c>
-      <c r="AB3" s="345"/>
+      <c r="AB3" s="346"/>
       <c r="AC3" s="84" t="s">
         <v>155</v>
       </c>
@@ -21111,7 +21118,7 @@
       <c r="AK3" s="84" t="s">
         <v>149</v>
       </c>
-      <c r="AL3" s="345"/>
+      <c r="AL3" s="346"/>
       <c r="AM3" s="84" t="s">
         <v>148</v>
       </c>
@@ -21151,7 +21158,7 @@
       <c r="AY3" s="84" t="s">
         <v>136</v>
       </c>
-      <c r="AZ3" s="345"/>
+      <c r="AZ3" s="346"/>
       <c r="BA3" s="83" t="s">
         <v>135</v>
       </c>
@@ -21179,7 +21186,7 @@
       <c r="BI3" s="83" t="s">
         <v>127</v>
       </c>
-      <c r="BJ3" s="345"/>
+      <c r="BJ3" s="346"/>
     </row>
     <row r="4" spans="1:62" s="44" customFormat="1" ht="60" x14ac:dyDescent="0.15">
       <c r="A4" s="89"/>
@@ -21201,7 +21208,7 @@
       <c r="G4" s="87" t="s">
         <v>122</v>
       </c>
-      <c r="H4" s="345"/>
+      <c r="H4" s="346"/>
       <c r="I4" s="86" t="s">
         <v>121</v>
       </c>
@@ -21244,7 +21251,7 @@
       <c r="V4" s="86" t="s">
         <v>108</v>
       </c>
-      <c r="W4" s="345"/>
+      <c r="W4" s="346"/>
       <c r="X4" s="85" t="s">
         <v>107</v>
       </c>
@@ -21257,7 +21264,7 @@
       <c r="AA4" s="85" t="s">
         <v>104</v>
       </c>
-      <c r="AB4" s="345"/>
+      <c r="AB4" s="346"/>
       <c r="AC4" s="84" t="s">
         <v>103</v>
       </c>
@@ -21285,7 +21292,7 @@
       <c r="AK4" s="84" t="s">
         <v>96</v>
       </c>
-      <c r="AL4" s="345"/>
+      <c r="AL4" s="346"/>
       <c r="AM4" s="84" t="s">
         <v>95</v>
       </c>
@@ -21325,7 +21332,7 @@
       <c r="AY4" s="84" t="s">
         <v>83</v>
       </c>
-      <c r="AZ4" s="345"/>
+      <c r="AZ4" s="346"/>
       <c r="BA4" s="83" t="s">
         <v>82</v>
       </c>
@@ -21353,7 +21360,7 @@
       <c r="BI4" s="83" t="s">
         <v>74</v>
       </c>
-      <c r="BJ4" s="345"/>
+      <c r="BJ4" s="346"/>
     </row>
     <row r="5" spans="1:62" s="44" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="54" t="s">
@@ -23550,16 +23557,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A1" s="347" t="s">
+      <c r="A1" s="348" t="s">
         <v>228</v>
       </c>
-      <c r="B1" s="347"/>
-      <c r="C1" s="347"/>
-      <c r="D1" s="347"/>
-      <c r="E1" s="347"/>
-      <c r="F1" s="347"/>
-      <c r="G1" s="347"/>
-      <c r="H1" s="347"/>
+      <c r="B1" s="348"/>
+      <c r="C1" s="348"/>
+      <c r="D1" s="348"/>
+      <c r="E1" s="348"/>
+      <c r="F1" s="348"/>
+      <c r="G1" s="348"/>
+      <c r="H1" s="348"/>
       <c r="I1" s="44"/>
       <c r="J1" s="44"/>
       <c r="K1" s="44"/>
@@ -23598,7 +23605,7 @@
       <c r="G2" s="87" t="s">
         <v>183</v>
       </c>
-      <c r="H2" s="345" t="s">
+      <c r="H2" s="346" t="s">
         <v>182</v>
       </c>
       <c r="I2" s="87" t="s">
@@ -23631,13 +23638,13 @@
       <c r="R2" s="87" t="s">
         <v>181</v>
       </c>
-      <c r="S2" s="345" t="s">
+      <c r="S2" s="346" t="s">
         <v>180</v>
       </c>
       <c r="T2" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="U2" s="345" t="s">
+      <c r="U2" s="346" t="s">
         <v>179</v>
       </c>
       <c r="V2" s="87" t="s">
@@ -23667,7 +23674,7 @@
       <c r="AD2" s="87" t="s">
         <v>178</v>
       </c>
-      <c r="AE2" s="345" t="s">
+      <c r="AE2" s="346" t="s">
         <v>227</v>
       </c>
       <c r="AF2" s="87" t="s">
@@ -23679,7 +23686,7 @@
       <c r="AH2" s="87" t="s">
         <v>226</v>
       </c>
-      <c r="AI2" s="345" t="s">
+      <c r="AI2" s="346" t="s">
         <v>225</v>
       </c>
     </row>
@@ -23693,7 +23700,7 @@
       <c r="G3" s="87" t="s">
         <v>172</v>
       </c>
-      <c r="H3" s="345"/>
+      <c r="H3" s="346"/>
       <c r="I3" s="87" t="s">
         <v>224</v>
       </c>
@@ -23724,11 +23731,11 @@
       <c r="R3" s="87" t="s">
         <v>159</v>
       </c>
-      <c r="S3" s="345"/>
+      <c r="S3" s="346"/>
       <c r="T3" s="87" t="s">
         <v>156</v>
       </c>
-      <c r="U3" s="345"/>
+      <c r="U3" s="346"/>
       <c r="V3" s="87" t="s">
         <v>215</v>
       </c>
@@ -23756,7 +23763,7 @@
       <c r="AD3" s="87" t="s">
         <v>207</v>
       </c>
-      <c r="AE3" s="345"/>
+      <c r="AE3" s="346"/>
       <c r="AF3" s="87" t="s">
         <v>206</v>
       </c>
@@ -23766,7 +23773,7 @@
       <c r="AH3" s="87" t="s">
         <v>136</v>
       </c>
-      <c r="AI3" s="345"/>
+      <c r="AI3" s="346"/>
     </row>
     <row r="4" spans="1:35" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="90"/>
@@ -23788,7 +23795,7 @@
       <c r="G4" s="87" t="s">
         <v>122</v>
       </c>
-      <c r="H4" s="345"/>
+      <c r="H4" s="346"/>
       <c r="I4" s="87" t="s">
         <v>205</v>
       </c>
@@ -23819,11 +23826,11 @@
       <c r="R4" s="87" t="s">
         <v>108</v>
       </c>
-      <c r="S4" s="345"/>
+      <c r="S4" s="346"/>
       <c r="T4" s="87" t="s">
         <v>104</v>
       </c>
-      <c r="U4" s="345"/>
+      <c r="U4" s="346"/>
       <c r="V4" s="87" t="s">
         <v>196</v>
       </c>
@@ -23851,7 +23858,7 @@
       <c r="AD4" s="87" t="s">
         <v>188</v>
       </c>
-      <c r="AE4" s="345"/>
+      <c r="AE4" s="346"/>
       <c r="AF4" s="87" t="s">
         <v>187</v>
       </c>
@@ -23861,7 +23868,7 @@
       <c r="AH4" s="87" t="s">
         <v>83</v>
       </c>
-      <c r="AI4" s="345"/>
+      <c r="AI4" s="346"/>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A5" s="93" t="s">

</xml_diff>

<commit_message>
update extractor CA Indispo counter
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7302EF8-8DE6-1A43-8AD2-8669F817114E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D77EB23-DE49-7A4C-AAEA-EFF1BADE4F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" activeTab="3" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
   <sheets>
     <sheet name="ACCUEIL" sheetId="33" r:id="rId1"/>
@@ -7156,7 +7156,3047 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{6FC886D6-2077-B34D-B1DF-739B068A66D1}"/>
     <cellStyle name="Normal 3" xfId="4" xr:uid="{6BD57324-3FD5-D341-A299-730D14794802}"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="314">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -8014,7 +11054,7 @@
   </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -20207,8 +23247,8 @@
   </sheetPr>
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F1" sqref="D1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20505,45 +23545,71 @@
     <mergeCell ref="U4:V4"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:F4">
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="31" priority="16">
       <formula>IF(LEFT($A$3,2)&lt;&gt;"TJ",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:V151">
-    <cfRule type="expression" dxfId="8" priority="12">
+    <cfRule type="expression" dxfId="30" priority="18">
       <formula>AND(ISBLANK($C6)=FALSE,ISBLANK($E6)=TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:F1048576">
-    <cfRule type="expression" dxfId="7" priority="1">
-      <formula>AND($D1="5. TOTAL JLD CIVIL",OR(_xlfn.NUMBERVALUE($L1-$L2-$L3)-_xlfn.NUMBERVALUE($L4)&lt;&gt;0,_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3)-_xlfn.NUMBERVALUE($S4)&lt;&gt;0,_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3)-_xlfn.NUMBERVALUE($U4)&lt;&gt;0))</formula>
+    <cfRule type="expression" dxfId="16" priority="7">
+      <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($L1)-_xlfn.NUMBERVALUE($L2)-_xlfn.NUMBERVALUE($L3)-_xlfn.NUMBERVALUE($L4)-_xlfn.NUMBERVALUE($L5)-_xlfn.NUMBERVALUE($L6)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="29" priority="12">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",OR(_xlfn.NUMBERVALUE($L1)-_xlfn.NUMBERVALUE($L2)-_xlfn.NUMBERVALUE($L3)&lt;&gt;0,_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3)&lt;&gt;0,_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3)&lt;&gt;0))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="2">
+      <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3)-_xlfn.NUMBERVALUE($S4)-_xlfn.NUMBERVALUE($S5)&lt;&gt;0)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="1" stopIfTrue="1">
+      <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3)-_xlfn.NUMBERVALUE($U4)-_xlfn.NUMBERVALUE($U5)&lt;&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7:F7">
+    <cfRule type="expression" dxfId="26" priority="6">
+      <formula>OR(_xlfn.NUMBERVALUE($L7)&lt;&gt;_xlfn.NUMBERVALUE($L6),_xlfn.NUMBERVALUE($S7)&lt;&gt;_xlfn.NUMBERVALUE($S6),_xlfn.NUMBERVALUE($U7)&lt;&gt;_xlfn.NUMBERVALUE($U6))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:M1048576">
-    <cfRule type="expression" dxfId="5" priority="5">
-      <formula>AND($D1="5. TOTAL JLD CIVIL",_xlfn.NUMBERVALUE($L1)-_xlfn.NUMBERVALUE($L2)-_xlfn.NUMBERVALUE($L3)-_xlfn.NUMBERVALUE($L4)&lt;&gt;0)</formula>
+    <cfRule type="expression" dxfId="25" priority="11" stopIfTrue="1">
+      <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($L1)-_xlfn.NUMBERVALUE($L2)-_xlfn.NUMBERVALUE($L3)-_xlfn.NUMBERVALUE($L4)-_xlfn.NUMBERVALUE($L5)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="9">
+    <cfRule type="expression" dxfId="24" priority="15" stopIfTrue="1">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",_xlfn.NUMBERVALUE($L1)-_xlfn.NUMBERVALUE($L2)-_xlfn.NUMBERVALUE($L3)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="G7:M7">
+    <cfRule type="expression" dxfId="23" priority="5">
+      <formula>_xlfn.NUMBERVALUE($L7)&lt;&gt;_xlfn.NUMBERVALUE($L6)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="N1:T1048576">
-    <cfRule type="expression" dxfId="3" priority="4">
-      <formula>AND($D1="5. TOTAL JLD CIVIL",_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3)-_xlfn.NUMBERVALUE($S4)&lt;&gt;0)</formula>
+    <cfRule type="expression" dxfId="22" priority="10" stopIfTrue="1">
+      <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3)-_xlfn.NUMBERVALUE($S4)-_xlfn.NUMBERVALUE($S5)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="8">
+    <cfRule type="expression" dxfId="21" priority="14" stopIfTrue="1">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="N7:T7">
+    <cfRule type="expression" dxfId="20" priority="4">
+      <formula>_xlfn.NUMBERVALUE($S7)&lt;&gt;_xlfn.NUMBERVALUE($S6)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="U1:V1048576">
-    <cfRule type="expression" dxfId="1" priority="3">
-      <formula>AND($D1="5. TOTAL JLD CIVIL",_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3)-_xlfn.NUMBERVALUE($U4)&lt;&gt;0)</formula>
+    <cfRule type="expression" dxfId="19" priority="9" stopIfTrue="1">
+      <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3)-_xlfn.NUMBERVALUE($U4)-_xlfn.NUMBERVALUE($U5)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="7">
+    <cfRule type="expression" dxfId="18" priority="13" stopIfTrue="1">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3)&lt;&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U7:V7">
+    <cfRule type="expression" dxfId="17" priority="3">
+      <formula>_xlfn.NUMBERVALUE($U7)&lt;&gt;_xlfn.NUMBERVALUE($U6)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update validation conditionnelle agregats
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D77EB23-DE49-7A4C-AAEA-EFF1BADE4F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3095B4-999B-FB46-9889-DD77E8729181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" activeTab="3" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
@@ -7156,7 +7156,7 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{6FC886D6-2077-B34D-B1DF-739B068A66D1}"/>
     <cellStyle name="Normal 3" xfId="4" xr:uid="{6BD57324-3FD5-D341-A299-730D14794802}"/>
   </cellStyles>
-  <dxfs count="314">
+  <dxfs count="240">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -8878,6 +8878,26 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <fgColor theme="5" tint="0.79998168889431442"/>
@@ -8896,6 +8916,26 @@
       <font>
         <color theme="0"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -9158,6 +9198,26 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <fgColor theme="5" tint="0.79998168889431442"/>
@@ -9176,6 +9236,26 @@
       <font>
         <color theme="0"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -9336,826 +9416,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -23248,7 +22508,7 @@
   <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F1" sqref="D1:F1048576"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -23452,13 +22712,13 @@
         <v>#N/A</v>
       </c>
       <c r="L6" s="19" t="e">
-        <f>SUMIFS(
+        <f>ROUND(SUMIFS(
 INDEX('ETPT Format DDG'!$A:$DU,
 ,
 IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))
 ),
 'ETPT Format DDG'!$C:$C,$A$3,
-'ETPT Format DDG'!$G:$G,"Magistrat")</f>
+'ETPT Format DDG'!$G:$G,"Magistrat"),3)</f>
         <v>#N/A</v>
       </c>
       <c r="M6" s="299" t="str">
@@ -23486,13 +22746,13 @@
         <v>#N/A</v>
       </c>
       <c r="S6" s="19" t="e">
-        <f>SUMIFS(
+        <f>ROUND(SUMIFS(
 INDEX('ETPT Format DDG'!$A:$DU,
 ,
 IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))
 ),
 'ETPT Format DDG'!$C:$C,$A$3,
-'ETPT Format DDG'!$G:$G,"Greffe")</f>
+'ETPT Format DDG'!$G:$G,"Greffe"),3)</f>
         <v>#N/A</v>
       </c>
       <c r="T6" s="298" t="str">
@@ -23500,13 +22760,13 @@
         <v/>
       </c>
       <c r="U6" s="19" t="e">
-        <f>SUMIFS(
+        <f>ROUND(SUMIFS(
 INDEX('ETPT Format DDG'!$A:$DU,
 ,
 IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))
 ),'ETPT Format DDG'!$FG:$FG,"C",
 'ETPT Format DDG'!$C:$C,$A$3,
-'ETPT Format DDG'!$G:$G,"Autour du magistrat")</f>
+'ETPT Format DDG'!$G:$G,"Autour du magistrat"),3)</f>
         <v>#N/A</v>
       </c>
       <c r="V6" s="299" t="str">
@@ -23555,60 +22815,60 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:F1048576">
-    <cfRule type="expression" dxfId="16" priority="7">
-      <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($L1)-_xlfn.NUMBERVALUE($L2)-_xlfn.NUMBERVALUE($L3)-_xlfn.NUMBERVALUE($L4)-_xlfn.NUMBERVALUE($L5)-_xlfn.NUMBERVALUE($L6)&lt;&gt;0)</formula>
+    <cfRule type="expression" dxfId="16" priority="1" stopIfTrue="1">
+      <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($U1)-(_xlfn.NUMBERVALUE($U2)+_xlfn.NUMBERVALUE($U3)+_xlfn.NUMBERVALUE($U4)+_xlfn.NUMBERVALUE($U5)+_xlfn.NUMBERVALUE($U6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="12">
-      <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",OR(_xlfn.NUMBERVALUE($L1)-_xlfn.NUMBERVALUE($L2)-_xlfn.NUMBERVALUE($L3)&lt;&gt;0,_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3)&lt;&gt;0,_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3)&lt;&gt;0))</formula>
+    <cfRule type="expression" dxfId="17" priority="2" stopIfTrue="1">
+      <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($S1)-(_xlfn.NUMBERVALUE($S2)+_xlfn.NUMBERVALUE($S3)+_xlfn.NUMBERVALUE($S4)+_xlfn.NUMBERVALUE($S5)+_xlfn.NUMBERVALUE($S6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="2">
-      <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3)-_xlfn.NUMBERVALUE($S4)-_xlfn.NUMBERVALUE($S5)&lt;&gt;0)</formula>
+    <cfRule type="expression" dxfId="18" priority="7" stopIfTrue="1">
+      <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3)+_xlfn.NUMBERVALUE($L4)-_xlfn.NUMBERVALUE($L5)+_xlfn.NUMBERVALUE($L6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="1" stopIfTrue="1">
-      <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3)-_xlfn.NUMBERVALUE($U4)-_xlfn.NUMBERVALUE($U5)&lt;&gt;0)</formula>
+    <cfRule type="expression" dxfId="19" priority="12" stopIfTrue="1">
+      <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",OR(_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3))&lt;&gt;0,_xlfn.NUMBERVALUE($S1)-(_xlfn.NUMBERVALUE($S2)+_xlfn.NUMBERVALUE($S3))&lt;&gt;0,_xlfn.NUMBERVALUE($U1)-(_xlfn.NUMBERVALUE($U2)+_xlfn.NUMBERVALUE($U3))&lt;&gt;0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:F7">
-    <cfRule type="expression" dxfId="26" priority="6">
+    <cfRule type="expression" dxfId="29" priority="6" stopIfTrue="1">
       <formula>OR(_xlfn.NUMBERVALUE($L7)&lt;&gt;_xlfn.NUMBERVALUE($L6),_xlfn.NUMBERVALUE($S7)&lt;&gt;_xlfn.NUMBERVALUE($S6),_xlfn.NUMBERVALUE($U7)&lt;&gt;_xlfn.NUMBERVALUE($U6))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:M1048576">
-    <cfRule type="expression" dxfId="25" priority="11" stopIfTrue="1">
-      <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($L1)-_xlfn.NUMBERVALUE($L2)-_xlfn.NUMBERVALUE($L3)-_xlfn.NUMBERVALUE($L4)-_xlfn.NUMBERVALUE($L5)&lt;&gt;0)</formula>
+    <cfRule type="expression" dxfId="28" priority="11" stopIfTrue="1">
+      <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3)+_xlfn.NUMBERVALUE($L4)+_xlfn.NUMBERVALUE($L5)+_xlfn.NUMBERVALUE($L6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="15" stopIfTrue="1">
-      <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",_xlfn.NUMBERVALUE($L1)-_xlfn.NUMBERVALUE($L2)-_xlfn.NUMBERVALUE($L3)&lt;&gt;0)</formula>
+    <cfRule type="expression" dxfId="27" priority="15">
+      <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3))&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:M7">
-    <cfRule type="expression" dxfId="23" priority="5">
+    <cfRule type="expression" dxfId="26" priority="5">
       <formula>_xlfn.NUMBERVALUE($L7)&lt;&gt;_xlfn.NUMBERVALUE($L6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:T1048576">
-    <cfRule type="expression" dxfId="22" priority="10" stopIfTrue="1">
-      <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3)-_xlfn.NUMBERVALUE($S4)-_xlfn.NUMBERVALUE($S5)&lt;&gt;0)</formula>
+    <cfRule type="expression" dxfId="25" priority="10" stopIfTrue="1">
+      <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($S1)-(_xlfn.NUMBERVALUE($S2)+_xlfn.NUMBERVALUE($S3)+_xlfn.NUMBERVALUE($S4)+_xlfn.NUMBERVALUE($S5)+_xlfn.NUMBERVALUE($S6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="14" stopIfTrue="1">
-      <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3)&lt;&gt;0)</formula>
+    <cfRule type="expression" dxfId="24" priority="14">
+      <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",_xlfn.NUMBERVALUE($S1)-(_xlfn.NUMBERVALUE($S2)+_xlfn.NUMBERVALUE($S3))&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7:T7">
-    <cfRule type="expression" dxfId="20" priority="4">
+    <cfRule type="expression" dxfId="23" priority="4">
       <formula>_xlfn.NUMBERVALUE($S7)&lt;&gt;_xlfn.NUMBERVALUE($S6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:V1048576">
-    <cfRule type="expression" dxfId="19" priority="9" stopIfTrue="1">
-      <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3)-_xlfn.NUMBERVALUE($U4)-_xlfn.NUMBERVALUE($U5)&lt;&gt;0)</formula>
+    <cfRule type="expression" dxfId="22" priority="9">
+      <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($U1)-(_xlfn.NUMBERVALUE($U2)+_xlfn.NUMBERVALUE($U3)+_xlfn.NUMBERVALUE($U4)+_xlfn.NUMBERVALUE($U5)+_xlfn.NUMBERVALUE($U6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="13" stopIfTrue="1">
-      <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3)&lt;&gt;0)</formula>
+    <cfRule type="expression" dxfId="21" priority="13">
+      <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",_xlfn.NUMBERVALUE($U1)-(_xlfn.NUMBERVALUE($U2)+_xlfn.NUMBERVALUE($U3))&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U7:V7">
-    <cfRule type="expression" dxfId="17" priority="3">
+    <cfRule type="expression" dxfId="20" priority="3">
       <formula>_xlfn.NUMBERVALUE($U7)&lt;&gt;_xlfn.NUMBERVALUE($U6)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add CA indicator for red flags aggregats and add message for TJ and CA
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3095B4-999B-FB46-9889-DD77E8729181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FC65B3-C932-D543-B071-ECABC4D66B10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" activeTab="3" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
@@ -5955,7 +5955,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="357">
+  <cellXfs count="358">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -7025,6 +7025,9 @@
     </xf>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -7156,2247 +7159,7 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{6FC886D6-2077-B34D-B1DF-739B068A66D1}"/>
     <cellStyle name="Normal 3" xfId="4" xr:uid="{6BD57324-3FD5-D341-A299-730D14794802}"/>
   </cellStyles>
-  <dxfs count="240">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
+  <dxfs count="16">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -10335,11 +8098,11 @@
       <c r="B1" s="129" t="s">
         <v>239</v>
       </c>
-      <c r="C1" s="319" t="s">
+      <c r="C1" s="320" t="s">
         <v>240</v>
       </c>
-      <c r="D1" s="319"/>
-      <c r="E1" s="319"/>
+      <c r="D1" s="320"/>
+      <c r="E1" s="320"/>
       <c r="F1" s="130"/>
       <c r="H1" s="26" t="s">
         <v>0</v>
@@ -10348,11 +8111,11 @@
     <row r="2" spans="1:8" s="134" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="131"/>
       <c r="B2" s="132"/>
-      <c r="C2" s="320" t="s">
+      <c r="C2" s="321" t="s">
         <v>241</v>
       </c>
-      <c r="D2" s="320"/>
-      <c r="E2" s="320"/>
+      <c r="D2" s="321"/>
+      <c r="E2" s="321"/>
       <c r="F2" s="133"/>
       <c r="H2" s="26" t="s">
         <v>0</v>
@@ -10376,10 +8139,10 @@
       <c r="D4" s="139" t="s">
         <v>244</v>
       </c>
-      <c r="E4" s="326" t="s">
+      <c r="E4" s="327" t="s">
         <v>245</v>
       </c>
-      <c r="F4" s="327"/>
+      <c r="F4" s="328"/>
       <c r="G4" s="148"/>
       <c r="H4" s="26" t="s">
         <v>0</v>
@@ -10396,10 +8159,10 @@
       <c r="D5" s="145" t="s">
         <v>248</v>
       </c>
-      <c r="E5" s="328" t="s">
+      <c r="E5" s="329" t="s">
         <v>261</v>
       </c>
-      <c r="F5" s="329"/>
+      <c r="F5" s="330"/>
       <c r="G5" s="147"/>
       <c r="H5" s="26" t="s">
         <v>0</v>
@@ -10416,10 +8179,10 @@
       <c r="D6" s="146" t="s">
         <v>251</v>
       </c>
-      <c r="E6" s="330" t="s">
+      <c r="E6" s="331" t="s">
         <v>262</v>
       </c>
-      <c r="F6" s="331"/>
+      <c r="F6" s="332"/>
       <c r="G6" s="147"/>
       <c r="H6" s="26" t="s">
         <v>0</v>
@@ -10436,10 +8199,10 @@
       <c r="D7" s="146" t="s">
         <v>254</v>
       </c>
-      <c r="E7" s="330" t="s">
+      <c r="E7" s="331" t="s">
         <v>261</v>
       </c>
-      <c r="F7" s="331"/>
+      <c r="F7" s="332"/>
       <c r="G7" s="147"/>
       <c r="H7" s="26" t="s">
         <v>0</v>
@@ -10450,16 +8213,16 @@
       <c r="B8" s="155" t="s">
         <v>255</v>
       </c>
-      <c r="C8" s="321" t="s">
+      <c r="C8" s="322" t="s">
         <v>256</v>
       </c>
-      <c r="D8" s="321" t="s">
+      <c r="D8" s="322" t="s">
         <v>257</v>
       </c>
-      <c r="E8" s="332" t="s">
+      <c r="E8" s="333" t="s">
         <v>263</v>
       </c>
-      <c r="F8" s="333"/>
+      <c r="F8" s="334"/>
       <c r="G8" s="147"/>
       <c r="H8" s="26" t="s">
         <v>0</v>
@@ -10470,10 +8233,10 @@
       <c r="B9" s="156" t="s">
         <v>258</v>
       </c>
-      <c r="C9" s="321"/>
-      <c r="D9" s="321"/>
-      <c r="E9" s="334"/>
-      <c r="F9" s="335"/>
+      <c r="C9" s="322"/>
+      <c r="D9" s="322"/>
+      <c r="E9" s="335"/>
+      <c r="F9" s="336"/>
       <c r="G9" s="147"/>
       <c r="H9" s="26" t="s">
         <v>0</v>
@@ -10484,10 +8247,10 @@
       <c r="B10" s="157" t="s">
         <v>259</v>
       </c>
-      <c r="C10" s="322"/>
-      <c r="D10" s="322"/>
-      <c r="E10" s="336"/>
-      <c r="F10" s="337"/>
+      <c r="C10" s="323"/>
+      <c r="D10" s="323"/>
+      <c r="E10" s="337"/>
+      <c r="F10" s="338"/>
       <c r="G10" s="147"/>
       <c r="H10" s="26" t="s">
         <v>0</v>
@@ -10507,11 +8270,11 @@
     <row r="12" spans="1:8" s="26" customFormat="1" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="135"/>
       <c r="B12" s="149"/>
-      <c r="C12" s="325" t="s">
+      <c r="C12" s="326" t="s">
         <v>260</v>
       </c>
-      <c r="D12" s="325"/>
-      <c r="E12" s="325"/>
+      <c r="D12" s="326"/>
+      <c r="E12" s="326"/>
       <c r="F12" s="150"/>
       <c r="H12" s="26" t="s">
         <v>0</v>
@@ -10525,14 +8288,14 @@
       </c>
     </row>
     <row r="14" spans="1:8" s="26" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="323" t="s">
+      <c r="A14" s="324" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="323"/>
-      <c r="C14" s="323"/>
-      <c r="D14" s="323"/>
-      <c r="E14" s="323"/>
-      <c r="F14" s="324"/>
+      <c r="B14" s="324"/>
+      <c r="C14" s="324"/>
+      <c r="D14" s="324"/>
+      <c r="E14" s="324"/>
+      <c r="F14" s="325"/>
       <c r="H14" s="26" t="s">
         <v>0</v>
       </c>
@@ -10605,13 +8368,13 @@
       <c r="G2" s="87" t="s">
         <v>181</v>
       </c>
-      <c r="H2" s="346" t="s">
+      <c r="H2" s="347" t="s">
         <v>180</v>
       </c>
       <c r="I2" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="J2" s="346" t="s">
+      <c r="J2" s="347" t="s">
         <v>179</v>
       </c>
     </row>
@@ -10625,11 +8388,11 @@
       <c r="G3" s="87" t="s">
         <v>159</v>
       </c>
-      <c r="H3" s="346"/>
+      <c r="H3" s="347"/>
       <c r="I3" s="87" t="s">
         <v>156</v>
       </c>
-      <c r="J3" s="346"/>
+      <c r="J3" s="347"/>
     </row>
     <row r="4" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A4" s="109"/>
@@ -10651,11 +8414,11 @@
       <c r="G4" s="87" t="s">
         <v>108</v>
       </c>
-      <c r="H4" s="346"/>
+      <c r="H4" s="347"/>
       <c r="I4" s="87" t="s">
         <v>104</v>
       </c>
-      <c r="J4" s="346"/>
+      <c r="J4" s="347"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="103" t="s">
@@ -11059,7 +8822,7 @@
       <c r="G2" s="87" t="s">
         <v>183</v>
       </c>
-      <c r="H2" s="346" t="s">
+      <c r="H2" s="347" t="s">
         <v>182</v>
       </c>
       <c r="I2" s="86" t="s">
@@ -11104,7 +8867,7 @@
       <c r="V2" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="W2" s="346" t="s">
+      <c r="W2" s="347" t="s">
         <v>180</v>
       </c>
       <c r="X2" s="87" t="s">
@@ -11119,7 +8882,7 @@
       <c r="AA2" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="AB2" s="346" t="s">
+      <c r="AB2" s="347" t="s">
         <v>179</v>
       </c>
       <c r="AC2" s="84" t="s">
@@ -11149,7 +8912,7 @@
       <c r="AK2" s="84" t="s">
         <v>178</v>
       </c>
-      <c r="AL2" s="346" t="s">
+      <c r="AL2" s="347" t="s">
         <v>177</v>
       </c>
       <c r="AM2" s="84" t="s">
@@ -11191,7 +8954,7 @@
       <c r="AY2" s="84" t="s">
         <v>176</v>
       </c>
-      <c r="AZ2" s="346" t="s">
+      <c r="AZ2" s="347" t="s">
         <v>175</v>
       </c>
       <c r="BA2" s="83" t="s">
@@ -11221,7 +8984,7 @@
       <c r="BI2" s="83" t="s">
         <v>174</v>
       </c>
-      <c r="BJ2" s="346" t="s">
+      <c r="BJ2" s="347" t="s">
         <v>173</v>
       </c>
       <c r="BK2"/>
@@ -11236,7 +8999,7 @@
       <c r="G3" s="87" t="s">
         <v>172</v>
       </c>
-      <c r="H3" s="346"/>
+      <c r="H3" s="347"/>
       <c r="I3" s="86" t="s">
         <v>171</v>
       </c>
@@ -11277,7 +9040,7 @@
       <c r="V3" s="86" t="s">
         <v>159</v>
       </c>
-      <c r="W3" s="346"/>
+      <c r="W3" s="347"/>
       <c r="X3" s="82"/>
       <c r="Y3" s="87" t="s">
         <v>158</v>
@@ -11288,7 +9051,7 @@
       <c r="AA3" s="87" t="s">
         <v>156</v>
       </c>
-      <c r="AB3" s="346"/>
+      <c r="AB3" s="347"/>
       <c r="AC3" s="84" t="s">
         <v>155</v>
       </c>
@@ -11316,7 +9079,7 @@
       <c r="AK3" s="84" t="s">
         <v>149</v>
       </c>
-      <c r="AL3" s="346"/>
+      <c r="AL3" s="347"/>
       <c r="AM3" s="84" t="s">
         <v>148</v>
       </c>
@@ -11356,7 +9119,7 @@
       <c r="AY3" s="84" t="s">
         <v>136</v>
       </c>
-      <c r="AZ3" s="346"/>
+      <c r="AZ3" s="347"/>
       <c r="BA3" s="83" t="s">
         <v>135</v>
       </c>
@@ -11384,7 +9147,7 @@
       <c r="BI3" s="83" t="s">
         <v>127</v>
       </c>
-      <c r="BJ3" s="346"/>
+      <c r="BJ3" s="347"/>
     </row>
     <row r="4" spans="1:63" s="44" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="89"/>
@@ -11406,7 +9169,7 @@
       <c r="G4" s="87" t="s">
         <v>122</v>
       </c>
-      <c r="H4" s="346"/>
+      <c r="H4" s="347"/>
       <c r="I4" s="86" t="s">
         <v>121</v>
       </c>
@@ -11449,7 +9212,7 @@
       <c r="V4" s="86" t="s">
         <v>108</v>
       </c>
-      <c r="W4" s="346"/>
+      <c r="W4" s="347"/>
       <c r="X4" s="85" t="s">
         <v>107</v>
       </c>
@@ -11462,7 +9225,7 @@
       <c r="AA4" s="85" t="s">
         <v>104</v>
       </c>
-      <c r="AB4" s="346"/>
+      <c r="AB4" s="347"/>
       <c r="AC4" s="84" t="s">
         <v>103</v>
       </c>
@@ -11490,7 +9253,7 @@
       <c r="AK4" s="84" t="s">
         <v>96</v>
       </c>
-      <c r="AL4" s="346"/>
+      <c r="AL4" s="347"/>
       <c r="AM4" s="84" t="s">
         <v>95</v>
       </c>
@@ -11530,7 +9293,7 @@
       <c r="AY4" s="84" t="s">
         <v>83</v>
       </c>
-      <c r="AZ4" s="346"/>
+      <c r="AZ4" s="347"/>
       <c r="BA4" s="83" t="s">
         <v>82</v>
       </c>
@@ -11558,7 +9321,7 @@
       <c r="BI4" s="83" t="s">
         <v>74</v>
       </c>
-      <c r="BJ4" s="346"/>
+      <c r="BJ4" s="347"/>
       <c r="BK4"/>
     </row>
     <row r="5" spans="1:63" s="44" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -14308,7 +12071,7 @@
       <c r="G2" s="87" t="s">
         <v>183</v>
       </c>
-      <c r="H2" s="346" t="s">
+      <c r="H2" s="347" t="s">
         <v>182</v>
       </c>
       <c r="I2" s="87" t="s">
@@ -14341,13 +12104,13 @@
       <c r="R2" s="87" t="s">
         <v>181</v>
       </c>
-      <c r="S2" s="346" t="s">
+      <c r="S2" s="347" t="s">
         <v>180</v>
       </c>
       <c r="T2" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="U2" s="346" t="s">
+      <c r="U2" s="347" t="s">
         <v>179</v>
       </c>
       <c r="V2" s="87" t="s">
@@ -14377,7 +12140,7 @@
       <c r="AD2" s="87" t="s">
         <v>178</v>
       </c>
-      <c r="AE2" s="346" t="s">
+      <c r="AE2" s="347" t="s">
         <v>227</v>
       </c>
       <c r="AF2" s="87" t="s">
@@ -14389,7 +12152,7 @@
       <c r="AH2" s="87" t="s">
         <v>226</v>
       </c>
-      <c r="AI2" s="346" t="s">
+      <c r="AI2" s="347" t="s">
         <v>225</v>
       </c>
     </row>
@@ -14403,7 +12166,7 @@
       <c r="G3" s="87" t="s">
         <v>172</v>
       </c>
-      <c r="H3" s="346"/>
+      <c r="H3" s="347"/>
       <c r="I3" s="87" t="s">
         <v>224</v>
       </c>
@@ -14434,11 +12197,11 @@
       <c r="R3" s="87" t="s">
         <v>159</v>
       </c>
-      <c r="S3" s="346"/>
+      <c r="S3" s="347"/>
       <c r="T3" s="87" t="s">
         <v>156</v>
       </c>
-      <c r="U3" s="346"/>
+      <c r="U3" s="347"/>
       <c r="V3" s="87" t="s">
         <v>215</v>
       </c>
@@ -14466,7 +12229,7 @@
       <c r="AD3" s="87" t="s">
         <v>207</v>
       </c>
-      <c r="AE3" s="346"/>
+      <c r="AE3" s="347"/>
       <c r="AF3" s="87" t="s">
         <v>206</v>
       </c>
@@ -14476,7 +12239,7 @@
       <c r="AH3" s="87" t="s">
         <v>136</v>
       </c>
-      <c r="AI3" s="346"/>
+      <c r="AI3" s="347"/>
     </row>
     <row r="4" spans="1:62" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="90"/>
@@ -14498,7 +12261,7 @@
       <c r="G4" s="87" t="s">
         <v>122</v>
       </c>
-      <c r="H4" s="346"/>
+      <c r="H4" s="347"/>
       <c r="I4" s="87" t="s">
         <v>205</v>
       </c>
@@ -14529,11 +12292,11 @@
       <c r="R4" s="87" t="s">
         <v>108</v>
       </c>
-      <c r="S4" s="346"/>
+      <c r="S4" s="347"/>
       <c r="T4" s="87" t="s">
         <v>104</v>
       </c>
-      <c r="U4" s="346"/>
+      <c r="U4" s="347"/>
       <c r="V4" s="87" t="s">
         <v>196</v>
       </c>
@@ -14561,7 +12324,7 @@
       <c r="AD4" s="87" t="s">
         <v>188</v>
       </c>
-      <c r="AE4" s="346"/>
+      <c r="AE4" s="347"/>
       <c r="AF4" s="87" t="s">
         <v>187</v>
       </c>
@@ -14571,7 +12334,7 @@
       <c r="AH4" s="87" t="s">
         <v>83</v>
       </c>
-      <c r="AI4" s="346"/>
+      <c r="AI4" s="347"/>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A5" s="93" t="s">
@@ -16328,13 +14091,13 @@
       <c r="G2" s="87" t="s">
         <v>181</v>
       </c>
-      <c r="H2" s="346" t="s">
+      <c r="H2" s="347" t="s">
         <v>180</v>
       </c>
       <c r="I2" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="J2" s="346" t="s">
+      <c r="J2" s="347" t="s">
         <v>179</v>
       </c>
     </row>
@@ -16348,11 +14111,11 @@
       <c r="G3" s="87" t="s">
         <v>159</v>
       </c>
-      <c r="H3" s="346"/>
+      <c r="H3" s="347"/>
       <c r="I3" s="87" t="s">
         <v>156</v>
       </c>
-      <c r="J3" s="346"/>
+      <c r="J3" s="347"/>
     </row>
     <row r="4" spans="1:62" ht="36" x14ac:dyDescent="0.2">
       <c r="A4" s="109"/>
@@ -16374,11 +14137,11 @@
       <c r="G4" s="87" t="s">
         <v>108</v>
       </c>
-      <c r="H4" s="346"/>
+      <c r="H4" s="347"/>
       <c r="I4" s="87" t="s">
         <v>104</v>
       </c>
-      <c r="J4" s="346"/>
+      <c r="J4" s="347"/>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A5" s="103" t="s">
@@ -16773,13 +14536,13 @@
   <sheetData>
     <row r="1" spans="1:61" s="168" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="167"/>
-      <c r="B1" s="350" t="s">
+      <c r="B1" s="351" t="s">
         <v>184</v>
       </c>
-      <c r="C1" s="350"/>
-      <c r="D1" s="350"/>
-      <c r="E1" s="350"/>
-      <c r="F1" s="350"/>
+      <c r="C1" s="351"/>
+      <c r="D1" s="351"/>
+      <c r="E1" s="351"/>
+      <c r="F1" s="351"/>
       <c r="G1" s="169"/>
       <c r="H1" s="169"/>
       <c r="I1" s="169"/>
@@ -16824,7 +14587,7 @@
       <c r="O2" s="171" t="s">
         <v>178</v>
       </c>
-      <c r="P2" s="349" t="s">
+      <c r="P2" s="350" t="s">
         <v>177</v>
       </c>
       <c r="Q2" s="171" t="s">
@@ -16866,7 +14629,7 @@
       <c r="AC2" s="171" t="s">
         <v>176</v>
       </c>
-      <c r="AD2" s="349" t="s">
+      <c r="AD2" s="350" t="s">
         <v>175</v>
       </c>
       <c r="AE2" s="172" t="s">
@@ -16896,7 +14659,7 @@
       <c r="AM2" s="172" t="s">
         <v>174</v>
       </c>
-      <c r="AN2" s="349" t="s">
+      <c r="AN2" s="350" t="s">
         <v>173</v>
       </c>
       <c r="AQ2" s="171"/>
@@ -16907,7 +14670,7 @@
       <c r="AV2" s="171"/>
       <c r="AW2" s="171"/>
       <c r="AX2" s="171"/>
-      <c r="AY2" s="349"/>
+      <c r="AY2" s="350"/>
       <c r="AZ2" s="172"/>
       <c r="BA2" s="172"/>
       <c r="BB2" s="172"/>
@@ -16917,7 +14680,7 @@
       <c r="BF2" s="172"/>
       <c r="BG2" s="172"/>
       <c r="BH2" s="172"/>
-      <c r="BI2" s="349"/>
+      <c r="BI2" s="350"/>
     </row>
     <row r="3" spans="1:61" s="168" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="170"/>
@@ -16953,7 +14716,7 @@
       <c r="O3" s="171" t="s">
         <v>149</v>
       </c>
-      <c r="P3" s="349"/>
+      <c r="P3" s="350"/>
       <c r="Q3" s="171" t="s">
         <v>148</v>
       </c>
@@ -16993,7 +14756,7 @@
       <c r="AC3" s="171" t="s">
         <v>136</v>
       </c>
-      <c r="AD3" s="349"/>
+      <c r="AD3" s="350"/>
       <c r="AE3" s="172" t="s">
         <v>135</v>
       </c>
@@ -17021,7 +14784,7 @@
       <c r="AM3" s="172" t="s">
         <v>127</v>
       </c>
-      <c r="AN3" s="349"/>
+      <c r="AN3" s="350"/>
       <c r="AQ3" s="171"/>
       <c r="AR3" s="171"/>
       <c r="AS3" s="171"/>
@@ -17030,7 +14793,7 @@
       <c r="AV3" s="171"/>
       <c r="AW3" s="171"/>
       <c r="AX3" s="171"/>
-      <c r="AY3" s="349"/>
+      <c r="AY3" s="350"/>
       <c r="AZ3" s="172"/>
       <c r="BA3" s="172"/>
       <c r="BB3" s="172"/>
@@ -17040,7 +14803,7 @@
       <c r="BF3" s="172"/>
       <c r="BG3" s="172"/>
       <c r="BH3" s="172"/>
-      <c r="BI3" s="349"/>
+      <c r="BI3" s="350"/>
     </row>
     <row r="4" spans="1:61" s="168" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="173"/>
@@ -17086,7 +14849,7 @@
       <c r="O4" s="171" t="s">
         <v>96</v>
       </c>
-      <c r="P4" s="349"/>
+      <c r="P4" s="350"/>
       <c r="Q4" s="171" t="s">
         <v>95</v>
       </c>
@@ -17126,7 +14889,7 @@
       <c r="AC4" s="171" t="s">
         <v>83</v>
       </c>
-      <c r="AD4" s="349"/>
+      <c r="AD4" s="350"/>
       <c r="AE4" s="172" t="s">
         <v>82</v>
       </c>
@@ -17154,7 +14917,7 @@
       <c r="AM4" s="172" t="s">
         <v>74</v>
       </c>
-      <c r="AN4" s="349"/>
+      <c r="AN4" s="350"/>
       <c r="AQ4" s="171"/>
       <c r="AR4" s="171"/>
       <c r="AS4" s="171"/>
@@ -17163,7 +14926,7 @@
       <c r="AV4" s="171"/>
       <c r="AW4" s="171"/>
       <c r="AX4" s="171"/>
-      <c r="AY4" s="349"/>
+      <c r="AY4" s="350"/>
       <c r="AZ4" s="172"/>
       <c r="BA4" s="172"/>
       <c r="BB4" s="172"/>
@@ -17173,7 +14936,7 @@
       <c r="BF4" s="172"/>
       <c r="BG4" s="172"/>
       <c r="BH4" s="172"/>
-      <c r="BI4" s="349"/>
+      <c r="BI4" s="350"/>
     </row>
     <row r="5" spans="1:61" s="168" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="175" t="s">
@@ -18900,14 +16663,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="351" t="s">
+      <c r="A1" s="352" t="s">
         <v>228</v>
       </c>
-      <c r="B1" s="351"/>
-      <c r="C1" s="351"/>
-      <c r="D1" s="351"/>
-      <c r="E1" s="351"/>
-      <c r="F1" s="351"/>
+      <c r="B1" s="352"/>
+      <c r="C1" s="352"/>
+      <c r="D1" s="352"/>
+      <c r="E1" s="352"/>
+      <c r="F1" s="352"/>
       <c r="G1" s="200"/>
       <c r="H1" s="200"/>
       <c r="I1" s="200"/>
@@ -18957,7 +16720,7 @@
       <c r="O2" s="203" t="s">
         <v>178</v>
       </c>
-      <c r="P2" s="352" t="s">
+      <c r="P2" s="353" t="s">
         <v>227</v>
       </c>
       <c r="Q2" s="203" t="s">
@@ -18969,7 +16732,7 @@
       <c r="S2" s="203" t="s">
         <v>226</v>
       </c>
-      <c r="T2" s="352" t="s">
+      <c r="T2" s="353" t="s">
         <v>225</v>
       </c>
     </row>
@@ -19007,7 +16770,7 @@
       <c r="O3" s="203" t="s">
         <v>207</v>
       </c>
-      <c r="P3" s="352"/>
+      <c r="P3" s="353"/>
       <c r="Q3" s="203" t="s">
         <v>206</v>
       </c>
@@ -19017,7 +16780,7 @@
       <c r="S3" s="203" t="s">
         <v>136</v>
       </c>
-      <c r="T3" s="352"/>
+      <c r="T3" s="353"/>
     </row>
     <row r="4" spans="1:20" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="202"/>
@@ -19063,7 +16826,7 @@
       <c r="O4" s="203" t="s">
         <v>188</v>
       </c>
-      <c r="P4" s="352"/>
+      <c r="P4" s="353"/>
       <c r="Q4" s="203" t="s">
         <v>187</v>
       </c>
@@ -19073,7 +16836,7 @@
       <c r="S4" s="203" t="s">
         <v>83</v>
       </c>
-      <c r="T4" s="352"/>
+      <c r="T4" s="353"/>
     </row>
     <row r="5" spans="1:20" ht="317" x14ac:dyDescent="0.2">
       <c r="A5" s="206" t="s">
@@ -19664,16 +17427,16 @@
   <sheetData>
     <row r="1" spans="1:28" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="226"/>
-      <c r="B1" s="354" t="s">
+      <c r="B1" s="355" t="s">
         <v>184</v>
       </c>
-      <c r="C1" s="354"/>
-      <c r="D1" s="354"/>
-      <c r="E1" s="354"/>
-      <c r="F1" s="354"/>
-      <c r="G1" s="354"/>
-      <c r="H1" s="354"/>
-      <c r="I1" s="354"/>
+      <c r="C1" s="355"/>
+      <c r="D1" s="355"/>
+      <c r="E1" s="355"/>
+      <c r="F1" s="355"/>
+      <c r="G1" s="355"/>
+      <c r="H1" s="355"/>
+      <c r="I1" s="355"/>
       <c r="J1" s="223"/>
       <c r="K1" s="223"/>
       <c r="L1" s="223"/>
@@ -19704,7 +17467,7 @@
       <c r="G2" s="225" t="s">
         <v>183</v>
       </c>
-      <c r="H2" s="353" t="s">
+      <c r="H2" s="354" t="s">
         <v>182</v>
       </c>
       <c r="I2" s="228" t="s">
@@ -19749,7 +17512,7 @@
       <c r="V2" s="228" t="s">
         <v>181</v>
       </c>
-      <c r="W2" s="353" t="s">
+      <c r="W2" s="354" t="s">
         <v>180</v>
       </c>
       <c r="X2" s="225" t="s">
@@ -19764,7 +17527,7 @@
       <c r="AA2" s="225" t="s">
         <v>45</v>
       </c>
-      <c r="AB2" s="353" t="s">
+      <c r="AB2" s="354" t="s">
         <v>179</v>
       </c>
     </row>
@@ -19778,7 +17541,7 @@
       <c r="G3" s="225" t="s">
         <v>172</v>
       </c>
-      <c r="H3" s="353"/>
+      <c r="H3" s="354"/>
       <c r="I3" s="228" t="s">
         <v>171</v>
       </c>
@@ -19819,7 +17582,7 @@
       <c r="V3" s="228" t="s">
         <v>159</v>
       </c>
-      <c r="W3" s="353"/>
+      <c r="W3" s="354"/>
       <c r="X3" s="227"/>
       <c r="Y3" s="225" t="s">
         <v>158</v>
@@ -19830,7 +17593,7 @@
       <c r="AA3" s="225" t="s">
         <v>156</v>
       </c>
-      <c r="AB3" s="353"/>
+      <c r="AB3" s="354"/>
     </row>
     <row r="4" spans="1:28" ht="98" x14ac:dyDescent="0.2">
       <c r="A4" s="229"/>
@@ -19852,7 +17615,7 @@
       <c r="G4" s="225" t="s">
         <v>122</v>
       </c>
-      <c r="H4" s="353"/>
+      <c r="H4" s="354"/>
       <c r="I4" s="228" t="s">
         <v>121</v>
       </c>
@@ -19895,7 +17658,7 @@
       <c r="V4" s="231" t="s">
         <v>108</v>
       </c>
-      <c r="W4" s="353"/>
+      <c r="W4" s="354"/>
       <c r="X4" s="232" t="s">
         <v>107</v>
       </c>
@@ -19908,7 +17671,7 @@
       <c r="AA4" s="232" t="s">
         <v>104</v>
       </c>
-      <c r="AB4" s="353"/>
+      <c r="AB4" s="354"/>
     </row>
     <row r="5" spans="1:28" ht="196" x14ac:dyDescent="0.2">
       <c r="A5" s="233" t="s">
@@ -20807,16 +18570,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="356" t="s">
+      <c r="A1" s="357" t="s">
         <v>228</v>
       </c>
-      <c r="B1" s="356"/>
-      <c r="C1" s="356"/>
-      <c r="D1" s="356"/>
-      <c r="E1" s="356"/>
-      <c r="F1" s="356"/>
-      <c r="G1" s="356"/>
-      <c r="H1" s="356"/>
+      <c r="B1" s="357"/>
+      <c r="C1" s="357"/>
+      <c r="D1" s="357"/>
+      <c r="E1" s="357"/>
+      <c r="F1" s="357"/>
+      <c r="G1" s="357"/>
+      <c r="H1" s="357"/>
       <c r="I1" s="273"/>
       <c r="J1" s="273"/>
       <c r="K1" s="273"/>
@@ -20841,7 +18604,7 @@
       <c r="G2" s="275" t="s">
         <v>183</v>
       </c>
-      <c r="H2" s="355" t="s">
+      <c r="H2" s="356" t="s">
         <v>182</v>
       </c>
       <c r="I2" s="275" t="s">
@@ -20874,13 +18637,13 @@
       <c r="R2" s="275" t="s">
         <v>181</v>
       </c>
-      <c r="S2" s="355" t="s">
+      <c r="S2" s="356" t="s">
         <v>180</v>
       </c>
       <c r="T2" s="275" t="s">
         <v>45</v>
       </c>
-      <c r="U2" s="355" t="s">
+      <c r="U2" s="356" t="s">
         <v>179</v>
       </c>
     </row>
@@ -20894,7 +18657,7 @@
       <c r="G3" s="275" t="s">
         <v>172</v>
       </c>
-      <c r="H3" s="355"/>
+      <c r="H3" s="356"/>
       <c r="I3" s="275" t="s">
         <v>224</v>
       </c>
@@ -20925,11 +18688,11 @@
       <c r="R3" s="275" t="s">
         <v>159</v>
       </c>
-      <c r="S3" s="355"/>
+      <c r="S3" s="356"/>
       <c r="T3" s="275" t="s">
         <v>156</v>
       </c>
-      <c r="U3" s="355"/>
+      <c r="U3" s="356"/>
     </row>
     <row r="4" spans="1:21" ht="112" x14ac:dyDescent="0.2">
       <c r="A4" s="272"/>
@@ -20951,7 +18714,7 @@
       <c r="G4" s="275" t="s">
         <v>122</v>
       </c>
-      <c r="H4" s="355"/>
+      <c r="H4" s="356"/>
       <c r="I4" s="275" t="s">
         <v>205</v>
       </c>
@@ -20982,11 +18745,11 @@
       <c r="R4" s="275" t="s">
         <v>108</v>
       </c>
-      <c r="S4" s="355"/>
+      <c r="S4" s="356"/>
       <c r="T4" s="275" t="s">
         <v>104</v>
       </c>
-      <c r="U4" s="355"/>
+      <c r="U4" s="356"/>
     </row>
     <row r="5" spans="1:21" ht="196" x14ac:dyDescent="0.2">
       <c r="A5" s="278" t="s">
@@ -21682,13 +19445,13 @@
       <c r="K2" s="203" t="s">
         <v>181</v>
       </c>
-      <c r="L2" s="352" t="s">
+      <c r="L2" s="353" t="s">
         <v>180</v>
       </c>
       <c r="M2" s="203" t="s">
         <v>45</v>
       </c>
-      <c r="N2" s="352" t="s">
+      <c r="N2" s="353" t="s">
         <v>179</v>
       </c>
     </row>
@@ -21706,11 +19469,11 @@
       <c r="K3" s="203" t="s">
         <v>159</v>
       </c>
-      <c r="L3" s="352"/>
+      <c r="L3" s="353"/>
       <c r="M3" s="203" t="s">
         <v>156</v>
       </c>
-      <c r="N3" s="352"/>
+      <c r="N3" s="353"/>
     </row>
     <row r="4" spans="1:14" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="256"/>
@@ -21736,11 +19499,11 @@
       <c r="K4" s="203" t="s">
         <v>108</v>
       </c>
-      <c r="L4" s="352"/>
+      <c r="L4" s="353"/>
       <c r="M4" s="203" t="s">
         <v>104</v>
       </c>
-      <c r="N4" s="352"/>
+      <c r="N4" s="353"/>
     </row>
     <row r="5" spans="1:14" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="258"/>
@@ -22431,17 +20194,17 @@
       <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="FA1" s="338" t="s">
+      <c r="FA1" s="339" t="s">
         <v>237</v>
       </c>
-      <c r="FB1" s="338"/>
-      <c r="FC1" s="338"/>
-      <c r="FD1" s="338"/>
-      <c r="FE1" s="338"/>
-      <c r="FF1" s="338"/>
-      <c r="FG1" s="339"/>
-      <c r="FH1" s="339"/>
-      <c r="FI1" s="339"/>
+      <c r="FB1" s="339"/>
+      <c r="FC1" s="339"/>
+      <c r="FD1" s="339"/>
+      <c r="FE1" s="339"/>
+      <c r="FF1" s="339"/>
+      <c r="FG1" s="340"/>
+      <c r="FH1" s="340"/>
+      <c r="FI1" s="340"/>
       <c r="FJ1" s="4" t="s">
         <v>0</v>
       </c>
@@ -22507,8 +20270,8 @@
   </sheetPr>
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -22587,28 +20350,28 @@
       <c r="D4" s="294"/>
       <c r="E4" s="294"/>
       <c r="F4" s="294"/>
-      <c r="G4" s="340" t="s">
+      <c r="G4" s="341" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="341"/>
-      <c r="I4" s="341"/>
-      <c r="J4" s="341"/>
-      <c r="K4" s="341"/>
-      <c r="L4" s="342"/>
-      <c r="M4" s="343"/>
-      <c r="N4" s="344" t="s">
+      <c r="H4" s="342"/>
+      <c r="I4" s="342"/>
+      <c r="J4" s="342"/>
+      <c r="K4" s="342"/>
+      <c r="L4" s="343"/>
+      <c r="M4" s="344"/>
+      <c r="N4" s="345" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="342"/>
-      <c r="P4" s="342"/>
-      <c r="Q4" s="342"/>
-      <c r="R4" s="342"/>
-      <c r="S4" s="342"/>
-      <c r="T4" s="345"/>
-      <c r="U4" s="340" t="s">
+      <c r="O4" s="343"/>
+      <c r="P4" s="343"/>
+      <c r="Q4" s="343"/>
+      <c r="R4" s="343"/>
+      <c r="S4" s="343"/>
+      <c r="T4" s="346"/>
+      <c r="U4" s="341" t="s">
         <v>28</v>
       </c>
-      <c r="V4" s="343"/>
+      <c r="V4" s="344"/>
       <c r="W4" s="301"/>
       <c r="X4" t="s">
         <v>0</v>
@@ -22671,7 +20434,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
       <c r="C6" s="17" t="s">
         <v>23</v>
@@ -22682,7 +20445,7 @@
       <c r="E6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="319" t="s">
         <v>399</v>
       </c>
       <c r="G6" s="19" t="e">
@@ -22805,70 +20568,70 @@
     <mergeCell ref="U4:V4"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:F4">
-    <cfRule type="expression" dxfId="31" priority="16">
+    <cfRule type="expression" dxfId="15" priority="16">
       <formula>IF(LEFT($A$3,2)&lt;&gt;"TJ",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:V151">
-    <cfRule type="expression" dxfId="30" priority="18">
+    <cfRule type="expression" dxfId="14" priority="18">
       <formula>AND(ISBLANK($C6)=FALSE,ISBLANK($E6)=TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:F1048576">
-    <cfRule type="expression" dxfId="16" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="1" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($U1)-(_xlfn.NUMBERVALUE($U2)+_xlfn.NUMBERVALUE($U3)+_xlfn.NUMBERVALUE($U4)+_xlfn.NUMBERVALUE($U5)+_xlfn.NUMBERVALUE($U6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="2" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($S1)-(_xlfn.NUMBERVALUE($S2)+_xlfn.NUMBERVALUE($S3)+_xlfn.NUMBERVALUE($S4)+_xlfn.NUMBERVALUE($S5)+_xlfn.NUMBERVALUE($S6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="7" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3)+_xlfn.NUMBERVALUE($L4)-_xlfn.NUMBERVALUE($L5)+_xlfn.NUMBERVALUE($L6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="12" stopIfTrue="1">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",OR(_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3))&lt;&gt;0,_xlfn.NUMBERVALUE($S1)-(_xlfn.NUMBERVALUE($S2)+_xlfn.NUMBERVALUE($S3))&lt;&gt;0,_xlfn.NUMBERVALUE($U1)-(_xlfn.NUMBERVALUE($U2)+_xlfn.NUMBERVALUE($U3))&lt;&gt;0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:F7">
-    <cfRule type="expression" dxfId="29" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="6" stopIfTrue="1">
       <formula>OR(_xlfn.NUMBERVALUE($L7)&lt;&gt;_xlfn.NUMBERVALUE($L6),_xlfn.NUMBERVALUE($S7)&lt;&gt;_xlfn.NUMBERVALUE($S6),_xlfn.NUMBERVALUE($U7)&lt;&gt;_xlfn.NUMBERVALUE($U6))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:M1048576">
-    <cfRule type="expression" dxfId="28" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="11" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3)+_xlfn.NUMBERVALUE($L4)+_xlfn.NUMBERVALUE($L5)+_xlfn.NUMBERVALUE($L6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="15">
+    <cfRule type="expression" dxfId="7" priority="15">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3))&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:M7">
-    <cfRule type="expression" dxfId="26" priority="5">
+    <cfRule type="expression" dxfId="6" priority="5">
       <formula>_xlfn.NUMBERVALUE($L7)&lt;&gt;_xlfn.NUMBERVALUE($L6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:T1048576">
-    <cfRule type="expression" dxfId="25" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="10" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($S1)-(_xlfn.NUMBERVALUE($S2)+_xlfn.NUMBERVALUE($S3)+_xlfn.NUMBERVALUE($S4)+_xlfn.NUMBERVALUE($S5)+_xlfn.NUMBERVALUE($S6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="14">
+    <cfRule type="expression" dxfId="4" priority="14">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",_xlfn.NUMBERVALUE($S1)-(_xlfn.NUMBERVALUE($S2)+_xlfn.NUMBERVALUE($S3))&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7:T7">
-    <cfRule type="expression" dxfId="23" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>_xlfn.NUMBERVALUE($S7)&lt;&gt;_xlfn.NUMBERVALUE($S6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:V1048576">
-    <cfRule type="expression" dxfId="22" priority="9">
+    <cfRule type="expression" dxfId="2" priority="9">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($U1)-(_xlfn.NUMBERVALUE($U2)+_xlfn.NUMBERVALUE($U3)+_xlfn.NUMBERVALUE($U4)+_xlfn.NUMBERVALUE($U5)+_xlfn.NUMBERVALUE($U6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="13">
+    <cfRule type="expression" dxfId="1" priority="13">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",_xlfn.NUMBERVALUE($U1)-(_xlfn.NUMBERVALUE($U2)+_xlfn.NUMBERVALUE($U3))&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U7:V7">
-    <cfRule type="expression" dxfId="20" priority="3">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>_xlfn.NUMBERVALUE($U7)&lt;&gt;_xlfn.NUMBERVALUE($U6)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23269,16 +21032,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" s="44" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B1" s="347" t="s">
+      <c r="B1" s="348" t="s">
         <v>184</v>
       </c>
-      <c r="C1" s="347"/>
-      <c r="D1" s="347"/>
-      <c r="E1" s="347"/>
-      <c r="F1" s="347"/>
-      <c r="G1" s="347"/>
-      <c r="H1" s="347"/>
-      <c r="I1" s="347"/>
+      <c r="C1" s="348"/>
+      <c r="D1" s="348"/>
+      <c r="E1" s="348"/>
+      <c r="F1" s="348"/>
+      <c r="G1" s="348"/>
+      <c r="H1" s="348"/>
+      <c r="I1" s="348"/>
     </row>
     <row r="2" spans="1:62" s="44" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="90"/>
@@ -23290,7 +21053,7 @@
       <c r="G2" s="87" t="s">
         <v>183</v>
       </c>
-      <c r="H2" s="346" t="s">
+      <c r="H2" s="347" t="s">
         <v>182</v>
       </c>
       <c r="I2" s="86" t="s">
@@ -23335,7 +21098,7 @@
       <c r="V2" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="W2" s="346" t="s">
+      <c r="W2" s="347" t="s">
         <v>180</v>
       </c>
       <c r="X2" s="87" t="s">
@@ -23350,7 +21113,7 @@
       <c r="AA2" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="AB2" s="346" t="s">
+      <c r="AB2" s="347" t="s">
         <v>179</v>
       </c>
       <c r="AC2" s="84" t="s">
@@ -23380,7 +21143,7 @@
       <c r="AK2" s="84" t="s">
         <v>178</v>
       </c>
-      <c r="AL2" s="346" t="s">
+      <c r="AL2" s="347" t="s">
         <v>177</v>
       </c>
       <c r="AM2" s="84" t="s">
@@ -23422,7 +21185,7 @@
       <c r="AY2" s="84" t="s">
         <v>176</v>
       </c>
-      <c r="AZ2" s="346" t="s">
+      <c r="AZ2" s="347" t="s">
         <v>175</v>
       </c>
       <c r="BA2" s="83" t="s">
@@ -23452,7 +21215,7 @@
       <c r="BI2" s="83" t="s">
         <v>174</v>
       </c>
-      <c r="BJ2" s="346" t="s">
+      <c r="BJ2" s="347" t="s">
         <v>173</v>
       </c>
     </row>
@@ -23466,7 +21229,7 @@
       <c r="G3" s="87" t="s">
         <v>172</v>
       </c>
-      <c r="H3" s="346"/>
+      <c r="H3" s="347"/>
       <c r="I3" s="86" t="s">
         <v>171</v>
       </c>
@@ -23507,7 +21270,7 @@
       <c r="V3" s="86" t="s">
         <v>159</v>
       </c>
-      <c r="W3" s="346"/>
+      <c r="W3" s="347"/>
       <c r="X3" s="82"/>
       <c r="Y3" s="87" t="s">
         <v>158</v>
@@ -23518,7 +21281,7 @@
       <c r="AA3" s="87" t="s">
         <v>156</v>
       </c>
-      <c r="AB3" s="346"/>
+      <c r="AB3" s="347"/>
       <c r="AC3" s="84" t="s">
         <v>155</v>
       </c>
@@ -23546,7 +21309,7 @@
       <c r="AK3" s="84" t="s">
         <v>149</v>
       </c>
-      <c r="AL3" s="346"/>
+      <c r="AL3" s="347"/>
       <c r="AM3" s="84" t="s">
         <v>148</v>
       </c>
@@ -23586,7 +21349,7 @@
       <c r="AY3" s="84" t="s">
         <v>136</v>
       </c>
-      <c r="AZ3" s="346"/>
+      <c r="AZ3" s="347"/>
       <c r="BA3" s="83" t="s">
         <v>135</v>
       </c>
@@ -23614,7 +21377,7 @@
       <c r="BI3" s="83" t="s">
         <v>127</v>
       </c>
-      <c r="BJ3" s="346"/>
+      <c r="BJ3" s="347"/>
     </row>
     <row r="4" spans="1:62" s="44" customFormat="1" ht="60" x14ac:dyDescent="0.15">
       <c r="A4" s="89"/>
@@ -23636,7 +21399,7 @@
       <c r="G4" s="87" t="s">
         <v>122</v>
       </c>
-      <c r="H4" s="346"/>
+      <c r="H4" s="347"/>
       <c r="I4" s="86" t="s">
         <v>121</v>
       </c>
@@ -23679,7 +21442,7 @@
       <c r="V4" s="86" t="s">
         <v>108</v>
       </c>
-      <c r="W4" s="346"/>
+      <c r="W4" s="347"/>
       <c r="X4" s="85" t="s">
         <v>107</v>
       </c>
@@ -23692,7 +21455,7 @@
       <c r="AA4" s="85" t="s">
         <v>104</v>
       </c>
-      <c r="AB4" s="346"/>
+      <c r="AB4" s="347"/>
       <c r="AC4" s="84" t="s">
         <v>103</v>
       </c>
@@ -23720,7 +21483,7 @@
       <c r="AK4" s="84" t="s">
         <v>96</v>
       </c>
-      <c r="AL4" s="346"/>
+      <c r="AL4" s="347"/>
       <c r="AM4" s="84" t="s">
         <v>95</v>
       </c>
@@ -23760,7 +21523,7 @@
       <c r="AY4" s="84" t="s">
         <v>83</v>
       </c>
-      <c r="AZ4" s="346"/>
+      <c r="AZ4" s="347"/>
       <c r="BA4" s="83" t="s">
         <v>82</v>
       </c>
@@ -23788,7 +21551,7 @@
       <c r="BI4" s="83" t="s">
         <v>74</v>
       </c>
-      <c r="BJ4" s="346"/>
+      <c r="BJ4" s="347"/>
     </row>
     <row r="5" spans="1:62" s="44" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="54" t="s">
@@ -25985,16 +23748,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A1" s="348" t="s">
+      <c r="A1" s="349" t="s">
         <v>228</v>
       </c>
-      <c r="B1" s="348"/>
-      <c r="C1" s="348"/>
-      <c r="D1" s="348"/>
-      <c r="E1" s="348"/>
-      <c r="F1" s="348"/>
-      <c r="G1" s="348"/>
-      <c r="H1" s="348"/>
+      <c r="B1" s="349"/>
+      <c r="C1" s="349"/>
+      <c r="D1" s="349"/>
+      <c r="E1" s="349"/>
+      <c r="F1" s="349"/>
+      <c r="G1" s="349"/>
+      <c r="H1" s="349"/>
       <c r="I1" s="44"/>
       <c r="J1" s="44"/>
       <c r="K1" s="44"/>
@@ -26033,7 +23796,7 @@
       <c r="G2" s="87" t="s">
         <v>183</v>
       </c>
-      <c r="H2" s="346" t="s">
+      <c r="H2" s="347" t="s">
         <v>182</v>
       </c>
       <c r="I2" s="87" t="s">
@@ -26066,13 +23829,13 @@
       <c r="R2" s="87" t="s">
         <v>181</v>
       </c>
-      <c r="S2" s="346" t="s">
+      <c r="S2" s="347" t="s">
         <v>180</v>
       </c>
       <c r="T2" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="U2" s="346" t="s">
+      <c r="U2" s="347" t="s">
         <v>179</v>
       </c>
       <c r="V2" s="87" t="s">
@@ -26102,7 +23865,7 @@
       <c r="AD2" s="87" t="s">
         <v>178</v>
       </c>
-      <c r="AE2" s="346" t="s">
+      <c r="AE2" s="347" t="s">
         <v>227</v>
       </c>
       <c r="AF2" s="87" t="s">
@@ -26114,7 +23877,7 @@
       <c r="AH2" s="87" t="s">
         <v>226</v>
       </c>
-      <c r="AI2" s="346" t="s">
+      <c r="AI2" s="347" t="s">
         <v>225</v>
       </c>
     </row>
@@ -26128,7 +23891,7 @@
       <c r="G3" s="87" t="s">
         <v>172</v>
       </c>
-      <c r="H3" s="346"/>
+      <c r="H3" s="347"/>
       <c r="I3" s="87" t="s">
         <v>224</v>
       </c>
@@ -26159,11 +23922,11 @@
       <c r="R3" s="87" t="s">
         <v>159</v>
       </c>
-      <c r="S3" s="346"/>
+      <c r="S3" s="347"/>
       <c r="T3" s="87" t="s">
         <v>156</v>
       </c>
-      <c r="U3" s="346"/>
+      <c r="U3" s="347"/>
       <c r="V3" s="87" t="s">
         <v>215</v>
       </c>
@@ -26191,7 +23954,7 @@
       <c r="AD3" s="87" t="s">
         <v>207</v>
       </c>
-      <c r="AE3" s="346"/>
+      <c r="AE3" s="347"/>
       <c r="AF3" s="87" t="s">
         <v>206</v>
       </c>
@@ -26201,7 +23964,7 @@
       <c r="AH3" s="87" t="s">
         <v>136</v>
       </c>
-      <c r="AI3" s="346"/>
+      <c r="AI3" s="347"/>
     </row>
     <row r="4" spans="1:35" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="90"/>
@@ -26223,7 +23986,7 @@
       <c r="G4" s="87" t="s">
         <v>122</v>
       </c>
-      <c r="H4" s="346"/>
+      <c r="H4" s="347"/>
       <c r="I4" s="87" t="s">
         <v>205</v>
       </c>
@@ -26254,11 +24017,11 @@
       <c r="R4" s="87" t="s">
         <v>108</v>
       </c>
-      <c r="S4" s="346"/>
+      <c r="S4" s="347"/>
       <c r="T4" s="87" t="s">
         <v>104</v>
       </c>
-      <c r="U4" s="346"/>
+      <c r="U4" s="347"/>
       <c r="V4" s="87" t="s">
         <v>196</v>
       </c>
@@ -26286,7 +24049,7 @@
       <c r="AD4" s="87" t="s">
         <v>188</v>
       </c>
-      <c r="AE4" s="346"/>
+      <c r="AE4" s="347"/>
       <c r="AF4" s="87" t="s">
         <v>187</v>
       </c>
@@ -26296,7 +24059,7 @@
       <c r="AH4" s="87" t="s">
         <v>83</v>
       </c>
-      <c r="AI4" s="346"/>
+      <c r="AI4" s="347"/>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A5" s="93" t="s">

</xml_diff>

<commit_message>
update underline red extractor for gap cases
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FC65B3-C932-D543-B071-ECABC4D66B10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A7E359-D53B-D241-8BBF-656D9D6D4728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" activeTab="3" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" activeTab="2" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
   <sheets>
     <sheet name="ACCUEIL" sheetId="33" r:id="rId1"/>
@@ -5955,7 +5955,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="358">
+  <cellXfs count="357">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -7029,6 +7029,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="37" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="39" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7085,12 +7088,6 @@
     </xf>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -7159,7 +7156,27 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{6FC886D6-2077-B34D-B1DF-739B068A66D1}"/>
     <cellStyle name="Normal 3" xfId="4" xr:uid="{6BD57324-3FD5-D341-A299-730D14794802}"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -8098,11 +8115,11 @@
       <c r="B1" s="129" t="s">
         <v>239</v>
       </c>
-      <c r="C1" s="320" t="s">
+      <c r="C1" s="321" t="s">
         <v>240</v>
       </c>
-      <c r="D1" s="320"/>
-      <c r="E1" s="320"/>
+      <c r="D1" s="321"/>
+      <c r="E1" s="321"/>
       <c r="F1" s="130"/>
       <c r="H1" s="26" t="s">
         <v>0</v>
@@ -8111,11 +8128,11 @@
     <row r="2" spans="1:8" s="134" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="131"/>
       <c r="B2" s="132"/>
-      <c r="C2" s="321" t="s">
+      <c r="C2" s="322" t="s">
         <v>241</v>
       </c>
-      <c r="D2" s="321"/>
-      <c r="E2" s="321"/>
+      <c r="D2" s="322"/>
+      <c r="E2" s="322"/>
       <c r="F2" s="133"/>
       <c r="H2" s="26" t="s">
         <v>0</v>
@@ -8139,10 +8156,10 @@
       <c r="D4" s="139" t="s">
         <v>244</v>
       </c>
-      <c r="E4" s="327" t="s">
+      <c r="E4" s="328" t="s">
         <v>245</v>
       </c>
-      <c r="F4" s="328"/>
+      <c r="F4" s="329"/>
       <c r="G4" s="148"/>
       <c r="H4" s="26" t="s">
         <v>0</v>
@@ -8159,10 +8176,10 @@
       <c r="D5" s="145" t="s">
         <v>248</v>
       </c>
-      <c r="E5" s="329" t="s">
+      <c r="E5" s="330" t="s">
         <v>261</v>
       </c>
-      <c r="F5" s="330"/>
+      <c r="F5" s="331"/>
       <c r="G5" s="147"/>
       <c r="H5" s="26" t="s">
         <v>0</v>
@@ -8179,10 +8196,10 @@
       <c r="D6" s="146" t="s">
         <v>251</v>
       </c>
-      <c r="E6" s="331" t="s">
+      <c r="E6" s="332" t="s">
         <v>262</v>
       </c>
-      <c r="F6" s="332"/>
+      <c r="F6" s="333"/>
       <c r="G6" s="147"/>
       <c r="H6" s="26" t="s">
         <v>0</v>
@@ -8199,10 +8216,10 @@
       <c r="D7" s="146" t="s">
         <v>254</v>
       </c>
-      <c r="E7" s="331" t="s">
+      <c r="E7" s="332" t="s">
         <v>261</v>
       </c>
-      <c r="F7" s="332"/>
+      <c r="F7" s="333"/>
       <c r="G7" s="147"/>
       <c r="H7" s="26" t="s">
         <v>0</v>
@@ -8213,16 +8230,16 @@
       <c r="B8" s="155" t="s">
         <v>255</v>
       </c>
-      <c r="C8" s="322" t="s">
+      <c r="C8" s="323" t="s">
         <v>256</v>
       </c>
-      <c r="D8" s="322" t="s">
+      <c r="D8" s="323" t="s">
         <v>257</v>
       </c>
-      <c r="E8" s="333" t="s">
+      <c r="E8" s="334" t="s">
         <v>263</v>
       </c>
-      <c r="F8" s="334"/>
+      <c r="F8" s="335"/>
       <c r="G8" s="147"/>
       <c r="H8" s="26" t="s">
         <v>0</v>
@@ -8233,10 +8250,10 @@
       <c r="B9" s="156" t="s">
         <v>258</v>
       </c>
-      <c r="C9" s="322"/>
-      <c r="D9" s="322"/>
-      <c r="E9" s="335"/>
-      <c r="F9" s="336"/>
+      <c r="C9" s="323"/>
+      <c r="D9" s="323"/>
+      <c r="E9" s="336"/>
+      <c r="F9" s="337"/>
       <c r="G9" s="147"/>
       <c r="H9" s="26" t="s">
         <v>0</v>
@@ -8247,10 +8264,10 @@
       <c r="B10" s="157" t="s">
         <v>259</v>
       </c>
-      <c r="C10" s="323"/>
-      <c r="D10" s="323"/>
-      <c r="E10" s="337"/>
-      <c r="F10" s="338"/>
+      <c r="C10" s="324"/>
+      <c r="D10" s="324"/>
+      <c r="E10" s="338"/>
+      <c r="F10" s="339"/>
       <c r="G10" s="147"/>
       <c r="H10" s="26" t="s">
         <v>0</v>
@@ -8270,11 +8287,11 @@
     <row r="12" spans="1:8" s="26" customFormat="1" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="135"/>
       <c r="B12" s="149"/>
-      <c r="C12" s="326" t="s">
+      <c r="C12" s="327" t="s">
         <v>260</v>
       </c>
-      <c r="D12" s="326"/>
-      <c r="E12" s="326"/>
+      <c r="D12" s="327"/>
+      <c r="E12" s="327"/>
       <c r="F12" s="150"/>
       <c r="H12" s="26" t="s">
         <v>0</v>
@@ -8288,14 +8305,14 @@
       </c>
     </row>
     <row r="14" spans="1:8" s="26" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="324" t="s">
+      <c r="A14" s="325" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="324"/>
-      <c r="C14" s="324"/>
-      <c r="D14" s="324"/>
-      <c r="E14" s="324"/>
-      <c r="F14" s="325"/>
+      <c r="B14" s="325"/>
+      <c r="C14" s="325"/>
+      <c r="D14" s="325"/>
+      <c r="E14" s="325"/>
+      <c r="F14" s="326"/>
       <c r="H14" s="26" t="s">
         <v>0</v>
       </c>
@@ -8368,13 +8385,13 @@
       <c r="G2" s="87" t="s">
         <v>181</v>
       </c>
-      <c r="H2" s="347" t="s">
+      <c r="H2" s="346" t="s">
         <v>180</v>
       </c>
       <c r="I2" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="J2" s="347" t="s">
+      <c r="J2" s="346" t="s">
         <v>179</v>
       </c>
     </row>
@@ -8388,11 +8405,11 @@
       <c r="G3" s="87" t="s">
         <v>159</v>
       </c>
-      <c r="H3" s="347"/>
+      <c r="H3" s="346"/>
       <c r="I3" s="87" t="s">
         <v>156</v>
       </c>
-      <c r="J3" s="347"/>
+      <c r="J3" s="346"/>
     </row>
     <row r="4" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A4" s="109"/>
@@ -8414,11 +8431,11 @@
       <c r="G4" s="87" t="s">
         <v>108</v>
       </c>
-      <c r="H4" s="347"/>
+      <c r="H4" s="346"/>
       <c r="I4" s="87" t="s">
         <v>104</v>
       </c>
-      <c r="J4" s="347"/>
+      <c r="J4" s="346"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="103" t="s">
@@ -8822,7 +8839,7 @@
       <c r="G2" s="87" t="s">
         <v>183</v>
       </c>
-      <c r="H2" s="347" t="s">
+      <c r="H2" s="346" t="s">
         <v>182</v>
       </c>
       <c r="I2" s="86" t="s">
@@ -8867,7 +8884,7 @@
       <c r="V2" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="W2" s="347" t="s">
+      <c r="W2" s="346" t="s">
         <v>180</v>
       </c>
       <c r="X2" s="87" t="s">
@@ -8882,7 +8899,7 @@
       <c r="AA2" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="AB2" s="347" t="s">
+      <c r="AB2" s="346" t="s">
         <v>179</v>
       </c>
       <c r="AC2" s="84" t="s">
@@ -8912,7 +8929,7 @@
       <c r="AK2" s="84" t="s">
         <v>178</v>
       </c>
-      <c r="AL2" s="347" t="s">
+      <c r="AL2" s="346" t="s">
         <v>177</v>
       </c>
       <c r="AM2" s="84" t="s">
@@ -8954,7 +8971,7 @@
       <c r="AY2" s="84" t="s">
         <v>176</v>
       </c>
-      <c r="AZ2" s="347" t="s">
+      <c r="AZ2" s="346" t="s">
         <v>175</v>
       </c>
       <c r="BA2" s="83" t="s">
@@ -8984,7 +9001,7 @@
       <c r="BI2" s="83" t="s">
         <v>174</v>
       </c>
-      <c r="BJ2" s="347" t="s">
+      <c r="BJ2" s="346" t="s">
         <v>173</v>
       </c>
       <c r="BK2"/>
@@ -8999,7 +9016,7 @@
       <c r="G3" s="87" t="s">
         <v>172</v>
       </c>
-      <c r="H3" s="347"/>
+      <c r="H3" s="346"/>
       <c r="I3" s="86" t="s">
         <v>171</v>
       </c>
@@ -9040,7 +9057,7 @@
       <c r="V3" s="86" t="s">
         <v>159</v>
       </c>
-      <c r="W3" s="347"/>
+      <c r="W3" s="346"/>
       <c r="X3" s="82"/>
       <c r="Y3" s="87" t="s">
         <v>158</v>
@@ -9051,7 +9068,7 @@
       <c r="AA3" s="87" t="s">
         <v>156</v>
       </c>
-      <c r="AB3" s="347"/>
+      <c r="AB3" s="346"/>
       <c r="AC3" s="84" t="s">
         <v>155</v>
       </c>
@@ -9079,7 +9096,7 @@
       <c r="AK3" s="84" t="s">
         <v>149</v>
       </c>
-      <c r="AL3" s="347"/>
+      <c r="AL3" s="346"/>
       <c r="AM3" s="84" t="s">
         <v>148</v>
       </c>
@@ -9119,7 +9136,7 @@
       <c r="AY3" s="84" t="s">
         <v>136</v>
       </c>
-      <c r="AZ3" s="347"/>
+      <c r="AZ3" s="346"/>
       <c r="BA3" s="83" t="s">
         <v>135</v>
       </c>
@@ -9147,7 +9164,7 @@
       <c r="BI3" s="83" t="s">
         <v>127</v>
       </c>
-      <c r="BJ3" s="347"/>
+      <c r="BJ3" s="346"/>
     </row>
     <row r="4" spans="1:63" s="44" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="89"/>
@@ -9169,7 +9186,7 @@
       <c r="G4" s="87" t="s">
         <v>122</v>
       </c>
-      <c r="H4" s="347"/>
+      <c r="H4" s="346"/>
       <c r="I4" s="86" t="s">
         <v>121</v>
       </c>
@@ -9212,7 +9229,7 @@
       <c r="V4" s="86" t="s">
         <v>108</v>
       </c>
-      <c r="W4" s="347"/>
+      <c r="W4" s="346"/>
       <c r="X4" s="85" t="s">
         <v>107</v>
       </c>
@@ -9225,7 +9242,7 @@
       <c r="AA4" s="85" t="s">
         <v>104</v>
       </c>
-      <c r="AB4" s="347"/>
+      <c r="AB4" s="346"/>
       <c r="AC4" s="84" t="s">
         <v>103</v>
       </c>
@@ -9253,7 +9270,7 @@
       <c r="AK4" s="84" t="s">
         <v>96</v>
       </c>
-      <c r="AL4" s="347"/>
+      <c r="AL4" s="346"/>
       <c r="AM4" s="84" t="s">
         <v>95</v>
       </c>
@@ -9293,7 +9310,7 @@
       <c r="AY4" s="84" t="s">
         <v>83</v>
       </c>
-      <c r="AZ4" s="347"/>
+      <c r="AZ4" s="346"/>
       <c r="BA4" s="83" t="s">
         <v>82</v>
       </c>
@@ -9321,7 +9338,7 @@
       <c r="BI4" s="83" t="s">
         <v>74</v>
       </c>
-      <c r="BJ4" s="347"/>
+      <c r="BJ4" s="346"/>
       <c r="BK4"/>
     </row>
     <row r="5" spans="1:63" s="44" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -12071,7 +12088,7 @@
       <c r="G2" s="87" t="s">
         <v>183</v>
       </c>
-      <c r="H2" s="347" t="s">
+      <c r="H2" s="346" t="s">
         <v>182</v>
       </c>
       <c r="I2" s="87" t="s">
@@ -12104,13 +12121,13 @@
       <c r="R2" s="87" t="s">
         <v>181</v>
       </c>
-      <c r="S2" s="347" t="s">
+      <c r="S2" s="346" t="s">
         <v>180</v>
       </c>
       <c r="T2" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="U2" s="347" t="s">
+      <c r="U2" s="346" t="s">
         <v>179</v>
       </c>
       <c r="V2" s="87" t="s">
@@ -12140,7 +12157,7 @@
       <c r="AD2" s="87" t="s">
         <v>178</v>
       </c>
-      <c r="AE2" s="347" t="s">
+      <c r="AE2" s="346" t="s">
         <v>227</v>
       </c>
       <c r="AF2" s="87" t="s">
@@ -12152,7 +12169,7 @@
       <c r="AH2" s="87" t="s">
         <v>226</v>
       </c>
-      <c r="AI2" s="347" t="s">
+      <c r="AI2" s="346" t="s">
         <v>225</v>
       </c>
     </row>
@@ -12166,7 +12183,7 @@
       <c r="G3" s="87" t="s">
         <v>172</v>
       </c>
-      <c r="H3" s="347"/>
+      <c r="H3" s="346"/>
       <c r="I3" s="87" t="s">
         <v>224</v>
       </c>
@@ -12197,11 +12214,11 @@
       <c r="R3" s="87" t="s">
         <v>159</v>
       </c>
-      <c r="S3" s="347"/>
+      <c r="S3" s="346"/>
       <c r="T3" s="87" t="s">
         <v>156</v>
       </c>
-      <c r="U3" s="347"/>
+      <c r="U3" s="346"/>
       <c r="V3" s="87" t="s">
         <v>215</v>
       </c>
@@ -12229,7 +12246,7 @@
       <c r="AD3" s="87" t="s">
         <v>207</v>
       </c>
-      <c r="AE3" s="347"/>
+      <c r="AE3" s="346"/>
       <c r="AF3" s="87" t="s">
         <v>206</v>
       </c>
@@ -12239,7 +12256,7 @@
       <c r="AH3" s="87" t="s">
         <v>136</v>
       </c>
-      <c r="AI3" s="347"/>
+      <c r="AI3" s="346"/>
     </row>
     <row r="4" spans="1:62" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="90"/>
@@ -12261,7 +12278,7 @@
       <c r="G4" s="87" t="s">
         <v>122</v>
       </c>
-      <c r="H4" s="347"/>
+      <c r="H4" s="346"/>
       <c r="I4" s="87" t="s">
         <v>205</v>
       </c>
@@ -12292,11 +12309,11 @@
       <c r="R4" s="87" t="s">
         <v>108</v>
       </c>
-      <c r="S4" s="347"/>
+      <c r="S4" s="346"/>
       <c r="T4" s="87" t="s">
         <v>104</v>
       </c>
-      <c r="U4" s="347"/>
+      <c r="U4" s="346"/>
       <c r="V4" s="87" t="s">
         <v>196</v>
       </c>
@@ -12324,7 +12341,7 @@
       <c r="AD4" s="87" t="s">
         <v>188</v>
       </c>
-      <c r="AE4" s="347"/>
+      <c r="AE4" s="346"/>
       <c r="AF4" s="87" t="s">
         <v>187</v>
       </c>
@@ -12334,7 +12351,7 @@
       <c r="AH4" s="87" t="s">
         <v>83</v>
       </c>
-      <c r="AI4" s="347"/>
+      <c r="AI4" s="346"/>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A5" s="93" t="s">
@@ -14091,13 +14108,13 @@
       <c r="G2" s="87" t="s">
         <v>181</v>
       </c>
-      <c r="H2" s="347" t="s">
+      <c r="H2" s="346" t="s">
         <v>180</v>
       </c>
       <c r="I2" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="J2" s="347" t="s">
+      <c r="J2" s="346" t="s">
         <v>179</v>
       </c>
     </row>
@@ -14111,11 +14128,11 @@
       <c r="G3" s="87" t="s">
         <v>159</v>
       </c>
-      <c r="H3" s="347"/>
+      <c r="H3" s="346"/>
       <c r="I3" s="87" t="s">
         <v>156</v>
       </c>
-      <c r="J3" s="347"/>
+      <c r="J3" s="346"/>
     </row>
     <row r="4" spans="1:62" ht="36" x14ac:dyDescent="0.2">
       <c r="A4" s="109"/>
@@ -14137,11 +14154,11 @@
       <c r="G4" s="87" t="s">
         <v>108</v>
       </c>
-      <c r="H4" s="347"/>
+      <c r="H4" s="346"/>
       <c r="I4" s="87" t="s">
         <v>104</v>
       </c>
-      <c r="J4" s="347"/>
+      <c r="J4" s="346"/>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A5" s="103" t="s">
@@ -14536,13 +14553,13 @@
   <sheetData>
     <row r="1" spans="1:61" s="168" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="167"/>
-      <c r="B1" s="351" t="s">
+      <c r="B1" s="350" t="s">
         <v>184</v>
       </c>
-      <c r="C1" s="351"/>
-      <c r="D1" s="351"/>
-      <c r="E1" s="351"/>
-      <c r="F1" s="351"/>
+      <c r="C1" s="350"/>
+      <c r="D1" s="350"/>
+      <c r="E1" s="350"/>
+      <c r="F1" s="350"/>
       <c r="G1" s="169"/>
       <c r="H1" s="169"/>
       <c r="I1" s="169"/>
@@ -14587,7 +14604,7 @@
       <c r="O2" s="171" t="s">
         <v>178</v>
       </c>
-      <c r="P2" s="350" t="s">
+      <c r="P2" s="349" t="s">
         <v>177</v>
       </c>
       <c r="Q2" s="171" t="s">
@@ -14629,7 +14646,7 @@
       <c r="AC2" s="171" t="s">
         <v>176</v>
       </c>
-      <c r="AD2" s="350" t="s">
+      <c r="AD2" s="349" t="s">
         <v>175</v>
       </c>
       <c r="AE2" s="172" t="s">
@@ -14659,7 +14676,7 @@
       <c r="AM2" s="172" t="s">
         <v>174</v>
       </c>
-      <c r="AN2" s="350" t="s">
+      <c r="AN2" s="349" t="s">
         <v>173</v>
       </c>
       <c r="AQ2" s="171"/>
@@ -14670,7 +14687,7 @@
       <c r="AV2" s="171"/>
       <c r="AW2" s="171"/>
       <c r="AX2" s="171"/>
-      <c r="AY2" s="350"/>
+      <c r="AY2" s="349"/>
       <c r="AZ2" s="172"/>
       <c r="BA2" s="172"/>
       <c r="BB2" s="172"/>
@@ -14680,7 +14697,7 @@
       <c r="BF2" s="172"/>
       <c r="BG2" s="172"/>
       <c r="BH2" s="172"/>
-      <c r="BI2" s="350"/>
+      <c r="BI2" s="349"/>
     </row>
     <row r="3" spans="1:61" s="168" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="170"/>
@@ -14716,7 +14733,7 @@
       <c r="O3" s="171" t="s">
         <v>149</v>
       </c>
-      <c r="P3" s="350"/>
+      <c r="P3" s="349"/>
       <c r="Q3" s="171" t="s">
         <v>148</v>
       </c>
@@ -14756,7 +14773,7 @@
       <c r="AC3" s="171" t="s">
         <v>136</v>
       </c>
-      <c r="AD3" s="350"/>
+      <c r="AD3" s="349"/>
       <c r="AE3" s="172" t="s">
         <v>135</v>
       </c>
@@ -14784,7 +14801,7 @@
       <c r="AM3" s="172" t="s">
         <v>127</v>
       </c>
-      <c r="AN3" s="350"/>
+      <c r="AN3" s="349"/>
       <c r="AQ3" s="171"/>
       <c r="AR3" s="171"/>
       <c r="AS3" s="171"/>
@@ -14793,7 +14810,7 @@
       <c r="AV3" s="171"/>
       <c r="AW3" s="171"/>
       <c r="AX3" s="171"/>
-      <c r="AY3" s="350"/>
+      <c r="AY3" s="349"/>
       <c r="AZ3" s="172"/>
       <c r="BA3" s="172"/>
       <c r="BB3" s="172"/>
@@ -14803,7 +14820,7 @@
       <c r="BF3" s="172"/>
       <c r="BG3" s="172"/>
       <c r="BH3" s="172"/>
-      <c r="BI3" s="350"/>
+      <c r="BI3" s="349"/>
     </row>
     <row r="4" spans="1:61" s="168" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="173"/>
@@ -14849,7 +14866,7 @@
       <c r="O4" s="171" t="s">
         <v>96</v>
       </c>
-      <c r="P4" s="350"/>
+      <c r="P4" s="349"/>
       <c r="Q4" s="171" t="s">
         <v>95</v>
       </c>
@@ -14889,7 +14906,7 @@
       <c r="AC4" s="171" t="s">
         <v>83</v>
       </c>
-      <c r="AD4" s="350"/>
+      <c r="AD4" s="349"/>
       <c r="AE4" s="172" t="s">
         <v>82</v>
       </c>
@@ -14917,7 +14934,7 @@
       <c r="AM4" s="172" t="s">
         <v>74</v>
       </c>
-      <c r="AN4" s="350"/>
+      <c r="AN4" s="349"/>
       <c r="AQ4" s="171"/>
       <c r="AR4" s="171"/>
       <c r="AS4" s="171"/>
@@ -14926,7 +14943,7 @@
       <c r="AV4" s="171"/>
       <c r="AW4" s="171"/>
       <c r="AX4" s="171"/>
-      <c r="AY4" s="350"/>
+      <c r="AY4" s="349"/>
       <c r="AZ4" s="172"/>
       <c r="BA4" s="172"/>
       <c r="BB4" s="172"/>
@@ -14936,7 +14953,7 @@
       <c r="BF4" s="172"/>
       <c r="BG4" s="172"/>
       <c r="BH4" s="172"/>
-      <c r="BI4" s="350"/>
+      <c r="BI4" s="349"/>
     </row>
     <row r="5" spans="1:61" s="168" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="175" t="s">
@@ -16663,14 +16680,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="352" t="s">
+      <c r="A1" s="351" t="s">
         <v>228</v>
       </c>
-      <c r="B1" s="352"/>
-      <c r="C1" s="352"/>
-      <c r="D1" s="352"/>
-      <c r="E1" s="352"/>
-      <c r="F1" s="352"/>
+      <c r="B1" s="351"/>
+      <c r="C1" s="351"/>
+      <c r="D1" s="351"/>
+      <c r="E1" s="351"/>
+      <c r="F1" s="351"/>
       <c r="G1" s="200"/>
       <c r="H1" s="200"/>
       <c r="I1" s="200"/>
@@ -16720,7 +16737,7 @@
       <c r="O2" s="203" t="s">
         <v>178</v>
       </c>
-      <c r="P2" s="353" t="s">
+      <c r="P2" s="352" t="s">
         <v>227</v>
       </c>
       <c r="Q2" s="203" t="s">
@@ -16732,7 +16749,7 @@
       <c r="S2" s="203" t="s">
         <v>226</v>
       </c>
-      <c r="T2" s="353" t="s">
+      <c r="T2" s="352" t="s">
         <v>225</v>
       </c>
     </row>
@@ -16770,7 +16787,7 @@
       <c r="O3" s="203" t="s">
         <v>207</v>
       </c>
-      <c r="P3" s="353"/>
+      <c r="P3" s="352"/>
       <c r="Q3" s="203" t="s">
         <v>206</v>
       </c>
@@ -16780,7 +16797,7 @@
       <c r="S3" s="203" t="s">
         <v>136</v>
       </c>
-      <c r="T3" s="353"/>
+      <c r="T3" s="352"/>
     </row>
     <row r="4" spans="1:20" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="202"/>
@@ -16826,7 +16843,7 @@
       <c r="O4" s="203" t="s">
         <v>188</v>
       </c>
-      <c r="P4" s="353"/>
+      <c r="P4" s="352"/>
       <c r="Q4" s="203" t="s">
         <v>187</v>
       </c>
@@ -16836,7 +16853,7 @@
       <c r="S4" s="203" t="s">
         <v>83</v>
       </c>
-      <c r="T4" s="353"/>
+      <c r="T4" s="352"/>
     </row>
     <row r="5" spans="1:20" ht="317" x14ac:dyDescent="0.2">
       <c r="A5" s="206" t="s">
@@ -17427,16 +17444,16 @@
   <sheetData>
     <row r="1" spans="1:28" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="226"/>
-      <c r="B1" s="355" t="s">
+      <c r="B1" s="354" t="s">
         <v>184</v>
       </c>
-      <c r="C1" s="355"/>
-      <c r="D1" s="355"/>
-      <c r="E1" s="355"/>
-      <c r="F1" s="355"/>
-      <c r="G1" s="355"/>
-      <c r="H1" s="355"/>
-      <c r="I1" s="355"/>
+      <c r="C1" s="354"/>
+      <c r="D1" s="354"/>
+      <c r="E1" s="354"/>
+      <c r="F1" s="354"/>
+      <c r="G1" s="354"/>
+      <c r="H1" s="354"/>
+      <c r="I1" s="354"/>
       <c r="J1" s="223"/>
       <c r="K1" s="223"/>
       <c r="L1" s="223"/>
@@ -17467,7 +17484,7 @@
       <c r="G2" s="225" t="s">
         <v>183</v>
       </c>
-      <c r="H2" s="354" t="s">
+      <c r="H2" s="353" t="s">
         <v>182</v>
       </c>
       <c r="I2" s="228" t="s">
@@ -17512,7 +17529,7 @@
       <c r="V2" s="228" t="s">
         <v>181</v>
       </c>
-      <c r="W2" s="354" t="s">
+      <c r="W2" s="353" t="s">
         <v>180</v>
       </c>
       <c r="X2" s="225" t="s">
@@ -17527,7 +17544,7 @@
       <c r="AA2" s="225" t="s">
         <v>45</v>
       </c>
-      <c r="AB2" s="354" t="s">
+      <c r="AB2" s="353" t="s">
         <v>179</v>
       </c>
     </row>
@@ -17541,7 +17558,7 @@
       <c r="G3" s="225" t="s">
         <v>172</v>
       </c>
-      <c r="H3" s="354"/>
+      <c r="H3" s="353"/>
       <c r="I3" s="228" t="s">
         <v>171</v>
       </c>
@@ -17582,7 +17599,7 @@
       <c r="V3" s="228" t="s">
         <v>159</v>
       </c>
-      <c r="W3" s="354"/>
+      <c r="W3" s="353"/>
       <c r="X3" s="227"/>
       <c r="Y3" s="225" t="s">
         <v>158</v>
@@ -17593,7 +17610,7 @@
       <c r="AA3" s="225" t="s">
         <v>156</v>
       </c>
-      <c r="AB3" s="354"/>
+      <c r="AB3" s="353"/>
     </row>
     <row r="4" spans="1:28" ht="98" x14ac:dyDescent="0.2">
       <c r="A4" s="229"/>
@@ -17615,7 +17632,7 @@
       <c r="G4" s="225" t="s">
         <v>122</v>
       </c>
-      <c r="H4" s="354"/>
+      <c r="H4" s="353"/>
       <c r="I4" s="228" t="s">
         <v>121</v>
       </c>
@@ -17658,7 +17675,7 @@
       <c r="V4" s="231" t="s">
         <v>108</v>
       </c>
-      <c r="W4" s="354"/>
+      <c r="W4" s="353"/>
       <c r="X4" s="232" t="s">
         <v>107</v>
       </c>
@@ -17671,7 +17688,7 @@
       <c r="AA4" s="232" t="s">
         <v>104</v>
       </c>
-      <c r="AB4" s="354"/>
+      <c r="AB4" s="353"/>
     </row>
     <row r="5" spans="1:28" ht="196" x14ac:dyDescent="0.2">
       <c r="A5" s="233" t="s">
@@ -18570,16 +18587,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="357" t="s">
+      <c r="A1" s="356" t="s">
         <v>228</v>
       </c>
-      <c r="B1" s="357"/>
-      <c r="C1" s="357"/>
-      <c r="D1" s="357"/>
-      <c r="E1" s="357"/>
-      <c r="F1" s="357"/>
-      <c r="G1" s="357"/>
-      <c r="H1" s="357"/>
+      <c r="B1" s="356"/>
+      <c r="C1" s="356"/>
+      <c r="D1" s="356"/>
+      <c r="E1" s="356"/>
+      <c r="F1" s="356"/>
+      <c r="G1" s="356"/>
+      <c r="H1" s="356"/>
       <c r="I1" s="273"/>
       <c r="J1" s="273"/>
       <c r="K1" s="273"/>
@@ -18604,7 +18621,7 @@
       <c r="G2" s="275" t="s">
         <v>183</v>
       </c>
-      <c r="H2" s="356" t="s">
+      <c r="H2" s="355" t="s">
         <v>182</v>
       </c>
       <c r="I2" s="275" t="s">
@@ -18637,13 +18654,13 @@
       <c r="R2" s="275" t="s">
         <v>181</v>
       </c>
-      <c r="S2" s="356" t="s">
+      <c r="S2" s="355" t="s">
         <v>180</v>
       </c>
       <c r="T2" s="275" t="s">
         <v>45</v>
       </c>
-      <c r="U2" s="356" t="s">
+      <c r="U2" s="355" t="s">
         <v>179</v>
       </c>
     </row>
@@ -18657,7 +18674,7 @@
       <c r="G3" s="275" t="s">
         <v>172</v>
       </c>
-      <c r="H3" s="356"/>
+      <c r="H3" s="355"/>
       <c r="I3" s="275" t="s">
         <v>224</v>
       </c>
@@ -18688,11 +18705,11 @@
       <c r="R3" s="275" t="s">
         <v>159</v>
       </c>
-      <c r="S3" s="356"/>
+      <c r="S3" s="355"/>
       <c r="T3" s="275" t="s">
         <v>156</v>
       </c>
-      <c r="U3" s="356"/>
+      <c r="U3" s="355"/>
     </row>
     <row r="4" spans="1:21" ht="112" x14ac:dyDescent="0.2">
       <c r="A4" s="272"/>
@@ -18714,7 +18731,7 @@
       <c r="G4" s="275" t="s">
         <v>122</v>
       </c>
-      <c r="H4" s="356"/>
+      <c r="H4" s="355"/>
       <c r="I4" s="275" t="s">
         <v>205</v>
       </c>
@@ -18745,11 +18762,11 @@
       <c r="R4" s="275" t="s">
         <v>108</v>
       </c>
-      <c r="S4" s="356"/>
+      <c r="S4" s="355"/>
       <c r="T4" s="275" t="s">
         <v>104</v>
       </c>
-      <c r="U4" s="356"/>
+      <c r="U4" s="355"/>
     </row>
     <row r="5" spans="1:21" ht="196" x14ac:dyDescent="0.2">
       <c r="A5" s="278" t="s">
@@ -19445,13 +19462,13 @@
       <c r="K2" s="203" t="s">
         <v>181</v>
       </c>
-      <c r="L2" s="353" t="s">
+      <c r="L2" s="352" t="s">
         <v>180</v>
       </c>
       <c r="M2" s="203" t="s">
         <v>45</v>
       </c>
-      <c r="N2" s="353" t="s">
+      <c r="N2" s="352" t="s">
         <v>179</v>
       </c>
     </row>
@@ -19469,11 +19486,11 @@
       <c r="K3" s="203" t="s">
         <v>159</v>
       </c>
-      <c r="L3" s="353"/>
+      <c r="L3" s="352"/>
       <c r="M3" s="203" t="s">
         <v>156</v>
       </c>
-      <c r="N3" s="353"/>
+      <c r="N3" s="352"/>
     </row>
     <row r="4" spans="1:14" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="256"/>
@@ -19499,11 +19516,11 @@
       <c r="K4" s="203" t="s">
         <v>108</v>
       </c>
-      <c r="L4" s="353"/>
+      <c r="L4" s="352"/>
       <c r="M4" s="203" t="s">
         <v>104</v>
       </c>
-      <c r="N4" s="353"/>
+      <c r="N4" s="352"/>
     </row>
     <row r="5" spans="1:14" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="258"/>
@@ -20162,8 +20179,8 @@
   </sheetPr>
   <dimension ref="A1:FJ4"/>
   <sheetViews>
-    <sheetView showFormulas="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A187" sqref="A187"/>
+    <sheetView showFormulas="1" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20194,17 +20211,17 @@
       <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="FA1" s="339" t="s">
+      <c r="FA1" s="320" t="s">
         <v>237</v>
       </c>
-      <c r="FB1" s="339"/>
-      <c r="FC1" s="339"/>
-      <c r="FD1" s="339"/>
-      <c r="FE1" s="339"/>
-      <c r="FF1" s="339"/>
-      <c r="FG1" s="340"/>
-      <c r="FH1" s="340"/>
-      <c r="FI1" s="340"/>
+      <c r="FB1" s="320"/>
+      <c r="FC1" s="320"/>
+      <c r="FD1" s="320"/>
+      <c r="FE1" s="320"/>
+      <c r="FF1" s="320"/>
+      <c r="FG1" s="320"/>
+      <c r="FH1"/>
+      <c r="FI1"/>
       <c r="FJ1" s="4" t="s">
         <v>0</v>
       </c>
@@ -20254,9 +20271,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A2:DT2" xr:uid="{3B89445B-6ECC-4440-B85C-E593AE209933}"/>
-  <mergeCells count="1">
-    <mergeCell ref="FA1:FI1"/>
-  </mergeCells>
+  <conditionalFormatting sqref="A1:FG1048576">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+      <formula>AND(OR($N1&lt;&gt;"-",$O1&lt;&gt;0,$P1&lt;&gt;0),ROW()&gt;2,$A1&lt;&gt;"")</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
@@ -20270,7 +20289,7 @@
   </sheetPr>
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="H1" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
@@ -20350,28 +20369,28 @@
       <c r="D4" s="294"/>
       <c r="E4" s="294"/>
       <c r="F4" s="294"/>
-      <c r="G4" s="341" t="s">
+      <c r="G4" s="340" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="342"/>
-      <c r="I4" s="342"/>
-      <c r="J4" s="342"/>
-      <c r="K4" s="342"/>
-      <c r="L4" s="343"/>
-      <c r="M4" s="344"/>
-      <c r="N4" s="345" t="s">
+      <c r="H4" s="341"/>
+      <c r="I4" s="341"/>
+      <c r="J4" s="341"/>
+      <c r="K4" s="341"/>
+      <c r="L4" s="342"/>
+      <c r="M4" s="343"/>
+      <c r="N4" s="344" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="343"/>
-      <c r="P4" s="343"/>
-      <c r="Q4" s="343"/>
-      <c r="R4" s="343"/>
-      <c r="S4" s="343"/>
-      <c r="T4" s="346"/>
-      <c r="U4" s="341" t="s">
+      <c r="O4" s="342"/>
+      <c r="P4" s="342"/>
+      <c r="Q4" s="342"/>
+      <c r="R4" s="342"/>
+      <c r="S4" s="342"/>
+      <c r="T4" s="345"/>
+      <c r="U4" s="340" t="s">
         <v>28</v>
       </c>
-      <c r="V4" s="344"/>
+      <c r="V4" s="343"/>
       <c r="W4" s="301"/>
       <c r="X4" t="s">
         <v>0</v>
@@ -20568,70 +20587,70 @@
     <mergeCell ref="U4:V4"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:F4">
-    <cfRule type="expression" dxfId="15" priority="16">
+    <cfRule type="expression" dxfId="17" priority="16">
       <formula>IF(LEFT($A$3,2)&lt;&gt;"TJ",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:V151">
-    <cfRule type="expression" dxfId="14" priority="18">
+    <cfRule type="expression" dxfId="16" priority="18">
       <formula>AND(ISBLANK($C6)=FALSE,ISBLANK($E6)=TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:F1048576">
-    <cfRule type="expression" dxfId="13" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="1" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($U1)-(_xlfn.NUMBERVALUE($U2)+_xlfn.NUMBERVALUE($U3)+_xlfn.NUMBERVALUE($U4)+_xlfn.NUMBERVALUE($U5)+_xlfn.NUMBERVALUE($U6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="2" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($S1)-(_xlfn.NUMBERVALUE($S2)+_xlfn.NUMBERVALUE($S3)+_xlfn.NUMBERVALUE($S4)+_xlfn.NUMBERVALUE($S5)+_xlfn.NUMBERVALUE($S6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="7" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3)+_xlfn.NUMBERVALUE($L4)-_xlfn.NUMBERVALUE($L5)+_xlfn.NUMBERVALUE($L6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="12" stopIfTrue="1">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",OR(_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3))&lt;&gt;0,_xlfn.NUMBERVALUE($S1)-(_xlfn.NUMBERVALUE($S2)+_xlfn.NUMBERVALUE($S3))&lt;&gt;0,_xlfn.NUMBERVALUE($U1)-(_xlfn.NUMBERVALUE($U2)+_xlfn.NUMBERVALUE($U3))&lt;&gt;0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:F7">
-    <cfRule type="expression" dxfId="9" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="6" stopIfTrue="1">
       <formula>OR(_xlfn.NUMBERVALUE($L7)&lt;&gt;_xlfn.NUMBERVALUE($L6),_xlfn.NUMBERVALUE($S7)&lt;&gt;_xlfn.NUMBERVALUE($S6),_xlfn.NUMBERVALUE($U7)&lt;&gt;_xlfn.NUMBERVALUE($U6))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:M1048576">
-    <cfRule type="expression" dxfId="8" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="11" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3)+_xlfn.NUMBERVALUE($L4)+_xlfn.NUMBERVALUE($L5)+_xlfn.NUMBERVALUE($L6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="15">
+    <cfRule type="expression" dxfId="9" priority="15">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3))&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:M7">
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="8" priority="5">
       <formula>_xlfn.NUMBERVALUE($L7)&lt;&gt;_xlfn.NUMBERVALUE($L6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:T1048576">
-    <cfRule type="expression" dxfId="5" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="10" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($S1)-(_xlfn.NUMBERVALUE($S2)+_xlfn.NUMBERVALUE($S3)+_xlfn.NUMBERVALUE($S4)+_xlfn.NUMBERVALUE($S5)+_xlfn.NUMBERVALUE($S6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="14">
+    <cfRule type="expression" dxfId="6" priority="14">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",_xlfn.NUMBERVALUE($S1)-(_xlfn.NUMBERVALUE($S2)+_xlfn.NUMBERVALUE($S3))&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7:T7">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>_xlfn.NUMBERVALUE($S7)&lt;&gt;_xlfn.NUMBERVALUE($S6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:V1048576">
-    <cfRule type="expression" dxfId="2" priority="9">
+    <cfRule type="expression" dxfId="4" priority="9">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($U1)-(_xlfn.NUMBERVALUE($U2)+_xlfn.NUMBERVALUE($U3)+_xlfn.NUMBERVALUE($U4)+_xlfn.NUMBERVALUE($U5)+_xlfn.NUMBERVALUE($U6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="13">
+    <cfRule type="expression" dxfId="3" priority="13">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",_xlfn.NUMBERVALUE($U1)-(_xlfn.NUMBERVALUE($U2)+_xlfn.NUMBERVALUE($U3))&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U7:V7">
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>_xlfn.NUMBERVALUE($U7)&lt;&gt;_xlfn.NUMBERVALUE($U6)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21032,16 +21051,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" s="44" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B1" s="348" t="s">
+      <c r="B1" s="347" t="s">
         <v>184</v>
       </c>
-      <c r="C1" s="348"/>
-      <c r="D1" s="348"/>
-      <c r="E1" s="348"/>
-      <c r="F1" s="348"/>
-      <c r="G1" s="348"/>
-      <c r="H1" s="348"/>
-      <c r="I1" s="348"/>
+      <c r="C1" s="347"/>
+      <c r="D1" s="347"/>
+      <c r="E1" s="347"/>
+      <c r="F1" s="347"/>
+      <c r="G1" s="347"/>
+      <c r="H1" s="347"/>
+      <c r="I1" s="347"/>
     </row>
     <row r="2" spans="1:62" s="44" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="90"/>
@@ -21053,7 +21072,7 @@
       <c r="G2" s="87" t="s">
         <v>183</v>
       </c>
-      <c r="H2" s="347" t="s">
+      <c r="H2" s="346" t="s">
         <v>182</v>
       </c>
       <c r="I2" s="86" t="s">
@@ -21098,7 +21117,7 @@
       <c r="V2" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="W2" s="347" t="s">
+      <c r="W2" s="346" t="s">
         <v>180</v>
       </c>
       <c r="X2" s="87" t="s">
@@ -21113,7 +21132,7 @@
       <c r="AA2" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="AB2" s="347" t="s">
+      <c r="AB2" s="346" t="s">
         <v>179</v>
       </c>
       <c r="AC2" s="84" t="s">
@@ -21143,7 +21162,7 @@
       <c r="AK2" s="84" t="s">
         <v>178</v>
       </c>
-      <c r="AL2" s="347" t="s">
+      <c r="AL2" s="346" t="s">
         <v>177</v>
       </c>
       <c r="AM2" s="84" t="s">
@@ -21185,7 +21204,7 @@
       <c r="AY2" s="84" t="s">
         <v>176</v>
       </c>
-      <c r="AZ2" s="347" t="s">
+      <c r="AZ2" s="346" t="s">
         <v>175</v>
       </c>
       <c r="BA2" s="83" t="s">
@@ -21215,7 +21234,7 @@
       <c r="BI2" s="83" t="s">
         <v>174</v>
       </c>
-      <c r="BJ2" s="347" t="s">
+      <c r="BJ2" s="346" t="s">
         <v>173</v>
       </c>
     </row>
@@ -21229,7 +21248,7 @@
       <c r="G3" s="87" t="s">
         <v>172</v>
       </c>
-      <c r="H3" s="347"/>
+      <c r="H3" s="346"/>
       <c r="I3" s="86" t="s">
         <v>171</v>
       </c>
@@ -21270,7 +21289,7 @@
       <c r="V3" s="86" t="s">
         <v>159</v>
       </c>
-      <c r="W3" s="347"/>
+      <c r="W3" s="346"/>
       <c r="X3" s="82"/>
       <c r="Y3" s="87" t="s">
         <v>158</v>
@@ -21281,7 +21300,7 @@
       <c r="AA3" s="87" t="s">
         <v>156</v>
       </c>
-      <c r="AB3" s="347"/>
+      <c r="AB3" s="346"/>
       <c r="AC3" s="84" t="s">
         <v>155</v>
       </c>
@@ -21309,7 +21328,7 @@
       <c r="AK3" s="84" t="s">
         <v>149</v>
       </c>
-      <c r="AL3" s="347"/>
+      <c r="AL3" s="346"/>
       <c r="AM3" s="84" t="s">
         <v>148</v>
       </c>
@@ -21349,7 +21368,7 @@
       <c r="AY3" s="84" t="s">
         <v>136</v>
       </c>
-      <c r="AZ3" s="347"/>
+      <c r="AZ3" s="346"/>
       <c r="BA3" s="83" t="s">
         <v>135</v>
       </c>
@@ -21377,7 +21396,7 @@
       <c r="BI3" s="83" t="s">
         <v>127</v>
       </c>
-      <c r="BJ3" s="347"/>
+      <c r="BJ3" s="346"/>
     </row>
     <row r="4" spans="1:62" s="44" customFormat="1" ht="60" x14ac:dyDescent="0.15">
       <c r="A4" s="89"/>
@@ -21399,7 +21418,7 @@
       <c r="G4" s="87" t="s">
         <v>122</v>
       </c>
-      <c r="H4" s="347"/>
+      <c r="H4" s="346"/>
       <c r="I4" s="86" t="s">
         <v>121</v>
       </c>
@@ -21442,7 +21461,7 @@
       <c r="V4" s="86" t="s">
         <v>108</v>
       </c>
-      <c r="W4" s="347"/>
+      <c r="W4" s="346"/>
       <c r="X4" s="85" t="s">
         <v>107</v>
       </c>
@@ -21455,7 +21474,7 @@
       <c r="AA4" s="85" t="s">
         <v>104</v>
       </c>
-      <c r="AB4" s="347"/>
+      <c r="AB4" s="346"/>
       <c r="AC4" s="84" t="s">
         <v>103</v>
       </c>
@@ -21483,7 +21502,7 @@
       <c r="AK4" s="84" t="s">
         <v>96</v>
       </c>
-      <c r="AL4" s="347"/>
+      <c r="AL4" s="346"/>
       <c r="AM4" s="84" t="s">
         <v>95</v>
       </c>
@@ -21523,7 +21542,7 @@
       <c r="AY4" s="84" t="s">
         <v>83</v>
       </c>
-      <c r="AZ4" s="347"/>
+      <c r="AZ4" s="346"/>
       <c r="BA4" s="83" t="s">
         <v>82</v>
       </c>
@@ -21551,7 +21570,7 @@
       <c r="BI4" s="83" t="s">
         <v>74</v>
       </c>
-      <c r="BJ4" s="347"/>
+      <c r="BJ4" s="346"/>
     </row>
     <row r="5" spans="1:62" s="44" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="54" t="s">
@@ -23748,16 +23767,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A1" s="349" t="s">
+      <c r="A1" s="348" t="s">
         <v>228</v>
       </c>
-      <c r="B1" s="349"/>
-      <c r="C1" s="349"/>
-      <c r="D1" s="349"/>
-      <c r="E1" s="349"/>
-      <c r="F1" s="349"/>
-      <c r="G1" s="349"/>
-      <c r="H1" s="349"/>
+      <c r="B1" s="348"/>
+      <c r="C1" s="348"/>
+      <c r="D1" s="348"/>
+      <c r="E1" s="348"/>
+      <c r="F1" s="348"/>
+      <c r="G1" s="348"/>
+      <c r="H1" s="348"/>
       <c r="I1" s="44"/>
       <c r="J1" s="44"/>
       <c r="K1" s="44"/>
@@ -23796,7 +23815,7 @@
       <c r="G2" s="87" t="s">
         <v>183</v>
       </c>
-      <c r="H2" s="347" t="s">
+      <c r="H2" s="346" t="s">
         <v>182</v>
       </c>
       <c r="I2" s="87" t="s">
@@ -23829,13 +23848,13 @@
       <c r="R2" s="87" t="s">
         <v>181</v>
       </c>
-      <c r="S2" s="347" t="s">
+      <c r="S2" s="346" t="s">
         <v>180</v>
       </c>
       <c r="T2" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="U2" s="347" t="s">
+      <c r="U2" s="346" t="s">
         <v>179</v>
       </c>
       <c r="V2" s="87" t="s">
@@ -23865,7 +23884,7 @@
       <c r="AD2" s="87" t="s">
         <v>178</v>
       </c>
-      <c r="AE2" s="347" t="s">
+      <c r="AE2" s="346" t="s">
         <v>227</v>
       </c>
       <c r="AF2" s="87" t="s">
@@ -23877,7 +23896,7 @@
       <c r="AH2" s="87" t="s">
         <v>226</v>
       </c>
-      <c r="AI2" s="347" t="s">
+      <c r="AI2" s="346" t="s">
         <v>225</v>
       </c>
     </row>
@@ -23891,7 +23910,7 @@
       <c r="G3" s="87" t="s">
         <v>172</v>
       </c>
-      <c r="H3" s="347"/>
+      <c r="H3" s="346"/>
       <c r="I3" s="87" t="s">
         <v>224</v>
       </c>
@@ -23922,11 +23941,11 @@
       <c r="R3" s="87" t="s">
         <v>159</v>
       </c>
-      <c r="S3" s="347"/>
+      <c r="S3" s="346"/>
       <c r="T3" s="87" t="s">
         <v>156</v>
       </c>
-      <c r="U3" s="347"/>
+      <c r="U3" s="346"/>
       <c r="V3" s="87" t="s">
         <v>215</v>
       </c>
@@ -23954,7 +23973,7 @@
       <c r="AD3" s="87" t="s">
         <v>207</v>
       </c>
-      <c r="AE3" s="347"/>
+      <c r="AE3" s="346"/>
       <c r="AF3" s="87" t="s">
         <v>206</v>
       </c>
@@ -23964,7 +23983,7 @@
       <c r="AH3" s="87" t="s">
         <v>136</v>
       </c>
-      <c r="AI3" s="347"/>
+      <c r="AI3" s="346"/>
     </row>
     <row r="4" spans="1:35" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="90"/>
@@ -23986,7 +24005,7 @@
       <c r="G4" s="87" t="s">
         <v>122</v>
       </c>
-      <c r="H4" s="347"/>
+      <c r="H4" s="346"/>
       <c r="I4" s="87" t="s">
         <v>205</v>
       </c>
@@ -24017,11 +24036,11 @@
       <c r="R4" s="87" t="s">
         <v>108</v>
       </c>
-      <c r="S4" s="347"/>
+      <c r="S4" s="346"/>
       <c r="T4" s="87" t="s">
         <v>104</v>
       </c>
-      <c r="U4" s="347"/>
+      <c r="U4" s="346"/>
       <c r="V4" s="87" t="s">
         <v>196</v>
       </c>
@@ -24049,7 +24068,7 @@
       <c r="AD4" s="87" t="s">
         <v>188</v>
       </c>
-      <c r="AE4" s="347"/>
+      <c r="AE4" s="346"/>
       <c r="AF4" s="87" t="s">
         <v>187</v>
       </c>
@@ -24059,7 +24078,7 @@
       <c r="AH4" s="87" t="s">
         <v>83</v>
       </c>
-      <c r="AI4" s="347"/>
+      <c r="AI4" s="346"/>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A5" s="93" t="s">

</xml_diff>

<commit_message>
update mme DE JONG full matrice
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A7E359-D53B-D241-8BBF-656D9D6D4728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3995F21F-6950-954B-9481-B601979F7EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" activeTab="2" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
   <sheets>
     <sheet name="ACCUEIL" sheetId="33" r:id="rId1"/>
@@ -5289,7 +5289,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="32">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5473,6 +5473,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5955,7 +5961,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="357">
+  <cellXfs count="359">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -7145,6 +7151,14 @@
     </xf>
     <xf numFmtId="0" fontId="53" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="24" fillId="32" borderId="12" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="65" fillId="13" borderId="12" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
       <protection hidden="1"/>
     </xf>
   </cellXfs>
@@ -7156,27 +7170,7 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{6FC886D6-2077-B34D-B1DF-739B068A66D1}"/>
     <cellStyle name="Normal 3" xfId="4" xr:uid="{6BD57324-3FD5-D341-A299-730D14794802}"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="17">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -7336,6 +7330,16 @@
       <font>
         <color theme="0"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -8094,7 +8098,7 @@
   </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -8350,7 +8354,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20179,8 +20183,8 @@
   </sheetPr>
   <dimension ref="A1:FJ4"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView showFormulas="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="FD2" sqref="FD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20272,7 +20276,7 @@
   </sheetData>
   <autoFilter ref="A2:DT2" xr:uid="{3B89445B-6ECC-4440-B85C-E593AE209933}"/>
   <conditionalFormatting sqref="A1:FG1048576">
-    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="1" stopIfTrue="1">
       <formula>AND(OR($N1&lt;&gt;"-",$O1&lt;&gt;0,$P1&lt;&gt;0),ROW()&gt;2,$A1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20289,8 +20293,8 @@
   </sheetPr>
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20468,7 +20472,7 @@
         <v>399</v>
       </c>
       <c r="G6" s="19" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FG:$FG,"M-TIT",'ETPT Format DDG'!$C:$C,$A$3)</f>
+        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FG,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FG:$FG,"M-TIT",'ETPT Format DDG'!$C:$C,$A$3)</f>
         <v>#N/A</v>
       </c>
       <c r="H6" s="298" t="str">
@@ -20476,16 +20480,16 @@
         <v/>
       </c>
       <c r="I6" s="18" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FG:$FG,"M-PLAC-ADD",'ETPT Format DDG'!$C:$C,$A$3)</f>
+        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FG,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FG:$FG,"M-PLAC-ADD",'ETPT Format DDG'!$C:$C,$A$3)</f>
         <v>#N/A</v>
       </c>
       <c r="J6" s="18" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FG:$FG,"M-PLAC-SUB",'ETPT Format DDG'!$C:$C,$A$3)</f>
+        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FG,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FG:$FG,"M-PLAC-SUB",'ETPT Format DDG'!$C:$C,$A$3)</f>
         <v>#N/A</v>
       </c>
       <c r="K6" s="18" t="e">
         <f>SUMIFS(
-INDEX('ETPT Format DDG'!$A:$DU,
+INDEX('ETPT Format DDG'!$A:$FG,
 ,
 IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))
 ),'ETPT Format DDG'!$FG:$FG,"C",
@@ -20495,7 +20499,7 @@
       </c>
       <c r="L6" s="19" t="e">
         <f>ROUND(SUMIFS(
-INDEX('ETPT Format DDG'!$A:$DU,
+INDEX('ETPT Format DDG'!$A:$FG,
 ,
 IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))
 ),
@@ -20508,7 +20512,7 @@
         <v/>
       </c>
       <c r="N6" s="18" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FG:$FG,"F-TIT",'ETPT Format DDG'!$C:$C,$A$3)</f>
+        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FG,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FG:$FG,"F-TIT",'ETPT Format DDG'!$C:$C,$A$3)</f>
         <v>#N/A</v>
       </c>
       <c r="O6" s="298" t="str">
@@ -20516,20 +20520,20 @@
         <v/>
       </c>
       <c r="P6" s="18" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FG:$FG,"F-PLAC-ADD",'ETPT Format DDG'!$C:$C,$A$3)</f>
+        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FG,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FG:$FG,"F-PLAC-ADD",'ETPT Format DDG'!$C:$C,$A$3)</f>
         <v>#N/A</v>
       </c>
       <c r="Q6" s="18" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FG:$FG,"F-PLAC-SUB",'ETPT Format DDG'!$C:$C,$A$3)</f>
+        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FG,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FG:$FG,"F-PLAC-SUB",'ETPT Format DDG'!$C:$C,$A$3)</f>
         <v>#N/A</v>
       </c>
       <c r="R6" s="18" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FG:$FG,"C",'ETPT Format DDG'!$C:$C,$A$3,'ETPT Format DDG'!$G:$G,"Greffe")</f>
+        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FG,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FG:$FG,"C",'ETPT Format DDG'!$C:$C,$A$3,'ETPT Format DDG'!$G:$G,"Greffe")</f>
         <v>#N/A</v>
       </c>
       <c r="S6" s="19" t="e">
         <f>ROUND(SUMIFS(
-INDEX('ETPT Format DDG'!$A:$DU,
+INDEX('ETPT Format DDG'!$A:$FG,
 ,
 IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))
 ),
@@ -20543,7 +20547,7 @@
       </c>
       <c r="U6" s="19" t="e">
         <f>ROUND(SUMIFS(
-INDEX('ETPT Format DDG'!$A:$DU,
+INDEX('ETPT Format DDG'!$A:$FG,
 ,
 IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))
 ),'ETPT Format DDG'!$FG:$FG,"C",
@@ -20587,70 +20591,70 @@
     <mergeCell ref="U4:V4"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:F4">
-    <cfRule type="expression" dxfId="17" priority="16">
+    <cfRule type="expression" dxfId="15" priority="16">
       <formula>IF(LEFT($A$3,2)&lt;&gt;"TJ",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:V151">
-    <cfRule type="expression" dxfId="16" priority="18">
+    <cfRule type="expression" dxfId="14" priority="18">
       <formula>AND(ISBLANK($C6)=FALSE,ISBLANK($E6)=TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:F1048576">
-    <cfRule type="expression" dxfId="15" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="1" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($U1)-(_xlfn.NUMBERVALUE($U2)+_xlfn.NUMBERVALUE($U3)+_xlfn.NUMBERVALUE($U4)+_xlfn.NUMBERVALUE($U5)+_xlfn.NUMBERVALUE($U6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="2" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($S1)-(_xlfn.NUMBERVALUE($S2)+_xlfn.NUMBERVALUE($S3)+_xlfn.NUMBERVALUE($S4)+_xlfn.NUMBERVALUE($S5)+_xlfn.NUMBERVALUE($S6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="7" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3)+_xlfn.NUMBERVALUE($L4)-_xlfn.NUMBERVALUE($L5)+_xlfn.NUMBERVALUE($L6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="12" stopIfTrue="1">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",OR(_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3))&lt;&gt;0,_xlfn.NUMBERVALUE($S1)-(_xlfn.NUMBERVALUE($S2)+_xlfn.NUMBERVALUE($S3))&lt;&gt;0,_xlfn.NUMBERVALUE($U1)-(_xlfn.NUMBERVALUE($U2)+_xlfn.NUMBERVALUE($U3))&lt;&gt;0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:F7">
-    <cfRule type="expression" dxfId="11" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="6" stopIfTrue="1">
       <formula>OR(_xlfn.NUMBERVALUE($L7)&lt;&gt;_xlfn.NUMBERVALUE($L6),_xlfn.NUMBERVALUE($S7)&lt;&gt;_xlfn.NUMBERVALUE($S6),_xlfn.NUMBERVALUE($U7)&lt;&gt;_xlfn.NUMBERVALUE($U6))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:M1048576">
-    <cfRule type="expression" dxfId="10" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="11" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3)+_xlfn.NUMBERVALUE($L4)+_xlfn.NUMBERVALUE($L5)+_xlfn.NUMBERVALUE($L6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="15">
+    <cfRule type="expression" dxfId="7" priority="15">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3))&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:M7">
-    <cfRule type="expression" dxfId="8" priority="5">
+    <cfRule type="expression" dxfId="6" priority="5">
       <formula>_xlfn.NUMBERVALUE($L7)&lt;&gt;_xlfn.NUMBERVALUE($L6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:T1048576">
-    <cfRule type="expression" dxfId="7" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="10" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($S1)-(_xlfn.NUMBERVALUE($S2)+_xlfn.NUMBERVALUE($S3)+_xlfn.NUMBERVALUE($S4)+_xlfn.NUMBERVALUE($S5)+_xlfn.NUMBERVALUE($S6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="14">
+    <cfRule type="expression" dxfId="4" priority="14">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",_xlfn.NUMBERVALUE($S1)-(_xlfn.NUMBERVALUE($S2)+_xlfn.NUMBERVALUE($S3))&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7:T7">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>_xlfn.NUMBERVALUE($S7)&lt;&gt;_xlfn.NUMBERVALUE($S6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:V1048576">
-    <cfRule type="expression" dxfId="4" priority="9">
+    <cfRule type="expression" dxfId="2" priority="9">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($U1)-(_xlfn.NUMBERVALUE($U2)+_xlfn.NUMBERVALUE($U3)+_xlfn.NUMBERVALUE($U4)+_xlfn.NUMBERVALUE($U5)+_xlfn.NUMBERVALUE($U6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="13">
+    <cfRule type="expression" dxfId="1" priority="13">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",_xlfn.NUMBERVALUE($U1)-(_xlfn.NUMBERVALUE($U2)+_xlfn.NUMBERVALUE($U3))&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U7:V7">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>_xlfn.NUMBERVALUE($U7)&lt;&gt;_xlfn.NUMBERVALUE($U6)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21023,12 +21027,12 @@
   </sheetPr>
   <dimension ref="A1:BJ24"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="139" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G12" activePane="bottomRight" state="frozen"/>
+    <sheetView topLeftCell="D1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
-      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomRight" activeCell="AJ6" sqref="AJ6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21705,46 +21709,42 @@
       <c r="AQ5" s="75"/>
       <c r="AR5" s="75"/>
       <c r="AS5" s="58" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("1.1. DÉPARTAGE PRUD'HOMAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("1.1. DÉPARTAGE PRUD'HOMAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")+
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("1.1. DÉPARTAGE PRUD'HOMAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")</f>
         <v>#N/A</v>
       </c>
       <c r="AT5" s="56" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("4.0. CONTENTIEUX GÉNÉRAL &lt;10.000€",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("4.0. CONTENTIEUX GÉNÉRAL &lt;10.000€",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")+
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("4.0. CONTENTIEUX GÉNÉRAL &lt;10.000€",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")</f>
         <v>#N/A</v>
       </c>
       <c r="AU5" s="56" t="e">
         <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("3.43. INJONCTIONS DE PAYER",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")+
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("3.44. SAISIE DES RÉMUNÉRATIONS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")</f>
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("3.43. INJONCTIONS DE PAYER",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")+
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("3.44. SAISIE DES RÉMUNÉRATIONS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")+
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("3.44. SAISIE DES RÉMUNÉRATIONS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")</f>
         <v>#N/A</v>
       </c>
       <c r="AV5" s="56" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("1. TOTAL CONTENTIEUX SOCIAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")-
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("1.1. DÉPARTAGE PRUD'HOMAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("1. TOTAL CONTENTIEUX SOCIAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")+
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("1. TOTAL CONTENTIEUX SOCIAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")-
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("1.1. DÉPARTAGE PRUD'HOMAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")-
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("1.1. DÉPARTAGE PRUD'HOMAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")</f>
         <v>#N/A</v>
       </c>
       <c r="AW5" s="165" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("2. TOTAL CONTENTIEUX JAF",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("2. TOTAL CONTENTIEUX JAF",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")+
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("2. TOTAL CONTENTIEUX JAF",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")</f>
         <v>#N/A</v>
       </c>
       <c r="AX5" s="58" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilés sur la période (contentieux civils et sociaux)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")-
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("3. TOTAL CONTENTIEUX DE LA PROTECTION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")+
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("3.43. INJONCTIONS DE PAYER",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")+
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("3.44. SAISIE DES RÉMUNÉRATIONS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")-
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("6.1. ACTIVITÉ CIVILE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")-
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("5. TOTAL JLD CIVIL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("4. TOTAL CIVIL NON SPÉCIALISÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")-
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("4.0. CONTENTIEUX GÉNÉRAL &lt;10.000€",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")</f>
         <v>#N/A</v>
       </c>
       <c r="AY5" s="58" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilés sur la période (contentieux civils et sociaux)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")-
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("3.2. PROTECTION DES MAJEURS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")-
-(SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("3. TOTAL CONTENTIEUX DE LA PROTECTION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")-
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("3.2. PROTECTION DES MAJEURS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")-
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("3.43. INJONCTIONS DE PAYER",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")-
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("3.44. SAISIE DES RÉMUNÉRATIONS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS"))-
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("6.1. ACTIVITÉ CIVILE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")-
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("5. TOTAL JLD CIVIL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")-
-SUM(AS5:AW5)</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("4. TOTAL CIVIL NON SPÉCIALISÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")-
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("4.0. CONTENTIEUX GÉNÉRAL &lt;10.000€",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")</f>
         <v>#N/A</v>
       </c>
       <c r="AZ5" s="49" t="e">
@@ -21944,7 +21944,15 @@
 SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("8.4. AUTRES SECTIONS SPÉCIALISÉES",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")-
 SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9. TOTAL JAP",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")-
 SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("6.2. ACTIVITÉ PÉNALE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")-
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("10. TOTAL JLD PÉNAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")</f>
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("10. TOTAL JLD PÉNAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")-
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("7.5. COUR D'ASSISES HORS JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")-
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("7.51. COUR D'ASSISES JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")-
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("7.52. COUR CRIMINELLE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")-
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("7.121. COLLÉGIALES JIRS ECO-FI",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")-
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("7.12. COLLÉGIALES JIRS CRIM-ORG",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")-
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("7.122. COLLÉGIALES AUTRES SECTIONS SPÉCIALISÉES",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")-
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("7.6. TRIBUNAL DE POLICE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")-
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("7.7. OP CONTRAVENTIONNELLES",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")</f>
         <v>#N/A</v>
       </c>
       <c r="AY6" s="74" t="e">
@@ -21956,7 +21964,14 @@
 SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9. TOTAL JAP",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")-
 SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("6.2. ACTIVITÉ PÉNALE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")-
 SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("10. TOTAL JLD PÉNAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")-
-SUM(AM6:AW6)</f>
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("7.5. COUR D'ASSISES HORS JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")-
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("7.51. COUR D'ASSISES JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")-
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("7.52. COUR CRIMINELLE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")-
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("7.121. COLLÉGIALES JIRS ECO-FI",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")-
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("7.12. COLLÉGIALES JIRS CRIM-ORG",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")-
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("7.122. COLLÉGIALES AUTRES SECTIONS SPÉCIALISÉES",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")-
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("7.6. TRIBUNAL DE POLICE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")-
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("7.7. OP CONTRAVENTIONNELLES",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")</f>
         <v>#N/A</v>
       </c>
       <c r="AZ6" s="49" t="e">
@@ -22730,13 +22745,19 @@
       <c r="AD12" s="56" t="e">
         <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"JCP")+
 SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"VPCP")+
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"1VPCP")</f>
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"1VPCP")-
+(SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"JCP")+
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"VPCP")+
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"1VPCP"))</f>
         <v>#N/A</v>
       </c>
       <c r="AE12" s="56" t="e">
         <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"JI")+
 SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"VPI")+
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"1VPI")</f>
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"1VPI")-
+(SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"JI")+
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"VPI")+
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"1VPI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AF12" s="66"/>
@@ -22745,18 +22766,26 @@
       <c r="AI12" s="56" t="e">
         <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"JAP")+
 SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"VPAP")+
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"1VPAP")</f>
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"1VPAP")-
+(SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"JAP")+
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"VPAP")+
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"1VPAP"))</f>
         <v>#N/A</v>
       </c>
       <c r="AJ12" s="56" t="e">
         <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"JE")+
 SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"VPE")+
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"1VPE")</f>
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"1VPE")-
+(SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"JE")+
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"VPE")+
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"1VPE"))</f>
         <v>#N/A</v>
       </c>
       <c r="AK12" s="56" t="e">
         <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"VPLD")+
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"1VPLD")</f>
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"1VPLD")-
+(SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"VPLD")+
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"1VPLD"))</f>
         <v>#N/A</v>
       </c>
       <c r="AL12" s="49" t="e">
@@ -22776,7 +22805,8 @@
       <c r="AW12" s="66"/>
       <c r="AX12" s="66"/>
       <c r="AY12" s="56" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")-
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")</f>
         <v>#N/A</v>
       </c>
       <c r="AZ12" s="49" t="e">
@@ -22912,7 +22942,7 @@
       <c r="AW13" s="66"/>
       <c r="AX13" s="66"/>
       <c r="AY13" s="303" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$H:$H,"Magistrat SIEGE NS")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")</f>
         <v>#N/A</v>
       </c>
       <c r="AZ13" s="49" t="e">
@@ -22949,13 +22979,13 @@
       <c r="F14" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="G14" s="63">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilé sur la période (y.c. indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH placé ADD")</f>
-        <v>0</v>
-      </c>
-      <c r="H14" s="62">
+      <c r="G14" s="63" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("ETPT sur la période hors indisponibilités",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH placé ADD")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H14" s="62" t="e">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="I14" s="61" t="e">
         <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.8. FONCTIONNAIRES AFFECTÉS AUX ACTIVITÉS CIVILES ET COMMERCIALES DU PARQUET",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")</f>
@@ -23023,7 +23053,7 @@
         <v>#N/A</v>
       </c>
       <c r="V14" s="166" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilé sur la période (y.c. indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")-
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("ETPT sur la période hors indisponibilités",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")-
 SUM(I14:U14)-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.7. FONCTIONNAIRES AFFECTÉS AU CPH",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH placé ADD")</f>
         <v>#N/A</v>
       </c>
@@ -23134,7 +23164,7 @@
       </c>
       <c r="AX14" s="57"/>
       <c r="AY14" s="56" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilé sur la période (y.c. indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé ADD")-SUM(AC14:AK14)-SUM(AM14:AX14)</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("ETPT sur la période hors indisponibilités",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé ADD")-SUM(AC14:AK14)-SUM(AM14:AX14)</f>
         <v>#N/A</v>
       </c>
       <c r="AZ14" s="49" t="e">
@@ -23171,13 +23201,13 @@
       <c r="F15" s="64" t="s">
         <v>51</v>
       </c>
-      <c r="G15" s="63">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilé sur la période (y.c. indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH placé SUB")</f>
-        <v>0</v>
-      </c>
-      <c r="H15" s="62">
+      <c r="G15" s="63" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("ETPT sur la période hors indisponibilités",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH placé SUB")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H15" s="62" t="e">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="I15" s="61" t="e">
         <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.8. FONCTIONNAIRES AFFECTÉS AUX ACTIVITÉS CIVILES ET COMMERCIALES DU PARQUET",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")</f>
@@ -23245,7 +23275,7 @@
         <v>#N/A</v>
       </c>
       <c r="V15" s="166" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilé sur la période (y.c. indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")-
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("ETPT sur la période hors indisponibilités",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")-
 SUM(I15:U15)-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.7. FONCTIONNAIRES AFFECTÉS AU CPH",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH placé SUB")</f>
         <v>#N/A</v>
       </c>
@@ -23356,7 +23386,7 @@
       </c>
       <c r="AX15" s="57"/>
       <c r="AY15" s="56" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilé sur la période (y.c. indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé SUB")-SUM(AC15:AK15)-SUM(AM15:AX15)</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("ETPT sur la période hors indisponibilités",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé SUB")-SUM(AC15:AK15)-SUM(AM15:AX15)</f>
         <v>#N/A</v>
       </c>
       <c r="AZ15" s="49" t="e">
@@ -23751,11 +23781,11 @@
   </sheetPr>
   <dimension ref="A1:AI19"/>
   <sheetViews>
-    <sheetView zoomScale="161" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="O13" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="141" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="6" ySplit="1" topLeftCell="AC6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R19" sqref="R19"/>
+      <selection pane="bottomRight" activeCell="AH18" sqref="AH18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24159,8 +24189,8 @@
         <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("3.2. PROTECTION DES MAJEURS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")</f>
         <v>#N/A</v>
       </c>
-      <c r="Z5" s="164"/>
-      <c r="AA5" s="164"/>
+      <c r="Z5" s="57"/>
+      <c r="AA5" s="57"/>
       <c r="AB5" s="57"/>
       <c r="AC5" s="57"/>
       <c r="AD5" s="57"/>
@@ -24174,7 +24204,11 @@
         <v>#N/A</v>
       </c>
       <c r="AH5" s="56" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilés sur la période (contentieux civils et sociaux)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")-SUM(V5:AD5)-AF5-AG5-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("6.1. ACTIVITÉ CIVILE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("5. TOTAL JLD CIVIL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("2. TOTAL CONTENTIEUX JAF",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilés sur la période (contentieux civils et sociaux)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("3. TOTAL CONTENTIEUX DE LA PROTECTION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")-
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("1.1. DÉPARTAGE PRUD'HOMAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")-
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("6.1. ACTIVITÉ CIVILE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")-
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("5. TOTAL JLD CIVIL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")-
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("2. TOTAL CONTENTIEUX JAF",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")</f>
         <v>#N/A</v>
       </c>
       <c r="AI5" s="94" t="e">
@@ -24287,8 +24321,8 @@
       <c r="W7" s="66"/>
       <c r="X7" s="66"/>
       <c r="Y7" s="66"/>
-      <c r="Z7" s="66"/>
-      <c r="AA7" s="66"/>
+      <c r="Z7" s="57"/>
+      <c r="AA7" s="57"/>
       <c r="AB7" s="57"/>
       <c r="AC7" s="57"/>
       <c r="AD7" s="57"/>
@@ -24357,8 +24391,8 @@
       <c r="W8" s="66"/>
       <c r="X8" s="66"/>
       <c r="Y8" s="66"/>
-      <c r="Z8" s="66"/>
-      <c r="AA8" s="66"/>
+      <c r="Z8" s="57"/>
+      <c r="AA8" s="57"/>
       <c r="AB8" s="57"/>
       <c r="AC8" s="57"/>
       <c r="AD8" s="57"/>
@@ -24368,13 +24402,10 @@
       </c>
       <c r="AF8" s="66"/>
       <c r="AG8" s="66"/>
-      <c r="AH8" s="61" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.51. ACCUEIL DU JUSTICIABLE (DONT SAUJ)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AI8" s="94" t="e">
+      <c r="AH8" s="66"/>
+      <c r="AI8" s="94">
         <f t="shared" si="4"/>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.2">
@@ -24437,8 +24468,8 @@
       <c r="W9" s="66"/>
       <c r="X9" s="66"/>
       <c r="Y9" s="66"/>
-      <c r="Z9" s="66"/>
-      <c r="AA9" s="66"/>
+      <c r="Z9" s="57"/>
+      <c r="AA9" s="57"/>
       <c r="AB9" s="57"/>
       <c r="AC9" s="57"/>
       <c r="AD9" s="57"/>
@@ -24512,8 +24543,8 @@
       <c r="W10" s="66"/>
       <c r="X10" s="66"/>
       <c r="Y10" s="66"/>
-      <c r="Z10" s="66"/>
-      <c r="AA10" s="66"/>
+      <c r="Z10" s="57"/>
+      <c r="AA10" s="57"/>
       <c r="AB10" s="57"/>
       <c r="AC10" s="57"/>
       <c r="AD10" s="57"/>
@@ -24585,8 +24616,8 @@
       <c r="W11" s="66"/>
       <c r="X11" s="66"/>
       <c r="Y11" s="66"/>
-      <c r="Z11" s="66"/>
-      <c r="AA11" s="66"/>
+      <c r="Z11" s="57"/>
+      <c r="AA11" s="57"/>
       <c r="AB11" s="57"/>
       <c r="AC11" s="57"/>
       <c r="AD11" s="57"/>
@@ -24661,8 +24692,8 @@
       <c r="W12" s="66"/>
       <c r="X12" s="66"/>
       <c r="Y12" s="66"/>
-      <c r="Z12" s="66"/>
-      <c r="AA12" s="66"/>
+      <c r="Z12" s="57"/>
+      <c r="AA12" s="57"/>
       <c r="AB12" s="57"/>
       <c r="AC12" s="57"/>
       <c r="AD12" s="57"/>
@@ -24673,7 +24704,8 @@
       <c r="AF12" s="66"/>
       <c r="AG12" s="66"/>
       <c r="AH12" s="56" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")-
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")</f>
         <v>#N/A</v>
       </c>
       <c r="AI12" s="94" t="e">
@@ -24734,8 +24766,8 @@
       <c r="W13" s="66"/>
       <c r="X13" s="66"/>
       <c r="Y13" s="66"/>
-      <c r="Z13" s="66"/>
-      <c r="AA13" s="66"/>
+      <c r="Z13" s="57"/>
+      <c r="AA13" s="57"/>
       <c r="AB13" s="57"/>
       <c r="AC13" s="57"/>
       <c r="AD13" s="57"/>
@@ -24745,7 +24777,7 @@
       </c>
       <c r="AF13" s="66"/>
       <c r="AG13" s="66"/>
-      <c r="AH13" s="303" t="e">
+      <c r="AH13" s="358" t="e">
         <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")</f>
         <v>#N/A</v>
       </c>
@@ -24770,13 +24802,13 @@
       <c r="F14" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="G14" s="63">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilé sur la période (y.c. indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH placé ADD")</f>
-        <v>0</v>
-      </c>
-      <c r="H14" s="94">
+      <c r="G14" s="63" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("ETPT sur la période hors indisponibilités",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH placé ADD")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H14" s="94" t="e">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="I14" s="95"/>
       <c r="J14" s="61" t="e">
@@ -24800,8 +24832,9 @@
       <c r="O14" s="57"/>
       <c r="P14" s="57"/>
       <c r="Q14" s="66"/>
-      <c r="R14" s="166" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilé sur la période (y.c. indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")-SUM(I14:Q14)-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.7. FONCTIONNAIRES AFFECTÉS AU CPH",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH placé ADD")</f>
+      <c r="R14" s="357" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("ETPT sur la période hors indisponibilités",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")-SUM(I14:Q14)-
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.7. FONCTIONNAIRES AFFECTÉS AU CPH",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH placé ADD")</f>
         <v>#N/A</v>
       </c>
       <c r="S14" s="49" t="e">
@@ -24830,13 +24863,13 @@
         <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("3.2. PROTECTION DES MAJEURS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé ADD")</f>
         <v>#N/A</v>
       </c>
-      <c r="Z14" s="164"/>
-      <c r="AA14" s="164"/>
+      <c r="Z14" s="57"/>
+      <c r="AA14" s="57"/>
       <c r="AB14" s="57"/>
       <c r="AC14" s="57"/>
       <c r="AD14" s="57"/>
       <c r="AE14" s="94" t="e">
-        <f t="shared" si="3"/>
+        <f>SUM(V14:AD14)</f>
         <v>#N/A</v>
       </c>
       <c r="AF14" s="57"/>
@@ -24844,8 +24877,8 @@
         <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("1.1. DÉPARTAGE PRUD'HOMAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé ADD")</f>
         <v>#N/A</v>
       </c>
-      <c r="AH14" s="165" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilé sur la période (y.c. indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé ADD")-SUM(AE14:AG14)</f>
+      <c r="AH14" s="56" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("ETPT sur la période hors indisponibilités",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé ADD")-SUM(V14:AD14)-SUM(AF14:AG14)</f>
         <v>#N/A</v>
       </c>
       <c r="AI14" s="94" t="e">
@@ -24869,13 +24902,13 @@
       <c r="F15" s="65" t="s">
         <v>51</v>
       </c>
-      <c r="G15" s="63">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilé sur la période (y.c. indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH placé SUB")</f>
-        <v>0</v>
-      </c>
-      <c r="H15" s="94">
+      <c r="G15" s="63" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("ETPT sur la période hors indisponibilités",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH placé SUB")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H15" s="94" t="e">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="I15" s="95"/>
       <c r="J15" s="61" t="e">
@@ -24899,8 +24932,9 @@
       <c r="O15" s="57"/>
       <c r="P15" s="57"/>
       <c r="Q15" s="66"/>
-      <c r="R15" s="166" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilé sur la période (y.c. indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")-SUM(I15:Q15)-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.7. FONCTIONNAIRES AFFECTÉS AU CPH",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH placé SUB")</f>
+      <c r="R15" s="357" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("ETPT sur la période hors indisponibilités",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")-SUM(I15:Q15)-
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.7. FONCTIONNAIRES AFFECTÉS AU CPH",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH placé SUB")</f>
         <v>#N/A</v>
       </c>
       <c r="S15" s="49" t="e">
@@ -24929,8 +24963,8 @@
         <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("3.2. PROTECTION DES MAJEURS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé SUB")</f>
         <v>#N/A</v>
       </c>
-      <c r="Z15" s="164"/>
-      <c r="AA15" s="164"/>
+      <c r="Z15" s="57"/>
+      <c r="AA15" s="57"/>
       <c r="AB15" s="57"/>
       <c r="AC15" s="57"/>
       <c r="AD15" s="57"/>
@@ -24943,8 +24977,8 @@
         <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("1.1. DÉPARTAGE PRUD'HOMAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé SUB")</f>
         <v>#N/A</v>
       </c>
-      <c r="AH15" s="165" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilé sur la période (y.c. indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé SUB")-SUM(AE15:AG15)</f>
+      <c r="AH15" s="56" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("ETPT sur la période hors indisponibilités",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé SUB")-SUM(V15:AD15)-SUM(AF15:AG15)</f>
         <v>#N/A</v>
       </c>
       <c r="AI15" s="94" t="e">

</xml_diff>

<commit_message>
extractor add ns tprox W X Y col
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3995F21F-6950-954B-9481-B601979F7EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C54CD53-D25B-7142-9BDF-EB6E9B501194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
@@ -21028,11 +21028,11 @@
   <dimension ref="A1:BJ24"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="AV2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
-      <selection pane="bottomRight" activeCell="AJ6" sqref="AJ6"/>
+      <selection pane="bottomRight" activeCell="AY9" sqref="AY9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23782,10 +23782,10 @@
   <dimension ref="A1:AI19"/>
   <sheetViews>
     <sheetView zoomScale="141" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="AC6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AH18" sqref="AH18"/>
+      <selection pane="bottomRight" activeCell="AB5" sqref="AB5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24175,18 +24175,25 @@
       <c r="V5" s="60"/>
       <c r="W5" s="61" t="e">
         <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("3.43. INJONCTIONS DE PAYER",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")+
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("3.44. SAISIE DES RÉMUNÉRATIONS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")+
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("3.43. INJONCTIONS DE PAYER",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")+
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("3.44. SAISIE DES RÉMUNÉRATIONS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="X5" s="61" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("3. TOTAL CONTENTIEUX DE LA PROTECTION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")+
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("3. TOTAL CONTENTIEUX DE LA PROTECTION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")-
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("3.2. PROTECTION DES MAJEURS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")-
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("3.2. PROTECTION DES MAJEURS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")-
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("3.43. INJONCTIONS DE PAYER",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")-
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("3.43. INJONCTIONS DE PAYER",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")-
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("3.44. SAISIE DES RÉMUNÉRATIONS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")-
 SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("3.44. SAISIE DES RÉMUNÉRATIONS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")</f>
         <v>#N/A</v>
       </c>
-      <c r="X5" s="61" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("3. TOTAL CONTENTIEUX DE LA PROTECTION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")-
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("3.2. PROTECTION DES MAJEURS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")-
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("3.43. INJONCTIONS DE PAYER",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")-
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("3.44. SAISIE DES RÉMUNÉRATIONS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")</f>
-        <v>#N/A</v>
-      </c>
       <c r="Y5" s="61" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("3.2. PROTECTION DES MAJEURS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("3.2. PROTECTION DES MAJEURS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE S")+
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("3.2. PROTECTION DES MAJEURS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE NS")</f>
         <v>#N/A</v>
       </c>
       <c r="Z5" s="57"/>

</xml_diff>

<commit_message>
automatisation des formules CA
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -8,29 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD38D8C-2855-4A4F-8DA1-232A21640553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26444862-8F27-8C4D-A082-DAFA947950F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
   <sheets>
     <sheet name="ACCUEIL" sheetId="33" r:id="rId1"/>
     <sheet name="ETPT A-JUST" sheetId="1" r:id="rId2"/>
     <sheet name="ETPT Format DDG" sheetId="9" r:id="rId3"/>
     <sheet name="Agrégats DDG" sheetId="10" r:id="rId4"/>
-    <sheet name="codage tribunal" sheetId="12" r:id="rId5"/>
-    <sheet name="Juridictions" sheetId="17" r:id="rId6"/>
-    <sheet name="Table_Fonctions" sheetId="19" r:id="rId7"/>
-    <sheet name="ETPT_TJ" sheetId="25" r:id="rId8"/>
-    <sheet name="ETPT_TPRX" sheetId="26" r:id="rId9"/>
-    <sheet name="ETPT_CPH" sheetId="27" r:id="rId10"/>
+    <sheet name="codage tribunal" sheetId="12" state="hidden" r:id="rId5"/>
+    <sheet name="Juridictions" sheetId="17" state="hidden" r:id="rId6"/>
+    <sheet name="Table_Fonctions" sheetId="19" state="hidden" r:id="rId7"/>
+    <sheet name="ETPT_TJ" sheetId="25" state="hidden" r:id="rId8"/>
+    <sheet name="ETPT_TPRX" sheetId="26" state="hidden" r:id="rId9"/>
+    <sheet name="ETPT_CPH" sheetId="27" state="hidden" r:id="rId10"/>
     <sheet name="ETPT_TJ_DDG" sheetId="28" r:id="rId11"/>
     <sheet name="ETPT_TPRX_DDG" sheetId="29" r:id="rId12"/>
     <sheet name="ETPT_CPH_DDG" sheetId="30" r:id="rId13"/>
-    <sheet name="ETPT_TJ_corresp-SIEGE-TJ" sheetId="24" r:id="rId14"/>
-    <sheet name="ETPT_TPROX_corresp-SIEGE-TPROX" sheetId="34" r:id="rId15"/>
-    <sheet name="ETPT_TJ_corresp-GREFFE-TJ" sheetId="35" r:id="rId16"/>
-    <sheet name="ETPT_TROX_corresp-GREFFE-TPROX" sheetId="36" r:id="rId17"/>
-    <sheet name="ETPT_CPH_corresp-GREFFE-CPH" sheetId="37" r:id="rId18"/>
+    <sheet name="ETPT_TJ_corresp-SIEGE-TJ" sheetId="24" state="hidden" r:id="rId14"/>
+    <sheet name="ETPT_TPROX_corresp-SIEGE-TPROX" sheetId="34" state="hidden" r:id="rId15"/>
+    <sheet name="ETPT_TJ_corresp-GREFFE-TJ" sheetId="35" state="hidden" r:id="rId16"/>
+    <sheet name="ETPT_TROX_corresp-GREFFE-TPROX" sheetId="36" state="hidden" r:id="rId17"/>
+    <sheet name="ETPT_CPH_corresp-GREFFE-CPH" sheetId="37" state="hidden" r:id="rId18"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ETPT A-JUST'!$A$2:$DN$2</definedName>
@@ -8083,7 +8083,7 @@
   </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -8727,7 +8727,7 @@
   </sheetPr>
   <dimension ref="A1:BK21"/>
   <sheetViews>
-    <sheetView topLeftCell="AS1" zoomScale="125" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="125" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -20168,7 +20168,7 @@
   </sheetPr>
   <dimension ref="A1:FE4"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" zoomScale="94" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showFormulas="1" zoomScale="94" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>

</xml_diff>

<commit_message>
maj mise en forme onglet agregat ddg
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26444862-8F27-8C4D-A082-DAFA947950F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F68F44F-B77B-2C4A-9B96-14988F96AD57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
   <sheets>
     <sheet name="ACCUEIL" sheetId="33" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1584" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1584" uniqueCount="432">
   <si>
     <t>#! END_ROW</t>
   </si>
@@ -4762,6 +4762,9 @@
   </si>
   <si>
     <t>Fonction agrégat</t>
+  </si>
+  <si>
+    <t>#! DUMP_COLS subtitles1</t>
   </si>
 </sst>
 </file>
@@ -20172,7 +20175,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20199,7 +20202,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6" t="s">
-        <v>6</v>
+        <v>431</v>
       </c>
       <c r="FA1" s="320" t="s">
         <v>232</v>

</xml_diff>

<commit_message>
size of column extractor resize
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F68F44F-B77B-2C4A-9B96-14988F96AD57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1CFD4B4-6148-7D41-8052-F1C174D564C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" activeTab="2" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
   <sheets>
     <sheet name="ACCUEIL" sheetId="33" r:id="rId1"/>
@@ -5949,7 +5949,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="359">
+  <cellXfs count="360">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -7148,6 +7148,9 @@
     <xf numFmtId="0" fontId="53" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -8086,7 +8089,7 @@
   </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -20171,11 +20174,11 @@
   </sheetPr>
   <dimension ref="A1:FE4"/>
   <sheetViews>
-    <sheetView showFormulas="1" zoomScale="94" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showFormulas="1" tabSelected="1" zoomScale="58" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20235,6 +20238,9 @@
       <c r="B3" t="s">
         <v>10</v>
       </c>
+      <c r="N3" s="359"/>
+      <c r="O3" s="359"/>
+      <c r="P3" s="359"/>
     </row>
     <row r="4" spans="1:161" x14ac:dyDescent="0.2">
       <c r="B4" s="27" t="s">

</xml_diff>

<commit_message>
update nomenclature for extractor add jirs param
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B904EEE-7121-DA47-B624-F62FF37BCC9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89872010-548C-AA4A-A687-CB1FFA214E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" activeTab="2" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
@@ -7129,7 +7129,27 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{6FC886D6-2077-B34D-B1DF-739B068A66D1}"/>
     <cellStyle name="Normal 3" xfId="4" xr:uid="{6BD57324-3FD5-D341-A299-730D14794802}"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -7289,16 +7309,6 @@
       <font>
         <color theme="0"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -20143,10 +20153,10 @@
   <dimension ref="A1:FD4"/>
   <sheetViews>
     <sheetView showFormulas="1" tabSelected="1" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20212,8 +20222,8 @@
   </sheetData>
   <autoFilter ref="A2:DT2" xr:uid="{3B89445B-6ECC-4440-B85C-E593AE209933}"/>
   <conditionalFormatting sqref="A1:G1 I1:EY1 A2:EZ2 A3:FB1048576">
-    <cfRule type="expression" dxfId="16" priority="1">
-      <formula>AND(OR($P1&lt;&gt;"-",$Q1&lt;&gt;0,$R1&lt;&gt;0),ROW()&gt;2,$A1&lt;&gt;"")</formula>
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+      <formula>AND(OR($Q1&lt;&gt;"-",$R1&lt;&gt;0,$S1&lt;&gt;0),ROW()&gt;2,$A1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20229,8 +20239,8 @@
   </sheetPr>
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="H1" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20408,7 +20418,10 @@
         <v>387</v>
       </c>
       <c r="G6" s="19" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FB,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FB:$FB,"M-TIT",'ETPT Format DDG'!$C:$C,$A$3)</f>
+        <f>SUMIFS(
+INDEX('ETPT Format DDG'!$A:$ZZ,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction agrégat",'ETPT Format DDG'!2:2,0)),"M-TIT",
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$A$3)</f>
         <v>#N/A</v>
       </c>
       <c r="H6" s="294" t="str">
@@ -20416,31 +20429,32 @@
         <v/>
       </c>
       <c r="I6" s="18" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FB,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FB:$FB,"M-PLAC-ADD",'ETPT Format DDG'!$C:$C,$A$3)</f>
+        <f>SUMIFS(
+INDEX('ETPT Format DDG'!$A:$ZZ,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction agrégat",'ETPT Format DDG'!2:2,0)),"M-PLAC-ADD",
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$A$3)</f>
         <v>#N/A</v>
       </c>
       <c r="J6" s="18" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FB,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FB:$FB,"M-PLAC-SUB",'ETPT Format DDG'!$C:$C,$A$3)</f>
+        <f>SUMIFS(
+INDEX('ETPT Format DDG'!$A:$ZZ,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction agrégat",'ETPT Format DDG'!2:2,0)),"M-PLAC-SUB",
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$A$3)</f>
         <v>#N/A</v>
       </c>
       <c r="K6" s="18" t="e">
         <f>SUMIFS(
-INDEX('ETPT Format DDG'!$A:$FB,
-,
-IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))
-),'ETPT Format DDG'!$FB:$FB,"C",
-'ETPT Format DDG'!$C:$C,$A$3,
-'ETPT Format DDG'!$G:$G,"Magistrat")</f>
+INDEX('ETPT Format DDG'!$A:$ZZ,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction agrégat",'ETPT Format DDG'!2:2,0)),"C",
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$A$3,
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Catégorie",'ETPT Format DDG'!2:2,0)),"Magistrat")</f>
         <v>#N/A</v>
       </c>
       <c r="L6" s="19" t="e">
         <f>ROUND(SUMIFS(
-INDEX('ETPT Format DDG'!$A:$FB,
-,
-IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))
-),
-'ETPT Format DDG'!$C:$C,$A$3,
-'ETPT Format DDG'!$G:$G,"Magistrat"),3)</f>
+INDEX('ETPT Format DDG'!$A:$ZZ,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$A$3,
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Catégorie",'ETPT Format DDG'!2:2,0)),"Magistrat"),3)</f>
         <v>#N/A</v>
       </c>
       <c r="M6" s="295" t="str">
@@ -20448,7 +20462,10 @@
         <v/>
       </c>
       <c r="N6" s="18" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FB,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FB:$FB,"F-TIT",'ETPT Format DDG'!$C:$C,$A$3)</f>
+        <f>SUMIFS(
+INDEX('ETPT Format DDG'!$A:$ZZ,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction agrégat",'ETPT Format DDG'!2:2,0)),"F-TIT",
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$A$3)</f>
         <v>#N/A</v>
       </c>
       <c r="O6" s="294" t="str">
@@ -20456,25 +20473,32 @@
         <v/>
       </c>
       <c r="P6" s="18" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FB,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FB:$FB,"F-PLAC-ADD",'ETPT Format DDG'!$C:$C,$A$3)</f>
+        <f>SUMIFS(
+INDEX('ETPT Format DDG'!$A:$FB,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction agrégat",'ETPT Format DDG'!2:2,0)),"F-PLAC-ADD",
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$A$3)</f>
         <v>#N/A</v>
       </c>
       <c r="Q6" s="18" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FB,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FB:$FB,"F-PLAC-SUB",'ETPT Format DDG'!$C:$C,$A$3)</f>
+        <f>SUMIFS(
+INDEX('ETPT Format DDG'!$A:$FB,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction agrégat",'ETPT Format DDG'!2:2,0)),"F-PLAC-SUB",
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$A$3)</f>
         <v>#N/A</v>
       </c>
       <c r="R6" s="18" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FB,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FB:$FB,"C",'ETPT Format DDG'!$C:$C,$A$3,'ETPT Format DDG'!$G:$G,"Greffe")</f>
+        <f>SUMIFS(
+INDEX('ETPT Format DDG'!$A:$FB,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction agrégat",'ETPT Format DDG'!2:2,0)),"C",
+'ETPT Format DDG'!$G:$G,"Greffe",
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$A$3)</f>
         <v>#N/A</v>
       </c>
       <c r="S6" s="19" t="e">
         <f>ROUND(SUMIFS(
-INDEX('ETPT Format DDG'!$A:$FB,
-,
-IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))
-),
-'ETPT Format DDG'!$C:$C,$A$3,
-'ETPT Format DDG'!$G:$G,"Greffe"),3)</f>
+INDEX('ETPT Format DDG'!$A:$FB,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Catégorie",'ETPT Format DDG'!2:2,0)),"Greffe",
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$A$3),3)</f>
         <v>#N/A</v>
       </c>
       <c r="T6" s="294" t="str">
@@ -20483,12 +20507,10 @@
       </c>
       <c r="U6" s="19" t="e">
         <f>ROUND(SUMIFS(
-INDEX('ETPT Format DDG'!$A:$FB,
-,
-IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))
-),'ETPT Format DDG'!$FB:$FB,"C",
-'ETPT Format DDG'!$C:$C,$A$3,
-'ETPT Format DDG'!$G:$G,"Autour du magistrat"),3)</f>
+INDEX('ETPT Format DDG'!$A:$FB,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction agrégat",'ETPT Format DDG'!2:2,0)),"C",
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$A$3,
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Catégorie",'ETPT Format DDG'!2:2,0)),"Autour du magistrat"),3)</f>
         <v>#N/A</v>
       </c>
       <c r="V6" s="295" t="str">
@@ -20527,70 +20549,70 @@
     <mergeCell ref="U4:V4"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:F4">
-    <cfRule type="expression" dxfId="15" priority="16">
+    <cfRule type="expression" dxfId="17" priority="16">
       <formula>IF(LEFT($A$3,2)&lt;&gt;"TJ",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:V151">
-    <cfRule type="expression" dxfId="14" priority="18">
+    <cfRule type="expression" dxfId="16" priority="18">
       <formula>AND(ISBLANK($C6)=FALSE,ISBLANK($E6)=TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:F1048576">
-    <cfRule type="expression" dxfId="13" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="1" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($U1)-(_xlfn.NUMBERVALUE($U2)+_xlfn.NUMBERVALUE($U3)+_xlfn.NUMBERVALUE($U4)+_xlfn.NUMBERVALUE($U5)+_xlfn.NUMBERVALUE($U6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="2" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($S1)-(_xlfn.NUMBERVALUE($S2)+_xlfn.NUMBERVALUE($S3)+_xlfn.NUMBERVALUE($S4)+_xlfn.NUMBERVALUE($S5)+_xlfn.NUMBERVALUE($S6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="7" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3)+_xlfn.NUMBERVALUE($L4)-_xlfn.NUMBERVALUE($L5)+_xlfn.NUMBERVALUE($L6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="12" stopIfTrue="1">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",OR(_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3))&lt;&gt;0,_xlfn.NUMBERVALUE($S1)-(_xlfn.NUMBERVALUE($S2)+_xlfn.NUMBERVALUE($S3))&lt;&gt;0,_xlfn.NUMBERVALUE($U1)-(_xlfn.NUMBERVALUE($U2)+_xlfn.NUMBERVALUE($U3))&lt;&gt;0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:F7">
-    <cfRule type="expression" dxfId="9" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="6" stopIfTrue="1">
       <formula>OR(_xlfn.NUMBERVALUE($L7)&lt;&gt;_xlfn.NUMBERVALUE($L6),_xlfn.NUMBERVALUE($S7)&lt;&gt;_xlfn.NUMBERVALUE($S6),_xlfn.NUMBERVALUE($U7)&lt;&gt;_xlfn.NUMBERVALUE($U6))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:M1048576">
-    <cfRule type="expression" dxfId="8" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="11" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3)+_xlfn.NUMBERVALUE($L4)+_xlfn.NUMBERVALUE($L5)+_xlfn.NUMBERVALUE($L6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="15">
+    <cfRule type="expression" dxfId="9" priority="15">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3))&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:M7">
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="8" priority="5">
       <formula>_xlfn.NUMBERVALUE($L7)&lt;&gt;_xlfn.NUMBERVALUE($L6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:T1048576">
-    <cfRule type="expression" dxfId="5" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="10" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($S1)-(_xlfn.NUMBERVALUE($S2)+_xlfn.NUMBERVALUE($S3)+_xlfn.NUMBERVALUE($S4)+_xlfn.NUMBERVALUE($S5)+_xlfn.NUMBERVALUE($S6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="14">
+    <cfRule type="expression" dxfId="6" priority="14">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",_xlfn.NUMBERVALUE($S1)-(_xlfn.NUMBERVALUE($S2)+_xlfn.NUMBERVALUE($S3))&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7:T7">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>_xlfn.NUMBERVALUE($S7)&lt;&gt;_xlfn.NUMBERVALUE($S6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:V1048576">
-    <cfRule type="expression" dxfId="2" priority="9">
+    <cfRule type="expression" dxfId="4" priority="9">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($U1)-(_xlfn.NUMBERVALUE($U2)+_xlfn.NUMBERVALUE($U3)+_xlfn.NUMBERVALUE($U4)+_xlfn.NUMBERVALUE($U5)+_xlfn.NUMBERVALUE($U6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="13">
+    <cfRule type="expression" dxfId="3" priority="13">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",_xlfn.NUMBERVALUE($U1)-(_xlfn.NUMBERVALUE($U2)+_xlfn.NUMBERVALUE($U3))&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U7:V7">
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>_xlfn.NUMBERVALUE($U7)&lt;&gt;_xlfn.NUMBERVALUE($U6)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
create Extractor CA VF
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3A6E75-74D1-5945-8006-EE38F7EEDD36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3CA5426-8F3A-E749-BA9A-8EB3AEE04FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
@@ -9690,6 +9690,21 @@
     <xf numFmtId="0" fontId="23" fillId="19" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="38" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -9808,23 +9823,8 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="30" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -10882,11 +10882,11 @@
       <c r="B1" s="115" t="s">
         <v>227</v>
       </c>
-      <c r="C1" s="334" t="s">
+      <c r="C1" s="339" t="s">
         <v>228</v>
       </c>
-      <c r="D1" s="334"/>
-      <c r="E1" s="334"/>
+      <c r="D1" s="339"/>
+      <c r="E1" s="339"/>
       <c r="F1" s="116"/>
       <c r="H1" s="26" t="s">
         <v>0</v>
@@ -10895,11 +10895,11 @@
     <row r="2" spans="1:8" s="120" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="117"/>
       <c r="B2" s="118"/>
-      <c r="C2" s="335" t="s">
+      <c r="C2" s="340" t="s">
         <v>229</v>
       </c>
-      <c r="D2" s="335"/>
-      <c r="E2" s="335"/>
+      <c r="D2" s="340"/>
+      <c r="E2" s="340"/>
       <c r="F2" s="119"/>
       <c r="H2" s="26" t="s">
         <v>0</v>
@@ -10923,10 +10923,10 @@
       <c r="D4" s="125" t="s">
         <v>232</v>
       </c>
-      <c r="E4" s="341" t="s">
+      <c r="E4" s="346" t="s">
         <v>233</v>
       </c>
-      <c r="F4" s="342"/>
+      <c r="F4" s="347"/>
       <c r="G4" s="134"/>
       <c r="H4" s="26" t="s">
         <v>0</v>
@@ -10943,10 +10943,10 @@
       <c r="D5" s="131" t="s">
         <v>236</v>
       </c>
-      <c r="E5" s="343" t="s">
+      <c r="E5" s="348" t="s">
         <v>249</v>
       </c>
-      <c r="F5" s="344"/>
+      <c r="F5" s="349"/>
       <c r="G5" s="133"/>
       <c r="H5" s="26" t="s">
         <v>0</v>
@@ -10963,10 +10963,10 @@
       <c r="D6" s="132" t="s">
         <v>239</v>
       </c>
-      <c r="E6" s="345" t="s">
+      <c r="E6" s="350" t="s">
         <v>250</v>
       </c>
-      <c r="F6" s="346"/>
+      <c r="F6" s="351"/>
       <c r="G6" s="133"/>
       <c r="H6" s="26" t="s">
         <v>0</v>
@@ -10983,10 +10983,10 @@
       <c r="D7" s="132" t="s">
         <v>242</v>
       </c>
-      <c r="E7" s="345" t="s">
+      <c r="E7" s="350" t="s">
         <v>249</v>
       </c>
-      <c r="F7" s="346"/>
+      <c r="F7" s="351"/>
       <c r="G7" s="133"/>
       <c r="H7" s="26" t="s">
         <v>0</v>
@@ -10997,16 +10997,16 @@
       <c r="B8" s="141" t="s">
         <v>243</v>
       </c>
-      <c r="C8" s="336" t="s">
+      <c r="C8" s="341" t="s">
         <v>244</v>
       </c>
-      <c r="D8" s="336" t="s">
+      <c r="D8" s="341" t="s">
         <v>245</v>
       </c>
-      <c r="E8" s="347" t="s">
+      <c r="E8" s="352" t="s">
         <v>251</v>
       </c>
-      <c r="F8" s="348"/>
+      <c r="F8" s="353"/>
       <c r="G8" s="133"/>
       <c r="H8" s="26" t="s">
         <v>0</v>
@@ -11017,10 +11017,10 @@
       <c r="B9" s="142" t="s">
         <v>246</v>
       </c>
-      <c r="C9" s="336"/>
-      <c r="D9" s="336"/>
-      <c r="E9" s="349"/>
-      <c r="F9" s="350"/>
+      <c r="C9" s="341"/>
+      <c r="D9" s="341"/>
+      <c r="E9" s="354"/>
+      <c r="F9" s="355"/>
       <c r="G9" s="133"/>
       <c r="H9" s="26" t="s">
         <v>0</v>
@@ -11031,10 +11031,10 @@
       <c r="B10" s="143" t="s">
         <v>247</v>
       </c>
-      <c r="C10" s="337"/>
-      <c r="D10" s="337"/>
-      <c r="E10" s="351"/>
-      <c r="F10" s="352"/>
+      <c r="C10" s="342"/>
+      <c r="D10" s="342"/>
+      <c r="E10" s="356"/>
+      <c r="F10" s="357"/>
       <c r="G10" s="133"/>
       <c r="H10" s="26" t="s">
         <v>0</v>
@@ -11054,11 +11054,11 @@
     <row r="12" spans="1:8" s="26" customFormat="1" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="121"/>
       <c r="B12" s="135"/>
-      <c r="C12" s="340" t="s">
+      <c r="C12" s="345" t="s">
         <v>248</v>
       </c>
-      <c r="D12" s="340"/>
-      <c r="E12" s="340"/>
+      <c r="D12" s="345"/>
+      <c r="E12" s="345"/>
       <c r="F12" s="136"/>
       <c r="H12" s="26" t="s">
         <v>0</v>
@@ -11072,14 +11072,14 @@
       </c>
     </row>
     <row r="14" spans="1:8" s="26" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="338" t="s">
+      <c r="A14" s="343" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="338"/>
-      <c r="C14" s="338"/>
-      <c r="D14" s="338"/>
-      <c r="E14" s="338"/>
-      <c r="F14" s="339"/>
+      <c r="B14" s="343"/>
+      <c r="C14" s="343"/>
+      <c r="D14" s="343"/>
+      <c r="E14" s="343"/>
+      <c r="F14" s="344"/>
       <c r="H14" s="26" t="s">
         <v>0</v>
       </c>
@@ -11212,7 +11212,7 @@
       <c r="G2" s="75" t="s">
         <v>172</v>
       </c>
-      <c r="H2" s="359" t="s">
+      <c r="H2" s="364" t="s">
         <v>171</v>
       </c>
       <c r="I2" s="74" t="s">
@@ -11257,7 +11257,7 @@
       <c r="V2" s="74" t="s">
         <v>170</v>
       </c>
-      <c r="W2" s="359" t="s">
+      <c r="W2" s="364" t="s">
         <v>169</v>
       </c>
       <c r="X2" s="73" t="s">
@@ -11287,7 +11287,7 @@
       <c r="AF2" s="73" t="s">
         <v>167</v>
       </c>
-      <c r="AG2" s="359" t="s">
+      <c r="AG2" s="364" t="s">
         <v>166</v>
       </c>
       <c r="AH2" s="73" t="s">
@@ -11329,7 +11329,7 @@
       <c r="AT2" s="73" t="s">
         <v>165</v>
       </c>
-      <c r="AU2" s="359" t="s">
+      <c r="AU2" s="364" t="s">
         <v>164</v>
       </c>
       <c r="AV2" s="72" t="s">
@@ -11359,7 +11359,7 @@
       <c r="BD2" s="72" t="s">
         <v>163</v>
       </c>
-      <c r="BE2" s="359" t="s">
+      <c r="BE2" s="364" t="s">
         <v>162</v>
       </c>
       <c r="BF2"/>
@@ -11374,7 +11374,7 @@
       <c r="G3" s="75" t="s">
         <v>161</v>
       </c>
-      <c r="H3" s="359"/>
+      <c r="H3" s="364"/>
       <c r="I3" s="74" t="s">
         <v>160</v>
       </c>
@@ -11415,7 +11415,7 @@
       <c r="V3" s="74" t="s">
         <v>148</v>
       </c>
-      <c r="W3" s="359"/>
+      <c r="W3" s="364"/>
       <c r="X3" s="73" t="s">
         <v>144</v>
       </c>
@@ -11443,7 +11443,7 @@
       <c r="AF3" s="73" t="s">
         <v>138</v>
       </c>
-      <c r="AG3" s="359"/>
+      <c r="AG3" s="364"/>
       <c r="AH3" s="73" t="s">
         <v>137</v>
       </c>
@@ -11483,7 +11483,7 @@
       <c r="AT3" s="73" t="s">
         <v>125</v>
       </c>
-      <c r="AU3" s="359"/>
+      <c r="AU3" s="364"/>
       <c r="AV3" s="72" t="s">
         <v>124</v>
       </c>
@@ -11511,7 +11511,7 @@
       <c r="BD3" s="72" t="s">
         <v>116</v>
       </c>
-      <c r="BE3" s="359"/>
+      <c r="BE3" s="364"/>
     </row>
     <row r="4" spans="1:58" s="41" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="77"/>
@@ -11533,7 +11533,7 @@
       <c r="G4" s="75" t="s">
         <v>111</v>
       </c>
-      <c r="H4" s="359"/>
+      <c r="H4" s="364"/>
       <c r="I4" s="74" t="s">
         <v>110</v>
       </c>
@@ -11576,7 +11576,7 @@
       <c r="V4" s="74" t="s">
         <v>97</v>
       </c>
-      <c r="W4" s="359"/>
+      <c r="W4" s="364"/>
       <c r="X4" s="73" t="s">
         <v>92</v>
       </c>
@@ -11604,7 +11604,7 @@
       <c r="AF4" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="AG4" s="359"/>
+      <c r="AG4" s="364"/>
       <c r="AH4" s="73" t="s">
         <v>84</v>
       </c>
@@ -11644,7 +11644,7 @@
       <c r="AT4" s="73" t="s">
         <v>72</v>
       </c>
-      <c r="AU4" s="359"/>
+      <c r="AU4" s="364"/>
       <c r="AV4" s="72" t="s">
         <v>71</v>
       </c>
@@ -11672,7 +11672,7 @@
       <c r="BD4" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="BE4" s="359"/>
+      <c r="BE4" s="364"/>
       <c r="BF4"/>
     </row>
     <row r="5" spans="1:58" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -14176,7 +14176,7 @@
       <c r="G2" s="75" t="s">
         <v>172</v>
       </c>
-      <c r="H2" s="359" t="s">
+      <c r="H2" s="364" t="s">
         <v>171</v>
       </c>
       <c r="I2" s="75" t="s">
@@ -14209,7 +14209,7 @@
       <c r="R2" s="75" t="s">
         <v>170</v>
       </c>
-      <c r="S2" s="359" t="s">
+      <c r="S2" s="364" t="s">
         <v>169</v>
       </c>
       <c r="T2" s="75" t="s">
@@ -14239,7 +14239,7 @@
       <c r="AB2" s="75" t="s">
         <v>167</v>
       </c>
-      <c r="AC2" s="359" t="s">
+      <c r="AC2" s="364" t="s">
         <v>216</v>
       </c>
       <c r="AD2" s="75" t="s">
@@ -14251,7 +14251,7 @@
       <c r="AF2" s="75" t="s">
         <v>215</v>
       </c>
-      <c r="AG2" s="359" t="s">
+      <c r="AG2" s="364" t="s">
         <v>214</v>
       </c>
     </row>
@@ -14262,7 +14262,7 @@
       <c r="G3" s="75" t="s">
         <v>161</v>
       </c>
-      <c r="H3" s="359"/>
+      <c r="H3" s="364"/>
       <c r="I3" s="75" t="s">
         <v>213</v>
       </c>
@@ -14293,7 +14293,7 @@
       <c r="R3" s="75" t="s">
         <v>148</v>
       </c>
-      <c r="S3" s="359"/>
+      <c r="S3" s="364"/>
       <c r="T3" s="75" t="s">
         <v>204</v>
       </c>
@@ -14321,7 +14321,7 @@
       <c r="AB3" s="75" t="s">
         <v>196</v>
       </c>
-      <c r="AC3" s="359"/>
+      <c r="AC3" s="364"/>
       <c r="AD3" s="75" t="s">
         <v>195</v>
       </c>
@@ -14331,7 +14331,7 @@
       <c r="AF3" s="75" t="s">
         <v>125</v>
       </c>
-      <c r="AG3" s="359"/>
+      <c r="AG3" s="364"/>
     </row>
     <row r="4" spans="1:60" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="78"/>
@@ -14353,7 +14353,7 @@
       <c r="G4" s="75" t="s">
         <v>111</v>
       </c>
-      <c r="H4" s="359"/>
+      <c r="H4" s="364"/>
       <c r="I4" s="75" t="s">
         <v>194</v>
       </c>
@@ -14384,7 +14384,7 @@
       <c r="R4" s="75" t="s">
         <v>97</v>
       </c>
-      <c r="S4" s="359"/>
+      <c r="S4" s="364"/>
       <c r="T4" s="75" t="s">
         <v>185</v>
       </c>
@@ -14412,7 +14412,7 @@
       <c r="AB4" s="75" t="s">
         <v>177</v>
       </c>
-      <c r="AC4" s="359"/>
+      <c r="AC4" s="364"/>
       <c r="AD4" s="75" t="s">
         <v>176</v>
       </c>
@@ -14422,7 +14422,7 @@
       <c r="AF4" s="75" t="s">
         <v>72</v>
       </c>
-      <c r="AG4" s="359"/>
+      <c r="AG4" s="364"/>
     </row>
     <row r="5" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A5" s="81" t="s">
@@ -16077,13 +16077,13 @@
       <c r="G2" s="75" t="s">
         <v>170</v>
       </c>
-      <c r="H2" s="359" t="s">
+      <c r="H2" s="364" t="s">
         <v>169</v>
       </c>
       <c r="I2" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="359" t="s">
+      <c r="J2" s="364" t="s">
         <v>168</v>
       </c>
     </row>
@@ -16091,11 +16091,11 @@
       <c r="G3" s="75" t="s">
         <v>148</v>
       </c>
-      <c r="H3" s="359"/>
+      <c r="H3" s="364"/>
       <c r="I3" s="75" t="s">
         <v>145</v>
       </c>
-      <c r="J3" s="359"/>
+      <c r="J3" s="364"/>
     </row>
     <row r="4" spans="1:62" ht="36" x14ac:dyDescent="0.2">
       <c r="A4" s="97"/>
@@ -16117,11 +16117,11 @@
       <c r="G4" s="75" t="s">
         <v>97</v>
       </c>
-      <c r="H4" s="359"/>
+      <c r="H4" s="364"/>
       <c r="I4" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="J4" s="359"/>
+      <c r="J4" s="364"/>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A5" s="91" t="s">
@@ -16595,7 +16595,7 @@
       <c r="P2" s="316" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="362" t="s">
+      <c r="Q2" s="367" t="s">
         <v>434</v>
       </c>
     </row>
@@ -16636,7 +16636,7 @@
       <c r="P3" s="316" t="s">
         <v>441</v>
       </c>
-      <c r="Q3" s="362"/>
+      <c r="Q3" s="367"/>
     </row>
     <row r="4" spans="1:62" ht="70" x14ac:dyDescent="0.2">
       <c r="A4" s="317"/>
@@ -16685,7 +16685,7 @@
       <c r="P4" s="319" t="s">
         <v>452</v>
       </c>
-      <c r="Q4" s="362"/>
+      <c r="Q4" s="367"/>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A5" s="320" t="s">
@@ -17548,13 +17548,13 @@
   <sheetData>
     <row r="1" spans="1:61" s="151" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="150"/>
-      <c r="B1" s="364" t="s">
+      <c r="B1" s="369" t="s">
         <v>173</v>
       </c>
-      <c r="C1" s="364"/>
-      <c r="D1" s="364"/>
-      <c r="E1" s="364"/>
-      <c r="F1" s="364"/>
+      <c r="C1" s="369"/>
+      <c r="D1" s="369"/>
+      <c r="E1" s="369"/>
+      <c r="F1" s="369"/>
       <c r="G1" s="152"/>
       <c r="H1" s="152"/>
       <c r="I1" s="152"/>
@@ -17599,7 +17599,7 @@
       <c r="O2" s="154" t="s">
         <v>167</v>
       </c>
-      <c r="P2" s="363" t="s">
+      <c r="P2" s="368" t="s">
         <v>166</v>
       </c>
       <c r="Q2" s="154" t="s">
@@ -17641,7 +17641,7 @@
       <c r="AC2" s="154" t="s">
         <v>165</v>
       </c>
-      <c r="AD2" s="363" t="s">
+      <c r="AD2" s="368" t="s">
         <v>164</v>
       </c>
       <c r="AE2" s="155" t="s">
@@ -17671,7 +17671,7 @@
       <c r="AM2" s="155" t="s">
         <v>163</v>
       </c>
-      <c r="AN2" s="363" t="s">
+      <c r="AN2" s="368" t="s">
         <v>162</v>
       </c>
       <c r="AQ2" s="154"/>
@@ -17682,7 +17682,7 @@
       <c r="AV2" s="154"/>
       <c r="AW2" s="154"/>
       <c r="AX2" s="154"/>
-      <c r="AY2" s="363"/>
+      <c r="AY2" s="368"/>
       <c r="AZ2" s="155"/>
       <c r="BA2" s="155"/>
       <c r="BB2" s="155"/>
@@ -17692,7 +17692,7 @@
       <c r="BF2" s="155"/>
       <c r="BG2" s="155"/>
       <c r="BH2" s="155"/>
-      <c r="BI2" s="363"/>
+      <c r="BI2" s="368"/>
     </row>
     <row r="3" spans="1:61" s="151" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="153"/>
@@ -17728,7 +17728,7 @@
       <c r="O3" s="154" t="s">
         <v>138</v>
       </c>
-      <c r="P3" s="363"/>
+      <c r="P3" s="368"/>
       <c r="Q3" s="154" t="s">
         <v>137</v>
       </c>
@@ -17768,7 +17768,7 @@
       <c r="AC3" s="154" t="s">
         <v>125</v>
       </c>
-      <c r="AD3" s="363"/>
+      <c r="AD3" s="368"/>
       <c r="AE3" s="155" t="s">
         <v>124</v>
       </c>
@@ -17796,7 +17796,7 @@
       <c r="AM3" s="155" t="s">
         <v>116</v>
       </c>
-      <c r="AN3" s="363"/>
+      <c r="AN3" s="368"/>
       <c r="AQ3" s="154"/>
       <c r="AR3" s="154"/>
       <c r="AS3" s="154"/>
@@ -17805,7 +17805,7 @@
       <c r="AV3" s="154"/>
       <c r="AW3" s="154"/>
       <c r="AX3" s="154"/>
-      <c r="AY3" s="363"/>
+      <c r="AY3" s="368"/>
       <c r="AZ3" s="155"/>
       <c r="BA3" s="155"/>
       <c r="BB3" s="155"/>
@@ -17815,7 +17815,7 @@
       <c r="BF3" s="155"/>
       <c r="BG3" s="155"/>
       <c r="BH3" s="155"/>
-      <c r="BI3" s="363"/>
+      <c r="BI3" s="368"/>
     </row>
     <row r="4" spans="1:61" s="151" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="156"/>
@@ -17861,7 +17861,7 @@
       <c r="O4" s="154" t="s">
         <v>85</v>
       </c>
-      <c r="P4" s="363"/>
+      <c r="P4" s="368"/>
       <c r="Q4" s="154" t="s">
         <v>84</v>
       </c>
@@ -17901,7 +17901,7 @@
       <c r="AC4" s="154" t="s">
         <v>72</v>
       </c>
-      <c r="AD4" s="363"/>
+      <c r="AD4" s="368"/>
       <c r="AE4" s="155" t="s">
         <v>71</v>
       </c>
@@ -17929,7 +17929,7 @@
       <c r="AM4" s="155" t="s">
         <v>63</v>
       </c>
-      <c r="AN4" s="363"/>
+      <c r="AN4" s="368"/>
       <c r="AQ4" s="154"/>
       <c r="AR4" s="154"/>
       <c r="AS4" s="154"/>
@@ -17938,7 +17938,7 @@
       <c r="AV4" s="154"/>
       <c r="AW4" s="154"/>
       <c r="AX4" s="154"/>
-      <c r="AY4" s="363"/>
+      <c r="AY4" s="368"/>
       <c r="AZ4" s="155"/>
       <c r="BA4" s="155"/>
       <c r="BB4" s="155"/>
@@ -17948,7 +17948,7 @@
       <c r="BF4" s="155"/>
       <c r="BG4" s="155"/>
       <c r="BH4" s="155"/>
-      <c r="BI4" s="363"/>
+      <c r="BI4" s="368"/>
     </row>
     <row r="5" spans="1:61" s="151" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="158" t="s">
@@ -19675,14 +19675,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="365" t="s">
+      <c r="A1" s="370" t="s">
         <v>217</v>
       </c>
-      <c r="B1" s="365"/>
-      <c r="C1" s="365"/>
-      <c r="D1" s="365"/>
-      <c r="E1" s="365"/>
-      <c r="F1" s="365"/>
+      <c r="B1" s="370"/>
+      <c r="C1" s="370"/>
+      <c r="D1" s="370"/>
+      <c r="E1" s="370"/>
+      <c r="F1" s="370"/>
       <c r="G1" s="183"/>
       <c r="H1" s="183"/>
       <c r="I1" s="183"/>
@@ -19732,7 +19732,7 @@
       <c r="O2" s="186" t="s">
         <v>167</v>
       </c>
-      <c r="P2" s="366" t="s">
+      <c r="P2" s="371" t="s">
         <v>216</v>
       </c>
       <c r="Q2" s="186" t="s">
@@ -19744,7 +19744,7 @@
       <c r="S2" s="186" t="s">
         <v>215</v>
       </c>
-      <c r="T2" s="366" t="s">
+      <c r="T2" s="371" t="s">
         <v>214</v>
       </c>
     </row>
@@ -19782,7 +19782,7 @@
       <c r="O3" s="186" t="s">
         <v>196</v>
       </c>
-      <c r="P3" s="366"/>
+      <c r="P3" s="371"/>
       <c r="Q3" s="186" t="s">
         <v>195</v>
       </c>
@@ -19792,7 +19792,7 @@
       <c r="S3" s="186" t="s">
         <v>125</v>
       </c>
-      <c r="T3" s="366"/>
+      <c r="T3" s="371"/>
     </row>
     <row r="4" spans="1:20" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="185"/>
@@ -19838,7 +19838,7 @@
       <c r="O4" s="186" t="s">
         <v>177</v>
       </c>
-      <c r="P4" s="366"/>
+      <c r="P4" s="371"/>
       <c r="Q4" s="186" t="s">
         <v>176</v>
       </c>
@@ -19848,7 +19848,7 @@
       <c r="S4" s="186" t="s">
         <v>72</v>
       </c>
-      <c r="T4" s="366"/>
+      <c r="T4" s="371"/>
     </row>
     <row r="5" spans="1:20" ht="317" x14ac:dyDescent="0.2">
       <c r="A5" s="189" t="s">
@@ -20439,16 +20439,16 @@
   <sheetData>
     <row r="1" spans="1:28" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="209"/>
-      <c r="B1" s="368" t="s">
+      <c r="B1" s="373" t="s">
         <v>173</v>
       </c>
-      <c r="C1" s="368"/>
-      <c r="D1" s="368"/>
-      <c r="E1" s="368"/>
-      <c r="F1" s="368"/>
-      <c r="G1" s="368"/>
-      <c r="H1" s="368"/>
-      <c r="I1" s="368"/>
+      <c r="C1" s="373"/>
+      <c r="D1" s="373"/>
+      <c r="E1" s="373"/>
+      <c r="F1" s="373"/>
+      <c r="G1" s="373"/>
+      <c r="H1" s="373"/>
+      <c r="I1" s="373"/>
       <c r="J1" s="206"/>
       <c r="K1" s="206"/>
       <c r="L1" s="206"/>
@@ -20479,7 +20479,7 @@
       <c r="G2" s="208" t="s">
         <v>172</v>
       </c>
-      <c r="H2" s="367" t="s">
+      <c r="H2" s="372" t="s">
         <v>171</v>
       </c>
       <c r="I2" s="211" t="s">
@@ -20524,7 +20524,7 @@
       <c r="V2" s="211" t="s">
         <v>170</v>
       </c>
-      <c r="W2" s="367" t="s">
+      <c r="W2" s="372" t="s">
         <v>169</v>
       </c>
       <c r="X2" s="208" t="s">
@@ -20539,7 +20539,7 @@
       <c r="AA2" s="208" t="s">
         <v>38</v>
       </c>
-      <c r="AB2" s="367" t="s">
+      <c r="AB2" s="372" t="s">
         <v>168</v>
       </c>
     </row>
@@ -20553,7 +20553,7 @@
       <c r="G3" s="208" t="s">
         <v>161</v>
       </c>
-      <c r="H3" s="367"/>
+      <c r="H3" s="372"/>
       <c r="I3" s="211" t="s">
         <v>160</v>
       </c>
@@ -20594,7 +20594,7 @@
       <c r="V3" s="211" t="s">
         <v>148</v>
       </c>
-      <c r="W3" s="367"/>
+      <c r="W3" s="372"/>
       <c r="X3" s="210"/>
       <c r="Y3" s="208" t="s">
         <v>147</v>
@@ -20605,7 +20605,7 @@
       <c r="AA3" s="208" t="s">
         <v>145</v>
       </c>
-      <c r="AB3" s="367"/>
+      <c r="AB3" s="372"/>
     </row>
     <row r="4" spans="1:28" ht="98" x14ac:dyDescent="0.2">
       <c r="A4" s="212"/>
@@ -20627,7 +20627,7 @@
       <c r="G4" s="208" t="s">
         <v>111</v>
       </c>
-      <c r="H4" s="367"/>
+      <c r="H4" s="372"/>
       <c r="I4" s="211" t="s">
         <v>110</v>
       </c>
@@ -20670,7 +20670,7 @@
       <c r="V4" s="214" t="s">
         <v>97</v>
       </c>
-      <c r="W4" s="367"/>
+      <c r="W4" s="372"/>
       <c r="X4" s="215" t="s">
         <v>96</v>
       </c>
@@ -20683,7 +20683,7 @@
       <c r="AA4" s="215" t="s">
         <v>93</v>
       </c>
-      <c r="AB4" s="367"/>
+      <c r="AB4" s="372"/>
     </row>
     <row r="5" spans="1:28" ht="196" x14ac:dyDescent="0.2">
       <c r="A5" s="216" t="s">
@@ -21582,16 +21582,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="370" t="s">
+      <c r="A1" s="375" t="s">
         <v>217</v>
       </c>
-      <c r="B1" s="370"/>
-      <c r="C1" s="370"/>
-      <c r="D1" s="370"/>
-      <c r="E1" s="370"/>
-      <c r="F1" s="370"/>
-      <c r="G1" s="370"/>
-      <c r="H1" s="370"/>
+      <c r="B1" s="375"/>
+      <c r="C1" s="375"/>
+      <c r="D1" s="375"/>
+      <c r="E1" s="375"/>
+      <c r="F1" s="375"/>
+      <c r="G1" s="375"/>
+      <c r="H1" s="375"/>
       <c r="I1" s="256"/>
       <c r="J1" s="256"/>
       <c r="K1" s="256"/>
@@ -21616,7 +21616,7 @@
       <c r="G2" s="258" t="s">
         <v>172</v>
       </c>
-      <c r="H2" s="369" t="s">
+      <c r="H2" s="374" t="s">
         <v>171</v>
       </c>
       <c r="I2" s="258" t="s">
@@ -21649,13 +21649,13 @@
       <c r="R2" s="258" t="s">
         <v>170</v>
       </c>
-      <c r="S2" s="369" t="s">
+      <c r="S2" s="374" t="s">
         <v>169</v>
       </c>
       <c r="T2" s="258" t="s">
         <v>38</v>
       </c>
-      <c r="U2" s="369" t="s">
+      <c r="U2" s="374" t="s">
         <v>168</v>
       </c>
     </row>
@@ -21669,7 +21669,7 @@
       <c r="G3" s="258" t="s">
         <v>161</v>
       </c>
-      <c r="H3" s="369"/>
+      <c r="H3" s="374"/>
       <c r="I3" s="258" t="s">
         <v>213</v>
       </c>
@@ -21700,11 +21700,11 @@
       <c r="R3" s="258" t="s">
         <v>148</v>
       </c>
-      <c r="S3" s="369"/>
+      <c r="S3" s="374"/>
       <c r="T3" s="258" t="s">
         <v>145</v>
       </c>
-      <c r="U3" s="369"/>
+      <c r="U3" s="374"/>
     </row>
     <row r="4" spans="1:21" ht="112" x14ac:dyDescent="0.2">
       <c r="A4" s="255"/>
@@ -21726,7 +21726,7 @@
       <c r="G4" s="258" t="s">
         <v>111</v>
       </c>
-      <c r="H4" s="369"/>
+      <c r="H4" s="374"/>
       <c r="I4" s="258" t="s">
         <v>194</v>
       </c>
@@ -21757,11 +21757,11 @@
       <c r="R4" s="258" t="s">
         <v>97</v>
       </c>
-      <c r="S4" s="369"/>
+      <c r="S4" s="374"/>
       <c r="T4" s="258" t="s">
         <v>93</v>
       </c>
-      <c r="U4" s="369"/>
+      <c r="U4" s="374"/>
     </row>
     <row r="5" spans="1:21" ht="196" x14ac:dyDescent="0.2">
       <c r="A5" s="261" t="s">
@@ -22457,13 +22457,13 @@
       <c r="K2" s="186" t="s">
         <v>170</v>
       </c>
-      <c r="L2" s="366" t="s">
+      <c r="L2" s="371" t="s">
         <v>169</v>
       </c>
       <c r="M2" s="186" t="s">
         <v>38</v>
       </c>
-      <c r="N2" s="366" t="s">
+      <c r="N2" s="371" t="s">
         <v>168</v>
       </c>
     </row>
@@ -22481,11 +22481,11 @@
       <c r="K3" s="186" t="s">
         <v>148</v>
       </c>
-      <c r="L3" s="366"/>
+      <c r="L3" s="371"/>
       <c r="M3" s="186" t="s">
         <v>145</v>
       </c>
-      <c r="N3" s="366"/>
+      <c r="N3" s="371"/>
     </row>
     <row r="4" spans="1:14" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="239"/>
@@ -22511,11 +22511,11 @@
       <c r="K4" s="186" t="s">
         <v>97</v>
       </c>
-      <c r="L4" s="366"/>
+      <c r="L4" s="371"/>
       <c r="M4" s="186" t="s">
         <v>93</v>
       </c>
-      <c r="N4" s="366"/>
+      <c r="N4" s="371"/>
     </row>
     <row r="5" spans="1:14" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="241"/>
@@ -23189,25 +23189,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" s="371"/>
-      <c r="B1" s="372" t="s">
+      <c r="A1" s="334"/>
+      <c r="B1" s="376" t="s">
         <v>455</v>
       </c>
-      <c r="C1" s="372"/>
-      <c r="D1" s="372"/>
-      <c r="E1" s="372"/>
-      <c r="F1" s="373"/>
-      <c r="G1" s="371"/>
-      <c r="H1" s="371"/>
-      <c r="I1" s="371"/>
-      <c r="J1" s="371"/>
-      <c r="K1" s="371"/>
-      <c r="L1" s="371"/>
-      <c r="M1" s="371"/>
-      <c r="N1" s="371"/>
-      <c r="O1" s="371"/>
-      <c r="P1" s="371"/>
-      <c r="Q1" s="371"/>
+      <c r="C1" s="376"/>
+      <c r="D1" s="376"/>
+      <c r="E1" s="376"/>
+      <c r="F1" s="335"/>
+      <c r="G1" s="334"/>
+      <c r="H1" s="334"/>
+      <c r="I1" s="334"/>
+      <c r="J1" s="334"/>
+      <c r="K1" s="334"/>
+      <c r="L1" s="334"/>
+      <c r="M1" s="334"/>
+      <c r="N1" s="334"/>
+      <c r="O1" s="334"/>
+      <c r="P1" s="334"/>
+      <c r="Q1" s="334"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="313"/>
@@ -23246,7 +23246,7 @@
       <c r="P2" s="316" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="362" t="s">
+      <c r="Q2" s="367" t="s">
         <v>434</v>
       </c>
     </row>
@@ -23287,9 +23287,9 @@
       <c r="P3" s="316" t="s">
         <v>441</v>
       </c>
-      <c r="Q3" s="362"/>
-    </row>
-    <row r="4" spans="1:17" ht="98" x14ac:dyDescent="0.2">
+      <c r="Q3" s="367"/>
+    </row>
+    <row r="4" spans="1:17" ht="70" x14ac:dyDescent="0.2">
       <c r="A4" s="317"/>
       <c r="B4" s="318" t="s">
         <v>115</v>
@@ -23336,9 +23336,9 @@
       <c r="P4" s="319" t="s">
         <v>452</v>
       </c>
-      <c r="Q4" s="362"/>
-    </row>
-    <row r="5" spans="1:17" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="Q4" s="367"/>
+    </row>
+    <row r="5" spans="1:17" ht="398" x14ac:dyDescent="0.2">
       <c r="A5" s="320" t="s">
         <v>453</v>
       </c>
@@ -23382,7 +23382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" ht="266" x14ac:dyDescent="0.2">
       <c r="A6" s="320" t="s">
         <v>453</v>
       </c>
@@ -23426,7 +23426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="252" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" ht="224" x14ac:dyDescent="0.2">
       <c r="A7" s="320" t="s">
         <v>453</v>
       </c>
@@ -23472,7 +23472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="371" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" ht="345" x14ac:dyDescent="0.2">
       <c r="A8" s="320" t="s">
         <v>453</v>
       </c>
@@ -23518,7 +23518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="238" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" ht="210" x14ac:dyDescent="0.2">
       <c r="A9" s="320" t="s">
         <v>453</v>
       </c>
@@ -23564,7 +23564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="224" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" ht="196" x14ac:dyDescent="0.2">
       <c r="A10" s="320" t="s">
         <v>453</v>
       </c>
@@ -23610,7 +23610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="306" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" ht="280" x14ac:dyDescent="0.2">
       <c r="A11" s="320" t="s">
         <v>453</v>
       </c>
@@ -23656,7 +23656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="306" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" ht="280" x14ac:dyDescent="0.2">
       <c r="A12" s="320" t="s">
         <v>453</v>
       </c>
@@ -23703,11 +23703,11 @@
       </c>
     </row>
     <row r="13" spans="1:17" ht="28" x14ac:dyDescent="0.2">
-      <c r="A13" s="374"/>
-      <c r="B13" s="375"/>
-      <c r="C13" s="375"/>
-      <c r="D13" s="376"/>
-      <c r="E13" s="375"/>
+      <c r="A13" s="336"/>
+      <c r="B13" s="337"/>
+      <c r="C13" s="337"/>
+      <c r="D13" s="338"/>
+      <c r="E13" s="337"/>
       <c r="F13" s="328" t="s">
         <v>39</v>
       </c>
@@ -23860,8 +23860,8 @@
   </sheetPr>
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="X4" sqref="X4"/>
+    <sheetView zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -23940,28 +23940,28 @@
       <c r="D4" s="277"/>
       <c r="E4" s="277"/>
       <c r="F4" s="277"/>
-      <c r="G4" s="353" t="s">
+      <c r="G4" s="358" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="354"/>
-      <c r="I4" s="354"/>
-      <c r="J4" s="354"/>
-      <c r="K4" s="354"/>
-      <c r="L4" s="355"/>
-      <c r="M4" s="356"/>
-      <c r="N4" s="357" t="s">
+      <c r="H4" s="359"/>
+      <c r="I4" s="359"/>
+      <c r="J4" s="359"/>
+      <c r="K4" s="359"/>
+      <c r="L4" s="360"/>
+      <c r="M4" s="361"/>
+      <c r="N4" s="362" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="355"/>
-      <c r="P4" s="355"/>
-      <c r="Q4" s="355"/>
-      <c r="R4" s="355"/>
-      <c r="S4" s="355"/>
-      <c r="T4" s="358"/>
-      <c r="U4" s="353" t="s">
+      <c r="O4" s="360"/>
+      <c r="P4" s="360"/>
+      <c r="Q4" s="360"/>
+      <c r="R4" s="360"/>
+      <c r="S4" s="360"/>
+      <c r="T4" s="363"/>
+      <c r="U4" s="358" t="s">
         <v>28</v>
       </c>
-      <c r="V4" s="356"/>
+      <c r="V4" s="361"/>
       <c r="W4" s="284"/>
       <c r="X4" t="s">
         <v>0</v>
@@ -24046,7 +24046,7 @@
         <v>#N/A</v>
       </c>
       <c r="H6" s="281" t="str">
-        <f>IF(AND(OR(LEFT(C6,3)="12.",LEFT(E6,3)="12.",LEFT(E6,5)="CET &gt;",IFERROR(G6/$G$6,"")=0),NOT(AND(LEFT(E6,5)="12.31",IFERROR(G6/$G$6,"")&lt;&gt;0)),NOT(AND(LEFT(E6,5)="12.32",IFERROR(G6/$G$6,"")&lt;&gt;0))),"", IFERROR(G6/$G$6,""))</f>
+        <f>IF(AND(OR(LEFT(C6,3)="12.",LEFT(E6,3)="12.",LEFT(E6,5)="CET &gt;",IFERROR(G6/$G$6,"")=0),NOT(AND(LEFT(E6,4)="12.8",IFERROR(G6/$G$6,"")&lt;&gt;0)),NOT(AND(LEFT(E6,5)="12.31",IFERROR(G6/$G$6,"")&lt;&gt;0)),NOT(AND(LEFT(E6,5)="12.32",IFERROR(G6/$G$6,"")&lt;&gt;0))),"", IFERROR(G6/$G$6,""))</f>
         <v/>
       </c>
       <c r="I6" s="18" t="e">
@@ -24079,7 +24079,7 @@
         <v>#N/A</v>
       </c>
       <c r="M6" s="282" t="str">
-        <f>IF(AND(OR(LEFT(C6,3)="12.",LEFT(E6,3)="12.",LEFT(E6,5)="CET &gt;", IFERROR(L6/$L$6,"")=0),NOT(AND(LEFT(E6,5)="12.31",IFERROR(L6/$G$6,"")&lt;&gt;0)),NOT(AND(LEFT(E6,5)="12.32",IFERROR(L6/$G$6,"")&lt;&gt;0))),"", IFERROR(L6/$L$6,""))</f>
+        <f>IF(AND(OR(LEFT(C6,3)="12.",LEFT(E6,3)="12.",LEFT(E6,5)="CET &gt;", IFERROR(L6/$L$6,"")=0),NOT(AND(LEFT(E6,4)="12.8",IFERROR(G6/$G$6,"")&lt;&gt;0)),NOT(AND(LEFT(E6,5)="12.31",IFERROR(L6/$G$6,"")&lt;&gt;0)),NOT(AND(LEFT(E6,5)="12.32",IFERROR(L6/$G$6,"")&lt;&gt;0))),"", IFERROR(L6/$L$6,""))</f>
         <v/>
       </c>
       <c r="N6" s="18" t="e">
@@ -24090,7 +24090,7 @@
         <v>#N/A</v>
       </c>
       <c r="O6" s="281" t="str">
-        <f>IF(AND(OR(LEFT(C6,3)="12.",LEFT(E6,3)="12.",LEFT(E6,5)="CET &gt;",IFERROR(N6/$N$6,"")=0),NOT(AND(LEFT(E6,5)="12.31",IFERROR(N6/$G$6,"")&lt;&gt;0)),NOT(AND(LEFT(E6,5)="12.32",IFERROR(N6/$G$6,"")&lt;&gt;0))),"",IFERROR(N6/$N$6,""))</f>
+        <f>IF(AND(OR(LEFT(C6,3)="12.",LEFT(E6,3)="12.",LEFT(E6,5)="CET &gt;",IFERROR(N6/$N$6,"")=0),NOT(AND(LEFT(E6,4)="12.8",IFERROR(G6/$G$6,"")&lt;&gt;0)),NOT(AND(LEFT(E6,5)="12.31",IFERROR(N6/$G$6,"")&lt;&gt;0)),NOT(AND(LEFT(E6,5)="12.32",IFERROR(N6/$G$6,"")&lt;&gt;0))),"",IFERROR(N6/$N$6,""))</f>
         <v/>
       </c>
       <c r="P6" s="18" t="e">
@@ -24123,7 +24123,7 @@
         <v>#N/A</v>
       </c>
       <c r="T6" s="281" t="str">
-        <f>IF(AND(OR(LEFT(C6,3)="12.",LEFT(E6,3)="12.",LEFT(E6,5)="CET &gt;",IFERROR(S6/$S$6,"")=0),NOT(AND(LEFT(E6,5)="12.31",IFERROR(S6/$G$6,"")&lt;&gt;0)),NOT(AND(LEFT(E6,5)="12.32",IFERROR(S6/$G$6,"")&lt;&gt;0))),"", IFERROR(S6/$S$6,""))</f>
+        <f>IF(AND(OR(LEFT(C6,3)="12.",LEFT(E6,3)="12.",LEFT(E6,5)="CET &gt;",IFERROR(S6/$S$6,"")=0),NOT(AND(LEFT(E6,4)="12.8",IFERROR(G6/$G$6,"")&lt;&gt;0)),NOT(AND(LEFT(E6,5)="12.31",IFERROR(S6/$G$6,"")&lt;&gt;0)),NOT(AND(LEFT(E6,5)="12.32",IFERROR(S6/$G$6,"")&lt;&gt;0))),"", IFERROR(S6/$S$6,""))</f>
         <v/>
       </c>
       <c r="U6" s="19" t="e">
@@ -24135,7 +24135,7 @@
         <v>#N/A</v>
       </c>
       <c r="V6" s="282" t="str">
-        <f>IF(AND(OR(LEFT(C6,3)="12.",LEFT(E6,3)="12.",LEFT(E6,5)="CET &gt;",IFERROR(U6/$U$6,"")=0),NOT(AND(LEFT(E6,5)="12.31",IFERROR(U6/$G$6,"")&lt;&gt;0)),NOT(AND(LEFT(E6,5)="12.32",IFERROR(U6/$G$6,"")&lt;&gt;0))),"", IFERROR(U6/$U$6,""))</f>
+        <f>IF(AND(OR(LEFT(C6,3)="12.",LEFT(E6,3)="12.",LEFT(E6,5)="CET &gt;",IFERROR(U6/$U$6,"")=0),NOT(AND(LEFT(E6,4)="12.8",IFERROR(G6/$G$6,"")&lt;&gt;0)),NOT(AND(LEFT(E6,5)="12.31",IFERROR(U6/$G$6,"")&lt;&gt;0)),NOT(AND(LEFT(E6,5)="12.32",IFERROR(U6/$G$6,"")&lt;&gt;0))),"", IFERROR(U6/$U$6,""))</f>
         <v/>
       </c>
       <c r="W6" t="s">
@@ -24390,16 +24390,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:57" s="41" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B1" s="360" t="s">
+      <c r="B1" s="365" t="s">
         <v>173</v>
       </c>
-      <c r="C1" s="360"/>
-      <c r="D1" s="360"/>
-      <c r="E1" s="360"/>
-      <c r="F1" s="360"/>
-      <c r="G1" s="360"/>
-      <c r="H1" s="360"/>
-      <c r="I1" s="360"/>
+      <c r="C1" s="365"/>
+      <c r="D1" s="365"/>
+      <c r="E1" s="365"/>
+      <c r="F1" s="365"/>
+      <c r="G1" s="365"/>
+      <c r="H1" s="365"/>
+      <c r="I1" s="365"/>
     </row>
     <row r="2" spans="1:57" s="41" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="78"/>
@@ -24411,7 +24411,7 @@
       <c r="G2" s="75" t="s">
         <v>172</v>
       </c>
-      <c r="H2" s="359" t="s">
+      <c r="H2" s="364" t="s">
         <v>171</v>
       </c>
       <c r="I2" s="74" t="s">
@@ -24456,7 +24456,7 @@
       <c r="V2" s="74" t="s">
         <v>170</v>
       </c>
-      <c r="W2" s="359" t="s">
+      <c r="W2" s="364" t="s">
         <v>169</v>
       </c>
       <c r="X2" s="73" t="s">
@@ -24486,7 +24486,7 @@
       <c r="AF2" s="73" t="s">
         <v>167</v>
       </c>
-      <c r="AG2" s="359" t="s">
+      <c r="AG2" s="364" t="s">
         <v>166</v>
       </c>
       <c r="AH2" s="73" t="s">
@@ -24528,7 +24528,7 @@
       <c r="AT2" s="73" t="s">
         <v>165</v>
       </c>
-      <c r="AU2" s="359" t="s">
+      <c r="AU2" s="364" t="s">
         <v>164</v>
       </c>
       <c r="AV2" s="72" t="s">
@@ -24558,7 +24558,7 @@
       <c r="BD2" s="72" t="s">
         <v>163</v>
       </c>
-      <c r="BE2" s="359" t="s">
+      <c r="BE2" s="364" t="s">
         <v>162</v>
       </c>
     </row>
@@ -24572,7 +24572,7 @@
       <c r="G3" s="75" t="s">
         <v>161</v>
       </c>
-      <c r="H3" s="359"/>
+      <c r="H3" s="364"/>
       <c r="I3" s="74" t="s">
         <v>160</v>
       </c>
@@ -24613,7 +24613,7 @@
       <c r="V3" s="74" t="s">
         <v>148</v>
       </c>
-      <c r="W3" s="359"/>
+      <c r="W3" s="364"/>
       <c r="X3" s="73" t="s">
         <v>144</v>
       </c>
@@ -24641,7 +24641,7 @@
       <c r="AF3" s="73" t="s">
         <v>138</v>
       </c>
-      <c r="AG3" s="359"/>
+      <c r="AG3" s="364"/>
       <c r="AH3" s="73" t="s">
         <v>137</v>
       </c>
@@ -24681,7 +24681,7 @@
       <c r="AT3" s="73" t="s">
         <v>125</v>
       </c>
-      <c r="AU3" s="359"/>
+      <c r="AU3" s="364"/>
       <c r="AV3" s="72" t="s">
         <v>124</v>
       </c>
@@ -24709,7 +24709,7 @@
       <c r="BD3" s="72" t="s">
         <v>116</v>
       </c>
-      <c r="BE3" s="359"/>
+      <c r="BE3" s="364"/>
     </row>
     <row r="4" spans="1:57" s="41" customFormat="1" ht="60" x14ac:dyDescent="0.15">
       <c r="A4" s="77"/>
@@ -24731,7 +24731,7 @@
       <c r="G4" s="75" t="s">
         <v>111</v>
       </c>
-      <c r="H4" s="359"/>
+      <c r="H4" s="364"/>
       <c r="I4" s="74" t="s">
         <v>110</v>
       </c>
@@ -24774,7 +24774,7 @@
       <c r="V4" s="74" t="s">
         <v>97</v>
       </c>
-      <c r="W4" s="359"/>
+      <c r="W4" s="364"/>
       <c r="X4" s="73" t="s">
         <v>92</v>
       </c>
@@ -24802,7 +24802,7 @@
       <c r="AF4" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="AG4" s="359"/>
+      <c r="AG4" s="364"/>
       <c r="AH4" s="73" t="s">
         <v>84</v>
       </c>
@@ -24842,7 +24842,7 @@
       <c r="AT4" s="73" t="s">
         <v>72</v>
       </c>
-      <c r="AU4" s="359"/>
+      <c r="AU4" s="364"/>
       <c r="AV4" s="72" t="s">
         <v>71</v>
       </c>
@@ -24870,7 +24870,7 @@
       <c r="BD4" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="BE4" s="359"/>
+      <c r="BE4" s="364"/>
     </row>
     <row r="5" spans="1:57" s="41" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="51" t="s">
@@ -27737,16 +27737,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A1" s="361" t="s">
+      <c r="A1" s="366" t="s">
         <v>217</v>
       </c>
-      <c r="B1" s="361"/>
-      <c r="C1" s="361"/>
-      <c r="D1" s="361"/>
-      <c r="E1" s="361"/>
-      <c r="F1" s="361"/>
-      <c r="G1" s="361"/>
-      <c r="H1" s="361"/>
+      <c r="B1" s="366"/>
+      <c r="C1" s="366"/>
+      <c r="D1" s="366"/>
+      <c r="E1" s="366"/>
+      <c r="F1" s="366"/>
+      <c r="G1" s="366"/>
+      <c r="H1" s="366"/>
       <c r="I1" s="41"/>
       <c r="J1" s="41"/>
       <c r="K1" s="41"/>
@@ -27783,7 +27783,7 @@
       <c r="G2" s="75" t="s">
         <v>172</v>
       </c>
-      <c r="H2" s="359" t="s">
+      <c r="H2" s="364" t="s">
         <v>171</v>
       </c>
       <c r="I2" s="75" t="s">
@@ -27816,7 +27816,7 @@
       <c r="R2" s="75" t="s">
         <v>170</v>
       </c>
-      <c r="S2" s="359" t="s">
+      <c r="S2" s="364" t="s">
         <v>169</v>
       </c>
       <c r="T2" s="75" t="s">
@@ -27846,7 +27846,7 @@
       <c r="AB2" s="75" t="s">
         <v>167</v>
       </c>
-      <c r="AC2" s="359" t="s">
+      <c r="AC2" s="364" t="s">
         <v>216</v>
       </c>
       <c r="AD2" s="75" t="s">
@@ -27858,7 +27858,7 @@
       <c r="AF2" s="75" t="s">
         <v>215</v>
       </c>
-      <c r="AG2" s="359" t="s">
+      <c r="AG2" s="364" t="s">
         <v>214</v>
       </c>
     </row>
@@ -27872,7 +27872,7 @@
       <c r="G3" s="75" t="s">
         <v>161</v>
       </c>
-      <c r="H3" s="359"/>
+      <c r="H3" s="364"/>
       <c r="I3" s="75" t="s">
         <v>213</v>
       </c>
@@ -27903,7 +27903,7 @@
       <c r="R3" s="75" t="s">
         <v>148</v>
       </c>
-      <c r="S3" s="359"/>
+      <c r="S3" s="364"/>
       <c r="T3" s="75" t="s">
         <v>204</v>
       </c>
@@ -27931,7 +27931,7 @@
       <c r="AB3" s="75" t="s">
         <v>196</v>
       </c>
-      <c r="AC3" s="359"/>
+      <c r="AC3" s="364"/>
       <c r="AD3" s="75" t="s">
         <v>195</v>
       </c>
@@ -27941,7 +27941,7 @@
       <c r="AF3" s="75" t="s">
         <v>125</v>
       </c>
-      <c r="AG3" s="359"/>
+      <c r="AG3" s="364"/>
     </row>
     <row r="4" spans="1:33" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="78"/>
@@ -27963,7 +27963,7 @@
       <c r="G4" s="75" t="s">
         <v>111</v>
       </c>
-      <c r="H4" s="359"/>
+      <c r="H4" s="364"/>
       <c r="I4" s="75" t="s">
         <v>194</v>
       </c>
@@ -27994,7 +27994,7 @@
       <c r="R4" s="75" t="s">
         <v>97</v>
       </c>
-      <c r="S4" s="359"/>
+      <c r="S4" s="364"/>
       <c r="T4" s="75" t="s">
         <v>185</v>
       </c>
@@ -28022,7 +28022,7 @@
       <c r="AB4" s="75" t="s">
         <v>177</v>
       </c>
-      <c r="AC4" s="359"/>
+      <c r="AC4" s="364"/>
       <c r="AD4" s="75" t="s">
         <v>176</v>
       </c>
@@ -28032,7 +28032,7 @@
       <c r="AF4" s="75" t="s">
         <v>72</v>
       </c>
-      <c r="AG4" s="359"/>
+      <c r="AG4" s="364"/>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A5" s="81" t="s">
@@ -29407,13 +29407,13 @@
       <c r="G2" s="75" t="s">
         <v>170</v>
       </c>
-      <c r="H2" s="359" t="s">
+      <c r="H2" s="364" t="s">
         <v>169</v>
       </c>
       <c r="I2" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="359" t="s">
+      <c r="J2" s="364" t="s">
         <v>168</v>
       </c>
     </row>
@@ -29427,11 +29427,11 @@
       <c r="G3" s="75" t="s">
         <v>148</v>
       </c>
-      <c r="H3" s="359"/>
+      <c r="H3" s="364"/>
       <c r="I3" s="75" t="s">
         <v>145</v>
       </c>
-      <c r="J3" s="359"/>
+      <c r="J3" s="364"/>
     </row>
     <row r="4" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A4" s="97"/>
@@ -29453,11 +29453,11 @@
       <c r="G4" s="75" t="s">
         <v>97</v>
       </c>
-      <c r="H4" s="359"/>
+      <c r="H4" s="364"/>
       <c r="I4" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="J4" s="359"/>
+      <c r="J4" s="364"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="91" t="s">
@@ -29883,7 +29883,7 @@
       <c r="P2" s="316" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="362" t="s">
+      <c r="Q2" s="367" t="s">
         <v>434</v>
       </c>
     </row>
@@ -29924,7 +29924,7 @@
       <c r="P3" s="316" t="s">
         <v>441</v>
       </c>
-      <c r="Q3" s="362"/>
+      <c r="Q3" s="367"/>
     </row>
     <row r="4" spans="1:62" ht="70" x14ac:dyDescent="0.2">
       <c r="A4" s="317"/>
@@ -29973,7 +29973,7 @@
       <c r="P4" s="319" t="s">
         <v>452</v>
       </c>
-      <c r="Q4" s="362"/>
+      <c r="Q4" s="367"/>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A5" s="320" t="s">

</xml_diff>

<commit_message>
extractor lines switch tj
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A4DF08-A0BA-A74B-A3A3-DB14EF00192D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D885D31A-70B3-374B-89AB-98BEDBE8ACC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
@@ -15817,6 +15817,50 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="4" applyFont="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="28" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="40" fontId="37" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="81" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="83" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="29" fillId="8" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="8" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="84" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="23" fillId="10" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="67" fillId="28" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="48" fillId="28" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="81" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="39" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -15974,50 +16018,6 @@
     </xf>
     <xf numFmtId="49" fontId="31" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="4" applyFont="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="28" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="40" fontId="37" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="81" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="83" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="29" fillId="8" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="8" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="84" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="23" fillId="10" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="67" fillId="28" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="48" fillId="28" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="81" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -17085,11 +17085,11 @@
       <c r="B1" s="115" t="s">
         <v>223</v>
       </c>
-      <c r="C1" s="347" t="s">
+      <c r="C1" s="363" t="s">
         <v>224</v>
       </c>
-      <c r="D1" s="347"/>
-      <c r="E1" s="347"/>
+      <c r="D1" s="363"/>
+      <c r="E1" s="363"/>
       <c r="F1" s="116"/>
       <c r="H1" s="26" t="s">
         <v>0</v>
@@ -17098,11 +17098,11 @@
     <row r="2" spans="1:8" s="120" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="117"/>
       <c r="B2" s="118"/>
-      <c r="C2" s="348" t="s">
+      <c r="C2" s="364" t="s">
         <v>225</v>
       </c>
-      <c r="D2" s="348"/>
-      <c r="E2" s="348"/>
+      <c r="D2" s="364"/>
+      <c r="E2" s="364"/>
       <c r="F2" s="119"/>
       <c r="H2" s="26" t="s">
         <v>0</v>
@@ -17126,10 +17126,10 @@
       <c r="D4" s="125" t="s">
         <v>228</v>
       </c>
-      <c r="E4" s="352" t="s">
+      <c r="E4" s="368" t="s">
         <v>229</v>
       </c>
-      <c r="F4" s="353"/>
+      <c r="F4" s="369"/>
       <c r="G4" s="134"/>
       <c r="H4" s="26" t="s">
         <v>0</v>
@@ -17146,10 +17146,10 @@
       <c r="D5" s="131" t="s">
         <v>232</v>
       </c>
-      <c r="E5" s="354" t="s">
+      <c r="E5" s="370" t="s">
         <v>245</v>
       </c>
-      <c r="F5" s="355"/>
+      <c r="F5" s="371"/>
       <c r="G5" s="133"/>
       <c r="H5" s="26" t="s">
         <v>0</v>
@@ -17166,10 +17166,10 @@
       <c r="D6" s="132" t="s">
         <v>235</v>
       </c>
-      <c r="E6" s="356" t="s">
+      <c r="E6" s="372" t="s">
         <v>246</v>
       </c>
-      <c r="F6" s="357"/>
+      <c r="F6" s="373"/>
       <c r="G6" s="133"/>
       <c r="H6" s="26" t="s">
         <v>0</v>
@@ -17186,10 +17186,10 @@
       <c r="D7" s="132" t="s">
         <v>238</v>
       </c>
-      <c r="E7" s="356" t="s">
+      <c r="E7" s="372" t="s">
         <v>245</v>
       </c>
-      <c r="F7" s="357"/>
+      <c r="F7" s="373"/>
       <c r="G7" s="133"/>
       <c r="H7" s="26" t="s">
         <v>0</v>
@@ -17200,16 +17200,16 @@
       <c r="B8" s="138" t="s">
         <v>239</v>
       </c>
-      <c r="C8" s="358" t="s">
+      <c r="C8" s="374" t="s">
         <v>240</v>
       </c>
-      <c r="D8" s="358" t="s">
+      <c r="D8" s="374" t="s">
         <v>241</v>
       </c>
-      <c r="E8" s="361" t="s">
+      <c r="E8" s="377" t="s">
         <v>247</v>
       </c>
-      <c r="F8" s="361"/>
+      <c r="F8" s="377"/>
       <c r="G8" s="133"/>
       <c r="H8" s="26" t="s">
         <v>0</v>
@@ -17220,10 +17220,10 @@
       <c r="B9" s="304" t="s">
         <v>242</v>
       </c>
-      <c r="C9" s="359"/>
-      <c r="D9" s="359"/>
-      <c r="E9" s="362"/>
-      <c r="F9" s="362"/>
+      <c r="C9" s="375"/>
+      <c r="D9" s="375"/>
+      <c r="E9" s="378"/>
+      <c r="F9" s="378"/>
       <c r="G9" s="133"/>
       <c r="H9" s="26" t="s">
         <v>0</v>
@@ -17234,10 +17234,10 @@
       <c r="B10" s="305" t="s">
         <v>243</v>
       </c>
-      <c r="C10" s="359"/>
-      <c r="D10" s="359"/>
-      <c r="E10" s="362"/>
-      <c r="F10" s="362"/>
+      <c r="C10" s="375"/>
+      <c r="D10" s="375"/>
+      <c r="E10" s="378"/>
+      <c r="F10" s="378"/>
       <c r="G10" s="133"/>
       <c r="H10" s="26" t="s">
         <v>0</v>
@@ -17248,10 +17248,10 @@
       <c r="B11" s="300" t="s">
         <v>367</v>
       </c>
-      <c r="C11" s="360"/>
-      <c r="D11" s="360"/>
-      <c r="E11" s="363"/>
-      <c r="F11" s="363"/>
+      <c r="C11" s="376"/>
+      <c r="D11" s="376"/>
+      <c r="E11" s="379"/>
+      <c r="F11" s="379"/>
       <c r="G11" s="133"/>
       <c r="H11" s="26" t="s">
         <v>0</v>
@@ -17271,11 +17271,11 @@
     <row r="13" spans="1:8" s="26" customFormat="1" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="121"/>
       <c r="B13" s="302"/>
-      <c r="C13" s="351" t="s">
+      <c r="C13" s="367" t="s">
         <v>244</v>
       </c>
-      <c r="D13" s="351"/>
-      <c r="E13" s="351"/>
+      <c r="D13" s="367"/>
+      <c r="E13" s="367"/>
       <c r="F13" s="303"/>
       <c r="H13" s="26" t="s">
         <v>0</v>
@@ -17289,14 +17289,14 @@
       </c>
     </row>
     <row r="15" spans="1:8" s="26" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="349" t="s">
+      <c r="A15" s="365" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="349"/>
-      <c r="C15" s="349"/>
-      <c r="D15" s="349"/>
-      <c r="E15" s="349"/>
-      <c r="F15" s="350"/>
+      <c r="B15" s="365"/>
+      <c r="C15" s="365"/>
+      <c r="D15" s="365"/>
+      <c r="E15" s="365"/>
+      <c r="F15" s="366"/>
       <c r="H15" s="26" t="s">
         <v>0</v>
       </c>
@@ -17425,13 +17425,13 @@
       <c r="A2" s="78"/>
       <c r="B2" s="78"/>
       <c r="C2" s="78"/>
-      <c r="D2" s="395"/>
-      <c r="E2" s="395"/>
-      <c r="F2" s="395"/>
+      <c r="D2" s="347"/>
+      <c r="E2" s="347"/>
+      <c r="F2" s="347"/>
       <c r="G2" s="75" t="s">
         <v>169</v>
       </c>
-      <c r="H2" s="373" t="s">
+      <c r="H2" s="389" t="s">
         <v>168</v>
       </c>
       <c r="I2" s="74" t="s">
@@ -17476,7 +17476,7 @@
       <c r="V2" s="74" t="s">
         <v>167</v>
       </c>
-      <c r="W2" s="373" t="s">
+      <c r="W2" s="389" t="s">
         <v>166</v>
       </c>
       <c r="X2" s="73" t="s">
@@ -17506,7 +17506,7 @@
       <c r="AF2" s="73" t="s">
         <v>164</v>
       </c>
-      <c r="AG2" s="373" t="s">
+      <c r="AG2" s="389" t="s">
         <v>163</v>
       </c>
       <c r="AH2" s="73" t="s">
@@ -17548,7 +17548,7 @@
       <c r="AT2" s="73" t="s">
         <v>162</v>
       </c>
-      <c r="AU2" s="373" t="s">
+      <c r="AU2" s="389" t="s">
         <v>161</v>
       </c>
       <c r="AV2" s="72" t="s">
@@ -17578,7 +17578,7 @@
       <c r="BD2" s="72" t="s">
         <v>160</v>
       </c>
-      <c r="BE2" s="373" t="s">
+      <c r="BE2" s="389" t="s">
         <v>159</v>
       </c>
       <c r="BF2"/>
@@ -17593,7 +17593,7 @@
       <c r="G3" s="75" t="s">
         <v>158</v>
       </c>
-      <c r="H3" s="373"/>
+      <c r="H3" s="389"/>
       <c r="I3" s="74" t="s">
         <v>157</v>
       </c>
@@ -17634,7 +17634,7 @@
       <c r="V3" s="74" t="s">
         <v>145</v>
       </c>
-      <c r="W3" s="373"/>
+      <c r="W3" s="389"/>
       <c r="X3" s="73" t="s">
         <v>141</v>
       </c>
@@ -17662,7 +17662,7 @@
       <c r="AF3" s="73" t="s">
         <v>135</v>
       </c>
-      <c r="AG3" s="373"/>
+      <c r="AG3" s="389"/>
       <c r="AH3" s="73" t="s">
         <v>134</v>
       </c>
@@ -17702,7 +17702,7 @@
       <c r="AT3" s="73" t="s">
         <v>122</v>
       </c>
-      <c r="AU3" s="373"/>
+      <c r="AU3" s="389"/>
       <c r="AV3" s="72" t="s">
         <v>121</v>
       </c>
@@ -17730,7 +17730,7 @@
       <c r="BD3" s="72" t="s">
         <v>113</v>
       </c>
-      <c r="BE3" s="373"/>
+      <c r="BE3" s="389"/>
     </row>
     <row r="4" spans="1:58" s="41" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="77"/>
@@ -17752,7 +17752,7 @@
       <c r="G4" s="75" t="s">
         <v>108</v>
       </c>
-      <c r="H4" s="373"/>
+      <c r="H4" s="389"/>
       <c r="I4" s="74" t="s">
         <v>107</v>
       </c>
@@ -17795,7 +17795,7 @@
       <c r="V4" s="74" t="s">
         <v>94</v>
       </c>
-      <c r="W4" s="373"/>
+      <c r="W4" s="389"/>
       <c r="X4" s="73" t="s">
         <v>92</v>
       </c>
@@ -17823,7 +17823,7 @@
       <c r="AF4" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="AG4" s="373"/>
+      <c r="AG4" s="389"/>
       <c r="AH4" s="73" t="s">
         <v>611</v>
       </c>
@@ -17863,7 +17863,7 @@
       <c r="AT4" s="73" t="s">
         <v>72</v>
       </c>
-      <c r="AU4" s="373"/>
+      <c r="AU4" s="389"/>
       <c r="AV4" s="72" t="s">
         <v>71</v>
       </c>
@@ -17891,7 +17891,7 @@
       <c r="BD4" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="BE4" s="373"/>
+      <c r="BE4" s="389"/>
       <c r="BF4"/>
     </row>
     <row r="5" spans="1:58" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -20241,273 +20241,273 @@
       </c>
     </row>
     <row r="17" spans="4:57" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D17" s="395"/>
-      <c r="E17" s="395"/>
-      <c r="F17" s="395"/>
-      <c r="G17" s="395"/>
-      <c r="H17" s="395"/>
-      <c r="I17" s="395"/>
-      <c r="J17" s="395"/>
-      <c r="K17" s="395"/>
-      <c r="L17" s="395"/>
-      <c r="M17" s="395"/>
-      <c r="N17" s="395"/>
-      <c r="O17" s="395"/>
-      <c r="P17" s="395"/>
-      <c r="Q17" s="395"/>
-      <c r="R17" s="395"/>
-      <c r="S17" s="395"/>
-      <c r="T17" s="395"/>
-      <c r="U17" s="395"/>
-      <c r="V17" s="395"/>
-      <c r="W17" s="396"/>
-      <c r="X17" s="395"/>
-      <c r="Y17" s="395"/>
-      <c r="Z17" s="395"/>
-      <c r="AA17" s="395"/>
-      <c r="AB17" s="395"/>
-      <c r="AC17" s="395"/>
-      <c r="AD17" s="395"/>
-      <c r="AE17" s="395"/>
-      <c r="AF17" s="395"/>
-      <c r="AG17" s="395"/>
-      <c r="AH17" s="395"/>
-      <c r="AI17" s="395"/>
-      <c r="AJ17" s="395"/>
-      <c r="AK17" s="395"/>
-      <c r="AL17" s="395"/>
-      <c r="AM17" s="395"/>
-      <c r="AN17" s="395"/>
-      <c r="AO17" s="395"/>
-      <c r="AP17" s="395"/>
-      <c r="AQ17" s="395"/>
-      <c r="AR17" s="395"/>
-      <c r="AS17" s="395"/>
-      <c r="AT17" s="395"/>
-      <c r="AU17" s="396"/>
-      <c r="AV17" s="395"/>
-      <c r="AW17" s="395"/>
-      <c r="AX17" s="395"/>
-      <c r="AY17" s="395"/>
-      <c r="AZ17" s="395"/>
-      <c r="BA17" s="395"/>
-      <c r="BB17" s="395"/>
-      <c r="BC17" s="395"/>
-      <c r="BD17" s="395"/>
-      <c r="BE17" s="395"/>
+      <c r="D17" s="347"/>
+      <c r="E17" s="347"/>
+      <c r="F17" s="347"/>
+      <c r="G17" s="347"/>
+      <c r="H17" s="347"/>
+      <c r="I17" s="347"/>
+      <c r="J17" s="347"/>
+      <c r="K17" s="347"/>
+      <c r="L17" s="347"/>
+      <c r="M17" s="347"/>
+      <c r="N17" s="347"/>
+      <c r="O17" s="347"/>
+      <c r="P17" s="347"/>
+      <c r="Q17" s="347"/>
+      <c r="R17" s="347"/>
+      <c r="S17" s="347"/>
+      <c r="T17" s="347"/>
+      <c r="U17" s="347"/>
+      <c r="V17" s="347"/>
+      <c r="W17" s="348"/>
+      <c r="X17" s="347"/>
+      <c r="Y17" s="347"/>
+      <c r="Z17" s="347"/>
+      <c r="AA17" s="347"/>
+      <c r="AB17" s="347"/>
+      <c r="AC17" s="347"/>
+      <c r="AD17" s="347"/>
+      <c r="AE17" s="347"/>
+      <c r="AF17" s="347"/>
+      <c r="AG17" s="347"/>
+      <c r="AH17" s="347"/>
+      <c r="AI17" s="347"/>
+      <c r="AJ17" s="347"/>
+      <c r="AK17" s="347"/>
+      <c r="AL17" s="347"/>
+      <c r="AM17" s="347"/>
+      <c r="AN17" s="347"/>
+      <c r="AO17" s="347"/>
+      <c r="AP17" s="347"/>
+      <c r="AQ17" s="347"/>
+      <c r="AR17" s="347"/>
+      <c r="AS17" s="347"/>
+      <c r="AT17" s="347"/>
+      <c r="AU17" s="348"/>
+      <c r="AV17" s="347"/>
+      <c r="AW17" s="347"/>
+      <c r="AX17" s="347"/>
+      <c r="AY17" s="347"/>
+      <c r="AZ17" s="347"/>
+      <c r="BA17" s="347"/>
+      <c r="BB17" s="347"/>
+      <c r="BC17" s="347"/>
+      <c r="BD17" s="347"/>
+      <c r="BE17" s="347"/>
     </row>
     <row r="18" spans="4:57" hidden="1" x14ac:dyDescent="0.2">
-      <c r="D18" s="395"/>
-      <c r="E18" s="395"/>
-      <c r="F18" s="395"/>
-      <c r="G18" s="395"/>
-      <c r="H18" s="395"/>
-      <c r="I18" s="395"/>
-      <c r="J18" s="395"/>
-      <c r="K18" s="395"/>
-      <c r="L18" s="395"/>
-      <c r="M18" s="395"/>
-      <c r="N18" s="395"/>
-      <c r="O18" s="395"/>
-      <c r="P18" s="395"/>
-      <c r="Q18" s="395"/>
-      <c r="R18" s="395"/>
-      <c r="S18" s="395"/>
-      <c r="T18" s="395"/>
-      <c r="U18" s="395"/>
-      <c r="V18" s="395"/>
-      <c r="W18" s="397"/>
-      <c r="X18" s="395"/>
-      <c r="Y18" s="395"/>
-      <c r="Z18" s="395"/>
-      <c r="AA18" s="395"/>
-      <c r="AB18" s="395"/>
-      <c r="AC18" s="395"/>
-      <c r="AD18" s="395"/>
-      <c r="AE18" s="395"/>
-      <c r="AF18" s="395"/>
-      <c r="AG18" s="395"/>
-      <c r="AH18" s="395"/>
-      <c r="AI18" s="395"/>
-      <c r="AJ18" s="395"/>
-      <c r="AK18" s="395"/>
-      <c r="AL18" s="395"/>
-      <c r="AM18" s="395"/>
-      <c r="AN18" s="395"/>
-      <c r="AO18" s="395"/>
-      <c r="AP18" s="395"/>
-      <c r="AQ18" s="395"/>
-      <c r="AR18" s="395"/>
-      <c r="AS18" s="395"/>
-      <c r="AT18" s="395"/>
-      <c r="AU18" s="397">
+      <c r="D18" s="347"/>
+      <c r="E18" s="347"/>
+      <c r="F18" s="347"/>
+      <c r="G18" s="347"/>
+      <c r="H18" s="347"/>
+      <c r="I18" s="347"/>
+      <c r="J18" s="347"/>
+      <c r="K18" s="347"/>
+      <c r="L18" s="347"/>
+      <c r="M18" s="347"/>
+      <c r="N18" s="347"/>
+      <c r="O18" s="347"/>
+      <c r="P18" s="347"/>
+      <c r="Q18" s="347"/>
+      <c r="R18" s="347"/>
+      <c r="S18" s="347"/>
+      <c r="T18" s="347"/>
+      <c r="U18" s="347"/>
+      <c r="V18" s="347"/>
+      <c r="W18" s="349"/>
+      <c r="X18" s="347"/>
+      <c r="Y18" s="347"/>
+      <c r="Z18" s="347"/>
+      <c r="AA18" s="347"/>
+      <c r="AB18" s="347"/>
+      <c r="AC18" s="347"/>
+      <c r="AD18" s="347"/>
+      <c r="AE18" s="347"/>
+      <c r="AF18" s="347"/>
+      <c r="AG18" s="347"/>
+      <c r="AH18" s="347"/>
+      <c r="AI18" s="347"/>
+      <c r="AJ18" s="347"/>
+      <c r="AK18" s="347"/>
+      <c r="AL18" s="347"/>
+      <c r="AM18" s="347"/>
+      <c r="AN18" s="347"/>
+      <c r="AO18" s="347"/>
+      <c r="AP18" s="347"/>
+      <c r="AQ18" s="347"/>
+      <c r="AR18" s="347"/>
+      <c r="AS18" s="347"/>
+      <c r="AT18" s="347"/>
+      <c r="AU18" s="349">
         <f>AU16+AG16-AU14-AG14-AU13-AU12-AG13-AG12</f>
         <v>0</v>
       </c>
-      <c r="AV18" s="395"/>
-      <c r="AW18" s="395"/>
-      <c r="AX18" s="395"/>
-      <c r="AY18" s="395"/>
-      <c r="AZ18" s="395"/>
-      <c r="BA18" s="395"/>
-      <c r="BB18" s="395"/>
-      <c r="BC18" s="395"/>
-      <c r="BD18" s="395"/>
-      <c r="BE18" s="395"/>
+      <c r="AV18" s="347"/>
+      <c r="AW18" s="347"/>
+      <c r="AX18" s="347"/>
+      <c r="AY18" s="347"/>
+      <c r="AZ18" s="347"/>
+      <c r="BA18" s="347"/>
+      <c r="BB18" s="347"/>
+      <c r="BC18" s="347"/>
+      <c r="BD18" s="347"/>
+      <c r="BE18" s="347"/>
     </row>
     <row r="19" spans="4:57" x14ac:dyDescent="0.2">
-      <c r="D19" s="395"/>
-      <c r="E19" s="395"/>
-      <c r="F19" s="395"/>
-      <c r="G19" s="395"/>
-      <c r="H19" s="395"/>
-      <c r="I19" s="395"/>
-      <c r="J19" s="395"/>
-      <c r="K19" s="395"/>
-      <c r="L19" s="395"/>
-      <c r="M19" s="395"/>
-      <c r="N19" s="395"/>
-      <c r="O19" s="395"/>
-      <c r="P19" s="395"/>
-      <c r="Q19" s="395"/>
-      <c r="R19" s="395"/>
-      <c r="S19" s="395"/>
-      <c r="T19" s="395"/>
-      <c r="U19" s="395"/>
-      <c r="V19" s="395"/>
-      <c r="W19" s="395"/>
-      <c r="X19" s="395"/>
-      <c r="Y19" s="395"/>
-      <c r="Z19" s="395"/>
-      <c r="AA19" s="395"/>
-      <c r="AB19" s="395"/>
-      <c r="AC19" s="395"/>
-      <c r="AD19" s="395"/>
-      <c r="AE19" s="395"/>
-      <c r="AF19" s="395"/>
-      <c r="AG19" s="395"/>
-      <c r="AH19" s="395"/>
-      <c r="AI19" s="395"/>
-      <c r="AJ19" s="395"/>
-      <c r="AK19" s="395"/>
-      <c r="AL19" s="395"/>
-      <c r="AM19" s="395"/>
-      <c r="AN19" s="395"/>
-      <c r="AO19" s="395"/>
-      <c r="AP19" s="395"/>
-      <c r="AQ19" s="395"/>
-      <c r="AR19" s="395"/>
-      <c r="AS19" s="395"/>
-      <c r="AT19" s="395"/>
-      <c r="AU19" s="395"/>
-      <c r="AV19" s="395"/>
-      <c r="AW19" s="395"/>
-      <c r="AX19" s="395"/>
-      <c r="AY19" s="395"/>
-      <c r="AZ19" s="395"/>
-      <c r="BA19" s="395"/>
-      <c r="BB19" s="395"/>
-      <c r="BC19" s="395"/>
-      <c r="BD19" s="395"/>
-      <c r="BE19" s="395"/>
+      <c r="D19" s="347"/>
+      <c r="E19" s="347"/>
+      <c r="F19" s="347"/>
+      <c r="G19" s="347"/>
+      <c r="H19" s="347"/>
+      <c r="I19" s="347"/>
+      <c r="J19" s="347"/>
+      <c r="K19" s="347"/>
+      <c r="L19" s="347"/>
+      <c r="M19" s="347"/>
+      <c r="N19" s="347"/>
+      <c r="O19" s="347"/>
+      <c r="P19" s="347"/>
+      <c r="Q19" s="347"/>
+      <c r="R19" s="347"/>
+      <c r="S19" s="347"/>
+      <c r="T19" s="347"/>
+      <c r="U19" s="347"/>
+      <c r="V19" s="347"/>
+      <c r="W19" s="347"/>
+      <c r="X19" s="347"/>
+      <c r="Y19" s="347"/>
+      <c r="Z19" s="347"/>
+      <c r="AA19" s="347"/>
+      <c r="AB19" s="347"/>
+      <c r="AC19" s="347"/>
+      <c r="AD19" s="347"/>
+      <c r="AE19" s="347"/>
+      <c r="AF19" s="347"/>
+      <c r="AG19" s="347"/>
+      <c r="AH19" s="347"/>
+      <c r="AI19" s="347"/>
+      <c r="AJ19" s="347"/>
+      <c r="AK19" s="347"/>
+      <c r="AL19" s="347"/>
+      <c r="AM19" s="347"/>
+      <c r="AN19" s="347"/>
+      <c r="AO19" s="347"/>
+      <c r="AP19" s="347"/>
+      <c r="AQ19" s="347"/>
+      <c r="AR19" s="347"/>
+      <c r="AS19" s="347"/>
+      <c r="AT19" s="347"/>
+      <c r="AU19" s="347"/>
+      <c r="AV19" s="347"/>
+      <c r="AW19" s="347"/>
+      <c r="AX19" s="347"/>
+      <c r="AY19" s="347"/>
+      <c r="AZ19" s="347"/>
+      <c r="BA19" s="347"/>
+      <c r="BB19" s="347"/>
+      <c r="BC19" s="347"/>
+      <c r="BD19" s="347"/>
+      <c r="BE19" s="347"/>
     </row>
     <row r="20" spans="4:57" ht="24" x14ac:dyDescent="0.2">
-      <c r="D20" s="395"/>
-      <c r="E20" s="395"/>
-      <c r="F20" s="398" t="s">
+      <c r="D20" s="347"/>
+      <c r="E20" s="347"/>
+      <c r="F20" s="350" t="s">
         <v>253</v>
       </c>
       <c r="G20" s="152" t="str">
         <f>IF(ISBLANK(ETPT_TJ_DDG!$D$5),"",IF(ISERROR(ETPT_TJ!G20),"",IF(ETPT_TJ!G20=0,"",ETPT_TJ!G20)))</f>
         <v/>
       </c>
-      <c r="H20" s="395"/>
-      <c r="I20" s="395"/>
-      <c r="J20" s="395"/>
-      <c r="K20" s="395"/>
-      <c r="L20" s="395"/>
-      <c r="M20" s="395"/>
-      <c r="N20" s="395"/>
-      <c r="O20" s="395"/>
-      <c r="P20" s="395"/>
-      <c r="Q20" s="395"/>
-      <c r="R20" s="395"/>
-      <c r="S20" s="395"/>
-      <c r="T20" s="395"/>
-      <c r="U20" s="399" t="s">
+      <c r="H20" s="347"/>
+      <c r="I20" s="347"/>
+      <c r="J20" s="347"/>
+      <c r="K20" s="347"/>
+      <c r="L20" s="347"/>
+      <c r="M20" s="347"/>
+      <c r="N20" s="347"/>
+      <c r="O20" s="347"/>
+      <c r="P20" s="347"/>
+      <c r="Q20" s="347"/>
+      <c r="R20" s="347"/>
+      <c r="S20" s="347"/>
+      <c r="T20" s="347"/>
+      <c r="U20" s="351" t="s">
         <v>254</v>
       </c>
       <c r="V20" s="152" t="str">
         <f>IF(ISBLANK(ETPT_TJ_DDG!$D$5),"",IF(ISERROR(ETPT_TJ!V20),"",IF(ETPT_TJ!V20=0,"",ETPT_TJ!V20)))</f>
         <v/>
       </c>
-      <c r="W20" s="395"/>
-      <c r="X20" s="395"/>
-      <c r="Y20" s="395"/>
-      <c r="Z20" s="395"/>
-      <c r="AA20" s="395"/>
-      <c r="AB20" s="395"/>
-      <c r="AC20" s="400"/>
-      <c r="AD20" s="395"/>
-      <c r="AE20" s="395"/>
-      <c r="AF20" s="395"/>
-      <c r="AG20" s="395"/>
-      <c r="AH20" s="395"/>
-      <c r="AI20" s="395"/>
-      <c r="AJ20" s="395"/>
-      <c r="AK20" s="395"/>
-      <c r="AL20" s="395"/>
-      <c r="AM20" s="395"/>
-      <c r="AN20" s="395"/>
-      <c r="AO20" s="395"/>
-      <c r="AP20" s="395"/>
-      <c r="AQ20" s="395"/>
-      <c r="AR20" s="395"/>
-      <c r="AS20" s="399" t="s">
+      <c r="W20" s="347"/>
+      <c r="X20" s="347"/>
+      <c r="Y20" s="347"/>
+      <c r="Z20" s="347"/>
+      <c r="AA20" s="347"/>
+      <c r="AB20" s="347"/>
+      <c r="AC20" s="352"/>
+      <c r="AD20" s="347"/>
+      <c r="AE20" s="347"/>
+      <c r="AF20" s="347"/>
+      <c r="AG20" s="347"/>
+      <c r="AH20" s="347"/>
+      <c r="AI20" s="347"/>
+      <c r="AJ20" s="347"/>
+      <c r="AK20" s="347"/>
+      <c r="AL20" s="347"/>
+      <c r="AM20" s="347"/>
+      <c r="AN20" s="347"/>
+      <c r="AO20" s="347"/>
+      <c r="AP20" s="347"/>
+      <c r="AQ20" s="347"/>
+      <c r="AR20" s="347"/>
+      <c r="AS20" s="351" t="s">
         <v>252</v>
       </c>
       <c r="AT20" s="152" t="str">
         <f>IF(ISBLANK(ETPT_TJ_DDG!$D$5),"",IF(ISERROR(ETPT_TJ!AT20),"",IF(ETPT_TJ!AT20=0,"",ETPT_TJ!AT20)))</f>
         <v/>
       </c>
-      <c r="AU20" s="395"/>
-      <c r="AV20" s="395"/>
-      <c r="AW20" s="395"/>
-      <c r="AX20" s="395"/>
-      <c r="AY20" s="395"/>
-      <c r="AZ20" s="395"/>
-      <c r="BA20" s="395"/>
-      <c r="BB20" s="395"/>
-      <c r="BC20" s="395"/>
-      <c r="BD20" s="395"/>
-      <c r="BE20" s="395"/>
+      <c r="AU20" s="347"/>
+      <c r="AV20" s="347"/>
+      <c r="AW20" s="347"/>
+      <c r="AX20" s="347"/>
+      <c r="AY20" s="347"/>
+      <c r="AZ20" s="347"/>
+      <c r="BA20" s="347"/>
+      <c r="BB20" s="347"/>
+      <c r="BC20" s="347"/>
+      <c r="BD20" s="347"/>
+      <c r="BE20" s="347"/>
     </row>
     <row r="21" spans="4:57" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E21" s="39"/>
     </row>
     <row r="22" spans="4:57" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E22" s="377" t="s">
+      <c r="E22" s="393" t="s">
         <v>370</v>
       </c>
-      <c r="F22" s="378"/>
-      <c r="G22" s="378"/>
-      <c r="H22" s="378"/>
-      <c r="I22" s="378"/>
-      <c r="J22" s="378"/>
-      <c r="K22" s="378"/>
-      <c r="L22" s="378"/>
-      <c r="M22" s="378"/>
-      <c r="N22" s="378"/>
-      <c r="O22" s="378"/>
-      <c r="P22" s="378"/>
-      <c r="Q22" s="378"/>
-      <c r="R22" s="378"/>
-      <c r="S22" s="378"/>
-      <c r="T22" s="378"/>
-      <c r="U22" s="378"/>
-      <c r="V22" s="378"/>
-      <c r="W22" s="378"/>
-      <c r="X22" s="379"/>
+      <c r="F22" s="394"/>
+      <c r="G22" s="394"/>
+      <c r="H22" s="394"/>
+      <c r="I22" s="394"/>
+      <c r="J22" s="394"/>
+      <c r="K22" s="394"/>
+      <c r="L22" s="394"/>
+      <c r="M22" s="394"/>
+      <c r="N22" s="394"/>
+      <c r="O22" s="394"/>
+      <c r="P22" s="394"/>
+      <c r="Q22" s="394"/>
+      <c r="R22" s="394"/>
+      <c r="S22" s="394"/>
+      <c r="T22" s="394"/>
+      <c r="U22" s="394"/>
+      <c r="V22" s="394"/>
+      <c r="W22" s="394"/>
+      <c r="X22" s="395"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -20613,13 +20613,13 @@
       <c r="A2" s="78"/>
       <c r="B2" s="78"/>
       <c r="C2" s="78"/>
-      <c r="D2" s="395"/>
-      <c r="E2" s="395"/>
-      <c r="F2" s="395"/>
+      <c r="D2" s="347"/>
+      <c r="E2" s="347"/>
+      <c r="F2" s="347"/>
       <c r="G2" s="75" t="s">
         <v>169</v>
       </c>
-      <c r="H2" s="373" t="s">
+      <c r="H2" s="389" t="s">
         <v>168</v>
       </c>
       <c r="I2" s="75" t="s">
@@ -20652,7 +20652,7 @@
       <c r="R2" s="75" t="s">
         <v>167</v>
       </c>
-      <c r="S2" s="373" t="s">
+      <c r="S2" s="389" t="s">
         <v>166</v>
       </c>
       <c r="T2" s="75" t="s">
@@ -20682,7 +20682,7 @@
       <c r="AB2" s="75" t="s">
         <v>164</v>
       </c>
-      <c r="AC2" s="373" t="s">
+      <c r="AC2" s="389" t="s">
         <v>213</v>
       </c>
       <c r="AD2" s="75" t="s">
@@ -20694,7 +20694,7 @@
       <c r="AF2" s="75" t="s">
         <v>212</v>
       </c>
-      <c r="AG2" s="373" t="s">
+      <c r="AG2" s="389" t="s">
         <v>211</v>
       </c>
     </row>
@@ -20702,13 +20702,13 @@
       <c r="A3" s="78"/>
       <c r="B3" s="78"/>
       <c r="C3" s="78"/>
-      <c r="D3" s="395"/>
-      <c r="E3" s="395"/>
-      <c r="F3" s="395"/>
+      <c r="D3" s="347"/>
+      <c r="E3" s="347"/>
+      <c r="F3" s="347"/>
       <c r="G3" s="75" t="s">
         <v>158</v>
       </c>
-      <c r="H3" s="373"/>
+      <c r="H3" s="389"/>
       <c r="I3" s="75" t="s">
         <v>210</v>
       </c>
@@ -20739,7 +20739,7 @@
       <c r="R3" s="75" t="s">
         <v>145</v>
       </c>
-      <c r="S3" s="373"/>
+      <c r="S3" s="389"/>
       <c r="T3" s="75" t="s">
         <v>201</v>
       </c>
@@ -20767,7 +20767,7 @@
       <c r="AB3" s="75" t="s">
         <v>193</v>
       </c>
-      <c r="AC3" s="373"/>
+      <c r="AC3" s="389"/>
       <c r="AD3" s="75" t="s">
         <v>192</v>
       </c>
@@ -20777,7 +20777,7 @@
       <c r="AF3" s="75" t="s">
         <v>122</v>
       </c>
-      <c r="AG3" s="373"/>
+      <c r="AG3" s="389"/>
     </row>
     <row r="4" spans="1:60" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="78"/>
@@ -20799,7 +20799,7 @@
       <c r="G4" s="75" t="s">
         <v>108</v>
       </c>
-      <c r="H4" s="373"/>
+      <c r="H4" s="389"/>
       <c r="I4" s="75" t="s">
         <v>191</v>
       </c>
@@ -20830,7 +20830,7 @@
       <c r="R4" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="S4" s="373"/>
+      <c r="S4" s="389"/>
       <c r="T4" s="75" t="s">
         <v>182</v>
       </c>
@@ -20858,7 +20858,7 @@
       <c r="AB4" s="75" t="s">
         <v>174</v>
       </c>
-      <c r="AC4" s="373"/>
+      <c r="AC4" s="389"/>
       <c r="AD4" s="75" t="s">
         <v>616</v>
       </c>
@@ -20868,7 +20868,7 @@
       <c r="AF4" s="75" t="s">
         <v>72</v>
       </c>
-      <c r="AG4" s="373"/>
+      <c r="AG4" s="389"/>
     </row>
     <row r="5" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A5" s="81" t="s">
@@ -22361,83 +22361,83 @@
       </c>
     </row>
     <row r="17" spans="4:33" x14ac:dyDescent="0.2">
-      <c r="D17" s="395"/>
-      <c r="E17" s="395"/>
-      <c r="F17" s="395"/>
-      <c r="G17" s="395"/>
-      <c r="H17" s="395"/>
-      <c r="I17" s="395"/>
-      <c r="J17" s="395"/>
-      <c r="K17" s="395"/>
-      <c r="L17" s="395"/>
-      <c r="M17" s="395"/>
-      <c r="N17" s="395"/>
-      <c r="O17" s="395"/>
-      <c r="P17" s="395"/>
-      <c r="Q17" s="395"/>
-      <c r="R17" s="395"/>
-      <c r="S17" s="396"/>
-      <c r="T17" s="395"/>
-      <c r="U17" s="395"/>
-      <c r="V17" s="395"/>
-      <c r="W17" s="395"/>
-      <c r="X17" s="395"/>
-      <c r="Y17" s="395"/>
-      <c r="Z17" s="395"/>
-      <c r="AA17" s="395"/>
-      <c r="AB17" s="395"/>
-      <c r="AC17" s="395"/>
-      <c r="AD17" s="395"/>
-      <c r="AE17" s="395"/>
-      <c r="AF17" s="395"/>
-      <c r="AG17" s="395"/>
+      <c r="D17" s="347"/>
+      <c r="E17" s="347"/>
+      <c r="F17" s="347"/>
+      <c r="G17" s="347"/>
+      <c r="H17" s="347"/>
+      <c r="I17" s="347"/>
+      <c r="J17" s="347"/>
+      <c r="K17" s="347"/>
+      <c r="L17" s="347"/>
+      <c r="M17" s="347"/>
+      <c r="N17" s="347"/>
+      <c r="O17" s="347"/>
+      <c r="P17" s="347"/>
+      <c r="Q17" s="347"/>
+      <c r="R17" s="347"/>
+      <c r="S17" s="348"/>
+      <c r="T17" s="347"/>
+      <c r="U17" s="347"/>
+      <c r="V17" s="347"/>
+      <c r="W17" s="347"/>
+      <c r="X17" s="347"/>
+      <c r="Y17" s="347"/>
+      <c r="Z17" s="347"/>
+      <c r="AA17" s="347"/>
+      <c r="AB17" s="347"/>
+      <c r="AC17" s="347"/>
+      <c r="AD17" s="347"/>
+      <c r="AE17" s="347"/>
+      <c r="AF17" s="347"/>
+      <c r="AG17" s="347"/>
     </row>
     <row r="18" spans="4:33" ht="24" x14ac:dyDescent="0.2">
-      <c r="D18" s="401"/>
-      <c r="E18" s="402"/>
-      <c r="F18" s="398" t="s">
+      <c r="D18" s="353"/>
+      <c r="E18" s="354"/>
+      <c r="F18" s="350" t="s">
         <v>253</v>
       </c>
       <c r="G18" s="152" t="str">
         <f>IF(ISBLANK(ETPT_TPRX_DDG!$D$5),"",IF(ISERROR(ETPT_TPRX!G18),"",IF(ETPT_TPRX!G18=0,"",ETPT_TPRX!G18)))</f>
         <v/>
       </c>
-      <c r="H18" s="402"/>
-      <c r="I18" s="402"/>
-      <c r="J18" s="402"/>
-      <c r="K18" s="402"/>
-      <c r="L18" s="395"/>
-      <c r="M18" s="395"/>
-      <c r="N18" s="395"/>
-      <c r="O18" s="395"/>
-      <c r="P18" s="395"/>
-      <c r="Q18" s="399" t="s">
+      <c r="H18" s="354"/>
+      <c r="I18" s="354"/>
+      <c r="J18" s="354"/>
+      <c r="K18" s="354"/>
+      <c r="L18" s="347"/>
+      <c r="M18" s="347"/>
+      <c r="N18" s="347"/>
+      <c r="O18" s="347"/>
+      <c r="P18" s="347"/>
+      <c r="Q18" s="351" t="s">
         <v>254</v>
       </c>
       <c r="R18" s="152" t="str">
         <f>IF(ISBLANK(ETPT_TPRX_DDG!$D$5),"",IF(ISERROR(ETPT_TPRX!R18),"",IF(ETPT_TPRX!R18=0,"",ETPT_TPRX!R18)))</f>
         <v/>
       </c>
-      <c r="S18" s="395"/>
-      <c r="T18" s="395"/>
-      <c r="U18" s="395"/>
-      <c r="V18" s="395"/>
-      <c r="W18" s="395"/>
-      <c r="X18" s="395"/>
-      <c r="Y18" s="395"/>
-      <c r="Z18" s="395"/>
-      <c r="AA18" s="395"/>
-      <c r="AB18" s="395"/>
-      <c r="AC18" s="395"/>
-      <c r="AD18" s="402"/>
-      <c r="AE18" s="399" t="s">
+      <c r="S18" s="347"/>
+      <c r="T18" s="347"/>
+      <c r="U18" s="347"/>
+      <c r="V18" s="347"/>
+      <c r="W18" s="347"/>
+      <c r="X18" s="347"/>
+      <c r="Y18" s="347"/>
+      <c r="Z18" s="347"/>
+      <c r="AA18" s="347"/>
+      <c r="AB18" s="347"/>
+      <c r="AC18" s="347"/>
+      <c r="AD18" s="354"/>
+      <c r="AE18" s="351" t="s">
         <v>252</v>
       </c>
       <c r="AF18" s="152" t="str">
         <f>IF(ISBLANK(ETPT_TPRX_DDG!$D$5),"",IF(ISERROR(ETPT_TPRX!AF18),"",IF(ETPT_TPRX!AF18=0,"",ETPT_TPRX!AF18)))</f>
         <v/>
       </c>
-      <c r="AG18" s="395"/>
+      <c r="AG18" s="347"/>
     </row>
     <row r="20" spans="4:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E20" s="139" t="s">
@@ -22451,32 +22451,32 @@
       <c r="K20" s="140"/>
     </row>
     <row r="21" spans="4:33" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E21" s="380" t="s">
+      <c r="E21" s="396" t="s">
         <v>371</v>
       </c>
-      <c r="F21" s="381"/>
-      <c r="G21" s="381"/>
-      <c r="H21" s="381"/>
-      <c r="I21" s="381"/>
-      <c r="J21" s="381"/>
-      <c r="K21" s="381"/>
-      <c r="L21" s="381"/>
-      <c r="M21" s="381"/>
-      <c r="N21" s="381"/>
-      <c r="O21" s="381"/>
-      <c r="P21" s="381"/>
-      <c r="Q21" s="381"/>
-      <c r="R21" s="381"/>
-      <c r="S21" s="381"/>
-      <c r="T21" s="381"/>
-      <c r="U21" s="381"/>
-      <c r="V21" s="381"/>
-      <c r="W21" s="381"/>
-      <c r="X21" s="381"/>
-      <c r="Y21" s="381"/>
-      <c r="Z21" s="381"/>
-      <c r="AA21" s="381"/>
-      <c r="AB21" s="382"/>
+      <c r="F21" s="397"/>
+      <c r="G21" s="397"/>
+      <c r="H21" s="397"/>
+      <c r="I21" s="397"/>
+      <c r="J21" s="397"/>
+      <c r="K21" s="397"/>
+      <c r="L21" s="397"/>
+      <c r="M21" s="397"/>
+      <c r="N21" s="397"/>
+      <c r="O21" s="397"/>
+      <c r="P21" s="397"/>
+      <c r="Q21" s="397"/>
+      <c r="R21" s="397"/>
+      <c r="S21" s="397"/>
+      <c r="T21" s="397"/>
+      <c r="U21" s="397"/>
+      <c r="V21" s="397"/>
+      <c r="W21" s="397"/>
+      <c r="X21" s="397"/>
+      <c r="Y21" s="397"/>
+      <c r="Z21" s="397"/>
+      <c r="AA21" s="397"/>
+      <c r="AB21" s="398"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -22584,7 +22584,7 @@
       <c r="G2" s="75" t="s">
         <v>167</v>
       </c>
-      <c r="H2" s="373" t="s">
+      <c r="H2" s="389" t="s">
         <v>166</v>
       </c>
     </row>
@@ -22592,7 +22592,7 @@
       <c r="G3" s="75" t="s">
         <v>145</v>
       </c>
-      <c r="H3" s="373"/>
+      <c r="H3" s="389"/>
     </row>
     <row r="4" spans="1:62" ht="36" x14ac:dyDescent="0.2">
       <c r="A4" s="97"/>
@@ -22614,7 +22614,7 @@
       <c r="G4" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="H4" s="373"/>
+      <c r="H4" s="389"/>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A5" s="91" t="s">
@@ -22868,15 +22868,15 @@
       <c r="J16" s="21"/>
     </row>
     <row r="17" spans="4:10" ht="99" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D17" s="383" t="s">
+      <c r="D17" s="399" t="s">
         <v>372</v>
       </c>
-      <c r="E17" s="384"/>
-      <c r="F17" s="384"/>
-      <c r="G17" s="384"/>
-      <c r="H17" s="384"/>
-      <c r="I17" s="384"/>
-      <c r="J17" s="385"/>
+      <c r="E17" s="400"/>
+      <c r="F17" s="400"/>
+      <c r="G17" s="400"/>
+      <c r="H17" s="400"/>
+      <c r="I17" s="400"/>
+      <c r="J17" s="401"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -23010,7 +23010,7 @@
       <c r="P2" s="277" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="376" t="s">
+      <c r="Q2" s="392" t="s">
         <v>274</v>
       </c>
     </row>
@@ -23051,7 +23051,7 @@
       <c r="P3" s="277" t="s">
         <v>281</v>
       </c>
-      <c r="Q3" s="376"/>
+      <c r="Q3" s="392"/>
     </row>
     <row r="4" spans="1:62" ht="36" x14ac:dyDescent="0.2">
       <c r="A4" s="278"/>
@@ -23061,13 +23061,13 @@
       <c r="C4" s="279" t="s">
         <v>111</v>
       </c>
-      <c r="D4" s="403" t="s">
+      <c r="D4" s="355" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="403" t="s">
+      <c r="E4" s="355" t="s">
         <v>282</v>
       </c>
-      <c r="F4" s="403" t="s">
+      <c r="F4" s="355" t="s">
         <v>109</v>
       </c>
       <c r="G4" s="277" t="s">
@@ -23100,7 +23100,7 @@
       <c r="P4" s="277" t="s">
         <v>292</v>
       </c>
-      <c r="Q4" s="376"/>
+      <c r="Q4" s="392"/>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A5" s="281" t="s">
@@ -23112,43 +23112,43 @@
       <c r="E5" s="282" t="s">
         <v>62</v>
       </c>
-      <c r="F5" s="404" t="s">
+      <c r="F5" s="356" t="s">
         <v>61</v>
       </c>
-      <c r="G5" s="409"/>
-      <c r="H5" s="410" t="str">
+      <c r="G5" s="361"/>
+      <c r="H5" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!H5),"",IF(ISERROR(ETPT_JUR_ASS!H5),"",IF(ETPT_JUR_ASS!H5=0,"",ETPT_JUR_ASS!H5)))</f>
         <v/>
       </c>
-      <c r="I5" s="410" t="str">
+      <c r="I5" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!I5),"",IF(ISERROR(ETPT_JUR_ASS!I5),"",IF(ETPT_JUR_ASS!I5=0,"",ETPT_JUR_ASS!I5)))</f>
         <v/>
       </c>
-      <c r="J5" s="410" t="str">
+      <c r="J5" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!J5),"",IF(ISERROR(ETPT_JUR_ASS!J5),"",IF(ETPT_JUR_ASS!J5=0,"",ETPT_JUR_ASS!J5)))</f>
         <v/>
       </c>
-      <c r="K5" s="410" t="str">
+      <c r="K5" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!K5),"",IF(ISERROR(ETPT_JUR_ASS!K5),"",IF(ETPT_JUR_ASS!K5=0,"",ETPT_JUR_ASS!K5)))</f>
         <v/>
       </c>
-      <c r="L5" s="410" t="str">
+      <c r="L5" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!L5),"",IF(ISERROR(ETPT_JUR_ASS!L5),"",IF(ETPT_JUR_ASS!L5=0,"",ETPT_JUR_ASS!L5)))</f>
         <v/>
       </c>
-      <c r="M5" s="410" t="str">
+      <c r="M5" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!M5),"",IF(ISERROR(ETPT_JUR_ASS!M5),"",IF(ETPT_JUR_ASS!M5=0,"",ETPT_JUR_ASS!M5)))</f>
         <v/>
       </c>
-      <c r="N5" s="410" t="str">
+      <c r="N5" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!N5),"",IF(ISERROR(ETPT_JUR_ASS!N5),"",IF(ETPT_JUR_ASS!N5=0,"",ETPT_JUR_ASS!N5)))</f>
         <v/>
       </c>
-      <c r="O5" s="410" t="str">
+      <c r="O5" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!O5),"",IF(ISERROR(ETPT_JUR_ASS!O5),"",IF(ETPT_JUR_ASS!O5=0,"",ETPT_JUR_ASS!O5)))</f>
         <v/>
       </c>
-      <c r="P5" s="410" t="str">
+      <c r="P5" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!P5),"",IF(ISERROR(ETPT_JUR_ASS!P5),"",IF(ETPT_JUR_ASS!P5=0,"",ETPT_JUR_ASS!P5)))</f>
         <v/>
       </c>
@@ -23170,43 +23170,43 @@
       <c r="E6" s="282" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="404" t="s">
+      <c r="F6" s="356" t="s">
         <v>59</v>
       </c>
-      <c r="G6" s="408"/>
-      <c r="H6" s="410" t="str">
+      <c r="G6" s="360"/>
+      <c r="H6" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!H6),"",IF(ISERROR(ETPT_JUR_ASS!H6),"",IF(ETPT_JUR_ASS!H6=0,"",ETPT_JUR_ASS!H6)))</f>
         <v/>
       </c>
-      <c r="I6" s="410" t="str">
+      <c r="I6" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!I6),"",IF(ISERROR(ETPT_JUR_ASS!I6),"",IF(ETPT_JUR_ASS!I6=0,"",ETPT_JUR_ASS!I6)))</f>
         <v/>
       </c>
-      <c r="J6" s="410" t="str">
+      <c r="J6" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!J6),"",IF(ISERROR(ETPT_JUR_ASS!J6),"",IF(ETPT_JUR_ASS!J6=0,"",ETPT_JUR_ASS!J6)))</f>
         <v/>
       </c>
-      <c r="K6" s="410" t="str">
+      <c r="K6" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!K6),"",IF(ISERROR(ETPT_JUR_ASS!K6),"",IF(ETPT_JUR_ASS!K6=0,"",ETPT_JUR_ASS!K6)))</f>
         <v/>
       </c>
-      <c r="L6" s="410" t="str">
+      <c r="L6" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!L6),"",IF(ISERROR(ETPT_JUR_ASS!L6),"",IF(ETPT_JUR_ASS!L6=0,"",ETPT_JUR_ASS!L6)))</f>
         <v/>
       </c>
-      <c r="M6" s="410" t="str">
+      <c r="M6" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!M6),"",IF(ISERROR(ETPT_JUR_ASS!M6),"",IF(ETPT_JUR_ASS!M6=0,"",ETPT_JUR_ASS!M6)))</f>
         <v/>
       </c>
-      <c r="N6" s="410" t="str">
+      <c r="N6" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!N6),"",IF(ISERROR(ETPT_JUR_ASS!N6),"",IF(ETPT_JUR_ASS!N6=0,"",ETPT_JUR_ASS!N6)))</f>
         <v/>
       </c>
-      <c r="O6" s="410" t="str">
+      <c r="O6" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!O6),"",IF(ISERROR(ETPT_JUR_ASS!O6),"",IF(ETPT_JUR_ASS!O6=0,"",ETPT_JUR_ASS!O6)))</f>
         <v/>
       </c>
-      <c r="P6" s="410" t="str">
+      <c r="P6" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!P6),"",IF(ISERROR(ETPT_JUR_ASS!P6),"",IF(ETPT_JUR_ASS!P6=0,"",ETPT_JUR_ASS!P6)))</f>
         <v/>
       </c>
@@ -23228,43 +23228,43 @@
       <c r="E7" s="282" t="s">
         <v>56</v>
       </c>
-      <c r="F7" s="404" t="s">
+      <c r="F7" s="356" t="s">
         <v>55</v>
       </c>
-      <c r="G7" s="408"/>
-      <c r="H7" s="410" t="str">
+      <c r="G7" s="360"/>
+      <c r="H7" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!H7),"",IF(ISERROR(ETPT_JUR_ASS!H7),"",IF(ETPT_JUR_ASS!H7=0,"",ETPT_JUR_ASS!H7)))</f>
         <v/>
       </c>
-      <c r="I7" s="410" t="str">
+      <c r="I7" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!I7),"",IF(ISERROR(ETPT_JUR_ASS!I7),"",IF(ETPT_JUR_ASS!I7=0,"",ETPT_JUR_ASS!I7)))</f>
         <v/>
       </c>
-      <c r="J7" s="410" t="str">
+      <c r="J7" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!J7),"",IF(ISERROR(ETPT_JUR_ASS!J7),"",IF(ETPT_JUR_ASS!J7=0,"",ETPT_JUR_ASS!J7)))</f>
         <v/>
       </c>
-      <c r="K7" s="410" t="str">
+      <c r="K7" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!K7),"",IF(ISERROR(ETPT_JUR_ASS!K7),"",IF(ETPT_JUR_ASS!K7=0,"",ETPT_JUR_ASS!K7)))</f>
         <v/>
       </c>
-      <c r="L7" s="410" t="str">
+      <c r="L7" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!L7),"",IF(ISERROR(ETPT_JUR_ASS!L7),"",IF(ETPT_JUR_ASS!L7=0,"",ETPT_JUR_ASS!L7)))</f>
         <v/>
       </c>
-      <c r="M7" s="410" t="str">
+      <c r="M7" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!M7),"",IF(ISERROR(ETPT_JUR_ASS!M7),"",IF(ETPT_JUR_ASS!M7=0,"",ETPT_JUR_ASS!M7)))</f>
         <v/>
       </c>
-      <c r="N7" s="410" t="str">
+      <c r="N7" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!N7),"",IF(ISERROR(ETPT_JUR_ASS!N7),"",IF(ETPT_JUR_ASS!N7=0,"",ETPT_JUR_ASS!N7)))</f>
         <v/>
       </c>
-      <c r="O7" s="410" t="str">
+      <c r="O7" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!O7),"",IF(ISERROR(ETPT_JUR_ASS!O7),"",IF(ETPT_JUR_ASS!O7=0,"",ETPT_JUR_ASS!O7)))</f>
         <v/>
       </c>
-      <c r="P7" s="410" t="str">
+      <c r="P7" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!P7),"",IF(ISERROR(ETPT_JUR_ASS!P7),"",IF(ETPT_JUR_ASS!P7=0,"",ETPT_JUR_ASS!P7)))</f>
         <v/>
       </c>
@@ -23286,43 +23286,43 @@
       <c r="E8" s="282" t="s">
         <v>54</v>
       </c>
-      <c r="F8" s="404" t="s">
+      <c r="F8" s="356" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="408"/>
-      <c r="H8" s="410" t="str">
+      <c r="G8" s="360"/>
+      <c r="H8" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!H8),"",IF(ISERROR(ETPT_JUR_ASS!H8),"",IF(ETPT_JUR_ASS!H8=0,"",ETPT_JUR_ASS!H8)))</f>
         <v/>
       </c>
-      <c r="I8" s="410" t="str">
+      <c r="I8" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!I8),"",IF(ISERROR(ETPT_JUR_ASS!I8),"",IF(ETPT_JUR_ASS!I8=0,"",ETPT_JUR_ASS!I8)))</f>
         <v/>
       </c>
-      <c r="J8" s="410" t="str">
+      <c r="J8" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!J8),"",IF(ISERROR(ETPT_JUR_ASS!J8),"",IF(ETPT_JUR_ASS!J8=0,"",ETPT_JUR_ASS!J8)))</f>
         <v/>
       </c>
-      <c r="K8" s="410" t="str">
+      <c r="K8" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!K8),"",IF(ISERROR(ETPT_JUR_ASS!K8),"",IF(ETPT_JUR_ASS!K8=0,"",ETPT_JUR_ASS!K8)))</f>
         <v/>
       </c>
-      <c r="L8" s="410" t="str">
+      <c r="L8" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!L8),"",IF(ISERROR(ETPT_JUR_ASS!L8),"",IF(ETPT_JUR_ASS!L8=0,"",ETPT_JUR_ASS!L8)))</f>
         <v/>
       </c>
-      <c r="M8" s="410" t="str">
+      <c r="M8" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!M8),"",IF(ISERROR(ETPT_JUR_ASS!M8),"",IF(ETPT_JUR_ASS!M8=0,"",ETPT_JUR_ASS!M8)))</f>
         <v/>
       </c>
-      <c r="N8" s="410" t="str">
+      <c r="N8" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!N8),"",IF(ISERROR(ETPT_JUR_ASS!N8),"",IF(ETPT_JUR_ASS!N8=0,"",ETPT_JUR_ASS!N8)))</f>
         <v/>
       </c>
-      <c r="O8" s="410" t="str">
+      <c r="O8" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!O8),"",IF(ISERROR(ETPT_JUR_ASS!O8),"",IF(ETPT_JUR_ASS!O8=0,"",ETPT_JUR_ASS!O8)))</f>
         <v/>
       </c>
-      <c r="P8" s="410" t="str">
+      <c r="P8" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!P8),"",IF(ISERROR(ETPT_JUR_ASS!P8),"",IF(ETPT_JUR_ASS!P8=0,"",ETPT_JUR_ASS!P8)))</f>
         <v/>
       </c>
@@ -23344,43 +23344,43 @@
       <c r="E9" s="282" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="404" t="s">
+      <c r="F9" s="356" t="s">
         <v>51</v>
       </c>
-      <c r="G9" s="408"/>
-      <c r="H9" s="410" t="str">
+      <c r="G9" s="360"/>
+      <c r="H9" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!H9),"",IF(ISERROR(ETPT_JUR_ASS!H9),"",IF(ETPT_JUR_ASS!H9=0,"",ETPT_JUR_ASS!H9)))</f>
         <v/>
       </c>
-      <c r="I9" s="410" t="str">
+      <c r="I9" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!I9),"",IF(ISERROR(ETPT_JUR_ASS!I9),"",IF(ETPT_JUR_ASS!I9=0,"",ETPT_JUR_ASS!I9)))</f>
         <v/>
       </c>
-      <c r="J9" s="410" t="str">
+      <c r="J9" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!J9),"",IF(ISERROR(ETPT_JUR_ASS!J9),"",IF(ETPT_JUR_ASS!J9=0,"",ETPT_JUR_ASS!J9)))</f>
         <v/>
       </c>
-      <c r="K9" s="410" t="str">
+      <c r="K9" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!K9),"",IF(ISERROR(ETPT_JUR_ASS!K9),"",IF(ETPT_JUR_ASS!K9=0,"",ETPT_JUR_ASS!K9)))</f>
         <v/>
       </c>
-      <c r="L9" s="410" t="str">
+      <c r="L9" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!L9),"",IF(ISERROR(ETPT_JUR_ASS!L9),"",IF(ETPT_JUR_ASS!L9=0,"",ETPT_JUR_ASS!L9)))</f>
         <v/>
       </c>
-      <c r="M9" s="410" t="str">
+      <c r="M9" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!M9),"",IF(ISERROR(ETPT_JUR_ASS!M9),"",IF(ETPT_JUR_ASS!M9=0,"",ETPT_JUR_ASS!M9)))</f>
         <v/>
       </c>
-      <c r="N9" s="410" t="str">
+      <c r="N9" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!N9),"",IF(ISERROR(ETPT_JUR_ASS!N9),"",IF(ETPT_JUR_ASS!N9=0,"",ETPT_JUR_ASS!N9)))</f>
         <v/>
       </c>
-      <c r="O9" s="410" t="str">
+      <c r="O9" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!O9),"",IF(ISERROR(ETPT_JUR_ASS!O9),"",IF(ETPT_JUR_ASS!O9=0,"",ETPT_JUR_ASS!O9)))</f>
         <v/>
       </c>
-      <c r="P9" s="410" t="str">
+      <c r="P9" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!P9),"",IF(ISERROR(ETPT_JUR_ASS!P9),"",IF(ETPT_JUR_ASS!P9=0,"",ETPT_JUR_ASS!P9)))</f>
         <v/>
       </c>
@@ -23402,43 +23402,43 @@
       <c r="E10" s="282" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="404" t="s">
+      <c r="F10" s="356" t="s">
         <v>49</v>
       </c>
-      <c r="G10" s="408"/>
-      <c r="H10" s="410" t="str">
+      <c r="G10" s="360"/>
+      <c r="H10" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!H10),"",IF(ISERROR(ETPT_JUR_ASS!H10),"",IF(ETPT_JUR_ASS!H10=0,"",ETPT_JUR_ASS!H10)))</f>
         <v/>
       </c>
-      <c r="I10" s="410" t="str">
+      <c r="I10" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!I10),"",IF(ISERROR(ETPT_JUR_ASS!I10),"",IF(ETPT_JUR_ASS!I10=0,"",ETPT_JUR_ASS!I10)))</f>
         <v/>
       </c>
-      <c r="J10" s="410" t="str">
+      <c r="J10" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!J10),"",IF(ISERROR(ETPT_JUR_ASS!J10),"",IF(ETPT_JUR_ASS!J10=0,"",ETPT_JUR_ASS!J10)))</f>
         <v/>
       </c>
-      <c r="K10" s="410" t="str">
+      <c r="K10" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!K10),"",IF(ISERROR(ETPT_JUR_ASS!K10),"",IF(ETPT_JUR_ASS!K10=0,"",ETPT_JUR_ASS!K10)))</f>
         <v/>
       </c>
-      <c r="L10" s="410" t="str">
+      <c r="L10" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!L10),"",IF(ISERROR(ETPT_JUR_ASS!L10),"",IF(ETPT_JUR_ASS!L10=0,"",ETPT_JUR_ASS!L10)))</f>
         <v/>
       </c>
-      <c r="M10" s="410" t="str">
+      <c r="M10" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!M10),"",IF(ISERROR(ETPT_JUR_ASS!M10),"",IF(ETPT_JUR_ASS!M10=0,"",ETPT_JUR_ASS!M10)))</f>
         <v/>
       </c>
-      <c r="N10" s="410" t="str">
+      <c r="N10" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!N10),"",IF(ISERROR(ETPT_JUR_ASS!N10),"",IF(ETPT_JUR_ASS!N10=0,"",ETPT_JUR_ASS!N10)))</f>
         <v/>
       </c>
-      <c r="O10" s="410" t="str">
+      <c r="O10" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!O10),"",IF(ISERROR(ETPT_JUR_ASS!O10),"",IF(ETPT_JUR_ASS!O10=0,"",ETPT_JUR_ASS!O10)))</f>
         <v/>
       </c>
-      <c r="P10" s="410" t="str">
+      <c r="P10" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!P10),"",IF(ISERROR(ETPT_JUR_ASS!P10),"",IF(ETPT_JUR_ASS!P10=0,"",ETPT_JUR_ASS!P10)))</f>
         <v/>
       </c>
@@ -23460,43 +23460,43 @@
       <c r="E11" s="282" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="404" t="s">
+      <c r="F11" s="356" t="s">
         <v>47</v>
       </c>
-      <c r="G11" s="408"/>
-      <c r="H11" s="410" t="str">
+      <c r="G11" s="360"/>
+      <c r="H11" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!H11),"",IF(ISERROR(ETPT_JUR_ASS!H11),"",IF(ETPT_JUR_ASS!H11=0,"",ETPT_JUR_ASS!H11)))</f>
         <v/>
       </c>
-      <c r="I11" s="410" t="str">
+      <c r="I11" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!I11),"",IF(ISERROR(ETPT_JUR_ASS!I11),"",IF(ETPT_JUR_ASS!I11=0,"",ETPT_JUR_ASS!I11)))</f>
         <v/>
       </c>
-      <c r="J11" s="410" t="str">
+      <c r="J11" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!J11),"",IF(ISERROR(ETPT_JUR_ASS!J11),"",IF(ETPT_JUR_ASS!J11=0,"",ETPT_JUR_ASS!J11)))</f>
         <v/>
       </c>
-      <c r="K11" s="410" t="str">
+      <c r="K11" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!K11),"",IF(ISERROR(ETPT_JUR_ASS!K11),"",IF(ETPT_JUR_ASS!K11=0,"",ETPT_JUR_ASS!K11)))</f>
         <v/>
       </c>
-      <c r="L11" s="410" t="str">
+      <c r="L11" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!L11),"",IF(ISERROR(ETPT_JUR_ASS!L11),"",IF(ETPT_JUR_ASS!L11=0,"",ETPT_JUR_ASS!L11)))</f>
         <v/>
       </c>
-      <c r="M11" s="410" t="str">
+      <c r="M11" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!M11),"",IF(ISERROR(ETPT_JUR_ASS!M11),"",IF(ETPT_JUR_ASS!M11=0,"",ETPT_JUR_ASS!M11)))</f>
         <v/>
       </c>
-      <c r="N11" s="410" t="str">
+      <c r="N11" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!N11),"",IF(ISERROR(ETPT_JUR_ASS!N11),"",IF(ETPT_JUR_ASS!N11=0,"",ETPT_JUR_ASS!N11)))</f>
         <v/>
       </c>
-      <c r="O11" s="410" t="str">
+      <c r="O11" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!O11),"",IF(ISERROR(ETPT_JUR_ASS!O11),"",IF(ETPT_JUR_ASS!O11=0,"",ETPT_JUR_ASS!O11)))</f>
         <v/>
       </c>
-      <c r="P11" s="410" t="str">
+      <c r="P11" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!P11),"",IF(ISERROR(ETPT_JUR_ASS!P11),"",IF(ETPT_JUR_ASS!P11=0,"",ETPT_JUR_ASS!P11)))</f>
         <v/>
       </c>
@@ -23518,43 +23518,43 @@
       <c r="E12" s="282" t="s">
         <v>46</v>
       </c>
-      <c r="F12" s="404" t="s">
+      <c r="F12" s="356" t="s">
         <v>45</v>
       </c>
-      <c r="G12" s="408"/>
-      <c r="H12" s="410" t="str">
+      <c r="G12" s="360"/>
+      <c r="H12" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!H12),"",IF(ISERROR(ETPT_JUR_ASS!H12),"",IF(ETPT_JUR_ASS!H12=0,"",ETPT_JUR_ASS!H12)))</f>
         <v/>
       </c>
-      <c r="I12" s="410" t="str">
+      <c r="I12" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!I12),"",IF(ISERROR(ETPT_JUR_ASS!I12),"",IF(ETPT_JUR_ASS!I12=0,"",ETPT_JUR_ASS!I12)))</f>
         <v/>
       </c>
-      <c r="J12" s="410" t="str">
+      <c r="J12" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!J12),"",IF(ISERROR(ETPT_JUR_ASS!J12),"",IF(ETPT_JUR_ASS!J12=0,"",ETPT_JUR_ASS!J12)))</f>
         <v/>
       </c>
-      <c r="K12" s="410" t="str">
+      <c r="K12" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!K12),"",IF(ISERROR(ETPT_JUR_ASS!K12),"",IF(ETPT_JUR_ASS!K12=0,"",ETPT_JUR_ASS!K12)))</f>
         <v/>
       </c>
-      <c r="L12" s="410" t="str">
+      <c r="L12" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!L12),"",IF(ISERROR(ETPT_JUR_ASS!L12),"",IF(ETPT_JUR_ASS!L12=0,"",ETPT_JUR_ASS!L12)))</f>
         <v/>
       </c>
-      <c r="M12" s="410" t="str">
+      <c r="M12" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!M12),"",IF(ISERROR(ETPT_JUR_ASS!M12),"",IF(ETPT_JUR_ASS!M12=0,"",ETPT_JUR_ASS!M12)))</f>
         <v/>
       </c>
-      <c r="N12" s="410" t="str">
+      <c r="N12" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!N12),"",IF(ISERROR(ETPT_JUR_ASS!N12),"",IF(ETPT_JUR_ASS!N12=0,"",ETPT_JUR_ASS!N12)))</f>
         <v/>
       </c>
-      <c r="O12" s="410" t="str">
+      <c r="O12" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!O12),"",IF(ISERROR(ETPT_JUR_ASS!O12),"",IF(ETPT_JUR_ASS!O12=0,"",ETPT_JUR_ASS!O12)))</f>
         <v/>
       </c>
-      <c r="P12" s="410" t="str">
+      <c r="P12" s="362" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!P12),"",IF(ISERROR(ETPT_JUR_ASS!P12),"",IF(ETPT_JUR_ASS!P12=0,"",ETPT_JUR_ASS!P12)))</f>
         <v/>
       </c>
@@ -23567,9 +23567,9 @@
       <c r="A13" s="291"/>
       <c r="B13" s="291"/>
       <c r="C13" s="291"/>
-      <c r="D13" s="405"/>
-      <c r="E13" s="406"/>
-      <c r="F13" s="407" t="s">
+      <c r="D13" s="357"/>
+      <c r="E13" s="358"/>
+      <c r="F13" s="359" t="s">
         <v>39</v>
       </c>
       <c r="G13" s="287">
@@ -23963,13 +23963,13 @@
   <sheetData>
     <row r="1" spans="1:61" s="142" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="141"/>
-      <c r="B1" s="387" t="s">
+      <c r="B1" s="403" t="s">
         <v>170</v>
       </c>
-      <c r="C1" s="387"/>
-      <c r="D1" s="387"/>
-      <c r="E1" s="387"/>
-      <c r="F1" s="387"/>
+      <c r="C1" s="403"/>
+      <c r="D1" s="403"/>
+      <c r="E1" s="403"/>
+      <c r="F1" s="403"/>
       <c r="G1" s="143"/>
       <c r="H1" s="143"/>
       <c r="I1" s="143"/>
@@ -24014,7 +24014,7 @@
       <c r="O2" s="145" t="s">
         <v>164</v>
       </c>
-      <c r="P2" s="386" t="s">
+      <c r="P2" s="402" t="s">
         <v>163</v>
       </c>
       <c r="Q2" s="145" t="s">
@@ -24056,7 +24056,7 @@
       <c r="AC2" s="145" t="s">
         <v>162</v>
       </c>
-      <c r="AD2" s="386" t="s">
+      <c r="AD2" s="402" t="s">
         <v>161</v>
       </c>
       <c r="AE2" s="146" t="s">
@@ -24086,7 +24086,7 @@
       <c r="AM2" s="146" t="s">
         <v>160</v>
       </c>
-      <c r="AN2" s="386" t="s">
+      <c r="AN2" s="402" t="s">
         <v>159</v>
       </c>
       <c r="AZ2" s="146"/>
@@ -24098,7 +24098,7 @@
       <c r="BF2" s="146"/>
       <c r="BG2" s="146"/>
       <c r="BH2" s="146"/>
-      <c r="BI2" s="386"/>
+      <c r="BI2" s="402"/>
     </row>
     <row r="3" spans="1:61" s="142" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="144"/>
@@ -24134,7 +24134,7 @@
       <c r="O3" s="145" t="s">
         <v>135</v>
       </c>
-      <c r="P3" s="386"/>
+      <c r="P3" s="402"/>
       <c r="Q3" s="145" t="s">
         <v>134</v>
       </c>
@@ -24174,7 +24174,7 @@
       <c r="AC3" s="145" t="s">
         <v>122</v>
       </c>
-      <c r="AD3" s="386"/>
+      <c r="AD3" s="402"/>
       <c r="AE3" s="146" t="s">
         <v>121</v>
       </c>
@@ -24202,7 +24202,7 @@
       <c r="AM3" s="146" t="s">
         <v>113</v>
       </c>
-      <c r="AN3" s="386"/>
+      <c r="AN3" s="402"/>
       <c r="AZ3" s="146"/>
       <c r="BA3" s="146"/>
       <c r="BB3" s="146"/>
@@ -24212,7 +24212,7 @@
       <c r="BF3" s="146"/>
       <c r="BG3" s="146"/>
       <c r="BH3" s="146"/>
-      <c r="BI3" s="386"/>
+      <c r="BI3" s="402"/>
     </row>
     <row r="4" spans="1:61" s="142" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="147"/>
@@ -24258,7 +24258,7 @@
       <c r="O4" s="145" t="s">
         <v>85</v>
       </c>
-      <c r="P4" s="386"/>
+      <c r="P4" s="402"/>
       <c r="Q4" s="145" t="s">
         <v>84</v>
       </c>
@@ -24298,7 +24298,7 @@
       <c r="AC4" s="145" t="s">
         <v>72</v>
       </c>
-      <c r="AD4" s="386"/>
+      <c r="AD4" s="402"/>
       <c r="AE4" s="146" t="s">
         <v>71</v>
       </c>
@@ -24326,7 +24326,7 @@
       <c r="AM4" s="146" t="s">
         <v>63</v>
       </c>
-      <c r="AN4" s="386"/>
+      <c r="AN4" s="402"/>
       <c r="AZ4" s="146"/>
       <c r="BA4" s="146"/>
       <c r="BB4" s="146"/>
@@ -24336,7 +24336,7 @@
       <c r="BF4" s="146"/>
       <c r="BG4" s="146"/>
       <c r="BH4" s="146"/>
-      <c r="BI4" s="386"/>
+      <c r="BI4" s="402"/>
     </row>
     <row r="5" spans="1:61" s="142" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="149" t="s">
@@ -25977,14 +25977,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="388" t="s">
+      <c r="A1" s="404" t="s">
         <v>214</v>
       </c>
-      <c r="B1" s="388"/>
-      <c r="C1" s="388"/>
-      <c r="D1" s="388"/>
-      <c r="E1" s="388"/>
-      <c r="F1" s="388"/>
+      <c r="B1" s="404"/>
+      <c r="C1" s="404"/>
+      <c r="D1" s="404"/>
+      <c r="E1" s="404"/>
+      <c r="F1" s="404"/>
       <c r="G1" s="319"/>
       <c r="H1" s="319"/>
       <c r="I1" s="319"/>
@@ -26034,7 +26034,7 @@
       <c r="O2" s="173" t="s">
         <v>164</v>
       </c>
-      <c r="P2" s="389" t="s">
+      <c r="P2" s="405" t="s">
         <v>213</v>
       </c>
       <c r="Q2" s="173" t="s">
@@ -26046,7 +26046,7 @@
       <c r="S2" s="173" t="s">
         <v>212</v>
       </c>
-      <c r="T2" s="389" t="s">
+      <c r="T2" s="405" t="s">
         <v>211</v>
       </c>
     </row>
@@ -26084,7 +26084,7 @@
       <c r="O3" s="173" t="s">
         <v>193</v>
       </c>
-      <c r="P3" s="389"/>
+      <c r="P3" s="405"/>
       <c r="Q3" s="173" t="s">
         <v>192</v>
       </c>
@@ -26094,7 +26094,7 @@
       <c r="S3" s="173" t="s">
         <v>122</v>
       </c>
-      <c r="T3" s="389"/>
+      <c r="T3" s="405"/>
     </row>
     <row r="4" spans="1:20" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="172"/>
@@ -26140,7 +26140,7 @@
       <c r="O4" s="173" t="s">
         <v>174</v>
       </c>
-      <c r="P4" s="389"/>
+      <c r="P4" s="405"/>
       <c r="Q4" s="173" t="s">
         <v>173</v>
       </c>
@@ -26150,7 +26150,7 @@
       <c r="S4" s="173" t="s">
         <v>72</v>
       </c>
-      <c r="T4" s="389"/>
+      <c r="T4" s="405"/>
     </row>
     <row r="5" spans="1:20" ht="204" x14ac:dyDescent="0.2">
       <c r="A5" s="321" t="s">
@@ -26749,16 +26749,16 @@
   <sheetData>
     <row r="1" spans="1:23" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="181"/>
-      <c r="B1" s="390" t="s">
+      <c r="B1" s="406" t="s">
         <v>170</v>
       </c>
-      <c r="C1" s="390"/>
-      <c r="D1" s="390"/>
-      <c r="E1" s="390"/>
-      <c r="F1" s="390"/>
-      <c r="G1" s="390"/>
-      <c r="H1" s="390"/>
-      <c r="I1" s="390"/>
+      <c r="C1" s="406"/>
+      <c r="D1" s="406"/>
+      <c r="E1" s="406"/>
+      <c r="F1" s="406"/>
+      <c r="G1" s="406"/>
+      <c r="H1" s="406"/>
+      <c r="I1" s="406"/>
       <c r="J1" s="178"/>
       <c r="K1" s="178"/>
       <c r="L1" s="178"/>
@@ -26784,7 +26784,7 @@
       <c r="G2" s="180" t="s">
         <v>169</v>
       </c>
-      <c r="H2" s="391" t="s">
+      <c r="H2" s="407" t="s">
         <v>168</v>
       </c>
       <c r="I2" s="182" t="s">
@@ -26829,7 +26829,7 @@
       <c r="V2" s="182" t="s">
         <v>167</v>
       </c>
-      <c r="W2" s="391" t="s">
+      <c r="W2" s="407" t="s">
         <v>166</v>
       </c>
     </row>
@@ -26843,7 +26843,7 @@
       <c r="G3" s="180" t="s">
         <v>158</v>
       </c>
-      <c r="H3" s="391"/>
+      <c r="H3" s="407"/>
       <c r="I3" s="182" t="s">
         <v>157</v>
       </c>
@@ -26884,7 +26884,7 @@
       <c r="V3" s="182" t="s">
         <v>145</v>
       </c>
-      <c r="W3" s="391"/>
+      <c r="W3" s="407"/>
     </row>
     <row r="4" spans="1:23" ht="98" x14ac:dyDescent="0.2">
       <c r="A4" s="183"/>
@@ -26906,7 +26906,7 @@
       <c r="G4" s="180" t="s">
         <v>108</v>
       </c>
-      <c r="H4" s="391"/>
+      <c r="H4" s="407"/>
       <c r="I4" s="182" t="s">
         <v>107</v>
       </c>
@@ -26949,7 +26949,7 @@
       <c r="V4" s="185" t="s">
         <v>94</v>
       </c>
-      <c r="W4" s="391"/>
+      <c r="W4" s="407"/>
     </row>
     <row r="5" spans="1:23" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A5" s="186" t="s">
@@ -27660,16 +27660,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="393" t="s">
+      <c r="A1" s="409" t="s">
         <v>214</v>
       </c>
-      <c r="B1" s="393"/>
-      <c r="C1" s="393"/>
-      <c r="D1" s="393"/>
-      <c r="E1" s="393"/>
-      <c r="F1" s="393"/>
-      <c r="G1" s="393"/>
-      <c r="H1" s="393"/>
+      <c r="B1" s="409"/>
+      <c r="C1" s="409"/>
+      <c r="D1" s="409"/>
+      <c r="E1" s="409"/>
+      <c r="F1" s="409"/>
+      <c r="G1" s="409"/>
+      <c r="H1" s="409"/>
       <c r="I1" s="220"/>
       <c r="J1" s="220"/>
       <c r="K1" s="220"/>
@@ -27694,7 +27694,7 @@
       <c r="G2" s="222" t="s">
         <v>169</v>
       </c>
-      <c r="H2" s="392" t="s">
+      <c r="H2" s="408" t="s">
         <v>168</v>
       </c>
       <c r="I2" s="222" t="s">
@@ -27727,7 +27727,7 @@
       <c r="R2" s="222" t="s">
         <v>167</v>
       </c>
-      <c r="S2" s="392" t="s">
+      <c r="S2" s="408" t="s">
         <v>166</v>
       </c>
     </row>
@@ -27741,7 +27741,7 @@
       <c r="G3" s="222" t="s">
         <v>158</v>
       </c>
-      <c r="H3" s="392"/>
+      <c r="H3" s="408"/>
       <c r="I3" s="222" t="s">
         <v>210</v>
       </c>
@@ -27772,7 +27772,7 @@
       <c r="R3" s="222" t="s">
         <v>145</v>
       </c>
-      <c r="S3" s="392"/>
+      <c r="S3" s="408"/>
     </row>
     <row r="4" spans="1:21" ht="112" x14ac:dyDescent="0.2">
       <c r="A4" s="219"/>
@@ -27794,7 +27794,7 @@
       <c r="G4" s="222" t="s">
         <v>108</v>
       </c>
-      <c r="H4" s="392"/>
+      <c r="H4" s="408"/>
       <c r="I4" s="222" t="s">
         <v>191</v>
       </c>
@@ -27825,7 +27825,7 @@
       <c r="R4" s="222" t="s">
         <v>94</v>
       </c>
-      <c r="S4" s="392"/>
+      <c r="S4" s="408"/>
     </row>
     <row r="5" spans="1:21" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A5" s="225" t="s">
@@ -28461,13 +28461,13 @@
       <c r="K2" s="173" t="s">
         <v>167</v>
       </c>
-      <c r="L2" s="389" t="s">
+      <c r="L2" s="405" t="s">
         <v>166</v>
       </c>
       <c r="M2" s="173" t="s">
         <v>38</v>
       </c>
-      <c r="N2" s="389" t="s">
+      <c r="N2" s="405" t="s">
         <v>165</v>
       </c>
     </row>
@@ -28485,11 +28485,11 @@
       <c r="K3" s="173" t="s">
         <v>145</v>
       </c>
-      <c r="L3" s="389"/>
+      <c r="L3" s="405"/>
       <c r="M3" s="173" t="s">
         <v>142</v>
       </c>
-      <c r="N3" s="389"/>
+      <c r="N3" s="405"/>
     </row>
     <row r="4" spans="1:14" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="204"/>
@@ -28515,11 +28515,11 @@
       <c r="K4" s="173" t="s">
         <v>94</v>
       </c>
-      <c r="L4" s="389"/>
+      <c r="L4" s="405"/>
       <c r="M4" s="173" t="s">
         <v>93</v>
       </c>
-      <c r="N4" s="389"/>
+      <c r="N4" s="405"/>
     </row>
     <row r="5" spans="1:14" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="206"/>
@@ -29192,12 +29192,12 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="294"/>
-      <c r="B1" s="394" t="s">
+      <c r="B1" s="410" t="s">
         <v>295</v>
       </c>
-      <c r="C1" s="394"/>
-      <c r="D1" s="394"/>
-      <c r="E1" s="394"/>
+      <c r="C1" s="410"/>
+      <c r="D1" s="410"/>
+      <c r="E1" s="410"/>
       <c r="F1" s="295"/>
       <c r="G1" s="294"/>
       <c r="H1" s="294"/>
@@ -29248,7 +29248,7 @@
       <c r="P2" s="277" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="376" t="s">
+      <c r="Q2" s="392" t="s">
         <v>274</v>
       </c>
     </row>
@@ -29289,7 +29289,7 @@
       <c r="P3" s="277" t="s">
         <v>281</v>
       </c>
-      <c r="Q3" s="376"/>
+      <c r="Q3" s="392"/>
     </row>
     <row r="4" spans="1:17" ht="70" x14ac:dyDescent="0.2">
       <c r="A4" s="278"/>
@@ -29338,7 +29338,7 @@
       <c r="P4" s="280" t="s">
         <v>292</v>
       </c>
-      <c r="Q4" s="376"/>
+      <c r="Q4" s="392"/>
     </row>
     <row r="5" spans="1:17" ht="398" x14ac:dyDescent="0.2">
       <c r="A5" s="281" t="s">
@@ -29801,22 +29801,22 @@
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="364" t="s">
+      <c r="D1" s="380" t="s">
         <v>368</v>
       </c>
-      <c r="E1" s="365"/>
-      <c r="F1" s="365"/>
-      <c r="G1" s="365"/>
-      <c r="H1" s="365"/>
-      <c r="I1" s="365"/>
-      <c r="J1" s="366"/>
-      <c r="K1" s="366"/>
-      <c r="L1" s="366"/>
-      <c r="M1" s="366"/>
-      <c r="N1" s="366"/>
-      <c r="O1" s="366"/>
-      <c r="P1" s="366"/>
-      <c r="Q1" s="366"/>
+      <c r="E1" s="381"/>
+      <c r="F1" s="381"/>
+      <c r="G1" s="381"/>
+      <c r="H1" s="381"/>
+      <c r="I1" s="381"/>
+      <c r="J1" s="382"/>
+      <c r="K1" s="382"/>
+      <c r="L1" s="382"/>
+      <c r="M1" s="382"/>
+      <c r="N1" s="382"/>
+      <c r="O1" s="382"/>
+      <c r="P1" s="382"/>
+      <c r="Q1" s="382"/>
       <c r="R1" s="6" t="s">
         <v>263</v>
       </c>
@@ -29966,28 +29966,28 @@
       <c r="D4" s="239"/>
       <c r="E4" s="239"/>
       <c r="F4" s="239"/>
-      <c r="G4" s="367" t="s">
+      <c r="G4" s="383" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="368"/>
-      <c r="I4" s="368"/>
-      <c r="J4" s="368"/>
-      <c r="K4" s="368"/>
-      <c r="L4" s="369"/>
-      <c r="M4" s="370"/>
-      <c r="N4" s="371" t="s">
+      <c r="H4" s="384"/>
+      <c r="I4" s="384"/>
+      <c r="J4" s="384"/>
+      <c r="K4" s="384"/>
+      <c r="L4" s="385"/>
+      <c r="M4" s="386"/>
+      <c r="N4" s="387" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="369"/>
-      <c r="P4" s="369"/>
-      <c r="Q4" s="369"/>
-      <c r="R4" s="369"/>
-      <c r="S4" s="369"/>
-      <c r="T4" s="372"/>
-      <c r="U4" s="367" t="s">
+      <c r="O4" s="385"/>
+      <c r="P4" s="385"/>
+      <c r="Q4" s="385"/>
+      <c r="R4" s="385"/>
+      <c r="S4" s="385"/>
+      <c r="T4" s="388"/>
+      <c r="U4" s="383" t="s">
         <v>28</v>
       </c>
-      <c r="V4" s="370"/>
+      <c r="V4" s="386"/>
       <c r="W4" s="246"/>
       <c r="X4" t="s">
         <v>0</v>
@@ -30416,16 +30416,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:57" s="41" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B1" s="374" t="s">
+      <c r="B1" s="390" t="s">
         <v>170</v>
       </c>
-      <c r="C1" s="374"/>
-      <c r="D1" s="374"/>
-      <c r="E1" s="374"/>
-      <c r="F1" s="374"/>
-      <c r="G1" s="374"/>
-      <c r="H1" s="374"/>
-      <c r="I1" s="374"/>
+      <c r="C1" s="390"/>
+      <c r="D1" s="390"/>
+      <c r="E1" s="390"/>
+      <c r="F1" s="390"/>
+      <c r="G1" s="390"/>
+      <c r="H1" s="390"/>
+      <c r="I1" s="390"/>
     </row>
     <row r="2" spans="1:57" s="41" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="78"/>
@@ -30437,7 +30437,7 @@
       <c r="G2" s="75" t="s">
         <v>169</v>
       </c>
-      <c r="H2" s="373" t="s">
+      <c r="H2" s="389" t="s">
         <v>168</v>
       </c>
       <c r="I2" s="74" t="s">
@@ -30482,7 +30482,7 @@
       <c r="V2" s="74" t="s">
         <v>167</v>
       </c>
-      <c r="W2" s="373" t="s">
+      <c r="W2" s="389" t="s">
         <v>166</v>
       </c>
       <c r="X2" s="73" t="s">
@@ -30512,7 +30512,7 @@
       <c r="AF2" s="73" t="s">
         <v>164</v>
       </c>
-      <c r="AG2" s="373" t="s">
+      <c r="AG2" s="389" t="s">
         <v>163</v>
       </c>
       <c r="AH2" s="73" t="s">
@@ -30554,7 +30554,7 @@
       <c r="AT2" s="73" t="s">
         <v>162</v>
       </c>
-      <c r="AU2" s="373" t="s">
+      <c r="AU2" s="389" t="s">
         <v>161</v>
       </c>
       <c r="AV2" s="72" t="s">
@@ -30584,7 +30584,7 @@
       <c r="BD2" s="72" t="s">
         <v>160</v>
       </c>
-      <c r="BE2" s="373" t="s">
+      <c r="BE2" s="389" t="s">
         <v>159</v>
       </c>
     </row>
@@ -30598,7 +30598,7 @@
       <c r="G3" s="75" t="s">
         <v>158</v>
       </c>
-      <c r="H3" s="373"/>
+      <c r="H3" s="389"/>
       <c r="I3" s="74" t="s">
         <v>157</v>
       </c>
@@ -30639,7 +30639,7 @@
       <c r="V3" s="74" t="s">
         <v>145</v>
       </c>
-      <c r="W3" s="373"/>
+      <c r="W3" s="389"/>
       <c r="X3" s="73" t="s">
         <v>141</v>
       </c>
@@ -30667,7 +30667,7 @@
       <c r="AF3" s="73" t="s">
         <v>135</v>
       </c>
-      <c r="AG3" s="373"/>
+      <c r="AG3" s="389"/>
       <c r="AH3" s="73" t="s">
         <v>134</v>
       </c>
@@ -30707,7 +30707,7 @@
       <c r="AT3" s="73" t="s">
         <v>122</v>
       </c>
-      <c r="AU3" s="373"/>
+      <c r="AU3" s="389"/>
       <c r="AV3" s="72" t="s">
         <v>121</v>
       </c>
@@ -30735,7 +30735,7 @@
       <c r="BD3" s="72" t="s">
         <v>113</v>
       </c>
-      <c r="BE3" s="373"/>
+      <c r="BE3" s="389"/>
     </row>
     <row r="4" spans="1:57" s="41" customFormat="1" ht="60" x14ac:dyDescent="0.15">
       <c r="A4" s="77"/>
@@ -30757,7 +30757,7 @@
       <c r="G4" s="75" t="s">
         <v>108</v>
       </c>
-      <c r="H4" s="373"/>
+      <c r="H4" s="389"/>
       <c r="I4" s="74" t="s">
         <v>107</v>
       </c>
@@ -30800,7 +30800,7 @@
       <c r="V4" s="74" t="s">
         <v>94</v>
       </c>
-      <c r="W4" s="373"/>
+      <c r="W4" s="389"/>
       <c r="X4" s="73" t="s">
         <v>92</v>
       </c>
@@ -30828,7 +30828,7 @@
       <c r="AF4" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="AG4" s="373"/>
+      <c r="AG4" s="389"/>
       <c r="AH4" s="73" t="s">
         <v>84</v>
       </c>
@@ -30868,7 +30868,7 @@
       <c r="AT4" s="73" t="s">
         <v>72</v>
       </c>
-      <c r="AU4" s="373"/>
+      <c r="AU4" s="389"/>
       <c r="AV4" s="72" t="s">
         <v>71</v>
       </c>
@@ -30896,7 +30896,7 @@
       <c r="BD4" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="BE4" s="373"/>
+      <c r="BE4" s="389"/>
     </row>
     <row r="5" spans="1:57" s="41" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="51" t="s">
@@ -33763,16 +33763,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A1" s="375" t="s">
+      <c r="A1" s="391" t="s">
         <v>214</v>
       </c>
-      <c r="B1" s="375"/>
-      <c r="C1" s="375"/>
-      <c r="D1" s="375"/>
-      <c r="E1" s="375"/>
-      <c r="F1" s="375"/>
-      <c r="G1" s="375"/>
-      <c r="H1" s="375"/>
+      <c r="B1" s="391"/>
+      <c r="C1" s="391"/>
+      <c r="D1" s="391"/>
+      <c r="E1" s="391"/>
+      <c r="F1" s="391"/>
+      <c r="G1" s="391"/>
+      <c r="H1" s="391"/>
       <c r="I1" s="41"/>
       <c r="J1" s="41"/>
       <c r="K1" s="41"/>
@@ -33809,7 +33809,7 @@
       <c r="G2" s="75" t="s">
         <v>169</v>
       </c>
-      <c r="H2" s="373" t="s">
+      <c r="H2" s="389" t="s">
         <v>168</v>
       </c>
       <c r="I2" s="75" t="s">
@@ -33842,7 +33842,7 @@
       <c r="R2" s="75" t="s">
         <v>167</v>
       </c>
-      <c r="S2" s="373" t="s">
+      <c r="S2" s="389" t="s">
         <v>166</v>
       </c>
       <c r="T2" s="75" t="s">
@@ -33872,7 +33872,7 @@
       <c r="AB2" s="75" t="s">
         <v>164</v>
       </c>
-      <c r="AC2" s="373" t="s">
+      <c r="AC2" s="389" t="s">
         <v>213</v>
       </c>
       <c r="AD2" s="75" t="s">
@@ -33884,7 +33884,7 @@
       <c r="AF2" s="75" t="s">
         <v>212</v>
       </c>
-      <c r="AG2" s="373" t="s">
+      <c r="AG2" s="389" t="s">
         <v>211</v>
       </c>
     </row>
@@ -33898,7 +33898,7 @@
       <c r="G3" s="75" t="s">
         <v>158</v>
       </c>
-      <c r="H3" s="373"/>
+      <c r="H3" s="389"/>
       <c r="I3" s="75" t="s">
         <v>210</v>
       </c>
@@ -33929,7 +33929,7 @@
       <c r="R3" s="75" t="s">
         <v>145</v>
       </c>
-      <c r="S3" s="373"/>
+      <c r="S3" s="389"/>
       <c r="T3" s="75" t="s">
         <v>201</v>
       </c>
@@ -33957,7 +33957,7 @@
       <c r="AB3" s="75" t="s">
         <v>193</v>
       </c>
-      <c r="AC3" s="373"/>
+      <c r="AC3" s="389"/>
       <c r="AD3" s="75" t="s">
         <v>192</v>
       </c>
@@ -33967,7 +33967,7 @@
       <c r="AF3" s="75" t="s">
         <v>122</v>
       </c>
-      <c r="AG3" s="373"/>
+      <c r="AG3" s="389"/>
     </row>
     <row r="4" spans="1:33" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="78"/>
@@ -33989,7 +33989,7 @@
       <c r="G4" s="75" t="s">
         <v>108</v>
       </c>
-      <c r="H4" s="373"/>
+      <c r="H4" s="389"/>
       <c r="I4" s="75" t="s">
         <v>191</v>
       </c>
@@ -34020,7 +34020,7 @@
       <c r="R4" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="S4" s="373"/>
+      <c r="S4" s="389"/>
       <c r="T4" s="75" t="s">
         <v>182</v>
       </c>
@@ -34048,7 +34048,7 @@
       <c r="AB4" s="75" t="s">
         <v>174</v>
       </c>
-      <c r="AC4" s="373"/>
+      <c r="AC4" s="389"/>
       <c r="AD4" s="75" t="s">
         <v>173</v>
       </c>
@@ -34058,7 +34058,7 @@
       <c r="AF4" s="75" t="s">
         <v>72</v>
       </c>
-      <c r="AG4" s="373"/>
+      <c r="AG4" s="389"/>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A5" s="81" t="s">
@@ -35433,13 +35433,13 @@
       <c r="G2" s="75" t="s">
         <v>167</v>
       </c>
-      <c r="H2" s="373" t="s">
+      <c r="H2" s="389" t="s">
         <v>166</v>
       </c>
       <c r="I2" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="373" t="s">
+      <c r="J2" s="389" t="s">
         <v>165</v>
       </c>
     </row>
@@ -35453,11 +35453,11 @@
       <c r="G3" s="75" t="s">
         <v>145</v>
       </c>
-      <c r="H3" s="373"/>
+      <c r="H3" s="389"/>
       <c r="I3" s="75" t="s">
         <v>142</v>
       </c>
-      <c r="J3" s="373"/>
+      <c r="J3" s="389"/>
     </row>
     <row r="4" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A4" s="97"/>
@@ -35479,11 +35479,11 @@
       <c r="G4" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="H4" s="373"/>
+      <c r="H4" s="389"/>
       <c r="I4" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="J4" s="373"/>
+      <c r="J4" s="389"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="91" t="s">
@@ -35909,7 +35909,7 @@
       <c r="P2" s="277" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="376" t="s">
+      <c r="Q2" s="392" t="s">
         <v>274</v>
       </c>
     </row>
@@ -35950,7 +35950,7 @@
       <c r="P3" s="277" t="s">
         <v>281</v>
       </c>
-      <c r="Q3" s="376"/>
+      <c r="Q3" s="392"/>
     </row>
     <row r="4" spans="1:62" ht="70" x14ac:dyDescent="0.2">
       <c r="A4" s="278"/>
@@ -35999,7 +35999,7 @@
       <c r="P4" s="280" t="s">
         <v>292</v>
       </c>
-      <c r="Q4" s="376"/>
+      <c r="Q4" s="392"/>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A5" s="281" t="s">

</xml_diff>

<commit_message>
fix cph multifactor formulas extractors
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3164879A-4450-2D4C-ACDA-E91C3253F07B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1408546-923B-464B-9BAC-DB85FD1D9A2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
@@ -15900,6 +15900,52 @@
     <xf numFmtId="0" fontId="24" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="30" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="4" applyFont="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="35" fillId="8" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="10" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="8" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="85" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="40" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -16058,52 +16104,6 @@
     <xf numFmtId="49" fontId="32" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="25" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="30" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="4" applyFont="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="35" fillId="8" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="10" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="25" fillId="8" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="85" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma 2" xfId="2" xr:uid="{C877C5E8-FCBF-114F-9ECB-F75EF7C9C0EB}"/>
@@ -17170,11 +17170,11 @@
       <c r="B1" s="115" t="s">
         <v>220</v>
       </c>
-      <c r="C1" s="360" t="s">
+      <c r="C1" s="376" t="s">
         <v>221</v>
       </c>
-      <c r="D1" s="360"/>
-      <c r="E1" s="360"/>
+      <c r="D1" s="376"/>
+      <c r="E1" s="376"/>
       <c r="F1" s="116"/>
       <c r="H1" s="26" t="s">
         <v>0</v>
@@ -17183,11 +17183,11 @@
     <row r="2" spans="1:8" s="120" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="117"/>
       <c r="B2" s="118"/>
-      <c r="C2" s="361" t="s">
+      <c r="C2" s="377" t="s">
         <v>222</v>
       </c>
-      <c r="D2" s="361"/>
-      <c r="E2" s="361"/>
+      <c r="D2" s="377"/>
+      <c r="E2" s="377"/>
       <c r="F2" s="119"/>
       <c r="H2" s="26" t="s">
         <v>0</v>
@@ -17211,10 +17211,10 @@
       <c r="D4" s="125" t="s">
         <v>225</v>
       </c>
-      <c r="E4" s="365" t="s">
+      <c r="E4" s="381" t="s">
         <v>226</v>
       </c>
-      <c r="F4" s="366"/>
+      <c r="F4" s="382"/>
       <c r="G4" s="134"/>
       <c r="H4" s="26" t="s">
         <v>0</v>
@@ -17231,10 +17231,10 @@
       <c r="D5" s="131" t="s">
         <v>229</v>
       </c>
-      <c r="E5" s="367" t="s">
+      <c r="E5" s="383" t="s">
         <v>242</v>
       </c>
-      <c r="F5" s="368"/>
+      <c r="F5" s="384"/>
       <c r="G5" s="133"/>
       <c r="H5" s="26" t="s">
         <v>0</v>
@@ -17251,10 +17251,10 @@
       <c r="D6" s="132" t="s">
         <v>232</v>
       </c>
-      <c r="E6" s="369" t="s">
+      <c r="E6" s="385" t="s">
         <v>243</v>
       </c>
-      <c r="F6" s="370"/>
+      <c r="F6" s="386"/>
       <c r="G6" s="133"/>
       <c r="H6" s="26" t="s">
         <v>0</v>
@@ -17271,10 +17271,10 @@
       <c r="D7" s="132" t="s">
         <v>235</v>
       </c>
-      <c r="E7" s="369" t="s">
+      <c r="E7" s="385" t="s">
         <v>242</v>
       </c>
-      <c r="F7" s="370"/>
+      <c r="F7" s="386"/>
       <c r="G7" s="133"/>
       <c r="H7" s="26" t="s">
         <v>0</v>
@@ -17285,16 +17285,16 @@
       <c r="B8" s="138" t="s">
         <v>236</v>
       </c>
-      <c r="C8" s="371" t="s">
+      <c r="C8" s="387" t="s">
         <v>237</v>
       </c>
-      <c r="D8" s="371" t="s">
+      <c r="D8" s="387" t="s">
         <v>238</v>
       </c>
-      <c r="E8" s="374" t="s">
+      <c r="E8" s="390" t="s">
         <v>244</v>
       </c>
-      <c r="F8" s="374"/>
+      <c r="F8" s="390"/>
       <c r="G8" s="133"/>
       <c r="H8" s="26" t="s">
         <v>0</v>
@@ -17305,10 +17305,10 @@
       <c r="B9" s="304" t="s">
         <v>239</v>
       </c>
-      <c r="C9" s="372"/>
-      <c r="D9" s="372"/>
-      <c r="E9" s="375"/>
-      <c r="F9" s="375"/>
+      <c r="C9" s="388"/>
+      <c r="D9" s="388"/>
+      <c r="E9" s="391"/>
+      <c r="F9" s="391"/>
       <c r="G9" s="133"/>
       <c r="H9" s="26" t="s">
         <v>0</v>
@@ -17319,10 +17319,10 @@
       <c r="B10" s="305" t="s">
         <v>240</v>
       </c>
-      <c r="C10" s="372"/>
-      <c r="D10" s="372"/>
-      <c r="E10" s="375"/>
-      <c r="F10" s="375"/>
+      <c r="C10" s="388"/>
+      <c r="D10" s="388"/>
+      <c r="E10" s="391"/>
+      <c r="F10" s="391"/>
       <c r="G10" s="133"/>
       <c r="H10" s="26" t="s">
         <v>0</v>
@@ -17333,10 +17333,10 @@
       <c r="B11" s="300" t="s">
         <v>364</v>
       </c>
-      <c r="C11" s="373"/>
-      <c r="D11" s="373"/>
-      <c r="E11" s="376"/>
-      <c r="F11" s="376"/>
+      <c r="C11" s="389"/>
+      <c r="D11" s="389"/>
+      <c r="E11" s="392"/>
+      <c r="F11" s="392"/>
       <c r="G11" s="133"/>
       <c r="H11" s="26" t="s">
         <v>0</v>
@@ -17356,11 +17356,11 @@
     <row r="13" spans="1:8" s="26" customFormat="1" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="121"/>
       <c r="B13" s="302"/>
-      <c r="C13" s="364" t="s">
+      <c r="C13" s="380" t="s">
         <v>241</v>
       </c>
-      <c r="D13" s="364"/>
-      <c r="E13" s="364"/>
+      <c r="D13" s="380"/>
+      <c r="E13" s="380"/>
       <c r="F13" s="303"/>
       <c r="H13" s="26" t="s">
         <v>0</v>
@@ -17374,14 +17374,14 @@
       </c>
     </row>
     <row r="15" spans="1:8" s="26" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="362" t="s">
+      <c r="A15" s="378" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="362"/>
-      <c r="C15" s="362"/>
-      <c r="D15" s="362"/>
-      <c r="E15" s="362"/>
-      <c r="F15" s="363"/>
+      <c r="B15" s="378"/>
+      <c r="C15" s="378"/>
+      <c r="D15" s="378"/>
+      <c r="E15" s="378"/>
+      <c r="F15" s="379"/>
       <c r="H15" s="26" t="s">
         <v>0</v>
       </c>
@@ -17516,7 +17516,7 @@
       <c r="G2" s="75" t="s">
         <v>169</v>
       </c>
-      <c r="H2" s="386" t="s">
+      <c r="H2" s="402" t="s">
         <v>168</v>
       </c>
       <c r="I2" s="74" t="s">
@@ -17561,7 +17561,7 @@
       <c r="V2" s="74" t="s">
         <v>167</v>
       </c>
-      <c r="W2" s="386" t="s">
+      <c r="W2" s="402" t="s">
         <v>166</v>
       </c>
       <c r="X2" s="73" t="s">
@@ -17591,7 +17591,7 @@
       <c r="AF2" s="73" t="s">
         <v>164</v>
       </c>
-      <c r="AG2" s="386" t="s">
+      <c r="AG2" s="402" t="s">
         <v>163</v>
       </c>
       <c r="AH2" s="73" t="s">
@@ -17633,7 +17633,7 @@
       <c r="AT2" s="73" t="s">
         <v>162</v>
       </c>
-      <c r="AU2" s="386" t="s">
+      <c r="AU2" s="402" t="s">
         <v>161</v>
       </c>
       <c r="AV2" s="72" t="s">
@@ -17663,7 +17663,7 @@
       <c r="BD2" s="72" t="s">
         <v>160</v>
       </c>
-      <c r="BE2" s="386" t="s">
+      <c r="BE2" s="402" t="s">
         <v>159</v>
       </c>
       <c r="BF2"/>
@@ -17678,7 +17678,7 @@
       <c r="G3" s="75" t="s">
         <v>158</v>
       </c>
-      <c r="H3" s="386"/>
+      <c r="H3" s="402"/>
       <c r="I3" s="74" t="s">
         <v>157</v>
       </c>
@@ -17719,7 +17719,7 @@
       <c r="V3" s="74" t="s">
         <v>145</v>
       </c>
-      <c r="W3" s="386"/>
+      <c r="W3" s="402"/>
       <c r="X3" s="73" t="s">
         <v>141</v>
       </c>
@@ -17747,7 +17747,7 @@
       <c r="AF3" s="73" t="s">
         <v>135</v>
       </c>
-      <c r="AG3" s="386"/>
+      <c r="AG3" s="402"/>
       <c r="AH3" s="73" t="s">
         <v>134</v>
       </c>
@@ -17787,7 +17787,7 @@
       <c r="AT3" s="73" t="s">
         <v>122</v>
       </c>
-      <c r="AU3" s="386"/>
+      <c r="AU3" s="402"/>
       <c r="AV3" s="72" t="s">
         <v>121</v>
       </c>
@@ -17815,7 +17815,7 @@
       <c r="BD3" s="72" t="s">
         <v>113</v>
       </c>
-      <c r="BE3" s="386"/>
+      <c r="BE3" s="402"/>
     </row>
     <row r="4" spans="1:58" s="41" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="77"/>
@@ -17837,7 +17837,7 @@
       <c r="G4" s="75" t="s">
         <v>108</v>
       </c>
-      <c r="H4" s="386"/>
+      <c r="H4" s="402"/>
       <c r="I4" s="74" t="s">
         <v>107</v>
       </c>
@@ -17880,7 +17880,7 @@
       <c r="V4" s="74" t="s">
         <v>94</v>
       </c>
-      <c r="W4" s="386"/>
+      <c r="W4" s="402"/>
       <c r="X4" s="73" t="s">
         <v>92</v>
       </c>
@@ -17908,7 +17908,7 @@
       <c r="AF4" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="AG4" s="386"/>
+      <c r="AG4" s="402"/>
       <c r="AH4" s="73" t="s">
         <v>608</v>
       </c>
@@ -17948,7 +17948,7 @@
       <c r="AT4" s="73" t="s">
         <v>72</v>
       </c>
-      <c r="AU4" s="386"/>
+      <c r="AU4" s="402"/>
       <c r="AV4" s="72" t="s">
         <v>71</v>
       </c>
@@ -17976,7 +17976,7 @@
       <c r="BD4" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="BE4" s="386"/>
+      <c r="BE4" s="402"/>
       <c r="BF4"/>
     </row>
     <row r="5" spans="1:58" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -20571,28 +20571,28 @@
       <c r="E21" s="39"/>
     </row>
     <row r="22" spans="4:57" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E22" s="390" t="s">
+      <c r="E22" s="406" t="s">
         <v>367</v>
       </c>
-      <c r="F22" s="391"/>
-      <c r="G22" s="391"/>
-      <c r="H22" s="391"/>
-      <c r="I22" s="391"/>
-      <c r="J22" s="391"/>
-      <c r="K22" s="391"/>
-      <c r="L22" s="391"/>
-      <c r="M22" s="391"/>
-      <c r="N22" s="391"/>
-      <c r="O22" s="391"/>
-      <c r="P22" s="391"/>
-      <c r="Q22" s="391"/>
-      <c r="R22" s="391"/>
-      <c r="S22" s="391"/>
-      <c r="T22" s="391"/>
-      <c r="U22" s="391"/>
-      <c r="V22" s="391"/>
-      <c r="W22" s="391"/>
-      <c r="X22" s="392"/>
+      <c r="F22" s="407"/>
+      <c r="G22" s="407"/>
+      <c r="H22" s="407"/>
+      <c r="I22" s="407"/>
+      <c r="J22" s="407"/>
+      <c r="K22" s="407"/>
+      <c r="L22" s="407"/>
+      <c r="M22" s="407"/>
+      <c r="N22" s="407"/>
+      <c r="O22" s="407"/>
+      <c r="P22" s="407"/>
+      <c r="Q22" s="407"/>
+      <c r="R22" s="407"/>
+      <c r="S22" s="407"/>
+      <c r="T22" s="407"/>
+      <c r="U22" s="407"/>
+      <c r="V22" s="407"/>
+      <c r="W22" s="407"/>
+      <c r="X22" s="408"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -20701,82 +20701,82 @@
       <c r="D2" s="347"/>
       <c r="E2" s="347"/>
       <c r="F2" s="347"/>
-      <c r="G2" s="408" t="s">
+      <c r="G2" s="360" t="s">
         <v>108</v>
       </c>
       <c r="H2" s="359" t="s">
         <v>168</v>
       </c>
-      <c r="I2" s="408" t="s">
+      <c r="I2" s="360" t="s">
         <v>191</v>
       </c>
-      <c r="J2" s="408" t="s">
+      <c r="J2" s="360" t="s">
         <v>190</v>
       </c>
-      <c r="K2" s="408" t="s">
+      <c r="K2" s="360" t="s">
         <v>189</v>
       </c>
-      <c r="L2" s="408" t="s">
+      <c r="L2" s="360" t="s">
         <v>188</v>
       </c>
-      <c r="M2" s="408" t="s">
+      <c r="M2" s="360" t="s">
         <v>187</v>
       </c>
-      <c r="N2" s="408" t="s">
+      <c r="N2" s="360" t="s">
         <v>186</v>
       </c>
-      <c r="O2" s="408" t="s">
+      <c r="O2" s="360" t="s">
         <v>185</v>
       </c>
-      <c r="P2" s="408" t="s">
+      <c r="P2" s="360" t="s">
         <v>184</v>
       </c>
-      <c r="Q2" s="408" t="s">
+      <c r="Q2" s="360" t="s">
         <v>183</v>
       </c>
-      <c r="R2" s="408" t="s">
+      <c r="R2" s="360" t="s">
         <v>624</v>
       </c>
       <c r="S2" s="359" t="s">
         <v>166</v>
       </c>
-      <c r="T2" s="408" t="s">
+      <c r="T2" s="360" t="s">
         <v>182</v>
       </c>
-      <c r="U2" s="408" t="s">
+      <c r="U2" s="360" t="s">
         <v>181</v>
       </c>
-      <c r="V2" s="408" t="s">
+      <c r="V2" s="360" t="s">
         <v>625</v>
       </c>
-      <c r="W2" s="408" t="s">
+      <c r="W2" s="360" t="s">
         <v>179</v>
       </c>
-      <c r="X2" s="408" t="s">
+      <c r="X2" s="360" t="s">
         <v>178</v>
       </c>
-      <c r="Y2" s="408" t="s">
+      <c r="Y2" s="360" t="s">
         <v>177</v>
       </c>
-      <c r="Z2" s="408" t="s">
+      <c r="Z2" s="360" t="s">
         <v>176</v>
       </c>
-      <c r="AA2" s="408" t="s">
+      <c r="AA2" s="360" t="s">
         <v>175</v>
       </c>
-      <c r="AB2" s="408" t="s">
+      <c r="AB2" s="360" t="s">
         <v>174</v>
       </c>
       <c r="AC2" s="359" t="s">
         <v>213</v>
       </c>
-      <c r="AD2" s="408" t="s">
+      <c r="AD2" s="360" t="s">
         <v>613</v>
       </c>
-      <c r="AE2" s="408" t="s">
+      <c r="AE2" s="360" t="s">
         <v>78</v>
       </c>
-      <c r="AF2" s="408" t="s">
+      <c r="AF2" s="360" t="s">
         <v>72</v>
       </c>
       <c r="AG2" s="359" t="s">
@@ -20790,82 +20790,82 @@
       <c r="D3" s="347"/>
       <c r="E3" s="347"/>
       <c r="F3" s="347"/>
-      <c r="G3" s="408" t="s">
+      <c r="G3" s="360" t="s">
         <v>108</v>
       </c>
       <c r="H3" s="359" t="s">
         <v>168</v>
       </c>
-      <c r="I3" s="408" t="s">
+      <c r="I3" s="360" t="s">
         <v>191</v>
       </c>
-      <c r="J3" s="408" t="s">
+      <c r="J3" s="360" t="s">
         <v>190</v>
       </c>
-      <c r="K3" s="408" t="s">
+      <c r="K3" s="360" t="s">
         <v>189</v>
       </c>
-      <c r="L3" s="408" t="s">
+      <c r="L3" s="360" t="s">
         <v>188</v>
       </c>
-      <c r="M3" s="408" t="s">
+      <c r="M3" s="360" t="s">
         <v>187</v>
       </c>
-      <c r="N3" s="408" t="s">
+      <c r="N3" s="360" t="s">
         <v>186</v>
       </c>
-      <c r="O3" s="408" t="s">
+      <c r="O3" s="360" t="s">
         <v>185</v>
       </c>
-      <c r="P3" s="408" t="s">
+      <c r="P3" s="360" t="s">
         <v>184</v>
       </c>
-      <c r="Q3" s="408" t="s">
+      <c r="Q3" s="360" t="s">
         <v>183</v>
       </c>
-      <c r="R3" s="408" t="s">
+      <c r="R3" s="360" t="s">
         <v>624</v>
       </c>
       <c r="S3" s="359" t="s">
         <v>166</v>
       </c>
-      <c r="T3" s="408" t="s">
+      <c r="T3" s="360" t="s">
         <v>182</v>
       </c>
-      <c r="U3" s="408" t="s">
+      <c r="U3" s="360" t="s">
         <v>181</v>
       </c>
-      <c r="V3" s="408" t="s">
+      <c r="V3" s="360" t="s">
         <v>625</v>
       </c>
-      <c r="W3" s="408" t="s">
+      <c r="W3" s="360" t="s">
         <v>179</v>
       </c>
-      <c r="X3" s="408" t="s">
+      <c r="X3" s="360" t="s">
         <v>178</v>
       </c>
-      <c r="Y3" s="408" t="s">
+      <c r="Y3" s="360" t="s">
         <v>177</v>
       </c>
-      <c r="Z3" s="408" t="s">
+      <c r="Z3" s="360" t="s">
         <v>176</v>
       </c>
-      <c r="AA3" s="408" t="s">
+      <c r="AA3" s="360" t="s">
         <v>175</v>
       </c>
-      <c r="AB3" s="408" t="s">
+      <c r="AB3" s="360" t="s">
         <v>174</v>
       </c>
       <c r="AC3" s="359" t="s">
         <v>213</v>
       </c>
-      <c r="AD3" s="408" t="s">
+      <c r="AD3" s="360" t="s">
         <v>613</v>
       </c>
-      <c r="AE3" s="408" t="s">
+      <c r="AE3" s="360" t="s">
         <v>78</v>
       </c>
-      <c r="AF3" s="408" t="s">
+      <c r="AF3" s="360" t="s">
         <v>72</v>
       </c>
       <c r="AG3" s="359" t="s">
@@ -20889,82 +20889,82 @@
       <c r="F4" s="76" t="s">
         <v>109</v>
       </c>
-      <c r="G4" s="408" t="s">
+      <c r="G4" s="360" t="s">
         <v>108</v>
       </c>
       <c r="H4" s="359" t="s">
         <v>168</v>
       </c>
-      <c r="I4" s="408" t="s">
+      <c r="I4" s="360" t="s">
         <v>191</v>
       </c>
-      <c r="J4" s="408" t="s">
+      <c r="J4" s="360" t="s">
         <v>190</v>
       </c>
-      <c r="K4" s="408" t="s">
+      <c r="K4" s="360" t="s">
         <v>189</v>
       </c>
-      <c r="L4" s="408" t="s">
+      <c r="L4" s="360" t="s">
         <v>188</v>
       </c>
-      <c r="M4" s="408" t="s">
+      <c r="M4" s="360" t="s">
         <v>187</v>
       </c>
-      <c r="N4" s="408" t="s">
+      <c r="N4" s="360" t="s">
         <v>186</v>
       </c>
-      <c r="O4" s="408" t="s">
+      <c r="O4" s="360" t="s">
         <v>185</v>
       </c>
-      <c r="P4" s="408" t="s">
+      <c r="P4" s="360" t="s">
         <v>184</v>
       </c>
-      <c r="Q4" s="408" t="s">
+      <c r="Q4" s="360" t="s">
         <v>183</v>
       </c>
-      <c r="R4" s="408" t="s">
+      <c r="R4" s="360" t="s">
         <v>624</v>
       </c>
       <c r="S4" s="359" t="s">
         <v>166</v>
       </c>
-      <c r="T4" s="408" t="s">
+      <c r="T4" s="360" t="s">
         <v>182</v>
       </c>
-      <c r="U4" s="408" t="s">
+      <c r="U4" s="360" t="s">
         <v>181</v>
       </c>
-      <c r="V4" s="408" t="s">
+      <c r="V4" s="360" t="s">
         <v>625</v>
       </c>
-      <c r="W4" s="408" t="s">
+      <c r="W4" s="360" t="s">
         <v>179</v>
       </c>
-      <c r="X4" s="408" t="s">
+      <c r="X4" s="360" t="s">
         <v>178</v>
       </c>
-      <c r="Y4" s="408" t="s">
+      <c r="Y4" s="360" t="s">
         <v>177</v>
       </c>
-      <c r="Z4" s="408" t="s">
+      <c r="Z4" s="360" t="s">
         <v>176</v>
       </c>
-      <c r="AA4" s="408" t="s">
+      <c r="AA4" s="360" t="s">
         <v>175</v>
       </c>
-      <c r="AB4" s="408" t="s">
+      <c r="AB4" s="360" t="s">
         <v>174</v>
       </c>
       <c r="AC4" s="359" t="s">
         <v>213</v>
       </c>
-      <c r="AD4" s="408" t="s">
+      <c r="AD4" s="360" t="s">
         <v>613</v>
       </c>
-      <c r="AE4" s="408" t="s">
+      <c r="AE4" s="360" t="s">
         <v>78</v>
       </c>
-      <c r="AF4" s="408" t="s">
+      <c r="AF4" s="360" t="s">
         <v>72</v>
       </c>
       <c r="AG4" s="359" t="s">
@@ -20981,7 +20981,7 @@
       <c r="E5" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="F5" s="411" t="s">
+      <c r="F5" s="363" t="s">
         <v>61</v>
       </c>
       <c r="G5" s="106" t="str">
@@ -21106,7 +21106,7 @@
       <c r="E6" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="411" t="s">
+      <c r="F6" s="363" t="s">
         <v>59</v>
       </c>
       <c r="G6" s="106" t="str">
@@ -21231,7 +21231,7 @@
       <c r="E7" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="F7" s="411" t="s">
+      <c r="F7" s="363" t="s">
         <v>57</v>
       </c>
       <c r="G7" s="106" t="str">
@@ -21356,7 +21356,7 @@
       <c r="E8" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="F8" s="411" t="s">
+      <c r="F8" s="363" t="s">
         <v>55</v>
       </c>
       <c r="G8" s="106" t="str">
@@ -21481,7 +21481,7 @@
       <c r="E9" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="F9" s="411" t="s">
+      <c r="F9" s="363" t="s">
         <v>53</v>
       </c>
       <c r="G9" s="106" t="str">
@@ -21606,7 +21606,7 @@
       <c r="E10" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="411" t="s">
+      <c r="F10" s="363" t="s">
         <v>51</v>
       </c>
       <c r="G10" s="106" t="str">
@@ -21731,7 +21731,7 @@
       <c r="E11" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="411" t="s">
+      <c r="F11" s="363" t="s">
         <v>49</v>
       </c>
       <c r="G11" s="106" t="str">
@@ -21856,7 +21856,7 @@
       <c r="E12" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="F12" s="411" t="s">
+      <c r="F12" s="363" t="s">
         <v>47</v>
       </c>
       <c r="G12" s="106" t="str">
@@ -21981,7 +21981,7 @@
       <c r="E13" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="411" t="s">
+      <c r="F13" s="363" t="s">
         <v>45</v>
       </c>
       <c r="G13" s="106" t="str">
@@ -22106,7 +22106,7 @@
       <c r="E14" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="F14" s="411" t="s">
+      <c r="F14" s="363" t="s">
         <v>43</v>
       </c>
       <c r="G14" s="106" t="str">
@@ -22231,7 +22231,7 @@
       <c r="E15" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="411" t="s">
+      <c r="F15" s="363" t="s">
         <v>40</v>
       </c>
       <c r="G15" s="106" t="str">
@@ -22349,7 +22349,7 @@
       <c r="C16" s="80"/>
       <c r="D16" s="80"/>
       <c r="E16" s="80"/>
-      <c r="F16" s="412" t="s">
+      <c r="F16" s="364" t="s">
         <v>39</v>
       </c>
       <c r="G16" s="46">
@@ -22552,32 +22552,32 @@
       <c r="K20" s="140"/>
     </row>
     <row r="21" spans="4:33" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E21" s="393" t="s">
+      <c r="E21" s="409" t="s">
         <v>368</v>
       </c>
-      <c r="F21" s="394"/>
-      <c r="G21" s="394"/>
-      <c r="H21" s="394"/>
-      <c r="I21" s="394"/>
-      <c r="J21" s="394"/>
-      <c r="K21" s="394"/>
-      <c r="L21" s="394"/>
-      <c r="M21" s="394"/>
-      <c r="N21" s="394"/>
-      <c r="O21" s="394"/>
-      <c r="P21" s="394"/>
-      <c r="Q21" s="394"/>
-      <c r="R21" s="394"/>
-      <c r="S21" s="394"/>
-      <c r="T21" s="394"/>
-      <c r="U21" s="394"/>
-      <c r="V21" s="394"/>
-      <c r="W21" s="394"/>
-      <c r="X21" s="394"/>
-      <c r="Y21" s="394"/>
-      <c r="Z21" s="394"/>
-      <c r="AA21" s="394"/>
-      <c r="AB21" s="395"/>
+      <c r="F21" s="410"/>
+      <c r="G21" s="410"/>
+      <c r="H21" s="410"/>
+      <c r="I21" s="410"/>
+      <c r="J21" s="410"/>
+      <c r="K21" s="410"/>
+      <c r="L21" s="410"/>
+      <c r="M21" s="410"/>
+      <c r="N21" s="410"/>
+      <c r="O21" s="410"/>
+      <c r="P21" s="410"/>
+      <c r="Q21" s="410"/>
+      <c r="R21" s="410"/>
+      <c r="S21" s="410"/>
+      <c r="T21" s="410"/>
+      <c r="U21" s="410"/>
+      <c r="V21" s="410"/>
+      <c r="W21" s="410"/>
+      <c r="X21" s="410"/>
+      <c r="Y21" s="410"/>
+      <c r="Z21" s="410"/>
+      <c r="AA21" s="410"/>
+      <c r="AB21" s="411"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -22678,33 +22678,33 @@
       <c r="BJ1" s="37"/>
     </row>
     <row r="2" spans="1:62" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="416"/>
-      <c r="B2" s="416"/>
-      <c r="C2" s="416"/>
-      <c r="D2" s="416"/>
-      <c r="E2" s="416"/>
-      <c r="F2" s="416"/>
+      <c r="A2" s="368"/>
+      <c r="B2" s="368"/>
+      <c r="C2" s="368"/>
+      <c r="D2" s="368"/>
+      <c r="E2" s="368"/>
+      <c r="F2" s="368"/>
       <c r="G2" s="75" t="s">
         <v>167</v>
       </c>
-      <c r="H2" s="386" t="s">
+      <c r="H2" s="402" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:62" ht="36" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="416"/>
-      <c r="B3" s="416"/>
-      <c r="C3" s="416"/>
-      <c r="D3" s="416"/>
-      <c r="E3" s="416"/>
-      <c r="F3" s="416"/>
+      <c r="A3" s="368"/>
+      <c r="B3" s="368"/>
+      <c r="C3" s="368"/>
+      <c r="D3" s="368"/>
+      <c r="E3" s="368"/>
+      <c r="F3" s="368"/>
       <c r="G3" s="75" t="s">
         <v>145</v>
       </c>
-      <c r="H3" s="386"/>
+      <c r="H3" s="402"/>
     </row>
     <row r="4" spans="1:62" ht="36" x14ac:dyDescent="0.2">
-      <c r="A4" s="417"/>
+      <c r="A4" s="369"/>
       <c r="B4" s="96" t="s">
         <v>112</v>
       </c>
@@ -22723,7 +22723,7 @@
       <c r="G4" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="H4" s="386"/>
+      <c r="H4" s="402"/>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A5" s="91" t="s">
@@ -22735,7 +22735,7 @@
       <c r="E5" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="F5" s="409" t="s">
+      <c r="F5" s="361" t="s">
         <v>61</v>
       </c>
       <c r="G5" s="105" t="str">
@@ -22760,7 +22760,7 @@
       <c r="E6" s="90" t="s">
         <v>56</v>
       </c>
-      <c r="F6" s="409" t="s">
+      <c r="F6" s="361" t="s">
         <v>55</v>
       </c>
       <c r="G6" s="105" t="str">
@@ -22785,7 +22785,7 @@
       <c r="E7" s="90" t="s">
         <v>54</v>
       </c>
-      <c r="F7" s="409" t="s">
+      <c r="F7" s="361" t="s">
         <v>53</v>
       </c>
       <c r="G7" s="105" t="str">
@@ -22810,7 +22810,7 @@
       <c r="E8" s="90" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="409" t="s">
+      <c r="F8" s="361" t="s">
         <v>51</v>
       </c>
       <c r="G8" s="105" t="str">
@@ -22835,7 +22835,7 @@
       <c r="E9" s="90" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="409" t="s">
+      <c r="F9" s="361" t="s">
         <v>49</v>
       </c>
       <c r="G9" s="105" t="str">
@@ -22860,7 +22860,7 @@
       <c r="E10" s="90" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="409" t="s">
+      <c r="F10" s="361" t="s">
         <v>47</v>
       </c>
       <c r="G10" s="105" t="str">
@@ -22885,7 +22885,7 @@
       <c r="E11" s="90" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="409" t="s">
+      <c r="F11" s="361" t="s">
         <v>45</v>
       </c>
       <c r="G11" s="105" t="str">
@@ -22910,7 +22910,7 @@
       <c r="E12" s="90" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="409" t="s">
+      <c r="F12" s="361" t="s">
         <v>43</v>
       </c>
       <c r="G12" s="105" t="str">
@@ -22935,7 +22935,7 @@
       <c r="E13" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="409" t="s">
+      <c r="F13" s="361" t="s">
         <v>40</v>
       </c>
       <c r="G13" s="105" t="str">
@@ -22948,12 +22948,12 @@
       </c>
     </row>
     <row r="14" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A14" s="418"/>
+      <c r="A14" s="370"/>
       <c r="B14" s="61"/>
       <c r="C14" s="61"/>
       <c r="D14" s="61"/>
       <c r="E14" s="80"/>
-      <c r="F14" s="410" t="s">
+      <c r="F14" s="362" t="s">
         <v>39</v>
       </c>
       <c r="G14" s="84">
@@ -22977,15 +22977,15 @@
       <c r="J16" s="21"/>
     </row>
     <row r="17" spans="4:10" ht="99" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D17" s="396" t="s">
+      <c r="D17" s="412" t="s">
         <v>369</v>
       </c>
-      <c r="E17" s="397"/>
-      <c r="F17" s="397"/>
-      <c r="G17" s="397"/>
-      <c r="H17" s="397"/>
-      <c r="I17" s="397"/>
-      <c r="J17" s="398"/>
+      <c r="E17" s="413"/>
+      <c r="F17" s="413"/>
+      <c r="G17" s="413"/>
+      <c r="H17" s="413"/>
+      <c r="I17" s="413"/>
+      <c r="J17" s="414"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -23083,7 +23083,7 @@
       <c r="BJ1"/>
     </row>
     <row r="2" spans="1:62" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="414"/>
+      <c r="A2" s="366"/>
       <c r="B2" s="275"/>
       <c r="C2" s="275"/>
       <c r="D2" s="275"/>
@@ -23119,12 +23119,12 @@
       <c r="P2" s="277" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="389" t="s">
+      <c r="Q2" s="405" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:62" ht="24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="414"/>
+      <c r="A3" s="366"/>
       <c r="B3" s="275"/>
       <c r="C3" s="275"/>
       <c r="D3" s="275"/>
@@ -23160,10 +23160,10 @@
       <c r="P3" s="277" t="s">
         <v>278</v>
       </c>
-      <c r="Q3" s="389"/>
+      <c r="Q3" s="405"/>
     </row>
     <row r="4" spans="1:62" ht="36" x14ac:dyDescent="0.2">
-      <c r="A4" s="415"/>
+      <c r="A4" s="367"/>
       <c r="B4" s="355" t="s">
         <v>112</v>
       </c>
@@ -23179,37 +23179,37 @@
       <c r="F4" s="355" t="s">
         <v>109</v>
       </c>
-      <c r="G4" s="408" t="s">
+      <c r="G4" s="360" t="s">
         <v>614</v>
       </c>
-      <c r="H4" s="408" t="s">
+      <c r="H4" s="360" t="s">
         <v>615</v>
       </c>
-      <c r="I4" s="408" t="s">
+      <c r="I4" s="360" t="s">
         <v>616</v>
       </c>
-      <c r="J4" s="408" t="s">
+      <c r="J4" s="360" t="s">
         <v>93</v>
       </c>
-      <c r="K4" s="408" t="s">
+      <c r="K4" s="360" t="s">
         <v>617</v>
       </c>
-      <c r="L4" s="408" t="s">
+      <c r="L4" s="360" t="s">
         <v>618</v>
       </c>
-      <c r="M4" s="408" t="s">
+      <c r="M4" s="360" t="s">
         <v>619</v>
       </c>
-      <c r="N4" s="408" t="s">
+      <c r="N4" s="360" t="s">
         <v>620</v>
       </c>
-      <c r="O4" s="408" t="s">
+      <c r="O4" s="360" t="s">
         <v>621</v>
       </c>
-      <c r="P4" s="408" t="s">
+      <c r="P4" s="360" t="s">
         <v>622</v>
       </c>
-      <c r="Q4" s="389"/>
+      <c r="Q4" s="405"/>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A5" s="281" t="s">
@@ -23641,11 +23641,11 @@
       </c>
       <c r="B12" s="282"/>
       <c r="C12" s="282"/>
-      <c r="D12" s="420">
+      <c r="D12" s="372">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E12" s="421" t="s">
+      <c r="E12" s="373" t="s">
         <v>46</v>
       </c>
       <c r="F12" s="356" t="s">
@@ -23700,9 +23700,9 @@
       <c r="A13" s="357"/>
       <c r="B13" s="357"/>
       <c r="C13" s="357"/>
-      <c r="D13" s="422"/>
-      <c r="E13" s="423"/>
-      <c r="F13" s="419" t="s">
+      <c r="D13" s="374"/>
+      <c r="E13" s="375"/>
+      <c r="F13" s="371" t="s">
         <v>39</v>
       </c>
       <c r="G13" s="287">
@@ -24096,13 +24096,13 @@
   <sheetData>
     <row r="1" spans="1:61" s="142" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="141"/>
-      <c r="B1" s="400" t="s">
+      <c r="B1" s="416" t="s">
         <v>170</v>
       </c>
-      <c r="C1" s="400"/>
-      <c r="D1" s="400"/>
-      <c r="E1" s="400"/>
-      <c r="F1" s="400"/>
+      <c r="C1" s="416"/>
+      <c r="D1" s="416"/>
+      <c r="E1" s="416"/>
+      <c r="F1" s="416"/>
       <c r="G1" s="143"/>
       <c r="H1" s="143"/>
       <c r="I1" s="143"/>
@@ -24147,7 +24147,7 @@
       <c r="O2" s="145" t="s">
         <v>164</v>
       </c>
-      <c r="P2" s="399" t="s">
+      <c r="P2" s="415" t="s">
         <v>163</v>
       </c>
       <c r="Q2" s="145" t="s">
@@ -24189,7 +24189,7 @@
       <c r="AC2" s="145" t="s">
         <v>162</v>
       </c>
-      <c r="AD2" s="399" t="s">
+      <c r="AD2" s="415" t="s">
         <v>161</v>
       </c>
       <c r="AE2" s="146" t="s">
@@ -24219,7 +24219,7 @@
       <c r="AM2" s="146" t="s">
         <v>160</v>
       </c>
-      <c r="AN2" s="399" t="s">
+      <c r="AN2" s="415" t="s">
         <v>159</v>
       </c>
       <c r="AZ2" s="146"/>
@@ -24231,7 +24231,7 @@
       <c r="BF2" s="146"/>
       <c r="BG2" s="146"/>
       <c r="BH2" s="146"/>
-      <c r="BI2" s="399"/>
+      <c r="BI2" s="415"/>
     </row>
     <row r="3" spans="1:61" s="142" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="144"/>
@@ -24267,7 +24267,7 @@
       <c r="O3" s="145" t="s">
         <v>135</v>
       </c>
-      <c r="P3" s="399"/>
+      <c r="P3" s="415"/>
       <c r="Q3" s="145" t="s">
         <v>134</v>
       </c>
@@ -24307,7 +24307,7 @@
       <c r="AC3" s="145" t="s">
         <v>122</v>
       </c>
-      <c r="AD3" s="399"/>
+      <c r="AD3" s="415"/>
       <c r="AE3" s="146" t="s">
         <v>121</v>
       </c>
@@ -24335,7 +24335,7 @@
       <c r="AM3" s="146" t="s">
         <v>113</v>
       </c>
-      <c r="AN3" s="399"/>
+      <c r="AN3" s="415"/>
       <c r="AZ3" s="146"/>
       <c r="BA3" s="146"/>
       <c r="BB3" s="146"/>
@@ -24345,7 +24345,7 @@
       <c r="BF3" s="146"/>
       <c r="BG3" s="146"/>
       <c r="BH3" s="146"/>
-      <c r="BI3" s="399"/>
+      <c r="BI3" s="415"/>
     </row>
     <row r="4" spans="1:61" s="142" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="147"/>
@@ -24391,7 +24391,7 @@
       <c r="O4" s="145" t="s">
         <v>85</v>
       </c>
-      <c r="P4" s="399"/>
+      <c r="P4" s="415"/>
       <c r="Q4" s="145" t="s">
         <v>84</v>
       </c>
@@ -24431,7 +24431,7 @@
       <c r="AC4" s="145" t="s">
         <v>72</v>
       </c>
-      <c r="AD4" s="399"/>
+      <c r="AD4" s="415"/>
       <c r="AE4" s="146" t="s">
         <v>71</v>
       </c>
@@ -24459,7 +24459,7 @@
       <c r="AM4" s="146" t="s">
         <v>63</v>
       </c>
-      <c r="AN4" s="399"/>
+      <c r="AN4" s="415"/>
       <c r="AZ4" s="146"/>
       <c r="BA4" s="146"/>
       <c r="BB4" s="146"/>
@@ -24469,7 +24469,7 @@
       <c r="BF4" s="146"/>
       <c r="BG4" s="146"/>
       <c r="BH4" s="146"/>
-      <c r="BI4" s="399"/>
+      <c r="BI4" s="415"/>
     </row>
     <row r="5" spans="1:61" s="142" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="149" t="s">
@@ -26110,14 +26110,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="401" t="s">
+      <c r="A1" s="417" t="s">
         <v>214</v>
       </c>
-      <c r="B1" s="401"/>
-      <c r="C1" s="401"/>
-      <c r="D1" s="401"/>
-      <c r="E1" s="401"/>
-      <c r="F1" s="401"/>
+      <c r="B1" s="417"/>
+      <c r="C1" s="417"/>
+      <c r="D1" s="417"/>
+      <c r="E1" s="417"/>
+      <c r="F1" s="417"/>
       <c r="G1" s="319"/>
       <c r="H1" s="319"/>
       <c r="I1" s="319"/>
@@ -26167,7 +26167,7 @@
       <c r="O2" s="173" t="s">
         <v>164</v>
       </c>
-      <c r="P2" s="402" t="s">
+      <c r="P2" s="418" t="s">
         <v>213</v>
       </c>
       <c r="Q2" s="173" t="s">
@@ -26179,7 +26179,7 @@
       <c r="S2" s="173" t="s">
         <v>212</v>
       </c>
-      <c r="T2" s="402" t="s">
+      <c r="T2" s="418" t="s">
         <v>211</v>
       </c>
     </row>
@@ -26217,7 +26217,7 @@
       <c r="O3" s="173" t="s">
         <v>193</v>
       </c>
-      <c r="P3" s="402"/>
+      <c r="P3" s="418"/>
       <c r="Q3" s="173" t="s">
         <v>192</v>
       </c>
@@ -26227,7 +26227,7 @@
       <c r="S3" s="173" t="s">
         <v>122</v>
       </c>
-      <c r="T3" s="402"/>
+      <c r="T3" s="418"/>
     </row>
     <row r="4" spans="1:20" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="172"/>
@@ -26273,7 +26273,7 @@
       <c r="O4" s="173" t="s">
         <v>174</v>
       </c>
-      <c r="P4" s="402"/>
+      <c r="P4" s="418"/>
       <c r="Q4" s="173" t="s">
         <v>173</v>
       </c>
@@ -26283,7 +26283,7 @@
       <c r="S4" s="173" t="s">
         <v>72</v>
       </c>
-      <c r="T4" s="402"/>
+      <c r="T4" s="418"/>
     </row>
     <row r="5" spans="1:20" ht="204" x14ac:dyDescent="0.2">
       <c r="A5" s="321" t="s">
@@ -26882,16 +26882,16 @@
   <sheetData>
     <row r="1" spans="1:23" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="181"/>
-      <c r="B1" s="403" t="s">
+      <c r="B1" s="419" t="s">
         <v>170</v>
       </c>
-      <c r="C1" s="403"/>
-      <c r="D1" s="403"/>
-      <c r="E1" s="403"/>
-      <c r="F1" s="403"/>
-      <c r="G1" s="403"/>
-      <c r="H1" s="403"/>
-      <c r="I1" s="403"/>
+      <c r="C1" s="419"/>
+      <c r="D1" s="419"/>
+      <c r="E1" s="419"/>
+      <c r="F1" s="419"/>
+      <c r="G1" s="419"/>
+      <c r="H1" s="419"/>
+      <c r="I1" s="419"/>
       <c r="J1" s="178"/>
       <c r="K1" s="178"/>
       <c r="L1" s="178"/>
@@ -26917,7 +26917,7 @@
       <c r="G2" s="180" t="s">
         <v>169</v>
       </c>
-      <c r="H2" s="404" t="s">
+      <c r="H2" s="420" t="s">
         <v>168</v>
       </c>
       <c r="I2" s="182" t="s">
@@ -26962,7 +26962,7 @@
       <c r="V2" s="182" t="s">
         <v>167</v>
       </c>
-      <c r="W2" s="404" t="s">
+      <c r="W2" s="420" t="s">
         <v>166</v>
       </c>
     </row>
@@ -26976,7 +26976,7 @@
       <c r="G3" s="180" t="s">
         <v>158</v>
       </c>
-      <c r="H3" s="404"/>
+      <c r="H3" s="420"/>
       <c r="I3" s="182" t="s">
         <v>157</v>
       </c>
@@ -27017,7 +27017,7 @@
       <c r="V3" s="182" t="s">
         <v>145</v>
       </c>
-      <c r="W3" s="404"/>
+      <c r="W3" s="420"/>
     </row>
     <row r="4" spans="1:23" ht="98" x14ac:dyDescent="0.2">
       <c r="A4" s="183"/>
@@ -27039,7 +27039,7 @@
       <c r="G4" s="180" t="s">
         <v>108</v>
       </c>
-      <c r="H4" s="404"/>
+      <c r="H4" s="420"/>
       <c r="I4" s="182" t="s">
         <v>107</v>
       </c>
@@ -27082,7 +27082,7 @@
       <c r="V4" s="185" t="s">
         <v>94</v>
       </c>
-      <c r="W4" s="404"/>
+      <c r="W4" s="420"/>
     </row>
     <row r="5" spans="1:23" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A5" s="186" t="s">
@@ -27793,16 +27793,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="406" t="s">
+      <c r="A1" s="422" t="s">
         <v>214</v>
       </c>
-      <c r="B1" s="406"/>
-      <c r="C1" s="406"/>
-      <c r="D1" s="406"/>
-      <c r="E1" s="406"/>
-      <c r="F1" s="406"/>
-      <c r="G1" s="406"/>
-      <c r="H1" s="406"/>
+      <c r="B1" s="422"/>
+      <c r="C1" s="422"/>
+      <c r="D1" s="422"/>
+      <c r="E1" s="422"/>
+      <c r="F1" s="422"/>
+      <c r="G1" s="422"/>
+      <c r="H1" s="422"/>
       <c r="I1" s="220"/>
       <c r="J1" s="220"/>
       <c r="K1" s="220"/>
@@ -27827,7 +27827,7 @@
       <c r="G2" s="222" t="s">
         <v>169</v>
       </c>
-      <c r="H2" s="405" t="s">
+      <c r="H2" s="421" t="s">
         <v>168</v>
       </c>
       <c r="I2" s="222" t="s">
@@ -27860,7 +27860,7 @@
       <c r="R2" s="222" t="s">
         <v>167</v>
       </c>
-      <c r="S2" s="405" t="s">
+      <c r="S2" s="421" t="s">
         <v>166</v>
       </c>
     </row>
@@ -27874,7 +27874,7 @@
       <c r="G3" s="222" t="s">
         <v>158</v>
       </c>
-      <c r="H3" s="405"/>
+      <c r="H3" s="421"/>
       <c r="I3" s="222" t="s">
         <v>210</v>
       </c>
@@ -27905,7 +27905,7 @@
       <c r="R3" s="222" t="s">
         <v>145</v>
       </c>
-      <c r="S3" s="405"/>
+      <c r="S3" s="421"/>
     </row>
     <row r="4" spans="1:21" ht="112" x14ac:dyDescent="0.2">
       <c r="A4" s="219"/>
@@ -27927,7 +27927,7 @@
       <c r="G4" s="222" t="s">
         <v>108</v>
       </c>
-      <c r="H4" s="405"/>
+      <c r="H4" s="421"/>
       <c r="I4" s="222" t="s">
         <v>191</v>
       </c>
@@ -27958,7 +27958,7 @@
       <c r="R4" s="222" t="s">
         <v>94</v>
       </c>
-      <c r="S4" s="405"/>
+      <c r="S4" s="421"/>
     </row>
     <row r="5" spans="1:21" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A5" s="225" t="s">
@@ -28594,13 +28594,13 @@
       <c r="K2" s="173" t="s">
         <v>167</v>
       </c>
-      <c r="L2" s="402" t="s">
+      <c r="L2" s="418" t="s">
         <v>166</v>
       </c>
       <c r="M2" s="173" t="s">
         <v>38</v>
       </c>
-      <c r="N2" s="402" t="s">
+      <c r="N2" s="418" t="s">
         <v>165</v>
       </c>
     </row>
@@ -28618,11 +28618,11 @@
       <c r="K3" s="173" t="s">
         <v>145</v>
       </c>
-      <c r="L3" s="402"/>
+      <c r="L3" s="418"/>
       <c r="M3" s="173" t="s">
         <v>142</v>
       </c>
-      <c r="N3" s="402"/>
+      <c r="N3" s="418"/>
     </row>
     <row r="4" spans="1:14" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="204"/>
@@ -28648,11 +28648,11 @@
       <c r="K4" s="173" t="s">
         <v>94</v>
       </c>
-      <c r="L4" s="402"/>
+      <c r="L4" s="418"/>
       <c r="M4" s="173" t="s">
         <v>93</v>
       </c>
-      <c r="N4" s="402"/>
+      <c r="N4" s="418"/>
     </row>
     <row r="5" spans="1:14" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="206"/>
@@ -29325,12 +29325,12 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="294"/>
-      <c r="B1" s="407" t="s">
+      <c r="B1" s="423" t="s">
         <v>292</v>
       </c>
-      <c r="C1" s="407"/>
-      <c r="D1" s="407"/>
-      <c r="E1" s="407"/>
+      <c r="C1" s="423"/>
+      <c r="D1" s="423"/>
+      <c r="E1" s="423"/>
       <c r="F1" s="295"/>
       <c r="G1" s="294"/>
       <c r="H1" s="294"/>
@@ -29381,7 +29381,7 @@
       <c r="P2" s="277" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="389" t="s">
+      <c r="Q2" s="405" t="s">
         <v>271</v>
       </c>
     </row>
@@ -29422,7 +29422,7 @@
       <c r="P3" s="277" t="s">
         <v>278</v>
       </c>
-      <c r="Q3" s="389"/>
+      <c r="Q3" s="405"/>
     </row>
     <row r="4" spans="1:17" ht="70" x14ac:dyDescent="0.2">
       <c r="A4" s="278"/>
@@ -29471,7 +29471,7 @@
       <c r="P4" s="280" t="s">
         <v>289</v>
       </c>
-      <c r="Q4" s="389"/>
+      <c r="Q4" s="405"/>
     </row>
     <row r="5" spans="1:17" ht="398" x14ac:dyDescent="0.2">
       <c r="A5" s="281" t="s">
@@ -29934,22 +29934,22 @@
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="377" t="s">
+      <c r="D1" s="393" t="s">
         <v>365</v>
       </c>
-      <c r="E1" s="378"/>
-      <c r="F1" s="378"/>
-      <c r="G1" s="378"/>
-      <c r="H1" s="378"/>
-      <c r="I1" s="378"/>
-      <c r="J1" s="379"/>
-      <c r="K1" s="379"/>
-      <c r="L1" s="379"/>
-      <c r="M1" s="379"/>
-      <c r="N1" s="379"/>
-      <c r="O1" s="379"/>
-      <c r="P1" s="379"/>
-      <c r="Q1" s="379"/>
+      <c r="E1" s="394"/>
+      <c r="F1" s="394"/>
+      <c r="G1" s="394"/>
+      <c r="H1" s="394"/>
+      <c r="I1" s="394"/>
+      <c r="J1" s="395"/>
+      <c r="K1" s="395"/>
+      <c r="L1" s="395"/>
+      <c r="M1" s="395"/>
+      <c r="N1" s="395"/>
+      <c r="O1" s="395"/>
+      <c r="P1" s="395"/>
+      <c r="Q1" s="395"/>
       <c r="R1" s="6" t="s">
         <v>260</v>
       </c>
@@ -30099,28 +30099,28 @@
       <c r="D4" s="239"/>
       <c r="E4" s="239"/>
       <c r="F4" s="239"/>
-      <c r="G4" s="380" t="s">
+      <c r="G4" s="396" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="381"/>
-      <c r="I4" s="381"/>
-      <c r="J4" s="381"/>
-      <c r="K4" s="381"/>
-      <c r="L4" s="382"/>
-      <c r="M4" s="383"/>
-      <c r="N4" s="384" t="s">
+      <c r="H4" s="397"/>
+      <c r="I4" s="397"/>
+      <c r="J4" s="397"/>
+      <c r="K4" s="397"/>
+      <c r="L4" s="398"/>
+      <c r="M4" s="399"/>
+      <c r="N4" s="400" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="382"/>
-      <c r="P4" s="382"/>
-      <c r="Q4" s="382"/>
-      <c r="R4" s="382"/>
-      <c r="S4" s="382"/>
-      <c r="T4" s="385"/>
-      <c r="U4" s="380" t="s">
+      <c r="O4" s="398"/>
+      <c r="P4" s="398"/>
+      <c r="Q4" s="398"/>
+      <c r="R4" s="398"/>
+      <c r="S4" s="398"/>
+      <c r="T4" s="401"/>
+      <c r="U4" s="396" t="s">
         <v>28</v>
       </c>
-      <c r="V4" s="383"/>
+      <c r="V4" s="399"/>
       <c r="W4" s="246"/>
       <c r="X4" t="s">
         <v>0</v>
@@ -30522,11 +30522,11 @@
   <dimension ref="A1:BE24"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
-      <selection pane="bottomRight" activeCell="T15" sqref="T15"/>
+      <selection pane="bottomRight" activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -30549,16 +30549,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:57" s="41" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B1" s="387" t="s">
+      <c r="B1" s="403" t="s">
         <v>170</v>
       </c>
-      <c r="C1" s="387"/>
-      <c r="D1" s="387"/>
-      <c r="E1" s="387"/>
-      <c r="F1" s="387"/>
-      <c r="G1" s="387"/>
-      <c r="H1" s="387"/>
-      <c r="I1" s="387"/>
+      <c r="C1" s="403"/>
+      <c r="D1" s="403"/>
+      <c r="E1" s="403"/>
+      <c r="F1" s="403"/>
+      <c r="G1" s="403"/>
+      <c r="H1" s="403"/>
+      <c r="I1" s="403"/>
     </row>
     <row r="2" spans="1:57" s="41" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="78"/>
@@ -30570,7 +30570,7 @@
       <c r="G2" s="75" t="s">
         <v>169</v>
       </c>
-      <c r="H2" s="386" t="s">
+      <c r="H2" s="402" t="s">
         <v>168</v>
       </c>
       <c r="I2" s="74" t="s">
@@ -30615,7 +30615,7 @@
       <c r="V2" s="74" t="s">
         <v>167</v>
       </c>
-      <c r="W2" s="386" t="s">
+      <c r="W2" s="402" t="s">
         <v>166</v>
       </c>
       <c r="X2" s="73" t="s">
@@ -30645,7 +30645,7 @@
       <c r="AF2" s="73" t="s">
         <v>164</v>
       </c>
-      <c r="AG2" s="386" t="s">
+      <c r="AG2" s="402" t="s">
         <v>163</v>
       </c>
       <c r="AH2" s="73" t="s">
@@ -30687,7 +30687,7 @@
       <c r="AT2" s="73" t="s">
         <v>162</v>
       </c>
-      <c r="AU2" s="386" t="s">
+      <c r="AU2" s="402" t="s">
         <v>161</v>
       </c>
       <c r="AV2" s="72" t="s">
@@ -30717,7 +30717,7 @@
       <c r="BD2" s="72" t="s">
         <v>160</v>
       </c>
-      <c r="BE2" s="386" t="s">
+      <c r="BE2" s="402" t="s">
         <v>159</v>
       </c>
     </row>
@@ -30731,7 +30731,7 @@
       <c r="G3" s="75" t="s">
         <v>158</v>
       </c>
-      <c r="H3" s="386"/>
+      <c r="H3" s="402"/>
       <c r="I3" s="74" t="s">
         <v>157</v>
       </c>
@@ -30772,7 +30772,7 @@
       <c r="V3" s="74" t="s">
         <v>145</v>
       </c>
-      <c r="W3" s="386"/>
+      <c r="W3" s="402"/>
       <c r="X3" s="73" t="s">
         <v>141</v>
       </c>
@@ -30800,7 +30800,7 @@
       <c r="AF3" s="73" t="s">
         <v>135</v>
       </c>
-      <c r="AG3" s="386"/>
+      <c r="AG3" s="402"/>
       <c r="AH3" s="73" t="s">
         <v>134</v>
       </c>
@@ -30840,7 +30840,7 @@
       <c r="AT3" s="73" t="s">
         <v>122</v>
       </c>
-      <c r="AU3" s="386"/>
+      <c r="AU3" s="402"/>
       <c r="AV3" s="72" t="s">
         <v>121</v>
       </c>
@@ -30868,7 +30868,7 @@
       <c r="BD3" s="72" t="s">
         <v>113</v>
       </c>
-      <c r="BE3" s="386"/>
+      <c r="BE3" s="402"/>
     </row>
     <row r="4" spans="1:57" s="41" customFormat="1" ht="60" x14ac:dyDescent="0.15">
       <c r="A4" s="77"/>
@@ -30890,7 +30890,7 @@
       <c r="G4" s="75" t="s">
         <v>108</v>
       </c>
-      <c r="H4" s="386"/>
+      <c r="H4" s="402"/>
       <c r="I4" s="74" t="s">
         <v>107</v>
       </c>
@@ -30933,7 +30933,7 @@
       <c r="V4" s="74" t="s">
         <v>94</v>
       </c>
-      <c r="W4" s="386"/>
+      <c r="W4" s="402"/>
       <c r="X4" s="73" t="s">
         <v>92</v>
       </c>
@@ -30961,7 +30961,7 @@
       <c r="AF4" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="AG4" s="386"/>
+      <c r="AG4" s="402"/>
       <c r="AH4" s="73" t="s">
         <v>84</v>
       </c>
@@ -31001,7 +31001,7 @@
       <c r="AT4" s="73" t="s">
         <v>72</v>
       </c>
-      <c r="AU4" s="386"/>
+      <c r="AU4" s="402"/>
       <c r="AV4" s="72" t="s">
         <v>71</v>
       </c>
@@ -31029,7 +31029,7 @@
       <c r="BD4" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="BE4" s="386"/>
+      <c r="BE4" s="402"/>
     </row>
     <row r="5" spans="1:57" s="41" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="51" t="s">
@@ -31047,50 +31047,50 @@
       <c r="F5" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="G5" s="101" t="e" cm="1">
-        <f t="array" ref="G5">SUM(SUMIFS(
+      <c r="G5" s="101" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("1. TOTAL CONTENTIEUX SOCIAL",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire CTECH",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("2. TOTAL CONTENTIEUX JAF",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire CTECH",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3. TOTAL CONTENTIEUX DE LA PROTECTION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire CTECH",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("4. TOTAL CIVIL NON SPÉCIALISÉ",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire CTECH",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("5. TOTAL JLD CIVIL",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire CTECH",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("6.1. ACTIVITÉ CIVILE",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire CTECH",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.7. FONCTIONNAIRES AFFECTÉS AU CPH",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire CTECH",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.8. FONCTIONNAIRES AFFECTÉS AUX ACTIVITÉS CIVILES ET COMMERCIALES DU PARQUET",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire CTECH",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="H5" s="59" t="e">
         <f t="shared" ref="H5:H15" si="0">SUM(G5)</f>
         <v>#N/A</v>
       </c>
-      <c r="I5" s="58" t="e" cm="1">
-        <f t="array" ref="I5">SUM(SUMIFS(
+      <c r="I5" s="58" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.8. FONCTIONNAIRES AFFECTÉS AUX ACTIVITÉS CIVILES ET COMMERCIALES DU PARQUET",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="J5" s="70"/>
@@ -31099,81 +31099,81 @@
       <c r="M5" s="70"/>
       <c r="N5" s="70"/>
       <c r="O5" s="70"/>
-      <c r="P5" s="58" t="e" cm="1">
-        <f t="array" ref="P5">SUM(SUMIFS(
+      <c r="P5" s="58" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3.2. PROTECTION DES MAJEURS",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q5" s="58" t="e" cm="1">
-        <f t="array" ref="Q5">SUM(SUMIFS(
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q5" s="58" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3. TOTAL CONTENTIEUX DE LA PROTECTION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))-
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3.2. PROTECTION DES MAJEURS",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))-
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3.43. INJONCTIONS DE PAYER",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))-
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3.44. SAISIE DES RÉMUNÉRATIONS",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R5" s="58" t="e" cm="1">
-        <f t="array" ref="R5">SUM(SUMIFS(
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R5" s="58" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("5. TOTAL JLD CIVIL",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("6.1. ACTIVITÉ CIVILE",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="S5" s="58" t="e" cm="1">
-        <f t="array" ref="S5">SUM(SUMIFS(
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="S5" s="58" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3.43. INJONCTIONS DE PAYER",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3.44. SAISIE DES RÉMUNÉRATIONS",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="T5" s="58" t="e" cm="1">
-        <f t="array" ref="T5">SUM(SUMIFS(
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="T5" s="58" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("4.0. CONTENTIEUX GÉNÉRAL &lt;10.000€",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="U5" s="58" t="e" cm="1">
-        <f t="array" ref="U5">SUM(SUMIFS(
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U5" s="58" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("1. TOTAL CONTENTIEUX SOCIAL",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="V5" s="58" t="e" cm="1">
-        <f t="array" ref="V5">SUM(SUMIFS(
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="V5" s="58" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("2. TOTAL CONTENTIEUX JAF",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("4. TOTAL CIVIL NON SPÉCIALISÉ",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))-
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("4.0. CONTENTIEUX GÉNÉRAL &lt;10.000€",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="W5" s="46" t="e">
@@ -31184,26 +31184,26 @@
         <f t="array" ref="X5">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3.2. PROTECTION DES MAJEURS",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"Magistrat SIEGE S";"Magistrat SIEGE NS"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="Y5" s="53" t="e" cm="1">
         <f t="array" ref="Y5">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3. TOTAL CONTENTIEUX DE LA PROTECTION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"Magistrat SIEGE S";"Magistrat SIEGE NS"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))-
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3.2. PROTECTION DES MAJEURS",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"Magistrat SIEGE S";"Magistrat SIEGE NS"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))-
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3.43. INJONCTIONS DE PAYER",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"Magistrat SIEGE S";"Magistrat SIEGE NS"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))-
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3.44. SAISIE DES RÉMUNÉRATIONS",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"Magistrat SIEGE S";"Magistrat SIEGE NS"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="Z5" s="68"/>
@@ -31237,36 +31237,36 @@
         <f t="array" ref="AN5">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("1.1. DÉPARTAGE PRUD'HOMAL",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"Magistrat SIEGE S";"Magistrat SIEGE NS"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AO5" s="53" t="e" cm="1">
         <f t="array" ref="AO5">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("4.0. CONTENTIEUX GÉNÉRAL &lt;10.000€",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"Magistrat SIEGE S";"Magistrat SIEGE NS"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AP5" s="53" t="e" cm="1">
         <f t="array" ref="AP5">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3.43. INJONCTIONS DE PAYER",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"Magistrat SIEGE S";"Magistrat SIEGE NS"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3.44. SAISIE DES RÉMUNÉRATIONS",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"Magistrat SIEGE S";"Magistrat SIEGE NS"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AQ5" s="53" t="e" cm="1">
         <f t="array" ref="AQ5">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("1. TOTAL CONTENTIEUX SOCIAL",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"Magistrat SIEGE S";"Magistrat SIEGE NS"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))-
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("1.1. DÉPARTAGE PRUD'HOMAL",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"Magistrat SIEGE S";"Magistrat SIEGE NS"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AR5" s="55" t="e" cm="1">
@@ -31275,26 +31275,26 @@
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"Magistrat SIEGE S";"Magistrat SIEGE NS"}))</f>
         <v>#N/A</v>
       </c>
-      <c r="AS5" s="55" t="e" cm="1">
-        <f t="array" ref="AS5">SUM(SUMIFS(
+      <c r="AS5" s="55" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("4. TOTAL CIVIL NON SPÉCIALISÉ",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat SIEGE S",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))-
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("4.0. CONTENTIEUX GÉNÉRAL &lt;10.000€",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat SIEGE S",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AT5" s="55" t="e" cm="1">
-        <f t="array" ref="AT5">SUM(SUMIFS(
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AT5" s="55" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("4. TOTAL CIVIL NON SPÉCIALISÉ",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat SIEGE NS",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))-
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("4.0. CONTENTIEUX GÉNÉRAL &lt;10.000€",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat SIEGE NS",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AU5" s="46" t="e">
@@ -31695,14 +31695,14 @@
         <f t="array" ref="Y7">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.5. CSM",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JCP";"VPCP";"1VPCP"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="Z7" s="53" t="e" cm="1">
         <f t="array" ref="Z7">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.5. CSM",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JI";"VPI";"1VPI"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AA7" s="62"/>
@@ -31712,21 +31712,21 @@
         <f t="array" ref="AD7">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.5. CSM",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JAP";"VPAP";"1VPAP"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AE7" s="53" t="e" cm="1">
         <f t="array" ref="AE7">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.5. CSM",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JE";"VPE";"1VPE"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AF7" s="53" t="e" cm="1">
         <f t="array" ref="AF7">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.5. CSM",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"VPLD";"1VPLD"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AG7" s="46" t="e">
@@ -31745,11 +31745,11 @@
       <c r="AQ7" s="62"/>
       <c r="AR7" s="266"/>
       <c r="AS7" s="62"/>
-      <c r="AT7" s="53" t="e" cm="1">
-        <f t="array" ref="AT7">SUM(SUMIFS(
+      <c r="AT7" s="53" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.5. CSM",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat SIEGE NS",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AU7" s="46" t="e">
@@ -31786,11 +31786,11 @@
       <c r="F8" s="60" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="101" t="e" cm="1">
-        <f t="array" ref="G8">SUM(SUMIFS(
+      <c r="G8" s="101" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.51. ACCUEIL DU JUSTICIABLE (DONT SAUJ)",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire CTECH",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="H8" s="59" t="e">
@@ -31810,11 +31810,11 @@
       <c r="S8" s="62"/>
       <c r="T8" s="62"/>
       <c r="U8" s="62"/>
-      <c r="V8" s="53" t="e" cm="1">
-        <f t="array" ref="V8">SUM(SUMIFS(
+      <c r="V8" s="53" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.51. ACCUEIL DU JUSTICIABLE (DONT SAUJ)",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="W8" s="46" t="e">
@@ -31826,14 +31826,14 @@
         <f t="array" ref="Y8">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.51. ACCUEIL DU JUSTICIABLE (DONT SAUJ)",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JCP";"VPCP";"1VPCP"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="Z8" s="53" t="e" cm="1">
         <f t="array" ref="Z8">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.51. ACCUEIL DU JUSTICIABLE (DONT SAUJ)",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JI";"VPI";"1VPI"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AA8" s="62"/>
@@ -31843,21 +31843,21 @@
         <f t="array" ref="AD8">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.51. ACCUEIL DU JUSTICIABLE (DONT SAUJ)",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JAP";"VPAP";"1VPAP"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AE8" s="53" t="e" cm="1">
         <f t="array" ref="AE8">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.51. ACCUEIL DU JUSTICIABLE (DONT SAUJ)",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JE";"VPE";"1VPE"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AF8" s="53" t="e" cm="1">
         <f t="array" ref="AF8">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.51. ACCUEIL DU JUSTICIABLE (DONT SAUJ)",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"VPLD";"1VPLD"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AG8" s="46" t="e">
@@ -31876,11 +31876,11 @@
       <c r="AQ8" s="62"/>
       <c r="AR8" s="62"/>
       <c r="AS8" s="62"/>
-      <c r="AT8" s="53" t="e" cm="1">
-        <f t="array" ref="AT8">SUM(SUMIFS(
+      <c r="AT8" s="53" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.51. ACCUEIL DU JUSTICIABLE (DONT SAUJ)",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat SIEGE NS",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AU8" s="46" t="e">
@@ -31917,19 +31917,19 @@
       <c r="F9" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="101" t="e" cm="1">
-        <f t="array" ref="G9">SUM(SUMIFS(
+      <c r="G9" s="101" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.1. SOUTIEN (HORS FORMATIONS SUIVIES)",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire CTECH",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.2. FORMATIONS SUIVIES",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire CTECH",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.6. AUTRES ACTIVITÉS NON JURIDICTIONNELLES",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire CTECH",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="H9" s="59" t="e">
@@ -31949,19 +31949,19 @@
       <c r="S9" s="62"/>
       <c r="T9" s="62"/>
       <c r="U9" s="62"/>
-      <c r="V9" s="53" t="e" cm="1">
-        <f t="array" ref="V9">SUM(SUMIFS(
+      <c r="V9" s="53" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.1. SOUTIEN (HORS FORMATIONS SUIVIES)",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.2. FORMATIONS SUIVIES",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.6. AUTRES ACTIVITÉS NON JURIDICTIONNELLES",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="W9" s="46" t="e">
@@ -31973,30 +31973,30 @@
         <f t="array" ref="Y9">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.1. SOUTIEN (HORS FORMATIONS SUIVIES)",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JCP";"VPCP";"1VPCP"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.2. FORMATIONS SUIVIES",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JCP";"VPCP";"1VPCP"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.6. AUTRES ACTIVITÉS NON JURIDICTIONNELLES",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JCP";"VPCP";"1VPCP"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="Z9" s="53" t="e" cm="1">
         <f t="array" ref="Z9">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.1. SOUTIEN (HORS FORMATIONS SUIVIES)",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JI";"VPI";"1VPI"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.2. FORMATIONS SUIVIES",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JI";"VPI";"1VPI"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.6. AUTRES ACTIVITÉS NON JURIDICTIONNELLES",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JI";"VPI";"1VPI"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AA9" s="62"/>
@@ -32006,45 +32006,45 @@
         <f t="array" ref="AD9">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.1. SOUTIEN (HORS FORMATIONS SUIVIES)",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JAP";"VPAP";"1VPAP"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.2. FORMATIONS SUIVIES",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JAP";"VPAP";"1VPAP"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.6. AUTRES ACTIVITÉS NON JURIDICTIONNELLES",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JAP";"VPAP";"1VPAP"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AE9" s="53" t="e" cm="1">
         <f t="array" ref="AE9">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.1. SOUTIEN (HORS FORMATIONS SUIVIES)",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JE";"VPE";"1VPE"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.2. FORMATIONS SUIVIES",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JE";"VPE";"1VPE"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.6. AUTRES ACTIVITÉS NON JURIDICTIONNELLES",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JE";"VPE";"1VPE"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AF9" s="53" t="e" cm="1">
         <f t="array" ref="AF9">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.1. SOUTIEN (HORS FORMATIONS SUIVIES)",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"VPLD";"1VPLD"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.2. FORMATIONS SUIVIES",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"VPLD";"1VPLD"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.6. AUTRES ACTIVITÉS NON JURIDICTIONNELLES",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"VPLD";"1VPLD"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AG9" s="46" t="e">
@@ -32063,19 +32063,19 @@
       <c r="AQ9" s="62"/>
       <c r="AR9" s="62"/>
       <c r="AS9" s="62"/>
-      <c r="AT9" s="53" t="e" cm="1">
-        <f t="array" ref="AT9">SUM(SUMIFS(
+      <c r="AT9" s="53" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.1. SOUTIEN (HORS FORMATIONS SUIVIES)",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat SIEGE NS",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.2. FORMATIONS SUIVIES",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat SIEGE NS",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.6. AUTRES ACTIVITÉS NON JURIDICTIONNELLES",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat SIEGE NS",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AU9" s="46" t="e">
@@ -32112,11 +32112,11 @@
       <c r="F10" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="G10" s="101" t="e" cm="1">
-        <f t="array" ref="G10">SUM(SUMIFS(
+      <c r="G10" s="101" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.3. FORMATIONS DISPENSÉES",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire CTECH",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="H10" s="59" t="e">
@@ -32136,11 +32136,11 @@
       <c r="S10" s="62"/>
       <c r="T10" s="62"/>
       <c r="U10" s="62"/>
-      <c r="V10" s="53" t="e" cm="1">
-        <f t="array" ref="V10">SUM(SUMIFS(
+      <c r="V10" s="53" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.3. FORMATIONS DISPENSÉES",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="W10" s="46" t="e">
@@ -32152,14 +32152,14 @@
         <f t="array" ref="Y10">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.3. FORMATIONS DISPENSÉES",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JCP";"VPCP";"1VPCP"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="Z10" s="53" t="e" cm="1">
         <f t="array" ref="Z10">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.3. FORMATIONS DISPENSÉES",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JI";"VPI";"1VPI"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AA10" s="62"/>
@@ -32169,21 +32169,21 @@
         <f t="array" ref="AD10">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.3. FORMATIONS DISPENSÉES",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JAP";"VPAP";"1VPAP"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AE10" s="53" t="e" cm="1">
         <f t="array" ref="AE10">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.3. FORMATIONS DISPENSÉES",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JE";"VPE";"1VPE"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AF10" s="53" t="e" cm="1">
         <f t="array" ref="AF10">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.3. FORMATIONS DISPENSÉES",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"VPLD";"1VPLD"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AG10" s="46" t="e">
@@ -32202,11 +32202,11 @@
       <c r="AQ10" s="62"/>
       <c r="AR10" s="62"/>
       <c r="AS10" s="62"/>
-      <c r="AT10" s="53" t="e" cm="1">
-        <f t="array" ref="AT10">SUM(SUMIFS(
+      <c r="AT10" s="53" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.3. FORMATIONS DISPENSÉES",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat SIEGE NS",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AU10" s="46" t="e">
@@ -32243,11 +32243,11 @@
       <c r="F11" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="G11" s="101" t="e" cm="1">
-        <f t="array" ref="G11">SUM(SUMIFS(
+      <c r="G11" s="101" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.4. ACCÈS AU DROIT ET À LA JUSTICE",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire CTECH",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="H11" s="59" t="e">
@@ -32267,11 +32267,11 @@
       <c r="S11" s="62"/>
       <c r="T11" s="62"/>
       <c r="U11" s="62"/>
-      <c r="V11" s="53" t="e" cm="1">
-        <f t="array" ref="V11">SUM(SUMIFS(
+      <c r="V11" s="53" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.4. ACCÈS AU DROIT ET À LA JUSTICE",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="W11" s="46" t="e">
@@ -32283,14 +32283,14 @@
         <f t="array" ref="Y11">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.4. ACCÈS AU DROIT ET À LA JUSTICE",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JCP";"VPCP";"1VPCP"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="Z11" s="53" t="e" cm="1">
         <f t="array" ref="Z11">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.4. ACCÈS AU DROIT ET À LA JUSTICE",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JI";"VPI";"1VPI"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AA11" s="64"/>
@@ -32300,21 +32300,21 @@
         <f t="array" ref="AD11">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.4. ACCÈS AU DROIT ET À LA JUSTICE",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JAP";"VPAP";"1VPAP"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AE11" s="53" t="e" cm="1">
         <f t="array" ref="AE11">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.4. ACCÈS AU DROIT ET À LA JUSTICE",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JE";"VPE";"1VPE"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AF11" s="53" t="e" cm="1">
         <f t="array" ref="AF11">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.4. ACCÈS AU DROIT ET À LA JUSTICE",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"VPLD";"1VPLD"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AG11" s="59" t="e">
@@ -32333,11 +32333,11 @@
       <c r="AQ11" s="62"/>
       <c r="AR11" s="62"/>
       <c r="AS11" s="62"/>
-      <c r="AT11" s="53" t="e" cm="1">
-        <f t="array" ref="AT11">SUM(SUMIFS(
+      <c r="AT11" s="53" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.4. ACCÈS AU DROIT ET À LA JUSTICE",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat SIEGE NS",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AU11" s="46" t="e">
@@ -32374,15 +32374,15 @@
       <c r="F12" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="G12" s="101" t="e" cm="1">
-        <f t="array" ref="G12">SUM(SUMIFS(
+      <c r="G12" s="101" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire CTECH",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))-
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire CTECH",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="H12" s="59" t="e">
@@ -32402,15 +32402,15 @@
       <c r="S12" s="62"/>
       <c r="T12" s="62"/>
       <c r="U12" s="62"/>
-      <c r="V12" s="53" t="e" cm="1">
-        <f t="array" ref="V12">SUM(SUMIFS(
+      <c r="V12" s="53" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))-
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="W12" s="46" t="e">
@@ -32422,22 +32422,22 @@
         <f t="array" ref="Y12">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JCP";"VPCP";"1VPCP"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))-
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JCP";"VPCP";"1VPCP"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="Z12" s="53" t="e" cm="1">
         <f t="array" ref="Z12">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JI";"VPI";"1VPI"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))-
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JI";"VPI";"1VPI"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AA12" s="62"/>
@@ -32447,33 +32447,33 @@
         <f t="array" ref="AD12">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JAP";"VPAP";"1VPAP"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))-
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JAP";"VPAP";"1VPAP"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AE12" s="53" t="e" cm="1">
         <f t="array" ref="AE12">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JE";"VPE";"1VPE"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))-
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JE";"VPE";"1VPE"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AF12" s="53" t="e" cm="1">
         <f t="array" ref="AF12">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"VPLD";"1VPLD"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))-
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"VPLD";"1VPLD"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AG12" s="46" t="e">
@@ -32492,15 +32492,15 @@
       <c r="AQ12" s="62"/>
       <c r="AR12" s="62"/>
       <c r="AS12" s="62"/>
-      <c r="AT12" s="53" t="e" cm="1">
-        <f t="array" ref="AT12">SUM(SUMIFS(
+      <c r="AT12" s="53" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat SIEGE NS",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))-
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat SIEGE NS",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AU12" s="46" t="e">
@@ -32537,15 +32537,15 @@
       <c r="F13" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="G13" s="101" t="e" cm="1">
-        <f t="array" ref="G13">SUM(SUMIFS(
+      <c r="G13" s="101" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire CTECH",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("13. TOTAL CONTENTIEUX LOCAUX SPÉCIFIQUES",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire CTECH",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="H13" s="59" t="e">
@@ -32565,15 +32565,15 @@
       <c r="S13" s="62"/>
       <c r="T13" s="62"/>
       <c r="U13" s="62"/>
-      <c r="V13" s="53" t="e" cm="1">
-        <f t="array" ref="V13">SUM(SUMIFS(
+      <c r="V13" s="53" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("13. TOTAL CONTENTIEUX LOCAUX SPÉCIFIQUES",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="W13" s="46" t="e">
@@ -32585,14 +32585,14 @@
         <f t="array" ref="Y13">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JCP";"VPCP";"1VPCP"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="Z13" s="53" t="e" cm="1">
         <f t="array" ref="Z13">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JI";"VPI";"1VPI"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AA13" s="62"/>
@@ -32602,21 +32602,21 @@
         <f t="array" ref="AD13">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JAP";"VPAP";"1VPAP"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AE13" s="53" t="e" cm="1">
         <f t="array" ref="AE13">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JE";"VPE";"1VPE"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AF13" s="53" t="e" cm="1">
         <f t="array" ref="AF13">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"VPLD";"1VPLD"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AG13" s="46" t="e">
@@ -32634,22 +32634,22 @@
       <c r="AP13" s="62"/>
       <c r="AQ13" s="62"/>
       <c r="AR13" s="62"/>
-      <c r="AS13" s="53" t="e" cm="1">
-        <f t="array" ref="AS13">SUM(SUMIFS(
+      <c r="AS13" s="53" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("13. TOTAL CONTENTIEUX LOCAUX SPÉCIFIQUES",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat SIEGE S",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AT13" s="53" t="e" cm="1">
-        <f t="array" ref="AT13">SUM(SUMIFS(
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AT13" s="53" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat SIEGE NS",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("13. TOTAL CONTENTIEUX LOCAUX SPÉCIFIQUES",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat SIEGE NS",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AU13" s="46" t="e">
@@ -32686,22 +32686,22 @@
       <c r="F14" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="G14" s="101" t="e" cm="1">
-        <f t="array" ref="G14">SUM(SUMIFS(
+      <c r="G14" s="101" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Temps ventilés sur la période (hors action 99)",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire CTECH placé ADD",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="H14" s="59" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="I14" s="58" t="e" cm="1">
-        <f t="array" ref="I14">SUM(SUMIFS(
+      <c r="I14" s="58" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.8. FONCTIONNAIRES AFFECTÉS AUX ACTIVITÉS CIVILES ET COMMERCIALES DU PARQUET",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR placé ADD",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="J14" s="58" t="e">
@@ -32748,30 +32748,30 @@
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Jirs",'ETPT Format DDG'!2:2,0)),""))</f>
         <v>#N/A</v>
       </c>
-      <c r="P14" s="58" t="e" cm="1">
-        <f t="array" ref="P14">SUM(SUMIFS(
+      <c r="P14" s="58" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3.2. PROTECTION DES MAJEURS",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR placé ADD",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q14" s="58" t="e" cm="1">
-        <f t="array" ref="Q14">SUM(SUMIFS(
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q14" s="58" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3. TOTAL CONTENTIEUX DE LA PROTECTION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR placé ADD",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))-
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3.2. PROTECTION DES MAJEURS",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR placé ADD",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))-
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3.43. INJONCTIONS DE PAYER",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR placé ADD",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))-
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3.44. SAISIE DES RÉMUNÉRATIONS",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR placé ADD",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="R14" s="58" t="e">
@@ -32792,52 +32792,52 @@
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR placé ADD"))</f>
         <v>#N/A</v>
       </c>
-      <c r="S14" s="58" t="e" cm="1">
-        <f t="array" ref="S14">SUM(SUMIFS(
+      <c r="S14" s="58" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3.43. INJONCTIONS DE PAYER",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR placé ADD",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3.44. SAISIE DES RÉMUNÉRATIONS",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR placé ADD",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="T14" s="58" t="e" cm="1">
-        <f t="array" ref="T14">SUM(SUMIFS(
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="T14" s="58" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("4.0. CONTENTIEUX GÉNÉRAL &lt;10.000€",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR placé ADD",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="U14" s="58" t="e" cm="1">
-        <f t="array" ref="U14">SUM(SUMIFS(
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U14" s="58" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("1. TOTAL CONTENTIEUX SOCIAL",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR placé ADD",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="V14" s="53" t="e" cm="1">
-        <f t="array" ref="V14">SUM(SUMIFS(
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="V14" s="53" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("2. TOTAL CONTENTIEUX JAF",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR placé ADD",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("4. TOTAL CIVIL NON SPÉCIALISÉ",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR placé ADD",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("6.1. ACTIVITÉ CIVILE",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR placé ADD",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("13. TOTAL CONTENTIEUX LOCAUX SPÉCIFIQUES",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR placé ADD",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))-
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("4.0. CONTENTIEUX GÉNÉRAL &lt;10.000€",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR placé ADD",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("7.1. COLLÉGIALES HORS JIRS",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR placé ADD")+
@@ -32877,30 +32877,30 @@
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="X14" s="53" t="e" cm="1">
-        <f t="array" ref="X14">SUM(SUMIFS(
+      <c r="X14" s="53" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3.2. PROTECTION DES MAJEURS",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat placé ADD",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Y14" s="53" t="e" cm="1">
-        <f t="array" ref="Y14">SUM(SUMIFS(
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Y14" s="53" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3. TOTAL CONTENTIEUX DE LA PROTECTION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat placé ADD",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))-
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3.2. PROTECTION DES MAJEURS",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat placé ADD",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))-
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3.43. INJONCTIONS DE PAYER",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat placé ADD",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))-
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3.44. SAISIE DES RÉMUNÉRATIONS",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat placé ADD",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="Z14" s="53" t="e">
@@ -33005,40 +33005,40 @@
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat placé ADD"))</f>
         <v>#N/A</v>
       </c>
-      <c r="AN14" s="53" t="e" cm="1">
-        <f t="array" ref="AN14">SUM(SUMIFS(
+      <c r="AN14" s="53" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("1.1. DÉPARTAGE PRUD'HOMAL",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat placé ADD",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AO14" s="53" t="e" cm="1">
-        <f t="array" ref="AO14">SUM(SUMIFS(
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AO14" s="53" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("4.0. CONTENTIEUX GÉNÉRAL &lt;10.000€",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat placé ADD",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AP14" s="53" t="e" cm="1">
-        <f t="array" ref="AP14">SUM(SUMIFS(
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AP14" s="53" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3.43. INJONCTIONS DE PAYER",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat placé ADD",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3.44. SAISIE DES RÉMUNÉRATIONS",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat placé ADD",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AQ14" s="53" t="e" cm="1">
-        <f t="array" ref="AQ14">SUM(SUMIFS(
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AQ14" s="53" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("1. TOTAL CONTENTIEUX SOCIAL",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat placé ADD",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))-
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("1.1. DÉPARTAGE PRUD'HOMAL",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat placé ADD",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AR14" s="53" t="e">
@@ -33048,15 +33048,15 @@
         <v>#N/A</v>
       </c>
       <c r="AS14" s="54"/>
-      <c r="AT14" s="53" t="e" cm="1">
-        <f t="array" ref="AT14">SUM(SUMIFS(
+      <c r="AT14" s="53" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("4. TOTAL CIVIL NON SPÉCIALISÉ",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat placé ADD",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))-
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("4.0. CONTENTIEUX GÉNÉRAL &lt;10.000€",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat placé ADD",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("7.1. COLLÉGIALES HORS JIRS",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat placé ADD")+
@@ -33117,22 +33117,22 @@
       <c r="F15" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="G15" s="101" t="e" cm="1">
-        <f t="array" ref="G15">SUM(SUMIFS(
+      <c r="G15" s="101" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Temps ventilés sur la période (hors action 99)",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire CTECH placé SUB",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="H15" s="59" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="I15" s="58" t="e" cm="1">
-        <f t="array" ref="I15">SUM(SUMIFS(
+      <c r="I15" s="58" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.8. FONCTIONNAIRES AFFECTÉS AUX ACTIVITÉS CIVILES ET COMMERCIALES DU PARQUET",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR placé SUB",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="J15" s="58" t="e">
@@ -33179,30 +33179,30 @@
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Jirs",'ETPT Format DDG'!2:2,0)),""))</f>
         <v>#N/A</v>
       </c>
-      <c r="P15" s="58" t="e" cm="1">
-        <f t="array" ref="P15">SUM(SUMIFS(
+      <c r="P15" s="58" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3.2. PROTECTION DES MAJEURS",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR placé SUB",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q15" s="58" t="e" cm="1">
-        <f t="array" ref="Q15">SUM(SUMIFS(
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q15" s="58" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3. TOTAL CONTENTIEUX DE LA PROTECTION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR placé SUB",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))-
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3.2. PROTECTION DES MAJEURS",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR placé SUB",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))-
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3.43. INJONCTIONS DE PAYER",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR placé SUB",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))-
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3.44. SAISIE DES RÉMUNÉRATIONS",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR placé SUB",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="R15" s="58" t="e">
@@ -33223,52 +33223,52 @@
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR placé SUB"))</f>
         <v>#N/A</v>
       </c>
-      <c r="S15" s="58" t="e" cm="1">
-        <f t="array" ref="S15">SUM(SUMIFS(
+      <c r="S15" s="58" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3.43. INJONCTIONS DE PAYER",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR placé SUB",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3.44. SAISIE DES RÉMUNÉRATIONS",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR placé SUB",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="T15" s="58" t="e" cm="1">
-        <f t="array" ref="T15">SUM(SUMIFS(
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="T15" s="58" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("4.0. CONTENTIEUX GÉNÉRAL &lt;10.000€",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR placé SUB",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="U15" s="58" t="e" cm="1">
-        <f t="array" ref="U15">SUM(SUMIFS(
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U15" s="58" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("1. TOTAL CONTENTIEUX SOCIAL",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR placé SUB",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="V15" s="53" t="e" cm="1">
-        <f t="array" ref="V15">SUM(SUMIFS(
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="V15" s="53" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("2. TOTAL CONTENTIEUX JAF",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR placé SUB",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("4. TOTAL CIVIL NON SPÉCIALISÉ",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR placé SUB",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("6.1. ACTIVITÉ CIVILE",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR placé SUB",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("13. TOTAL CONTENTIEUX LOCAUX SPÉCIFIQUES",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR placé SUB",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))-
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("4.0. CONTENTIEUX GÉNÉRAL &lt;10.000€",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR placé SUB",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("7.1. COLLÉGIALES HORS JIRS",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR placé SUB")+
@@ -33308,30 +33308,30 @@
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="X15" s="53" t="e" cm="1">
-        <f t="array" ref="X15">SUM(SUMIFS(
+      <c r="X15" s="53" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3.2. PROTECTION DES MAJEURS",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat placé SUB",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Y15" s="53" t="e" cm="1">
-        <f t="array" ref="Y15">SUM(SUMIFS(
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Y15" s="53" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3. TOTAL CONTENTIEUX DE LA PROTECTION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat placé SUB",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))-
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3.2. PROTECTION DES MAJEURS",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat placé SUB",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))-
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3.43. INJONCTIONS DE PAYER",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat placé SUB",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))-
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3.44. SAISIE DES RÉMUNÉRATIONS",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat placé SUB",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="Z15" s="53" t="e">
@@ -33436,40 +33436,40 @@
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat placé SUB"))</f>
         <v>#N/A</v>
       </c>
-      <c r="AN15" s="53" t="e" cm="1">
-        <f t="array" ref="AN15">SUM(SUMIFS(
+      <c r="AN15" s="53" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("1.1. DÉPARTAGE PRUD'HOMAL",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat placé SUB",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AO15" s="53" t="e" cm="1">
-        <f t="array" ref="AO15">SUM(SUMIFS(
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AO15" s="53" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("4.0. CONTENTIEUX GÉNÉRAL &lt;10.000€",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat placé SUB",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AP15" s="53" t="e" cm="1">
-        <f t="array" ref="AP15">SUM(SUMIFS(
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AP15" s="53" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3.43. INJONCTIONS DE PAYER",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat placé SUB",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3.44. SAISIE DES RÉMUNÉRATIONS",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat placé SUB",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AQ15" s="53" t="e" cm="1">
-        <f t="array" ref="AQ15">SUM(SUMIFS(
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AQ15" s="53" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("1. TOTAL CONTENTIEUX SOCIAL",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat placé SUB",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))-
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("1.1. DÉPARTAGE PRUD'HOMAL",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat placé SUB",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AR15" s="53" t="e">
@@ -33479,15 +33479,15 @@
         <v>#N/A</v>
       </c>
       <c r="AS15" s="54"/>
-      <c r="AT15" s="53" t="e" cm="1">
-        <f t="array" ref="AT15">SUM(SUMIFS(
+      <c r="AT15" s="53" t="e">
+        <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("4. TOTAL CIVIL NON SPÉCIALISÉ",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat placé SUB",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))-
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("4.0. CONTENTIEUX GÉNÉRAL &lt;10.000€",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat placé SUB",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))+
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))+
 SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("7.1. COLLÉGIALES HORS JIRS",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat placé SUB")+
@@ -33823,7 +33823,7 @@
         <f t="array" ref="G20">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"Fonctionnaire CTECH placé ADD";"Fonctionnaire CTECH placé SUB"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="U20" s="250" t="s">
@@ -33833,7 +33833,7 @@
         <f t="array" ref="V20">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"Fonctionnaire A-B-CBUR placé ADD";"Fonctionnaire A-B-CBUR placé SUB"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="W20" s="38"/>
@@ -33844,7 +33844,7 @@
         <f t="array" ref="AT20">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"Magistrat placé ADD";"Magistrat placé SUB"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),TJCPH))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
         <v>#N/A</v>
       </c>
       <c r="AU20" s="38"/>
@@ -33896,16 +33896,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A1" s="388" t="s">
+      <c r="A1" s="404" t="s">
         <v>214</v>
       </c>
-      <c r="B1" s="388"/>
-      <c r="C1" s="388"/>
-      <c r="D1" s="388"/>
-      <c r="E1" s="388"/>
-      <c r="F1" s="388"/>
-      <c r="G1" s="388"/>
-      <c r="H1" s="388"/>
+      <c r="B1" s="404"/>
+      <c r="C1" s="404"/>
+      <c r="D1" s="404"/>
+      <c r="E1" s="404"/>
+      <c r="F1" s="404"/>
+      <c r="G1" s="404"/>
+      <c r="H1" s="404"/>
       <c r="I1" s="41"/>
       <c r="J1" s="41"/>
       <c r="K1" s="41"/>
@@ -33942,7 +33942,7 @@
       <c r="G2" s="75" t="s">
         <v>169</v>
       </c>
-      <c r="H2" s="386" t="s">
+      <c r="H2" s="402" t="s">
         <v>168</v>
       </c>
       <c r="I2" s="75" t="s">
@@ -33975,7 +33975,7 @@
       <c r="R2" s="75" t="s">
         <v>167</v>
       </c>
-      <c r="S2" s="386" t="s">
+      <c r="S2" s="402" t="s">
         <v>166</v>
       </c>
       <c r="T2" s="75" t="s">
@@ -34005,7 +34005,7 @@
       <c r="AB2" s="75" t="s">
         <v>164</v>
       </c>
-      <c r="AC2" s="386" t="s">
+      <c r="AC2" s="402" t="s">
         <v>213</v>
       </c>
       <c r="AD2" s="75" t="s">
@@ -34017,7 +34017,7 @@
       <c r="AF2" s="75" t="s">
         <v>212</v>
       </c>
-      <c r="AG2" s="386" t="s">
+      <c r="AG2" s="402" t="s">
         <v>211</v>
       </c>
     </row>
@@ -34031,7 +34031,7 @@
       <c r="G3" s="75" t="s">
         <v>158</v>
       </c>
-      <c r="H3" s="386"/>
+      <c r="H3" s="402"/>
       <c r="I3" s="75" t="s">
         <v>210</v>
       </c>
@@ -34062,7 +34062,7 @@
       <c r="R3" s="75" t="s">
         <v>145</v>
       </c>
-      <c r="S3" s="386"/>
+      <c r="S3" s="402"/>
       <c r="T3" s="75" t="s">
         <v>201</v>
       </c>
@@ -34090,7 +34090,7 @@
       <c r="AB3" s="75" t="s">
         <v>193</v>
       </c>
-      <c r="AC3" s="386"/>
+      <c r="AC3" s="402"/>
       <c r="AD3" s="75" t="s">
         <v>192</v>
       </c>
@@ -34100,7 +34100,7 @@
       <c r="AF3" s="75" t="s">
         <v>122</v>
       </c>
-      <c r="AG3" s="386"/>
+      <c r="AG3" s="402"/>
     </row>
     <row r="4" spans="1:33" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="78"/>
@@ -34122,7 +34122,7 @@
       <c r="G4" s="75" t="s">
         <v>108</v>
       </c>
-      <c r="H4" s="386"/>
+      <c r="H4" s="402"/>
       <c r="I4" s="75" t="s">
         <v>191</v>
       </c>
@@ -34153,7 +34153,7 @@
       <c r="R4" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="S4" s="386"/>
+      <c r="S4" s="402"/>
       <c r="T4" s="75" t="s">
         <v>182</v>
       </c>
@@ -34181,7 +34181,7 @@
       <c r="AB4" s="75" t="s">
         <v>174</v>
       </c>
-      <c r="AC4" s="386"/>
+      <c r="AC4" s="402"/>
       <c r="AD4" s="75" t="s">
         <v>173</v>
       </c>
@@ -34191,7 +34191,7 @@
       <c r="AF4" s="75" t="s">
         <v>72</v>
       </c>
-      <c r="AG4" s="386"/>
+      <c r="AG4" s="402"/>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A5" s="81" t="s">
@@ -35566,13 +35566,13 @@
       <c r="G2" s="75" t="s">
         <v>167</v>
       </c>
-      <c r="H2" s="386" t="s">
+      <c r="H2" s="402" t="s">
         <v>166</v>
       </c>
       <c r="I2" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="386" t="s">
+      <c r="J2" s="402" t="s">
         <v>165</v>
       </c>
     </row>
@@ -35586,11 +35586,11 @@
       <c r="G3" s="75" t="s">
         <v>145</v>
       </c>
-      <c r="H3" s="386"/>
+      <c r="H3" s="402"/>
       <c r="I3" s="75" t="s">
         <v>142</v>
       </c>
-      <c r="J3" s="386"/>
+      <c r="J3" s="402"/>
     </row>
     <row r="4" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A4" s="97"/>
@@ -35612,11 +35612,11 @@
       <c r="G4" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="H4" s="386"/>
+      <c r="H4" s="402"/>
       <c r="I4" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="J4" s="386"/>
+      <c r="J4" s="402"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="91" t="s">
@@ -35926,7 +35926,7 @@
   <dimension ref="A1:BJ145"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -36042,7 +36042,7 @@
       <c r="P2" s="277" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="389" t="s">
+      <c r="Q2" s="405" t="s">
         <v>271</v>
       </c>
     </row>
@@ -36083,7 +36083,7 @@
       <c r="P3" s="277" t="s">
         <v>278</v>
       </c>
-      <c r="Q3" s="389"/>
+      <c r="Q3" s="405"/>
     </row>
     <row r="4" spans="1:62" ht="36" x14ac:dyDescent="0.2">
       <c r="A4" s="278"/>
@@ -36102,37 +36102,37 @@
       <c r="F4" s="355" t="s">
         <v>109</v>
       </c>
-      <c r="G4" s="408" t="s">
+      <c r="G4" s="360" t="s">
         <v>614</v>
       </c>
-      <c r="H4" s="408" t="s">
+      <c r="H4" s="360" t="s">
         <v>615</v>
       </c>
-      <c r="I4" s="408" t="s">
+      <c r="I4" s="360" t="s">
         <v>616</v>
       </c>
-      <c r="J4" s="408" t="s">
+      <c r="J4" s="360" t="s">
         <v>93</v>
       </c>
-      <c r="K4" s="408" t="s">
+      <c r="K4" s="360" t="s">
         <v>617</v>
       </c>
-      <c r="L4" s="408" t="s">
+      <c r="L4" s="360" t="s">
         <v>618</v>
       </c>
-      <c r="M4" s="408" t="s">
+      <c r="M4" s="360" t="s">
         <v>619</v>
       </c>
-      <c r="N4" s="408" t="s">
+      <c r="N4" s="360" t="s">
         <v>620</v>
       </c>
-      <c r="O4" s="408" t="s">
+      <c r="O4" s="360" t="s">
         <v>621</v>
       </c>
-      <c r="P4" s="408" t="s">
+      <c r="P4" s="360" t="s">
         <v>622</v>
       </c>
-      <c r="Q4" s="389"/>
+      <c r="Q4" s="405"/>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A5" s="281" t="s">
@@ -37110,7 +37110,7 @@
       <c r="F17" s="291"/>
       <c r="G17" s="291"/>
       <c r="H17" s="291"/>
-      <c r="I17" s="413" t="s">
+      <c r="I17" s="365" t="s">
         <v>626</v>
       </c>
       <c r="J17" s="290"/>
@@ -37131,7 +37131,7 @@
       <c r="F18" s="291"/>
       <c r="G18" s="291"/>
       <c r="H18" s="291"/>
-      <c r="I18" s="413" t="s">
+      <c r="I18" s="365" t="s">
         <v>627</v>
       </c>
       <c r="J18" s="290"/>

</xml_diff>

<commit_message>
update gaps condition for TJ extractor
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1408546-923B-464B-9BAC-DB85FD1D9A2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9A3B61-4C4A-7C4E-91AA-DFD07D02FBFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
@@ -3626,21 +3626,6 @@
     <t>ETPT_ATTACHES_JUSTICE_DDG</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">                  Extracteur de données d'effectifs - Format DDG (avec réintégration de l'absentéisme)
-                  </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Corps)"/>
-      </rPr>
-      <t>Les lignes en rouge invitent à des vérifications dans les colonnes Q, R et S</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">                     Agrégats DDG</t>
   </si>
   <si>
@@ -13482,6 +13467,21 @@
   </si>
   <si>
     <t xml:space="preserve">                 DÉCLARATION ETPT TJ</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                  Extracteur de données d'effectifs - Format DDG (avec réintégration de l'absentéisme)
+                  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Corps)"/>
+      </rPr>
+      <t>Les lignes en rouge invitent à des vérifications dans les colonnes R, S et T</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -16255,6 +16255,26 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <fgColor theme="5" tint="0.79998168889431442"/>
@@ -16273,26 +16293,6 @@
       <font>
         <color theme="0"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -17450,7 +17450,7 @@
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
       <c r="D1" s="3" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="E1" s="7"/>
       <c r="F1" s="6"/>
@@ -17845,7 +17845,7 @@
         <v>106</v>
       </c>
       <c r="K4" s="74" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="L4" s="74" t="s">
         <v>104</v>
@@ -17910,7 +17910,7 @@
       </c>
       <c r="AG4" s="402"/>
       <c r="AH4" s="73" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="AI4" s="73" t="s">
         <v>83</v>
@@ -17956,16 +17956,16 @@
         <v>70</v>
       </c>
       <c r="AX4" s="72" t="s">
+        <v>608</v>
+      </c>
+      <c r="AY4" s="72" t="s">
         <v>609</v>
       </c>
-      <c r="AY4" s="72" t="s">
+      <c r="AZ4" s="72" t="s">
         <v>610</v>
       </c>
-      <c r="AZ4" s="72" t="s">
+      <c r="BA4" s="72" t="s">
         <v>611</v>
-      </c>
-      <c r="BA4" s="72" t="s">
-        <v>612</v>
       </c>
       <c r="BB4" s="72" t="s">
         <v>65</v>
@@ -20572,7 +20572,7 @@
     </row>
     <row r="22" spans="4:57" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E22" s="406" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F22" s="407"/>
       <c r="G22" s="407"/>
@@ -20635,7 +20635,7 @@
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
       <c r="D1" s="3" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="E1" s="7"/>
       <c r="F1" s="6"/>
@@ -20735,7 +20735,7 @@
         <v>183</v>
       </c>
       <c r="R2" s="360" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="S2" s="359" t="s">
         <v>166</v>
@@ -20747,7 +20747,7 @@
         <v>181</v>
       </c>
       <c r="V2" s="360" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="W2" s="360" t="s">
         <v>179</v>
@@ -20771,7 +20771,7 @@
         <v>213</v>
       </c>
       <c r="AD2" s="360" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="AE2" s="360" t="s">
         <v>78</v>
@@ -20824,7 +20824,7 @@
         <v>183</v>
       </c>
       <c r="R3" s="360" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="S3" s="359" t="s">
         <v>166</v>
@@ -20836,7 +20836,7 @@
         <v>181</v>
       </c>
       <c r="V3" s="360" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="W3" s="360" t="s">
         <v>179</v>
@@ -20860,7 +20860,7 @@
         <v>213</v>
       </c>
       <c r="AD3" s="360" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="AE3" s="360" t="s">
         <v>78</v>
@@ -20923,7 +20923,7 @@
         <v>183</v>
       </c>
       <c r="R4" s="360" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="S4" s="359" t="s">
         <v>166</v>
@@ -20935,7 +20935,7 @@
         <v>181</v>
       </c>
       <c r="V4" s="360" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="W4" s="360" t="s">
         <v>179</v>
@@ -20959,7 +20959,7 @@
         <v>213</v>
       </c>
       <c r="AD4" s="360" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="AE4" s="360" t="s">
         <v>78</v>
@@ -22553,7 +22553,7 @@
     </row>
     <row r="21" spans="4:33" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E21" s="409" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F21" s="410"/>
       <c r="G21" s="410"/>
@@ -22616,7 +22616,7 @@
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
       <c r="D1" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="E1" s="7"/>
       <c r="F1" s="6"/>
@@ -22978,7 +22978,7 @@
     </row>
     <row r="17" spans="4:10" ht="99" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D17" s="412" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E17" s="413"/>
       <c r="F17" s="413"/>
@@ -23021,7 +23021,7 @@
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
       <c r="D1" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E1" s="7"/>
       <c r="F1" s="6"/>
@@ -23180,34 +23180,34 @@
         <v>109</v>
       </c>
       <c r="G4" s="360" t="s">
+        <v>613</v>
+      </c>
+      <c r="H4" s="360" t="s">
         <v>614</v>
       </c>
-      <c r="H4" s="360" t="s">
+      <c r="I4" s="360" t="s">
         <v>615</v>
-      </c>
-      <c r="I4" s="360" t="s">
-        <v>616</v>
       </c>
       <c r="J4" s="360" t="s">
         <v>93</v>
       </c>
       <c r="K4" s="360" t="s">
+        <v>616</v>
+      </c>
+      <c r="L4" s="360" t="s">
         <v>617</v>
       </c>
-      <c r="L4" s="360" t="s">
+      <c r="M4" s="360" t="s">
         <v>618</v>
       </c>
-      <c r="M4" s="360" t="s">
+      <c r="N4" s="360" t="s">
         <v>619</v>
       </c>
-      <c r="N4" s="360" t="s">
+      <c r="O4" s="360" t="s">
         <v>620</v>
       </c>
-      <c r="O4" s="360" t="s">
+      <c r="P4" s="360" t="s">
         <v>621</v>
-      </c>
-      <c r="P4" s="360" t="s">
-        <v>622</v>
       </c>
       <c r="Q4" s="405"/>
     </row>
@@ -24485,10 +24485,10 @@
         <v>61</v>
       </c>
       <c r="G5" s="152" t="s">
+        <v>494</v>
+      </c>
+      <c r="H5" s="152" t="s">
         <v>495</v>
-      </c>
-      <c r="H5" s="152" t="s">
-        <v>496</v>
       </c>
       <c r="I5" s="154"/>
       <c r="J5" s="154"/>
@@ -24496,10 +24496,10 @@
       <c r="L5" s="154"/>
       <c r="M5" s="155"/>
       <c r="N5" s="152" t="s">
+        <v>496</v>
+      </c>
+      <c r="O5" s="152" t="s">
         <v>497</v>
-      </c>
-      <c r="O5" s="152" t="s">
-        <v>498</v>
       </c>
       <c r="P5" s="153">
         <f>SUMIF($G$2:O$2,O$2,$G5:O5)</f>
@@ -24512,25 +24512,25 @@
       <c r="U5" s="154"/>
       <c r="V5" s="154"/>
       <c r="W5" s="325" t="s">
+        <v>498</v>
+      </c>
+      <c r="X5" s="325" t="s">
         <v>499</v>
       </c>
-      <c r="X5" s="325" t="s">
+      <c r="Y5" s="325" t="s">
         <v>500</v>
       </c>
-      <c r="Y5" s="325" t="s">
+      <c r="Z5" s="325" t="s">
         <v>501</v>
       </c>
-      <c r="Z5" s="325" t="s">
+      <c r="AA5" s="325" t="s">
         <v>502</v>
       </c>
-      <c r="AA5" s="325" t="s">
+      <c r="AB5" s="325" t="s">
         <v>503</v>
       </c>
-      <c r="AB5" s="325" t="s">
+      <c r="AC5" s="325" t="s">
         <v>504</v>
-      </c>
-      <c r="AC5" s="325" t="s">
-        <v>505</v>
       </c>
       <c r="AD5" s="153">
         <f>SUMIF($G$2:AC$2,Y$2,$G5:AC5)</f>
@@ -24576,47 +24576,47 @@
       <c r="G6" s="154"/>
       <c r="H6" s="154"/>
       <c r="I6" s="152" t="s">
+        <v>505</v>
+      </c>
+      <c r="J6" s="152" t="s">
         <v>506</v>
       </c>
-      <c r="J6" s="152" t="s">
+      <c r="K6" s="152" t="s">
         <v>507</v>
       </c>
-      <c r="K6" s="152" t="s">
+      <c r="L6" s="341" t="s">
         <v>508</v>
       </c>
-      <c r="L6" s="341" t="s">
+      <c r="M6" s="152" t="s">
         <v>509</v>
       </c>
-      <c r="M6" s="152" t="s">
+      <c r="N6" s="152" t="s">
         <v>510</v>
       </c>
-      <c r="N6" s="152" t="s">
+      <c r="O6" s="152" t="s">
         <v>511</v>
-      </c>
-      <c r="O6" s="152" t="s">
-        <v>512</v>
       </c>
       <c r="P6" s="153">
         <f>SUMIF($G$2:O$2,O$2,$G6:O6)</f>
         <v>0</v>
       </c>
       <c r="Q6" s="325" t="s">
+        <v>512</v>
+      </c>
+      <c r="R6" s="325" t="s">
         <v>513</v>
       </c>
-      <c r="R6" s="325" t="s">
+      <c r="S6" s="342" t="s">
         <v>514</v>
       </c>
-      <c r="S6" s="342" t="s">
+      <c r="T6" s="325" t="s">
         <v>515</v>
       </c>
-      <c r="T6" s="325" t="s">
+      <c r="U6" s="343" t="s">
         <v>516</v>
       </c>
-      <c r="U6" s="343" t="s">
+      <c r="V6" s="325" t="s">
         <v>517</v>
-      </c>
-      <c r="V6" s="325" t="s">
-        <v>518</v>
       </c>
       <c r="W6" s="154"/>
       <c r="X6" s="154"/>
@@ -24624,10 +24624,10 @@
       <c r="Z6" s="154"/>
       <c r="AA6" s="154"/>
       <c r="AB6" s="325" t="s">
+        <v>518</v>
+      </c>
+      <c r="AC6" s="325" t="s">
         <v>519</v>
-      </c>
-      <c r="AC6" s="325" t="s">
-        <v>520</v>
       </c>
       <c r="AD6" s="153">
         <f>SUMIF($G$2:AC$2,Y$2,$G6:AC6)</f>
@@ -24672,22 +24672,22 @@
       </c>
       <c r="G7" s="158"/>
       <c r="H7" s="152" t="s">
+        <v>520</v>
+      </c>
+      <c r="I7" s="152" t="s">
         <v>521</v>
-      </c>
-      <c r="I7" s="152" t="s">
-        <v>522</v>
       </c>
       <c r="J7" s="158"/>
       <c r="K7" s="158"/>
       <c r="L7" s="158"/>
       <c r="M7" s="152" t="s">
+        <v>522</v>
+      </c>
+      <c r="N7" s="152" t="s">
         <v>523</v>
       </c>
-      <c r="N7" s="152" t="s">
+      <c r="O7" s="152" t="s">
         <v>524</v>
-      </c>
-      <c r="O7" s="152" t="s">
-        <v>525</v>
       </c>
       <c r="P7" s="153">
         <f>SUMIF($G$2:O$2,O$2,$G7:O7)</f>
@@ -24706,7 +24706,7 @@
       <c r="AA7" s="158"/>
       <c r="AB7" s="158"/>
       <c r="AC7" s="152" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="AD7" s="153">
         <f>SUMIF($G$2:AC$2,Y$2,$G7:AC7)</f>
@@ -24751,22 +24751,22 @@
       </c>
       <c r="G8" s="344"/>
       <c r="H8" s="341" t="s">
+        <v>526</v>
+      </c>
+      <c r="I8" s="341" t="s">
         <v>527</v>
-      </c>
-      <c r="I8" s="341" t="s">
-        <v>528</v>
       </c>
       <c r="J8" s="344"/>
       <c r="K8" s="344"/>
       <c r="L8" s="344"/>
       <c r="M8" s="341" t="s">
+        <v>528</v>
+      </c>
+      <c r="N8" s="341" t="s">
         <v>529</v>
       </c>
-      <c r="N8" s="341" t="s">
+      <c r="O8" s="341" t="s">
         <v>530</v>
-      </c>
-      <c r="O8" s="341" t="s">
-        <v>531</v>
       </c>
       <c r="P8" s="153">
         <f>SUMIF($G$2:O$2,O$2,$G8:O8)</f>
@@ -24785,7 +24785,7 @@
       <c r="AA8" s="165"/>
       <c r="AB8" s="165"/>
       <c r="AC8" s="341" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="AD8" s="153">
         <f>SUMIF($G$2:AC$2,Y$2,$G8:AC8)</f>
@@ -24830,22 +24830,22 @@
       </c>
       <c r="G9" s="160"/>
       <c r="H9" s="325" t="s">
+        <v>532</v>
+      </c>
+      <c r="I9" s="325" t="s">
         <v>533</v>
-      </c>
-      <c r="I9" s="325" t="s">
-        <v>534</v>
       </c>
       <c r="J9" s="161"/>
       <c r="K9" s="161"/>
       <c r="L9" s="161"/>
       <c r="M9" s="325" t="s">
+        <v>534</v>
+      </c>
+      <c r="N9" s="325" t="s">
         <v>535</v>
       </c>
-      <c r="N9" s="325" t="s">
+      <c r="O9" s="325" t="s">
         <v>536</v>
-      </c>
-      <c r="O9" s="325" t="s">
-        <v>537</v>
       </c>
       <c r="P9" s="162">
         <f>SUMIF($G$2:O$2,O$2,$G9:O9)</f>
@@ -24864,7 +24864,7 @@
       <c r="AA9" s="158"/>
       <c r="AB9" s="158"/>
       <c r="AC9" s="325" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="AD9" s="153">
         <f>SUMIF($G$2:AC$2,Y$2,$G9:AC9)</f>
@@ -24909,22 +24909,22 @@
       </c>
       <c r="G10" s="160"/>
       <c r="H10" s="152" t="s">
+        <v>538</v>
+      </c>
+      <c r="I10" s="152" t="s">
         <v>539</v>
-      </c>
-      <c r="I10" s="152" t="s">
-        <v>540</v>
       </c>
       <c r="J10" s="161"/>
       <c r="K10" s="161"/>
       <c r="L10" s="161"/>
       <c r="M10" s="152" t="s">
+        <v>540</v>
+      </c>
+      <c r="N10" s="152" t="s">
         <v>541</v>
       </c>
-      <c r="N10" s="152" t="s">
+      <c r="O10" s="152" t="s">
         <v>542</v>
-      </c>
-      <c r="O10" s="152" t="s">
-        <v>543</v>
       </c>
       <c r="P10" s="162">
         <f>SUMIF($G$2:O$2,O$2,$G10:O10)</f>
@@ -24943,7 +24943,7 @@
       <c r="AA10" s="158"/>
       <c r="AB10" s="158"/>
       <c r="AC10" s="152" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="AD10" s="153">
         <f>SUMIF($G$2:AC$2,Y$2,$G10:AC10)</f>
@@ -24988,22 +24988,22 @@
       </c>
       <c r="G11" s="160"/>
       <c r="H11" s="152" t="s">
+        <v>544</v>
+      </c>
+      <c r="I11" s="152" t="s">
         <v>545</v>
-      </c>
-      <c r="I11" s="152" t="s">
-        <v>546</v>
       </c>
       <c r="J11" s="161"/>
       <c r="K11" s="161"/>
       <c r="L11" s="161"/>
       <c r="M11" s="152" t="s">
+        <v>546</v>
+      </c>
+      <c r="N11" s="152" t="s">
         <v>547</v>
       </c>
-      <c r="N11" s="152" t="s">
+      <c r="O11" s="152" t="s">
         <v>548</v>
-      </c>
-      <c r="O11" s="152" t="s">
-        <v>549</v>
       </c>
       <c r="P11" s="162">
         <f>SUMIF($G$2:O$2,O$2,$G11:O11)</f>
@@ -25022,7 +25022,7 @@
       <c r="AA11" s="158"/>
       <c r="AB11" s="158"/>
       <c r="AC11" s="152" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="AD11" s="153">
         <f>SUMIF($G$2:AC$2,Y$2,$G11:AC11)</f>
@@ -25067,22 +25067,22 @@
       </c>
       <c r="G12" s="160"/>
       <c r="H12" s="325" t="s">
+        <v>550</v>
+      </c>
+      <c r="I12" s="325" t="s">
         <v>551</v>
-      </c>
-      <c r="I12" s="325" t="s">
-        <v>552</v>
       </c>
       <c r="J12" s="161"/>
       <c r="K12" s="161"/>
       <c r="L12" s="161"/>
       <c r="M12" s="325" t="s">
+        <v>552</v>
+      </c>
+      <c r="N12" s="325" t="s">
         <v>553</v>
       </c>
-      <c r="N12" s="325" t="s">
+      <c r="O12" s="325" t="s">
         <v>554</v>
-      </c>
-      <c r="O12" s="325" t="s">
-        <v>555</v>
       </c>
       <c r="P12" s="162">
         <f>SUMIF($G$2:O$2,O$2,$G12:O12)</f>
@@ -25101,7 +25101,7 @@
       <c r="AA12" s="158"/>
       <c r="AB12" s="158"/>
       <c r="AC12" s="325" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="AD12" s="153">
         <f>SUMIF($G$2:AC$2,Y$2,$G12:AC12)</f>
@@ -25146,22 +25146,22 @@
       </c>
       <c r="G13" s="163"/>
       <c r="H13" s="325" t="s">
+        <v>556</v>
+      </c>
+      <c r="I13" s="325" t="s">
         <v>557</v>
-      </c>
-      <c r="I13" s="325" t="s">
-        <v>558</v>
       </c>
       <c r="J13" s="161"/>
       <c r="K13" s="161"/>
       <c r="L13" s="161"/>
       <c r="M13" s="325" t="s">
+        <v>558</v>
+      </c>
+      <c r="N13" s="325" t="s">
         <v>559</v>
       </c>
-      <c r="N13" s="325" t="s">
+      <c r="O13" s="325" t="s">
         <v>560</v>
-      </c>
-      <c r="O13" s="325" t="s">
-        <v>561</v>
       </c>
       <c r="P13" s="153">
         <f>SUMIF($G$2:O$2,O$2,$G13:O13)</f>
@@ -25179,10 +25179,10 @@
       <c r="Z13" s="158"/>
       <c r="AA13" s="158"/>
       <c r="AB13" s="325" t="s">
+        <v>561</v>
+      </c>
+      <c r="AC13" s="325" t="s">
         <v>562</v>
-      </c>
-      <c r="AC13" s="325" t="s">
-        <v>563</v>
       </c>
       <c r="AD13" s="153">
         <f>SUMIF($G$2:AC$2,Y$2,$G13:AC13)</f>
@@ -25226,72 +25226,72 @@
         <v>43</v>
       </c>
       <c r="G14" s="152" t="s">
+        <v>563</v>
+      </c>
+      <c r="H14" s="152" t="s">
         <v>564</v>
       </c>
-      <c r="H14" s="152" t="s">
+      <c r="I14" s="152" t="s">
         <v>565</v>
       </c>
-      <c r="I14" s="152" t="s">
+      <c r="J14" s="152" t="s">
         <v>566</v>
       </c>
-      <c r="J14" s="152" t="s">
+      <c r="K14" s="152" t="s">
         <v>567</v>
       </c>
-      <c r="K14" s="152" t="s">
+      <c r="L14" s="341" t="s">
         <v>568</v>
       </c>
-      <c r="L14" s="341" t="s">
+      <c r="M14" s="152" t="s">
         <v>569</v>
       </c>
-      <c r="M14" s="152" t="s">
+      <c r="N14" s="152" t="s">
         <v>570</v>
       </c>
-      <c r="N14" s="152" t="s">
+      <c r="O14" s="152" t="s">
         <v>571</v>
-      </c>
-      <c r="O14" s="152" t="s">
-        <v>572</v>
       </c>
       <c r="P14" s="153">
         <f>SUMIF($G$2:O$2,O$2,$G14:O14)</f>
         <v>0</v>
       </c>
       <c r="Q14" s="325" t="s">
+        <v>572</v>
+      </c>
+      <c r="R14" s="325" t="s">
         <v>573</v>
       </c>
-      <c r="R14" s="325" t="s">
+      <c r="S14" s="342" t="s">
         <v>574</v>
       </c>
-      <c r="S14" s="342" t="s">
+      <c r="T14" s="325" t="s">
         <v>575</v>
       </c>
-      <c r="T14" s="325" t="s">
+      <c r="U14" s="343" t="s">
         <v>576</v>
       </c>
-      <c r="U14" s="343" t="s">
+      <c r="V14" s="325" t="s">
         <v>577</v>
       </c>
-      <c r="V14" s="325" t="s">
+      <c r="W14" s="325" t="s">
         <v>578</v>
       </c>
-      <c r="W14" s="325" t="s">
+      <c r="X14" s="325" t="s">
         <v>579</v>
       </c>
-      <c r="X14" s="325" t="s">
+      <c r="Y14" s="325" t="s">
         <v>580</v>
       </c>
-      <c r="Y14" s="325" t="s">
+      <c r="Z14" s="325" t="s">
         <v>581</v>
       </c>
-      <c r="Z14" s="325" t="s">
+      <c r="AA14" s="325" t="s">
         <v>582</v>
-      </c>
-      <c r="AA14" s="325" t="s">
-        <v>583</v>
       </c>
       <c r="AB14" s="165"/>
       <c r="AC14" s="341" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="AD14" s="153">
         <f>SUMIF($G$2:AC$2,Y$2,$G14:AC14)</f>
@@ -25335,72 +25335,72 @@
         <v>40</v>
       </c>
       <c r="G15" s="152" t="s">
+        <v>584</v>
+      </c>
+      <c r="H15" s="152" t="s">
         <v>585</v>
       </c>
-      <c r="H15" s="152" t="s">
+      <c r="I15" s="152" t="s">
         <v>586</v>
       </c>
-      <c r="I15" s="152" t="s">
+      <c r="J15" s="152" t="s">
         <v>587</v>
       </c>
-      <c r="J15" s="152" t="s">
+      <c r="K15" s="152" t="s">
         <v>588</v>
       </c>
-      <c r="K15" s="152" t="s">
+      <c r="L15" s="341" t="s">
         <v>589</v>
       </c>
-      <c r="L15" s="341" t="s">
+      <c r="M15" s="152" t="s">
         <v>590</v>
       </c>
-      <c r="M15" s="152" t="s">
+      <c r="N15" s="152" t="s">
         <v>591</v>
       </c>
-      <c r="N15" s="152" t="s">
+      <c r="O15" s="152" t="s">
         <v>592</v>
-      </c>
-      <c r="O15" s="152" t="s">
-        <v>593</v>
       </c>
       <c r="P15" s="153">
         <f>SUMIF($G$2:O$2,O$2,$G15:O15)</f>
         <v>0</v>
       </c>
       <c r="Q15" s="325" t="s">
+        <v>593</v>
+      </c>
+      <c r="R15" s="325" t="s">
         <v>594</v>
       </c>
-      <c r="R15" s="325" t="s">
+      <c r="S15" s="342" t="s">
         <v>595</v>
       </c>
-      <c r="S15" s="342" t="s">
+      <c r="T15" s="325" t="s">
         <v>596</v>
       </c>
-      <c r="T15" s="325" t="s">
+      <c r="U15" s="343" t="s">
         <v>597</v>
       </c>
-      <c r="U15" s="343" t="s">
+      <c r="V15" s="325" t="s">
         <v>598</v>
       </c>
-      <c r="V15" s="325" t="s">
+      <c r="W15" s="325" t="s">
         <v>599</v>
       </c>
-      <c r="W15" s="325" t="s">
+      <c r="X15" s="325" t="s">
         <v>600</v>
       </c>
-      <c r="X15" s="325" t="s">
+      <c r="Y15" s="325" t="s">
         <v>601</v>
       </c>
-      <c r="Y15" s="325" t="s">
+      <c r="Z15" s="325" t="s">
         <v>602</v>
       </c>
-      <c r="Z15" s="325" t="s">
+      <c r="AA15" s="325" t="s">
         <v>603</v>
-      </c>
-      <c r="AA15" s="325" t="s">
-        <v>604</v>
       </c>
       <c r="AB15" s="165"/>
       <c r="AC15" s="341" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="AD15" s="153">
         <f>SUMIF($G$2:AC$2,Y$2,$G15:AC15)</f>
@@ -25715,7 +25715,7 @@
         <v>249</v>
       </c>
       <c r="AC19" s="325" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="AD19" s="346"/>
       <c r="AE19" s="251"/>
@@ -26300,37 +26300,37 @@
       </c>
       <c r="G5" s="324"/>
       <c r="H5" s="325" t="s">
+        <v>465</v>
+      </c>
+      <c r="I5" s="325" t="s">
         <v>466</v>
       </c>
-      <c r="I5" s="325" t="s">
+      <c r="J5" s="325" t="s">
         <v>467</v>
       </c>
-      <c r="J5" s="325" t="s">
+      <c r="K5" s="326" t="s">
         <v>468</v>
       </c>
-      <c r="K5" s="326" t="s">
-        <v>469</v>
-      </c>
       <c r="L5" s="326" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="M5" s="177"/>
       <c r="N5" s="177"/>
       <c r="O5" s="326" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P5" s="327">
         <f t="shared" ref="P5:P15" si="0">SUM(G5:O5)</f>
         <v>0</v>
       </c>
       <c r="Q5" s="326" t="s">
+        <v>469</v>
+      </c>
+      <c r="R5" s="325" t="s">
         <v>470</v>
       </c>
-      <c r="R5" s="325" t="s">
+      <c r="S5" s="328" t="s">
         <v>471</v>
-      </c>
-      <c r="S5" s="328" t="s">
-        <v>472</v>
       </c>
       <c r="T5" s="327">
         <f t="shared" ref="T5:T15" si="1">SUM(Q5:S5)</f>
@@ -26357,20 +26357,20 @@
       <c r="K6" s="331"/>
       <c r="L6" s="331"/>
       <c r="M6" s="326" t="s">
+        <v>472</v>
+      </c>
+      <c r="N6" s="326" t="s">
         <v>473</v>
       </c>
-      <c r="N6" s="326" t="s">
-        <v>474</v>
-      </c>
       <c r="O6" s="326" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P6" s="327">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q6" s="326" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="R6" s="331"/>
       <c r="S6" s="177"/>
@@ -26408,7 +26408,7 @@
       <c r="Q7" s="331"/>
       <c r="R7" s="331"/>
       <c r="S7" s="325" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="T7" s="327">
         <f>SUM(Q7:S7)</f>
@@ -26444,7 +26444,7 @@
       <c r="Q8" s="334"/>
       <c r="R8" s="164"/>
       <c r="S8" s="325" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="T8" s="327">
         <f>SUM(Q8:R8)</f>
@@ -26480,7 +26480,7 @@
       <c r="Q9" s="334"/>
       <c r="R9" s="164"/>
       <c r="S9" s="325" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="T9" s="327">
         <f>SUM(Q9:R9)</f>
@@ -26516,7 +26516,7 @@
       <c r="Q10" s="334"/>
       <c r="R10" s="334"/>
       <c r="S10" s="325" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="T10" s="327">
         <f t="shared" si="1"/>
@@ -26552,7 +26552,7 @@
       <c r="Q11" s="334"/>
       <c r="R11" s="164"/>
       <c r="S11" s="325" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="T11" s="327">
         <f>SUM(Q11:R11)</f>
@@ -26588,7 +26588,7 @@
       <c r="Q12" s="334"/>
       <c r="R12" s="334"/>
       <c r="S12" s="325" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="T12" s="327">
         <f t="shared" si="1"/>
@@ -26609,7 +26609,7 @@
         <v>45</v>
       </c>
       <c r="G13" s="335" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="H13" s="334"/>
       <c r="I13" s="334"/>
@@ -26626,7 +26626,7 @@
       <c r="Q13" s="334"/>
       <c r="R13" s="334"/>
       <c r="S13" s="325" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="T13" s="327">
         <f t="shared" si="1"/>
@@ -26648,13 +26648,13 @@
       </c>
       <c r="G14" s="324"/>
       <c r="H14" s="325" t="s">
+        <v>483</v>
+      </c>
+      <c r="I14" s="325" t="s">
         <v>484</v>
       </c>
-      <c r="I14" s="325" t="s">
+      <c r="J14" s="325" t="s">
         <v>485</v>
-      </c>
-      <c r="J14" s="325" t="s">
-        <v>486</v>
       </c>
       <c r="K14" s="336"/>
       <c r="L14" s="336"/>
@@ -26667,10 +26667,10 @@
       </c>
       <c r="Q14" s="331"/>
       <c r="R14" s="325" t="s">
+        <v>486</v>
+      </c>
+      <c r="S14" s="325" t="s">
         <v>487</v>
-      </c>
-      <c r="S14" s="325" t="s">
-        <v>488</v>
       </c>
       <c r="T14" s="327">
         <f t="shared" si="1"/>
@@ -26692,13 +26692,13 @@
       </c>
       <c r="G15" s="324"/>
       <c r="H15" s="325" t="s">
+        <v>488</v>
+      </c>
+      <c r="I15" s="325" t="s">
         <v>489</v>
       </c>
-      <c r="I15" s="325" t="s">
+      <c r="J15" s="325" t="s">
         <v>490</v>
-      </c>
-      <c r="J15" s="325" t="s">
-        <v>491</v>
       </c>
       <c r="K15" s="336"/>
       <c r="L15" s="336"/>
@@ -26711,10 +26711,10 @@
       </c>
       <c r="Q15" s="334"/>
       <c r="R15" s="325" t="s">
+        <v>491</v>
+      </c>
+      <c r="S15" s="325" t="s">
         <v>492</v>
-      </c>
-      <c r="S15" s="325" t="s">
-        <v>493</v>
       </c>
       <c r="T15" s="327">
         <f t="shared" si="1"/>
@@ -26853,7 +26853,7 @@
         <v>249</v>
       </c>
       <c r="S19" s="325" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="T19" s="26"/>
     </row>
@@ -27098,14 +27098,14 @@
         <v>61</v>
       </c>
       <c r="G5" s="313" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="H5" s="190">
         <f>SUMIF($G$2:G$2,G$2,$G5:G5)</f>
         <v>0</v>
       </c>
       <c r="I5" s="307" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="J5" s="191"/>
       <c r="K5" s="192"/>
@@ -27114,25 +27114,25 @@
       <c r="N5" s="192"/>
       <c r="O5" s="192"/>
       <c r="P5" s="307" t="s">
+        <v>405</v>
+      </c>
+      <c r="Q5" s="307" t="s">
         <v>406</v>
       </c>
-      <c r="Q5" s="307" t="s">
+      <c r="R5" s="307" t="s">
         <v>407</v>
       </c>
-      <c r="R5" s="307" t="s">
+      <c r="S5" s="307" t="s">
         <v>408</v>
       </c>
-      <c r="S5" s="307" t="s">
+      <c r="T5" s="307" t="s">
         <v>409</v>
       </c>
-      <c r="T5" s="307" t="s">
+      <c r="U5" s="307" t="s">
         <v>410</v>
       </c>
-      <c r="U5" s="307" t="s">
+      <c r="V5" s="313" t="s">
         <v>411</v>
-      </c>
-      <c r="V5" s="313" t="s">
-        <v>412</v>
       </c>
       <c r="W5" s="190">
         <f>SUMIF($G$2:V$2,V$2,$G5:V5)</f>
@@ -27153,7 +27153,7 @@
         <v>59</v>
       </c>
       <c r="G6" s="307" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="H6" s="190">
         <f>SUMIF($G$2:G$2,G$2,$G6:G6)</f>
@@ -27161,33 +27161,33 @@
       </c>
       <c r="I6" s="191"/>
       <c r="J6" s="307" t="s">
+        <v>413</v>
+      </c>
+      <c r="K6" s="307" t="s">
         <v>414</v>
       </c>
-      <c r="K6" s="307" t="s">
+      <c r="L6" s="307" t="s">
         <v>415</v>
       </c>
-      <c r="L6" s="307" t="s">
+      <c r="M6" s="316" t="s">
         <v>416</v>
       </c>
-      <c r="M6" s="316" t="s">
+      <c r="N6" s="307" t="s">
         <v>417</v>
       </c>
-      <c r="N6" s="307" t="s">
+      <c r="O6" s="317" t="s">
         <v>418</v>
-      </c>
-      <c r="O6" s="317" t="s">
-        <v>419</v>
       </c>
       <c r="P6" s="192"/>
       <c r="Q6" s="192"/>
       <c r="R6" s="307" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="S6" s="192"/>
       <c r="T6" s="192"/>
       <c r="U6" s="192"/>
       <c r="V6" s="318" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="W6" s="190">
         <f>SUMIF($G$2:V$2,V$2,$G6:V6)</f>
@@ -27245,7 +27245,7 @@
         <v>55</v>
       </c>
       <c r="G8" s="307" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H8" s="190">
         <f>SUMIF($G$2:G$2,G$2,$G8:G8)</f>
@@ -27265,7 +27265,7 @@
       <c r="T8" s="194"/>
       <c r="U8" s="194"/>
       <c r="V8" s="307" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="W8" s="190">
         <f>SUMIF($G$2:V$2,V$2,$G8:V8)</f>
@@ -27286,7 +27286,7 @@
         <v>53</v>
       </c>
       <c r="G9" s="307" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H9" s="190">
         <f>SUMIF($G$2:G$2,G$2,$G9:G9)</f>
@@ -27306,7 +27306,7 @@
       <c r="T9" s="194"/>
       <c r="U9" s="194"/>
       <c r="V9" s="313" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="W9" s="190">
         <f>SUMIF($G$2:V$2,V$2,$G9:V9)</f>
@@ -27327,7 +27327,7 @@
         <v>51</v>
       </c>
       <c r="G10" s="307" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H10" s="190">
         <f>SUMIF($G$2:G$2,G$2,$G10:G10)</f>
@@ -27346,7 +27346,7 @@
       <c r="T10" s="194"/>
       <c r="U10" s="194"/>
       <c r="V10" s="307" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="W10" s="190">
         <f>SUMIF($G$2:V$2,V$2,$G10:V10)</f>
@@ -27367,7 +27367,7 @@
         <v>49</v>
       </c>
       <c r="G11" s="307" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H11" s="190">
         <f>SUMIF($G$2:G$2,G$2,$G11:G11)</f>
@@ -27387,7 +27387,7 @@
       <c r="T11" s="194"/>
       <c r="U11" s="194"/>
       <c r="V11" s="307" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="W11" s="190">
         <f>SUMIF($G$2:V$2,V$2,$G11:V11)</f>
@@ -27408,7 +27408,7 @@
         <v>47</v>
       </c>
       <c r="G12" s="307" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H12" s="190">
         <f>SUMIF($G$2:G$2,G$2,$G12:G12)</f>
@@ -27428,7 +27428,7 @@
       <c r="T12" s="194"/>
       <c r="U12" s="194"/>
       <c r="V12" s="307" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="W12" s="190">
         <f>SUMIF($G$2:V$2,V$2,$G12:V12)</f>
@@ -27449,7 +27449,7 @@
         <v>45</v>
       </c>
       <c r="G13" s="313" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H13" s="190">
         <f>SUMIF($G$2:G$2,G$2,$G13:G13)</f>
@@ -27469,7 +27469,7 @@
       <c r="T13" s="194"/>
       <c r="U13" s="194"/>
       <c r="V13" s="313" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="W13" s="190">
         <f>SUMIF($G$2:V$2,V$2,$G13:V13)</f>
@@ -27490,53 +27490,53 @@
         <v>43</v>
       </c>
       <c r="G14" s="307" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H14" s="190">
         <f>SUMIF($G$2:G$2,G$2,$G14:G14)</f>
         <v>0</v>
       </c>
       <c r="I14" s="307" t="s">
+        <v>434</v>
+      </c>
+      <c r="J14" s="313" t="s">
         <v>435</v>
       </c>
-      <c r="J14" s="313" t="s">
+      <c r="K14" s="313" t="s">
         <v>436</v>
       </c>
-      <c r="K14" s="313" t="s">
+      <c r="L14" s="313" t="s">
         <v>437</v>
       </c>
-      <c r="L14" s="313" t="s">
+      <c r="M14" s="316" t="s">
         <v>438</v>
       </c>
-      <c r="M14" s="316" t="s">
+      <c r="N14" s="313" t="s">
         <v>439</v>
       </c>
-      <c r="N14" s="313" t="s">
+      <c r="O14" s="317" t="s">
         <v>440</v>
       </c>
-      <c r="O14" s="317" t="s">
+      <c r="P14" s="307" t="s">
         <v>441</v>
       </c>
-      <c r="P14" s="307" t="s">
+      <c r="Q14" s="307" t="s">
         <v>442</v>
       </c>
-      <c r="Q14" s="307" t="s">
+      <c r="R14" s="313" t="s">
         <v>443</v>
       </c>
-      <c r="R14" s="313" t="s">
+      <c r="S14" s="307" t="s">
         <v>444</v>
       </c>
-      <c r="S14" s="307" t="s">
+      <c r="T14" s="307" t="s">
         <v>445</v>
       </c>
-      <c r="T14" s="307" t="s">
+      <c r="U14" s="307" t="s">
         <v>446</v>
       </c>
-      <c r="U14" s="307" t="s">
+      <c r="V14" s="313" t="s">
         <v>447</v>
-      </c>
-      <c r="V14" s="313" t="s">
-        <v>448</v>
       </c>
       <c r="W14" s="190">
         <f>SUMIF($G$2:V$2,V$2,$G14:V14)</f>
@@ -27557,53 +27557,53 @@
         <v>40</v>
       </c>
       <c r="G15" s="307" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="H15" s="190">
         <f>SUMIF($G$2:G$2,G$2,$G15:G15)</f>
         <v>0</v>
       </c>
       <c r="I15" s="307" t="s">
+        <v>449</v>
+      </c>
+      <c r="J15" s="313" t="s">
         <v>450</v>
       </c>
-      <c r="J15" s="313" t="s">
+      <c r="K15" s="313" t="s">
         <v>451</v>
       </c>
-      <c r="K15" s="313" t="s">
+      <c r="L15" s="313" t="s">
         <v>452</v>
       </c>
-      <c r="L15" s="313" t="s">
+      <c r="M15" s="316" t="s">
         <v>453</v>
       </c>
-      <c r="M15" s="316" t="s">
+      <c r="N15" s="313" t="s">
         <v>454</v>
       </c>
-      <c r="N15" s="313" t="s">
+      <c r="O15" s="317" t="s">
         <v>455</v>
       </c>
-      <c r="O15" s="317" t="s">
+      <c r="P15" s="307" t="s">
         <v>456</v>
       </c>
-      <c r="P15" s="307" t="s">
+      <c r="Q15" s="307" t="s">
         <v>457</v>
       </c>
-      <c r="Q15" s="307" t="s">
+      <c r="R15" s="313" t="s">
         <v>458</v>
       </c>
-      <c r="R15" s="313" t="s">
+      <c r="S15" s="307" t="s">
         <v>459</v>
       </c>
-      <c r="S15" s="307" t="s">
+      <c r="T15" s="307" t="s">
         <v>460</v>
       </c>
-      <c r="T15" s="307" t="s">
+      <c r="U15" s="307" t="s">
         <v>461</v>
       </c>
-      <c r="U15" s="307" t="s">
+      <c r="V15" s="313" t="s">
         <v>462</v>
-      </c>
-      <c r="V15" s="313" t="s">
-        <v>463</v>
       </c>
       <c r="W15" s="190">
         <f>SUMIF($G$2:V$2,V$2,$G15:V15)</f>
@@ -27745,7 +27745,7 @@
         <v>250</v>
       </c>
       <c r="G19" s="307" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="H19" s="254"/>
       <c r="I19" s="254"/>
@@ -27764,7 +27764,7 @@
         <v>251</v>
       </c>
       <c r="V19" s="307" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="W19" s="254"/>
     </row>
@@ -27974,7 +27974,7 @@
         <v>61</v>
       </c>
       <c r="G5" s="307" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="H5" s="228">
         <f t="shared" ref="H5:H15" si="0">SUM(G5)</f>
@@ -27982,27 +27982,27 @@
       </c>
       <c r="I5" s="229"/>
       <c r="J5" s="307" t="s">
+        <v>373</v>
+      </c>
+      <c r="K5" s="307" t="s">
         <v>374</v>
       </c>
-      <c r="K5" s="307" t="s">
+      <c r="L5" s="307" t="s">
         <v>375</v>
       </c>
-      <c r="L5" s="307" t="s">
+      <c r="M5" s="308" t="s">
         <v>376</v>
       </c>
-      <c r="M5" s="308" t="s">
-        <v>377</v>
-      </c>
       <c r="N5" s="308" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="O5" s="309"/>
       <c r="P5" s="309"/>
       <c r="Q5" s="308" t="s">
+        <v>376</v>
+      </c>
+      <c r="R5" s="307" t="s">
         <v>377</v>
-      </c>
-      <c r="R5" s="307" t="s">
-        <v>378</v>
       </c>
       <c r="S5" s="228">
         <f t="shared" ref="S5:S15" si="1">SUM(I5:R5)</f>
@@ -28034,16 +28034,16 @@
       <c r="M6" s="311"/>
       <c r="N6" s="312"/>
       <c r="O6" s="308" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P6" s="308" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="Q6" s="308" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="R6" s="308" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="S6" s="234">
         <f t="shared" si="1"/>
@@ -28097,7 +28097,7 @@
         <v>55</v>
       </c>
       <c r="G8" s="307" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H8" s="228">
         <f t="shared" si="0"/>
@@ -28113,7 +28113,7 @@
       <c r="P8" s="231"/>
       <c r="Q8" s="232"/>
       <c r="R8" s="307" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="S8" s="228">
         <f t="shared" si="1"/>
@@ -28134,7 +28134,7 @@
         <v>53</v>
       </c>
       <c r="G9" s="307" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="H9" s="228">
         <f t="shared" si="0"/>
@@ -28150,7 +28150,7 @@
       <c r="P9" s="231"/>
       <c r="Q9" s="232"/>
       <c r="R9" s="307" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="S9" s="228">
         <f t="shared" si="1"/>
@@ -28171,7 +28171,7 @@
         <v>51</v>
       </c>
       <c r="G10" s="307" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="H10" s="228">
         <f>SUM(G10)</f>
@@ -28187,7 +28187,7 @@
       <c r="P10" s="231"/>
       <c r="Q10" s="232"/>
       <c r="R10" s="307" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="S10" s="228">
         <f t="shared" si="1"/>
@@ -28208,7 +28208,7 @@
         <v>49</v>
       </c>
       <c r="G11" s="307" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="H11" s="228">
         <f>SUM(G11)</f>
@@ -28224,7 +28224,7 @@
       <c r="P11" s="231"/>
       <c r="Q11" s="232"/>
       <c r="R11" s="307" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="S11" s="228">
         <f t="shared" si="1"/>
@@ -28245,7 +28245,7 @@
         <v>47</v>
       </c>
       <c r="G12" s="307" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="H12" s="228">
         <f t="shared" si="0"/>
@@ -28261,7 +28261,7 @@
       <c r="P12" s="231"/>
       <c r="Q12" s="232"/>
       <c r="R12" s="307" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="S12" s="228">
         <f t="shared" si="1"/>
@@ -28282,14 +28282,14 @@
         <v>45</v>
       </c>
       <c r="G13" s="307" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H13" s="228">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I13" s="313" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="J13" s="232"/>
       <c r="K13" s="232"/>
@@ -28300,7 +28300,7 @@
       <c r="P13" s="231"/>
       <c r="Q13" s="232"/>
       <c r="R13" s="307" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="S13" s="228">
         <f t="shared" si="1"/>
@@ -28321,7 +28321,7 @@
         <v>43</v>
       </c>
       <c r="G14" s="307" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="H14" s="228">
         <f t="shared" si="0"/>
@@ -28329,13 +28329,13 @@
       </c>
       <c r="I14" s="229"/>
       <c r="J14" s="307" t="s">
+        <v>392</v>
+      </c>
+      <c r="K14" s="307" t="s">
         <v>393</v>
       </c>
-      <c r="K14" s="307" t="s">
+      <c r="L14" s="307" t="s">
         <v>394</v>
-      </c>
-      <c r="L14" s="307" t="s">
-        <v>395</v>
       </c>
       <c r="M14" s="230"/>
       <c r="N14" s="230"/>
@@ -28343,7 +28343,7 @@
       <c r="P14" s="231"/>
       <c r="Q14" s="232"/>
       <c r="R14" s="307" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="S14" s="228">
         <f t="shared" si="1"/>
@@ -28364,7 +28364,7 @@
         <v>40</v>
       </c>
       <c r="G15" s="307" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="H15" s="228">
         <f t="shared" si="0"/>
@@ -28372,13 +28372,13 @@
       </c>
       <c r="I15" s="229"/>
       <c r="J15" s="307" t="s">
+        <v>397</v>
+      </c>
+      <c r="K15" s="307" t="s">
         <v>398</v>
       </c>
-      <c r="K15" s="307" t="s">
+      <c r="L15" s="307" t="s">
         <v>399</v>
-      </c>
-      <c r="L15" s="307" t="s">
-        <v>400</v>
       </c>
       <c r="M15" s="230"/>
       <c r="N15" s="230"/>
@@ -28386,7 +28386,7 @@
       <c r="P15" s="231"/>
       <c r="Q15" s="232"/>
       <c r="R15" s="307" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="S15" s="228">
         <f t="shared" si="1"/>
@@ -28509,7 +28509,7 @@
         <v>250</v>
       </c>
       <c r="G19" s="307" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="H19" s="258"/>
       <c r="I19" s="258"/>
@@ -28524,7 +28524,7 @@
         <v>251</v>
       </c>
       <c r="R19" s="307" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="S19" s="258"/>
       <c r="T19" s="258"/>
@@ -28672,7 +28672,7 @@
         <v>61</v>
       </c>
       <c r="K5" s="306" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="L5" s="209">
         <f t="shared" ref="L5:L13" si="0">SUM(K5)</f>
@@ -28870,7 +28870,7 @@
         <v>43</v>
       </c>
       <c r="K12" s="306" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="L12" s="209">
         <f t="shared" si="0"/>
@@ -28900,7 +28900,7 @@
         <v>40</v>
       </c>
       <c r="K13" s="306" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="L13" s="209">
         <f t="shared" si="0"/>
@@ -29912,7 +29912,7 @@
       <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A248" sqref="A248"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -29935,7 +29935,7 @@
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="393" t="s">
-        <v>365</v>
+        <v>630</v>
       </c>
       <c r="E1" s="394"/>
       <c r="F1" s="394"/>
@@ -29992,14 +29992,9 @@
   <mergeCells count="1">
     <mergeCell ref="D1:Q1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A1:D1 R1 T1:EY1">
-    <cfRule type="expression" dxfId="17" priority="19" stopIfTrue="1">
-      <formula>AND(OR($Q1&lt;&gt;"-",#REF!&lt;&gt;0,#REF!&lt;&gt;0),ROW()&gt;2,$A1&lt;&gt;"")</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A2:EZ2 A3:FB1048576">
-    <cfRule type="expression" dxfId="16" priority="1" stopIfTrue="1">
-      <formula>AND(OR($Q2&lt;&gt;"-",$R2&lt;&gt;0,$S2&lt;&gt;0),ROW()&gt;2,$A2&lt;&gt;"")</formula>
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+      <formula>AND(OR($R1&lt;&gt;"-",$S1&lt;&gt;0,$T1&lt;&gt;0),ROW()&gt;2,$A1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -30038,7 +30033,7 @@
   <sheetData>
     <row r="1" spans="1:24" s="4" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="128" t="s">
@@ -30329,70 +30324,70 @@
     <mergeCell ref="U4:V4"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:F4">
-    <cfRule type="expression" dxfId="15" priority="16">
+    <cfRule type="expression" dxfId="17" priority="16">
       <formula>IF(LEFT($A$3,2)&lt;&gt;"TJ",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:V151">
-    <cfRule type="expression" dxfId="14" priority="18">
+    <cfRule type="expression" dxfId="16" priority="18">
       <formula>AND(ISBLANK($C6)=FALSE,ISBLANK($E6)=TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:F1048576">
-    <cfRule type="expression" dxfId="13" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="1" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($U1)-(_xlfn.NUMBERVALUE($U2)+_xlfn.NUMBERVALUE($U3)+_xlfn.NUMBERVALUE($U4)+_xlfn.NUMBERVALUE($U5)+_xlfn.NUMBERVALUE($U6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="2" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($S1)-(_xlfn.NUMBERVALUE($S2)+_xlfn.NUMBERVALUE($S3)+_xlfn.NUMBERVALUE($S4)+_xlfn.NUMBERVALUE($S5)+_xlfn.NUMBERVALUE($S6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="7" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3)+_xlfn.NUMBERVALUE($L4)-_xlfn.NUMBERVALUE($L5)+_xlfn.NUMBERVALUE($L6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="12" stopIfTrue="1">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",OR(_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3))&lt;&gt;0,_xlfn.NUMBERVALUE($S1)-(_xlfn.NUMBERVALUE($S2)+_xlfn.NUMBERVALUE($S3))&lt;&gt;0,_xlfn.NUMBERVALUE($U1)-(_xlfn.NUMBERVALUE($U2)+_xlfn.NUMBERVALUE($U3))&lt;&gt;0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:F7">
-    <cfRule type="expression" dxfId="9" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="6" stopIfTrue="1">
       <formula>OR(_xlfn.NUMBERVALUE($L7)&lt;&gt;_xlfn.NUMBERVALUE($L6),_xlfn.NUMBERVALUE($S7)&lt;&gt;_xlfn.NUMBERVALUE($S6),_xlfn.NUMBERVALUE($U7)&lt;&gt;_xlfn.NUMBERVALUE($U6))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:M1048576">
-    <cfRule type="expression" dxfId="8" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="11" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3)+_xlfn.NUMBERVALUE($L4)+_xlfn.NUMBERVALUE($L5)+_xlfn.NUMBERVALUE($L6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="15">
+    <cfRule type="expression" dxfId="9" priority="15">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3))&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:M7">
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="8" priority="5">
       <formula>_xlfn.NUMBERVALUE($L7)&lt;&gt;_xlfn.NUMBERVALUE($L6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:T1048576">
-    <cfRule type="expression" dxfId="5" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="10" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($S1)-(_xlfn.NUMBERVALUE($S2)+_xlfn.NUMBERVALUE($S3)+_xlfn.NUMBERVALUE($S4)+_xlfn.NUMBERVALUE($S5)+_xlfn.NUMBERVALUE($S6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="14">
+    <cfRule type="expression" dxfId="6" priority="14">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",_xlfn.NUMBERVALUE($S1)-(_xlfn.NUMBERVALUE($S2)+_xlfn.NUMBERVALUE($S3))&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7:T7">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>_xlfn.NUMBERVALUE($S7)&lt;&gt;_xlfn.NUMBERVALUE($S6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:V1048576">
-    <cfRule type="expression" dxfId="2" priority="9">
+    <cfRule type="expression" dxfId="4" priority="9">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($U1)-(_xlfn.NUMBERVALUE($U2)+_xlfn.NUMBERVALUE($U3)+_xlfn.NUMBERVALUE($U4)+_xlfn.NUMBERVALUE($U5)+_xlfn.NUMBERVALUE($U6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="13">
+    <cfRule type="expression" dxfId="3" priority="13">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",_xlfn.NUMBERVALUE($U1)-(_xlfn.NUMBERVALUE($U2)+_xlfn.NUMBERVALUE($U3))&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U7:V7">
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>_xlfn.NUMBERVALUE($U7)&lt;&gt;_xlfn.NUMBERVALUE($U6)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -36103,34 +36098,34 @@
         <v>109</v>
       </c>
       <c r="G4" s="360" t="s">
+        <v>613</v>
+      </c>
+      <c r="H4" s="360" t="s">
         <v>614</v>
       </c>
-      <c r="H4" s="360" t="s">
+      <c r="I4" s="360" t="s">
         <v>615</v>
-      </c>
-      <c r="I4" s="360" t="s">
-        <v>616</v>
       </c>
       <c r="J4" s="360" t="s">
         <v>93</v>
       </c>
       <c r="K4" s="360" t="s">
+        <v>616</v>
+      </c>
+      <c r="L4" s="360" t="s">
         <v>617</v>
       </c>
-      <c r="L4" s="360" t="s">
+      <c r="M4" s="360" t="s">
         <v>618</v>
       </c>
-      <c r="M4" s="360" t="s">
+      <c r="N4" s="360" t="s">
         <v>619</v>
       </c>
-      <c r="N4" s="360" t="s">
+      <c r="O4" s="360" t="s">
         <v>620</v>
       </c>
-      <c r="O4" s="360" t="s">
+      <c r="P4" s="360" t="s">
         <v>621</v>
-      </c>
-      <c r="P4" s="360" t="s">
-        <v>622</v>
       </c>
       <c r="Q4" s="405"/>
     </row>
@@ -37111,7 +37106,7 @@
       <c r="G17" s="291"/>
       <c r="H17" s="291"/>
       <c r="I17" s="365" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="J17" s="290"/>
       <c r="L17" s="290"/>
@@ -37132,7 +37127,7 @@
       <c r="G18" s="291"/>
       <c r="H18" s="291"/>
       <c r="I18" s="365" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J18" s="290"/>
       <c r="L18" s="290"/>

</xml_diff>

<commit_message>
update zoom for tj et ca extractor
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC793514-3200-1142-B289-DAE449AC69D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D163E9F-EF9A-EB49-A9BD-BFEE7DA6ED22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17740" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -18814,807 +18814,7 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{6FC886D6-2077-B34D-B1DF-739B068A66D1}"/>
     <cellStyle name="Normal 3" xfId="4" xr:uid="{6BD57324-3FD5-D341-A299-730D14794802}"/>
   </cellStyles>
-  <dxfs count="97">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
+  <dxfs count="17">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -20640,14 +19840,14 @@
   </sheetPr>
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
       <selection activeCell="V118" sqref="V118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="1.1640625" style="21" customWidth="1"/>
-    <col min="2" max="2" width="27.1640625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="30" style="21" customWidth="1"/>
     <col min="3" max="3" width="102.1640625" style="21" customWidth="1"/>
     <col min="4" max="4" width="56.33203125" style="21" customWidth="1"/>
     <col min="5" max="5" width="14" style="21" customWidth="1"/>
@@ -33539,7 +32739,7 @@
     <mergeCell ref="D1:Q1"/>
   </mergeCells>
   <conditionalFormatting sqref="A2:EZ2 A3:FB1048576">
-    <cfRule type="expression" dxfId="96" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="1" stopIfTrue="1">
       <formula>AND(OR($R1&lt;&gt;"-",$S1&lt;&gt;0,$T1&lt;&gt;0),ROW()&gt;2,$A1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -33870,70 +33070,70 @@
     <mergeCell ref="U4:V4"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:F4">
-    <cfRule type="expression" dxfId="31" priority="16">
+    <cfRule type="expression" dxfId="15" priority="16">
       <formula>IF(LEFT($A$3,2)&lt;&gt;"TJ",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:V151">
-    <cfRule type="expression" dxfId="30" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="18" stopIfTrue="1">
       <formula>AND(ISBLANK($C6)=FALSE,ISBLANK($E6)=TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:F1048576">
-    <cfRule type="expression" dxfId="29" priority="1">
+    <cfRule type="expression" dxfId="13" priority="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3)-_xlfn.NUMBERVALUE($U4)-_xlfn.NUMBERVALUE($U5)-_xlfn.NUMBERVALUE($U6),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="2">
+    <cfRule type="expression" dxfId="12" priority="2">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3)-_xlfn.NUMBERVALUE($S4)-_xlfn.NUMBERVALUE($S5)-_xlfn.NUMBERVALUE($S6),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="7" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($L1)-_xlfn.NUMBERVALUE($L2)-_xlfn.NUMBERVALUE($L3)-_xlfn.NUMBERVALUE($L4)-_xlfn.NUMBERVALUE($L5)-_xlfn.NUMBERVALUE($L6),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="12">
+    <cfRule type="expression" dxfId="10" priority="12">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",OR(ROUND(_xlfn.NUMBERVALUE($L1)-_xlfn.NUMBERVALUE($L2)-_xlfn.NUMBERVALUE($L3),3)&lt;&gt;0,ROUND(_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3),3)&lt;&gt;0,ROUND(_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3),3)&lt;&gt;0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:F7">
-    <cfRule type="expression" dxfId="25" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="6" stopIfTrue="1">
       <formula>OR(ROUND(_xlfn.NUMBERVALUE($L7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($L6),3),ROUND(_xlfn.NUMBERVALUE($S7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($S6),3),ROUND(_xlfn.NUMBERVALUE($U7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($U6),3))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:M1048576">
-    <cfRule type="expression" dxfId="24" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="11" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3)+_xlfn.NUMBERVALUE($L4)+_xlfn.NUMBERVALUE($L5)+_xlfn.NUMBERVALUE($L6)),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="15">
+    <cfRule type="expression" dxfId="7" priority="15">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",ROUND(_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3)),3)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:M7">
-    <cfRule type="expression" dxfId="22" priority="5">
+    <cfRule type="expression" dxfId="6" priority="5">
       <formula>ROUND(_xlfn.NUMBERVALUE($L7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($L6),3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:T1048576">
-    <cfRule type="expression" dxfId="21" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="10" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3)-_xlfn.NUMBERVALUE($S4)-_xlfn.NUMBERVALUE($S5)-_xlfn.NUMBERVALUE($S6),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="14">
+    <cfRule type="expression" dxfId="4" priority="14">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",ROUND(_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3),3)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7:T7">
-    <cfRule type="expression" dxfId="19" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>ROUND(_xlfn.NUMBERVALUE($S7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($S6),3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:V1048576">
-    <cfRule type="expression" dxfId="17" priority="9">
+    <cfRule type="expression" dxfId="2" priority="9">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3)-_xlfn.NUMBERVALUE($U4)-_xlfn.NUMBERVALUE($U5)-_xlfn.NUMBERVALUE($U6),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="13">
+    <cfRule type="expression" dxfId="1" priority="13">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",ROUND(_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3),3)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U7:V7">
-    <cfRule type="expression" dxfId="18" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
       <formula>ROUND(_xlfn.NUMBERVALUE($U7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($U6),3)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
update extractor red underline while no etpt
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D163E9F-EF9A-EB49-A9BD-BFEE7DA6ED22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C1F9DA-37DD-2E45-BE7A-648C2291B142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17740" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
@@ -18814,7 +18814,27 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{6FC886D6-2077-B34D-B1DF-739B068A66D1}"/>
     <cellStyle name="Normal 3" xfId="4" xr:uid="{6BD57324-3FD5-D341-A299-730D14794802}"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -18974,16 +18994,6 @@
       <font>
         <color theme="0"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -32739,8 +32749,8 @@
     <mergeCell ref="D1:Q1"/>
   </mergeCells>
   <conditionalFormatting sqref="A2:EZ2 A3:FB1048576">
-    <cfRule type="expression" dxfId="16" priority="1" stopIfTrue="1">
-      <formula>AND(OR($R1&lt;&gt;"-",$S1&lt;&gt;0,$T1&lt;&gt;0),ROW()&gt;2,$A1&lt;&gt;"")</formula>
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>AND(OR($R1&lt;&gt;"-",$S1&lt;&gt;0,$T1&lt;&gt;0,ISBLANK($P1)),ROW()&gt;2,$A1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -33070,70 +33080,70 @@
     <mergeCell ref="U4:V4"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:F4">
-    <cfRule type="expression" dxfId="15" priority="16">
+    <cfRule type="expression" dxfId="17" priority="16">
       <formula>IF(LEFT($A$3,2)&lt;&gt;"TJ",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:V151">
-    <cfRule type="expression" dxfId="14" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="18" stopIfTrue="1">
       <formula>AND(ISBLANK($C6)=FALSE,ISBLANK($E6)=TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:F1048576">
-    <cfRule type="expression" dxfId="13" priority="1">
+    <cfRule type="expression" dxfId="15" priority="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3)-_xlfn.NUMBERVALUE($U4)-_xlfn.NUMBERVALUE($U5)-_xlfn.NUMBERVALUE($U6),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="2">
+    <cfRule type="expression" dxfId="14" priority="2">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3)-_xlfn.NUMBERVALUE($S4)-_xlfn.NUMBERVALUE($S5)-_xlfn.NUMBERVALUE($S6),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="7" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($L1)-_xlfn.NUMBERVALUE($L2)-_xlfn.NUMBERVALUE($L3)-_xlfn.NUMBERVALUE($L4)-_xlfn.NUMBERVALUE($L5)-_xlfn.NUMBERVALUE($L6),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="12">
+    <cfRule type="expression" dxfId="12" priority="12">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",OR(ROUND(_xlfn.NUMBERVALUE($L1)-_xlfn.NUMBERVALUE($L2)-_xlfn.NUMBERVALUE($L3),3)&lt;&gt;0,ROUND(_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3),3)&lt;&gt;0,ROUND(_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3),3)&lt;&gt;0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:F7">
-    <cfRule type="expression" dxfId="9" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="6" stopIfTrue="1">
       <formula>OR(ROUND(_xlfn.NUMBERVALUE($L7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($L6),3),ROUND(_xlfn.NUMBERVALUE($S7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($S6),3),ROUND(_xlfn.NUMBERVALUE($U7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($U6),3))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:M1048576">
-    <cfRule type="expression" dxfId="8" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="11" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3)+_xlfn.NUMBERVALUE($L4)+_xlfn.NUMBERVALUE($L5)+_xlfn.NUMBERVALUE($L6)),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="15">
+    <cfRule type="expression" dxfId="9" priority="15">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",ROUND(_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3)),3)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:M7">
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="8" priority="5">
       <formula>ROUND(_xlfn.NUMBERVALUE($L7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($L6),3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:T1048576">
-    <cfRule type="expression" dxfId="5" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="10" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3)-_xlfn.NUMBERVALUE($S4)-_xlfn.NUMBERVALUE($S5)-_xlfn.NUMBERVALUE($S6),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="14">
+    <cfRule type="expression" dxfId="6" priority="14">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",ROUND(_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3),3)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7:T7">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>ROUND(_xlfn.NUMBERVALUE($S7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($S6),3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:V1048576">
-    <cfRule type="expression" dxfId="2" priority="9">
+    <cfRule type="expression" dxfId="4" priority="9">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3)-_xlfn.NUMBERVALUE($U4)-_xlfn.NUMBERVALUE($U5)-_xlfn.NUMBERVALUE($U6),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="13">
+    <cfRule type="expression" dxfId="3" priority="13">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",ROUND(_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3),3)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U7:V7">
-    <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
       <formula>ROUND(_xlfn.NUMBERVALUE($U7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($U6),3)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
remove lock on AJUST tab
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{748ECCA0-6141-774D-B98C-4C33A9F8161B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25557939-896D-1F41-9234-CFEB565BC808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15720" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
@@ -35636,7 +35636,7 @@
       <c r="C8" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" sort="0" autoFilter="0"/>
+  <sheetProtection sort="0" autoFilter="0"/>
   <autoFilter ref="A2:DN2" xr:uid="{F3674A8A-13E9-4EDB-B294-D1FF8F18362C}"/>
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update lock for dropdown
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{748ECCA0-6141-774D-B98C-4C33A9F8161B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF57EE2-9FE9-4949-9C0C-EC386BD939CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15720" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
@@ -36770,7 +36770,7 @@
       <c r="FA4" s="21"/>
     </row>
   </sheetData>
-  <sheetProtection sort="0" autoFilter="0"/>
+  <sheetProtection sheet="1" autoFilter="0"/>
   <autoFilter ref="A2:DT2" xr:uid="{3B89445B-6ECC-4440-B85C-E593AE209933}"/>
   <mergeCells count="1">
     <mergeCell ref="D1:Q1"/>

</xml_diff>

<commit_message>
feat: Update Excel template with new Attaché de Justice formulas
- Add formulas for 3 new recoded functions in ETPT_JUR_ASS tab:
  * JA/AttJ Siege Assises
  * JA/AttJ Siege CCD
  * JA/AttJ JLD PÉNAL

- Update formula arrays to include new function variants
- Ensures proper calculation of ETPT for new Attaché de Justice roles
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dinum-327809/Documents/a-just-clean/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF0681A9-AC29-A745-9551-49B4DCC99555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6B9269-C0E1-5A4D-A26F-754C1F2A9340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11060" yWindow="760" windowWidth="30240" windowHeight="17700" firstSheet="4" activeTab="6" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" firstSheet="1" activeTab="9" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
   <sheets>
     <sheet name="ACCUEIL" sheetId="33" r:id="rId1"/>
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1828" uniqueCount="684">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1832" uniqueCount="686">
   <si>
     <t>#! END_ROW</t>
   </si>
@@ -16485,6 +16485,12 @@
       <t xml:space="preserve">
 *figurant dans l'onglet ETPT A-JUST</t>
     </r>
+  </si>
+  <si>
+    <t>Attachés de justice parquet affectés aux assises</t>
+  </si>
+  <si>
+    <t>Attachés de justice parquet affectés aux CDD</t>
   </si>
 </sst>
 </file>
@@ -20549,10 +20555,10 @@
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
-  <dimension ref="A1:BJ145"/>
+  <dimension ref="A1:BL145"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20560,10 +20566,10 @@
     <col min="1" max="2" width="10.83203125" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="73.83203125" customWidth="1"/>
-    <col min="7" max="16" width="13.33203125" customWidth="1"/>
+    <col min="7" max="18" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" s="4" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:64" s="4" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>217</v>
       </c>
@@ -20630,8 +20636,10 @@
       <c r="BH1" s="7"/>
       <c r="BI1" s="7"/>
       <c r="BJ1" s="7"/>
-    </row>
-    <row r="2" spans="1:62" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BK1" s="7"/>
+      <c r="BL1" s="7"/>
+    </row>
+    <row r="2" spans="1:64" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="206"/>
       <c r="B2" s="207"/>
       <c r="C2" s="207"/>
@@ -20652,23 +20660,25 @@
       <c r="L2" s="208" t="s">
         <v>38</v>
       </c>
-      <c r="M2" s="208" t="s">
-        <v>38</v>
-      </c>
-      <c r="N2" s="208" t="s">
-        <v>38</v>
-      </c>
+      <c r="M2" s="208"/>
+      <c r="N2" s="208"/>
       <c r="O2" s="208" t="s">
         <v>38</v>
       </c>
       <c r="P2" s="208" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="418" t="s">
+      <c r="Q2" s="208" t="s">
+        <v>38</v>
+      </c>
+      <c r="R2" s="208" t="s">
+        <v>38</v>
+      </c>
+      <c r="S2" s="418" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="3" spans="1:62" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:64" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="206"/>
       <c r="B3" s="207"/>
       <c r="C3" s="207"/>
@@ -20689,21 +20699,23 @@
       <c r="L3" s="208" t="s">
         <v>144</v>
       </c>
-      <c r="M3" s="208" t="s">
+      <c r="M3" s="208"/>
+      <c r="N3" s="208"/>
+      <c r="O3" s="208" t="s">
         <v>275</v>
       </c>
-      <c r="N3" s="208" t="s">
+      <c r="P3" s="208" t="s">
         <v>276</v>
       </c>
-      <c r="O3" s="208" t="s">
+      <c r="Q3" s="208" t="s">
         <v>277</v>
       </c>
-      <c r="P3" s="208" t="s">
+      <c r="R3" s="208" t="s">
         <v>278</v>
       </c>
-      <c r="Q3" s="418"/>
-    </row>
-    <row r="4" spans="1:62" ht="36" x14ac:dyDescent="0.2">
+      <c r="S3" s="418"/>
+    </row>
+    <row r="4" spans="1:64" ht="36" x14ac:dyDescent="0.2">
       <c r="A4" s="209"/>
       <c r="B4" s="210" t="s">
         <v>112</v>
@@ -20739,20 +20751,26 @@
         <v>677</v>
       </c>
       <c r="M4" s="249" t="s">
+        <v>684</v>
+      </c>
+      <c r="N4" s="249" t="s">
+        <v>685</v>
+      </c>
+      <c r="O4" s="249" t="s">
         <v>678</v>
       </c>
-      <c r="N4" s="249" t="s">
+      <c r="P4" s="249" t="s">
         <v>679</v>
       </c>
-      <c r="O4" s="249" t="s">
+      <c r="Q4" s="249" t="s">
         <v>680</v>
       </c>
-      <c r="P4" s="249" t="s">
+      <c r="R4" s="249" t="s">
         <v>676</v>
       </c>
-      <c r="Q4" s="418"/>
-    </row>
-    <row r="5" spans="1:62" x14ac:dyDescent="0.2">
+      <c r="S4" s="418"/>
+    </row>
+    <row r="5" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A5" s="211" t="s">
         <v>290</v>
       </c>
@@ -20809,19 +20827,19 @@
       <c r="I5" s="280" t="e" cm="1">
         <f t="array" ref="I5">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("2. TOTAL CONTENTIEUX JAF",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Social"},
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD";"JA/AttJ Social"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3. TOTAL CONTENTIEUX DE LA PROTECTION",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Social"},
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD";"JA/AttJ Social"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("4. TOTAL CIVIL NON SPÉCIALISÉ",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Social"},
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD";"JA/AttJ Social"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.7. FONCTIONNAIRES AFFECTÉS AU CPH",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Social"},
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD";"JA/AttJ Social"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
@@ -20830,26 +20848,28 @@
       <c r="L5" s="280" t="e" cm="1">
         <f t="array" ref="L5">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.8. FONCTIONNAIRES AFFECTÉS AUX ACTIVITÉS CIVILES ET COMMERCIALES DU PARQUET",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Social"},
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD";"JA/AttJ Social"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
       <c r="M5" s="280"/>
-      <c r="N5" s="280" t="e" cm="1">
-        <f t="array" ref="N5">SUM(SUMIFS(
+      <c r="N5" s="280"/>
+      <c r="O5" s="280"/>
+      <c r="P5" s="280" t="e" cm="1">
+        <f t="array" ref="P5">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("6.1. ACTIVITÉ CIVILE",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Social"},
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD";"JA/AttJ Social"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
-      <c r="O5" s="280"/>
-      <c r="P5" s="280"/>
-      <c r="Q5" s="278">
-        <f>_xlfn.AGGREGATE(9,6,G5:P5)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:62" x14ac:dyDescent="0.2">
+      <c r="Q5" s="280"/>
+      <c r="R5" s="280"/>
+      <c r="S5" s="278">
+        <f>_xlfn.AGGREGATE(9,6,G5:R5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A6" s="211" t="s">
         <v>290</v>
       </c>
@@ -20902,7 +20922,7 @@
       <c r="I6" s="280" t="e" cm="1">
         <f t="array" ref="I6">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("7. TOTAL SIÈGE PÉNAL",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Social"},
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD";"JA/AttJ Social"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
@@ -20911,48 +20931,50 @@
       <c r="L6" s="280" t="e" cm="1">
         <f t="array" ref="L6">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.9. FONCTIONNAIRES AFFECTÉS À L'EXÉCUTION DES PEINES",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Social"},
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD";"JA/AttJ Social"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.10. AUTRES FONCTIONNAIRES AFFECTÉS AU PARQUET",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Social"},
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD";"JA/AttJ Social"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
-      <c r="M6" s="280" t="e" cm="1">
-        <f t="array" ref="M6">SUM(SUMIFS(
+      <c r="M6" s="280"/>
+      <c r="N6" s="280"/>
+      <c r="O6" s="280" t="e" cm="1">
+        <f t="array" ref="O6">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("9. TOTAL JAP",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Social"},
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD";"JA/AttJ Social"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
-      <c r="N6" s="280" t="e" cm="1">
-        <f t="array" ref="N6">SUM(SUMIFS(
+      <c r="P6" s="280" t="e" cm="1">
+        <f t="array" ref="P6">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("6.2. ACTIVITÉ PÉNALE",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Social"},
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD";"JA/AttJ Social"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
-      <c r="O6" s="280" t="e" cm="1">
-        <f t="array" ref="O6">SUM(SUMIFS(
+      <c r="Q6" s="280" t="e" cm="1">
+        <f t="array" ref="Q6">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("8. TOTAL JUGES D'INSTRUCTION",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Social"},
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD";"JA/AttJ Social"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
-      <c r="P6" s="280" t="e" cm="1">
-        <f t="array" ref="P6">SUM(SUMIFS(
+      <c r="R6" s="280" t="e" cm="1">
+        <f t="array" ref="R6">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("10. TOTAL JLD PÉNAL",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Social"},
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD";"JA/AttJ Social"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
-      <c r="Q6" s="278">
-        <f>_xlfn.AGGREGATE(9,6,G6:P6)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:62" x14ac:dyDescent="0.2">
+      <c r="S6" s="278">
+        <f>_xlfn.AGGREGATE(9,6,G6:R6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A7" s="211" t="s">
         <v>290</v>
       </c>
@@ -20998,40 +21020,42 @@
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
-      <c r="M7" s="280" t="e">
+      <c r="M7" s="280"/>
+      <c r="N7" s="280"/>
+      <c r="O7" s="280" t="e">
         <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.51. ACCUEIL DU JUSTICIABLE (DONT SAUJ)",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JAP",
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
-      <c r="N7" s="280" t="e">
+      <c r="P7" s="280" t="e">
         <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.51. ACCUEIL DU JUSTICIABLE (DONT SAUJ)",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JE",
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
-      <c r="O7" s="280" t="e">
+      <c r="Q7" s="280" t="e">
         <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.51. ACCUEIL DU JUSTICIABLE (DONT SAUJ)",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JI",
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
-      <c r="P7" s="280" t="e">
+      <c r="R7" s="280" t="e">
         <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.51. ACCUEIL DU JUSTICIABLE (DONT SAUJ)",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JLD",
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JLD PÉNAL",
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
-      <c r="Q7" s="278">
-        <f>_xlfn.AGGREGATE(9,6,G7:P7)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:62" x14ac:dyDescent="0.2">
+      <c r="S7" s="278">
+        <f>_xlfn.AGGREGATE(9,6,G7:R7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A8" s="211" t="s">
         <v>290</v>
       </c>
@@ -21109,7 +21133,9 @@
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
-      <c r="M8" s="280" t="e">
+      <c r="M8" s="280"/>
+      <c r="N8" s="280"/>
+      <c r="O8" s="280" t="e">
         <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.1. SOUTIEN (HORS FORMATIONS SUIVIES)",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JAP",
@@ -21124,7 +21150,7 @@
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
-      <c r="N8" s="280" t="e">
+      <c r="P8" s="280" t="e">
         <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.1. SOUTIEN (HORS FORMATIONS SUIVIES)",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JE",
@@ -21139,7 +21165,7 @@
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
-      <c r="O8" s="280" t="e">
+      <c r="Q8" s="280" t="e">
         <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.1. SOUTIEN (HORS FORMATIONS SUIVIES)",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JI",
@@ -21154,27 +21180,27 @@
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
-      <c r="P8" s="280" t="e">
+      <c r="R8" s="280" t="e">
         <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.1. SOUTIEN (HORS FORMATIONS SUIVIES)",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JLD",
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JLD PÉNAL",
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.2. FORMATIONS SUIVIES",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JLD",
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JLD PÉNAL",
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.6. AUTRES ACTIVITÉS NON JURIDICTIONNELLES",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JLD",
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JLD PÉNAL",
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
-      <c r="Q8" s="278">
-        <f>_xlfn.AGGREGATE(9,6,G8:P8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:62" x14ac:dyDescent="0.2">
+      <c r="S8" s="278">
+        <f>_xlfn.AGGREGATE(9,6,G8:R8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A9" s="211" t="s">
         <v>290</v>
       </c>
@@ -21220,40 +21246,42 @@
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
-      <c r="M9" s="280" t="e">
+      <c r="M9" s="280"/>
+      <c r="N9" s="280"/>
+      <c r="O9" s="280" t="e">
         <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.3. FORMATIONS DISPENSÉES",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JAP",
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
-      <c r="N9" s="280" t="e">
+      <c r="P9" s="280" t="e">
         <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.3. FORMATIONS DISPENSÉES",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JE",
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
-      <c r="O9" s="280" t="e">
+      <c r="Q9" s="280" t="e">
         <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.3. FORMATIONS DISPENSÉES",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JI",
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
-      <c r="P9" s="280" t="e">
+      <c r="R9" s="280" t="e">
         <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.3. FORMATIONS DISPENSÉES",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JLD",
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JLD PÉNAL",
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
-      <c r="Q9" s="278">
-        <f>_xlfn.AGGREGATE(9,6,G9:P9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:62" x14ac:dyDescent="0.2">
+      <c r="S9" s="278">
+        <f>_xlfn.AGGREGATE(9,6,G9:R9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A10" s="211" t="s">
         <v>290</v>
       </c>
@@ -21299,40 +21327,42 @@
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
-      <c r="M10" s="280" t="e">
+      <c r="M10" s="280"/>
+      <c r="N10" s="280"/>
+      <c r="O10" s="280" t="e">
         <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.4. ACCÈS AU DROIT ET À LA JUSTICE",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JAP",
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
-      <c r="N10" s="280" t="e">
+      <c r="P10" s="280" t="e">
         <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.4. ACCÈS AU DROIT ET À LA JUSTICE",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JE",
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
-      <c r="O10" s="280" t="e">
+      <c r="Q10" s="280" t="e">
         <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.4. ACCÈS AU DROIT ET À LA JUSTICE",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JI",
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
-      <c r="P10" s="280" t="e">
+      <c r="R10" s="280" t="e">
         <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.4. ACCÈS AU DROIT ET À LA JUSTICE",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JLD",
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JLD PÉNAL",
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
-      <c r="Q10" s="278">
-        <f>_xlfn.AGGREGATE(9,6,G10:P10)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:62" x14ac:dyDescent="0.2">
+      <c r="S10" s="278">
+        <f>_xlfn.AGGREGATE(9,6,G10:R10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A11" s="211" t="s">
         <v>290</v>
       </c>
@@ -21394,7 +21424,9 @@
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
-      <c r="M11" s="280" t="e">
+      <c r="M11" s="280"/>
+      <c r="N11" s="280"/>
+      <c r="O11" s="280" t="e">
         <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JAP",
@@ -21405,7 +21437,7 @@
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
-      <c r="N11" s="280" t="e">
+      <c r="P11" s="280" t="e">
         <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JE",
@@ -21416,7 +21448,7 @@
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
-      <c r="O11" s="280" t="e">
+      <c r="Q11" s="280" t="e">
         <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JI",
@@ -21427,23 +21459,23 @@
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
-      <c r="P11" s="280" t="e">
+      <c r="R11" s="280" t="e">
         <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JLD",
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JLD PÉNAL",
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JLD",
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JLD PÉNAL",
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
-      <c r="Q11" s="278">
-        <f>_xlfn.AGGREGATE(9,6,G11:P11)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:62" x14ac:dyDescent="0.2">
+      <c r="S11" s="278">
+        <f>_xlfn.AGGREGATE(9,6,G11:R11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A12" s="211" t="s">
         <v>290</v>
       </c>
@@ -21505,7 +21537,9 @@
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5)),0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M12" s="280" t="e">
+      <c r="M12" s="280"/>
+      <c r="N12" s="280"/>
+      <c r="O12" s="280" t="e">
         <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JAP",
@@ -21516,7 +21550,7 @@
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5)),0)</f>
         <v>#N/A</v>
       </c>
-      <c r="N12" s="280" t="e">
+      <c r="P12" s="280" t="e">
         <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JE",
@@ -21527,7 +21561,7 @@
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5)),0)</f>
         <v>#N/A</v>
       </c>
-      <c r="O12" s="280" t="e">
+      <c r="Q12" s="280" t="e">
         <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JI",
@@ -21538,23 +21572,23 @@
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5)),0)</f>
         <v>#N/A</v>
       </c>
-      <c r="P12" s="280" t="e">
+      <c r="R12" s="280" t="e">
         <f>SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JLD",
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JLD PÉNAL",
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))+
 _xlfn.IFNA(SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("13. TOTAL CONTENTIEUX LOCAUX SPÉCIFIQUES",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JLD",
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JLD PÉNAL",
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5)),0)</f>
         <v>#N/A</v>
       </c>
-      <c r="Q12" s="278">
-        <f>_xlfn.AGGREGATE(9,6,G12:P12)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:62" ht="16" x14ac:dyDescent="0.2">
+      <c r="S12" s="278">
+        <f>_xlfn.AGGREGATE(9,6,G12:R12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:64" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="217"/>
       <c r="B13" s="217"/>
       <c r="C13" s="217"/>
@@ -21572,7 +21606,7 @@
         <v>0</v>
       </c>
       <c r="I13" s="278">
-        <f t="shared" ref="I13:P13" si="0">_xlfn.AGGREGATE(9,6,I5:I12)</f>
+        <f t="shared" ref="I13:R13" si="0">_xlfn.AGGREGATE(9,6,I5:I12)</f>
         <v>0</v>
       </c>
       <c r="J13" s="278">
@@ -21604,11 +21638,19 @@
         <v>0</v>
       </c>
       <c r="Q13" s="278">
-        <f>_xlfn.AGGREGATE(9,6,Q5:Q12)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:62" ht="16" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R13" s="278">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S13" s="278">
+        <f>_xlfn.AGGREGATE(9,6,S5:S12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:64" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="217"/>
       <c r="B14" s="217"/>
       <c r="C14" s="217"/>
@@ -21626,8 +21668,10 @@
       <c r="O14" s="216"/>
       <c r="P14" s="216"/>
       <c r="Q14" s="216"/>
-    </row>
-    <row r="15" spans="1:62" ht="16" x14ac:dyDescent="0.2">
+      <c r="R14" s="216"/>
+      <c r="S14" s="216"/>
+    </row>
+    <row r="15" spans="1:64" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="217"/>
       <c r="B15" s="217"/>
       <c r="C15" s="217"/>
@@ -21639,13 +21683,13 @@
       <c r="I15" s="216"/>
       <c r="J15" s="216"/>
       <c r="K15" s="216"/>
-      <c r="M15" s="216"/>
-      <c r="N15" s="216"/>
       <c r="O15" s="216"/>
       <c r="P15" s="216"/>
       <c r="Q15" s="216"/>
-    </row>
-    <row r="16" spans="1:62" ht="16" x14ac:dyDescent="0.2">
+      <c r="R15" s="216"/>
+      <c r="S15" s="216"/>
+    </row>
+    <row r="16" spans="1:64" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="217"/>
       <c r="B16" s="217"/>
       <c r="C16" s="217"/>
@@ -21657,13 +21701,13 @@
       <c r="I16" s="216"/>
       <c r="J16" s="216"/>
       <c r="K16" s="216"/>
-      <c r="M16" s="216"/>
-      <c r="N16" s="216"/>
       <c r="O16" s="216"/>
       <c r="P16" s="216"/>
       <c r="Q16" s="216"/>
-    </row>
-    <row r="17" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="R16" s="216"/>
+      <c r="S16" s="216"/>
+    </row>
+    <row r="17" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="217"/>
       <c r="B17" s="217"/>
       <c r="C17" s="217"/>
@@ -21675,14 +21719,14 @@
       <c r="I17" s="216"/>
       <c r="J17" s="216"/>
       <c r="K17" s="216"/>
-      <c r="M17" s="216"/>
-      <c r="N17" s="216"/>
       <c r="O17" s="216"/>
       <c r="P17" s="216"/>
       <c r="Q17" s="216"/>
       <c r="R17" s="216"/>
-    </row>
-    <row r="18" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S17" s="216"/>
+      <c r="T17" s="216"/>
+    </row>
+    <row r="18" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="217"/>
       <c r="B18" s="217"/>
       <c r="C18" s="217"/>
@@ -21694,14 +21738,14 @@
       <c r="I18" s="216"/>
       <c r="J18" s="216"/>
       <c r="K18" s="216"/>
-      <c r="M18" s="216"/>
-      <c r="N18" s="216"/>
       <c r="O18" s="216"/>
       <c r="P18" s="216"/>
       <c r="Q18" s="216"/>
       <c r="R18" s="216"/>
-    </row>
-    <row r="19" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S18" s="216"/>
+      <c r="T18" s="216"/>
+    </row>
+    <row r="19" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="217"/>
       <c r="B19" s="217"/>
       <c r="C19" s="217"/>
@@ -21713,14 +21757,14 @@
       <c r="I19" s="216"/>
       <c r="J19" s="216"/>
       <c r="K19" s="216"/>
-      <c r="M19" s="216"/>
-      <c r="N19" s="216"/>
       <c r="O19" s="216"/>
       <c r="P19" s="216"/>
       <c r="Q19" s="216"/>
       <c r="R19" s="216"/>
-    </row>
-    <row r="20" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S19" s="216"/>
+      <c r="T19" s="216"/>
+    </row>
+    <row r="20" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="217"/>
       <c r="B20" s="217"/>
       <c r="C20" s="217"/>
@@ -21732,14 +21776,14 @@
       <c r="I20" s="216"/>
       <c r="J20" s="216"/>
       <c r="K20" s="216"/>
-      <c r="M20" s="216"/>
-      <c r="N20" s="216"/>
       <c r="O20" s="216"/>
       <c r="P20" s="216"/>
       <c r="Q20" s="216"/>
       <c r="R20" s="216"/>
-    </row>
-    <row r="21" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S20" s="216"/>
+      <c r="T20" s="216"/>
+    </row>
+    <row r="21" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="217"/>
       <c r="B21" s="217"/>
       <c r="C21" s="217"/>
@@ -21751,14 +21795,14 @@
       <c r="I21" s="216"/>
       <c r="J21" s="216"/>
       <c r="K21" s="216"/>
-      <c r="M21" s="216"/>
-      <c r="N21" s="216"/>
       <c r="O21" s="216"/>
       <c r="P21" s="216"/>
       <c r="Q21" s="216"/>
       <c r="R21" s="216"/>
-    </row>
-    <row r="22" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S21" s="216"/>
+      <c r="T21" s="216"/>
+    </row>
+    <row r="22" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="217"/>
       <c r="B22" s="217"/>
       <c r="C22" s="217"/>
@@ -21770,14 +21814,14 @@
       <c r="I22" s="216"/>
       <c r="J22" s="216"/>
       <c r="K22" s="216"/>
-      <c r="M22" s="216"/>
-      <c r="N22" s="216"/>
       <c r="O22" s="216"/>
       <c r="P22" s="216"/>
       <c r="Q22" s="216"/>
       <c r="R22" s="216"/>
-    </row>
-    <row r="23" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S22" s="216"/>
+      <c r="T22" s="216"/>
+    </row>
+    <row r="23" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="217"/>
       <c r="B23" s="217"/>
       <c r="C23" s="217"/>
@@ -21796,8 +21840,10 @@
       <c r="P23" s="216"/>
       <c r="Q23" s="216"/>
       <c r="R23" s="216"/>
-    </row>
-    <row r="24" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S23" s="216"/>
+      <c r="T23" s="216"/>
+    </row>
+    <row r="24" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="217"/>
       <c r="B24" s="217"/>
       <c r="C24" s="217"/>
@@ -21816,8 +21862,10 @@
       <c r="P24" s="216"/>
       <c r="Q24" s="216"/>
       <c r="R24" s="216"/>
-    </row>
-    <row r="25" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S24" s="216"/>
+      <c r="T24" s="216"/>
+    </row>
+    <row r="25" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="217"/>
       <c r="B25" s="217"/>
       <c r="C25" s="217"/>
@@ -21836,8 +21884,10 @@
       <c r="P25" s="216"/>
       <c r="Q25" s="216"/>
       <c r="R25" s="216"/>
-    </row>
-    <row r="26" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S25" s="216"/>
+      <c r="T25" s="216"/>
+    </row>
+    <row r="26" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="217"/>
       <c r="B26" s="217"/>
       <c r="C26" s="217"/>
@@ -21856,8 +21906,10 @@
       <c r="P26" s="216"/>
       <c r="Q26" s="216"/>
       <c r="R26" s="216"/>
-    </row>
-    <row r="27" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S26" s="216"/>
+      <c r="T26" s="216"/>
+    </row>
+    <row r="27" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="217"/>
       <c r="B27" s="217"/>
       <c r="C27" s="217"/>
@@ -21876,8 +21928,10 @@
       <c r="P27" s="216"/>
       <c r="Q27" s="216"/>
       <c r="R27" s="216"/>
-    </row>
-    <row r="28" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S27" s="216"/>
+      <c r="T27" s="216"/>
+    </row>
+    <row r="28" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="217"/>
       <c r="B28" s="217"/>
       <c r="C28" s="217"/>
@@ -21896,8 +21950,10 @@
       <c r="P28" s="216"/>
       <c r="Q28" s="216"/>
       <c r="R28" s="216"/>
-    </row>
-    <row r="29" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S28" s="216"/>
+      <c r="T28" s="216"/>
+    </row>
+    <row r="29" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="217"/>
       <c r="B29" s="217"/>
       <c r="C29" s="217"/>
@@ -21916,8 +21972,10 @@
       <c r="P29" s="216"/>
       <c r="Q29" s="216"/>
       <c r="R29" s="216"/>
-    </row>
-    <row r="30" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S29" s="216"/>
+      <c r="T29" s="216"/>
+    </row>
+    <row r="30" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="217"/>
       <c r="B30" s="217"/>
       <c r="C30" s="217"/>
@@ -21936,8 +21994,10 @@
       <c r="P30" s="216"/>
       <c r="Q30" s="216"/>
       <c r="R30" s="216"/>
-    </row>
-    <row r="31" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S30" s="216"/>
+      <c r="T30" s="216"/>
+    </row>
+    <row r="31" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="217"/>
       <c r="B31" s="217"/>
       <c r="C31" s="217"/>
@@ -21956,8 +22016,10 @@
       <c r="P31" s="216"/>
       <c r="Q31" s="216"/>
       <c r="R31" s="216"/>
-    </row>
-    <row r="32" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S31" s="216"/>
+      <c r="T31" s="216"/>
+    </row>
+    <row r="32" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="217"/>
       <c r="B32" s="217"/>
       <c r="C32" s="217"/>
@@ -21976,8 +22038,10 @@
       <c r="P32" s="216"/>
       <c r="Q32" s="216"/>
       <c r="R32" s="216"/>
-    </row>
-    <row r="33" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S32" s="216"/>
+      <c r="T32" s="216"/>
+    </row>
+    <row r="33" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="217"/>
       <c r="B33" s="217"/>
       <c r="C33" s="217"/>
@@ -21996,8 +22060,10 @@
       <c r="P33" s="216"/>
       <c r="Q33" s="216"/>
       <c r="R33" s="216"/>
-    </row>
-    <row r="34" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S33" s="216"/>
+      <c r="T33" s="216"/>
+    </row>
+    <row r="34" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="217"/>
       <c r="B34" s="217"/>
       <c r="C34" s="217"/>
@@ -22016,8 +22082,10 @@
       <c r="P34" s="216"/>
       <c r="Q34" s="216"/>
       <c r="R34" s="216"/>
-    </row>
-    <row r="35" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S34" s="216"/>
+      <c r="T34" s="216"/>
+    </row>
+    <row r="35" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="217"/>
       <c r="B35" s="217"/>
       <c r="C35" s="217"/>
@@ -22036,8 +22104,10 @@
       <c r="P35" s="216"/>
       <c r="Q35" s="216"/>
       <c r="R35" s="216"/>
-    </row>
-    <row r="36" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S35" s="216"/>
+      <c r="T35" s="216"/>
+    </row>
+    <row r="36" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="217"/>
       <c r="B36" s="217"/>
       <c r="C36" s="217"/>
@@ -22056,8 +22126,10 @@
       <c r="P36" s="216"/>
       <c r="Q36" s="216"/>
       <c r="R36" s="216"/>
-    </row>
-    <row r="37" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S36" s="216"/>
+      <c r="T36" s="216"/>
+    </row>
+    <row r="37" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="217"/>
       <c r="B37" s="217"/>
       <c r="C37" s="217"/>
@@ -22076,8 +22148,10 @@
       <c r="P37" s="216"/>
       <c r="Q37" s="216"/>
       <c r="R37" s="216"/>
-    </row>
-    <row r="38" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S37" s="216"/>
+      <c r="T37" s="216"/>
+    </row>
+    <row r="38" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="217"/>
       <c r="B38" s="217"/>
       <c r="C38" s="217"/>
@@ -22096,8 +22170,10 @@
       <c r="P38" s="216"/>
       <c r="Q38" s="216"/>
       <c r="R38" s="216"/>
-    </row>
-    <row r="39" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S38" s="216"/>
+      <c r="T38" s="216"/>
+    </row>
+    <row r="39" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="217"/>
       <c r="B39" s="217"/>
       <c r="C39" s="217"/>
@@ -22116,8 +22192,10 @@
       <c r="P39" s="216"/>
       <c r="Q39" s="216"/>
       <c r="R39" s="216"/>
-    </row>
-    <row r="40" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S39" s="216"/>
+      <c r="T39" s="216"/>
+    </row>
+    <row r="40" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="217"/>
       <c r="B40" s="217"/>
       <c r="C40" s="217"/>
@@ -22136,8 +22214,10 @@
       <c r="P40" s="216"/>
       <c r="Q40" s="216"/>
       <c r="R40" s="216"/>
-    </row>
-    <row r="41" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S40" s="216"/>
+      <c r="T40" s="216"/>
+    </row>
+    <row r="41" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="217"/>
       <c r="B41" s="217"/>
       <c r="C41" s="217"/>
@@ -22156,8 +22236,10 @@
       <c r="P41" s="216"/>
       <c r="Q41" s="216"/>
       <c r="R41" s="216"/>
-    </row>
-    <row r="42" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S41" s="216"/>
+      <c r="T41" s="216"/>
+    </row>
+    <row r="42" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="217"/>
       <c r="B42" s="217"/>
       <c r="C42" s="217"/>
@@ -22176,8 +22258,10 @@
       <c r="P42" s="216"/>
       <c r="Q42" s="216"/>
       <c r="R42" s="216"/>
-    </row>
-    <row r="43" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S42" s="216"/>
+      <c r="T42" s="216"/>
+    </row>
+    <row r="43" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="217"/>
       <c r="B43" s="217"/>
       <c r="C43" s="217"/>
@@ -22196,8 +22280,10 @@
       <c r="P43" s="216"/>
       <c r="Q43" s="216"/>
       <c r="R43" s="216"/>
-    </row>
-    <row r="44" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S43" s="216"/>
+      <c r="T43" s="216"/>
+    </row>
+    <row r="44" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="217"/>
       <c r="B44" s="217"/>
       <c r="C44" s="217"/>
@@ -22216,8 +22302,10 @@
       <c r="P44" s="216"/>
       <c r="Q44" s="216"/>
       <c r="R44" s="216"/>
-    </row>
-    <row r="45" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S44" s="216"/>
+      <c r="T44" s="216"/>
+    </row>
+    <row r="45" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="217"/>
       <c r="B45" s="217"/>
       <c r="C45" s="217"/>
@@ -22236,8 +22324,10 @@
       <c r="P45" s="216"/>
       <c r="Q45" s="216"/>
       <c r="R45" s="216"/>
-    </row>
-    <row r="46" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S45" s="216"/>
+      <c r="T45" s="216"/>
+    </row>
+    <row r="46" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="217"/>
       <c r="B46" s="217"/>
       <c r="C46" s="217"/>
@@ -22256,8 +22346,10 @@
       <c r="P46" s="216"/>
       <c r="Q46" s="216"/>
       <c r="R46" s="216"/>
-    </row>
-    <row r="47" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S46" s="216"/>
+      <c r="T46" s="216"/>
+    </row>
+    <row r="47" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="217"/>
       <c r="B47" s="217"/>
       <c r="C47" s="217"/>
@@ -22276,8 +22368,10 @@
       <c r="P47" s="216"/>
       <c r="Q47" s="216"/>
       <c r="R47" s="216"/>
-    </row>
-    <row r="48" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S47" s="216"/>
+      <c r="T47" s="216"/>
+    </row>
+    <row r="48" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="217"/>
       <c r="B48" s="217"/>
       <c r="C48" s="217"/>
@@ -22296,8 +22390,10 @@
       <c r="P48" s="216"/>
       <c r="Q48" s="216"/>
       <c r="R48" s="216"/>
-    </row>
-    <row r="49" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S48" s="216"/>
+      <c r="T48" s="216"/>
+    </row>
+    <row r="49" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="217"/>
       <c r="B49" s="217"/>
       <c r="C49" s="217"/>
@@ -22316,8 +22412,10 @@
       <c r="P49" s="216"/>
       <c r="Q49" s="216"/>
       <c r="R49" s="216"/>
-    </row>
-    <row r="50" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S49" s="216"/>
+      <c r="T49" s="216"/>
+    </row>
+    <row r="50" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="217"/>
       <c r="B50" s="217"/>
       <c r="C50" s="217"/>
@@ -22336,8 +22434,10 @@
       <c r="P50" s="216"/>
       <c r="Q50" s="216"/>
       <c r="R50" s="216"/>
-    </row>
-    <row r="51" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S50" s="216"/>
+      <c r="T50" s="216"/>
+    </row>
+    <row r="51" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="217"/>
       <c r="B51" s="217"/>
       <c r="C51" s="217"/>
@@ -22356,8 +22456,10 @@
       <c r="P51" s="216"/>
       <c r="Q51" s="216"/>
       <c r="R51" s="216"/>
-    </row>
-    <row r="52" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S51" s="216"/>
+      <c r="T51" s="216"/>
+    </row>
+    <row r="52" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="217"/>
       <c r="B52" s="217"/>
       <c r="C52" s="217"/>
@@ -22376,8 +22478,10 @@
       <c r="P52" s="216"/>
       <c r="Q52" s="216"/>
       <c r="R52" s="216"/>
-    </row>
-    <row r="53" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S52" s="216"/>
+      <c r="T52" s="216"/>
+    </row>
+    <row r="53" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="217"/>
       <c r="B53" s="217"/>
       <c r="C53" s="217"/>
@@ -22396,8 +22500,10 @@
       <c r="P53" s="216"/>
       <c r="Q53" s="216"/>
       <c r="R53" s="216"/>
-    </row>
-    <row r="54" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S53" s="216"/>
+      <c r="T53" s="216"/>
+    </row>
+    <row r="54" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="217"/>
       <c r="B54" s="217"/>
       <c r="C54" s="217"/>
@@ -22416,8 +22522,10 @@
       <c r="P54" s="216"/>
       <c r="Q54" s="216"/>
       <c r="R54" s="216"/>
-    </row>
-    <row r="55" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S54" s="216"/>
+      <c r="T54" s="216"/>
+    </row>
+    <row r="55" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="217"/>
       <c r="B55" s="217"/>
       <c r="C55" s="217"/>
@@ -22436,8 +22544,10 @@
       <c r="P55" s="216"/>
       <c r="Q55" s="216"/>
       <c r="R55" s="216"/>
-    </row>
-    <row r="56" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S55" s="216"/>
+      <c r="T55" s="216"/>
+    </row>
+    <row r="56" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="217"/>
       <c r="B56" s="217"/>
       <c r="C56" s="217"/>
@@ -22456,8 +22566,10 @@
       <c r="P56" s="216"/>
       <c r="Q56" s="216"/>
       <c r="R56" s="216"/>
-    </row>
-    <row r="57" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S56" s="216"/>
+      <c r="T56" s="216"/>
+    </row>
+    <row r="57" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="217"/>
       <c r="B57" s="217"/>
       <c r="C57" s="217"/>
@@ -22476,8 +22588,10 @@
       <c r="P57" s="216"/>
       <c r="Q57" s="216"/>
       <c r="R57" s="216"/>
-    </row>
-    <row r="58" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S57" s="216"/>
+      <c r="T57" s="216"/>
+    </row>
+    <row r="58" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="217"/>
       <c r="B58" s="217"/>
       <c r="C58" s="217"/>
@@ -22496,8 +22610,10 @@
       <c r="P58" s="216"/>
       <c r="Q58" s="216"/>
       <c r="R58" s="216"/>
-    </row>
-    <row r="59" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S58" s="216"/>
+      <c r="T58" s="216"/>
+    </row>
+    <row r="59" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="217"/>
       <c r="B59" s="217"/>
       <c r="C59" s="217"/>
@@ -22516,8 +22632,10 @@
       <c r="P59" s="216"/>
       <c r="Q59" s="216"/>
       <c r="R59" s="216"/>
-    </row>
-    <row r="60" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S59" s="216"/>
+      <c r="T59" s="216"/>
+    </row>
+    <row r="60" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="217"/>
       <c r="B60" s="217"/>
       <c r="C60" s="217"/>
@@ -22536,8 +22654,10 @@
       <c r="P60" s="216"/>
       <c r="Q60" s="216"/>
       <c r="R60" s="216"/>
-    </row>
-    <row r="61" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S60" s="216"/>
+      <c r="T60" s="216"/>
+    </row>
+    <row r="61" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="217"/>
       <c r="B61" s="217"/>
       <c r="C61" s="217"/>
@@ -22556,8 +22676,10 @@
       <c r="P61" s="216"/>
       <c r="Q61" s="216"/>
       <c r="R61" s="216"/>
-    </row>
-    <row r="62" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S61" s="216"/>
+      <c r="T61" s="216"/>
+    </row>
+    <row r="62" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="217"/>
       <c r="B62" s="217"/>
       <c r="C62" s="217"/>
@@ -22576,8 +22698,10 @@
       <c r="P62" s="216"/>
       <c r="Q62" s="216"/>
       <c r="R62" s="216"/>
-    </row>
-    <row r="63" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S62" s="216"/>
+      <c r="T62" s="216"/>
+    </row>
+    <row r="63" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="217"/>
       <c r="B63" s="217"/>
       <c r="C63" s="217"/>
@@ -22596,8 +22720,10 @@
       <c r="P63" s="216"/>
       <c r="Q63" s="216"/>
       <c r="R63" s="216"/>
-    </row>
-    <row r="64" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S63" s="216"/>
+      <c r="T63" s="216"/>
+    </row>
+    <row r="64" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="217"/>
       <c r="B64" s="217"/>
       <c r="C64" s="217"/>
@@ -22616,8 +22742,10 @@
       <c r="P64" s="216"/>
       <c r="Q64" s="216"/>
       <c r="R64" s="216"/>
-    </row>
-    <row r="65" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S64" s="216"/>
+      <c r="T64" s="216"/>
+    </row>
+    <row r="65" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="217"/>
       <c r="B65" s="217"/>
       <c r="C65" s="217"/>
@@ -22636,8 +22764,10 @@
       <c r="P65" s="216"/>
       <c r="Q65" s="216"/>
       <c r="R65" s="216"/>
-    </row>
-    <row r="66" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S65" s="216"/>
+      <c r="T65" s="216"/>
+    </row>
+    <row r="66" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="217"/>
       <c r="B66" s="217"/>
       <c r="C66" s="217"/>
@@ -22656,8 +22786,10 @@
       <c r="P66" s="216"/>
       <c r="Q66" s="216"/>
       <c r="R66" s="216"/>
-    </row>
-    <row r="67" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S66" s="216"/>
+      <c r="T66" s="216"/>
+    </row>
+    <row r="67" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="217"/>
       <c r="B67" s="217"/>
       <c r="C67" s="217"/>
@@ -22676,8 +22808,10 @@
       <c r="P67" s="216"/>
       <c r="Q67" s="216"/>
       <c r="R67" s="216"/>
-    </row>
-    <row r="68" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S67" s="216"/>
+      <c r="T67" s="216"/>
+    </row>
+    <row r="68" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="217"/>
       <c r="B68" s="217"/>
       <c r="C68" s="217"/>
@@ -22696,8 +22830,10 @@
       <c r="P68" s="216"/>
       <c r="Q68" s="216"/>
       <c r="R68" s="216"/>
-    </row>
-    <row r="69" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S68" s="216"/>
+      <c r="T68" s="216"/>
+    </row>
+    <row r="69" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="217"/>
       <c r="B69" s="217"/>
       <c r="C69" s="217"/>
@@ -22716,8 +22852,10 @@
       <c r="P69" s="216"/>
       <c r="Q69" s="216"/>
       <c r="R69" s="216"/>
-    </row>
-    <row r="70" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S69" s="216"/>
+      <c r="T69" s="216"/>
+    </row>
+    <row r="70" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="217"/>
       <c r="B70" s="217"/>
       <c r="C70" s="217"/>
@@ -22736,8 +22874,10 @@
       <c r="P70" s="216"/>
       <c r="Q70" s="216"/>
       <c r="R70" s="216"/>
-    </row>
-    <row r="71" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S70" s="216"/>
+      <c r="T70" s="216"/>
+    </row>
+    <row r="71" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="217"/>
       <c r="B71" s="217"/>
       <c r="C71" s="217"/>
@@ -22756,8 +22896,10 @@
       <c r="P71" s="216"/>
       <c r="Q71" s="216"/>
       <c r="R71" s="216"/>
-    </row>
-    <row r="72" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S71" s="216"/>
+      <c r="T71" s="216"/>
+    </row>
+    <row r="72" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="217"/>
       <c r="B72" s="217"/>
       <c r="C72" s="217"/>
@@ -22776,8 +22918,10 @@
       <c r="P72" s="216"/>
       <c r="Q72" s="216"/>
       <c r="R72" s="216"/>
-    </row>
-    <row r="73" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S72" s="216"/>
+      <c r="T72" s="216"/>
+    </row>
+    <row r="73" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="217"/>
       <c r="B73" s="217"/>
       <c r="C73" s="217"/>
@@ -22796,8 +22940,10 @@
       <c r="P73" s="216"/>
       <c r="Q73" s="216"/>
       <c r="R73" s="216"/>
-    </row>
-    <row r="74" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S73" s="216"/>
+      <c r="T73" s="216"/>
+    </row>
+    <row r="74" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="217"/>
       <c r="B74" s="217"/>
       <c r="C74" s="217"/>
@@ -22816,8 +22962,10 @@
       <c r="P74" s="216"/>
       <c r="Q74" s="216"/>
       <c r="R74" s="216"/>
-    </row>
-    <row r="75" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S74" s="216"/>
+      <c r="T74" s="216"/>
+    </row>
+    <row r="75" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="217"/>
       <c r="B75" s="217"/>
       <c r="C75" s="217"/>
@@ -22836,8 +22984,10 @@
       <c r="P75" s="216"/>
       <c r="Q75" s="216"/>
       <c r="R75" s="216"/>
-    </row>
-    <row r="76" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S75" s="216"/>
+      <c r="T75" s="216"/>
+    </row>
+    <row r="76" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="217"/>
       <c r="B76" s="217"/>
       <c r="C76" s="217"/>
@@ -22856,8 +23006,10 @@
       <c r="P76" s="216"/>
       <c r="Q76" s="216"/>
       <c r="R76" s="216"/>
-    </row>
-    <row r="77" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S76" s="216"/>
+      <c r="T76" s="216"/>
+    </row>
+    <row r="77" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="217"/>
       <c r="B77" s="217"/>
       <c r="C77" s="217"/>
@@ -22876,8 +23028,10 @@
       <c r="P77" s="216"/>
       <c r="Q77" s="216"/>
       <c r="R77" s="216"/>
-    </row>
-    <row r="78" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S77" s="216"/>
+      <c r="T77" s="216"/>
+    </row>
+    <row r="78" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="217"/>
       <c r="B78" s="217"/>
       <c r="C78" s="217"/>
@@ -22896,8 +23050,10 @@
       <c r="P78" s="216"/>
       <c r="Q78" s="216"/>
       <c r="R78" s="216"/>
-    </row>
-    <row r="79" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S78" s="216"/>
+      <c r="T78" s="216"/>
+    </row>
+    <row r="79" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="217"/>
       <c r="B79" s="217"/>
       <c r="C79" s="217"/>
@@ -22916,8 +23072,10 @@
       <c r="P79" s="216"/>
       <c r="Q79" s="216"/>
       <c r="R79" s="216"/>
-    </row>
-    <row r="80" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S79" s="216"/>
+      <c r="T79" s="216"/>
+    </row>
+    <row r="80" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="217"/>
       <c r="B80" s="217"/>
       <c r="C80" s="217"/>
@@ -22936,8 +23094,10 @@
       <c r="P80" s="216"/>
       <c r="Q80" s="216"/>
       <c r="R80" s="216"/>
-    </row>
-    <row r="81" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S80" s="216"/>
+      <c r="T80" s="216"/>
+    </row>
+    <row r="81" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="217"/>
       <c r="B81" s="217"/>
       <c r="C81" s="217"/>
@@ -22956,8 +23116,10 @@
       <c r="P81" s="216"/>
       <c r="Q81" s="216"/>
       <c r="R81" s="216"/>
-    </row>
-    <row r="82" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S81" s="216"/>
+      <c r="T81" s="216"/>
+    </row>
+    <row r="82" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="217"/>
       <c r="B82" s="217"/>
       <c r="C82" s="217"/>
@@ -22976,8 +23138,10 @@
       <c r="P82" s="216"/>
       <c r="Q82" s="216"/>
       <c r="R82" s="216"/>
-    </row>
-    <row r="83" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S82" s="216"/>
+      <c r="T82" s="216"/>
+    </row>
+    <row r="83" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="217"/>
       <c r="B83" s="217"/>
       <c r="C83" s="217"/>
@@ -22996,8 +23160,10 @@
       <c r="P83" s="216"/>
       <c r="Q83" s="216"/>
       <c r="R83" s="216"/>
-    </row>
-    <row r="84" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S83" s="216"/>
+      <c r="T83" s="216"/>
+    </row>
+    <row r="84" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="217"/>
       <c r="B84" s="217"/>
       <c r="C84" s="217"/>
@@ -23016,8 +23182,10 @@
       <c r="P84" s="216"/>
       <c r="Q84" s="216"/>
       <c r="R84" s="216"/>
-    </row>
-    <row r="85" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S84" s="216"/>
+      <c r="T84" s="216"/>
+    </row>
+    <row r="85" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="217"/>
       <c r="B85" s="217"/>
       <c r="C85" s="217"/>
@@ -23036,8 +23204,10 @@
       <c r="P85" s="216"/>
       <c r="Q85" s="216"/>
       <c r="R85" s="216"/>
-    </row>
-    <row r="86" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S85" s="216"/>
+      <c r="T85" s="216"/>
+    </row>
+    <row r="86" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="217"/>
       <c r="B86" s="217"/>
       <c r="C86" s="217"/>
@@ -23056,8 +23226,10 @@
       <c r="P86" s="216"/>
       <c r="Q86" s="216"/>
       <c r="R86" s="216"/>
-    </row>
-    <row r="87" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S86" s="216"/>
+      <c r="T86" s="216"/>
+    </row>
+    <row r="87" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="217"/>
       <c r="B87" s="217"/>
       <c r="C87" s="217"/>
@@ -23076,8 +23248,10 @@
       <c r="P87" s="216"/>
       <c r="Q87" s="216"/>
       <c r="R87" s="216"/>
-    </row>
-    <row r="88" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S87" s="216"/>
+      <c r="T87" s="216"/>
+    </row>
+    <row r="88" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="217"/>
       <c r="B88" s="217"/>
       <c r="C88" s="217"/>
@@ -23096,8 +23270,10 @@
       <c r="P88" s="216"/>
       <c r="Q88" s="216"/>
       <c r="R88" s="216"/>
-    </row>
-    <row r="89" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S88" s="216"/>
+      <c r="T88" s="216"/>
+    </row>
+    <row r="89" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="217"/>
       <c r="B89" s="217"/>
       <c r="C89" s="217"/>
@@ -23116,8 +23292,10 @@
       <c r="P89" s="216"/>
       <c r="Q89" s="216"/>
       <c r="R89" s="216"/>
-    </row>
-    <row r="90" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S89" s="216"/>
+      <c r="T89" s="216"/>
+    </row>
+    <row r="90" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="217"/>
       <c r="B90" s="217"/>
       <c r="C90" s="217"/>
@@ -23136,8 +23314,10 @@
       <c r="P90" s="216"/>
       <c r="Q90" s="216"/>
       <c r="R90" s="216"/>
-    </row>
-    <row r="91" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S90" s="216"/>
+      <c r="T90" s="216"/>
+    </row>
+    <row r="91" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="217"/>
       <c r="B91" s="217"/>
       <c r="C91" s="217"/>
@@ -23156,8 +23336,10 @@
       <c r="P91" s="216"/>
       <c r="Q91" s="216"/>
       <c r="R91" s="216"/>
-    </row>
-    <row r="92" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S91" s="216"/>
+      <c r="T91" s="216"/>
+    </row>
+    <row r="92" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="217"/>
       <c r="B92" s="217"/>
       <c r="C92" s="217"/>
@@ -23176,8 +23358,10 @@
       <c r="P92" s="216"/>
       <c r="Q92" s="216"/>
       <c r="R92" s="216"/>
-    </row>
-    <row r="93" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S92" s="216"/>
+      <c r="T92" s="216"/>
+    </row>
+    <row r="93" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="217"/>
       <c r="B93" s="217"/>
       <c r="C93" s="217"/>
@@ -23196,8 +23380,10 @@
       <c r="P93" s="216"/>
       <c r="Q93" s="216"/>
       <c r="R93" s="216"/>
-    </row>
-    <row r="94" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S93" s="216"/>
+      <c r="T93" s="216"/>
+    </row>
+    <row r="94" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="217"/>
       <c r="B94" s="217"/>
       <c r="C94" s="217"/>
@@ -23216,8 +23402,10 @@
       <c r="P94" s="216"/>
       <c r="Q94" s="216"/>
       <c r="R94" s="216"/>
-    </row>
-    <row r="95" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S94" s="216"/>
+      <c r="T94" s="216"/>
+    </row>
+    <row r="95" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="217"/>
       <c r="B95" s="217"/>
       <c r="C95" s="217"/>
@@ -23236,8 +23424,10 @@
       <c r="P95" s="216"/>
       <c r="Q95" s="216"/>
       <c r="R95" s="216"/>
-    </row>
-    <row r="96" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S95" s="216"/>
+      <c r="T95" s="216"/>
+    </row>
+    <row r="96" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="217"/>
       <c r="B96" s="217"/>
       <c r="C96" s="217"/>
@@ -23256,8 +23446,10 @@
       <c r="P96" s="216"/>
       <c r="Q96" s="216"/>
       <c r="R96" s="216"/>
-    </row>
-    <row r="97" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S96" s="216"/>
+      <c r="T96" s="216"/>
+    </row>
+    <row r="97" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="217"/>
       <c r="B97" s="217"/>
       <c r="C97" s="217"/>
@@ -23276,8 +23468,10 @@
       <c r="P97" s="216"/>
       <c r="Q97" s="216"/>
       <c r="R97" s="216"/>
-    </row>
-    <row r="98" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S97" s="216"/>
+      <c r="T97" s="216"/>
+    </row>
+    <row r="98" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="217"/>
       <c r="B98" s="217"/>
       <c r="C98" s="217"/>
@@ -23296,8 +23490,10 @@
       <c r="P98" s="216"/>
       <c r="Q98" s="216"/>
       <c r="R98" s="216"/>
-    </row>
-    <row r="99" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S98" s="216"/>
+      <c r="T98" s="216"/>
+    </row>
+    <row r="99" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="217"/>
       <c r="B99" s="217"/>
       <c r="C99" s="217"/>
@@ -23316,8 +23512,10 @@
       <c r="P99" s="216"/>
       <c r="Q99" s="216"/>
       <c r="R99" s="216"/>
-    </row>
-    <row r="100" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S99" s="216"/>
+      <c r="T99" s="216"/>
+    </row>
+    <row r="100" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="217"/>
       <c r="B100" s="217"/>
       <c r="C100" s="217"/>
@@ -23336,8 +23534,10 @@
       <c r="P100" s="216"/>
       <c r="Q100" s="216"/>
       <c r="R100" s="216"/>
-    </row>
-    <row r="101" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S100" s="216"/>
+      <c r="T100" s="216"/>
+    </row>
+    <row r="101" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="217"/>
       <c r="B101" s="217"/>
       <c r="C101" s="217"/>
@@ -23356,8 +23556,10 @@
       <c r="P101" s="216"/>
       <c r="Q101" s="216"/>
       <c r="R101" s="216"/>
-    </row>
-    <row r="102" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S101" s="216"/>
+      <c r="T101" s="216"/>
+    </row>
+    <row r="102" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="217"/>
       <c r="B102" s="217"/>
       <c r="C102" s="217"/>
@@ -23376,8 +23578,10 @@
       <c r="P102" s="216"/>
       <c r="Q102" s="216"/>
       <c r="R102" s="216"/>
-    </row>
-    <row r="103" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S102" s="216"/>
+      <c r="T102" s="216"/>
+    </row>
+    <row r="103" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="217"/>
       <c r="B103" s="217"/>
       <c r="C103" s="217"/>
@@ -23396,8 +23600,10 @@
       <c r="P103" s="216"/>
       <c r="Q103" s="216"/>
       <c r="R103" s="216"/>
-    </row>
-    <row r="104" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S103" s="216"/>
+      <c r="T103" s="216"/>
+    </row>
+    <row r="104" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="217"/>
       <c r="B104" s="217"/>
       <c r="C104" s="217"/>
@@ -23416,8 +23622,10 @@
       <c r="P104" s="216"/>
       <c r="Q104" s="216"/>
       <c r="R104" s="216"/>
-    </row>
-    <row r="105" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S104" s="216"/>
+      <c r="T104" s="216"/>
+    </row>
+    <row r="105" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="217"/>
       <c r="B105" s="217"/>
       <c r="C105" s="217"/>
@@ -23436,8 +23644,10 @@
       <c r="P105" s="216"/>
       <c r="Q105" s="216"/>
       <c r="R105" s="216"/>
-    </row>
-    <row r="106" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S105" s="216"/>
+      <c r="T105" s="216"/>
+    </row>
+    <row r="106" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="217"/>
       <c r="B106" s="217"/>
       <c r="C106" s="217"/>
@@ -23456,8 +23666,10 @@
       <c r="P106" s="216"/>
       <c r="Q106" s="216"/>
       <c r="R106" s="216"/>
-    </row>
-    <row r="107" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S106" s="216"/>
+      <c r="T106" s="216"/>
+    </row>
+    <row r="107" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="217"/>
       <c r="B107" s="217"/>
       <c r="C107" s="217"/>
@@ -23476,8 +23688,10 @@
       <c r="P107" s="216"/>
       <c r="Q107" s="216"/>
       <c r="R107" s="216"/>
-    </row>
-    <row r="108" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S107" s="216"/>
+      <c r="T107" s="216"/>
+    </row>
+    <row r="108" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="217"/>
       <c r="B108" s="217"/>
       <c r="C108" s="217"/>
@@ -23496,8 +23710,10 @@
       <c r="P108" s="216"/>
       <c r="Q108" s="216"/>
       <c r="R108" s="216"/>
-    </row>
-    <row r="109" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S108" s="216"/>
+      <c r="T108" s="216"/>
+    </row>
+    <row r="109" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" s="217"/>
       <c r="B109" s="217"/>
       <c r="C109" s="217"/>
@@ -23516,8 +23732,10 @@
       <c r="P109" s="216"/>
       <c r="Q109" s="216"/>
       <c r="R109" s="216"/>
-    </row>
-    <row r="110" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S109" s="216"/>
+      <c r="T109" s="216"/>
+    </row>
+    <row r="110" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="217"/>
       <c r="B110" s="217"/>
       <c r="C110" s="217"/>
@@ -23536,8 +23754,10 @@
       <c r="P110" s="216"/>
       <c r="Q110" s="216"/>
       <c r="R110" s="216"/>
-    </row>
-    <row r="111" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S110" s="216"/>
+      <c r="T110" s="216"/>
+    </row>
+    <row r="111" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="217"/>
       <c r="B111" s="217"/>
       <c r="C111" s="217"/>
@@ -23556,8 +23776,10 @@
       <c r="P111" s="216"/>
       <c r="Q111" s="216"/>
       <c r="R111" s="216"/>
-    </row>
-    <row r="112" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S111" s="216"/>
+      <c r="T111" s="216"/>
+    </row>
+    <row r="112" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A112" s="217"/>
       <c r="B112" s="217"/>
       <c r="C112" s="217"/>
@@ -23576,8 +23798,10 @@
       <c r="P112" s="216"/>
       <c r="Q112" s="216"/>
       <c r="R112" s="216"/>
-    </row>
-    <row r="113" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S112" s="216"/>
+      <c r="T112" s="216"/>
+    </row>
+    <row r="113" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="217"/>
       <c r="B113" s="217"/>
       <c r="C113" s="217"/>
@@ -23596,8 +23820,10 @@
       <c r="P113" s="216"/>
       <c r="Q113" s="216"/>
       <c r="R113" s="216"/>
-    </row>
-    <row r="114" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S113" s="216"/>
+      <c r="T113" s="216"/>
+    </row>
+    <row r="114" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="217"/>
       <c r="B114" s="217"/>
       <c r="C114" s="217"/>
@@ -23616,8 +23842,10 @@
       <c r="P114" s="216"/>
       <c r="Q114" s="216"/>
       <c r="R114" s="216"/>
-    </row>
-    <row r="115" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S114" s="216"/>
+      <c r="T114" s="216"/>
+    </row>
+    <row r="115" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A115" s="217"/>
       <c r="B115" s="217"/>
       <c r="C115" s="217"/>
@@ -23636,8 +23864,10 @@
       <c r="P115" s="216"/>
       <c r="Q115" s="216"/>
       <c r="R115" s="216"/>
-    </row>
-    <row r="116" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S115" s="216"/>
+      <c r="T115" s="216"/>
+    </row>
+    <row r="116" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A116" s="217"/>
       <c r="B116" s="217"/>
       <c r="C116" s="217"/>
@@ -23656,8 +23886,10 @@
       <c r="P116" s="216"/>
       <c r="Q116" s="216"/>
       <c r="R116" s="216"/>
-    </row>
-    <row r="117" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S116" s="216"/>
+      <c r="T116" s="216"/>
+    </row>
+    <row r="117" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A117" s="217"/>
       <c r="B117" s="217"/>
       <c r="C117" s="217"/>
@@ -23676,8 +23908,10 @@
       <c r="P117" s="216"/>
       <c r="Q117" s="216"/>
       <c r="R117" s="216"/>
-    </row>
-    <row r="118" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S117" s="216"/>
+      <c r="T117" s="216"/>
+    </row>
+    <row r="118" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A118" s="217"/>
       <c r="B118" s="217"/>
       <c r="C118" s="217"/>
@@ -23696,8 +23930,10 @@
       <c r="P118" s="216"/>
       <c r="Q118" s="216"/>
       <c r="R118" s="216"/>
-    </row>
-    <row r="119" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S118" s="216"/>
+      <c r="T118" s="216"/>
+    </row>
+    <row r="119" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A119" s="217"/>
       <c r="B119" s="217"/>
       <c r="C119" s="217"/>
@@ -23716,8 +23952,10 @@
       <c r="P119" s="216"/>
       <c r="Q119" s="216"/>
       <c r="R119" s="216"/>
-    </row>
-    <row r="120" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S119" s="216"/>
+      <c r="T119" s="216"/>
+    </row>
+    <row r="120" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A120" s="217"/>
       <c r="B120" s="217"/>
       <c r="C120" s="217"/>
@@ -23736,8 +23974,10 @@
       <c r="P120" s="216"/>
       <c r="Q120" s="216"/>
       <c r="R120" s="216"/>
-    </row>
-    <row r="121" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S120" s="216"/>
+      <c r="T120" s="216"/>
+    </row>
+    <row r="121" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A121" s="217"/>
       <c r="B121" s="217"/>
       <c r="C121" s="217"/>
@@ -23756,8 +23996,10 @@
       <c r="P121" s="216"/>
       <c r="Q121" s="216"/>
       <c r="R121" s="216"/>
-    </row>
-    <row r="122" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S121" s="216"/>
+      <c r="T121" s="216"/>
+    </row>
+    <row r="122" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A122" s="217"/>
       <c r="B122" s="217"/>
       <c r="C122" s="217"/>
@@ -23776,8 +24018,10 @@
       <c r="P122" s="216"/>
       <c r="Q122" s="216"/>
       <c r="R122" s="216"/>
-    </row>
-    <row r="123" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S122" s="216"/>
+      <c r="T122" s="216"/>
+    </row>
+    <row r="123" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A123" s="217"/>
       <c r="B123" s="217"/>
       <c r="C123" s="217"/>
@@ -23796,8 +24040,10 @@
       <c r="P123" s="216"/>
       <c r="Q123" s="216"/>
       <c r="R123" s="216"/>
-    </row>
-    <row r="124" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S123" s="216"/>
+      <c r="T123" s="216"/>
+    </row>
+    <row r="124" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A124" s="217"/>
       <c r="B124" s="217"/>
       <c r="C124" s="217"/>
@@ -23816,8 +24062,10 @@
       <c r="P124" s="216"/>
       <c r="Q124" s="216"/>
       <c r="R124" s="216"/>
-    </row>
-    <row r="125" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S124" s="216"/>
+      <c r="T124" s="216"/>
+    </row>
+    <row r="125" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A125" s="217"/>
       <c r="B125" s="217"/>
       <c r="C125" s="217"/>
@@ -23836,8 +24084,10 @@
       <c r="P125" s="216"/>
       <c r="Q125" s="216"/>
       <c r="R125" s="216"/>
-    </row>
-    <row r="126" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S125" s="216"/>
+      <c r="T125" s="216"/>
+    </row>
+    <row r="126" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A126" s="217"/>
       <c r="B126" s="217"/>
       <c r="C126" s="217"/>
@@ -23856,8 +24106,10 @@
       <c r="P126" s="216"/>
       <c r="Q126" s="216"/>
       <c r="R126" s="216"/>
-    </row>
-    <row r="127" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S126" s="216"/>
+      <c r="T126" s="216"/>
+    </row>
+    <row r="127" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A127" s="217"/>
       <c r="B127" s="217"/>
       <c r="C127" s="217"/>
@@ -23876,8 +24128,10 @@
       <c r="P127" s="216"/>
       <c r="Q127" s="216"/>
       <c r="R127" s="216"/>
-    </row>
-    <row r="128" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S127" s="216"/>
+      <c r="T127" s="216"/>
+    </row>
+    <row r="128" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A128" s="217"/>
       <c r="B128" s="217"/>
       <c r="C128" s="217"/>
@@ -23896,8 +24150,10 @@
       <c r="P128" s="216"/>
       <c r="Q128" s="216"/>
       <c r="R128" s="216"/>
-    </row>
-    <row r="129" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S128" s="216"/>
+      <c r="T128" s="216"/>
+    </row>
+    <row r="129" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A129" s="217"/>
       <c r="B129" s="217"/>
       <c r="C129" s="217"/>
@@ -23916,8 +24172,10 @@
       <c r="P129" s="216"/>
       <c r="Q129" s="216"/>
       <c r="R129" s="216"/>
-    </row>
-    <row r="130" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S129" s="216"/>
+      <c r="T129" s="216"/>
+    </row>
+    <row r="130" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A130" s="217"/>
       <c r="B130" s="217"/>
       <c r="C130" s="217"/>
@@ -23936,8 +24194,10 @@
       <c r="P130" s="216"/>
       <c r="Q130" s="216"/>
       <c r="R130" s="216"/>
-    </row>
-    <row r="131" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S130" s="216"/>
+      <c r="T130" s="216"/>
+    </row>
+    <row r="131" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A131" s="217"/>
       <c r="B131" s="217"/>
       <c r="C131" s="217"/>
@@ -23956,8 +24216,10 @@
       <c r="P131" s="216"/>
       <c r="Q131" s="216"/>
       <c r="R131" s="216"/>
-    </row>
-    <row r="132" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S131" s="216"/>
+      <c r="T131" s="216"/>
+    </row>
+    <row r="132" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A132" s="217"/>
       <c r="B132" s="217"/>
       <c r="C132" s="217"/>
@@ -23976,8 +24238,10 @@
       <c r="P132" s="216"/>
       <c r="Q132" s="216"/>
       <c r="R132" s="216"/>
-    </row>
-    <row r="133" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S132" s="216"/>
+      <c r="T132" s="216"/>
+    </row>
+    <row r="133" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A133" s="217"/>
       <c r="B133" s="217"/>
       <c r="C133" s="217"/>
@@ -23996,8 +24260,10 @@
       <c r="P133" s="216"/>
       <c r="Q133" s="216"/>
       <c r="R133" s="216"/>
-    </row>
-    <row r="134" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S133" s="216"/>
+      <c r="T133" s="216"/>
+    </row>
+    <row r="134" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A134" s="217"/>
       <c r="B134" s="217"/>
       <c r="C134" s="217"/>
@@ -24016,8 +24282,10 @@
       <c r="P134" s="216"/>
       <c r="Q134" s="216"/>
       <c r="R134" s="216"/>
-    </row>
-    <row r="135" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S134" s="216"/>
+      <c r="T134" s="216"/>
+    </row>
+    <row r="135" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A135" s="217"/>
       <c r="B135" s="217"/>
       <c r="C135" s="217"/>
@@ -24036,8 +24304,10 @@
       <c r="P135" s="216"/>
       <c r="Q135" s="216"/>
       <c r="R135" s="216"/>
-    </row>
-    <row r="136" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S135" s="216"/>
+      <c r="T135" s="216"/>
+    </row>
+    <row r="136" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A136" s="217"/>
       <c r="B136" s="217"/>
       <c r="C136" s="217"/>
@@ -24056,8 +24326,10 @@
       <c r="P136" s="216"/>
       <c r="Q136" s="216"/>
       <c r="R136" s="216"/>
-    </row>
-    <row r="137" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S136" s="216"/>
+      <c r="T136" s="216"/>
+    </row>
+    <row r="137" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A137" s="217"/>
       <c r="B137" s="217"/>
       <c r="C137" s="217"/>
@@ -24076,8 +24348,10 @@
       <c r="P137" s="216"/>
       <c r="Q137" s="216"/>
       <c r="R137" s="216"/>
-    </row>
-    <row r="138" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S137" s="216"/>
+      <c r="T137" s="216"/>
+    </row>
+    <row r="138" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A138" s="217"/>
       <c r="B138" s="217"/>
       <c r="C138" s="217"/>
@@ -24096,8 +24370,10 @@
       <c r="P138" s="216"/>
       <c r="Q138" s="216"/>
       <c r="R138" s="216"/>
-    </row>
-    <row r="139" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S138" s="216"/>
+      <c r="T138" s="216"/>
+    </row>
+    <row r="139" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A139" s="217"/>
       <c r="B139" s="217"/>
       <c r="C139" s="217"/>
@@ -24116,8 +24392,10 @@
       <c r="P139" s="216"/>
       <c r="Q139" s="216"/>
       <c r="R139" s="216"/>
-    </row>
-    <row r="140" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S139" s="216"/>
+      <c r="T139" s="216"/>
+    </row>
+    <row r="140" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A140" s="217"/>
       <c r="B140" s="217"/>
       <c r="C140" s="217"/>
@@ -24136,8 +24414,10 @@
       <c r="P140" s="216"/>
       <c r="Q140" s="216"/>
       <c r="R140" s="216"/>
-    </row>
-    <row r="141" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S140" s="216"/>
+      <c r="T140" s="216"/>
+    </row>
+    <row r="141" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A141" s="217"/>
       <c r="B141" s="217"/>
       <c r="C141" s="217"/>
@@ -24156,8 +24436,10 @@
       <c r="P141" s="216"/>
       <c r="Q141" s="216"/>
       <c r="R141" s="216"/>
-    </row>
-    <row r="142" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S141" s="216"/>
+      <c r="T141" s="216"/>
+    </row>
+    <row r="142" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A142" s="217"/>
       <c r="B142" s="217"/>
       <c r="C142" s="217"/>
@@ -24176,8 +24458,10 @@
       <c r="P142" s="216"/>
       <c r="Q142" s="216"/>
       <c r="R142" s="216"/>
-    </row>
-    <row r="143" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S142" s="216"/>
+      <c r="T142" s="216"/>
+    </row>
+    <row r="143" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A143" s="217"/>
       <c r="B143" s="217"/>
       <c r="C143" s="217"/>
@@ -24196,8 +24480,10 @@
       <c r="P143" s="216"/>
       <c r="Q143" s="216"/>
       <c r="R143" s="216"/>
-    </row>
-    <row r="144" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S143" s="216"/>
+      <c r="T143" s="216"/>
+    </row>
+    <row r="144" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A144" s="217"/>
       <c r="B144" s="217"/>
       <c r="C144" s="217"/>
@@ -24216,6 +24502,8 @@
       <c r="P144" s="216"/>
       <c r="Q144" s="216"/>
       <c r="R144" s="216"/>
+      <c r="S144" s="216"/>
+      <c r="T144" s="216"/>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" s="217"/>
@@ -24229,7 +24517,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="Q2:Q4"/>
+    <mergeCell ref="S2:S4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -24243,7 +24531,7 @@
   </sheetPr>
   <dimension ref="A1:BG22"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
@@ -29871,10 +30159,10 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:BJ17"/>
+  <dimension ref="A1:BL17"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -29882,10 +30170,10 @@
     <col min="1" max="3" width="0" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="16.83203125" customWidth="1"/>
     <col min="6" max="6" width="68.83203125" customWidth="1"/>
-    <col min="7" max="16" width="13.5" customWidth="1"/>
+    <col min="7" max="18" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" s="4" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:64" s="4" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -29905,8 +30193,8 @@
       <c r="O1" s="7"/>
       <c r="P1" s="7"/>
       <c r="Q1" s="7"/>
-      <c r="R1"/>
-      <c r="S1"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
       <c r="T1"/>
       <c r="U1"/>
       <c r="V1"/>
@@ -29950,8 +30238,10 @@
       <c r="BH1"/>
       <c r="BI1"/>
       <c r="BJ1"/>
-    </row>
-    <row r="2" spans="1:62" hidden="1" x14ac:dyDescent="0.2">
+      <c r="BK1"/>
+      <c r="BL1"/>
+    </row>
+    <row r="2" spans="1:64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="254"/>
       <c r="B2" s="207"/>
       <c r="C2" s="207"/>
@@ -29972,23 +30262,25 @@
       <c r="L2" s="208" t="s">
         <v>38</v>
       </c>
-      <c r="M2" s="208" t="s">
-        <v>38</v>
-      </c>
-      <c r="N2" s="208" t="s">
-        <v>38</v>
-      </c>
+      <c r="M2" s="208"/>
+      <c r="N2" s="208"/>
       <c r="O2" s="208" t="s">
         <v>38</v>
       </c>
       <c r="P2" s="208" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="418" t="s">
+      <c r="Q2" s="208" t="s">
+        <v>38</v>
+      </c>
+      <c r="R2" s="208" t="s">
+        <v>38</v>
+      </c>
+      <c r="S2" s="418" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="3" spans="1:62" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="254"/>
       <c r="B3" s="207"/>
       <c r="C3" s="207"/>
@@ -30009,21 +30301,23 @@
       <c r="L3" s="208" t="s">
         <v>144</v>
       </c>
-      <c r="M3" s="208" t="s">
+      <c r="M3" s="208"/>
+      <c r="N3" s="208"/>
+      <c r="O3" s="208" t="s">
         <v>275</v>
       </c>
-      <c r="N3" s="208" t="s">
+      <c r="P3" s="208" t="s">
         <v>276</v>
       </c>
-      <c r="O3" s="208" t="s">
+      <c r="Q3" s="208" t="s">
         <v>277</v>
       </c>
-      <c r="P3" s="208" t="s">
+      <c r="R3" s="208" t="s">
         <v>278</v>
       </c>
-      <c r="Q3" s="418"/>
-    </row>
-    <row r="4" spans="1:62" ht="36" x14ac:dyDescent="0.2">
+      <c r="S3" s="418"/>
+    </row>
+    <row r="4" spans="1:64" ht="36" x14ac:dyDescent="0.2">
       <c r="A4" s="255"/>
       <c r="B4" s="244" t="s">
         <v>112</v>
@@ -30059,20 +30353,26 @@
         <v>677</v>
       </c>
       <c r="M4" s="249" t="s">
+        <v>684</v>
+      </c>
+      <c r="N4" s="249" t="s">
+        <v>685</v>
+      </c>
+      <c r="O4" s="249" t="s">
         <v>678</v>
       </c>
-      <c r="N4" s="249" t="s">
+      <c r="P4" s="249" t="s">
         <v>679</v>
       </c>
-      <c r="O4" s="249" t="s">
+      <c r="Q4" s="249" t="s">
         <v>680</v>
       </c>
-      <c r="P4" s="249" t="s">
+      <c r="R4" s="249" t="s">
         <v>676</v>
       </c>
-      <c r="Q4" s="418"/>
-    </row>
-    <row r="5" spans="1:62" x14ac:dyDescent="0.2">
+      <c r="S4" s="418"/>
+    </row>
+    <row r="5" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A5" s="211" t="s">
         <v>290</v>
       </c>
@@ -30109,14 +30409,8 @@
         <f>IF(ISBLANK(ETPT_JUR_ASS!L5),"",IF(ISERROR(ETPT_JUR_ASS!L5),"",IF(ETPT_JUR_ASS!L5=0,"",ETPT_JUR_ASS!L5)))</f>
         <v/>
       </c>
-      <c r="M5" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_JUR_ASS!M5),"",IF(ISERROR(ETPT_JUR_ASS!M5),"",IF(ETPT_JUR_ASS!M5=0,"",ETPT_JUR_ASS!M5)))</f>
-        <v/>
-      </c>
-      <c r="N5" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_JUR_ASS!N5),"",IF(ISERROR(ETPT_JUR_ASS!N5),"",IF(ETPT_JUR_ASS!N5=0,"",ETPT_JUR_ASS!N5)))</f>
-        <v/>
-      </c>
+      <c r="M5" s="247"/>
+      <c r="N5" s="247"/>
       <c r="O5" s="247" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!O5),"",IF(ISERROR(ETPT_JUR_ASS!O5),"",IF(ETPT_JUR_ASS!O5=0,"",ETPT_JUR_ASS!O5)))</f>
         <v/>
@@ -30125,12 +30419,20 @@
         <f>IF(ISBLANK(ETPT_JUR_ASS!P5),"",IF(ISERROR(ETPT_JUR_ASS!P5),"",IF(ETPT_JUR_ASS!P5=0,"",ETPT_JUR_ASS!P5)))</f>
         <v/>
       </c>
-      <c r="Q5" s="214">
-        <f>ETPT_JUR_ASS!Q5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:62" x14ac:dyDescent="0.2">
+      <c r="Q5" s="247" t="str">
+        <f>IF(ISBLANK(ETPT_JUR_ASS!Q5),"",IF(ISERROR(ETPT_JUR_ASS!Q5),"",IF(ETPT_JUR_ASS!Q5=0,"",ETPT_JUR_ASS!Q5)))</f>
+        <v/>
+      </c>
+      <c r="R5" s="247" t="str">
+        <f>IF(ISBLANK(ETPT_JUR_ASS!R5),"",IF(ISERROR(ETPT_JUR_ASS!R5),"",IF(ETPT_JUR_ASS!R5=0,"",ETPT_JUR_ASS!R5)))</f>
+        <v/>
+      </c>
+      <c r="S5" s="214">
+        <f>ETPT_JUR_ASS!S5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A6" s="211" t="s">
         <v>290</v>
       </c>
@@ -30164,14 +30466,8 @@
         <f>IF(ISBLANK(ETPT_JUR_ASS!L6),"",IF(ISERROR(ETPT_JUR_ASS!L6),"",IF(ETPT_JUR_ASS!L6=0,"",ETPT_JUR_ASS!L6)))</f>
         <v/>
       </c>
-      <c r="M6" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_JUR_ASS!M6),"",IF(ISERROR(ETPT_JUR_ASS!M6),"",IF(ETPT_JUR_ASS!M6=0,"",ETPT_JUR_ASS!M6)))</f>
-        <v/>
-      </c>
-      <c r="N6" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_JUR_ASS!N6),"",IF(ISERROR(ETPT_JUR_ASS!N6),"",IF(ETPT_JUR_ASS!N6=0,"",ETPT_JUR_ASS!N6)))</f>
-        <v/>
-      </c>
+      <c r="M6" s="247"/>
+      <c r="N6" s="247"/>
       <c r="O6" s="247" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!O6),"",IF(ISERROR(ETPT_JUR_ASS!O6),"",IF(ETPT_JUR_ASS!O6=0,"",ETPT_JUR_ASS!O6)))</f>
         <v/>
@@ -30180,12 +30476,20 @@
         <f>IF(ISBLANK(ETPT_JUR_ASS!P6),"",IF(ISERROR(ETPT_JUR_ASS!P6),"",IF(ETPT_JUR_ASS!P6=0,"",ETPT_JUR_ASS!P6)))</f>
         <v/>
       </c>
-      <c r="Q6" s="214">
-        <f>ETPT_JUR_ASS!Q6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:62" x14ac:dyDescent="0.2">
+      <c r="Q6" s="247" t="str">
+        <f>IF(ISBLANK(ETPT_JUR_ASS!Q6),"",IF(ISERROR(ETPT_JUR_ASS!Q6),"",IF(ETPT_JUR_ASS!Q6=0,"",ETPT_JUR_ASS!Q6)))</f>
+        <v/>
+      </c>
+      <c r="R6" s="247" t="str">
+        <f>IF(ISBLANK(ETPT_JUR_ASS!R6),"",IF(ISERROR(ETPT_JUR_ASS!R6),"",IF(ETPT_JUR_ASS!R6=0,"",ETPT_JUR_ASS!R6)))</f>
+        <v/>
+      </c>
+      <c r="S6" s="214">
+        <f>ETPT_JUR_ASS!S6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A7" s="211" t="s">
         <v>290</v>
       </c>
@@ -30219,14 +30523,8 @@
         <f>IF(ISBLANK(ETPT_JUR_ASS!L7),"",IF(ISERROR(ETPT_JUR_ASS!L7),"",IF(ETPT_JUR_ASS!L7=0,"",ETPT_JUR_ASS!L7)))</f>
         <v/>
       </c>
-      <c r="M7" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_JUR_ASS!M7),"",IF(ISERROR(ETPT_JUR_ASS!M7),"",IF(ETPT_JUR_ASS!M7=0,"",ETPT_JUR_ASS!M7)))</f>
-        <v/>
-      </c>
-      <c r="N7" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_JUR_ASS!N7),"",IF(ISERROR(ETPT_JUR_ASS!N7),"",IF(ETPT_JUR_ASS!N7=0,"",ETPT_JUR_ASS!N7)))</f>
-        <v/>
-      </c>
+      <c r="M7" s="247"/>
+      <c r="N7" s="247"/>
       <c r="O7" s="247" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!O7),"",IF(ISERROR(ETPT_JUR_ASS!O7),"",IF(ETPT_JUR_ASS!O7=0,"",ETPT_JUR_ASS!O7)))</f>
         <v/>
@@ -30235,12 +30533,20 @@
         <f>IF(ISBLANK(ETPT_JUR_ASS!P7),"",IF(ISERROR(ETPT_JUR_ASS!P7),"",IF(ETPT_JUR_ASS!P7=0,"",ETPT_JUR_ASS!P7)))</f>
         <v/>
       </c>
-      <c r="Q7" s="214">
-        <f>ETPT_JUR_ASS!Q7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:62" x14ac:dyDescent="0.2">
+      <c r="Q7" s="247" t="str">
+        <f>IF(ISBLANK(ETPT_JUR_ASS!Q7),"",IF(ISERROR(ETPT_JUR_ASS!Q7),"",IF(ETPT_JUR_ASS!Q7=0,"",ETPT_JUR_ASS!Q7)))</f>
+        <v/>
+      </c>
+      <c r="R7" s="247" t="str">
+        <f>IF(ISBLANK(ETPT_JUR_ASS!R7),"",IF(ISERROR(ETPT_JUR_ASS!R7),"",IF(ETPT_JUR_ASS!R7=0,"",ETPT_JUR_ASS!R7)))</f>
+        <v/>
+      </c>
+      <c r="S7" s="214">
+        <f>ETPT_JUR_ASS!S7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A8" s="211" t="s">
         <v>290</v>
       </c>
@@ -30274,14 +30580,8 @@
         <f>IF(ISBLANK(ETPT_JUR_ASS!L8),"",IF(ISERROR(ETPT_JUR_ASS!L8),"",IF(ETPT_JUR_ASS!L8=0,"",ETPT_JUR_ASS!L8)))</f>
         <v/>
       </c>
-      <c r="M8" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_JUR_ASS!M8),"",IF(ISERROR(ETPT_JUR_ASS!M8),"",IF(ETPT_JUR_ASS!M8=0,"",ETPT_JUR_ASS!M8)))</f>
-        <v/>
-      </c>
-      <c r="N8" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_JUR_ASS!N8),"",IF(ISERROR(ETPT_JUR_ASS!N8),"",IF(ETPT_JUR_ASS!N8=0,"",ETPT_JUR_ASS!N8)))</f>
-        <v/>
-      </c>
+      <c r="M8" s="247"/>
+      <c r="N8" s="247"/>
       <c r="O8" s="247" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!O8),"",IF(ISERROR(ETPT_JUR_ASS!O8),"",IF(ETPT_JUR_ASS!O8=0,"",ETPT_JUR_ASS!O8)))</f>
         <v/>
@@ -30290,12 +30590,20 @@
         <f>IF(ISBLANK(ETPT_JUR_ASS!P8),"",IF(ISERROR(ETPT_JUR_ASS!P8),"",IF(ETPT_JUR_ASS!P8=0,"",ETPT_JUR_ASS!P8)))</f>
         <v/>
       </c>
-      <c r="Q8" s="214">
-        <f>ETPT_JUR_ASS!Q8</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:62" x14ac:dyDescent="0.2">
+      <c r="Q8" s="247" t="str">
+        <f>IF(ISBLANK(ETPT_JUR_ASS!Q8),"",IF(ISERROR(ETPT_JUR_ASS!Q8),"",IF(ETPT_JUR_ASS!Q8=0,"",ETPT_JUR_ASS!Q8)))</f>
+        <v/>
+      </c>
+      <c r="R8" s="247" t="str">
+        <f>IF(ISBLANK(ETPT_JUR_ASS!R8),"",IF(ISERROR(ETPT_JUR_ASS!R8),"",IF(ETPT_JUR_ASS!R8=0,"",ETPT_JUR_ASS!R8)))</f>
+        <v/>
+      </c>
+      <c r="S8" s="214">
+        <f>ETPT_JUR_ASS!S8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A9" s="211" t="s">
         <v>290</v>
       </c>
@@ -30329,14 +30637,8 @@
         <f>IF(ISBLANK(ETPT_JUR_ASS!L9),"",IF(ISERROR(ETPT_JUR_ASS!L9),"",IF(ETPT_JUR_ASS!L9=0,"",ETPT_JUR_ASS!L9)))</f>
         <v/>
       </c>
-      <c r="M9" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_JUR_ASS!M9),"",IF(ISERROR(ETPT_JUR_ASS!M9),"",IF(ETPT_JUR_ASS!M9=0,"",ETPT_JUR_ASS!M9)))</f>
-        <v/>
-      </c>
-      <c r="N9" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_JUR_ASS!N9),"",IF(ISERROR(ETPT_JUR_ASS!N9),"",IF(ETPT_JUR_ASS!N9=0,"",ETPT_JUR_ASS!N9)))</f>
-        <v/>
-      </c>
+      <c r="M9" s="247"/>
+      <c r="N9" s="247"/>
       <c r="O9" s="247" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!O9),"",IF(ISERROR(ETPT_JUR_ASS!O9),"",IF(ETPT_JUR_ASS!O9=0,"",ETPT_JUR_ASS!O9)))</f>
         <v/>
@@ -30345,12 +30647,20 @@
         <f>IF(ISBLANK(ETPT_JUR_ASS!P9),"",IF(ISERROR(ETPT_JUR_ASS!P9),"",IF(ETPT_JUR_ASS!P9=0,"",ETPT_JUR_ASS!P9)))</f>
         <v/>
       </c>
-      <c r="Q9" s="214">
-        <f>ETPT_JUR_ASS!Q9</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:62" x14ac:dyDescent="0.2">
+      <c r="Q9" s="247" t="str">
+        <f>IF(ISBLANK(ETPT_JUR_ASS!Q9),"",IF(ISERROR(ETPT_JUR_ASS!Q9),"",IF(ETPT_JUR_ASS!Q9=0,"",ETPT_JUR_ASS!Q9)))</f>
+        <v/>
+      </c>
+      <c r="R9" s="247" t="str">
+        <f>IF(ISBLANK(ETPT_JUR_ASS!R9),"",IF(ISERROR(ETPT_JUR_ASS!R9),"",IF(ETPT_JUR_ASS!R9=0,"",ETPT_JUR_ASS!R9)))</f>
+        <v/>
+      </c>
+      <c r="S9" s="214">
+        <f>ETPT_JUR_ASS!S9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A10" s="211" t="s">
         <v>290</v>
       </c>
@@ -30384,14 +30694,8 @@
         <f>IF(ISBLANK(ETPT_JUR_ASS!L10),"",IF(ISERROR(ETPT_JUR_ASS!L10),"",IF(ETPT_JUR_ASS!L10=0,"",ETPT_JUR_ASS!L10)))</f>
         <v/>
       </c>
-      <c r="M10" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_JUR_ASS!M10),"",IF(ISERROR(ETPT_JUR_ASS!M10),"",IF(ETPT_JUR_ASS!M10=0,"",ETPT_JUR_ASS!M10)))</f>
-        <v/>
-      </c>
-      <c r="N10" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_JUR_ASS!N10),"",IF(ISERROR(ETPT_JUR_ASS!N10),"",IF(ETPT_JUR_ASS!N10=0,"",ETPT_JUR_ASS!N10)))</f>
-        <v/>
-      </c>
+      <c r="M10" s="247"/>
+      <c r="N10" s="247"/>
       <c r="O10" s="247" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!O10),"",IF(ISERROR(ETPT_JUR_ASS!O10),"",IF(ETPT_JUR_ASS!O10=0,"",ETPT_JUR_ASS!O10)))</f>
         <v/>
@@ -30400,12 +30704,20 @@
         <f>IF(ISBLANK(ETPT_JUR_ASS!P10),"",IF(ISERROR(ETPT_JUR_ASS!P10),"",IF(ETPT_JUR_ASS!P10=0,"",ETPT_JUR_ASS!P10)))</f>
         <v/>
       </c>
-      <c r="Q10" s="214">
-        <f>ETPT_JUR_ASS!Q10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:62" x14ac:dyDescent="0.2">
+      <c r="Q10" s="247" t="str">
+        <f>IF(ISBLANK(ETPT_JUR_ASS!Q10),"",IF(ISERROR(ETPT_JUR_ASS!Q10),"",IF(ETPT_JUR_ASS!Q10=0,"",ETPT_JUR_ASS!Q10)))</f>
+        <v/>
+      </c>
+      <c r="R10" s="247" t="str">
+        <f>IF(ISBLANK(ETPT_JUR_ASS!R10),"",IF(ISERROR(ETPT_JUR_ASS!R10),"",IF(ETPT_JUR_ASS!R10=0,"",ETPT_JUR_ASS!R10)))</f>
+        <v/>
+      </c>
+      <c r="S10" s="214">
+        <f>ETPT_JUR_ASS!S10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A11" s="211" t="s">
         <v>290</v>
       </c>
@@ -30439,14 +30751,8 @@
         <f>IF(ISBLANK(ETPT_JUR_ASS!L11),"",IF(ISERROR(ETPT_JUR_ASS!L11),"",IF(ETPT_JUR_ASS!L11=0,"",ETPT_JUR_ASS!L11)))</f>
         <v/>
       </c>
-      <c r="M11" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_JUR_ASS!M11),"",IF(ISERROR(ETPT_JUR_ASS!M11),"",IF(ETPT_JUR_ASS!M11=0,"",ETPT_JUR_ASS!M11)))</f>
-        <v/>
-      </c>
-      <c r="N11" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_JUR_ASS!N11),"",IF(ISERROR(ETPT_JUR_ASS!N11),"",IF(ETPT_JUR_ASS!N11=0,"",ETPT_JUR_ASS!N11)))</f>
-        <v/>
-      </c>
+      <c r="M11" s="247"/>
+      <c r="N11" s="247"/>
       <c r="O11" s="247" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!O11),"",IF(ISERROR(ETPT_JUR_ASS!O11),"",IF(ETPT_JUR_ASS!O11=0,"",ETPT_JUR_ASS!O11)))</f>
         <v/>
@@ -30455,12 +30761,20 @@
         <f>IF(ISBLANK(ETPT_JUR_ASS!P11),"",IF(ISERROR(ETPT_JUR_ASS!P11),"",IF(ETPT_JUR_ASS!P11=0,"",ETPT_JUR_ASS!P11)))</f>
         <v/>
       </c>
-      <c r="Q11" s="214">
-        <f>ETPT_JUR_ASS!Q11</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:62" x14ac:dyDescent="0.2">
+      <c r="Q11" s="247" t="str">
+        <f>IF(ISBLANK(ETPT_JUR_ASS!Q11),"",IF(ISERROR(ETPT_JUR_ASS!Q11),"",IF(ETPT_JUR_ASS!Q11=0,"",ETPT_JUR_ASS!Q11)))</f>
+        <v/>
+      </c>
+      <c r="R11" s="247" t="str">
+        <f>IF(ISBLANK(ETPT_JUR_ASS!R11),"",IF(ISERROR(ETPT_JUR_ASS!R11),"",IF(ETPT_JUR_ASS!R11=0,"",ETPT_JUR_ASS!R11)))</f>
+        <v/>
+      </c>
+      <c r="S11" s="214">
+        <f>ETPT_JUR_ASS!S11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A12" s="211" t="s">
         <v>290</v>
       </c>
@@ -30494,14 +30808,8 @@
         <f>IF(ISBLANK(ETPT_JUR_ASS!L12),"",IF(ISERROR(ETPT_JUR_ASS!L12),"",IF(ETPT_JUR_ASS!L12=0,"",ETPT_JUR_ASS!L12)))</f>
         <v/>
       </c>
-      <c r="M12" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_JUR_ASS!M12),"",IF(ISERROR(ETPT_JUR_ASS!M12),"",IF(ETPT_JUR_ASS!M12=0,"",ETPT_JUR_ASS!M12)))</f>
-        <v/>
-      </c>
-      <c r="N12" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_JUR_ASS!N12),"",IF(ISERROR(ETPT_JUR_ASS!N12),"",IF(ETPT_JUR_ASS!N12=0,"",ETPT_JUR_ASS!N12)))</f>
-        <v/>
-      </c>
+      <c r="M12" s="247"/>
+      <c r="N12" s="247"/>
       <c r="O12" s="247" t="str">
         <f>IF(ISBLANK(ETPT_JUR_ASS!O12),"",IF(ISERROR(ETPT_JUR_ASS!O12),"",IF(ETPT_JUR_ASS!O12=0,"",ETPT_JUR_ASS!O12)))</f>
         <v/>
@@ -30510,12 +30818,20 @@
         <f>IF(ISBLANK(ETPT_JUR_ASS!P12),"",IF(ISERROR(ETPT_JUR_ASS!P12),"",IF(ETPT_JUR_ASS!P12=0,"",ETPT_JUR_ASS!P12)))</f>
         <v/>
       </c>
-      <c r="Q12" s="214">
-        <f>ETPT_JUR_ASS!Q12</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:62" x14ac:dyDescent="0.2">
+      <c r="Q12" s="247" t="str">
+        <f>IF(ISBLANK(ETPT_JUR_ASS!Q12),"",IF(ISERROR(ETPT_JUR_ASS!Q12),"",IF(ETPT_JUR_ASS!Q12=0,"",ETPT_JUR_ASS!Q12)))</f>
+        <v/>
+      </c>
+      <c r="R12" s="247" t="str">
+        <f>IF(ISBLANK(ETPT_JUR_ASS!R12),"",IF(ISERROR(ETPT_JUR_ASS!R12),"",IF(ETPT_JUR_ASS!R12=0,"",ETPT_JUR_ASS!R12)))</f>
+        <v/>
+      </c>
+      <c r="S12" s="214">
+        <f>ETPT_JUR_ASS!S12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A13" s="246"/>
       <c r="B13" s="246"/>
       <c r="C13" s="246"/>
@@ -30548,14 +30864,8 @@
         <f>ETPT_JUR_ASS!L13</f>
         <v>0</v>
       </c>
-      <c r="M13" s="214">
-        <f>ETPT_JUR_ASS!M13</f>
-        <v>0</v>
-      </c>
-      <c r="N13" s="214">
-        <f>ETPT_JUR_ASS!N13</f>
-        <v>0</v>
-      </c>
+      <c r="M13" s="214"/>
+      <c r="N13" s="214"/>
       <c r="O13" s="214">
         <f>ETPT_JUR_ASS!O13</f>
         <v>0</v>
@@ -30568,8 +30878,16 @@
         <f>ETPT_JUR_ASS!Q13</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:62" ht="16" x14ac:dyDescent="0.2">
+      <c r="R13" s="214">
+        <f>ETPT_JUR_ASS!R13</f>
+        <v>0</v>
+      </c>
+      <c r="S13" s="214">
+        <f>ETPT_JUR_ASS!S13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:64" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="217"/>
       <c r="B14" s="217"/>
       <c r="C14" s="217"/>
@@ -30588,8 +30906,10 @@
       <c r="P14" s="216"/>
       <c r="Q14" s="216"/>
       <c r="R14" s="216"/>
-    </row>
-    <row r="15" spans="1:62" ht="16" x14ac:dyDescent="0.2">
+      <c r="S14" s="216"/>
+      <c r="T14" s="216"/>
+    </row>
+    <row r="15" spans="1:64" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="217"/>
       <c r="B15" s="217"/>
       <c r="C15" s="217"/>
@@ -30609,8 +30929,10 @@
       <c r="P15" s="216"/>
       <c r="Q15" s="216"/>
       <c r="R15" s="216"/>
-    </row>
-    <row r="16" spans="1:62" ht="16" x14ac:dyDescent="0.2">
+      <c r="S15" s="216"/>
+      <c r="T15" s="216"/>
+    </row>
+    <row r="16" spans="1:64" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="217"/>
       <c r="B16" s="217"/>
       <c r="C16" s="217"/>
@@ -30628,8 +30950,10 @@
       <c r="O16" s="216"/>
       <c r="P16" s="216"/>
       <c r="Q16" s="216"/>
-    </row>
-    <row r="17" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="R16" s="216"/>
+      <c r="S16" s="216"/>
+    </row>
+    <row r="17" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="217"/>
       <c r="B17" s="217"/>
       <c r="C17" s="217"/>
@@ -30648,10 +30972,12 @@
       <c r="P17" s="216"/>
       <c r="Q17" s="216"/>
       <c r="R17" s="216"/>
+      <c r="S17" s="216"/>
+      <c r="T17" s="216"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="Q2:Q4"/>
+    <mergeCell ref="S2:S4"/>
   </mergeCells>
   <phoneticPr fontId="68" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -37299,7 +37625,7 @@
   <dimension ref="A1:H67"/>
   <sheetViews>
     <sheetView zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -37651,12 +37977,12 @@
   </sheetPr>
   <dimension ref="A1:BF24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="Y2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
-      <selection pane="bottomRight" activeCell="V14" sqref="V14"/>
+      <selection pane="bottomRight" activeCell="AF5" sqref="AF5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -38091,7 +38417,7 @@
         <v>86</v>
       </c>
       <c r="AF4" s="69" t="s">
-        <v>85</v>
+        <v>670</v>
       </c>
       <c r="AG4" s="415"/>
       <c r="AH4" s="69" t="s">

</xml_diff>

<commit_message>
Update tab names in template4.xlsx
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dinum-327809/Documents/a-just-dev/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B3E188-CE49-144E-96BF-F010583622E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B74B72-ED67-AE4D-A0C3-360C6D2F741D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" activeTab="13" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" activeTab="9" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
   <sheets>
     <sheet name="ACCUEIL" sheetId="33" r:id="rId1"/>
@@ -22,11 +22,11 @@
     <sheet name="ETPT_TJ" sheetId="25" state="hidden" r:id="rId7"/>
     <sheet name="ETPT_TPRX" sheetId="26" state="hidden" r:id="rId8"/>
     <sheet name="ETPT_CPH" sheetId="27" state="hidden" r:id="rId9"/>
-    <sheet name="ETPT_ATT_JUR" sheetId="38" state="hidden" r:id="rId10"/>
+    <sheet name="ETPT_ATTJ" sheetId="38" r:id="rId10"/>
     <sheet name="ETPT_TJ_DDG" sheetId="28" r:id="rId11"/>
     <sheet name="ETPT_TPRX_DDG" sheetId="29" r:id="rId12"/>
     <sheet name="ETPT_CPH_DDG" sheetId="30" r:id="rId13"/>
-    <sheet name="ETPT_ATT_JUR_DDG" sheetId="39" r:id="rId14"/>
+    <sheet name="ETPT_ATTJ_DDG" sheetId="39" r:id="rId14"/>
     <sheet name="Juridictions" sheetId="17" state="hidden" r:id="rId15"/>
     <sheet name="ETPT_TJ_corresp-SIEGE-TJ" sheetId="24" state="hidden" r:id="rId16"/>
     <sheet name="ETPT_TPROX_corresp-SIEGE-TPROX" sheetId="34" state="hidden" r:id="rId17"/>
@@ -20667,7 +20667,7 @@
   </sheetPr>
   <dimension ref="A1:BL145"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -20887,7 +20887,7 @@
       <c r="B5" s="212"/>
       <c r="C5" s="212"/>
       <c r="D5" s="212">
-        <f>ETPT_ATT_JUR_DDG!D5</f>
+        <f>ETPT_ATTJ_DDG!D5</f>
         <v>0</v>
       </c>
       <c r="E5" s="212" t="s">
@@ -20990,7 +20990,7 @@
       <c r="B6" s="212"/>
       <c r="C6" s="212"/>
       <c r="D6" s="212">
-        <f>ETPT_ATT_JUR_DDG!D6</f>
+        <f>ETPT_ATTJ_DDG!D6</f>
         <v>0</v>
       </c>
       <c r="E6" s="212" t="s">
@@ -21123,7 +21123,7 @@
       <c r="B7" s="212"/>
       <c r="C7" s="212"/>
       <c r="D7" s="212">
-        <f>ETPT_ATT_JUR_DDG!D7</f>
+        <f>ETPT_ATTJ_DDG!D7</f>
         <v>0</v>
       </c>
       <c r="E7" s="212" t="s">
@@ -21216,7 +21216,7 @@
       <c r="B8" s="212"/>
       <c r="C8" s="212"/>
       <c r="D8" s="212">
-        <f>ETPT_ATT_JUR_DDG!D8</f>
+        <f>ETPT_ATTJ_DDG!D8</f>
         <v>0</v>
       </c>
       <c r="E8" s="212" t="s">
@@ -21389,7 +21389,7 @@
       <c r="B9" s="212"/>
       <c r="C9" s="212"/>
       <c r="D9" s="212">
-        <f>ETPT_ATT_JUR_DDG!D9</f>
+        <f>ETPT_ATTJ_DDG!D9</f>
         <v>0</v>
       </c>
       <c r="E9" s="212" t="s">
@@ -21482,7 +21482,7 @@
       <c r="B10" s="212"/>
       <c r="C10" s="212"/>
       <c r="D10" s="212">
-        <f>ETPT_ATT_JUR_DDG!D10</f>
+        <f>ETPT_ATTJ_DDG!D10</f>
         <v>0</v>
       </c>
       <c r="E10" s="212" t="s">
@@ -21575,7 +21575,7 @@
       <c r="B11" s="212"/>
       <c r="C11" s="212"/>
       <c r="D11" s="212">
-        <f>ETPT_ATT_JUR_DDG!D11</f>
+        <f>ETPT_ATTJ_DDG!D11</f>
         <v>0</v>
       </c>
       <c r="E11" s="212" t="s">
@@ -21708,7 +21708,7 @@
       <c r="B12" s="212"/>
       <c r="C12" s="212"/>
       <c r="D12" s="212">
-        <f>ETPT_ATT_JUR_DDG!D12</f>
+        <f>ETPT_ATTJ_DDG!D12</f>
         <v>0</v>
       </c>
       <c r="E12" s="212" t="s">
@@ -24778,7 +24778,7 @@
   <dimension ref="A1:BG22"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -30407,8 +30407,8 @@
   </sheetPr>
   <dimension ref="A1:BL17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView showGridLines="0" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -30632,43 +30632,43 @@
         <v>61</v>
       </c>
       <c r="G5" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!G5),"",IF(ISERROR(ETPT_ATT_JUR!G5),"",IF(ETPT_ATT_JUR!G5=0,"",ETPT_ATT_JUR!G5)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!G5),"",IF(ISERROR(ETPT_ATTJ!G5),"",IF(ETPT_ATTJ!G5=0,"",ETPT_ATTJ!G5)))</f>
         <v/>
       </c>
       <c r="H5" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!H5),"",IF(ISERROR(ETPT_ATT_JUR!H5),"",IF(ETPT_ATT_JUR!H5=0,"",ETPT_ATT_JUR!H5)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!H5),"",IF(ISERROR(ETPT_ATTJ!H5),"",IF(ETPT_ATTJ!H5=0,"",ETPT_ATTJ!H5)))</f>
         <v/>
       </c>
       <c r="I5" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!I5),"",IF(ISERROR(ETPT_ATT_JUR!I5),"",IF(ETPT_ATT_JUR!I5=0,"",ETPT_ATT_JUR!I5)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!I5),"",IF(ISERROR(ETPT_ATTJ!I5),"",IF(ETPT_ATTJ!I5=0,"",ETPT_ATTJ!I5)))</f>
         <v/>
       </c>
       <c r="J5" s="247"/>
       <c r="K5" s="247"/>
       <c r="L5" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!L5),"",IF(ISERROR(ETPT_ATT_JUR!L5),"",IF(ETPT_ATT_JUR!L5=0,"",ETPT_ATT_JUR!L5)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!L5),"",IF(ISERROR(ETPT_ATTJ!L5),"",IF(ETPT_ATTJ!L5=0,"",ETPT_ATTJ!L5)))</f>
         <v/>
       </c>
       <c r="M5" s="247"/>
       <c r="N5" s="247"/>
       <c r="O5" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!O5),"",IF(ISERROR(ETPT_ATT_JUR!O5),"",IF(ETPT_ATT_JUR!O5=0,"",ETPT_ATT_JUR!O5)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!O5),"",IF(ISERROR(ETPT_ATTJ!O5),"",IF(ETPT_ATTJ!O5=0,"",ETPT_ATTJ!O5)))</f>
         <v/>
       </c>
       <c r="P5" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!P5),"",IF(ISERROR(ETPT_ATT_JUR!P5),"",IF(ETPT_ATT_JUR!P5=0,"",ETPT_ATT_JUR!P5)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!P5),"",IF(ISERROR(ETPT_ATTJ!P5),"",IF(ETPT_ATTJ!P5=0,"",ETPT_ATTJ!P5)))</f>
         <v/>
       </c>
       <c r="Q5" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!Q5),"",IF(ISERROR(ETPT_ATT_JUR!Q5),"",IF(ETPT_ATT_JUR!Q5=0,"",ETPT_ATT_JUR!Q5)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!Q5),"",IF(ISERROR(ETPT_ATTJ!Q5),"",IF(ETPT_ATTJ!Q5=0,"",ETPT_ATTJ!Q5)))</f>
         <v/>
       </c>
       <c r="R5" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!R5),"",IF(ISERROR(ETPT_ATT_JUR!R5),"",IF(ETPT_ATT_JUR!R5=0,"",ETPT_ATT_JUR!R5)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!R5),"",IF(ISERROR(ETPT_ATTJ!R5),"",IF(ETPT_ATTJ!R5=0,"",ETPT_ATTJ!R5)))</f>
         <v/>
       </c>
       <c r="S5" s="214">
-        <f>ETPT_ATT_JUR!S5</f>
+        <f>ETPT_ATTJ!S5</f>
         <v>0</v>
       </c>
     </row>
@@ -30689,49 +30689,49 @@
         <v>59</v>
       </c>
       <c r="G6" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!G6),"",IF(ISERROR(ETPT_ATT_JUR!G6),"",IF(ETPT_ATT_JUR!G6=0,"",ETPT_ATT_JUR!G6)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!G6),"",IF(ISERROR(ETPT_ATTJ!G6),"",IF(ETPT_ATTJ!G6=0,"",ETPT_ATTJ!G6)))</f>
         <v/>
       </c>
       <c r="H6" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!H6),"",IF(ISERROR(ETPT_ATT_JUR!H6),"",IF(ETPT_ATT_JUR!H6=0,"",ETPT_ATT_JUR!H6)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!H6),"",IF(ISERROR(ETPT_ATTJ!H6),"",IF(ETPT_ATTJ!H6=0,"",ETPT_ATTJ!H6)))</f>
         <v/>
       </c>
       <c r="I6" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!I6),"",IF(ISERROR(ETPT_ATT_JUR!I6),"",IF(ETPT_ATT_JUR!I6=0,"",ETPT_ATT_JUR!I6)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!I6),"",IF(ISERROR(ETPT_ATTJ!I6),"",IF(ETPT_ATTJ!I6=0,"",ETPT_ATTJ!I6)))</f>
         <v/>
       </c>
       <c r="J6" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!J6),"",IF(ISERROR(ETPT_ATT_JUR!J6),"",IF(ETPT_ATT_JUR!J6=0,"",ETPT_ATT_JUR!J6)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!J6),"",IF(ISERROR(ETPT_ATTJ!J6),"",IF(ETPT_ATTJ!J6=0,"",ETPT_ATTJ!J6)))</f>
         <v/>
       </c>
       <c r="K6" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!K6),"",IF(ISERROR(ETPT_ATT_JUR!K6),"",IF(ETPT_ATT_JUR!K6=0,"",ETPT_ATT_JUR!K6)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!K6),"",IF(ISERROR(ETPT_ATTJ!K6),"",IF(ETPT_ATTJ!K6=0,"",ETPT_ATTJ!K6)))</f>
         <v/>
       </c>
       <c r="L6" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!L6),"",IF(ISERROR(ETPT_ATT_JUR!L6),"",IF(ETPT_ATT_JUR!L6=0,"",ETPT_ATT_JUR!L6)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!L6),"",IF(ISERROR(ETPT_ATTJ!L6),"",IF(ETPT_ATTJ!L6=0,"",ETPT_ATTJ!L6)))</f>
         <v/>
       </c>
       <c r="M6" s="247"/>
       <c r="N6" s="247"/>
       <c r="O6" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!O6),"",IF(ISERROR(ETPT_ATT_JUR!O6),"",IF(ETPT_ATT_JUR!O6=0,"",ETPT_ATT_JUR!O6)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!O6),"",IF(ISERROR(ETPT_ATTJ!O6),"",IF(ETPT_ATTJ!O6=0,"",ETPT_ATTJ!O6)))</f>
         <v/>
       </c>
       <c r="P6" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!P6),"",IF(ISERROR(ETPT_ATT_JUR!P6),"",IF(ETPT_ATT_JUR!P6=0,"",ETPT_ATT_JUR!P6)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!P6),"",IF(ISERROR(ETPT_ATTJ!P6),"",IF(ETPT_ATTJ!P6=0,"",ETPT_ATTJ!P6)))</f>
         <v/>
       </c>
       <c r="Q6" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!Q6),"",IF(ISERROR(ETPT_ATT_JUR!Q6),"",IF(ETPT_ATT_JUR!Q6=0,"",ETPT_ATT_JUR!Q6)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!Q6),"",IF(ISERROR(ETPT_ATTJ!Q6),"",IF(ETPT_ATTJ!Q6=0,"",ETPT_ATTJ!Q6)))</f>
         <v/>
       </c>
       <c r="R6" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!R6),"",IF(ISERROR(ETPT_ATT_JUR!R6),"",IF(ETPT_ATT_JUR!R6=0,"",ETPT_ATT_JUR!R6)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!R6),"",IF(ISERROR(ETPT_ATTJ!R6),"",IF(ETPT_ATTJ!R6=0,"",ETPT_ATTJ!R6)))</f>
         <v/>
       </c>
       <c r="S6" s="214">
-        <f>ETPT_ATT_JUR!S6</f>
+        <f>ETPT_ATTJ!S6</f>
         <v>0</v>
       </c>
     </row>
@@ -30752,43 +30752,43 @@
         <v>55</v>
       </c>
       <c r="G7" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!G7),"",IF(ISERROR(ETPT_ATT_JUR!G7),"",IF(ETPT_ATT_JUR!G7=0,"",ETPT_ATT_JUR!G7)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!G7),"",IF(ISERROR(ETPT_ATTJ!G7),"",IF(ETPT_ATTJ!G7=0,"",ETPT_ATTJ!G7)))</f>
         <v/>
       </c>
       <c r="H7" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!H7),"",IF(ISERROR(ETPT_ATT_JUR!H7),"",IF(ETPT_ATT_JUR!H7=0,"",ETPT_ATT_JUR!H7)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!H7),"",IF(ISERROR(ETPT_ATTJ!H7),"",IF(ETPT_ATTJ!H7=0,"",ETPT_ATTJ!H7)))</f>
         <v/>
       </c>
       <c r="I7" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!I7),"",IF(ISERROR(ETPT_ATT_JUR!I7),"",IF(ETPT_ATT_JUR!I7=0,"",ETPT_ATT_JUR!I7)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!I7),"",IF(ISERROR(ETPT_ATTJ!I7),"",IF(ETPT_ATTJ!I7=0,"",ETPT_ATTJ!I7)))</f>
         <v/>
       </c>
       <c r="J7" s="247"/>
       <c r="K7" s="247"/>
       <c r="L7" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!L7),"",IF(ISERROR(ETPT_ATT_JUR!L7),"",IF(ETPT_ATT_JUR!L7=0,"",ETPT_ATT_JUR!L7)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!L7),"",IF(ISERROR(ETPT_ATTJ!L7),"",IF(ETPT_ATTJ!L7=0,"",ETPT_ATTJ!L7)))</f>
         <v/>
       </c>
       <c r="M7" s="247"/>
       <c r="N7" s="247"/>
       <c r="O7" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!O7),"",IF(ISERROR(ETPT_ATT_JUR!O7),"",IF(ETPT_ATT_JUR!O7=0,"",ETPT_ATT_JUR!O7)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!O7),"",IF(ISERROR(ETPT_ATTJ!O7),"",IF(ETPT_ATTJ!O7=0,"",ETPT_ATTJ!O7)))</f>
         <v/>
       </c>
       <c r="P7" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!P7),"",IF(ISERROR(ETPT_ATT_JUR!P7),"",IF(ETPT_ATT_JUR!P7=0,"",ETPT_ATT_JUR!P7)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!P7),"",IF(ISERROR(ETPT_ATTJ!P7),"",IF(ETPT_ATTJ!P7=0,"",ETPT_ATTJ!P7)))</f>
         <v/>
       </c>
       <c r="Q7" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!Q7),"",IF(ISERROR(ETPT_ATT_JUR!Q7),"",IF(ETPT_ATT_JUR!Q7=0,"",ETPT_ATT_JUR!Q7)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!Q7),"",IF(ISERROR(ETPT_ATTJ!Q7),"",IF(ETPT_ATTJ!Q7=0,"",ETPT_ATTJ!Q7)))</f>
         <v/>
       </c>
       <c r="R7" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!R7),"",IF(ISERROR(ETPT_ATT_JUR!R7),"",IF(ETPT_ATT_JUR!R7=0,"",ETPT_ATT_JUR!R7)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!R7),"",IF(ISERROR(ETPT_ATTJ!R7),"",IF(ETPT_ATTJ!R7=0,"",ETPT_ATTJ!R7)))</f>
         <v/>
       </c>
       <c r="S7" s="214">
-        <f>ETPT_ATT_JUR!S7</f>
+        <f>ETPT_ATTJ!S7</f>
         <v>0</v>
       </c>
     </row>
@@ -30809,43 +30809,43 @@
         <v>53</v>
       </c>
       <c r="G8" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!G8),"",IF(ISERROR(ETPT_ATT_JUR!G8),"",IF(ETPT_ATT_JUR!G8=0,"",ETPT_ATT_JUR!G8)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!G8),"",IF(ISERROR(ETPT_ATTJ!G8),"",IF(ETPT_ATTJ!G8=0,"",ETPT_ATTJ!G8)))</f>
         <v/>
       </c>
       <c r="H8" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!H8),"",IF(ISERROR(ETPT_ATT_JUR!H8),"",IF(ETPT_ATT_JUR!H8=0,"",ETPT_ATT_JUR!H8)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!H8),"",IF(ISERROR(ETPT_ATTJ!H8),"",IF(ETPT_ATTJ!H8=0,"",ETPT_ATTJ!H8)))</f>
         <v/>
       </c>
       <c r="I8" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!I8),"",IF(ISERROR(ETPT_ATT_JUR!I8),"",IF(ETPT_ATT_JUR!I8=0,"",ETPT_ATT_JUR!I8)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!I8),"",IF(ISERROR(ETPT_ATTJ!I8),"",IF(ETPT_ATTJ!I8=0,"",ETPT_ATTJ!I8)))</f>
         <v/>
       </c>
       <c r="J8" s="247"/>
       <c r="K8" s="247"/>
       <c r="L8" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!L8),"",IF(ISERROR(ETPT_ATT_JUR!L8),"",IF(ETPT_ATT_JUR!L8=0,"",ETPT_ATT_JUR!L8)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!L8),"",IF(ISERROR(ETPT_ATTJ!L8),"",IF(ETPT_ATTJ!L8=0,"",ETPT_ATTJ!L8)))</f>
         <v/>
       </c>
       <c r="M8" s="247"/>
       <c r="N8" s="247"/>
       <c r="O8" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!O8),"",IF(ISERROR(ETPT_ATT_JUR!O8),"",IF(ETPT_ATT_JUR!O8=0,"",ETPT_ATT_JUR!O8)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!O8),"",IF(ISERROR(ETPT_ATTJ!O8),"",IF(ETPT_ATTJ!O8=0,"",ETPT_ATTJ!O8)))</f>
         <v/>
       </c>
       <c r="P8" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!P8),"",IF(ISERROR(ETPT_ATT_JUR!P8),"",IF(ETPT_ATT_JUR!P8=0,"",ETPT_ATT_JUR!P8)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!P8),"",IF(ISERROR(ETPT_ATTJ!P8),"",IF(ETPT_ATTJ!P8=0,"",ETPT_ATTJ!P8)))</f>
         <v/>
       </c>
       <c r="Q8" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!Q8),"",IF(ISERROR(ETPT_ATT_JUR!Q8),"",IF(ETPT_ATT_JUR!Q8=0,"",ETPT_ATT_JUR!Q8)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!Q8),"",IF(ISERROR(ETPT_ATTJ!Q8),"",IF(ETPT_ATTJ!Q8=0,"",ETPT_ATTJ!Q8)))</f>
         <v/>
       </c>
       <c r="R8" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!R8),"",IF(ISERROR(ETPT_ATT_JUR!R8),"",IF(ETPT_ATT_JUR!R8=0,"",ETPT_ATT_JUR!R8)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!R8),"",IF(ISERROR(ETPT_ATTJ!R8),"",IF(ETPT_ATTJ!R8=0,"",ETPT_ATTJ!R8)))</f>
         <v/>
       </c>
       <c r="S8" s="214">
-        <f>ETPT_ATT_JUR!S8</f>
+        <f>ETPT_ATTJ!S8</f>
         <v>0</v>
       </c>
     </row>
@@ -30866,43 +30866,43 @@
         <v>51</v>
       </c>
       <c r="G9" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!G9),"",IF(ISERROR(ETPT_ATT_JUR!G9),"",IF(ETPT_ATT_JUR!G9=0,"",ETPT_ATT_JUR!G9)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!G9),"",IF(ISERROR(ETPT_ATTJ!G9),"",IF(ETPT_ATTJ!G9=0,"",ETPT_ATTJ!G9)))</f>
         <v/>
       </c>
       <c r="H9" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!H9),"",IF(ISERROR(ETPT_ATT_JUR!H9),"",IF(ETPT_ATT_JUR!H9=0,"",ETPT_ATT_JUR!H9)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!H9),"",IF(ISERROR(ETPT_ATTJ!H9),"",IF(ETPT_ATTJ!H9=0,"",ETPT_ATTJ!H9)))</f>
         <v/>
       </c>
       <c r="I9" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!I9),"",IF(ISERROR(ETPT_ATT_JUR!I9),"",IF(ETPT_ATT_JUR!I9=0,"",ETPT_ATT_JUR!I9)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!I9),"",IF(ISERROR(ETPT_ATTJ!I9),"",IF(ETPT_ATTJ!I9=0,"",ETPT_ATTJ!I9)))</f>
         <v/>
       </c>
       <c r="J9" s="247"/>
       <c r="K9" s="247"/>
       <c r="L9" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!L9),"",IF(ISERROR(ETPT_ATT_JUR!L9),"",IF(ETPT_ATT_JUR!L9=0,"",ETPT_ATT_JUR!L9)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!L9),"",IF(ISERROR(ETPT_ATTJ!L9),"",IF(ETPT_ATTJ!L9=0,"",ETPT_ATTJ!L9)))</f>
         <v/>
       </c>
       <c r="M9" s="247"/>
       <c r="N9" s="247"/>
       <c r="O9" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!O9),"",IF(ISERROR(ETPT_ATT_JUR!O9),"",IF(ETPT_ATT_JUR!O9=0,"",ETPT_ATT_JUR!O9)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!O9),"",IF(ISERROR(ETPT_ATTJ!O9),"",IF(ETPT_ATTJ!O9=0,"",ETPT_ATTJ!O9)))</f>
         <v/>
       </c>
       <c r="P9" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!P9),"",IF(ISERROR(ETPT_ATT_JUR!P9),"",IF(ETPT_ATT_JUR!P9=0,"",ETPT_ATT_JUR!P9)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!P9),"",IF(ISERROR(ETPT_ATTJ!P9),"",IF(ETPT_ATTJ!P9=0,"",ETPT_ATTJ!P9)))</f>
         <v/>
       </c>
       <c r="Q9" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!Q9),"",IF(ISERROR(ETPT_ATT_JUR!Q9),"",IF(ETPT_ATT_JUR!Q9=0,"",ETPT_ATT_JUR!Q9)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!Q9),"",IF(ISERROR(ETPT_ATTJ!Q9),"",IF(ETPT_ATTJ!Q9=0,"",ETPT_ATTJ!Q9)))</f>
         <v/>
       </c>
       <c r="R9" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!R9),"",IF(ISERROR(ETPT_ATT_JUR!R9),"",IF(ETPT_ATT_JUR!R9=0,"",ETPT_ATT_JUR!R9)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!R9),"",IF(ISERROR(ETPT_ATTJ!R9),"",IF(ETPT_ATTJ!R9=0,"",ETPT_ATTJ!R9)))</f>
         <v/>
       </c>
       <c r="S9" s="214">
-        <f>ETPT_ATT_JUR!S9</f>
+        <f>ETPT_ATTJ!S9</f>
         <v>0</v>
       </c>
     </row>
@@ -30923,43 +30923,43 @@
         <v>49</v>
       </c>
       <c r="G10" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!G10),"",IF(ISERROR(ETPT_ATT_JUR!G10),"",IF(ETPT_ATT_JUR!G10=0,"",ETPT_ATT_JUR!G10)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!G10),"",IF(ISERROR(ETPT_ATTJ!G10),"",IF(ETPT_ATTJ!G10=0,"",ETPT_ATTJ!G10)))</f>
         <v/>
       </c>
       <c r="H10" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!H10),"",IF(ISERROR(ETPT_ATT_JUR!H10),"",IF(ETPT_ATT_JUR!H10=0,"",ETPT_ATT_JUR!H10)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!H10),"",IF(ISERROR(ETPT_ATTJ!H10),"",IF(ETPT_ATTJ!H10=0,"",ETPT_ATTJ!H10)))</f>
         <v/>
       </c>
       <c r="I10" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!I10),"",IF(ISERROR(ETPT_ATT_JUR!I10),"",IF(ETPT_ATT_JUR!I10=0,"",ETPT_ATT_JUR!I10)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!I10),"",IF(ISERROR(ETPT_ATTJ!I10),"",IF(ETPT_ATTJ!I10=0,"",ETPT_ATTJ!I10)))</f>
         <v/>
       </c>
       <c r="J10" s="247"/>
       <c r="K10" s="247"/>
       <c r="L10" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!L10),"",IF(ISERROR(ETPT_ATT_JUR!L10),"",IF(ETPT_ATT_JUR!L10=0,"",ETPT_ATT_JUR!L10)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!L10),"",IF(ISERROR(ETPT_ATTJ!L10),"",IF(ETPT_ATTJ!L10=0,"",ETPT_ATTJ!L10)))</f>
         <v/>
       </c>
       <c r="M10" s="247"/>
       <c r="N10" s="247"/>
       <c r="O10" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!O10),"",IF(ISERROR(ETPT_ATT_JUR!O10),"",IF(ETPT_ATT_JUR!O10=0,"",ETPT_ATT_JUR!O10)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!O10),"",IF(ISERROR(ETPT_ATTJ!O10),"",IF(ETPT_ATTJ!O10=0,"",ETPT_ATTJ!O10)))</f>
         <v/>
       </c>
       <c r="P10" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!P10),"",IF(ISERROR(ETPT_ATT_JUR!P10),"",IF(ETPT_ATT_JUR!P10=0,"",ETPT_ATT_JUR!P10)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!P10),"",IF(ISERROR(ETPT_ATTJ!P10),"",IF(ETPT_ATTJ!P10=0,"",ETPT_ATTJ!P10)))</f>
         <v/>
       </c>
       <c r="Q10" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!Q10),"",IF(ISERROR(ETPT_ATT_JUR!Q10),"",IF(ETPT_ATT_JUR!Q10=0,"",ETPT_ATT_JUR!Q10)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!Q10),"",IF(ISERROR(ETPT_ATTJ!Q10),"",IF(ETPT_ATTJ!Q10=0,"",ETPT_ATTJ!Q10)))</f>
         <v/>
       </c>
       <c r="R10" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!R10),"",IF(ISERROR(ETPT_ATT_JUR!R10),"",IF(ETPT_ATT_JUR!R10=0,"",ETPT_ATT_JUR!R10)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!R10),"",IF(ISERROR(ETPT_ATTJ!R10),"",IF(ETPT_ATTJ!R10=0,"",ETPT_ATTJ!R10)))</f>
         <v/>
       </c>
       <c r="S10" s="214">
-        <f>ETPT_ATT_JUR!S10</f>
+        <f>ETPT_ATTJ!S10</f>
         <v>0</v>
       </c>
     </row>
@@ -30980,43 +30980,43 @@
         <v>47</v>
       </c>
       <c r="G11" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!G11),"",IF(ISERROR(ETPT_ATT_JUR!G11),"",IF(ETPT_ATT_JUR!G11=0,"",ETPT_ATT_JUR!G11)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!G11),"",IF(ISERROR(ETPT_ATTJ!G11),"",IF(ETPT_ATTJ!G11=0,"",ETPT_ATTJ!G11)))</f>
         <v/>
       </c>
       <c r="H11" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!H11),"",IF(ISERROR(ETPT_ATT_JUR!H11),"",IF(ETPT_ATT_JUR!H11=0,"",ETPT_ATT_JUR!H11)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!H11),"",IF(ISERROR(ETPT_ATTJ!H11),"",IF(ETPT_ATTJ!H11=0,"",ETPT_ATTJ!H11)))</f>
         <v/>
       </c>
       <c r="I11" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!I11),"",IF(ISERROR(ETPT_ATT_JUR!I11),"",IF(ETPT_ATT_JUR!I11=0,"",ETPT_ATT_JUR!I11)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!I11),"",IF(ISERROR(ETPT_ATTJ!I11),"",IF(ETPT_ATTJ!I11=0,"",ETPT_ATTJ!I11)))</f>
         <v/>
       </c>
       <c r="J11" s="247"/>
       <c r="K11" s="247"/>
       <c r="L11" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!L11),"",IF(ISERROR(ETPT_ATT_JUR!L11),"",IF(ETPT_ATT_JUR!L11=0,"",ETPT_ATT_JUR!L11)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!L11),"",IF(ISERROR(ETPT_ATTJ!L11),"",IF(ETPT_ATTJ!L11=0,"",ETPT_ATTJ!L11)))</f>
         <v/>
       </c>
       <c r="M11" s="247"/>
       <c r="N11" s="247"/>
       <c r="O11" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!O11),"",IF(ISERROR(ETPT_ATT_JUR!O11),"",IF(ETPT_ATT_JUR!O11=0,"",ETPT_ATT_JUR!O11)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!O11),"",IF(ISERROR(ETPT_ATTJ!O11),"",IF(ETPT_ATTJ!O11=0,"",ETPT_ATTJ!O11)))</f>
         <v/>
       </c>
       <c r="P11" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!P11),"",IF(ISERROR(ETPT_ATT_JUR!P11),"",IF(ETPT_ATT_JUR!P11=0,"",ETPT_ATT_JUR!P11)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!P11),"",IF(ISERROR(ETPT_ATTJ!P11),"",IF(ETPT_ATTJ!P11=0,"",ETPT_ATTJ!P11)))</f>
         <v/>
       </c>
       <c r="Q11" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!Q11),"",IF(ISERROR(ETPT_ATT_JUR!Q11),"",IF(ETPT_ATT_JUR!Q11=0,"",ETPT_ATT_JUR!Q11)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!Q11),"",IF(ISERROR(ETPT_ATTJ!Q11),"",IF(ETPT_ATTJ!Q11=0,"",ETPT_ATTJ!Q11)))</f>
         <v/>
       </c>
       <c r="R11" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!R11),"",IF(ISERROR(ETPT_ATT_JUR!R11),"",IF(ETPT_ATT_JUR!R11=0,"",ETPT_ATT_JUR!R11)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!R11),"",IF(ISERROR(ETPT_ATTJ!R11),"",IF(ETPT_ATTJ!R11=0,"",ETPT_ATTJ!R11)))</f>
         <v/>
       </c>
       <c r="S11" s="214">
-        <f>ETPT_ATT_JUR!S11</f>
+        <f>ETPT_ATTJ!S11</f>
         <v>0</v>
       </c>
     </row>
@@ -31037,43 +31037,43 @@
         <v>45</v>
       </c>
       <c r="G12" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!G12),"",IF(ISERROR(ETPT_ATT_JUR!G12),"",IF(ETPT_ATT_JUR!G12=0,"",ETPT_ATT_JUR!G12)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!G12),"",IF(ISERROR(ETPT_ATTJ!G12),"",IF(ETPT_ATTJ!G12=0,"",ETPT_ATTJ!G12)))</f>
         <v/>
       </c>
       <c r="H12" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!H12),"",IF(ISERROR(ETPT_ATT_JUR!H12),"",IF(ETPT_ATT_JUR!H12=0,"",ETPT_ATT_JUR!H12)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!H12),"",IF(ISERROR(ETPT_ATTJ!H12),"",IF(ETPT_ATTJ!H12=0,"",ETPT_ATTJ!H12)))</f>
         <v/>
       </c>
       <c r="I12" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!I12),"",IF(ISERROR(ETPT_ATT_JUR!I12),"",IF(ETPT_ATT_JUR!I12=0,"",ETPT_ATT_JUR!I12)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!I12),"",IF(ISERROR(ETPT_ATTJ!I12),"",IF(ETPT_ATTJ!I12=0,"",ETPT_ATTJ!I12)))</f>
         <v/>
       </c>
       <c r="J12" s="247"/>
       <c r="K12" s="247"/>
       <c r="L12" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!L12),"",IF(ISERROR(ETPT_ATT_JUR!L12),"",IF(ETPT_ATT_JUR!L12=0,"",ETPT_ATT_JUR!L12)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!L12),"",IF(ISERROR(ETPT_ATTJ!L12),"",IF(ETPT_ATTJ!L12=0,"",ETPT_ATTJ!L12)))</f>
         <v/>
       </c>
       <c r="M12" s="247"/>
       <c r="N12" s="247"/>
       <c r="O12" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!O12),"",IF(ISERROR(ETPT_ATT_JUR!O12),"",IF(ETPT_ATT_JUR!O12=0,"",ETPT_ATT_JUR!O12)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!O12),"",IF(ISERROR(ETPT_ATTJ!O12),"",IF(ETPT_ATTJ!O12=0,"",ETPT_ATTJ!O12)))</f>
         <v/>
       </c>
       <c r="P12" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!P12),"",IF(ISERROR(ETPT_ATT_JUR!P12),"",IF(ETPT_ATT_JUR!P12=0,"",ETPT_ATT_JUR!P12)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!P12),"",IF(ISERROR(ETPT_ATTJ!P12),"",IF(ETPT_ATTJ!P12=0,"",ETPT_ATTJ!P12)))</f>
         <v/>
       </c>
       <c r="Q12" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!Q12),"",IF(ISERROR(ETPT_ATT_JUR!Q12),"",IF(ETPT_ATT_JUR!Q12=0,"",ETPT_ATT_JUR!Q12)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!Q12),"",IF(ISERROR(ETPT_ATTJ!Q12),"",IF(ETPT_ATTJ!Q12=0,"",ETPT_ATTJ!Q12)))</f>
         <v/>
       </c>
       <c r="R12" s="247" t="str">
-        <f>IF(ISBLANK(ETPT_ATT_JUR!R12),"",IF(ISERROR(ETPT_ATT_JUR!R12),"",IF(ETPT_ATT_JUR!R12=0,"",ETPT_ATT_JUR!R12)))</f>
+        <f>IF(ISBLANK(ETPT_ATTJ!R12),"",IF(ISERROR(ETPT_ATTJ!R12),"",IF(ETPT_ATTJ!R12=0,"",ETPT_ATTJ!R12)))</f>
         <v/>
       </c>
       <c r="S12" s="214">
-        <f>ETPT_ATT_JUR!S12</f>
+        <f>ETPT_ATTJ!S12</f>
         <v>0</v>
       </c>
     </row>
@@ -31087,55 +31087,55 @@
         <v>39</v>
       </c>
       <c r="G13" s="214">
-        <f>ETPT_ATT_JUR!G13</f>
+        <f>ETPT_ATTJ!G13</f>
         <v>0</v>
       </c>
       <c r="H13" s="214">
-        <f>ETPT_ATT_JUR!H13</f>
+        <f>ETPT_ATTJ!H13</f>
         <v>0</v>
       </c>
       <c r="I13" s="214">
-        <f>ETPT_ATT_JUR!I13</f>
+        <f>ETPT_ATTJ!I13</f>
         <v>0</v>
       </c>
       <c r="J13" s="214">
-        <f>ETPT_ATT_JUR!J13</f>
+        <f>ETPT_ATTJ!J13</f>
         <v>0</v>
       </c>
       <c r="K13" s="214">
-        <f>ETPT_ATT_JUR!K13</f>
+        <f>ETPT_ATTJ!K13</f>
         <v>0</v>
       </c>
       <c r="L13" s="214">
-        <f>ETPT_ATT_JUR!L13</f>
+        <f>ETPT_ATTJ!L13</f>
         <v>0</v>
       </c>
       <c r="M13" s="214">
-        <f>ETPT_ATT_JUR!M13</f>
+        <f>ETPT_ATTJ!M13</f>
         <v>0</v>
       </c>
       <c r="N13" s="214">
-        <f>ETPT_ATT_JUR!N13</f>
+        <f>ETPT_ATTJ!N13</f>
         <v>0</v>
       </c>
       <c r="O13" s="214">
-        <f>ETPT_ATT_JUR!O13</f>
+        <f>ETPT_ATTJ!O13</f>
         <v>0</v>
       </c>
       <c r="P13" s="214">
-        <f>ETPT_ATT_JUR!P13</f>
+        <f>ETPT_ATTJ!P13</f>
         <v>0</v>
       </c>
       <c r="Q13" s="214">
-        <f>ETPT_ATT_JUR!Q13</f>
+        <f>ETPT_ATTJ!Q13</f>
         <v>0</v>
       </c>
       <c r="R13" s="214">
-        <f>ETPT_ATT_JUR!R13</f>
+        <f>ETPT_ATTJ!R13</f>
         <v>0</v>
       </c>
       <c r="S13" s="214">
-        <f>ETPT_ATT_JUR!S13</f>
+        <f>ETPT_ATTJ!S13</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix recodedFunction values for Att. J Siege Assises and CCD to match Excel formulas
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dinum-327809/Documents/a-just-dev/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67451E94-B29C-274D-8918-FE32A7FB46CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8633B384-6001-964A-B82D-5903BEEB9204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" activeTab="9" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
@@ -20939,27 +20939,27 @@
       <c r="I5" s="280" t="e" cm="1">
         <f t="array" ref="I5">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("1. TOTAL CONTENTIEUX SOCIAL",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("2. TOTAL CONTENTIEUX JAF",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("3. TOTAL CONTENTIEUX DE LA PROTECTION",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("4. TOTAL CIVIL NON SPÉCIALISÉ",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))+
 SUM(SUMIFS(
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("5. TOTAL JLD CIVIL",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("4. TOTAL CIVIL NON SPÉCIALISÉ",'ETPT Format DDG'!2:2,0)),
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.7. FONCTIONNAIRES AFFECTÉS AU CPH",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
@@ -20968,7 +20968,7 @@
       <c r="L5" s="280" t="e" cm="1">
         <f t="array" ref="L5">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.8. FONCTIONNAIRES AFFECTÉS AUX ACTIVITÉS CIVILES ET COMMERCIALES DU PARQUET",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
@@ -20978,7 +20978,7 @@
       <c r="P5" s="280" t="e" cm="1">
         <f t="array" ref="P5">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("6.1. ACTIVITÉ CIVILE",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
@@ -21042,48 +21042,48 @@
       <c r="I6" s="280" t="e" cm="1">
         <f t="array" ref="I6">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("7. TOTAL SIÈGE PÉNAL",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5)) -
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("7.51. COUR D'ASSISES JIRS",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5)) -
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("7.52. COUR CRIMINELLE",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("7.5. COUR D'ASSISES HORS JIRS",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
       <c r="J6" s="280" t="e" cm="1">
         <f t="array" ref="J6">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("7.5. COUR D'ASSISES HORS JIRS",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("7.51. COUR D'ASSISES JIRS",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
       <c r="K6" s="280" t="e" cm="1">
         <f t="array" ref="K6">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("7.52. COUR CRIMINELLE",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
       <c r="L6" s="280" t="e" cm="1">
         <f t="array" ref="L6">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.9. FONCTIONNAIRES AFFECTÉS À L'EXÉCUTION DES PEINES",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))+
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.10. AUTRES FONCTIONNAIRES AFFECTÉS AU PARQUET",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
@@ -21092,28 +21092,28 @@
       <c r="O6" s="280" t="e" cm="1">
         <f t="array" ref="O6">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("9. TOTAL JAP",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
       <c r="P6" s="280" t="e" cm="1">
         <f t="array" ref="P6">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("6.2. ACTIVITÉ PÉNALE",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
       <c r="Q6" s="280" t="e" cm="1">
         <f t="array" ref="Q6">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("8. TOTAL JUGES D'INSTRUCTION",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>
       <c r="R6" s="280" t="e" cm="1">
         <f t="array" ref="R6">SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("10. TOTAL JLD PÉNAL",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
         <v>#N/A</v>
       </c>

</xml_diff>

<commit_message>
Add conditional formatting rule to highlight rows where function code starts with 'JA'
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dinum-327809/Documents/a-just-dev/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{519EB016-6E2B-BF45-B5E5-B4BC372EEBC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9017EF-062B-544A-8703-0F0C6A643CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" activeTab="9" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" activeTab="2" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
   <sheets>
     <sheet name="ACCUEIL" sheetId="33" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="ETPT_TJ" sheetId="25" state="hidden" r:id="rId7"/>
     <sheet name="ETPT_TPRX" sheetId="26" state="hidden" r:id="rId8"/>
     <sheet name="ETPT_CPH" sheetId="27" state="hidden" r:id="rId9"/>
-    <sheet name="ETPT_ATTJ" sheetId="38" r:id="rId10"/>
+    <sheet name="ETPT_ATTJ" sheetId="38" state="hidden" r:id="rId10"/>
     <sheet name="ETPT_TJ_DDG" sheetId="28" r:id="rId11"/>
     <sheet name="ETPT_TPRX_DDG" sheetId="29" r:id="rId12"/>
     <sheet name="ETPT_CPH_DDG" sheetId="30" r:id="rId13"/>
@@ -19281,6 +19281,16 @@
   </cellStyles>
   <dxfs count="28">
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.79998168889431442"/>
@@ -19519,16 +19529,6 @@
       <font>
         <color theme="0"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -20667,8 +20667,8 @@
   </sheetPr>
   <dimension ref="A1:BL145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20954,6 +20954,10 @@
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))+
 SUM(SUMIFS(
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("5. TOTAL JLD CIVIL",'ETPT Format DDG'!2:2,0)),
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))+
+SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("11.7. FONCTIONNAIRES AFFECTÉS AU CPH",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
@@ -28002,7 +28006,7 @@
   <dimension ref="A1:BH22"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -31459,7 +31463,7 @@
   <dimension ref="A1:BJ27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="AC4" sqref="AC4"/>
@@ -36019,7 +36023,7 @@
   </sheetPr>
   <dimension ref="A1:DN8"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="AC136" sqref="AC136"/>
     </sheetView>
   </sheetViews>
@@ -36779,7 +36783,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AC9E93B-8E70-B54E-BC52-A477EEC4677F}">
   <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView topLeftCell="F6" workbookViewId="0">
+    <sheetView topLeftCell="J11" workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
@@ -37415,11 +37419,11 @@
   </sheetPr>
   <dimension ref="A1:FD4"/>
   <sheetViews>
-    <sheetView showFormulas="1" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="BL3" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="1" tabSelected="1" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -37502,8 +37506,8 @@
     <mergeCell ref="D1:Q1"/>
   </mergeCells>
   <conditionalFormatting sqref="A2:EZ2 A3:FB1048576">
-    <cfRule type="expression" dxfId="27" priority="1" stopIfTrue="1">
-      <formula>AND(OR($R1&lt;&gt;0,$S1&lt;&gt;0,$T1&lt;&gt;0,ISBLANK($P1)),ROW()&gt;2,$A1&lt;&gt;"")</formula>
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>OR(AND(OR($R1&lt;&gt;0,$S1&lt;&gt;0,$T1&lt;&gt;0,ISBLANK($P1)),ROW()&gt;2,$A1&lt;&gt;""),LEFT($F2,2)="JA")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -37833,70 +37837,70 @@
     <mergeCell ref="U4:V4"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:F4">
-    <cfRule type="expression" dxfId="26" priority="16">
+    <cfRule type="expression" dxfId="27" priority="16">
       <formula>IF(LEFT($A$3,2)&lt;&gt;"TJ",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:V151">
-    <cfRule type="expression" dxfId="25" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="18" stopIfTrue="1">
       <formula>AND(ISBLANK($C6)=FALSE,ISBLANK($E6)=TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:F1048576">
-    <cfRule type="expression" dxfId="24" priority="1">
+    <cfRule type="expression" dxfId="25" priority="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3)-_xlfn.NUMBERVALUE($U4)-_xlfn.NUMBERVALUE($U5)-_xlfn.NUMBERVALUE($U6),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="2">
+    <cfRule type="expression" dxfId="24" priority="2">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3)-_xlfn.NUMBERVALUE($S4)-_xlfn.NUMBERVALUE($S5)-_xlfn.NUMBERVALUE($S6),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="7" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($L1)-_xlfn.NUMBERVALUE($L2)-_xlfn.NUMBERVALUE($L3)-_xlfn.NUMBERVALUE($L4)-_xlfn.NUMBERVALUE($L5)-_xlfn.NUMBERVALUE($L6),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="12">
+    <cfRule type="expression" dxfId="22" priority="12">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",OR(ROUND(_xlfn.NUMBERVALUE($L1)-_xlfn.NUMBERVALUE($L2)-_xlfn.NUMBERVALUE($L3),3)&lt;&gt;0,ROUND(_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3),3)&lt;&gt;0,ROUND(_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3),3)&lt;&gt;0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:F7">
-    <cfRule type="expression" dxfId="20" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="6" stopIfTrue="1">
       <formula>OR(ROUND(_xlfn.NUMBERVALUE($L7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($L6),3),ROUND(_xlfn.NUMBERVALUE($S7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($S6),3),ROUND(_xlfn.NUMBERVALUE($U7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($U6),3))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:M1048576">
-    <cfRule type="expression" dxfId="19" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="11" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3)+_xlfn.NUMBERVALUE($L4)+_xlfn.NUMBERVALUE($L5)+_xlfn.NUMBERVALUE($L6)),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="15">
+    <cfRule type="expression" dxfId="19" priority="15">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",ROUND(_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3)),3)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:M7">
-    <cfRule type="expression" dxfId="17" priority="5">
+    <cfRule type="expression" dxfId="18" priority="5">
       <formula>ROUND(_xlfn.NUMBERVALUE($L7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($L6),3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:T1048576">
-    <cfRule type="expression" dxfId="16" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="10" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3)-_xlfn.NUMBERVALUE($S4)-_xlfn.NUMBERVALUE($S5)-_xlfn.NUMBERVALUE($S6),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="14">
+    <cfRule type="expression" dxfId="16" priority="14">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",ROUND(_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3),3)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7:T7">
-    <cfRule type="expression" dxfId="14" priority="4">
+    <cfRule type="expression" dxfId="15" priority="4">
       <formula>ROUND(_xlfn.NUMBERVALUE($S7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($S6),3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:V1048576">
-    <cfRule type="expression" dxfId="13" priority="9">
+    <cfRule type="expression" dxfId="14" priority="9">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3)-_xlfn.NUMBERVALUE($U4)-_xlfn.NUMBERVALUE($U5)-_xlfn.NUMBERVALUE($U6),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="13">
+    <cfRule type="expression" dxfId="13" priority="13">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",ROUND(_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3),3)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U7:V7">
-    <cfRule type="expression" dxfId="11" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="3" stopIfTrue="1">
       <formula>ROUND(_xlfn.NUMBERVALUE($U7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($U6),3)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -38199,57 +38203,57 @@
   </sheetData>
   <autoFilter ref="A1:V1" xr:uid="{02AF4949-5E39-2D4C-AD07-A4D8FB117F56}"/>
   <conditionalFormatting sqref="A1:B1">
-    <cfRule type="expression" dxfId="10" priority="30">
+    <cfRule type="expression" dxfId="11" priority="30">
       <formula>AND(OR($I1&lt;&gt;"-",#REF!&lt;&gt;0,#REF!&lt;&gt;0,ISBLANK($M1)),ROW()&gt;2,$A1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:F2">
-    <cfRule type="expression" dxfId="9" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="11" stopIfTrue="1">
       <formula>$F2="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:N2">
-    <cfRule type="expression" dxfId="8" priority="5">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>$F2="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:K2">
-    <cfRule type="expression" dxfId="7" priority="6">
+    <cfRule type="expression" dxfId="8" priority="6">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2">
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2">
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2">
-    <cfRule type="expression" dxfId="4" priority="9">
+    <cfRule type="expression" dxfId="5" priority="9">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:V2">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>$F2="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:R2">
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:T2">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fix conditional formatting column reference for function code check
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dinum-327809/Documents/a-just-dev/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9017EF-062B-544A-8703-0F0C6A643CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3A3F79-72D7-E047-84AC-5E68FF6DA48A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" activeTab="2" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
@@ -19279,7 +19279,17 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{6FC886D6-2077-B34D-B1DF-739B068A66D1}"/>
     <cellStyle name="Normal 3" xfId="4" xr:uid="{6BD57324-3FD5-D341-A299-730D14794802}"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="29">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -37420,10 +37430,10 @@
   <dimension ref="A1:FD4"/>
   <sheetViews>
     <sheetView showFormulas="1" tabSelected="1" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -37500,14 +37510,14 @@
       <c r="FA4" s="21"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" autoFilter="0"/>
+  <sheetProtection autoFilter="0"/>
   <autoFilter ref="A2:DT2" xr:uid="{3B89445B-6ECC-4440-B85C-E593AE209933}"/>
   <mergeCells count="1">
     <mergeCell ref="D1:Q1"/>
   </mergeCells>
   <conditionalFormatting sqref="A2:EZ2 A3:FB1048576">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>OR(AND(OR($R1&lt;&gt;0,$S1&lt;&gt;0,$T1&lt;&gt;0,ISBLANK($P1)),ROW()&gt;2,$A1&lt;&gt;""),LEFT($F2,2)="JA")</formula>
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>OR(AND(OR($R1&lt;&gt;0,$S1&lt;&gt;0,$T1&lt;&gt;0,ISBLANK($P1)),ROW()&gt;2,$A1&lt;&gt;""),LEFT($I2,2)="JA")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -37837,70 +37847,70 @@
     <mergeCell ref="U4:V4"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:F4">
-    <cfRule type="expression" dxfId="27" priority="16">
+    <cfRule type="expression" dxfId="28" priority="16">
       <formula>IF(LEFT($A$3,2)&lt;&gt;"TJ",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:V151">
-    <cfRule type="expression" dxfId="26" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="18" stopIfTrue="1">
       <formula>AND(ISBLANK($C6)=FALSE,ISBLANK($E6)=TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:F1048576">
-    <cfRule type="expression" dxfId="25" priority="1">
+    <cfRule type="expression" dxfId="26" priority="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3)-_xlfn.NUMBERVALUE($U4)-_xlfn.NUMBERVALUE($U5)-_xlfn.NUMBERVALUE($U6),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="2">
+    <cfRule type="expression" dxfId="25" priority="2">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3)-_xlfn.NUMBERVALUE($S4)-_xlfn.NUMBERVALUE($S5)-_xlfn.NUMBERVALUE($S6),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="7" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($L1)-_xlfn.NUMBERVALUE($L2)-_xlfn.NUMBERVALUE($L3)-_xlfn.NUMBERVALUE($L4)-_xlfn.NUMBERVALUE($L5)-_xlfn.NUMBERVALUE($L6),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="12">
+    <cfRule type="expression" dxfId="23" priority="12">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",OR(ROUND(_xlfn.NUMBERVALUE($L1)-_xlfn.NUMBERVALUE($L2)-_xlfn.NUMBERVALUE($L3),3)&lt;&gt;0,ROUND(_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3),3)&lt;&gt;0,ROUND(_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3),3)&lt;&gt;0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:F7">
-    <cfRule type="expression" dxfId="21" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="6" stopIfTrue="1">
       <formula>OR(ROUND(_xlfn.NUMBERVALUE($L7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($L6),3),ROUND(_xlfn.NUMBERVALUE($S7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($S6),3),ROUND(_xlfn.NUMBERVALUE($U7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($U6),3))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:M1048576">
-    <cfRule type="expression" dxfId="20" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="11" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3)+_xlfn.NUMBERVALUE($L4)+_xlfn.NUMBERVALUE($L5)+_xlfn.NUMBERVALUE($L6)),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="15">
+    <cfRule type="expression" dxfId="20" priority="15">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",ROUND(_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3)),3)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:M7">
-    <cfRule type="expression" dxfId="18" priority="5">
+    <cfRule type="expression" dxfId="19" priority="5">
       <formula>ROUND(_xlfn.NUMBERVALUE($L7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($L6),3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:T1048576">
-    <cfRule type="expression" dxfId="17" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="10" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3)-_xlfn.NUMBERVALUE($S4)-_xlfn.NUMBERVALUE($S5)-_xlfn.NUMBERVALUE($S6),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="14">
+    <cfRule type="expression" dxfId="17" priority="14">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",ROUND(_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3),3)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7:T7">
-    <cfRule type="expression" dxfId="15" priority="4">
+    <cfRule type="expression" dxfId="16" priority="4">
       <formula>ROUND(_xlfn.NUMBERVALUE($S7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($S6),3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:V1048576">
-    <cfRule type="expression" dxfId="14" priority="9">
+    <cfRule type="expression" dxfId="15" priority="9">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3)-_xlfn.NUMBERVALUE($U4)-_xlfn.NUMBERVALUE($U5)-_xlfn.NUMBERVALUE($U6),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="13">
+    <cfRule type="expression" dxfId="14" priority="13">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",ROUND(_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3),3)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U7:V7">
-    <cfRule type="expression" dxfId="12" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="3" stopIfTrue="1">
       <formula>ROUND(_xlfn.NUMBERVALUE($U7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($U6),3)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -38203,57 +38213,57 @@
   </sheetData>
   <autoFilter ref="A1:V1" xr:uid="{02AF4949-5E39-2D4C-AD07-A4D8FB117F56}"/>
   <conditionalFormatting sqref="A1:B1">
-    <cfRule type="expression" dxfId="11" priority="30">
+    <cfRule type="expression" dxfId="12" priority="30">
       <formula>AND(OR($I1&lt;&gt;"-",#REF!&lt;&gt;0,#REF!&lt;&gt;0,ISBLANK($M1)),ROW()&gt;2,$A1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:F2">
-    <cfRule type="expression" dxfId="10" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="11" stopIfTrue="1">
       <formula>$F2="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:N2">
-    <cfRule type="expression" dxfId="9" priority="5">
+    <cfRule type="expression" dxfId="10" priority="5">
       <formula>$F2="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:K2">
-    <cfRule type="expression" dxfId="8" priority="6">
+    <cfRule type="expression" dxfId="9" priority="6">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2">
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="8" priority="8">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2">
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="7" priority="7">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2">
-    <cfRule type="expression" dxfId="5" priority="9">
+    <cfRule type="expression" dxfId="6" priority="9">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:V2">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>$F2="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:R2">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:T2">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fix conditional formatting row offset - check current row instead of row below for JA function code
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dinum-327809/Documents/a-just-dev/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3A3F79-72D7-E047-84AC-5E68FF6DA48A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFF9B49-A96E-E448-8B02-56262FDE8ECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" activeTab="2" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
@@ -19279,17 +19279,7 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{6FC886D6-2077-B34D-B1DF-739B068A66D1}"/>
     <cellStyle name="Normal 3" xfId="4" xr:uid="{6BD57324-3FD5-D341-A299-730D14794802}"/>
   </cellStyles>
-  <dxfs count="29">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="28">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -37430,7 +37420,7 @@
   <dimension ref="A1:FD4"/>
   <sheetViews>
     <sheetView showFormulas="1" tabSelected="1" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
@@ -37510,14 +37500,14 @@
       <c r="FA4" s="21"/>
     </row>
   </sheetData>
-  <sheetProtection autoFilter="0"/>
+  <sheetProtection sheet="1" autoFilter="0"/>
   <autoFilter ref="A2:DT2" xr:uid="{3B89445B-6ECC-4440-B85C-E593AE209933}"/>
   <mergeCells count="1">
     <mergeCell ref="D1:Q1"/>
   </mergeCells>
   <conditionalFormatting sqref="A2:EZ2 A3:FB1048576">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>OR(AND(OR($R1&lt;&gt;0,$S1&lt;&gt;0,$T1&lt;&gt;0,ISBLANK($P1)),ROW()&gt;2,$A1&lt;&gt;""),LEFT($I2,2)="JA")</formula>
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>OR(AND(OR($R1&lt;&gt;0,$S1&lt;&gt;0,$T1&lt;&gt;0,ISBLANK($P1)),ROW()&gt;2,$A1&lt;&gt;""),LEFT($I1,2)="JA")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -37847,70 +37837,70 @@
     <mergeCell ref="U4:V4"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:F4">
-    <cfRule type="expression" dxfId="28" priority="16">
+    <cfRule type="expression" dxfId="27" priority="16">
       <formula>IF(LEFT($A$3,2)&lt;&gt;"TJ",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:V151">
-    <cfRule type="expression" dxfId="27" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="18" stopIfTrue="1">
       <formula>AND(ISBLANK($C6)=FALSE,ISBLANK($E6)=TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:F1048576">
-    <cfRule type="expression" dxfId="26" priority="1">
+    <cfRule type="expression" dxfId="25" priority="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3)-_xlfn.NUMBERVALUE($U4)-_xlfn.NUMBERVALUE($U5)-_xlfn.NUMBERVALUE($U6),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="2">
+    <cfRule type="expression" dxfId="24" priority="2">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3)-_xlfn.NUMBERVALUE($S4)-_xlfn.NUMBERVALUE($S5)-_xlfn.NUMBERVALUE($S6),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="7" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($L1)-_xlfn.NUMBERVALUE($L2)-_xlfn.NUMBERVALUE($L3)-_xlfn.NUMBERVALUE($L4)-_xlfn.NUMBERVALUE($L5)-_xlfn.NUMBERVALUE($L6),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="12">
+    <cfRule type="expression" dxfId="22" priority="12">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",OR(ROUND(_xlfn.NUMBERVALUE($L1)-_xlfn.NUMBERVALUE($L2)-_xlfn.NUMBERVALUE($L3),3)&lt;&gt;0,ROUND(_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3),3)&lt;&gt;0,ROUND(_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3),3)&lt;&gt;0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:F7">
-    <cfRule type="expression" dxfId="22" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="6" stopIfTrue="1">
       <formula>OR(ROUND(_xlfn.NUMBERVALUE($L7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($L6),3),ROUND(_xlfn.NUMBERVALUE($S7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($S6),3),ROUND(_xlfn.NUMBERVALUE($U7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($U6),3))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:M1048576">
-    <cfRule type="expression" dxfId="21" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="11" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3)+_xlfn.NUMBERVALUE($L4)+_xlfn.NUMBERVALUE($L5)+_xlfn.NUMBERVALUE($L6)),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="15">
+    <cfRule type="expression" dxfId="19" priority="15">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",ROUND(_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3)),3)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:M7">
-    <cfRule type="expression" dxfId="19" priority="5">
+    <cfRule type="expression" dxfId="18" priority="5">
       <formula>ROUND(_xlfn.NUMBERVALUE($L7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($L6),3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:T1048576">
-    <cfRule type="expression" dxfId="18" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="10" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3)-_xlfn.NUMBERVALUE($S4)-_xlfn.NUMBERVALUE($S5)-_xlfn.NUMBERVALUE($S6),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="14">
+    <cfRule type="expression" dxfId="16" priority="14">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",ROUND(_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3),3)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7:T7">
-    <cfRule type="expression" dxfId="16" priority="4">
+    <cfRule type="expression" dxfId="15" priority="4">
       <formula>ROUND(_xlfn.NUMBERVALUE($S7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($S6),3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:V1048576">
-    <cfRule type="expression" dxfId="15" priority="9">
+    <cfRule type="expression" dxfId="14" priority="9">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3)-_xlfn.NUMBERVALUE($U4)-_xlfn.NUMBERVALUE($U5)-_xlfn.NUMBERVALUE($U6),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="13">
+    <cfRule type="expression" dxfId="13" priority="13">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",ROUND(_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3),3)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U7:V7">
-    <cfRule type="expression" dxfId="13" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="3" stopIfTrue="1">
       <formula>ROUND(_xlfn.NUMBERVALUE($U7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($U6),3)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -38213,57 +38203,57 @@
   </sheetData>
   <autoFilter ref="A1:V1" xr:uid="{02AF4949-5E39-2D4C-AD07-A4D8FB117F56}"/>
   <conditionalFormatting sqref="A1:B1">
-    <cfRule type="expression" dxfId="12" priority="30">
+    <cfRule type="expression" dxfId="11" priority="30">
       <formula>AND(OR($I1&lt;&gt;"-",#REF!&lt;&gt;0,#REF!&lt;&gt;0,ISBLANK($M1)),ROW()&gt;2,$A1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:F2">
-    <cfRule type="expression" dxfId="11" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="11" stopIfTrue="1">
       <formula>$F2="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:N2">
-    <cfRule type="expression" dxfId="10" priority="5">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>$F2="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:K2">
-    <cfRule type="expression" dxfId="9" priority="6">
+    <cfRule type="expression" dxfId="8" priority="6">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2">
-    <cfRule type="expression" dxfId="8" priority="8">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2">
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2">
-    <cfRule type="expression" dxfId="6" priority="9">
+    <cfRule type="expression" dxfId="5" priority="9">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:V2">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>$F2="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:R2">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:T2">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Refine conditional formatting to match 'JA ' (with space) to exclude JAP function
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dinum-327809/Documents/a-just-dev/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFF9B49-A96E-E448-8B02-56262FDE8ECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81FCE37C-F06D-D34D-9018-EB66181FA98A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" activeTab="2" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
@@ -19279,7 +19279,27 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{6FC886D6-2077-B34D-B1DF-739B068A66D1}"/>
     <cellStyle name="Normal 3" xfId="4" xr:uid="{6BD57324-3FD5-D341-A299-730D14794802}"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="30">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -37423,7 +37443,7 @@
       <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -37500,14 +37520,14 @@
       <c r="FA4" s="21"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" autoFilter="0"/>
+  <sheetProtection autoFilter="0"/>
   <autoFilter ref="A2:DT2" xr:uid="{3B89445B-6ECC-4440-B85C-E593AE209933}"/>
   <mergeCells count="1">
     <mergeCell ref="D1:Q1"/>
   </mergeCells>
   <conditionalFormatting sqref="A2:EZ2 A3:FB1048576">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>OR(AND(OR($R1&lt;&gt;0,$S1&lt;&gt;0,$T1&lt;&gt;0,ISBLANK($P1)),ROW()&gt;2,$A1&lt;&gt;""),LEFT($I1,2)="JA")</formula>
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>OR(AND(OR($R1&lt;&gt;0,$S1&lt;&gt;0,$T1&lt;&gt;0,ISBLANK($P1)),ROW()&gt;2,$A1&lt;&gt;""),LEFT($I1,2)="JA ")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -37837,70 +37857,70 @@
     <mergeCell ref="U4:V4"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:F4">
-    <cfRule type="expression" dxfId="27" priority="16">
+    <cfRule type="expression" dxfId="29" priority="16">
       <formula>IF(LEFT($A$3,2)&lt;&gt;"TJ",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:V151">
-    <cfRule type="expression" dxfId="26" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="18" stopIfTrue="1">
       <formula>AND(ISBLANK($C6)=FALSE,ISBLANK($E6)=TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:F1048576">
-    <cfRule type="expression" dxfId="25" priority="1">
+    <cfRule type="expression" dxfId="27" priority="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3)-_xlfn.NUMBERVALUE($U4)-_xlfn.NUMBERVALUE($U5)-_xlfn.NUMBERVALUE($U6),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="2">
+    <cfRule type="expression" dxfId="26" priority="2">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3)-_xlfn.NUMBERVALUE($S4)-_xlfn.NUMBERVALUE($S5)-_xlfn.NUMBERVALUE($S6),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="7" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($L1)-_xlfn.NUMBERVALUE($L2)-_xlfn.NUMBERVALUE($L3)-_xlfn.NUMBERVALUE($L4)-_xlfn.NUMBERVALUE($L5)-_xlfn.NUMBERVALUE($L6),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="12">
+    <cfRule type="expression" dxfId="24" priority="12">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",OR(ROUND(_xlfn.NUMBERVALUE($L1)-_xlfn.NUMBERVALUE($L2)-_xlfn.NUMBERVALUE($L3),3)&lt;&gt;0,ROUND(_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3),3)&lt;&gt;0,ROUND(_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3),3)&lt;&gt;0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:F7">
-    <cfRule type="expression" dxfId="21" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="6" stopIfTrue="1">
       <formula>OR(ROUND(_xlfn.NUMBERVALUE($L7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($L6),3),ROUND(_xlfn.NUMBERVALUE($S7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($S6),3),ROUND(_xlfn.NUMBERVALUE($U7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($U6),3))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:M1048576">
-    <cfRule type="expression" dxfId="20" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="11" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3)+_xlfn.NUMBERVALUE($L4)+_xlfn.NUMBERVALUE($L5)+_xlfn.NUMBERVALUE($L6)),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="15">
+    <cfRule type="expression" dxfId="21" priority="15">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",ROUND(_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3)),3)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:M7">
-    <cfRule type="expression" dxfId="18" priority="5">
+    <cfRule type="expression" dxfId="20" priority="5">
       <formula>ROUND(_xlfn.NUMBERVALUE($L7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($L6),3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:T1048576">
-    <cfRule type="expression" dxfId="17" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="10" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3)-_xlfn.NUMBERVALUE($S4)-_xlfn.NUMBERVALUE($S5)-_xlfn.NUMBERVALUE($S6),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="14">
+    <cfRule type="expression" dxfId="18" priority="14">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",ROUND(_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3),3)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7:T7">
-    <cfRule type="expression" dxfId="15" priority="4">
+    <cfRule type="expression" dxfId="17" priority="4">
       <formula>ROUND(_xlfn.NUMBERVALUE($S7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($S6),3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:V1048576">
-    <cfRule type="expression" dxfId="14" priority="9">
+    <cfRule type="expression" dxfId="16" priority="9">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3)-_xlfn.NUMBERVALUE($U4)-_xlfn.NUMBERVALUE($U5)-_xlfn.NUMBERVALUE($U6),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="13">
+    <cfRule type="expression" dxfId="15" priority="13">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",ROUND(_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3),3)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U7:V7">
-    <cfRule type="expression" dxfId="12" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="3" stopIfTrue="1">
       <formula>ROUND(_xlfn.NUMBERVALUE($U7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($U6),3)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -38203,57 +38223,57 @@
   </sheetData>
   <autoFilter ref="A1:V1" xr:uid="{02AF4949-5E39-2D4C-AD07-A4D8FB117F56}"/>
   <conditionalFormatting sqref="A1:B1">
-    <cfRule type="expression" dxfId="11" priority="30">
+    <cfRule type="expression" dxfId="13" priority="30">
       <formula>AND(OR($I1&lt;&gt;"-",#REF!&lt;&gt;0,#REF!&lt;&gt;0,ISBLANK($M1)),ROW()&gt;2,$A1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:F2">
-    <cfRule type="expression" dxfId="10" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="11" stopIfTrue="1">
       <formula>$F2="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:N2">
-    <cfRule type="expression" dxfId="9" priority="5">
+    <cfRule type="expression" dxfId="11" priority="5">
       <formula>$F2="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:K2">
-    <cfRule type="expression" dxfId="8" priority="6">
+    <cfRule type="expression" dxfId="10" priority="6">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2">
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="9" priority="8">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2">
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="8" priority="7">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2">
-    <cfRule type="expression" dxfId="5" priority="9">
+    <cfRule type="expression" dxfId="7" priority="9">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:V2">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>$F2="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:R2">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:T2">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="4" priority="3">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fix GAUCHE to extract 3 characters for JA space check in conditional formatting
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dinum-327809/Documents/a-just-dev/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81FCE37C-F06D-D34D-9018-EB66181FA98A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1CB723-D4D5-6E4C-980E-5BC547F985EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" activeTab="2" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
@@ -19279,7 +19279,27 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{6FC886D6-2077-B34D-B1DF-739B068A66D1}"/>
     <cellStyle name="Normal 3" xfId="4" xr:uid="{6BD57324-3FD5-D341-A299-730D14794802}"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="32">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -37443,7 +37463,7 @@
       <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -37527,7 +37547,7 @@
   </mergeCells>
   <conditionalFormatting sqref="A2:EZ2 A3:FB1048576">
     <cfRule type="expression" dxfId="1" priority="1">
-      <formula>OR(AND(OR($R1&lt;&gt;0,$S1&lt;&gt;0,$T1&lt;&gt;0,ISBLANK($P1)),ROW()&gt;2,$A1&lt;&gt;""),LEFT($I1,2)="JA ")</formula>
+      <formula>OR(AND(OR($R1&lt;&gt;0,$S1&lt;&gt;0,$T1&lt;&gt;0,ISBLANK($P1)),ROW()&gt;2,$A1&lt;&gt;""),LEFT($I1,3)="JA ")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -37857,70 +37877,70 @@
     <mergeCell ref="U4:V4"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:F4">
-    <cfRule type="expression" dxfId="29" priority="16">
+    <cfRule type="expression" dxfId="31" priority="16">
       <formula>IF(LEFT($A$3,2)&lt;&gt;"TJ",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:V151">
-    <cfRule type="expression" dxfId="28" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="18" stopIfTrue="1">
       <formula>AND(ISBLANK($C6)=FALSE,ISBLANK($E6)=TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:F1048576">
-    <cfRule type="expression" dxfId="27" priority="1">
+    <cfRule type="expression" dxfId="29" priority="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3)-_xlfn.NUMBERVALUE($U4)-_xlfn.NUMBERVALUE($U5)-_xlfn.NUMBERVALUE($U6),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="2">
+    <cfRule type="expression" dxfId="28" priority="2">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3)-_xlfn.NUMBERVALUE($S4)-_xlfn.NUMBERVALUE($S5)-_xlfn.NUMBERVALUE($S6),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="7" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($L1)-_xlfn.NUMBERVALUE($L2)-_xlfn.NUMBERVALUE($L3)-_xlfn.NUMBERVALUE($L4)-_xlfn.NUMBERVALUE($L5)-_xlfn.NUMBERVALUE($L6),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="12">
+    <cfRule type="expression" dxfId="26" priority="12">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",OR(ROUND(_xlfn.NUMBERVALUE($L1)-_xlfn.NUMBERVALUE($L2)-_xlfn.NUMBERVALUE($L3),3)&lt;&gt;0,ROUND(_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3),3)&lt;&gt;0,ROUND(_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3),3)&lt;&gt;0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:F7">
-    <cfRule type="expression" dxfId="23" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="6" stopIfTrue="1">
       <formula>OR(ROUND(_xlfn.NUMBERVALUE($L7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($L6),3),ROUND(_xlfn.NUMBERVALUE($S7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($S6),3),ROUND(_xlfn.NUMBERVALUE($U7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($U6),3))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:M1048576">
-    <cfRule type="expression" dxfId="22" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="11" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3)+_xlfn.NUMBERVALUE($L4)+_xlfn.NUMBERVALUE($L5)+_xlfn.NUMBERVALUE($L6)),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="15">
+    <cfRule type="expression" dxfId="23" priority="15">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",ROUND(_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3)),3)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:M7">
-    <cfRule type="expression" dxfId="20" priority="5">
+    <cfRule type="expression" dxfId="22" priority="5">
       <formula>ROUND(_xlfn.NUMBERVALUE($L7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($L6),3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:T1048576">
-    <cfRule type="expression" dxfId="19" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="10" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3)-_xlfn.NUMBERVALUE($S4)-_xlfn.NUMBERVALUE($S5)-_xlfn.NUMBERVALUE($S6),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="14">
+    <cfRule type="expression" dxfId="20" priority="14">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",ROUND(_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3),3)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7:T7">
-    <cfRule type="expression" dxfId="17" priority="4">
+    <cfRule type="expression" dxfId="19" priority="4">
       <formula>ROUND(_xlfn.NUMBERVALUE($S7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($S6),3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:V1048576">
-    <cfRule type="expression" dxfId="16" priority="9">
+    <cfRule type="expression" dxfId="18" priority="9">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",ROUND(_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3)-_xlfn.NUMBERVALUE($U4)-_xlfn.NUMBERVALUE($U5)-_xlfn.NUMBERVALUE($U6),3)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="13">
+    <cfRule type="expression" dxfId="17" priority="13">
       <formula>AND($D1="6. TOTAL JUGES DES ENFANTS",ROUND(_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3),3)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U7:V7">
-    <cfRule type="expression" dxfId="14" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="3" stopIfTrue="1">
       <formula>ROUND(_xlfn.NUMBERVALUE($U7),3)&lt;&gt;ROUND(_xlfn.NUMBERVALUE($U6),3)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -38223,57 +38243,57 @@
   </sheetData>
   <autoFilter ref="A1:V1" xr:uid="{02AF4949-5E39-2D4C-AD07-A4D8FB117F56}"/>
   <conditionalFormatting sqref="A1:B1">
-    <cfRule type="expression" dxfId="13" priority="30">
+    <cfRule type="expression" dxfId="15" priority="30">
       <formula>AND(OR($I1&lt;&gt;"-",#REF!&lt;&gt;0,#REF!&lt;&gt;0,ISBLANK($M1)),ROW()&gt;2,$A1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:F2">
-    <cfRule type="expression" dxfId="12" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="11" stopIfTrue="1">
       <formula>$F2="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:N2">
-    <cfRule type="expression" dxfId="11" priority="5">
+    <cfRule type="expression" dxfId="13" priority="5">
       <formula>$F2="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:K2">
-    <cfRule type="expression" dxfId="10" priority="6">
+    <cfRule type="expression" dxfId="12" priority="6">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2">
-    <cfRule type="expression" dxfId="9" priority="8">
+    <cfRule type="expression" dxfId="11" priority="8">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2">
-    <cfRule type="expression" dxfId="8" priority="7">
+    <cfRule type="expression" dxfId="10" priority="7">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2">
-    <cfRule type="expression" dxfId="7" priority="9">
+    <cfRule type="expression" dxfId="9" priority="9">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:V2">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>$F2="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:R2">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="7" priority="4">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:T2">
-    <cfRule type="expression" dxfId="4" priority="3">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add additional MAX(0; flooring to more formulas in template4
</commit_message>
<xml_diff>
--- a/front/src/assets/template4.xlsx
+++ b/front/src/assets/template4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dinum-327809/Documents/a-just-dev/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1CB723-D4D5-6E4C-980E-5BC547F985EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A63A948-13E0-4949-B8D2-2BA472C0F735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" activeTab="2" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" activeTab="9" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
   <sheets>
     <sheet name="ACCUEIL" sheetId="33" r:id="rId1"/>
@@ -19,10 +19,10 @@
     <sheet name="Synthèse ETPT" sheetId="10" r:id="rId4"/>
     <sheet name="Table_Fonctions" sheetId="19" state="hidden" r:id="rId5"/>
     <sheet name="ETPT Format DDG DETAIL" sheetId="41" state="hidden" r:id="rId6"/>
-    <sheet name="ETPT_TJ" sheetId="25" state="hidden" r:id="rId7"/>
+    <sheet name="ETPT_TJ" sheetId="25" r:id="rId7"/>
     <sheet name="ETPT_TPRX" sheetId="26" state="hidden" r:id="rId8"/>
     <sheet name="ETPT_CPH" sheetId="27" state="hidden" r:id="rId9"/>
-    <sheet name="ETPT_ATTJ" sheetId="38" state="hidden" r:id="rId10"/>
+    <sheet name="ETPT_ATTJ" sheetId="38" r:id="rId10"/>
     <sheet name="ETPT_TJ_DDG" sheetId="28" r:id="rId11"/>
     <sheet name="ETPT_TPRX_DDG" sheetId="29" r:id="rId12"/>
     <sheet name="ETPT_CPH_DDG" sheetId="30" r:id="rId13"/>
@@ -20707,8 +20707,8 @@
   </sheetPr>
   <dimension ref="A1:BL145"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="G4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21080,7 +21080,7 @@
         <v>#N/A</v>
       </c>
       <c r="I6" s="280" t="e" cm="1">
-        <f t="array" ref="I6">SUM(SUMIFS(
+        <f t="array" ref="I6">MAX(0,SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("7. TOTAL SIÈGE PÉNAL",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5)) -
@@ -21095,7 +21095,7 @@
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("7.5. COUR D'ASSISES HORS JIRS",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"JA/AttJ JAP";"JA/AttJ JE";"JA/AttJ JI";"JA/AttJ JLD PÉNAL";"JA/AttJ Parquet";"JA/AttJ Siège autres";"JA/AttJ Siege Assises";"JA/AttJ Siege CCD"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5)))</f>
         <v>#N/A</v>
       </c>
       <c r="J6" s="280" t="e" cm="1">
@@ -21631,115 +21631,115 @@
         <v>47</v>
       </c>
       <c r="G11" s="279" t="e" cm="1">
-        <f t="array" ref="G11">SUM(SUMIFS(
+        <f t="array" ref="G11">MAX(0,SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"CONT A JP Siège";"CONT A VIF Siège"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"CONT A JP Siège";"CONT A VIF Siège"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5)))</f>
         <v>#N/A</v>
       </c>
       <c r="H11" s="279" t="e" cm="1">
-        <f t="array" ref="H11">SUM(SUMIFS(
+        <f t="array" ref="H11">MAX(0,SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"CONT A JP Parquet";"CONT A VIF Parquet"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),{"CONT A JP Parquet";"CONT A VIF Parquet"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5)))</f>
         <v>#N/A</v>
       </c>
       <c r="I11" s="280" t="e">
-        <f>SUM(SUMIFS(
+        <f>MAX(0,SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ Siège autres",
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ Siège autres",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5)))</f>
         <v>#N/A</v>
       </c>
       <c r="J11" s="280" t="e">
-        <f>SUM(SUMIFS(
+        <f>MAX(0,SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ Siege Assises",
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ Siege Assises",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5)))</f>
         <v>#N/A</v>
       </c>
       <c r="K11" s="280" t="e">
-        <f>SUM(SUMIFS(
+        <f>MAX(0,SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ Siege CCD",
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ Siege CCD",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5)))</f>
         <v>#N/A</v>
       </c>
       <c r="L11" s="280" t="e">
-        <f>SUM(SUMIFS(
+        <f>MAX(0,SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ Parquet",
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ Parquet",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5)))</f>
         <v>#N/A</v>
       </c>
       <c r="M11" s="280"/>
       <c r="N11" s="280"/>
       <c r="O11" s="280" t="e">
-        <f>SUM(SUMIFS(
+        <f>MAX(0,SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JAP",
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JAP",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5)))</f>
         <v>#N/A</v>
       </c>
       <c r="P11" s="280" t="e">
-        <f>SUM(SUMIFS(
+        <f>MAX(0,SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JE",
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JE",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5)))</f>
         <v>#N/A</v>
       </c>
       <c r="Q11" s="280" t="e">
-        <f>SUM(SUMIFS(
+        <f>MAX(0,SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JI",
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JI",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5)))</f>
         <v>#N/A</v>
       </c>
       <c r="R11" s="280" t="e">
-        <f>SUM(SUMIFS(
+        <f>MAX(0,SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JLD PÉNAL",
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"JA/AttJ JLD PÉNAL",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Juridiction",'ETPT Format DDG'!2:2,0)),$D$5)))</f>
         <v>#N/A</v>
       </c>
       <c r="S11" s="278">
@@ -24823,8 +24823,8 @@
   </sheetPr>
   <dimension ref="A1:BG22"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="AJ1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView showGridLines="0" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -37459,7 +37459,7 @@
   </sheetPr>
   <dimension ref="A1:FD4"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showFormulas="1" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -38310,11 +38310,11 @@
   <dimension ref="A1:BF24"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="AU2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
-      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
+      <selection pane="bottomRight" activeCell="AU15" sqref="AU15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -39066,14 +39066,14 @@
         <v>#N/A</v>
       </c>
       <c r="AS5" s="54" t="e">
-        <f>SUM(SUMIFS(
+        <f>MAX(0,SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("4. TOTAL CIVIL NON SPÉCIALISÉ",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat SIEGE S",
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("4.0. CONTENTIEUX GÉNÉRAL &lt;10.000€",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat SIEGE S",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI")))</f>
         <v>#N/A</v>
       </c>
       <c r="AT5" s="54" t="e" cm="1">
@@ -39083,14 +39083,14 @@
         <v>#N/A</v>
       </c>
       <c r="AU5" s="54" t="e">
-        <f>SUM(SUMIFS(
+        <f>MAX(0,SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("4. TOTAL CIVIL NON SPÉCIALISÉ",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat SIEGE NS",
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("4.0. CONTENTIEUX GÉNÉRAL &lt;10.000€",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat SIEGE NS",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI")))</f>
         <v>#N/A</v>
       </c>
       <c r="AV5" s="46">
@@ -39229,7 +39229,7 @@
         <v>270</v>
       </c>
       <c r="V6" s="202" t="e">
-        <f>SUM(SUMIFS(
+        <f>MAX(0,SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("7. TOTAL SIÈGE PÉNAL",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR"))+
 SUM(SUMIFS(
@@ -39252,7 +39252,7 @@
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("7.122. COLLÉGIALES AUTRES SECTIONS SPÉCIALISÉES",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR"))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR")))</f>
         <v>#N/A</v>
       </c>
       <c r="W6" s="46">
@@ -39363,7 +39363,7 @@
       <c r="AQ6" s="64"/>
       <c r="AR6" s="64"/>
       <c r="AS6" s="54" t="e">
-        <f>SUMIFS(
+        <f>MAX(0,SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("7. TOTAL SIÈGE PÉNAL",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat SIEGE S")-
 SUMIFS(
@@ -39389,12 +39389,12 @@
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat SIEGE S")-
 SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("7.7. OP CONTRAVENTIONNELLES",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat SIEGE S")</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat SIEGE S"))</f>
         <v>#N/A</v>
       </c>
       <c r="AT6" s="54"/>
       <c r="AU6" s="63" t="e">
-        <f>SUMIFS(
+        <f>MAX(0,SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("7. TOTAL SIÈGE PÉNAL",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat SIEGE NS")-
 SUMIFS(
@@ -39420,7 +39420,7 @@
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat SIEGE NS")-
 SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("7.7. OP CONTRAVENTIONNELLES",'ETPT Format DDG'!2:2,0)),
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat SIEGE NS")</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat SIEGE NS"))</f>
         <v>#N/A</v>
       </c>
       <c r="AV6" s="46">
@@ -40174,14 +40174,14 @@
         <v>47</v>
       </c>
       <c r="G12" s="89" t="e">
-        <f>SUM(SUMIFS(
+        <f>MAX(0,SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire CTECH",
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire CTECH",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI")))</f>
         <v>#N/A</v>
       </c>
       <c r="H12" s="57">
@@ -40202,14 +40202,14 @@
       <c r="T12" s="60"/>
       <c r="U12" s="60"/>
       <c r="V12" s="52" t="e">
-        <f>SUM(SUMIFS(
+        <f>MAX(0,SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR",
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Fonctionnaire A-B-CBUR",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI")))</f>
         <v>#N/A</v>
       </c>
       <c r="W12" s="46">
@@ -40229,50 +40229,50 @@
         <v>#N/A</v>
       </c>
       <c r="Z12" s="52" t="e" cm="1">
-        <f t="array" ref="Z12">SUM(SUMIFS(
+        <f t="array" ref="Z12">MAX(0,SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JI";"VPI";"1VPI"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JI";"VPI";"1VPI"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI")))</f>
         <v>#N/A</v>
       </c>
       <c r="AA12" s="60"/>
       <c r="AB12" s="60"/>
       <c r="AC12" s="60"/>
       <c r="AD12" s="52" t="e" cm="1">
-        <f t="array" ref="AD12">SUM(SUMIFS(
+        <f t="array" ref="AD12">MAX(0,SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JAP";"VPAP";"1VPAP"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JAP";"VPAP";"1VPAP"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI")))</f>
         <v>#N/A</v>
       </c>
       <c r="AE12" s="52" t="e" cm="1">
-        <f t="array" ref="AE12">SUM(SUMIFS(
+        <f t="array" ref="AE12">MAX(0,SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JE";"VPE";"1VPE"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"JE";"VPE";"1VPE"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI")))</f>
         <v>#N/A</v>
       </c>
       <c r="AF12" s="52" t="e" cm="1">
-        <f t="array" ref="AF12">SUM(SUMIFS(
+        <f t="array" ref="AF12">MAX(0,SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"VPLD";"1VPLD"},
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction",'ETPT Format DDG'!2:2,0)),{"VPLD";"1VPLD"},
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI")))</f>
         <v>#N/A</v>
       </c>
       <c r="AG12" s="46">
@@ -40293,14 +40293,14 @@
       <c r="AS12" s="60"/>
       <c r="AT12" s="60"/>
       <c r="AU12" s="52" t="e">
-        <f>SUM(SUMIFS(
+        <f>MAX(0,SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat SIEGE NS",
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("12.5. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),
 INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT Format DDG'!2:2,0)),"Magistrat SIEGE NS",
-INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI"))</f>
+INDEX( 'ETPT Format DDG'!$A:$ZZ,,MATCH("TJCPH",'ETPT Format DDG'!2:2,0)),"OUI")))</f>
         <v>#N/A</v>
       </c>
       <c r="AV12" s="46">
@@ -40844,14 +40844,14 @@
         <v>#N/A</v>
       </c>
       <c r="AQ14" s="52" t="e">
-        <f>SUM(SUMIFS(
+        <f>MAX(0,SUM(SUMIFS(
 INDEX( 'ETPT A-JUST'!$A:$ZZ,,MATCH("1. TOTAL CONTENTIEUX SOCIAL",'ETPT A-JUST'!2:2,0)),
 INDEX( 'ETPT A-JUST'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT A-JUST'!2:2,0)),"Magistrat placé ADD",
 INDEX( 'ETPT A-JUST'!$A:$ZZ,,MATCH("TJCPH",'ETPT A-JUST'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT A-JUST'!$A:$ZZ,,MATCH("1.1. DÉPARTAGE PRUD'HOMAL",'ETPT A-JUST'!2:2,0)),
 INDEX( 'ETPT A-JUST'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT A-JUST'!2:2,0)),"Magistrat placé ADD",
-INDEX( 'ETPT A-JUST'!$A:$ZZ,,MATCH("TJCPH",'ETPT A-JUST'!2:2,0)),"OUI"))</f>
+INDEX( 'ETPT A-JUST'!$A:$ZZ,,MATCH("TJCPH",'ETPT A-JUST'!2:2,0)),"OUI")))</f>
         <v>#N/A</v>
       </c>
       <c r="AR14" s="52" t="e">
@@ -40868,7 +40868,7 @@
         <v>#N/A</v>
       </c>
       <c r="AU14" s="265" t="e">
-        <f>SUM(SUMIFS(
+        <f>MAX(0,SUM(SUMIFS(
 INDEX( 'ETPT A-JUST'!$A:$ZZ,,MATCH("4. TOTAL CIVIL NON SPÉCIALISÉ",'ETPT A-JUST'!2:2,0)),
 INDEX( 'ETPT A-JUST'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT A-JUST'!2:2,0)),"Magistrat placé ADD",
 INDEX( 'ETPT A-JUST'!$A:$ZZ,,MATCH("TJCPH",'ETPT A-JUST'!2:2,0)),"OUI"))-
@@ -40935,7 +40935,7 @@
 INDEX( 'ETPT A-JUST'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT A-JUST'!2:2,0)),"Magistrat placé ADD"))-
 SUM(SUMIFS(
 INDEX( 'ETPT A-JUST'!$A:$ZZ,,MATCH("7.7. OP CONTRAVENTIONNELLES",'ETPT A-JUST'!2:2,0)),
-INDEX( 'ETPT A-JUST'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT A-JUST'!2:2,0)),"Magistrat placé ADD"))</f>
+INDEX( 'ETPT A-JUST'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT A-JUST'!2:2,0)),"Magistrat placé ADD")))</f>
         <v>#N/A</v>
       </c>
       <c r="AV14" s="46">
@@ -41186,7 +41186,7 @@
         <v>#N/A</v>
       </c>
       <c r="Y15" s="52" t="e">
-        <f>SUM(SUMIFS(
+        <f>MAX(0,SUM(SUMIFS(
 INDEX( 'ETPT A-JUST'!$A:$ZZ,,MATCH("3. TOTAL CONTENTIEUX DE LA PROTECTION",'ETPT A-JUST'!2:2,0)),
 INDEX( 'ETPT A-JUST'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT A-JUST'!2:2,0)),"Magistrat placé SUB",
 INDEX( 'ETPT A-JUST'!$A:$ZZ,,MATCH("TJCPH",'ETPT A-JUST'!2:2,0)),"OUI"))-
@@ -41201,7 +41201,7 @@
 SUM(SUMIFS(
 INDEX( 'ETPT A-JUST'!$A:$ZZ,,MATCH("3.44. SAISIE DES RÉMUNÉRATIONS",'ETPT A-JUST'!2:2,0)),
 INDEX( 'ETPT A-JUST'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT A-JUST'!2:2,0)),"Magistrat placé SUB",
-INDEX( 'ETPT A-JUST'!$A:$ZZ,,MATCH("TJCPH",'ETPT A-JUST'!2:2,0)),"OUI"))</f>
+INDEX( 'ETPT A-JUST'!$A:$ZZ,,MATCH("TJCPH",'ETPT A-JUST'!2:2,0)),"OUI")))</f>
         <v>#N/A</v>
       </c>
       <c r="Z15" s="52" t="e">
@@ -41329,14 +41329,14 @@
         <v>#N/A</v>
       </c>
       <c r="AQ15" s="52" t="e">
-        <f>SUM(SUMIFS(
+        <f>MAX(0,SUM(SUMIFS(
 INDEX( 'ETPT A-JUST'!$A:$ZZ,,MATCH("1. TOTAL CONTENTIEUX SOCIAL",'ETPT A-JUST'!2:2,0)),
 INDEX( 'ETPT A-JUST'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT A-JUST'!2:2,0)),"Magistrat placé SUB",
 INDEX( 'ETPT A-JUST'!$A:$ZZ,,MATCH("TJCPH",'ETPT A-JUST'!2:2,0)),"OUI"))-
 SUM(SUMIFS(
 INDEX( 'ETPT A-JUST'!$A:$ZZ,,MATCH("1.1. DÉPARTAGE PRUD'HOMAL",'ETPT A-JUST'!2:2,0)),
 INDEX( 'ETPT A-JUST'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT A-JUST'!2:2,0)),"Magistrat placé SUB",
-INDEX( 'ETPT A-JUST'!$A:$ZZ,,MATCH("TJCPH",'ETPT A-JUST'!2:2,0)),"OUI"))</f>
+INDEX( 'ETPT A-JUST'!$A:$ZZ,,MATCH("TJCPH",'ETPT A-JUST'!2:2,0)),"OUI")))</f>
         <v>#N/A</v>
       </c>
       <c r="AR15" s="52" t="e">

</xml_diff>